<commit_message>
Erroneous data input into Below Imperial Dam: Gila River.Local Inflow cleared. 2019 and 2020 added to the Frequency tab in the MTOM_EnsembleOutput file.
</commit_message>
<xml_diff>
--- a/Output Data/MtomToCrss_Annual.xlsx
+++ b/Output Data/MtomToCrss_Annual.xlsx
@@ -5,52 +5,50 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\MTOM\dev\Output Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\COM460\RiverWare Models\Monthly Models\MTOM_Production\_MAY18\Output Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15720" windowHeight="10980"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="9900"/>
   </bookViews>
   <sheets>
-    <sheet name="Trace38" sheetId="39" r:id="rId1"/>
-    <sheet name="Trace37" sheetId="38" r:id="rId2"/>
-    <sheet name="Trace36" sheetId="37" r:id="rId3"/>
-    <sheet name="Trace35" sheetId="36" r:id="rId4"/>
-    <sheet name="Trace34" sheetId="35" r:id="rId5"/>
-    <sheet name="Trace33" sheetId="34" r:id="rId6"/>
-    <sheet name="Trace32" sheetId="33" r:id="rId7"/>
-    <sheet name="Trace31" sheetId="32" r:id="rId8"/>
-    <sheet name="Trace30" sheetId="31" r:id="rId9"/>
-    <sheet name="Trace29" sheetId="30" r:id="rId10"/>
-    <sheet name="Trace28" sheetId="29" r:id="rId11"/>
-    <sheet name="Trace27" sheetId="28" r:id="rId12"/>
-    <sheet name="Trace26" sheetId="27" r:id="rId13"/>
-    <sheet name="Trace25" sheetId="26" r:id="rId14"/>
-    <sheet name="Trace24" sheetId="25" r:id="rId15"/>
-    <sheet name="Trace23" sheetId="24" r:id="rId16"/>
-    <sheet name="Trace22" sheetId="23" r:id="rId17"/>
-    <sheet name="Trace21" sheetId="22" r:id="rId18"/>
-    <sheet name="Trace20" sheetId="21" r:id="rId19"/>
-    <sheet name="Trace19" sheetId="20" r:id="rId20"/>
-    <sheet name="Trace18" sheetId="19" r:id="rId21"/>
-    <sheet name="Trace17" sheetId="18" r:id="rId22"/>
-    <sheet name="Trace16" sheetId="17" r:id="rId23"/>
-    <sheet name="Trace15" sheetId="16" r:id="rId24"/>
-    <sheet name="Trace14" sheetId="15" r:id="rId25"/>
-    <sheet name="Trace13" sheetId="14" r:id="rId26"/>
-    <sheet name="Trace12" sheetId="13" r:id="rId27"/>
-    <sheet name="Trace11" sheetId="12" r:id="rId28"/>
-    <sheet name="Trace10" sheetId="11" r:id="rId29"/>
-    <sheet name="Trace9" sheetId="10" r:id="rId30"/>
-    <sheet name="Trace8" sheetId="9" r:id="rId31"/>
-    <sheet name="Trace7" sheetId="8" r:id="rId32"/>
-    <sheet name="Trace6" sheetId="7" r:id="rId33"/>
-    <sheet name="Trace5" sheetId="6" r:id="rId34"/>
-    <sheet name="Trace4" sheetId="5" r:id="rId35"/>
-    <sheet name="Trace3" sheetId="4" r:id="rId36"/>
-    <sheet name="Trace2" sheetId="3" r:id="rId37"/>
-    <sheet name="Trace1" sheetId="2" r:id="rId38"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId39"/>
+    <sheet name="Trace38" sheetId="37" r:id="rId1"/>
+    <sheet name="Trace37" sheetId="36" r:id="rId2"/>
+    <sheet name="Trace36" sheetId="35" r:id="rId3"/>
+    <sheet name="Trace35" sheetId="34" r:id="rId4"/>
+    <sheet name="Trace34" sheetId="33" r:id="rId5"/>
+    <sheet name="Trace33" sheetId="32" r:id="rId6"/>
+    <sheet name="Trace32" sheetId="31" r:id="rId7"/>
+    <sheet name="Trace31" sheetId="30" r:id="rId8"/>
+    <sheet name="Trace30" sheetId="29" r:id="rId9"/>
+    <sheet name="Trace29" sheetId="28" r:id="rId10"/>
+    <sheet name="Trace28" sheetId="27" r:id="rId11"/>
+    <sheet name="Trace27" sheetId="26" r:id="rId12"/>
+    <sheet name="Trace26" sheetId="25" r:id="rId13"/>
+    <sheet name="Trace25" sheetId="24" r:id="rId14"/>
+    <sheet name="Trace24" sheetId="23" r:id="rId15"/>
+    <sheet name="Trace23" sheetId="22" r:id="rId16"/>
+    <sheet name="Trace22" sheetId="21" r:id="rId17"/>
+    <sheet name="Trace21" sheetId="20" r:id="rId18"/>
+    <sheet name="Trace20" sheetId="19" r:id="rId19"/>
+    <sheet name="Trace19" sheetId="18" r:id="rId20"/>
+    <sheet name="Trace18" sheetId="17" r:id="rId21"/>
+    <sheet name="Trace17" sheetId="16" r:id="rId22"/>
+    <sheet name="Trace16" sheetId="15" r:id="rId23"/>
+    <sheet name="Trace15" sheetId="14" r:id="rId24"/>
+    <sheet name="Trace14" sheetId="13" r:id="rId25"/>
+    <sheet name="Trace13" sheetId="12" r:id="rId26"/>
+    <sheet name="Trace12" sheetId="11" r:id="rId27"/>
+    <sheet name="Trace11" sheetId="10" r:id="rId28"/>
+    <sheet name="Trace10" sheetId="9" r:id="rId29"/>
+    <sheet name="Trace9" sheetId="8" r:id="rId30"/>
+    <sheet name="Trace8" sheetId="7" r:id="rId31"/>
+    <sheet name="Trace7" sheetId="6" r:id="rId32"/>
+    <sheet name="Trace6" sheetId="5" r:id="rId33"/>
+    <sheet name="Trace5" sheetId="4" r:id="rId34"/>
+    <sheet name="Trace4" sheetId="3" r:id="rId35"/>
+    <sheet name="Trace3" sheetId="2" r:id="rId36"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId37"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -62,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="9">
   <si>
     <t>ICS Credits.BiNationalICS_CA</t>
   </si>
@@ -414,9 +412,9 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -442,21 +440,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
       <c r="B2">
-        <v>23750.000000037602</v>
+        <v>23750.000000037599</v>
       </c>
       <c r="C2">
-        <v>38659.350000427432</v>
+        <v>38659.350000427519</v>
       </c>
       <c r="D2">
-        <v>80404.999999993175</v>
+        <v>80404.999999993204</v>
       </c>
       <c r="E2">
-        <v>142814.35000045819</v>
+        <v>142814.3500004583</v>
       </c>
       <c r="F2">
         <v>8999999.9999775533</v>
@@ -465,36 +463,36 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9127184.2205391396</v>
+        <v>9185872.9543969855</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
       <c r="B3">
-        <v>23750.000000037602</v>
+        <v>23750.000000037599</v>
       </c>
       <c r="C3">
-        <v>54150.395503639265</v>
+        <v>54150.395503639542</v>
       </c>
       <c r="D3">
-        <v>80404.999999993175</v>
+        <v>80404.999999993204</v>
       </c>
       <c r="E3">
-        <v>158305.39550367004</v>
+        <v>158305.39550367033</v>
       </c>
       <c r="F3">
-        <v>8789056.161036998</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>8900035.8202567063</v>
+        <v>9110979.6591972616</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -511,9 +509,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -539,21 +537,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
       <c r="B2">
-        <v>23750.000000037602</v>
+        <v>23750.000000037599</v>
       </c>
       <c r="C2">
-        <v>614659.3500000285</v>
+        <v>614659.35000002873</v>
       </c>
       <c r="D2">
-        <v>80404.999999993175</v>
+        <v>80404.999999993204</v>
       </c>
       <c r="E2">
-        <v>718814.35000005935</v>
+        <v>718814.35000005946</v>
       </c>
       <c r="F2">
         <v>8999999.9999775533</v>
@@ -562,27 +560,27 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9199058.3678916693</v>
+        <v>9252939.612821253</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
       <c r="B3">
-        <v>23750.000000037602</v>
+        <v>23750.000000037599</v>
       </c>
       <c r="C3">
-        <v>499219.56949983269</v>
+        <v>499219.56949983287</v>
       </c>
       <c r="D3">
-        <v>80404.999999993175</v>
+        <v>80404.999999993204</v>
       </c>
       <c r="E3">
-        <v>603374.56949986354</v>
+        <v>603374.56949986366</v>
       </c>
       <c r="F3">
         <v>8999999.9999775533</v>
@@ -608,9 +606,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -636,18 +634,18 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
       <c r="B2">
-        <v>23750.000000037602</v>
+        <v>23750.000000037599</v>
       </c>
       <c r="C2">
-        <v>472159.35000012722</v>
+        <v>472159.35000012728</v>
       </c>
       <c r="D2">
-        <v>80404.999999993175</v>
+        <v>80404.999999993204</v>
       </c>
       <c r="E2">
         <v>576314.35000015807</v>
@@ -659,24 +657,24 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9138544.9778916668</v>
+        <v>9197781.1928212512</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
       <c r="B3">
-        <v>23750.000000037602</v>
+        <v>23750.000000037599</v>
       </c>
       <c r="C3">
         <v>742994.56949992606</v>
       </c>
       <c r="D3">
-        <v>80404.999999993175</v>
+        <v>80404.999999993204</v>
       </c>
       <c r="E3">
         <v>847149.56949995691</v>
@@ -705,9 +703,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -733,21 +731,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
       <c r="B2">
-        <v>23750.000000037602</v>
+        <v>23750.000000037599</v>
       </c>
       <c r="C2">
-        <v>329659.35000022588</v>
+        <v>329659.350000226</v>
       </c>
       <c r="D2">
-        <v>80404.999999993175</v>
+        <v>80404.999999993204</v>
       </c>
       <c r="E2">
-        <v>433814.35000025667</v>
+        <v>433814.35000025679</v>
       </c>
       <c r="F2">
         <v>8999999.9999775533</v>
@@ -756,24 +754,24 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9088992.5878916681</v>
+        <v>9155077.7528212536</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
       <c r="B3">
-        <v>23750.000000037602</v>
+        <v>23750.000000037599</v>
       </c>
       <c r="C3">
-        <v>462269.56950012047</v>
+        <v>462269.56950012053</v>
       </c>
       <c r="D3">
-        <v>80404.999999993175</v>
+        <v>80404.999999993204</v>
       </c>
       <c r="E3">
         <v>566424.56950015132</v>
@@ -802,9 +800,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -830,18 +828,18 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
       <c r="B2">
-        <v>23750.000000037602</v>
+        <v>23750.000000037599</v>
       </c>
       <c r="C2">
-        <v>472159.35000012722</v>
+        <v>472159.35000012728</v>
       </c>
       <c r="D2">
-        <v>80404.999999993175</v>
+        <v>80404.999999993204</v>
       </c>
       <c r="E2">
         <v>576314.35000015807</v>
@@ -853,27 +851,27 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9139663.1978916675</v>
+        <v>9203414.6728212535</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
       <c r="B3">
-        <v>23750.000000037602</v>
+        <v>23750.000000037599</v>
       </c>
       <c r="C3">
-        <v>457994.56950012338</v>
+        <v>457994.5695001235</v>
       </c>
       <c r="D3">
-        <v>80404.999999993175</v>
+        <v>80404.999999993204</v>
       </c>
       <c r="E3">
-        <v>562149.56950015423</v>
+        <v>562149.56950015435</v>
       </c>
       <c r="F3">
         <v>8999999.9999775533</v>
@@ -899,9 +897,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -927,21 +925,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
       <c r="B2">
-        <v>23750.000000037602</v>
+        <v>23750.000000037599</v>
       </c>
       <c r="C2">
-        <v>232659.35000003097</v>
+        <v>232659.35000003106</v>
       </c>
       <c r="D2">
-        <v>80404.999999993175</v>
+        <v>80404.999999993204</v>
       </c>
       <c r="E2">
-        <v>336814.35000006174</v>
+        <v>336814.35000006185</v>
       </c>
       <c r="F2">
         <v>8999999.9999775533</v>
@@ -950,36 +948,36 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9139420.5478916671</v>
+        <v>9194343.6628212519</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
       <c r="B3">
-        <v>23750.000000037602</v>
+        <v>23750.000000037599</v>
       </c>
       <c r="C3">
-        <v>368179.5694999313</v>
+        <v>368179.56949993141</v>
       </c>
       <c r="D3">
-        <v>80404.999999993175</v>
+        <v>80404.999999993204</v>
       </c>
       <c r="E3">
-        <v>472334.56949996215</v>
+        <v>472334.56949996221</v>
       </c>
       <c r="F3">
-        <v>8894425.0164282173</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>9026072.4564282149</v>
+        <v>9131647.4399775527</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -996,9 +994,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1024,21 +1022,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
       <c r="B2">
-        <v>23750.000000037602</v>
+        <v>23750.000000037599</v>
       </c>
       <c r="C2">
-        <v>232659.35000003097</v>
+        <v>232659.35000003106</v>
       </c>
       <c r="D2">
-        <v>80404.999999993175</v>
+        <v>80404.999999993204</v>
       </c>
       <c r="E2">
-        <v>336814.35000006174</v>
+        <v>336814.35000006185</v>
       </c>
       <c r="F2">
         <v>8999999.9999775533</v>
@@ -1047,27 +1045,27 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9109125.4278916679</v>
+        <v>9160197.5628212541</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
       <c r="B3">
-        <v>23750.000000037602</v>
+        <v>23750.000000037599</v>
       </c>
       <c r="C3">
-        <v>128679.56949983508</v>
+        <v>128679.56949983518</v>
       </c>
       <c r="D3">
-        <v>80404.999999993175</v>
+        <v>80404.999999993204</v>
       </c>
       <c r="E3">
-        <v>232834.56949986584</v>
+        <v>232834.56949986599</v>
       </c>
       <c r="F3">
         <v>8229999.9999991106</v>
@@ -1093,9 +1091,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1121,18 +1119,18 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
       <c r="B2">
-        <v>23750.000000037602</v>
+        <v>23750.000000037599</v>
       </c>
       <c r="C2">
-        <v>472159.35000012722</v>
+        <v>472159.35000012728</v>
       </c>
       <c r="D2">
-        <v>80404.999999993175</v>
+        <v>80404.999999993204</v>
       </c>
       <c r="E2">
         <v>576314.35000015807</v>
@@ -1144,36 +1142,36 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9165171.3478916679</v>
+        <v>9222059.4728212543</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
       <c r="B3">
-        <v>23750.000000037602</v>
+        <v>23750.000000037599</v>
       </c>
       <c r="C3">
-        <v>360994.56949992839</v>
+        <v>360994.5694999285</v>
       </c>
       <c r="D3">
-        <v>80404.999999993175</v>
+        <v>80404.999999993204</v>
       </c>
       <c r="E3">
-        <v>465149.5694999593</v>
+        <v>465149.56949995935</v>
       </c>
       <c r="F3">
-        <v>8750733.5924881212</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>8856211.2724881209</v>
+        <v>9105477.679977553</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -1190,9 +1188,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1218,21 +1216,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
       <c r="B2">
-        <v>23750.000000037602</v>
+        <v>23750.000000037599</v>
       </c>
       <c r="C2">
-        <v>614659.3500000285</v>
+        <v>614659.35000002873</v>
       </c>
       <c r="D2">
-        <v>80404.999999993175</v>
+        <v>80404.999999993204</v>
       </c>
       <c r="E2">
-        <v>718814.35000005935</v>
+        <v>718814.35000005946</v>
       </c>
       <c r="F2">
         <v>8999999.9999775533</v>
@@ -1241,36 +1239,36 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9152799.5578916669</v>
+        <v>9201667.8928212523</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
       <c r="B3">
-        <v>23750.000000037602</v>
+        <v>23750.000000037599</v>
       </c>
       <c r="C3">
-        <v>738719.56949992897</v>
+        <v>738719.56949992909</v>
       </c>
       <c r="D3">
-        <v>80404.999999993175</v>
+        <v>80404.999999993204</v>
       </c>
       <c r="E3">
-        <v>842874.5694999597</v>
+        <v>842874.56949995994</v>
       </c>
       <c r="F3">
-        <v>8999999.9999775533</v>
+        <v>8783525.4984285031</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>9140628.0299775563</v>
+        <v>8924153.5284285061</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -1287,9 +1285,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1315,21 +1313,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
       <c r="B2">
-        <v>23750.000000037602</v>
+        <v>23750.000000037599</v>
       </c>
       <c r="C2">
-        <v>614659.3500000285</v>
+        <v>614659.35000002873</v>
       </c>
       <c r="D2">
-        <v>80404.999999993175</v>
+        <v>80404.999999993204</v>
       </c>
       <c r="E2">
-        <v>718814.35000005935</v>
+        <v>718814.35000005946</v>
       </c>
       <c r="F2">
         <v>8999999.9999775533</v>
@@ -1338,27 +1336,27 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9037939.7378916685</v>
+        <v>9108569.3928212523</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
       <c r="B3">
-        <v>23750.000000037602</v>
+        <v>23750.000000037599</v>
       </c>
       <c r="C3">
-        <v>897870.39550305484</v>
+        <v>897870.39550305519</v>
       </c>
       <c r="D3">
-        <v>80404.999999993175</v>
+        <v>80404.999999993204</v>
       </c>
       <c r="E3">
-        <v>1002025.3955030856</v>
+        <v>1002025.3955030859</v>
       </c>
       <c r="F3">
         <v>8999999.9999775533</v>
@@ -1384,9 +1382,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1412,21 +1410,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
       <c r="B2">
-        <v>23750.000000037602</v>
+        <v>23750.000000037599</v>
       </c>
       <c r="C2">
-        <v>614659.3500000285</v>
+        <v>614659.35000002873</v>
       </c>
       <c r="D2">
-        <v>80404.999999993175</v>
+        <v>80404.999999993204</v>
       </c>
       <c r="E2">
-        <v>718814.35000005935</v>
+        <v>718814.35000005946</v>
       </c>
       <c r="F2">
         <v>8999999.9999775533</v>
@@ -1435,27 +1433,27 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9082685.6578916665</v>
+        <v>9144260.822821252</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
       <c r="B3">
-        <v>23750.000000037602</v>
+        <v>23750.000000037599</v>
       </c>
       <c r="C3">
-        <v>881219.56949983025</v>
+        <v>881219.56949983037</v>
       </c>
       <c r="D3">
-        <v>80404.999999993175</v>
+        <v>80404.999999993204</v>
       </c>
       <c r="E3">
-        <v>985374.56949986098</v>
+        <v>985374.5694998611</v>
       </c>
       <c r="F3">
         <v>8999999.9999775533</v>
@@ -1481,9 +1479,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1509,21 +1507,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
       <c r="B2">
-        <v>23750.000000037602</v>
+        <v>23750.000000037599</v>
       </c>
       <c r="C2">
-        <v>38659.350000427432</v>
+        <v>38659.350000427519</v>
       </c>
       <c r="D2">
-        <v>80404.999999993175</v>
+        <v>80404.999999993204</v>
       </c>
       <c r="E2">
-        <v>142814.35000045819</v>
+        <v>142814.3500004583</v>
       </c>
       <c r="F2">
         <v>8999999.9999775533</v>
@@ -1532,27 +1530,27 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9124996.5949162971</v>
+        <v>9183520.734557284</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
       <c r="B3">
-        <v>23750.000000037602</v>
+        <v>9.0604259869818987E-12</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
-        <v>80404.999999993175</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>104155.00000003078</v>
+        <v>9.0604259869818987E-12</v>
       </c>
       <c r="F3">
         <v>8999999.9999775533</v>
@@ -1578,9 +1576,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1606,21 +1604,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
       <c r="B2">
-        <v>23750.000000037602</v>
+        <v>23750.000000037599</v>
       </c>
       <c r="C2">
-        <v>614659.3500000285</v>
+        <v>614659.35000002873</v>
       </c>
       <c r="D2">
-        <v>80404.999999993175</v>
+        <v>80404.999999993204</v>
       </c>
       <c r="E2">
-        <v>718814.35000005935</v>
+        <v>718814.35000005946</v>
       </c>
       <c r="F2">
         <v>8999999.9999775533</v>
@@ -1629,27 +1627,27 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9126074.1838916689</v>
+        <v>9170916.1488212533</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
       <c r="B3">
-        <v>23750.000000037602</v>
+        <v>23750.000000037599</v>
       </c>
       <c r="C3">
-        <v>881219.56949983025</v>
+        <v>881219.56949983037</v>
       </c>
       <c r="D3">
-        <v>80404.999999993175</v>
+        <v>80404.999999993204</v>
       </c>
       <c r="E3">
-        <v>985374.56949986098</v>
+        <v>985374.5694998611</v>
       </c>
       <c r="F3">
         <v>8999999.9999775533</v>
@@ -1675,9 +1673,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1703,21 +1701,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
       <c r="B2">
-        <v>23750.000000037602</v>
+        <v>23750.000000037599</v>
       </c>
       <c r="C2">
-        <v>614659.3500000285</v>
+        <v>614659.35000002873</v>
       </c>
       <c r="D2">
-        <v>80404.999999993175</v>
+        <v>80404.999999993204</v>
       </c>
       <c r="E2">
-        <v>718814.35000005935</v>
+        <v>718814.35000005946</v>
       </c>
       <c r="F2">
         <v>8999999.9999775533</v>
@@ -1726,27 +1724,27 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9170814.4678916689</v>
+        <v>9224772.7548212539</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
       <c r="B3">
-        <v>23750.000000037602</v>
+        <v>23750.000000037599</v>
       </c>
       <c r="C3">
-        <v>881219.56949983025</v>
+        <v>881219.56949983037</v>
       </c>
       <c r="D3">
-        <v>80404.999999993175</v>
+        <v>80404.999999993204</v>
       </c>
       <c r="E3">
-        <v>985374.56949986098</v>
+        <v>985374.5694998611</v>
       </c>
       <c r="F3">
         <v>8999999.9999775533</v>
@@ -1772,9 +1770,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1800,21 +1798,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
       <c r="B2">
-        <v>23750.000000037602</v>
+        <v>23750.000000037599</v>
       </c>
       <c r="C2">
-        <v>38659.350000427432</v>
+        <v>38659.350000427519</v>
       </c>
       <c r="D2">
-        <v>80404.999999993175</v>
+        <v>80404.999999993204</v>
       </c>
       <c r="E2">
-        <v>142814.35000045819</v>
+        <v>142814.3500004583</v>
       </c>
       <c r="F2">
         <v>8999999.9999775533</v>
@@ -1823,27 +1821,27 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9102833.229891669</v>
+        <v>9163943.7288212553</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
       <c r="B3">
-        <v>23750.000000037602</v>
+        <v>23750.000000037599</v>
       </c>
       <c r="C3">
-        <v>322499.56950021721</v>
+        <v>322499.56950021733</v>
       </c>
       <c r="D3">
-        <v>80404.999999993175</v>
+        <v>80404.999999993204</v>
       </c>
       <c r="E3">
-        <v>426654.56950024801</v>
+        <v>426654.56950024812</v>
       </c>
       <c r="F3">
         <v>8999999.9999775533</v>
@@ -1869,9 +1867,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1897,18 +1895,18 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
       <c r="B2">
-        <v>23750.000000037602</v>
+        <v>23750.000000037599</v>
       </c>
       <c r="C2">
-        <v>472159.35000012722</v>
+        <v>472159.35000012728</v>
       </c>
       <c r="D2">
-        <v>80404.999999993175</v>
+        <v>80404.999999993204</v>
       </c>
       <c r="E2">
         <v>576314.35000015807</v>
@@ -1920,27 +1918,27 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9166755.0538916681</v>
+        <v>9193988.4128212538</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
       <c r="B3">
-        <v>23750.000000037602</v>
+        <v>23750.000000037599</v>
       </c>
       <c r="C3">
-        <v>166994.5695003249</v>
+        <v>166994.56950032499</v>
       </c>
       <c r="D3">
-        <v>80404.999999993175</v>
+        <v>80404.999999993204</v>
       </c>
       <c r="E3">
-        <v>271149.56950035563</v>
+        <v>271149.56950035581</v>
       </c>
       <c r="F3">
         <v>8999999.9999775533</v>
@@ -1966,9 +1964,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1994,21 +1992,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
       <c r="B2">
-        <v>23750.000000037602</v>
+        <v>23750.000000037599</v>
       </c>
       <c r="C2">
-        <v>38659.350000427432</v>
+        <v>38659.350000427519</v>
       </c>
       <c r="D2">
-        <v>80404.999999993175</v>
+        <v>80404.999999993204</v>
       </c>
       <c r="E2">
-        <v>142814.35000045819</v>
+        <v>142814.3500004583</v>
       </c>
       <c r="F2">
         <v>8999999.9999775533</v>
@@ -2017,27 +2015,27 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9172360.887891667</v>
+        <v>9211313.3728212528</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
       <c r="B3">
-        <v>23750.000000037602</v>
+        <v>23750.000000037599</v>
       </c>
       <c r="C3">
-        <v>179999.56950031593</v>
+        <v>179999.56950031602</v>
       </c>
       <c r="D3">
-        <v>80404.999999993175</v>
+        <v>80404.999999993204</v>
       </c>
       <c r="E3">
-        <v>284154.56950034673</v>
+        <v>284154.56950034678</v>
       </c>
       <c r="F3">
         <v>8999999.9999775533</v>
@@ -2063,9 +2061,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2091,21 +2089,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
       <c r="B2">
-        <v>23750.000000037602</v>
+        <v>23750.000000037599</v>
       </c>
       <c r="C2">
-        <v>38659.350000427432</v>
+        <v>38659.350000427519</v>
       </c>
       <c r="D2">
-        <v>80404.999999993175</v>
+        <v>80404.999999993204</v>
       </c>
       <c r="E2">
-        <v>142814.35000045819</v>
+        <v>142814.3500004583</v>
       </c>
       <c r="F2">
         <v>8999999.9999775533</v>
@@ -2114,36 +2112,36 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9147119.3278916664</v>
+        <v>9197252.1768212523</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
       <c r="B3">
-        <v>23750.000000037602</v>
+        <v>9.0604259869818987E-12</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
-        <v>80404.999999993175</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>104155.00000003078</v>
+        <v>9.0604259869818987E-12</v>
       </c>
       <c r="F3">
-        <v>8808496.6745460033</v>
+        <v>8731768.8148539718</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>9048415.1625460032</v>
+        <v>8971687.3028539717</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -2160,9 +2158,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2188,21 +2186,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
       <c r="B2">
-        <v>23750.000000037602</v>
+        <v>23750.000000037599</v>
       </c>
       <c r="C2">
-        <v>38659.350000427432</v>
+        <v>38659.350000427519</v>
       </c>
       <c r="D2">
-        <v>80404.999999993175</v>
+        <v>80404.999999993204</v>
       </c>
       <c r="E2">
-        <v>142814.35000045819</v>
+        <v>142814.3500004583</v>
       </c>
       <c r="F2">
         <v>8999999.9999775533</v>
@@ -2211,27 +2209,27 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9125611.1918916684</v>
+        <v>9189896.8428212535</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
       <c r="B3">
-        <v>23750.000000037602</v>
+        <v>9.0604259869818987E-12</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
-        <v>80404.999999993175</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>104155.00000003078</v>
+        <v>9.0604259869818987E-12</v>
       </c>
       <c r="F3">
         <v>8999999.9999775533</v>
@@ -2257,9 +2255,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2285,21 +2283,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
       <c r="B2">
-        <v>23750.000000037602</v>
+        <v>23750.000000037599</v>
       </c>
       <c r="C2">
-        <v>232659.35000003097</v>
+        <v>232659.35000003106</v>
       </c>
       <c r="D2">
-        <v>80404.999999993175</v>
+        <v>80404.999999993204</v>
       </c>
       <c r="E2">
-        <v>336814.35000006174</v>
+        <v>336814.35000006185</v>
       </c>
       <c r="F2">
         <v>8999999.9999775533</v>
@@ -2308,36 +2306,36 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9121233.3098916672</v>
+        <v>9176745.7848212533</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
       <c r="B3">
-        <v>23750.000000037602</v>
+        <v>23750.000000037599</v>
       </c>
       <c r="C3">
-        <v>242330.39550325469</v>
+        <v>242330.39550325499</v>
       </c>
       <c r="D3">
-        <v>80404.999999993175</v>
+        <v>80404.999999993204</v>
       </c>
       <c r="E3">
-        <v>346485.39550328546</v>
+        <v>346485.39550328581</v>
       </c>
       <c r="F3">
-        <v>7479999.9999999981</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="G3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H3">
-        <v>7615993.4519999977</v>
+        <v>8365993.451999112</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -2354,9 +2352,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2382,21 +2380,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
       <c r="B2">
-        <v>23750.000000037602</v>
+        <v>23750.000000037599</v>
       </c>
       <c r="C2">
-        <v>38659.350000427432</v>
+        <v>38659.350000427519</v>
       </c>
       <c r="D2">
-        <v>80404.999999993175</v>
+        <v>80404.999999993204</v>
       </c>
       <c r="E2">
-        <v>142814.35000045819</v>
+        <v>142814.3500004583</v>
       </c>
       <c r="F2">
         <v>8999999.9999775533</v>
@@ -2405,36 +2403,36 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9138276.2378916703</v>
+        <v>9180840.0548212547</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
       <c r="B3">
-        <v>23750.000000037602</v>
+        <v>23750.000000037599</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
-        <v>80404.999999993175</v>
+        <v>19064.350000219743</v>
       </c>
       <c r="E3">
-        <v>104155.00000003078</v>
+        <v>42814.350000257342</v>
       </c>
       <c r="F3">
-        <v>8439635.6687704138</v>
+        <v>8550308.046185514</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>8590164.6947704144</v>
+        <v>8700837.0721855126</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -2451,9 +2449,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2479,21 +2477,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
       <c r="B2">
-        <v>23750.000000037602</v>
+        <v>23750.000000037599</v>
       </c>
       <c r="C2">
-        <v>232659.35000003097</v>
+        <v>232659.35000003106</v>
       </c>
       <c r="D2">
-        <v>80404.999999993175</v>
+        <v>80404.999999993204</v>
       </c>
       <c r="E2">
-        <v>336814.35000006174</v>
+        <v>336814.35000006185</v>
       </c>
       <c r="F2">
         <v>8999999.9999775533</v>
@@ -2502,36 +2500,36 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9159893.4438916687</v>
+        <v>9207686.2468212526</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
       <c r="B3">
-        <v>23750.000000037602</v>
+        <v>23750.000000037599</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
-        <v>80404.999999993175</v>
+        <v>13064.350000232018</v>
       </c>
       <c r="E3">
-        <v>104155.00000003078</v>
+        <v>36814.350000269616</v>
       </c>
       <c r="F3">
-        <v>8411349.4661967624</v>
+        <v>8878278.8726280574</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>8599499.2981967628</v>
+        <v>9066428.7046280578</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -2548,9 +2546,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2576,21 +2574,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
       <c r="B2">
-        <v>23750.000000037602</v>
+        <v>23750.000000037599</v>
       </c>
       <c r="C2">
-        <v>232659.35000003097</v>
+        <v>232659.35000003106</v>
       </c>
       <c r="D2">
-        <v>80404.999999993175</v>
+        <v>80404.999999993204</v>
       </c>
       <c r="E2">
-        <v>336814.35000006174</v>
+        <v>336814.35000006185</v>
       </c>
       <c r="F2">
         <v>8999999.9999775533</v>
@@ -2599,27 +2597,27 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9094917.4078916684</v>
+        <v>9164759.1828212533</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
       <c r="B3">
-        <v>23750.000000037602</v>
+        <v>23750.000000037599</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
-        <v>80404.999999993175</v>
+        <v>13064.350000232018</v>
       </c>
       <c r="E3">
-        <v>104155.00000003078</v>
+        <v>36814.350000269616</v>
       </c>
       <c r="F3">
         <v>8999999.9999775533</v>
@@ -2645,9 +2643,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2673,21 +2671,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
       <c r="B2">
-        <v>23750.000000037602</v>
+        <v>23750.000000037599</v>
       </c>
       <c r="C2">
-        <v>614659.3500000285</v>
+        <v>614659.35000002873</v>
       </c>
       <c r="D2">
-        <v>80404.999999993175</v>
+        <v>80404.999999993204</v>
       </c>
       <c r="E2">
-        <v>718814.35000005935</v>
+        <v>718814.35000005946</v>
       </c>
       <c r="F2">
         <v>8999999.9999775533</v>
@@ -2696,27 +2694,27 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9091688.6958916672</v>
+        <v>9136761.0628212541</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
       <c r="B3">
-        <v>23750.000000037602</v>
+        <v>23750.000000037599</v>
       </c>
       <c r="C3">
-        <v>499219.56949983269</v>
+        <v>499219.56949983287</v>
       </c>
       <c r="D3">
-        <v>80404.999999993175</v>
+        <v>80404.999999993204</v>
       </c>
       <c r="E3">
-        <v>603374.56949986354</v>
+        <v>603374.56949986366</v>
       </c>
       <c r="F3">
         <v>8999999.9999775533</v>
@@ -2742,9 +2740,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2770,21 +2768,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
       <c r="B2">
-        <v>23750.000000037602</v>
+        <v>23750.000000037599</v>
       </c>
       <c r="C2">
-        <v>232659.35000003097</v>
+        <v>232659.35000003106</v>
       </c>
       <c r="D2">
-        <v>80404.999999993175</v>
+        <v>80404.999999993204</v>
       </c>
       <c r="E2">
-        <v>336814.35000006174</v>
+        <v>336814.35000006185</v>
       </c>
       <c r="F2">
         <v>8999999.9999775533</v>
@@ -2793,24 +2791,24 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9127506.0498916674</v>
+        <v>9167370.2568212524</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
       <c r="B3">
-        <v>23750.000000037602</v>
+        <v>23750.000000037599</v>
       </c>
       <c r="C3">
         <v>510679.56949983269</v>
       </c>
       <c r="D3">
-        <v>80404.999999993175</v>
+        <v>80404.999999993204</v>
       </c>
       <c r="E3">
         <v>614834.56949986354</v>
@@ -2839,9 +2837,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2867,21 +2865,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
       <c r="B2">
-        <v>23750.000000037602</v>
+        <v>23750.000000037599</v>
       </c>
       <c r="C2">
-        <v>614659.3500000285</v>
+        <v>614659.35000002873</v>
       </c>
       <c r="D2">
-        <v>80404.999999993175</v>
+        <v>80404.999999993204</v>
       </c>
       <c r="E2">
-        <v>718814.35000005935</v>
+        <v>718814.35000005946</v>
       </c>
       <c r="F2">
         <v>8999999.9999775533</v>
@@ -2890,27 +2888,27 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9207654.1418916676</v>
+        <v>9251220.6648212522</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
       <c r="B3">
-        <v>23750.000000037602</v>
+        <v>23750.000000037599</v>
       </c>
       <c r="C3">
-        <v>499219.56949983269</v>
+        <v>499219.56949983287</v>
       </c>
       <c r="D3">
-        <v>80404.999999993175</v>
+        <v>80404.999999993204</v>
       </c>
       <c r="E3">
-        <v>603374.56949986354</v>
+        <v>603374.56949986366</v>
       </c>
       <c r="F3">
         <v>8999999.9999775533</v>
@@ -2936,9 +2934,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2964,21 +2962,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
       <c r="B2">
-        <v>23750.000000037602</v>
+        <v>23750.000000037599</v>
       </c>
       <c r="C2">
-        <v>614659.3500000285</v>
+        <v>614659.35000002873</v>
       </c>
       <c r="D2">
-        <v>80404.999999993175</v>
+        <v>80404.999999993204</v>
       </c>
       <c r="E2">
-        <v>718814.35000005935</v>
+        <v>718814.35000005946</v>
       </c>
       <c r="F2">
         <v>8999999.9999775533</v>
@@ -2987,36 +2985,36 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9197459.7058916688</v>
+        <v>9241641.0068212524</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
       <c r="B3">
-        <v>23750.000000037602</v>
+        <v>23750.000000037599</v>
       </c>
       <c r="C3">
-        <v>881219.56949983025</v>
+        <v>881219.56949983037</v>
       </c>
       <c r="D3">
-        <v>80404.999999993175</v>
+        <v>80404.999999993204</v>
       </c>
       <c r="E3">
-        <v>985374.56949986098</v>
+        <v>985374.5694998611</v>
       </c>
       <c r="F3">
-        <v>10606394.893707667</v>
+        <v>10689185.909036435</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>10891704.701707669</v>
+        <v>10974495.717036434</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -3033,9 +3031,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -3061,21 +3059,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
       <c r="B2">
-        <v>23750.000000037602</v>
+        <v>23750.000000037599</v>
       </c>
       <c r="C2">
-        <v>614659.3500000285</v>
+        <v>614659.35000002873</v>
       </c>
       <c r="D2">
-        <v>80404.999999993175</v>
+        <v>80404.999999993204</v>
       </c>
       <c r="E2">
-        <v>718814.35000005935</v>
+        <v>718814.35000005946</v>
       </c>
       <c r="F2">
         <v>8999999.9999775533</v>
@@ -3084,27 +3082,27 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9145365.4038916677</v>
+        <v>9199065.4748212527</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
       <c r="B3">
-        <v>23750.000000037602</v>
+        <v>23750.000000037599</v>
       </c>
       <c r="C3">
-        <v>881219.56949983025</v>
+        <v>881219.56949983037</v>
       </c>
       <c r="D3">
-        <v>80404.999999993175</v>
+        <v>80404.999999993204</v>
       </c>
       <c r="E3">
-        <v>985374.56949986098</v>
+        <v>985374.5694998611</v>
       </c>
       <c r="F3">
         <v>8999999.9999775533</v>
@@ -3130,9 +3128,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -3158,21 +3156,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
       <c r="B2">
-        <v>23750.000000037602</v>
+        <v>23750.000000037599</v>
       </c>
       <c r="C2">
-        <v>232659.35000003097</v>
+        <v>232659.35000003106</v>
       </c>
       <c r="D2">
-        <v>80404.999999993175</v>
+        <v>80404.999999993204</v>
       </c>
       <c r="E2">
-        <v>336814.35000006174</v>
+        <v>336814.35000006185</v>
       </c>
       <c r="F2">
         <v>8999999.9999775533</v>
@@ -3181,24 +3179,24 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9112330.2318916675</v>
+        <v>9173727.3788212538</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
       <c r="B3">
-        <v>23750.000000037602</v>
+        <v>23750.000000037599</v>
       </c>
       <c r="C3">
         <v>510679.56949983269</v>
       </c>
       <c r="D3">
-        <v>80404.999999993175</v>
+        <v>80404.999999993204</v>
       </c>
       <c r="E3">
         <v>614834.56949986354</v>
@@ -3227,9 +3225,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -3255,21 +3253,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
       <c r="B2">
-        <v>23750.000000037602</v>
+        <v>23750.000000037599</v>
       </c>
       <c r="C2">
-        <v>329659.35000022588</v>
+        <v>329659.350000226</v>
       </c>
       <c r="D2">
-        <v>80404.999999993175</v>
+        <v>80404.999999993204</v>
       </c>
       <c r="E2">
-        <v>433814.35000025667</v>
+        <v>433814.35000025679</v>
       </c>
       <c r="F2">
         <v>8999999.9999775533</v>
@@ -3278,27 +3276,27 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9122792.637891667</v>
+        <v>9183108.4428212531</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
       <c r="B3">
-        <v>23750.000000037602</v>
+        <v>23750.000000037599</v>
       </c>
       <c r="C3">
-        <v>319769.56950021914</v>
+        <v>319769.56950021919</v>
       </c>
       <c r="D3">
-        <v>80404.999999993175</v>
+        <v>80404.999999993204</v>
       </c>
       <c r="E3">
-        <v>423924.56950024987</v>
+        <v>423924.56950025004</v>
       </c>
       <c r="F3">
         <v>8999999.9999775533</v>
@@ -3319,206 +3317,12 @@
 </file>
 
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
-        <v>43101</v>
-      </c>
-      <c r="B2">
-        <v>23750.000000037602</v>
-      </c>
-      <c r="C2">
-        <v>329659.35000022588</v>
-      </c>
-      <c r="D2">
-        <v>80404.999999993175</v>
-      </c>
-      <c r="E2">
-        <v>433814.35000025667</v>
-      </c>
-      <c r="F2">
-        <v>8999999.9999775533</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>9107071.637891667</v>
-      </c>
-      <c r="I2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
-        <v>43466</v>
-      </c>
-      <c r="B3">
-        <v>23750.000000037602</v>
-      </c>
-      <c r="C3">
-        <v>319769.56950021914</v>
-      </c>
-      <c r="D3">
-        <v>80404.999999993175</v>
-      </c>
-      <c r="E3">
-        <v>423924.56950024987</v>
-      </c>
-      <c r="F3">
-        <v>8999999.9999775533</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3">
-        <v>9108851.9999775533</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
-        <v>43101</v>
-      </c>
-      <c r="B2">
-        <v>23750.000000037602</v>
-      </c>
-      <c r="C2">
-        <v>329659.35000022588</v>
-      </c>
-      <c r="D2">
-        <v>80404.999999993175</v>
-      </c>
-      <c r="E2">
-        <v>433814.35000025667</v>
-      </c>
-      <c r="F2">
-        <v>8999999.9999775533</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>9098550.637891667</v>
-      </c>
-      <c r="I2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
-        <v>43466</v>
-      </c>
-      <c r="B3">
-        <v>23750.000000037602</v>
-      </c>
-      <c r="C3">
-        <v>319769.56950021914</v>
-      </c>
-      <c r="D3">
-        <v>80404.999999993175</v>
-      </c>
-      <c r="E3">
-        <v>423924.56950024987</v>
-      </c>
-      <c r="F3">
-        <v>8605299.1975634433</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3">
-        <v>8703095.1975634433</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3530,9 +3334,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -3558,21 +3362,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
       <c r="B2">
-        <v>23750.000000037602</v>
+        <v>23750.000000037599</v>
       </c>
       <c r="C2">
-        <v>329659.35000022588</v>
+        <v>329659.350000226</v>
       </c>
       <c r="D2">
-        <v>80404.999999993175</v>
+        <v>80404.999999993204</v>
       </c>
       <c r="E2">
-        <v>433814.35000025667</v>
+        <v>433814.35000025679</v>
       </c>
       <c r="F2">
         <v>8999999.9999775533</v>
@@ -3581,27 +3385,27 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9080791.0978916697</v>
+        <v>9143773.3228212539</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
       <c r="B3">
-        <v>23750.000000037602</v>
+        <v>23750.000000037599</v>
       </c>
       <c r="C3">
-        <v>222769.56950002417</v>
+        <v>222769.56950002426</v>
       </c>
       <c r="D3">
-        <v>80404.999999993175</v>
+        <v>80404.999999993204</v>
       </c>
       <c r="E3">
-        <v>326924.56950005493</v>
+        <v>326924.56950005511</v>
       </c>
       <c r="F3">
         <v>8229999.9999991106</v>
@@ -3627,9 +3431,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -3655,21 +3459,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
       <c r="B2">
-        <v>23750.000000037602</v>
+        <v>23750.000000037599</v>
       </c>
       <c r="C2">
-        <v>614659.3500000285</v>
+        <v>614659.35000002873</v>
       </c>
       <c r="D2">
-        <v>80404.999999993175</v>
+        <v>80404.999999993204</v>
       </c>
       <c r="E2">
-        <v>718814.35000005935</v>
+        <v>718814.35000005946</v>
       </c>
       <c r="F2">
         <v>8999999.9999775533</v>
@@ -3678,36 +3482,36 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9185247.4178916682</v>
+        <v>9231126.6228212528</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
       <c r="B3">
-        <v>23750.000000037602</v>
+        <v>23750.000000037599</v>
       </c>
       <c r="C3">
-        <v>596219.56950002769</v>
+        <v>596219.56950002781</v>
       </c>
       <c r="D3">
-        <v>80404.999999993175</v>
+        <v>80404.999999993204</v>
       </c>
       <c r="E3">
-        <v>700374.56950005842</v>
+        <v>700374.56950005866</v>
       </c>
       <c r="F3">
-        <v>8999999.9999775533</v>
+        <v>8297238.1509485096</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>9061216.4199775551</v>
+        <v>8358454.5709485114</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -3724,9 +3528,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -3752,21 +3556,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
       <c r="B2">
-        <v>23750.000000037602</v>
+        <v>23750.000000037599</v>
       </c>
       <c r="C2">
-        <v>329659.35000022588</v>
+        <v>329659.350000226</v>
       </c>
       <c r="D2">
-        <v>80404.999999993175</v>
+        <v>80404.999999993204</v>
       </c>
       <c r="E2">
-        <v>433814.35000025667</v>
+        <v>433814.35000025679</v>
       </c>
       <c r="F2">
         <v>8999999.9999775533</v>
@@ -3775,36 +3579,36 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9141636.637891667</v>
+        <v>9197527.4428212531</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
       <c r="B3">
-        <v>23750.000000037602</v>
+        <v>23750.000000037599</v>
       </c>
       <c r="C3">
-        <v>604769.56950002175</v>
+        <v>604769.56950002187</v>
       </c>
       <c r="D3">
-        <v>80404.999999993175</v>
+        <v>80404.999999993204</v>
       </c>
       <c r="E3">
-        <v>708924.5695000526</v>
+        <v>708924.56950005272</v>
       </c>
       <c r="F3">
-        <v>11480671.832095766</v>
+        <v>10891795.124617375</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>11693366.842095764</v>
+        <v>11104490.134617373</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -3821,9 +3625,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -3849,21 +3653,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
       <c r="B2">
-        <v>23750.000000037602</v>
+        <v>23750.000000037599</v>
       </c>
       <c r="C2">
-        <v>232659.35000003097</v>
+        <v>232659.35000003106</v>
       </c>
       <c r="D2">
-        <v>80404.999999993175</v>
+        <v>80404.999999993204</v>
       </c>
       <c r="E2">
-        <v>336814.35000006174</v>
+        <v>336814.35000006185</v>
       </c>
       <c r="F2">
         <v>8999999.9999775533</v>
@@ -3872,27 +3676,27 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9137792.6078916676</v>
+        <v>9198730.9428212531</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
       <c r="B3">
-        <v>23750.000000037602</v>
+        <v>23750.000000037599</v>
       </c>
       <c r="C3">
-        <v>225679.56950003002</v>
+        <v>225679.56950003011</v>
       </c>
       <c r="D3">
-        <v>80404.999999993175</v>
+        <v>80404.999999993204</v>
       </c>
       <c r="E3">
-        <v>329834.56950006081</v>
+        <v>329834.56950006087</v>
       </c>
       <c r="F3">
         <v>8999999.9999775533</v>
@@ -3918,9 +3722,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -3946,21 +3750,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
       <c r="B2">
-        <v>23750.000000037602</v>
+        <v>23750.000000037599</v>
       </c>
       <c r="C2">
-        <v>38659.350000427432</v>
+        <v>38659.350000427519</v>
       </c>
       <c r="D2">
-        <v>80404.999999993175</v>
+        <v>80404.999999993204</v>
       </c>
       <c r="E2">
-        <v>142814.35000045819</v>
+        <v>142814.3500004583</v>
       </c>
       <c r="F2">
         <v>8999999.9999775533</v>
@@ -3969,27 +3773,27 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9162616.4278916679</v>
+        <v>9218013.362821253</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
       <c r="B3">
-        <v>23750.000000037602</v>
+        <v>23750.000000037599</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
-        <v>80404.999999993175</v>
+        <v>19064.350000219743</v>
       </c>
       <c r="E3">
-        <v>104155.00000003078</v>
+        <v>42814.350000257342</v>
       </c>
       <c r="F3">
         <v>8999999.9999775533</v>
@@ -4015,9 +3819,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -4043,21 +3847,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
       <c r="B2">
-        <v>23750.000000037602</v>
+        <v>23750.000000037599</v>
       </c>
       <c r="C2">
-        <v>232659.35000003097</v>
+        <v>232659.35000003106</v>
       </c>
       <c r="D2">
-        <v>80404.999999993175</v>
+        <v>80404.999999993204</v>
       </c>
       <c r="E2">
-        <v>336814.35000006174</v>
+        <v>336814.35000006185</v>
       </c>
       <c r="F2">
         <v>8999999.9999775533</v>
@@ -4066,27 +3870,27 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9113851.8378916681</v>
+        <v>9178179.6028212532</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
       <c r="B3">
-        <v>23750.000000037602</v>
+        <v>23750.000000037599</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
-        <v>80404.999999993175</v>
+        <v>13064.350000232018</v>
       </c>
       <c r="E3">
-        <v>104155.00000003078</v>
+        <v>36814.350000269616</v>
       </c>
       <c r="F3">
         <v>8999999.9999775533</v>

</xml_diff>

<commit_message>
June 2018 MTOM Unofficial Model Run. Includes updated CBRFC forecasts, model name, ruleset name and model output files. No model or ruleset changes.
</commit_message>
<xml_diff>
--- a/Output Data/MtomToCrss_Annual.xlsx
+++ b/Output Data/MtomToCrss_Annual.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\COM460\RiverWare Models\Monthly Models\MTOM_Production\_MAY18\Output Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\MTOM\dev\Output Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="9900"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12570" windowHeight="13590"/>
   </bookViews>
   <sheets>
     <sheet name="Trace38" sheetId="37" r:id="rId1"/>
@@ -463,7 +463,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9185872.9543969855</v>
+        <v>9233414.3667382021</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
@@ -477,22 +477,22 @@
         <v>23750.000000037599</v>
       </c>
       <c r="C3">
-        <v>54150.395503639542</v>
+        <v>54150.395504590306</v>
       </c>
       <c r="D3">
         <v>80404.999999993204</v>
       </c>
       <c r="E3">
-        <v>158305.39550367033</v>
+        <v>158305.39550462109</v>
       </c>
       <c r="F3">
-        <v>8999999.9999775533</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>9110979.6591972616</v>
+        <v>8340979.6592188207</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -560,7 +560,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9252939.612821253</v>
+        <v>9295861.1006182134</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
@@ -657,7 +657,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9197781.1928212512</v>
+        <v>9250550.2506182138</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
@@ -754,7 +754,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9155077.7528212536</v>
+        <v>9206430.700618213</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
@@ -851,7 +851,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9203414.6728212535</v>
+        <v>9250667.0606182124</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
@@ -948,7 +948,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9194343.6628212519</v>
+        <v>9236389.5306182131</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
@@ -1045,7 +1045,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9160197.5628212541</v>
+        <v>9206042.7306182124</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
@@ -1142,7 +1142,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9222059.4728212543</v>
+        <v>9255659.1806182135</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
@@ -1239,7 +1239,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9201667.8928212523</v>
+        <v>9248922.3406182136</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
@@ -1262,13 +1262,13 @@
         <v>842874.56949995994</v>
       </c>
       <c r="F3">
-        <v>8783525.4984285031</v>
+        <v>8684014.6675812695</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>8924153.5284285061</v>
+        <v>8824642.6975812688</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -1336,7 +1336,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9108569.3928212523</v>
+        <v>9170167.1706182137</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
@@ -1350,13 +1350,13 @@
         <v>23750.000000037599</v>
       </c>
       <c r="C3">
-        <v>897870.39550305519</v>
+        <v>897870.39550400607</v>
       </c>
       <c r="D3">
         <v>80404.999999993204</v>
       </c>
       <c r="E3">
-        <v>1002025.3955030859</v>
+        <v>1002025.3955040367</v>
       </c>
       <c r="F3">
         <v>8999999.9999775533</v>
@@ -1433,7 +1433,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9144260.822821252</v>
+        <v>9193136.5506182127</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
@@ -1530,7 +1530,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9183520.734557284</v>
+        <v>9235473.5634292122</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
@@ -1627,7 +1627,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9170916.1488212533</v>
+        <v>9222416.2486182135</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
@@ -1724,7 +1724,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9224772.7548212539</v>
+        <v>9252495.9286182113</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
@@ -1821,7 +1821,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9163943.7288212553</v>
+        <v>9211668.2466182131</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
@@ -1918,7 +1918,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9193988.4128212538</v>
+        <v>9220906.3186182119</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
@@ -1941,13 +1941,13 @@
         <v>271149.56950035581</v>
       </c>
       <c r="F3">
-        <v>8999999.9999775533</v>
+        <v>8989876.7032403443</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>9133190.7539775539</v>
+        <v>9123067.457240345</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -2015,7 +2015,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9211313.3728212528</v>
+        <v>9250696.2646182105</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
@@ -2112,7 +2112,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9197252.1768212523</v>
+        <v>9245005.176618211</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
@@ -2135,13 +2135,13 @@
         <v>9.0604259869818987E-12</v>
       </c>
       <c r="F3">
-        <v>8731768.8148539718</v>
+        <v>8532920.2607673369</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>8971687.3028539717</v>
+        <v>8772838.7487673368</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -2209,7 +2209,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9189896.8428212535</v>
+        <v>9250104.7266182136</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
@@ -2306,7 +2306,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9176745.7848212533</v>
+        <v>9240405.4026182126</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
@@ -2320,13 +2320,13 @@
         <v>23750.000000037599</v>
       </c>
       <c r="C3">
-        <v>242330.39550325499</v>
+        <v>242330.39550420572</v>
       </c>
       <c r="D3">
         <v>80404.999999993204</v>
       </c>
       <c r="E3">
-        <v>346485.39550328581</v>
+        <v>346485.39550423651</v>
       </c>
       <c r="F3">
         <v>8229999.9999991106</v>
@@ -2403,7 +2403,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9180840.0548212547</v>
+        <v>9222523.6566182133</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
@@ -2426,13 +2426,13 @@
         <v>42814.350000257342</v>
       </c>
       <c r="F3">
-        <v>8550308.046185514</v>
+        <v>8592245.0237977803</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>8700837.0721855126</v>
+        <v>8742774.0497977808</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -2500,7 +2500,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9207686.2468212526</v>
+        <v>9254135.5006182119</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
@@ -2523,13 +2523,13 @@
         <v>36814.350000269616</v>
       </c>
       <c r="F3">
-        <v>8878278.8726280574</v>
+        <v>8762028.3531198837</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>9066428.7046280578</v>
+        <v>8950178.1851198822</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -2597,7 +2597,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9164759.1828212533</v>
+        <v>9220465.9106182121</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
@@ -2694,7 +2694,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9136761.0628212541</v>
+        <v>9209879.1566182114</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
@@ -2791,7 +2791,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9167370.2568212524</v>
+        <v>9225251.6906182114</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
@@ -2888,7 +2888,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9251220.6648212522</v>
+        <v>9299916.012618212</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
@@ -2985,7 +2985,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9241641.0068212524</v>
+        <v>9257004.4646182116</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
@@ -3008,13 +3008,13 @@
         <v>985374.5694998611</v>
       </c>
       <c r="F3">
-        <v>10689185.909036435</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>10974495.717036434</v>
+        <v>9285309.8079775535</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -3082,7 +3082,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9199065.4748212527</v>
+        <v>9237555.8146182112</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
@@ -3179,7 +3179,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9173727.3788212538</v>
+        <v>9222508.3326182142</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
@@ -3276,7 +3276,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9183108.4428212531</v>
+        <v>9233958.1006182134</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
@@ -3385,7 +3385,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9143773.3228212539</v>
+        <v>9195730.0006182119</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
@@ -3482,7 +3482,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9231126.6228212528</v>
+        <v>9268541.3806182127</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
@@ -3505,13 +3505,13 @@
         <v>700374.56950005866</v>
       </c>
       <c r="F3">
-        <v>8297238.1509485096</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>8358454.5709485114</v>
+        <v>8291216.4199991124</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -3579,7 +3579,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9197527.4428212531</v>
+        <v>9243925.6506182123</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
@@ -3602,13 +3602,13 @@
         <v>708924.56950005272</v>
       </c>
       <c r="F3">
-        <v>10891795.124617375</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>11104490.134617373</v>
+        <v>9212695.0099775549</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -3676,7 +3676,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9198730.9428212531</v>
+        <v>9251713.6206182111</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
@@ -3690,13 +3690,13 @@
         <v>23750.000000037599</v>
       </c>
       <c r="C3">
-        <v>225679.56950003011</v>
+        <v>232659.35000003106</v>
       </c>
       <c r="D3">
         <v>80404.999999993204</v>
       </c>
       <c r="E3">
-        <v>329834.56950006087</v>
+        <v>336814.35000006185</v>
       </c>
       <c r="F3">
         <v>8999999.9999775533</v>
@@ -3708,7 +3708,7 @@
         <v>9183949.7199775539</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -3773,7 +3773,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9218013.362821253</v>
+        <v>9258068.0306182113</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
@@ -3870,7 +3870,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9178179.6028212532</v>
+        <v>9230093.4706182107</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
July 2018 Unofficial Model Run includes update to CBRFC forecasts, model name, ruleset name, and model output files. No model or ruleset changes. Cleared old files.
</commit_message>
<xml_diff>
--- a/Output Data/MtomToCrss_Annual.xlsx
+++ b/Output Data/MtomToCrss_Annual.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\MTOM\dev\Output Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\MTOM\Output Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12570" windowHeight="13590"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="9900"/>
   </bookViews>
   <sheets>
     <sheet name="Trace38" sheetId="37" r:id="rId1"/>
@@ -457,13 +457,13 @@
         <v>142814.3500004583</v>
       </c>
       <c r="F2">
-        <v>8999999.9999775533</v>
+        <v>8999999.9999775514</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9233414.3667382021</v>
+        <v>9277925.9766958896</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
@@ -477,13 +477,13 @@
         <v>23750.000000037599</v>
       </c>
       <c r="C3">
-        <v>54150.395504590306</v>
+        <v>52442.225504587172</v>
       </c>
       <c r="D3">
         <v>80404.999999993204</v>
       </c>
       <c r="E3">
-        <v>158305.39550462109</v>
+        <v>156597.22550461796</v>
       </c>
       <c r="F3">
         <v>8229999.9999991106</v>
@@ -554,13 +554,13 @@
         <v>718814.35000005946</v>
       </c>
       <c r="F2">
-        <v>8999999.9999775533</v>
+        <v>8999999.9999775514</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9295861.1006182134</v>
+        <v>9316918.7343768906</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
@@ -651,13 +651,13 @@
         <v>576314.35000015807</v>
       </c>
       <c r="F2">
-        <v>8999999.9999775533</v>
+        <v>8999999.9999775514</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9250550.2506182138</v>
+        <v>9282571.4043768886</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
@@ -748,13 +748,13 @@
         <v>433814.35000025679</v>
       </c>
       <c r="F2">
-        <v>8999999.9999775533</v>
+        <v>8999999.9999775514</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9206430.700618213</v>
+        <v>9244773.34437689</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
@@ -845,13 +845,13 @@
         <v>576314.35000015807</v>
       </c>
       <c r="F2">
-        <v>8999999.9999775533</v>
+        <v>8999999.9999775514</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9250667.0606182124</v>
+        <v>9277655.5343768895</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
@@ -874,13 +874,13 @@
         <v>562149.56950015435</v>
       </c>
       <c r="F3">
-        <v>8999999.9999775533</v>
+        <v>8963072.219684409</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>9104398.0899775531</v>
+        <v>9067470.3096844107</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -942,13 +942,13 @@
         <v>336814.35000006185</v>
       </c>
       <c r="F2">
-        <v>8999999.9999775533</v>
+        <v>8999999.9999775514</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9236389.5306182131</v>
+        <v>9267976.9443768915</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
@@ -1039,13 +1039,13 @@
         <v>336814.35000006185</v>
       </c>
       <c r="F2">
-        <v>8999999.9999775533</v>
+        <v>8999999.9999775514</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9206042.7306182124</v>
+        <v>9245007.5143768899</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
@@ -1136,13 +1136,13 @@
         <v>576314.35000015807</v>
       </c>
       <c r="F2">
-        <v>8999999.9999775533</v>
+        <v>8999999.9999775514</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9255659.1806182135</v>
+        <v>9282453.7343768906</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
@@ -1165,13 +1165,13 @@
         <v>465149.56949995935</v>
       </c>
       <c r="F3">
-        <v>8999999.9999775533</v>
+        <v>8998401.3091335408</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>9105477.679977553</v>
+        <v>9103878.9891335424</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -1233,13 +1233,13 @@
         <v>718814.35000005946</v>
       </c>
       <c r="F2">
-        <v>8999999.9999775533</v>
+        <v>8999999.9999775514</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9248922.3406182136</v>
+        <v>9282057.1743768901</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
@@ -1262,13 +1262,13 @@
         <v>842874.56949995994</v>
       </c>
       <c r="F3">
-        <v>8684014.6675812695</v>
+        <v>8607744.6591605637</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>8824642.6975812688</v>
+        <v>8748372.6891605649</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -1330,13 +1330,13 @@
         <v>718814.35000005946</v>
       </c>
       <c r="F2">
-        <v>8999999.9999775533</v>
+        <v>8999999.9999775514</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9170167.1706182137</v>
+        <v>9239252.5343768895</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
@@ -1350,13 +1350,13 @@
         <v>23750.000000037599</v>
       </c>
       <c r="C3">
-        <v>897870.39550400607</v>
+        <v>896162.22550400288</v>
       </c>
       <c r="D3">
         <v>80404.999999993204</v>
       </c>
       <c r="E3">
-        <v>1002025.3955040367</v>
+        <v>1000317.2255040336</v>
       </c>
       <c r="F3">
         <v>8999999.9999775533</v>
@@ -1427,13 +1427,13 @@
         <v>718814.35000005946</v>
       </c>
       <c r="F2">
-        <v>8999999.9999775533</v>
+        <v>8999999.9999775514</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9193136.5506182127</v>
+        <v>9239763.9443768878</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
@@ -1524,13 +1524,13 @@
         <v>142814.3500004583</v>
       </c>
       <c r="F2">
-        <v>8999999.9999775533</v>
+        <v>8999999.9999775514</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9235473.5634292122</v>
+        <v>9270713.8395012897</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
@@ -1621,13 +1621,13 @@
         <v>718814.35000005946</v>
       </c>
       <c r="F2">
-        <v>8999999.9999775533</v>
+        <v>8999999.9999775514</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9222416.2486182135</v>
+        <v>9266923.5183768906</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
@@ -1718,13 +1718,13 @@
         <v>718814.35000005946</v>
       </c>
       <c r="F2">
-        <v>8999999.9999775533</v>
+        <v>8999999.9999775514</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9252495.9286182113</v>
+        <v>9281489.4723768886</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
@@ -1815,13 +1815,13 @@
         <v>142814.3500004583</v>
       </c>
       <c r="F2">
-        <v>8999999.9999775533</v>
+        <v>8999999.9999775514</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9211668.2466182131</v>
+        <v>9258588.3923768923</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
@@ -1912,13 +1912,13 @@
         <v>576314.35000015807</v>
       </c>
       <c r="F2">
-        <v>8999999.9999775533</v>
+        <v>8999999.9999775514</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9220906.3186182119</v>
+        <v>9262125.0523768887</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
@@ -1941,13 +1941,13 @@
         <v>271149.56950035581</v>
       </c>
       <c r="F3">
-        <v>8989876.7032403443</v>
+        <v>8817940.3666410483</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>9123067.457240345</v>
+        <v>8951131.120641049</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -2009,13 +2009,13 @@
         <v>142814.3500004583</v>
       </c>
       <c r="F2">
-        <v>8999999.9999775533</v>
+        <v>8999999.9999775514</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9250696.2646182105</v>
+        <v>9295427.7283768877</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
@@ -2106,13 +2106,13 @@
         <v>142814.3500004583</v>
       </c>
       <c r="F2">
-        <v>8999999.9999775533</v>
+        <v>8999999.9999775514</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9245005.176618211</v>
+        <v>9271363.384376891</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
@@ -2135,13 +2135,13 @@
         <v>9.0604259869818987E-12</v>
       </c>
       <c r="F3">
-        <v>8532920.2607673369</v>
+        <v>8526633.0356878955</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>8772838.7487673368</v>
+        <v>8766551.5236878935</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -2203,13 +2203,13 @@
         <v>142814.3500004583</v>
       </c>
       <c r="F2">
-        <v>8999999.9999775533</v>
+        <v>8999999.9999775514</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9250104.7266182136</v>
+        <v>9286084.1643768903</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
@@ -2232,13 +2232,13 @@
         <v>9.0604259869818987E-12</v>
       </c>
       <c r="F3">
-        <v>8999999.9999775533</v>
+        <v>8944580.1798860673</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>9174276.6739775538</v>
+        <v>9118856.8538860679</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -2300,13 +2300,13 @@
         <v>336814.35000006185</v>
       </c>
       <c r="F2">
-        <v>8999999.9999775533</v>
+        <v>8999999.9999775514</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9240405.4026182126</v>
+        <v>9284462.0563768893</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
@@ -2320,13 +2320,13 @@
         <v>23750.000000037599</v>
       </c>
       <c r="C3">
-        <v>242330.39550420572</v>
+        <v>240622.22550420259</v>
       </c>
       <c r="D3">
         <v>80404.999999993204</v>
       </c>
       <c r="E3">
-        <v>346485.39550423651</v>
+        <v>344777.22550423339</v>
       </c>
       <c r="F3">
         <v>8229999.9999991106</v>
@@ -2397,13 +2397,13 @@
         <v>142814.3500004583</v>
       </c>
       <c r="F2">
-        <v>8999999.9999775533</v>
+        <v>8999999.9999775514</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9222523.6566182133</v>
+        <v>9265566.8143768925</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
@@ -2426,13 +2426,13 @@
         <v>42814.350000257342</v>
       </c>
       <c r="F3">
-        <v>8592245.0237977803</v>
+        <v>8527725.3983411361</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>8742774.0497977808</v>
+        <v>8678254.4243411366</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -2494,13 +2494,13 @@
         <v>336814.35000006185</v>
       </c>
       <c r="F2">
-        <v>8999999.9999775533</v>
+        <v>8999999.9999775514</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9254135.5006182119</v>
+        <v>9285977.6823768876</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
@@ -2523,13 +2523,13 @@
         <v>36814.350000269616</v>
       </c>
       <c r="F3">
-        <v>8762028.3531198837</v>
+        <v>8750166.6880306825</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>8950178.1851198822</v>
+        <v>8938316.5200306848</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -2591,13 +2591,13 @@
         <v>336814.35000006185</v>
       </c>
       <c r="F2">
-        <v>8999999.9999775533</v>
+        <v>8999999.9999775514</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9220465.9106182121</v>
+        <v>9259876.7743768897</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
@@ -2688,13 +2688,13 @@
         <v>718814.35000005946</v>
       </c>
       <c r="F2">
-        <v>8999999.9999775533</v>
+        <v>8999999.9999775514</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9209879.1566182114</v>
+        <v>9241904.838376889</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
@@ -2708,13 +2708,13 @@
         <v>23750.000000037599</v>
       </c>
       <c r="C3">
-        <v>499219.56949983287</v>
+        <v>614659.35000002873</v>
       </c>
       <c r="D3">
         <v>80404.999999993204</v>
       </c>
       <c r="E3">
-        <v>603374.56949986366</v>
+        <v>718814.35000005946</v>
       </c>
       <c r="F3">
         <v>8999999.9999775533</v>
@@ -2726,7 +2726,7 @@
         <v>9186800.7719775531</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2785,13 +2785,13 @@
         <v>336814.35000006185</v>
       </c>
       <c r="F2">
-        <v>8999999.9999775533</v>
+        <v>8999999.9999775514</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9225251.6906182114</v>
+        <v>9251313.4483768884</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
@@ -2882,13 +2882,13 @@
         <v>718814.35000005946</v>
       </c>
       <c r="F2">
-        <v>8999999.9999775533</v>
+        <v>8999999.9999775514</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9299916.012618212</v>
+        <v>9338103.5363768917</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
@@ -2979,13 +2979,13 @@
         <v>718814.35000005946</v>
       </c>
       <c r="F2">
-        <v>8999999.9999775533</v>
+        <v>8999999.9999775514</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9257004.4646182116</v>
+        <v>9306934.5663768891</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
@@ -3076,13 +3076,13 @@
         <v>718814.35000005946</v>
       </c>
       <c r="F2">
-        <v>8999999.9999775533</v>
+        <v>8999999.9999775514</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9237555.8146182112</v>
+        <v>9280548.6223768909</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
@@ -3173,13 +3173,13 @@
         <v>336814.35000006185</v>
       </c>
       <c r="F2">
-        <v>8999999.9999775533</v>
+        <v>8999999.9999775514</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9222508.3326182142</v>
+        <v>9264708.6483768895</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
@@ -3270,13 +3270,13 @@
         <v>433814.35000025679</v>
       </c>
       <c r="F2">
-        <v>8999999.9999775533</v>
+        <v>8999999.9999775514</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9233958.1006182134</v>
+        <v>9272009.6543768905</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
@@ -3379,13 +3379,13 @@
         <v>433814.35000025679</v>
       </c>
       <c r="F2">
-        <v>8999999.9999775533</v>
+        <v>8999999.9999775514</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9195730.0006182119</v>
+        <v>9238003.5843768921</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
@@ -3476,13 +3476,13 @@
         <v>718814.35000005946</v>
       </c>
       <c r="F2">
-        <v>8999999.9999775533</v>
+        <v>8999999.9999775514</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9268541.3806182127</v>
+        <v>9300298.2043768913</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
@@ -3573,13 +3573,13 @@
         <v>433814.35000025679</v>
       </c>
       <c r="F2">
-        <v>8999999.9999775533</v>
+        <v>8999999.9999775514</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9243925.6506182123</v>
+        <v>9278822.59437689</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
@@ -3670,13 +3670,13 @@
         <v>336814.35000006185</v>
       </c>
       <c r="F2">
-        <v>8999999.9999775533</v>
+        <v>8999999.9999775514</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9251713.6206182111</v>
+        <v>9291552.964376891</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
@@ -3699,13 +3699,13 @@
         <v>336814.35000006185</v>
       </c>
       <c r="F3">
-        <v>8999999.9999775533</v>
+        <v>8859553.2713664547</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>9183949.7199775539</v>
+        <v>9043502.9913664535</v>
       </c>
       <c r="I3">
         <v>1</v>
@@ -3767,13 +3767,13 @@
         <v>142814.3500004583</v>
       </c>
       <c r="F2">
-        <v>8999999.9999775533</v>
+        <v>8999999.9999775514</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9258068.0306182113</v>
+        <v>9285161.1243768912</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
@@ -3864,13 +3864,13 @@
         <v>336814.35000006185</v>
       </c>
       <c r="F2">
-        <v>8999999.9999775533</v>
+        <v>8999999.9999775514</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9230093.4706182107</v>
+        <v>9266173.9143768903</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
Files created when running MRM - should add to gitnore???
</commit_message>
<xml_diff>
--- a/Output Data/MtomToCrss_Annual.xlsx
+++ b/Output Data/MtomToCrss_Annual.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\MTOM\Output Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sabaker\Documents\2.MTOM Testbed\dev\Output Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -412,9 +412,9 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -440,7 +440,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
@@ -469,7 +469,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
@@ -509,9 +509,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -537,7 +537,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
@@ -566,7 +566,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
@@ -606,9 +606,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -634,7 +634,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
@@ -663,7 +663,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
@@ -703,9 +703,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -731,7 +731,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
@@ -760,7 +760,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
@@ -800,9 +800,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -828,7 +828,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
@@ -857,7 +857,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
@@ -897,9 +897,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -925,7 +925,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
@@ -954,7 +954,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
@@ -994,9 +994,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1022,7 +1022,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
@@ -1051,7 +1051,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
@@ -1091,9 +1091,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1119,7 +1119,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
@@ -1148,7 +1148,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
@@ -1188,9 +1188,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1216,7 +1216,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
@@ -1245,7 +1245,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
@@ -1285,9 +1285,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1313,7 +1313,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
@@ -1342,7 +1342,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
@@ -1382,9 +1382,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1410,7 +1410,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
@@ -1439,7 +1439,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
@@ -1479,9 +1479,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1507,7 +1507,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
@@ -1536,7 +1536,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
@@ -1576,9 +1576,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1604,7 +1604,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
@@ -1633,7 +1633,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
@@ -1673,9 +1673,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1701,7 +1701,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
@@ -1730,7 +1730,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
@@ -1770,9 +1770,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1798,7 +1798,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
@@ -1827,7 +1827,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
@@ -1867,9 +1867,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1895,7 +1895,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
@@ -1924,7 +1924,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
@@ -1964,9 +1964,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1992,7 +1992,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
@@ -2021,7 +2021,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
@@ -2061,9 +2061,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2089,7 +2089,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
@@ -2118,7 +2118,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
@@ -2158,9 +2158,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2186,7 +2186,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
@@ -2215,7 +2215,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
@@ -2255,9 +2255,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2283,7 +2283,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
@@ -2312,7 +2312,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
@@ -2352,9 +2352,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2380,7 +2380,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
@@ -2409,7 +2409,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
@@ -2449,9 +2449,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2477,7 +2477,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
@@ -2506,7 +2506,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
@@ -2546,9 +2546,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2574,7 +2574,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
@@ -2603,7 +2603,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
@@ -2643,9 +2643,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2671,7 +2671,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
@@ -2700,7 +2700,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
@@ -2740,9 +2740,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2768,7 +2768,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
@@ -2797,7 +2797,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
@@ -2837,9 +2837,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2865,7 +2865,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
@@ -2894,7 +2894,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
@@ -2934,9 +2934,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2962,7 +2962,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
@@ -2991,7 +2991,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
@@ -3031,9 +3031,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -3059,7 +3059,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
@@ -3088,7 +3088,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
@@ -3128,9 +3128,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -3156,7 +3156,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
@@ -3185,7 +3185,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
@@ -3225,9 +3225,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -3253,7 +3253,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
@@ -3282,7 +3282,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
@@ -3322,7 +3322,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3334,9 +3334,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -3362,7 +3362,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
@@ -3391,7 +3391,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
@@ -3431,9 +3431,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -3459,7 +3459,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
@@ -3488,7 +3488,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
@@ -3528,9 +3528,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -3556,7 +3556,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
@@ -3585,7 +3585,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
@@ -3625,9 +3625,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -3653,7 +3653,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
@@ -3682,7 +3682,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
@@ -3699,13 +3699,13 @@
         <v>336814.35000006185</v>
       </c>
       <c r="F3">
-        <v>8859553.2713664547</v>
+        <v>8855471.0505504292</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>9043502.9913664535</v>
+        <v>9039420.770550428</v>
       </c>
       <c r="I3">
         <v>1</v>
@@ -3722,9 +3722,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -3750,7 +3750,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
@@ -3779,7 +3779,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
@@ -3819,9 +3819,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -3847,7 +3847,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
@@ -3876,7 +3876,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>43466</v>
       </c>

</xml_diff>

<commit_message>
Edited rule 'Set Upper Balancing Release Volume'
Added TierIs() to execution constraints since it should be there instead of in an IF statement at the beginning of the rule. Removed the IF statement that starts the rule.
</commit_message>
<xml_diff>
--- a/Output Data/MtomToCrss_Annual.xlsx
+++ b/Output Data/MtomToCrss_Annual.xlsx
@@ -777,13 +777,13 @@
         <v>566424.56950015132</v>
       </c>
       <c r="F3">
-        <v>8999999.9999775533</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>9129167.7799775526</v>
+        <v>8359167.7799991118</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -874,13 +874,13 @@
         <v>562149.56950015435</v>
       </c>
       <c r="F3">
-        <v>8963072.219684409</v>
+        <v>8963461.9073324595</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>9067470.3096844107</v>
+        <v>9067859.9973324612</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -1165,13 +1165,13 @@
         <v>465149.56949995935</v>
       </c>
       <c r="F3">
-        <v>8998401.3091335408</v>
+        <v>8998279.095999198</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>9103878.9891335424</v>
+        <v>9103756.7759991977</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -1262,13 +1262,13 @@
         <v>842874.56949995994</v>
       </c>
       <c r="F3">
-        <v>8607744.6591605637</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>8748372.6891605649</v>
+        <v>8370628.0299991099</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -1941,13 +1941,13 @@
         <v>271149.56950035581</v>
       </c>
       <c r="F3">
-        <v>8817940.3666410483</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>8951131.120641049</v>
+        <v>8363190.7539991112</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -2038,13 +2038,13 @@
         <v>284154.56950034678</v>
       </c>
       <c r="F3">
-        <v>8999999.9999775533</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>9412167.4919775538</v>
+        <v>8642167.4919991121</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -2135,13 +2135,13 @@
         <v>9.0604259869818987E-12</v>
       </c>
       <c r="F3">
-        <v>8526633.0356878955</v>
+        <v>8526339.0774415266</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>8766551.5236878935</v>
+        <v>8766257.5654415246</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -2232,13 +2232,13 @@
         <v>9.0604259869818987E-12</v>
       </c>
       <c r="F3">
-        <v>8944580.1798860673</v>
+        <v>8943937.4051519353</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>9118856.8538860679</v>
+        <v>9118214.0791519359</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -2426,13 +2426,13 @@
         <v>42814.350000257342</v>
       </c>
       <c r="F3">
-        <v>8527725.3983411361</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>8678254.4243411366</v>
+        <v>8380529.0259991111</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -2523,13 +2523,13 @@
         <v>36814.350000269616</v>
       </c>
       <c r="F3">
-        <v>8750166.6880306825</v>
+        <v>8749436.6009142287</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>8938316.5200306848</v>
+        <v>8937586.4329142291</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -3699,13 +3699,13 @@
         <v>336814.35000006185</v>
       </c>
       <c r="F3">
-        <v>8855471.0505504292</v>
+        <v>8855621.3292080667</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>9039420.770550428</v>
+        <v>9039571.0492080655</v>
       </c>
       <c r="I3">
         <v>1</v>

</xml_diff>

<commit_message>
saved output of xlsx (no real changes)
</commit_message>
<xml_diff>
--- a/Output Data/MtomToCrss_Annual.xlsx
+++ b/Output Data/MtomToCrss_Annual.xlsx
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="8">
   <si>
     <t>ICS Credits.BiNationalICS_CA</t>
   </si>
@@ -84,9 +84,6 @@
   </si>
   <si>
     <t>SystemConditions.LBShortageTier</t>
-  </si>
-  <si>
-    <t>NaN</t>
   </si>
 </sst>
 </file>
@@ -465,8 +462,8 @@
       <c r="H2">
         <v>9277925.9766958896</v>
       </c>
-      <c r="I2" t="s">
-        <v>8</v>
+      <c r="I2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -562,8 +559,8 @@
       <c r="H2">
         <v>9316918.7343768906</v>
       </c>
-      <c r="I2" t="s">
-        <v>8</v>
+      <c r="I2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -659,8 +656,8 @@
       <c r="H2">
         <v>9282571.4043768886</v>
       </c>
-      <c r="I2" t="s">
-        <v>8</v>
+      <c r="I2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -756,8 +753,8 @@
       <c r="H2">
         <v>9244773.34437689</v>
       </c>
-      <c r="I2" t="s">
-        <v>8</v>
+      <c r="I2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -853,8 +850,8 @@
       <c r="H2">
         <v>9277655.5343768895</v>
       </c>
-      <c r="I2" t="s">
-        <v>8</v>
+      <c r="I2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -874,13 +871,13 @@
         <v>562149.56950015435</v>
       </c>
       <c r="F3">
-        <v>8963461.9073324595</v>
+        <v>8963712.0121370479</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>9067859.9973324612</v>
+        <v>9068110.1021370497</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -950,8 +947,8 @@
       <c r="H2">
         <v>9267976.9443768915</v>
       </c>
-      <c r="I2" t="s">
-        <v>8</v>
+      <c r="I2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -1047,8 +1044,8 @@
       <c r="H2">
         <v>9245007.5143768899</v>
       </c>
-      <c r="I2" t="s">
-        <v>8</v>
+      <c r="I2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -1144,8 +1141,8 @@
       <c r="H2">
         <v>9282453.7343768906</v>
       </c>
-      <c r="I2" t="s">
-        <v>8</v>
+      <c r="I2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -1165,13 +1162,13 @@
         <v>465149.56949995935</v>
       </c>
       <c r="F3">
-        <v>8998279.095999198</v>
+        <v>8998401.3091335408</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>9103756.7759991977</v>
+        <v>9103878.9891335424</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -1241,8 +1238,8 @@
       <c r="H2">
         <v>9282057.1743768901</v>
       </c>
-      <c r="I2" t="s">
-        <v>8</v>
+      <c r="I2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -1338,8 +1335,8 @@
       <c r="H2">
         <v>9239252.5343768895</v>
       </c>
-      <c r="I2" t="s">
-        <v>8</v>
+      <c r="I2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -1435,8 +1432,8 @@
       <c r="H2">
         <v>9239763.9443768878</v>
       </c>
-      <c r="I2" t="s">
-        <v>8</v>
+      <c r="I2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -1532,8 +1529,8 @@
       <c r="H2">
         <v>9270713.8395012897</v>
       </c>
-      <c r="I2" t="s">
-        <v>8</v>
+      <c r="I2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -1629,8 +1626,8 @@
       <c r="H2">
         <v>9266923.5183768906</v>
       </c>
-      <c r="I2" t="s">
-        <v>8</v>
+      <c r="I2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -1726,8 +1723,8 @@
       <c r="H2">
         <v>9281489.4723768886</v>
       </c>
-      <c r="I2" t="s">
-        <v>8</v>
+      <c r="I2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -1823,8 +1820,8 @@
       <c r="H2">
         <v>9258588.3923768923</v>
       </c>
-      <c r="I2" t="s">
-        <v>8</v>
+      <c r="I2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -1920,8 +1917,8 @@
       <c r="H2">
         <v>9262125.0523768887</v>
       </c>
-      <c r="I2" t="s">
-        <v>8</v>
+      <c r="I2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -2017,8 +2014,8 @@
       <c r="H2">
         <v>9295427.7283768877</v>
       </c>
-      <c r="I2" t="s">
-        <v>8</v>
+      <c r="I2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -2114,8 +2111,8 @@
       <c r="H2">
         <v>9271363.384376891</v>
       </c>
-      <c r="I2" t="s">
-        <v>8</v>
+      <c r="I2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -2135,13 +2132,13 @@
         <v>9.0604259869818987E-12</v>
       </c>
       <c r="F3">
-        <v>8526339.0774415266</v>
+        <v>8526633.0356878955</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>8766257.5654415246</v>
+        <v>8766551.5236878935</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -2211,8 +2208,8 @@
       <c r="H2">
         <v>9286084.1643768903</v>
       </c>
-      <c r="I2" t="s">
-        <v>8</v>
+      <c r="I2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -2232,13 +2229,13 @@
         <v>9.0604259869818987E-12</v>
       </c>
       <c r="F3">
-        <v>8943937.4051519353</v>
+        <v>8944580.1798860673</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>9118214.0791519359</v>
+        <v>9118856.8538860679</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -2308,8 +2305,8 @@
       <c r="H2">
         <v>9284462.0563768893</v>
       </c>
-      <c r="I2" t="s">
-        <v>8</v>
+      <c r="I2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -2405,8 +2402,8 @@
       <c r="H2">
         <v>9265566.8143768925</v>
       </c>
-      <c r="I2" t="s">
-        <v>8</v>
+      <c r="I2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -2502,8 +2499,8 @@
       <c r="H2">
         <v>9285977.6823768876</v>
       </c>
-      <c r="I2" t="s">
-        <v>8</v>
+      <c r="I2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -2523,13 +2520,13 @@
         <v>36814.350000269616</v>
       </c>
       <c r="F3">
-        <v>8749436.6009142287</v>
+        <v>8750166.6880306825</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>8937586.4329142291</v>
+        <v>8938316.5200306848</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -2599,8 +2596,8 @@
       <c r="H2">
         <v>9259876.7743768897</v>
       </c>
-      <c r="I2" t="s">
-        <v>8</v>
+      <c r="I2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -2696,8 +2693,8 @@
       <c r="H2">
         <v>9241904.838376889</v>
       </c>
-      <c r="I2" t="s">
-        <v>8</v>
+      <c r="I2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -2793,8 +2790,8 @@
       <c r="H2">
         <v>9251313.4483768884</v>
       </c>
-      <c r="I2" t="s">
-        <v>8</v>
+      <c r="I2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -2890,8 +2887,8 @@
       <c r="H2">
         <v>9338103.5363768917</v>
       </c>
-      <c r="I2" t="s">
-        <v>8</v>
+      <c r="I2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -2987,8 +2984,8 @@
       <c r="H2">
         <v>9306934.5663768891</v>
       </c>
-      <c r="I2" t="s">
-        <v>8</v>
+      <c r="I2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -3008,13 +3005,13 @@
         <v>985374.5694998611</v>
       </c>
       <c r="F3">
-        <v>8999999.9999775533</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>9285309.8079775535</v>
+        <v>8515309.8079991098</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -3084,8 +3081,8 @@
       <c r="H2">
         <v>9280548.6223768909</v>
       </c>
-      <c r="I2" t="s">
-        <v>8</v>
+      <c r="I2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -3181,8 +3178,8 @@
       <c r="H2">
         <v>9264708.6483768895</v>
       </c>
-      <c r="I2" t="s">
-        <v>8</v>
+      <c r="I2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -3278,8 +3275,8 @@
       <c r="H2">
         <v>9272009.6543768905</v>
       </c>
-      <c r="I2" t="s">
-        <v>8</v>
+      <c r="I2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -3387,8 +3384,8 @@
       <c r="H2">
         <v>9238003.5843768921</v>
       </c>
-      <c r="I2" t="s">
-        <v>8</v>
+      <c r="I2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -3484,8 +3481,8 @@
       <c r="H2">
         <v>9300298.2043768913</v>
       </c>
-      <c r="I2" t="s">
-        <v>8</v>
+      <c r="I2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -3581,8 +3578,8 @@
       <c r="H2">
         <v>9278822.59437689</v>
       </c>
-      <c r="I2" t="s">
-        <v>8</v>
+      <c r="I2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -3678,8 +3675,8 @@
       <c r="H2">
         <v>9291552.964376891</v>
       </c>
-      <c r="I2" t="s">
-        <v>8</v>
+      <c r="I2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -3699,13 +3696,13 @@
         <v>336814.35000006185</v>
       </c>
       <c r="F3">
-        <v>8855621.3292080667</v>
+        <v>8855121.830367364</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>9039571.0492080655</v>
+        <v>9039071.5503673628</v>
       </c>
       <c r="I3">
         <v>1</v>
@@ -3775,8 +3772,8 @@
       <c r="H2">
         <v>9285161.1243768912</v>
       </c>
-      <c r="I2" t="s">
-        <v>8</v>
+      <c r="I2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -3872,8 +3869,8 @@
       <c r="H2">
         <v>9266173.9143768903</v>
       </c>
-      <c r="I2" t="s">
-        <v>8</v>
+      <c r="I2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Reverted the reference in Redistribute MWD Nov & Dec Div Request to MWDDiversionData.MWDCanal_DailyCapacity and added MWDDiversionData slot back into the model. Included output files.
</commit_message>
<xml_diff>
--- a/Output Data/MtomToCrss_Annual.xlsx
+++ b/Output Data/MtomToCrss_Annual.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sabaker\Documents\2.MTOM Testbed\dev\Output Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\MTOM\Output Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="9900"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="1470"/>
   </bookViews>
   <sheets>
     <sheet name="Trace38" sheetId="37" r:id="rId1"/>
@@ -409,9 +409,9 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -437,7 +437,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
@@ -445,28 +445,28 @@
         <v>23750.000000037599</v>
       </c>
       <c r="C2">
-        <v>38659.350000427519</v>
+        <v>63516.570000201522</v>
       </c>
       <c r="D2">
-        <v>80404.999999993204</v>
+        <v>89397</v>
       </c>
       <c r="E2">
-        <v>142814.3500004583</v>
+        <v>176663.57000023909</v>
       </c>
       <c r="F2">
-        <v>8999999.9999775514</v>
+        <v>8999905.9942071997</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9277925.9766958896</v>
+        <v>9315465.9063824043</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
@@ -474,13 +474,13 @@
         <v>23750.000000037599</v>
       </c>
       <c r="C3">
-        <v>52442.225504587172</v>
+        <v>55577.672904369225</v>
       </c>
       <c r="D3">
-        <v>80404.999999993204</v>
+        <v>89397</v>
       </c>
       <c r="E3">
-        <v>156597.22550461796</v>
+        <v>168724.67290440682</v>
       </c>
       <c r="F3">
         <v>8229999.9999991106</v>
@@ -489,7 +489,7 @@
         <v>1</v>
       </c>
       <c r="H3">
-        <v>8340979.6592188207</v>
+        <v>8340981.0259991111</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -506,9 +506,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -534,7 +534,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
@@ -542,28 +542,28 @@
         <v>23750.000000037599</v>
       </c>
       <c r="C2">
-        <v>614659.35000002873</v>
+        <v>639516.56999980274</v>
       </c>
       <c r="D2">
-        <v>80404.999999993204</v>
+        <v>89397</v>
       </c>
       <c r="E2">
-        <v>718814.35000005946</v>
+        <v>752663.56999984034</v>
       </c>
       <c r="F2">
-        <v>8999999.9999775514</v>
+        <v>8999905.9942071997</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9316918.7343768906</v>
+        <v>9315465.9063824043</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
@@ -571,22 +571,22 @@
         <v>23750.000000037599</v>
       </c>
       <c r="C3">
-        <v>499219.56949983287</v>
+        <v>523331.0728996137</v>
       </c>
       <c r="D3">
-        <v>80404.999999993204</v>
+        <v>89397</v>
       </c>
       <c r="E3">
-        <v>603374.56949986366</v>
+        <v>636478.07289965136</v>
       </c>
       <c r="F3">
-        <v>8999999.9999775533</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>9166147.929977553</v>
+        <v>8396147.9299991112</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -603,9 +603,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -631,7 +631,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
@@ -639,28 +639,28 @@
         <v>23750.000000037599</v>
       </c>
       <c r="C2">
-        <v>472159.35000012728</v>
+        <v>497016.56999990129</v>
       </c>
       <c r="D2">
-        <v>80404.999999993204</v>
+        <v>89397</v>
       </c>
       <c r="E2">
-        <v>576314.35000015807</v>
+        <v>610163.56999993895</v>
       </c>
       <c r="F2">
-        <v>8999999.9999775514</v>
+        <v>8999905.9942071997</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9282571.4043768886</v>
+        <v>9315465.9063824043</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
@@ -668,22 +668,22 @@
         <v>23750.000000037599</v>
       </c>
       <c r="C3">
-        <v>742994.56949992606</v>
+        <v>767106.07289970689</v>
       </c>
       <c r="D3">
-        <v>80404.999999993204</v>
+        <v>89397</v>
       </c>
       <c r="E3">
-        <v>847149.56949995691</v>
+        <v>880253.0728997445</v>
       </c>
       <c r="F3">
-        <v>8999999.9999775533</v>
+        <v>8874579.3446566537</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>9263906.2799775526</v>
+        <v>9138485.624656653</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -700,9 +700,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -728,7 +728,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
@@ -736,28 +736,28 @@
         <v>23750.000000037599</v>
       </c>
       <c r="C2">
-        <v>329659.350000226</v>
+        <v>354516.57</v>
       </c>
       <c r="D2">
-        <v>80404.999999993204</v>
+        <v>89397</v>
       </c>
       <c r="E2">
-        <v>433814.35000025679</v>
+        <v>467663.57000003767</v>
       </c>
       <c r="F2">
-        <v>8999999.9999775514</v>
+        <v>8999905.9942071997</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9244773.34437689</v>
+        <v>9315465.9063824043</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
@@ -765,13 +765,13 @@
         <v>23750.000000037599</v>
       </c>
       <c r="C3">
-        <v>462269.56950012053</v>
+        <v>486381.07289990137</v>
       </c>
       <c r="D3">
-        <v>80404.999999993204</v>
+        <v>89397</v>
       </c>
       <c r="E3">
-        <v>566424.56950015132</v>
+        <v>599528.07289993903</v>
       </c>
       <c r="F3">
         <v>8229999.9999991106</v>
@@ -797,9 +797,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -825,7 +825,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
@@ -833,28 +833,28 @@
         <v>23750.000000037599</v>
       </c>
       <c r="C2">
-        <v>472159.35000012728</v>
+        <v>497016.56999990129</v>
       </c>
       <c r="D2">
-        <v>80404.999999993204</v>
+        <v>89397</v>
       </c>
       <c r="E2">
-        <v>576314.35000015807</v>
+        <v>610163.56999993895</v>
       </c>
       <c r="F2">
-        <v>8999999.9999775514</v>
+        <v>8999905.9942071997</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9277655.5343768895</v>
+        <v>9315465.9063824043</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
@@ -862,22 +862,22 @@
         <v>23750.000000037599</v>
       </c>
       <c r="C3">
-        <v>457994.5695001235</v>
+        <v>482106.07289990428</v>
       </c>
       <c r="D3">
-        <v>80404.999999993204</v>
+        <v>89397</v>
       </c>
       <c r="E3">
-        <v>562149.56950015435</v>
+        <v>595253.07289994194</v>
       </c>
       <c r="F3">
-        <v>8963712.0121370479</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>9068110.1021370497</v>
+        <v>8334398.0899991114</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -894,9 +894,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -922,7 +922,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
@@ -930,28 +930,28 @@
         <v>23750.000000037599</v>
       </c>
       <c r="C2">
-        <v>232659.35000003106</v>
+        <v>257516.56999980501</v>
       </c>
       <c r="D2">
-        <v>80404.999999993204</v>
+        <v>89397</v>
       </c>
       <c r="E2">
-        <v>336814.35000006185</v>
+        <v>370663.56999984261</v>
       </c>
       <c r="F2">
-        <v>8999999.9999775514</v>
+        <v>8999905.9942071997</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9267976.9443768915</v>
+        <v>9315465.9063824043</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
@@ -959,22 +959,22 @@
         <v>23750.000000037599</v>
       </c>
       <c r="C3">
-        <v>368179.56949993141</v>
+        <v>392291.07289971219</v>
       </c>
       <c r="D3">
-        <v>80404.999999993204</v>
+        <v>89397</v>
       </c>
       <c r="E3">
-        <v>472334.56949996221</v>
+        <v>505438.07289974985</v>
       </c>
       <c r="F3">
-        <v>8999999.9999775533</v>
+        <v>8738263.7609513756</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>9131647.4399775527</v>
+        <v>8869911.2009513751</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -991,9 +991,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1019,7 +1019,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
@@ -1027,28 +1027,28 @@
         <v>23750.000000037599</v>
       </c>
       <c r="C2">
-        <v>232659.35000003106</v>
+        <v>257516.56999980501</v>
       </c>
       <c r="D2">
-        <v>80404.999999993204</v>
+        <v>89397</v>
       </c>
       <c r="E2">
-        <v>336814.35000006185</v>
+        <v>370663.56999984261</v>
       </c>
       <c r="F2">
-        <v>8999999.9999775514</v>
+        <v>8999905.9942071997</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9245007.5143768899</v>
+        <v>9315465.9063824043</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
@@ -1056,13 +1056,13 @@
         <v>23750.000000037599</v>
       </c>
       <c r="C3">
-        <v>128679.56949983518</v>
+        <v>152791.07289961592</v>
       </c>
       <c r="D3">
-        <v>80404.999999993204</v>
+        <v>89397</v>
       </c>
       <c r="E3">
-        <v>232834.56949986599</v>
+        <v>265938.07289965352</v>
       </c>
       <c r="F3">
         <v>8229999.9999991106</v>
@@ -1088,9 +1088,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1116,7 +1116,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
@@ -1124,28 +1124,28 @@
         <v>23750.000000037599</v>
       </c>
       <c r="C2">
-        <v>472159.35000012728</v>
+        <v>497016.56999990129</v>
       </c>
       <c r="D2">
-        <v>80404.999999993204</v>
+        <v>89397</v>
       </c>
       <c r="E2">
-        <v>576314.35000015807</v>
+        <v>610163.56999993895</v>
       </c>
       <c r="F2">
-        <v>8999999.9999775514</v>
+        <v>8999905.9942071997</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9282453.7343768906</v>
+        <v>9315465.9063824043</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
@@ -1153,22 +1153,22 @@
         <v>23750.000000037599</v>
       </c>
       <c r="C3">
-        <v>360994.5694999285</v>
+        <v>385106.07289970928</v>
       </c>
       <c r="D3">
-        <v>80404.999999993204</v>
+        <v>89397</v>
       </c>
       <c r="E3">
-        <v>465149.56949995935</v>
+        <v>498253.07289974694</v>
       </c>
       <c r="F3">
-        <v>8998401.3091335408</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>9103878.9891335424</v>
+        <v>8335477.6799991112</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -1185,9 +1185,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1213,7 +1213,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
@@ -1221,28 +1221,28 @@
         <v>23750.000000037599</v>
       </c>
       <c r="C2">
-        <v>614659.35000002873</v>
+        <v>639516.56999980274</v>
       </c>
       <c r="D2">
-        <v>80404.999999993204</v>
+        <v>89397</v>
       </c>
       <c r="E2">
-        <v>718814.35000005946</v>
+        <v>752663.56999984034</v>
       </c>
       <c r="F2">
-        <v>8999999.9999775514</v>
+        <v>8999905.9942071997</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9282057.1743768901</v>
+        <v>9315465.9063824043</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
@@ -1250,13 +1250,13 @@
         <v>23750.000000037599</v>
       </c>
       <c r="C3">
-        <v>738719.56949992909</v>
+        <v>762831.07289970992</v>
       </c>
       <c r="D3">
-        <v>80404.999999993204</v>
+        <v>89397</v>
       </c>
       <c r="E3">
-        <v>842874.56949995994</v>
+        <v>875978.07289974764</v>
       </c>
       <c r="F3">
         <v>8229999.9999991106</v>
@@ -1282,9 +1282,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1310,7 +1310,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
@@ -1318,28 +1318,28 @@
         <v>23750.000000037599</v>
       </c>
       <c r="C2">
-        <v>614659.35000002873</v>
+        <v>639516.56999980274</v>
       </c>
       <c r="D2">
-        <v>80404.999999993204</v>
+        <v>89397</v>
       </c>
       <c r="E2">
-        <v>718814.35000005946</v>
+        <v>752663.56999984034</v>
       </c>
       <c r="F2">
-        <v>8999999.9999775514</v>
+        <v>8999905.9942071997</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9239252.5343768895</v>
+        <v>9315465.9063824043</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
@@ -1347,13 +1347,13 @@
         <v>23750.000000037599</v>
       </c>
       <c r="C3">
-        <v>896162.22550400288</v>
+        <v>905331.0728996112</v>
       </c>
       <c r="D3">
-        <v>80404.999999993204</v>
+        <v>89397</v>
       </c>
       <c r="E3">
-        <v>1000317.2255040336</v>
+        <v>1018478.0728996487</v>
       </c>
       <c r="F3">
         <v>8999999.9999775533</v>
@@ -1379,9 +1379,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1407,7 +1407,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
@@ -1415,28 +1415,28 @@
         <v>23750.000000037599</v>
       </c>
       <c r="C2">
-        <v>614659.35000002873</v>
+        <v>639516.56999980274</v>
       </c>
       <c r="D2">
-        <v>80404.999999993204</v>
+        <v>89397</v>
       </c>
       <c r="E2">
-        <v>718814.35000005946</v>
+        <v>752663.56999984034</v>
       </c>
       <c r="F2">
-        <v>8999999.9999775514</v>
+        <v>8999905.9942071997</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9239763.9443768878</v>
+        <v>9315465.9063824043</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
@@ -1444,22 +1444,22 @@
         <v>23750.000000037599</v>
       </c>
       <c r="C3">
-        <v>881219.56949983037</v>
+        <v>905331.0728996112</v>
       </c>
       <c r="D3">
-        <v>80404.999999993204</v>
+        <v>89397</v>
       </c>
       <c r="E3">
-        <v>985374.5694998611</v>
+        <v>1018478.0728996487</v>
       </c>
       <c r="F3">
-        <v>8999999.9999775533</v>
+        <v>8739170.2718241215</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>8910372.509977553</v>
+        <v>8649542.7818241194</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -1476,9 +1476,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1504,7 +1504,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
@@ -1512,33 +1512,33 @@
         <v>23750.000000037599</v>
       </c>
       <c r="C2">
-        <v>38659.350000427519</v>
+        <v>63516.570000201522</v>
       </c>
       <c r="D2">
-        <v>80404.999999993204</v>
+        <v>89397</v>
       </c>
       <c r="E2">
-        <v>142814.3500004583</v>
+        <v>176663.57000023909</v>
       </c>
       <c r="F2">
-        <v>8999999.9999775514</v>
+        <v>8999905.9942071997</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9270713.8395012897</v>
+        <v>9315465.9063824043</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
       <c r="B3">
-        <v>9.0604259869818987E-12</v>
+        <v>2.1140993969624428E-11</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -1547,16 +1547,16 @@
         <v>0</v>
       </c>
       <c r="E3">
-        <v>9.0604259869818987E-12</v>
+        <v>2.1140993969624428E-11</v>
       </c>
       <c r="F3">
-        <v>8999999.9999775533</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>9135927.889236426</v>
+        <v>8365931.8499991121</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -1573,9 +1573,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1601,7 +1601,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
@@ -1609,28 +1609,28 @@
         <v>23750.000000037599</v>
       </c>
       <c r="C2">
-        <v>614659.35000002873</v>
+        <v>639516.56999980274</v>
       </c>
       <c r="D2">
-        <v>80404.999999993204</v>
+        <v>89397</v>
       </c>
       <c r="E2">
-        <v>718814.35000005946</v>
+        <v>752663.56999984034</v>
       </c>
       <c r="F2">
-        <v>8999999.9999775514</v>
+        <v>8999905.9942071997</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9266923.5183768906</v>
+        <v>9315465.9063824043</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
@@ -1638,13 +1638,13 @@
         <v>23750.000000037599</v>
       </c>
       <c r="C3">
-        <v>881219.56949983037</v>
+        <v>905331.0728996112</v>
       </c>
       <c r="D3">
-        <v>80404.999999993204</v>
+        <v>89397</v>
       </c>
       <c r="E3">
-        <v>985374.5694998611</v>
+        <v>1018478.0728996487</v>
       </c>
       <c r="F3">
         <v>8999999.9999775533</v>
@@ -1653,7 +1653,7 @@
         <v>1</v>
       </c>
       <c r="H3">
-        <v>9062310.0039775558</v>
+        <v>9061671.6859775539</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -1670,9 +1670,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1698,7 +1698,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
@@ -1706,28 +1706,28 @@
         <v>23750.000000037599</v>
       </c>
       <c r="C2">
-        <v>614659.35000002873</v>
+        <v>639516.56999980274</v>
       </c>
       <c r="D2">
-        <v>80404.999999993204</v>
+        <v>89397</v>
       </c>
       <c r="E2">
-        <v>718814.35000005946</v>
+        <v>752663.56999984034</v>
       </c>
       <c r="F2">
-        <v>8999999.9999775514</v>
+        <v>8999905.9942071997</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9281489.4723768886</v>
+        <v>9315465.9063824043</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
@@ -1735,13 +1735,13 @@
         <v>23750.000000037599</v>
       </c>
       <c r="C3">
-        <v>881219.56949983037</v>
+        <v>905331.0728996112</v>
       </c>
       <c r="D3">
-        <v>80404.999999993204</v>
+        <v>89397</v>
       </c>
       <c r="E3">
-        <v>985374.5694998611</v>
+        <v>1018478.0728996487</v>
       </c>
       <c r="F3">
         <v>8999999.9999775533</v>
@@ -1750,7 +1750,7 @@
         <v>1</v>
       </c>
       <c r="H3">
-        <v>9130276.3439775538</v>
+        <v>9128518.731977554</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -1767,9 +1767,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1795,7 +1795,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
@@ -1803,28 +1803,28 @@
         <v>23750.000000037599</v>
       </c>
       <c r="C2">
-        <v>38659.350000427519</v>
+        <v>63516.570000201522</v>
       </c>
       <c r="D2">
-        <v>80404.999999993204</v>
+        <v>89397</v>
       </c>
       <c r="E2">
-        <v>142814.3500004583</v>
+        <v>176663.57000023909</v>
       </c>
       <c r="F2">
-        <v>8999999.9999775514</v>
+        <v>8999905.9942071997</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9258588.3923768923</v>
+        <v>9315465.9063824043</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
@@ -1832,22 +1832,22 @@
         <v>23750.000000037599</v>
       </c>
       <c r="C3">
-        <v>322499.56950021733</v>
+        <v>346611.07289999811</v>
       </c>
       <c r="D3">
-        <v>80404.999999993204</v>
+        <v>89397</v>
       </c>
       <c r="E3">
-        <v>426654.56950024812</v>
+        <v>459758.07290003583</v>
       </c>
       <c r="F3">
-        <v>8999999.9999775533</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>9284015.4139775541</v>
+        <v>8512420.3039991111</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -1864,9 +1864,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1892,7 +1892,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
@@ -1900,28 +1900,28 @@
         <v>23750.000000037599</v>
       </c>
       <c r="C2">
-        <v>472159.35000012728</v>
+        <v>497016.56999990129</v>
       </c>
       <c r="D2">
-        <v>80404.999999993204</v>
+        <v>89397</v>
       </c>
       <c r="E2">
-        <v>576314.35000015807</v>
+        <v>610163.56999993895</v>
       </c>
       <c r="F2">
-        <v>8999999.9999775514</v>
+        <v>8999905.9942071997</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9262125.0523768887</v>
+        <v>9315465.9063824043</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
@@ -1929,13 +1929,13 @@
         <v>23750.000000037599</v>
       </c>
       <c r="C3">
-        <v>166994.56950032499</v>
+        <v>191106.07290010579</v>
       </c>
       <c r="D3">
-        <v>80404.999999993204</v>
+        <v>89397</v>
       </c>
       <c r="E3">
-        <v>271149.56950035581</v>
+        <v>304253.07290014339</v>
       </c>
       <c r="F3">
         <v>8229999.9999991106</v>
@@ -1944,7 +1944,7 @@
         <v>1</v>
       </c>
       <c r="H3">
-        <v>8363190.7539991112</v>
+        <v>8362878.8059991114</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -1961,9 +1961,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1989,7 +1989,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
@@ -1997,28 +1997,28 @@
         <v>23750.000000037599</v>
       </c>
       <c r="C2">
-        <v>38659.350000427519</v>
+        <v>63516.570000201522</v>
       </c>
       <c r="D2">
-        <v>80404.999999993204</v>
+        <v>89397</v>
       </c>
       <c r="E2">
-        <v>142814.3500004583</v>
+        <v>176663.57000023909</v>
       </c>
       <c r="F2">
-        <v>8999999.9999775514</v>
+        <v>8999905.9942071997</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9295427.7283768877</v>
+        <v>9315465.9063824043</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
@@ -2026,13 +2026,13 @@
         <v>23750.000000037599</v>
       </c>
       <c r="C3">
-        <v>179999.56950031602</v>
+        <v>204111.0729000968</v>
       </c>
       <c r="D3">
-        <v>80404.999999993204</v>
+        <v>89397</v>
       </c>
       <c r="E3">
-        <v>284154.56950034678</v>
+        <v>317258.07290013437</v>
       </c>
       <c r="F3">
         <v>8229999.9999991106</v>
@@ -2041,7 +2041,7 @@
         <v>1</v>
       </c>
       <c r="H3">
-        <v>8642167.4919991121</v>
+        <v>8639818.2239991091</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -2058,9 +2058,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2086,7 +2086,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
@@ -2094,33 +2094,33 @@
         <v>23750.000000037599</v>
       </c>
       <c r="C2">
-        <v>38659.350000427519</v>
+        <v>63516.570000201522</v>
       </c>
       <c r="D2">
-        <v>80404.999999993204</v>
+        <v>89397</v>
       </c>
       <c r="E2">
-        <v>142814.3500004583</v>
+        <v>176663.57000023909</v>
       </c>
       <c r="F2">
-        <v>8999999.9999775514</v>
+        <v>8999905.9942071997</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9271363.384376891</v>
+        <v>9315465.9063824043</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
       <c r="B3">
-        <v>9.0604259869818987E-12</v>
+        <v>2.1140993969624428E-11</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -2129,16 +2129,16 @@
         <v>0</v>
       </c>
       <c r="E3">
-        <v>9.0604259869818987E-12</v>
+        <v>2.1140993969624428E-11</v>
       </c>
       <c r="F3">
-        <v>8526633.0356878955</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>8766551.5236878935</v>
+        <v>8469478.9159991127</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -2155,9 +2155,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2183,7 +2183,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
@@ -2191,33 +2191,33 @@
         <v>23750.000000037599</v>
       </c>
       <c r="C2">
-        <v>38659.350000427519</v>
+        <v>63516.570000201522</v>
       </c>
       <c r="D2">
-        <v>80404.999999993204</v>
+        <v>89397</v>
       </c>
       <c r="E2">
-        <v>142814.3500004583</v>
+        <v>176663.57000023909</v>
       </c>
       <c r="F2">
-        <v>8999999.9999775514</v>
+        <v>8999905.9942071997</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9286084.1643768903</v>
+        <v>9315465.9063824043</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
       <c r="B3">
-        <v>9.0604259869818987E-12</v>
+        <v>2.1140993969624428E-11</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -2226,16 +2226,16 @@
         <v>0</v>
       </c>
       <c r="E3">
-        <v>9.0604259869818987E-12</v>
+        <v>2.1140993969624428E-11</v>
       </c>
       <c r="F3">
-        <v>8944580.1798860673</v>
+        <v>8630866.5194425788</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>9118856.8538860679</v>
+        <v>8805455.7494425774</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -2252,9 +2252,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2280,7 +2280,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
@@ -2288,28 +2288,28 @@
         <v>23750.000000037599</v>
       </c>
       <c r="C2">
-        <v>232659.35000003106</v>
+        <v>257516.56999980501</v>
       </c>
       <c r="D2">
-        <v>80404.999999993204</v>
+        <v>89397</v>
       </c>
       <c r="E2">
-        <v>336814.35000006185</v>
+        <v>370663.56999984261</v>
       </c>
       <c r="F2">
-        <v>8999999.9999775514</v>
+        <v>8999905.9942071997</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9284462.0563768893</v>
+        <v>9315465.9063824043</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
@@ -2317,13 +2317,13 @@
         <v>23750.000000037599</v>
       </c>
       <c r="C3">
-        <v>240622.22550420259</v>
+        <v>243757.67290398461</v>
       </c>
       <c r="D3">
-        <v>80404.999999993204</v>
+        <v>89397</v>
       </c>
       <c r="E3">
-        <v>344777.22550423339</v>
+        <v>356904.67290402221</v>
       </c>
       <c r="F3">
         <v>8229999.9999991106</v>
@@ -2332,7 +2332,7 @@
         <v>1</v>
       </c>
       <c r="H3">
-        <v>8365993.451999112</v>
+        <v>8366493.4259991096</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -2349,9 +2349,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2377,7 +2377,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
@@ -2385,28 +2385,28 @@
         <v>23750.000000037599</v>
       </c>
       <c r="C2">
-        <v>38659.350000427519</v>
+        <v>63516.570000201522</v>
       </c>
       <c r="D2">
-        <v>80404.999999993204</v>
+        <v>89397</v>
       </c>
       <c r="E2">
-        <v>142814.3500004583</v>
+        <v>176663.57000023909</v>
       </c>
       <c r="F2">
-        <v>8999999.9999775514</v>
+        <v>8999905.9942071997</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9265566.8143768925</v>
+        <v>9315465.9063824043</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
@@ -2417,10 +2417,10 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <v>19064.350000219743</v>
+        <v>52913.570000000538</v>
       </c>
       <c r="E3">
-        <v>42814.350000257342</v>
+        <v>76663.570000038133</v>
       </c>
       <c r="F3">
         <v>8229999.9999991106</v>
@@ -2429,7 +2429,7 @@
         <v>1</v>
       </c>
       <c r="H3">
-        <v>8380529.0259991111</v>
+        <v>8380597.6699991105</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -2446,9 +2446,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2474,7 +2474,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
@@ -2482,28 +2482,28 @@
         <v>23750.000000037599</v>
       </c>
       <c r="C2">
-        <v>232659.35000003106</v>
+        <v>257516.56999980501</v>
       </c>
       <c r="D2">
-        <v>80404.999999993204</v>
+        <v>89397</v>
       </c>
       <c r="E2">
-        <v>336814.35000006185</v>
+        <v>370663.56999984261</v>
       </c>
       <c r="F2">
-        <v>8999999.9999775514</v>
+        <v>8999905.9942071997</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9285977.6823768876</v>
+        <v>9315465.9063824043</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
@@ -2514,19 +2514,19 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <v>13064.350000232018</v>
+        <v>46913.570000012776</v>
       </c>
       <c r="E3">
-        <v>36814.350000269616</v>
+        <v>70663.570000050371</v>
       </c>
       <c r="F3">
-        <v>8750166.6880306825</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>8938316.5200306848</v>
+        <v>8417833.5499991123</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -2543,9 +2543,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2571,7 +2571,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
@@ -2579,28 +2579,28 @@
         <v>23750.000000037599</v>
       </c>
       <c r="C2">
-        <v>232659.35000003106</v>
+        <v>257516.56999980501</v>
       </c>
       <c r="D2">
-        <v>80404.999999993204</v>
+        <v>89397</v>
       </c>
       <c r="E2">
-        <v>336814.35000006185</v>
+        <v>370663.56999984261</v>
       </c>
       <c r="F2">
-        <v>8999999.9999775514</v>
+        <v>8999905.9942071997</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9259876.7743768897</v>
+        <v>9315465.9063824043</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
@@ -2611,10 +2611,10 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <v>13064.350000232018</v>
+        <v>46913.570000012776</v>
       </c>
       <c r="E3">
-        <v>36814.350000269616</v>
+        <v>70663.570000050371</v>
       </c>
       <c r="F3">
         <v>8999999.9999775533</v>
@@ -2623,7 +2623,7 @@
         <v>1</v>
       </c>
       <c r="H3">
-        <v>9088056.6489048041</v>
+        <v>9088058.5399775542</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -2640,9 +2640,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2668,7 +2668,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
@@ -2676,28 +2676,28 @@
         <v>23750.000000037599</v>
       </c>
       <c r="C2">
-        <v>614659.35000002873</v>
+        <v>639516.56999980274</v>
       </c>
       <c r="D2">
-        <v>80404.999999993204</v>
+        <v>89397</v>
       </c>
       <c r="E2">
-        <v>718814.35000005946</v>
+        <v>752663.56999984034</v>
       </c>
       <c r="F2">
-        <v>8999999.9999775514</v>
+        <v>8999905.9942071997</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9241904.838376889</v>
+        <v>9315465.9063824043</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
@@ -2705,25 +2705,25 @@
         <v>23750.000000037599</v>
       </c>
       <c r="C3">
-        <v>614659.35000002873</v>
+        <v>523331.0728996137</v>
       </c>
       <c r="D3">
-        <v>80404.999999993204</v>
+        <v>89397</v>
       </c>
       <c r="E3">
-        <v>718814.35000005946</v>
+        <v>636478.07289965136</v>
       </c>
       <c r="F3">
-        <v>8999999.9999775533</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>9186800.7719775531</v>
+        <v>8417857.7959991079</v>
       </c>
       <c r="I3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2737,9 +2737,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2765,7 +2765,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
@@ -2773,28 +2773,28 @@
         <v>23750.000000037599</v>
       </c>
       <c r="C2">
-        <v>232659.35000003106</v>
+        <v>257516.56999980501</v>
       </c>
       <c r="D2">
-        <v>80404.999999993204</v>
+        <v>89397</v>
       </c>
       <c r="E2">
-        <v>336814.35000006185</v>
+        <v>370663.56999984261</v>
       </c>
       <c r="F2">
-        <v>8999999.9999775514</v>
+        <v>8999905.9942071997</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9251313.4483768884</v>
+        <v>9315465.9063824043</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
@@ -2802,13 +2802,13 @@
         <v>23750.000000037599</v>
       </c>
       <c r="C3">
-        <v>510679.56949983269</v>
+        <v>534791.07289961353</v>
       </c>
       <c r="D3">
-        <v>80404.999999993204</v>
+        <v>89397</v>
       </c>
       <c r="E3">
-        <v>614834.56949986354</v>
+        <v>647938.07289965113</v>
       </c>
       <c r="F3">
         <v>8999999.9999775533</v>
@@ -2817,7 +2817,7 @@
         <v>1</v>
       </c>
       <c r="H3">
-        <v>9147827.1659775525</v>
+        <v>9148032.6279775538</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -2834,9 +2834,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2862,7 +2862,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
@@ -2870,28 +2870,28 @@
         <v>23750.000000037599</v>
       </c>
       <c r="C2">
-        <v>614659.35000002873</v>
+        <v>639516.56999980274</v>
       </c>
       <c r="D2">
-        <v>80404.999999993204</v>
+        <v>89397</v>
       </c>
       <c r="E2">
-        <v>718814.35000005946</v>
+        <v>752663.56999984034</v>
       </c>
       <c r="F2">
-        <v>8999999.9999775514</v>
+        <v>8999905.9942071997</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9338103.5363768917</v>
+        <v>9315465.9063824043</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
@@ -2899,13 +2899,13 @@
         <v>23750.000000037599</v>
       </c>
       <c r="C3">
-        <v>499219.56949983287</v>
+        <v>523331.0728996137</v>
       </c>
       <c r="D3">
-        <v>80404.999999993204</v>
+        <v>89397</v>
       </c>
       <c r="E3">
-        <v>603374.56949986366</v>
+        <v>636478.07289965136</v>
       </c>
       <c r="F3">
         <v>8999999.9999775533</v>
@@ -2914,7 +2914,7 @@
         <v>1</v>
       </c>
       <c r="H3">
-        <v>9223577.1819775533</v>
+        <v>9224903.3319775537</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -2931,9 +2931,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2959,7 +2959,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
@@ -2967,28 +2967,28 @@
         <v>23750.000000037599</v>
       </c>
       <c r="C2">
-        <v>614659.35000002873</v>
+        <v>639516.56999980274</v>
       </c>
       <c r="D2">
-        <v>80404.999999993204</v>
+        <v>89397</v>
       </c>
       <c r="E2">
-        <v>718814.35000005946</v>
+        <v>752663.56999984034</v>
       </c>
       <c r="F2">
-        <v>8999999.9999775514</v>
+        <v>8999905.9942071997</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9306934.5663768891</v>
+        <v>9315465.9063824043</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
@@ -2996,13 +2996,13 @@
         <v>23750.000000037599</v>
       </c>
       <c r="C3">
-        <v>881219.56949983037</v>
+        <v>905331.0728996112</v>
       </c>
       <c r="D3">
-        <v>80404.999999993204</v>
+        <v>89397</v>
       </c>
       <c r="E3">
-        <v>985374.5694998611</v>
+        <v>1018478.0728996487</v>
       </c>
       <c r="F3">
         <v>8229999.9999991106</v>
@@ -3011,7 +3011,7 @@
         <v>1</v>
       </c>
       <c r="H3">
-        <v>8515309.8079991098</v>
+        <v>8521307.2019991111</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -3028,9 +3028,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -3056,7 +3056,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
@@ -3064,28 +3064,28 @@
         <v>23750.000000037599</v>
       </c>
       <c r="C2">
-        <v>614659.35000002873</v>
+        <v>639516.56999980274</v>
       </c>
       <c r="D2">
-        <v>80404.999999993204</v>
+        <v>89397</v>
       </c>
       <c r="E2">
-        <v>718814.35000005946</v>
+        <v>752663.56999984034</v>
       </c>
       <c r="F2">
-        <v>8999999.9999775514</v>
+        <v>8999905.9942071997</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9280548.6223768909</v>
+        <v>9315465.9063824043</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
@@ -3093,13 +3093,13 @@
         <v>23750.000000037599</v>
       </c>
       <c r="C3">
-        <v>881219.56949983037</v>
+        <v>905331.0728996112</v>
       </c>
       <c r="D3">
-        <v>80404.999999993204</v>
+        <v>89397</v>
       </c>
       <c r="E3">
-        <v>985374.5694998611</v>
+        <v>1018478.0728996487</v>
       </c>
       <c r="F3">
         <v>8999999.9999775533</v>
@@ -3108,7 +3108,7 @@
         <v>1</v>
       </c>
       <c r="H3">
-        <v>9259930.4659775551</v>
+        <v>9273849.8819775544</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -3125,9 +3125,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -3153,7 +3153,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
@@ -3161,28 +3161,28 @@
         <v>23750.000000037599</v>
       </c>
       <c r="C2">
-        <v>232659.35000003106</v>
+        <v>257516.56999980501</v>
       </c>
       <c r="D2">
-        <v>80404.999999993204</v>
+        <v>89397</v>
       </c>
       <c r="E2">
-        <v>336814.35000006185</v>
+        <v>370663.56999984261</v>
       </c>
       <c r="F2">
-        <v>8999999.9999775514</v>
+        <v>8999905.9942071997</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9264708.6483768895</v>
+        <v>9315465.9063824043</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
@@ -3190,13 +3190,13 @@
         <v>23750.000000037599</v>
       </c>
       <c r="C3">
-        <v>510679.56949983269</v>
+        <v>534791.07289961353</v>
       </c>
       <c r="D3">
-        <v>80404.999999993204</v>
+        <v>89397</v>
       </c>
       <c r="E3">
-        <v>614834.56949986354</v>
+        <v>647938.07289965113</v>
       </c>
       <c r="F3">
         <v>8999999.9999775533</v>
@@ -3205,7 +3205,7 @@
         <v>1</v>
       </c>
       <c r="H3">
-        <v>9187790.0259775519</v>
+        <v>9210604.3459775522</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -3222,9 +3222,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -3250,7 +3250,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
@@ -3258,28 +3258,28 @@
         <v>23750.000000037599</v>
       </c>
       <c r="C2">
-        <v>329659.350000226</v>
+        <v>354516.57</v>
       </c>
       <c r="D2">
-        <v>80404.999999993204</v>
+        <v>89397</v>
       </c>
       <c r="E2">
-        <v>433814.35000025679</v>
+        <v>467663.57000003767</v>
       </c>
       <c r="F2">
-        <v>8999999.9999775514</v>
+        <v>8999905.9942071997</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9272009.6543768905</v>
+        <v>9315465.9063824043</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
@@ -3287,22 +3287,22 @@
         <v>23750.000000037599</v>
       </c>
       <c r="C3">
-        <v>319769.56950021919</v>
+        <v>343881.07290000003</v>
       </c>
       <c r="D3">
-        <v>80404.999999993204</v>
+        <v>89397</v>
       </c>
       <c r="E3">
-        <v>423924.56950025004</v>
+        <v>457028.07290003763</v>
       </c>
       <c r="F3">
-        <v>8999999.9999775533</v>
+        <v>8914511.5349799581</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>9099952.9999775533</v>
+        <v>9014464.5349799562</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -3319,7 +3319,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3331,9 +3331,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -3359,7 +3359,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
@@ -3367,28 +3367,28 @@
         <v>23750.000000037599</v>
       </c>
       <c r="C2">
-        <v>329659.350000226</v>
+        <v>354516.57</v>
       </c>
       <c r="D2">
-        <v>80404.999999993204</v>
+        <v>89397</v>
       </c>
       <c r="E2">
-        <v>433814.35000025679</v>
+        <v>467663.57000003767</v>
       </c>
       <c r="F2">
-        <v>8999999.9999775514</v>
+        <v>8999905.9942071997</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9238003.5843768921</v>
+        <v>9315465.9063824043</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
@@ -3396,13 +3396,13 @@
         <v>23750.000000037599</v>
       </c>
       <c r="C3">
-        <v>222769.56950002426</v>
+        <v>246881.07289980506</v>
       </c>
       <c r="D3">
-        <v>80404.999999993204</v>
+        <v>89397</v>
       </c>
       <c r="E3">
-        <v>326924.56950005511</v>
+        <v>360028.07289984263</v>
       </c>
       <c r="F3">
         <v>8229999.9999991106</v>
@@ -3411,7 +3411,7 @@
         <v>1</v>
       </c>
       <c r="H3">
-        <v>8261774.3399991104</v>
+        <v>8261744.7299991101</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -3428,9 +3428,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -3456,7 +3456,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
@@ -3464,28 +3464,28 @@
         <v>23750.000000037599</v>
       </c>
       <c r="C2">
-        <v>614659.35000002873</v>
+        <v>639516.56999980274</v>
       </c>
       <c r="D2">
-        <v>80404.999999993204</v>
+        <v>89397</v>
       </c>
       <c r="E2">
-        <v>718814.35000005946</v>
+        <v>752663.56999984034</v>
       </c>
       <c r="F2">
-        <v>8999999.9999775514</v>
+        <v>8999905.9942071997</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9300298.2043768913</v>
+        <v>9315465.9063824043</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
@@ -3493,13 +3493,13 @@
         <v>23750.000000037599</v>
       </c>
       <c r="C3">
-        <v>596219.56950002781</v>
+        <v>620331.07289980864</v>
       </c>
       <c r="D3">
-        <v>80404.999999993204</v>
+        <v>89397</v>
       </c>
       <c r="E3">
-        <v>700374.56950005866</v>
+        <v>733478.07289984624</v>
       </c>
       <c r="F3">
         <v>8229999.9999991106</v>
@@ -3508,7 +3508,7 @@
         <v>1</v>
       </c>
       <c r="H3">
-        <v>8291216.4199991124</v>
+        <v>8291125.7399991108</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -3525,9 +3525,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -3553,7 +3553,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
@@ -3561,28 +3561,28 @@
         <v>23750.000000037599</v>
       </c>
       <c r="C2">
-        <v>329659.350000226</v>
+        <v>354516.57</v>
       </c>
       <c r="D2">
-        <v>80404.999999993204</v>
+        <v>89397</v>
       </c>
       <c r="E2">
-        <v>433814.35000025679</v>
+        <v>467663.57000003767</v>
       </c>
       <c r="F2">
-        <v>8999999.9999775514</v>
+        <v>8999905.9942071997</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9278822.59437689</v>
+        <v>9315465.9063824043</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
@@ -3590,13 +3590,13 @@
         <v>23750.000000037599</v>
       </c>
       <c r="C3">
-        <v>604769.56950002187</v>
+        <v>628881.07289980259</v>
       </c>
       <c r="D3">
-        <v>80404.999999993204</v>
+        <v>89397</v>
       </c>
       <c r="E3">
-        <v>708924.56950005272</v>
+        <v>742028.07289984031</v>
       </c>
       <c r="F3">
         <v>8999999.9999775533</v>
@@ -3622,9 +3622,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -3650,7 +3650,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
@@ -3658,28 +3658,28 @@
         <v>23750.000000037599</v>
       </c>
       <c r="C2">
-        <v>232659.35000003106</v>
+        <v>257516.56999980501</v>
       </c>
       <c r="D2">
-        <v>80404.999999993204</v>
+        <v>89397</v>
       </c>
       <c r="E2">
-        <v>336814.35000006185</v>
+        <v>370663.56999984261</v>
       </c>
       <c r="F2">
-        <v>8999999.9999775514</v>
+        <v>8999905.9942071997</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9291552.964376891</v>
+        <v>9315465.9063824043</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
@@ -3687,25 +3687,25 @@
         <v>23750.000000037599</v>
       </c>
       <c r="C3">
-        <v>232659.35000003106</v>
+        <v>249791.07289981085</v>
       </c>
       <c r="D3">
-        <v>80404.999999993204</v>
+        <v>89397</v>
       </c>
       <c r="E3">
-        <v>336814.35000006185</v>
+        <v>362938.07289984846</v>
       </c>
       <c r="F3">
-        <v>8855121.830367364</v>
+        <v>8628816.3028154261</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>9039071.5503673628</v>
+        <v>8812766.0228154249</v>
       </c>
       <c r="I3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -3719,9 +3719,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -3747,7 +3747,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
@@ -3755,28 +3755,28 @@
         <v>23750.000000037599</v>
       </c>
       <c r="C2">
-        <v>38659.350000427519</v>
+        <v>63516.570000201522</v>
       </c>
       <c r="D2">
-        <v>80404.999999993204</v>
+        <v>89397</v>
       </c>
       <c r="E2">
-        <v>142814.3500004583</v>
+        <v>176663.57000023909</v>
       </c>
       <c r="F2">
-        <v>8999999.9999775514</v>
+        <v>8999905.9942071997</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9285161.1243768912</v>
+        <v>9315465.9063824043</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
@@ -3787,10 +3787,10 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <v>19064.350000219743</v>
+        <v>52913.570000000538</v>
       </c>
       <c r="E3">
-        <v>42814.350000257342</v>
+        <v>76663.570000038133</v>
       </c>
       <c r="F3">
         <v>8999999.9999775533</v>
@@ -3816,9 +3816,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -3844,7 +3844,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43101</v>
       </c>
@@ -3852,28 +3852,28 @@
         <v>23750.000000037599</v>
       </c>
       <c r="C2">
-        <v>232659.35000003106</v>
+        <v>257516.56999980501</v>
       </c>
       <c r="D2">
-        <v>80404.999999993204</v>
+        <v>89397</v>
       </c>
       <c r="E2">
-        <v>336814.35000006185</v>
+        <v>370663.56999984261</v>
       </c>
       <c r="F2">
-        <v>8999999.9999775514</v>
+        <v>8999905.9942071997</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9266173.9143768903</v>
+        <v>9315465.9063824043</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43466</v>
       </c>
@@ -3884,10 +3884,10 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <v>13064.350000232018</v>
+        <v>46913.570000012776</v>
       </c>
       <c r="E3">
-        <v>36814.350000269616</v>
+        <v>70663.570000050371</v>
       </c>
       <c r="F3">
         <v>8999999.9999775533</v>
@@ -3896,7 +3896,7 @@
         <v>1</v>
       </c>
       <c r="H3">
-        <v>9186274.0599775538</v>
+        <v>9186027.3499775529</v>
       </c>
       <c r="I3">
         <v>0</v>

</xml_diff>

<commit_message>
November 2018 Unofficial Model Run includes update to CBRFC forecasts and model output files. No model or ruleset changes since last commit.
</commit_message>
<xml_diff>
--- a/Output Data/MtomToCrss_Annual.xlsx
+++ b/Output Data/MtomToCrss_Annual.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\MTOM\Output Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\MTOM\dev\Output Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="1470"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12570" windowHeight="13590"/>
   </bookViews>
   <sheets>
     <sheet name="Trace38" sheetId="37" r:id="rId1"/>
@@ -460,7 +460,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9315465.9063824043</v>
+        <v>9315862.6005992647</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -474,22 +474,22 @@
         <v>23750.000000037599</v>
       </c>
       <c r="C3">
-        <v>55577.672904369225</v>
+        <v>75719.528904368795</v>
       </c>
       <c r="D3">
         <v>89397</v>
       </c>
       <c r="E3">
-        <v>168724.67290440682</v>
+        <v>188866.52890440638</v>
       </c>
       <c r="F3">
-        <v>8229999.9999991106</v>
+        <v>8229999.9999999981</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>8340981.0259991111</v>
+        <v>8382461.3600577824</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -557,7 +557,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9315465.9063824043</v>
+        <v>9315862.6005992647</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -580,13 +580,13 @@
         <v>636478.07289965136</v>
       </c>
       <c r="F3">
-        <v>8229999.9999991106</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>8396147.9299991112</v>
+        <v>9196913.5740353391</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -654,7 +654,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9315465.9063824043</v>
+        <v>9315862.6005992647</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -677,13 +677,13 @@
         <v>880253.0728997445</v>
       </c>
       <c r="F3">
-        <v>8874579.3446566537</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>9138485.624656653</v>
+        <v>9295759.3240353372</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -751,7 +751,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9315465.9063824043</v>
+        <v>9315862.6005992647</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -774,13 +774,13 @@
         <v>599528.07289993903</v>
       </c>
       <c r="F3">
-        <v>8229999.9999991106</v>
+        <v>8229999.9999999981</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>8359167.7799991118</v>
+        <v>8409652.7440577839</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -848,7 +848,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9315465.9063824043</v>
+        <v>9315862.6005992647</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -871,13 +871,13 @@
         <v>595253.07289994194</v>
       </c>
       <c r="F3">
-        <v>8229999.9999991106</v>
+        <v>8772637.3478710875</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>8334398.0899991114</v>
+        <v>8917508.7719288729</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -945,7 +945,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9315465.9063824043</v>
+        <v>9315862.6005992647</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -968,13 +968,13 @@
         <v>505438.07289974985</v>
       </c>
       <c r="F3">
-        <v>8738263.7609513756</v>
+        <v>8229999.9999999981</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>8869911.2009513751</v>
+        <v>8404937.7940577827</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -1042,7 +1042,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9315465.9063824043</v>
+        <v>9315862.6005992647</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -1065,13 +1065,13 @@
         <v>265938.07289965352</v>
       </c>
       <c r="F3">
-        <v>8229999.9999991106</v>
+        <v>8229999.9999999981</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>8338713.64999911</v>
+        <v>8384084.7640577815</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -1139,7 +1139,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9315465.9063824043</v>
+        <v>9315862.6005992647</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -1162,13 +1162,13 @@
         <v>498253.07289974694</v>
       </c>
       <c r="F3">
-        <v>8229999.9999991106</v>
+        <v>8229999.9999999981</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>8335477.6799991112</v>
+        <v>8373740.0240577832</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -1236,7 +1236,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9315465.9063824043</v>
+        <v>9315862.6005992647</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -1259,13 +1259,13 @@
         <v>875978.07289974764</v>
       </c>
       <c r="F3">
-        <v>8229999.9999991106</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>8370628.0299991099</v>
+        <v>9179659.4840353373</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -1333,7 +1333,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9315465.9063824043</v>
+        <v>9315862.6005992647</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -1347,22 +1347,22 @@
         <v>23750.000000037599</v>
       </c>
       <c r="C3">
-        <v>905331.0728996112</v>
+        <v>919439.52890378458</v>
       </c>
       <c r="D3">
         <v>89397</v>
       </c>
       <c r="E3">
-        <v>1018478.0728996487</v>
+        <v>1032586.5289038221</v>
       </c>
       <c r="F3">
-        <v>8999999.9999775533</v>
+        <v>8626535.657290794</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>9203484.9599775542</v>
+        <v>8855643.4713485781</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -1430,7 +1430,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9315465.9063824043</v>
+        <v>9315862.6005992647</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -1453,13 +1453,13 @@
         <v>1018478.0728996487</v>
       </c>
       <c r="F3">
-        <v>8739170.2718241215</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>8649542.7818241194</v>
+        <v>8968184.204035338</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -1527,7 +1527,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9315465.9063824043</v>
+        <v>9315862.6005992647</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -1550,13 +1550,13 @@
         <v>2.1140993969624428E-11</v>
       </c>
       <c r="F3">
-        <v>8229999.9999991106</v>
+        <v>8737151.7454127055</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>8365931.8499991121</v>
+        <v>8908334.2294704895</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -1624,7 +1624,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9315465.9063824043</v>
+        <v>9315862.6005992647</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -1653,7 +1653,7 @@
         <v>1</v>
       </c>
       <c r="H3">
-        <v>9061671.6859775539</v>
+        <v>9105269.704035338</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -1721,7 +1721,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9315465.9063824043</v>
+        <v>9315862.6005992647</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -1750,7 +1750,7 @@
         <v>1</v>
       </c>
       <c r="H3">
-        <v>9128518.731977554</v>
+        <v>9166368.9920353387</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -1818,7 +1818,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9315465.9063824043</v>
+        <v>9315862.6005992647</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -1841,13 +1841,13 @@
         <v>459758.07290003583</v>
       </c>
       <c r="F3">
-        <v>8229999.9999991106</v>
+        <v>8229999.9999999981</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>8512420.3039991111</v>
+        <v>8550902.8760577813</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -1915,7 +1915,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9315465.9063824043</v>
+        <v>9315862.6005992647</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -1938,13 +1938,13 @@
         <v>304253.07290014339</v>
       </c>
       <c r="F3">
-        <v>8229999.9999991106</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>8362878.8059991114</v>
+        <v>9171027.6120353378</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -2012,7 +2012,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9315465.9063824043</v>
+        <v>9315862.6005992647</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -2035,13 +2035,13 @@
         <v>317258.07290013437</v>
       </c>
       <c r="F3">
-        <v>8229999.9999991106</v>
+        <v>8229999.9999999981</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>8639818.2239991091</v>
+        <v>8671869.3440577816</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -2109,7 +2109,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9315465.9063824043</v>
+        <v>9315862.6005992647</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -2132,13 +2132,13 @@
         <v>2.1140993969624428E-11</v>
       </c>
       <c r="F3">
-        <v>8229999.9999991106</v>
+        <v>8229999.9999999981</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>8469478.9159991127</v>
+        <v>8510853.7240577824</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -2206,7 +2206,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9315465.9063824043</v>
+        <v>9315862.6005992647</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -2229,13 +2229,13 @@
         <v>2.1140993969624428E-11</v>
       </c>
       <c r="F3">
-        <v>8630866.5194425788</v>
+        <v>8229999.9999999981</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>8805455.7494425774</v>
+        <v>8449825.4580577817</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -2303,7 +2303,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9315465.9063824043</v>
+        <v>9315862.6005992647</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -2317,22 +2317,22 @@
         <v>23750.000000037599</v>
       </c>
       <c r="C3">
-        <v>243757.67290398461</v>
+        <v>263899.52890398417</v>
       </c>
       <c r="D3">
         <v>89397</v>
       </c>
       <c r="E3">
-        <v>356904.67290402221</v>
+        <v>377046.52890402172</v>
       </c>
       <c r="F3">
-        <v>8229999.9999991106</v>
+        <v>8366132.5451393249</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>8366493.4259991096</v>
+        <v>8539234.8991971128</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -2400,7 +2400,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9315465.9063824043</v>
+        <v>9315862.6005992647</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -2423,13 +2423,13 @@
         <v>76663.570000038133</v>
       </c>
       <c r="F3">
-        <v>8229999.9999991106</v>
+        <v>8564528.281613294</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>8380597.6699991105</v>
+        <v>8745731.51567108</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -2497,7 +2497,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9315465.9063824043</v>
+        <v>9315862.6005992647</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -2520,13 +2520,13 @@
         <v>70663.570000050371</v>
       </c>
       <c r="F3">
-        <v>8229999.9999991106</v>
+        <v>8229999.9999999981</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>8417833.5499991123</v>
+        <v>8452673.5360577814</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -2594,7 +2594,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9315465.9063824043</v>
+        <v>9315862.6005992647</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -2617,13 +2617,13 @@
         <v>70663.570000050371</v>
       </c>
       <c r="F3">
-        <v>8999999.9999775533</v>
+        <v>8229999.9999999981</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>9088058.5399775542</v>
+        <v>8365743.0240577832</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -2691,7 +2691,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9315465.9063824043</v>
+        <v>9315862.6005992647</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -2714,13 +2714,13 @@
         <v>636478.07289965136</v>
       </c>
       <c r="F3">
-        <v>8229999.9999991106</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>8417857.7959991079</v>
+        <v>9220479.9720353391</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -2788,7 +2788,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9315465.9063824043</v>
+        <v>9315862.6005992647</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -2817,7 +2817,7 @@
         <v>1</v>
       </c>
       <c r="H3">
-        <v>9148032.6279775538</v>
+        <v>9182721.3480353393</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -2885,7 +2885,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9315465.9063824043</v>
+        <v>9315862.6005992647</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -2914,7 +2914,7 @@
         <v>1</v>
       </c>
       <c r="H3">
-        <v>9224903.3319775537</v>
+        <v>9253869.5300353374</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -2982,7 +2982,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9315465.9063824043</v>
+        <v>9315862.6005992647</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -3005,13 +3005,13 @@
         <v>1018478.0728996487</v>
       </c>
       <c r="F3">
-        <v>8229999.9999991106</v>
+        <v>8229999.9999999981</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>8521307.2019991111</v>
+        <v>8544080.4700577836</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -3079,7 +3079,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9315465.9063824043</v>
+        <v>9315862.6005992647</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -3108,7 +3108,7 @@
         <v>1</v>
       </c>
       <c r="H3">
-        <v>9273849.8819775544</v>
+        <v>9322938.8360353373</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -3176,7 +3176,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9315465.9063824043</v>
+        <v>9315862.6005992647</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -3199,13 +3199,13 @@
         <v>647938.07289965113</v>
       </c>
       <c r="F3">
-        <v>8999999.9999775533</v>
+        <v>8229999.9999999981</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>9210604.3459775522</v>
+        <v>8477489.750057783</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -3273,7 +3273,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9315465.9063824043</v>
+        <v>9315862.6005992647</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -3296,13 +3296,13 @@
         <v>457028.07290003763</v>
       </c>
       <c r="F3">
-        <v>8914511.5349799581</v>
+        <v>8854562.1209468655</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>9014464.5349799562</v>
+        <v>8998832.8250046521</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -3382,7 +3382,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9315465.9063824043</v>
+        <v>9315862.6005992647</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -3405,13 +3405,13 @@
         <v>360028.07289984263</v>
       </c>
       <c r="F3">
-        <v>8229999.9999991106</v>
+        <v>8229999.9999999981</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>8261744.7299991101</v>
+        <v>8314596.0640577823</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -3479,7 +3479,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9315465.9063824043</v>
+        <v>9315862.6005992647</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -3502,13 +3502,13 @@
         <v>733478.07289984624</v>
       </c>
       <c r="F3">
-        <v>8229999.9999991106</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>8291125.7399991108</v>
+        <v>9087757.4640353378</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -3576,7 +3576,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9315465.9063824043</v>
+        <v>9315862.6005992647</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -3599,13 +3599,13 @@
         <v>742028.07289984031</v>
       </c>
       <c r="F3">
-        <v>8999999.9999775533</v>
+        <v>8511829.9610227067</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>9212695.0099775549</v>
+        <v>8767557.2750804927</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -3673,7 +3673,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9315465.9063824043</v>
+        <v>9315862.6005992647</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -3696,13 +3696,13 @@
         <v>362938.07289984846</v>
       </c>
       <c r="F3">
-        <v>8628816.3028154261</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>8812766.0228154249</v>
+        <v>9219887.1840353366</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -3770,7 +3770,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9315465.9063824043</v>
+        <v>9315862.6005992647</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -3799,7 +3799,7 @@
         <v>1</v>
       </c>
       <c r="H3">
-        <v>9160152.0699775536</v>
+        <v>9196925.9240353368</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -3867,7 +3867,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>9315465.9063824043</v>
+        <v>9315862.6005992647</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -3890,13 +3890,13 @@
         <v>70663.570000050371</v>
       </c>
       <c r="F3">
-        <v>8999999.9999775533</v>
+        <v>8229999.9999999981</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>9186027.3499775529</v>
+        <v>8455034.3440577816</v>
       </c>
       <c r="I3">
         <v>0</v>

</xml_diff>

<commit_message>
December 2018 Unofficial Model Run includes update to CBRFC forecasts and model output files. No model or ruleset changes since last commit.
</commit_message>
<xml_diff>
--- a/Output Data/MtomToCrss_Annual.xlsx
+++ b/Output Data/MtomToCrss_Annual.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\MTOM\dev\Output Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\D_Drive\Modeling\MTOM_Production\_DEC18_Post-MTOM-dev\Output Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12570" windowHeight="13590"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12840" windowHeight="13530"/>
   </bookViews>
   <sheets>
     <sheet name="Trace38" sheetId="37" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="9">
   <si>
     <t>ICS Credits.BiNationalICS_CA</t>
   </si>
@@ -75,6 +75,9 @@
   </si>
   <si>
     <t>PowellOperation.PowellWYRelease</t>
+  </si>
+  <si>
+    <t>NaN</t>
   </si>
   <si>
     <t>SystemConditions.PowellRelTier</t>
@@ -428,13 +431,13 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -442,25 +445,25 @@
         <v>43101</v>
       </c>
       <c r="B2">
-        <v>23750.000000037599</v>
+        <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>63516.570000201522</v>
+        <v>468162.81999999995</v>
       </c>
       <c r="D2">
         <v>89397</v>
       </c>
       <c r="E2">
-        <v>176663.57000023909</v>
-      </c>
-      <c r="F2">
-        <v>8999905.9942071997</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>9315862.6005992647</v>
+        <v>605059.82000007527</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" t="s">
+        <v>5</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -471,25 +474,25 @@
         <v>43466</v>
       </c>
       <c r="B3">
-        <v>23750.000000037599</v>
+        <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>75719.528904368795</v>
+        <v>358617.98539980501</v>
       </c>
       <c r="D3">
         <v>89397</v>
       </c>
       <c r="E3">
-        <v>188866.52890440638</v>
+        <v>495514.98539988021</v>
       </c>
       <c r="F3">
-        <v>8229999.9999999981</v>
+        <v>8229999.9999999953</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>8382461.3600577824</v>
+        <v>8388765.7051400952</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -525,13 +528,13 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -539,25 +542,25 @@
         <v>43101</v>
       </c>
       <c r="B2">
-        <v>23750.000000037599</v>
+        <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>639516.56999980274</v>
+        <v>468162.81999999995</v>
       </c>
       <c r="D2">
         <v>89397</v>
       </c>
       <c r="E2">
-        <v>752663.56999984034</v>
-      </c>
-      <c r="F2">
-        <v>8999905.9942071997</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>9315862.6005992647</v>
+        <v>605059.82000007527</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" t="s">
+        <v>5</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -568,25 +571,25 @@
         <v>43466</v>
       </c>
       <c r="B3">
-        <v>23750.000000037599</v>
+        <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>523331.0728996137</v>
+        <v>358617.98539980501</v>
       </c>
       <c r="D3">
         <v>89397</v>
       </c>
       <c r="E3">
-        <v>636478.07289965136</v>
+        <v>495514.98539988021</v>
       </c>
       <c r="F3">
-        <v>8999999.9999775533</v>
+        <v>8948862.0448640604</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>9196913.5740353391</v>
+        <v>9136078.9540041573</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -622,13 +625,13 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -636,25 +639,25 @@
         <v>43101</v>
       </c>
       <c r="B2">
-        <v>23750.000000037599</v>
+        <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>497016.56999990129</v>
+        <v>468162.81999999995</v>
       </c>
       <c r="D2">
         <v>89397</v>
       </c>
       <c r="E2">
-        <v>610163.56999993895</v>
-      </c>
-      <c r="F2">
-        <v>8999905.9942071997</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>9315862.6005992647</v>
+        <v>605059.82000007527</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" t="s">
+        <v>5</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -665,25 +668,25 @@
         <v>43466</v>
       </c>
       <c r="B3">
-        <v>23750.000000037599</v>
+        <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>767106.07289970689</v>
+        <v>740617.98539980256</v>
       </c>
       <c r="D3">
         <v>89397</v>
       </c>
       <c r="E3">
-        <v>880253.0728997445</v>
+        <v>877514.98539987789</v>
       </c>
       <c r="F3">
-        <v>8999999.9999775533</v>
+        <v>8999999.9999775514</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>9295759.3240353372</v>
+        <v>9292478.2691176515</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -719,13 +722,13 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -733,25 +736,25 @@
         <v>43101</v>
       </c>
       <c r="B2">
-        <v>23750.000000037599</v>
+        <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>354516.57</v>
+        <v>468162.81999999995</v>
       </c>
       <c r="D2">
         <v>89397</v>
       </c>
       <c r="E2">
-        <v>467663.57000003767</v>
-      </c>
-      <c r="F2">
-        <v>8999905.9942071997</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>9315862.6005992647</v>
+        <v>605059.82000007527</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" t="s">
+        <v>5</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -762,25 +765,25 @@
         <v>43466</v>
       </c>
       <c r="B3">
-        <v>23750.000000037599</v>
+        <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>486381.07289990137</v>
+        <v>598117.98539990128</v>
       </c>
       <c r="D3">
         <v>89397</v>
       </c>
       <c r="E3">
-        <v>599528.07289993903</v>
+        <v>735014.98539997661</v>
       </c>
       <c r="F3">
-        <v>8229999.9999999981</v>
+        <v>8229999.9999999953</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>8409652.7440577839</v>
+        <v>8408732.8391400948</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -816,13 +819,13 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -830,25 +833,25 @@
         <v>43101</v>
       </c>
       <c r="B2">
-        <v>23750.000000037599</v>
+        <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>497016.56999990129</v>
+        <v>468162.81999999995</v>
       </c>
       <c r="D2">
         <v>89397</v>
       </c>
       <c r="E2">
-        <v>610163.56999993895</v>
-      </c>
-      <c r="F2">
-        <v>8999905.9942071997</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>9315862.6005992647</v>
+        <v>605059.82000007527</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" t="s">
+        <v>5</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -859,25 +862,25 @@
         <v>43466</v>
       </c>
       <c r="B3">
-        <v>23750.000000037599</v>
+        <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>482106.07289990428</v>
+        <v>455617.98539999995</v>
       </c>
       <c r="D3">
         <v>89397</v>
       </c>
       <c r="E3">
-        <v>595253.07289994194</v>
+        <v>592514.98540007521</v>
       </c>
       <c r="F3">
-        <v>8772637.3478710875</v>
+        <v>8740699.6356417686</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>8917508.7719288729</v>
+        <v>8890240.5747818686</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -913,13 +916,13 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -927,25 +930,25 @@
         <v>43101</v>
       </c>
       <c r="B2">
-        <v>23750.000000037599</v>
+        <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>257516.56999980501</v>
+        <v>468162.81999999995</v>
       </c>
       <c r="D2">
         <v>89397</v>
       </c>
       <c r="E2">
-        <v>370663.56999984261</v>
-      </c>
-      <c r="F2">
-        <v>8999905.9942071997</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>9315862.6005992647</v>
+        <v>605059.82000007527</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" t="s">
+        <v>5</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -956,25 +959,25 @@
         <v>43466</v>
       </c>
       <c r="B3">
-        <v>23750.000000037599</v>
+        <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>392291.07289971219</v>
+        <v>598117.98539990128</v>
       </c>
       <c r="D3">
         <v>89397</v>
       </c>
       <c r="E3">
-        <v>505438.07289974985</v>
+        <v>735014.98539997661</v>
       </c>
       <c r="F3">
-        <v>8229999.9999999981</v>
+        <v>8229999.9999999953</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>8404937.7940577827</v>
+        <v>8413596.5091400947</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -1010,13 +1013,13 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1024,25 +1027,25 @@
         <v>43101</v>
       </c>
       <c r="B2">
-        <v>23750.000000037599</v>
+        <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>257516.56999980501</v>
+        <v>468162.81999999995</v>
       </c>
       <c r="D2">
         <v>89397</v>
       </c>
       <c r="E2">
-        <v>370663.56999984261</v>
-      </c>
-      <c r="F2">
-        <v>8999905.9942071997</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>9315862.6005992647</v>
+        <v>605059.82000007527</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" t="s">
+        <v>5</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -1053,25 +1056,25 @@
         <v>43466</v>
       </c>
       <c r="B3">
-        <v>23750.000000037599</v>
+        <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>152791.07289961592</v>
+        <v>358617.98539980501</v>
       </c>
       <c r="D3">
         <v>89397</v>
       </c>
       <c r="E3">
-        <v>265938.07289965352</v>
+        <v>495514.98539988021</v>
       </c>
       <c r="F3">
-        <v>8229999.9999999981</v>
+        <v>8229999.9999999953</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>8384084.7640577815</v>
+        <v>8392216.709140094</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -1107,13 +1110,13 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1121,25 +1124,25 @@
         <v>43101</v>
       </c>
       <c r="B2">
-        <v>23750.000000037599</v>
+        <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>497016.56999990129</v>
+        <v>468162.81999999995</v>
       </c>
       <c r="D2">
         <v>89397</v>
       </c>
       <c r="E2">
-        <v>610163.56999993895</v>
-      </c>
-      <c r="F2">
-        <v>8999905.9942071997</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>9315862.6005992647</v>
+        <v>605059.82000007527</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" t="s">
+        <v>5</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -1150,25 +1153,25 @@
         <v>43466</v>
       </c>
       <c r="B3">
-        <v>23750.000000037599</v>
+        <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>385106.07289970928</v>
+        <v>358617.98539980501</v>
       </c>
       <c r="D3">
         <v>89397</v>
       </c>
       <c r="E3">
-        <v>498253.07289974694</v>
+        <v>495514.98539988021</v>
       </c>
       <c r="F3">
-        <v>8229999.9999999981</v>
+        <v>8989416.0613516401</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>8373740.0240577832</v>
+        <v>9134957.0204917379</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -1204,13 +1207,13 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1218,25 +1221,25 @@
         <v>43101</v>
       </c>
       <c r="B2">
-        <v>23750.000000037599</v>
+        <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>639516.56999980274</v>
+        <v>468162.81999999995</v>
       </c>
       <c r="D2">
         <v>89397</v>
       </c>
       <c r="E2">
-        <v>752663.56999984034</v>
-      </c>
-      <c r="F2">
-        <v>8999905.9942071997</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>9315862.6005992647</v>
+        <v>605059.82000007527</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" t="s">
+        <v>5</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -1247,25 +1250,25 @@
         <v>43466</v>
       </c>
       <c r="B3">
-        <v>23750.000000037599</v>
+        <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>762831.07289970992</v>
+        <v>598117.98539990128</v>
       </c>
       <c r="D3">
         <v>89397</v>
       </c>
       <c r="E3">
-        <v>875978.07289974764</v>
+        <v>735014.98539997661</v>
       </c>
       <c r="F3">
-        <v>8999999.9999775533</v>
+        <v>8999999.9999775514</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>9179659.4840353373</v>
+        <v>9197021.5391176511</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -1301,13 +1304,13 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1315,25 +1318,25 @@
         <v>43101</v>
       </c>
       <c r="B2">
-        <v>23750.000000037599</v>
+        <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>639516.56999980274</v>
+        <v>468162.81999999995</v>
       </c>
       <c r="D2">
         <v>89397</v>
       </c>
       <c r="E2">
-        <v>752663.56999984034</v>
-      </c>
-      <c r="F2">
-        <v>8999905.9942071997</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>9315862.6005992647</v>
+        <v>605059.82000007527</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" t="s">
+        <v>5</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -1344,25 +1347,25 @@
         <v>43466</v>
       </c>
       <c r="B3">
-        <v>23750.000000037599</v>
+        <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>919439.52890378458</v>
+        <v>740617.98539980256</v>
       </c>
       <c r="D3">
         <v>89397</v>
       </c>
       <c r="E3">
-        <v>1032586.5289038221</v>
+        <v>877514.98539987789</v>
       </c>
       <c r="F3">
-        <v>8626535.657290794</v>
+        <v>8533443.8018583804</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>8855643.4713485781</v>
+        <v>8759816.7209984809</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -1398,13 +1401,13 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1412,25 +1415,25 @@
         <v>43101</v>
       </c>
       <c r="B2">
-        <v>23750.000000037599</v>
+        <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>639516.56999980274</v>
+        <v>468162.81999999995</v>
       </c>
       <c r="D2">
         <v>89397</v>
       </c>
       <c r="E2">
-        <v>752663.56999984034</v>
-      </c>
-      <c r="F2">
-        <v>8999905.9942071997</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>9315862.6005992647</v>
+        <v>605059.82000007527</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" t="s">
+        <v>5</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -1441,25 +1444,25 @@
         <v>43466</v>
       </c>
       <c r="B3">
-        <v>23750.000000037599</v>
+        <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>905331.0728996112</v>
+        <v>740617.98539980256</v>
       </c>
       <c r="D3">
         <v>89397</v>
       </c>
       <c r="E3">
-        <v>1018478.0728996487</v>
+        <v>877514.98539987789</v>
       </c>
       <c r="F3">
-        <v>8999999.9999775533</v>
+        <v>8999999.9999775514</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>8968184.204035338</v>
+        <v>8992754.249117652</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -1495,13 +1498,13 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1509,25 +1512,25 @@
         <v>43101</v>
       </c>
       <c r="B2">
-        <v>23750.000000037599</v>
+        <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>63516.570000201522</v>
+        <v>468162.81999999995</v>
       </c>
       <c r="D2">
         <v>89397</v>
       </c>
       <c r="E2">
-        <v>176663.57000023909</v>
-      </c>
-      <c r="F2">
-        <v>8999905.9942071997</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>9315862.6005992647</v>
+        <v>605059.82000007527</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" t="s">
+        <v>5</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -1538,25 +1541,25 @@
         <v>43466</v>
       </c>
       <c r="B3">
-        <v>2.1140993969624428E-11</v>
+        <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>164617.98540020152</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>89397</v>
       </c>
       <c r="E3">
-        <v>2.1140993969624428E-11</v>
+        <v>301514.98540027672</v>
       </c>
       <c r="F3">
-        <v>8737151.7454127055</v>
+        <v>8863769.7982449085</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>8908334.2294704895</v>
+        <v>9044296.1673850119</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -1592,13 +1595,13 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1606,25 +1609,25 @@
         <v>43101</v>
       </c>
       <c r="B2">
-        <v>23750.000000037599</v>
+        <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>639516.56999980274</v>
+        <v>468162.81999999995</v>
       </c>
       <c r="D2">
         <v>89397</v>
       </c>
       <c r="E2">
-        <v>752663.56999984034</v>
-      </c>
-      <c r="F2">
-        <v>8999905.9942071997</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>9315862.6005992647</v>
+        <v>605059.82000007527</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" t="s">
+        <v>5</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -1635,25 +1638,25 @@
         <v>43466</v>
       </c>
       <c r="B3">
-        <v>23750.000000037599</v>
+        <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>905331.0728996112</v>
+        <v>740617.98539980256</v>
       </c>
       <c r="D3">
         <v>89397</v>
       </c>
       <c r="E3">
-        <v>1018478.0728996487</v>
+        <v>877514.98539987789</v>
       </c>
       <c r="F3">
-        <v>8999999.9999775533</v>
+        <v>8999999.9999775514</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>9105269.704035338</v>
+        <v>9102933.0971176531</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -1689,13 +1692,13 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1703,25 +1706,25 @@
         <v>43101</v>
       </c>
       <c r="B2">
-        <v>23750.000000037599</v>
+        <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>639516.56999980274</v>
+        <v>468162.81999999995</v>
       </c>
       <c r="D2">
         <v>89397</v>
       </c>
       <c r="E2">
-        <v>752663.56999984034</v>
-      </c>
-      <c r="F2">
-        <v>8999905.9942071997</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>9315862.6005992647</v>
+        <v>605059.82000007527</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" t="s">
+        <v>5</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -1732,25 +1735,25 @@
         <v>43466</v>
       </c>
       <c r="B3">
-        <v>23750.000000037599</v>
+        <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>905331.0728996112</v>
+        <v>740617.98539980256</v>
       </c>
       <c r="D3">
         <v>89397</v>
       </c>
       <c r="E3">
-        <v>1018478.0728996487</v>
+        <v>877514.98539987789</v>
       </c>
       <c r="F3">
-        <v>8999999.9999775533</v>
+        <v>8999999.9999775514</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>9166368.9920353387</v>
+        <v>9162744.8791176509</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -1786,13 +1789,13 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1800,25 +1803,25 @@
         <v>43101</v>
       </c>
       <c r="B2">
-        <v>23750.000000037599</v>
+        <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>63516.570000201522</v>
+        <v>468162.81999999995</v>
       </c>
       <c r="D2">
         <v>89397</v>
       </c>
       <c r="E2">
-        <v>176663.57000023909</v>
-      </c>
-      <c r="F2">
-        <v>8999905.9942071997</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>9315862.6005992647</v>
+        <v>605059.82000007527</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" t="s">
+        <v>5</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -1829,25 +1832,25 @@
         <v>43466</v>
       </c>
       <c r="B3">
-        <v>23750.000000037599</v>
+        <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>346611.07289999811</v>
+        <v>740617.98539980256</v>
       </c>
       <c r="D3">
         <v>89397</v>
       </c>
       <c r="E3">
-        <v>459758.07290003583</v>
+        <v>877514.98539987789</v>
       </c>
       <c r="F3">
-        <v>8229999.9999999981</v>
+        <v>8229999.9999999953</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>8550902.8760577813</v>
+        <v>8559437.0931400936</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -1883,13 +1886,13 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1897,25 +1900,25 @@
         <v>43101</v>
       </c>
       <c r="B2">
-        <v>23750.000000037599</v>
+        <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>497016.56999990129</v>
+        <v>468162.81999999995</v>
       </c>
       <c r="D2">
         <v>89397</v>
       </c>
       <c r="E2">
-        <v>610163.56999993895</v>
-      </c>
-      <c r="F2">
-        <v>8999905.9942071997</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>9315862.6005992647</v>
+        <v>605059.82000007527</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" t="s">
+        <v>5</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -1926,25 +1929,25 @@
         <v>43466</v>
       </c>
       <c r="B3">
-        <v>23750.000000037599</v>
+        <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>191106.07290010579</v>
+        <v>164617.98540020152</v>
       </c>
       <c r="D3">
         <v>89397</v>
       </c>
       <c r="E3">
-        <v>304253.07290014339</v>
+        <v>301514.98540027672</v>
       </c>
       <c r="F3">
-        <v>8999999.9999775533</v>
+        <v>8999999.9999775514</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>9171027.6120353378</v>
+        <v>9171077.2611176502</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -1980,13 +1983,13 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1994,25 +1997,25 @@
         <v>43101</v>
       </c>
       <c r="B2">
-        <v>23750.000000037599</v>
+        <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>63516.570000201522</v>
+        <v>468162.81999999995</v>
       </c>
       <c r="D2">
         <v>89397</v>
       </c>
       <c r="E2">
-        <v>176663.57000023909</v>
-      </c>
-      <c r="F2">
-        <v>8999905.9942071997</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>9315862.6005992647</v>
+        <v>605059.82000007527</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" t="s">
+        <v>5</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -2023,25 +2026,25 @@
         <v>43466</v>
       </c>
       <c r="B3">
-        <v>23750.000000037599</v>
+        <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>204111.0729000968</v>
+        <v>598117.98539990128</v>
       </c>
       <c r="D3">
         <v>89397</v>
       </c>
       <c r="E3">
-        <v>317258.07290013437</v>
+        <v>735014.98539997661</v>
       </c>
       <c r="F3">
-        <v>8229999.9999999981</v>
+        <v>8229999.9999999953</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>8671869.3440577816</v>
+        <v>8673106.0491400938</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -2077,13 +2080,13 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -2091,25 +2094,25 @@
         <v>43101</v>
       </c>
       <c r="B2">
-        <v>23750.000000037599</v>
+        <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>63516.570000201522</v>
+        <v>468162.81999999995</v>
       </c>
       <c r="D2">
         <v>89397</v>
       </c>
       <c r="E2">
-        <v>176663.57000023909</v>
-      </c>
-      <c r="F2">
-        <v>8999905.9942071997</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>9315862.6005992647</v>
+        <v>605059.82000007527</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" t="s">
+        <v>5</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -2120,25 +2123,25 @@
         <v>43466</v>
       </c>
       <c r="B3">
-        <v>2.1140993969624428E-11</v>
+        <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>164617.98540020152</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>89397</v>
       </c>
       <c r="E3">
-        <v>2.1140993969624428E-11</v>
+        <v>301514.98540027672</v>
       </c>
       <c r="F3">
-        <v>8229999.9999999981</v>
+        <v>8380749.950453992</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>8510853.7240577824</v>
+        <v>8664809.0955940932</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -2174,13 +2177,13 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -2188,25 +2191,25 @@
         <v>43101</v>
       </c>
       <c r="B2">
-        <v>23750.000000037599</v>
+        <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>63516.570000201522</v>
+        <v>468162.81999999995</v>
       </c>
       <c r="D2">
         <v>89397</v>
       </c>
       <c r="E2">
-        <v>176663.57000023909</v>
-      </c>
-      <c r="F2">
-        <v>8999905.9942071997</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>9315862.6005992647</v>
+        <v>605059.82000007527</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" t="s">
+        <v>5</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -2217,25 +2220,25 @@
         <v>43466</v>
       </c>
       <c r="B3">
-        <v>2.1140993969624428E-11</v>
+        <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>164617.98540020152</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>89397</v>
       </c>
       <c r="E3">
-        <v>2.1140993969624428E-11</v>
+        <v>301514.98540027672</v>
       </c>
       <c r="F3">
-        <v>8229999.9999999981</v>
+        <v>8229999.9999999953</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>8449825.4580577817</v>
+        <v>8457531.0571400952</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -2271,13 +2274,13 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -2285,25 +2288,25 @@
         <v>43101</v>
       </c>
       <c r="B2">
-        <v>23750.000000037599</v>
+        <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>257516.56999980501</v>
+        <v>468162.81999999995</v>
       </c>
       <c r="D2">
         <v>89397</v>
       </c>
       <c r="E2">
-        <v>370663.56999984261</v>
-      </c>
-      <c r="F2">
-        <v>8999905.9942071997</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>9315862.6005992647</v>
+        <v>605059.82000007527</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" t="s">
+        <v>5</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -2314,25 +2317,25 @@
         <v>43466</v>
       </c>
       <c r="B3">
-        <v>23750.000000037599</v>
+        <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>263899.52890398417</v>
+        <v>303290.95565411646</v>
       </c>
       <c r="D3">
         <v>89397</v>
       </c>
       <c r="E3">
-        <v>377046.52890402172</v>
+        <v>440187.95565419167</v>
       </c>
       <c r="F3">
-        <v>8366132.5451393249</v>
+        <v>8229999.9999999953</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>8539234.8991971128</v>
+        <v>8413681.6251400951</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -2368,13 +2371,13 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -2382,25 +2385,25 @@
         <v>43101</v>
       </c>
       <c r="B2">
-        <v>23750.000000037599</v>
+        <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>63516.570000201522</v>
+        <v>468162.81999999995</v>
       </c>
       <c r="D2">
         <v>89397</v>
       </c>
       <c r="E2">
-        <v>176663.57000023909</v>
-      </c>
-      <c r="F2">
-        <v>8999905.9942071997</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>9315862.6005992647</v>
+        <v>605059.82000007527</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" t="s">
+        <v>5</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -2411,25 +2414,25 @@
         <v>43466</v>
       </c>
       <c r="B3">
-        <v>23750.000000037599</v>
+        <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>358617.98539980501</v>
       </c>
       <c r="D3">
-        <v>52913.570000000538</v>
+        <v>89397</v>
       </c>
       <c r="E3">
-        <v>76663.570000038133</v>
+        <v>495514.98539988021</v>
       </c>
       <c r="F3">
-        <v>8564528.281613294</v>
+        <v>8619895.7065850906</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>8745731.51567108</v>
+        <v>8804912.1857251916</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -2465,13 +2468,13 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -2479,25 +2482,25 @@
         <v>43101</v>
       </c>
       <c r="B2">
-        <v>23750.000000037599</v>
+        <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>257516.56999980501</v>
+        <v>468162.81999999995</v>
       </c>
       <c r="D2">
         <v>89397</v>
       </c>
       <c r="E2">
-        <v>370663.56999984261</v>
-      </c>
-      <c r="F2">
-        <v>8999905.9942071997</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>9315862.6005992647</v>
+        <v>605059.82000007527</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" t="s">
+        <v>5</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -2508,25 +2511,25 @@
         <v>43466</v>
       </c>
       <c r="B3">
-        <v>23750.000000037599</v>
+        <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>164617.98540020152</v>
       </c>
       <c r="D3">
-        <v>46913.570000012776</v>
+        <v>89397</v>
       </c>
       <c r="E3">
-        <v>70663.570000050371</v>
+        <v>301514.98540027672</v>
       </c>
       <c r="F3">
-        <v>8229999.9999999981</v>
+        <v>8229999.9999999953</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>8452673.5360577814</v>
+        <v>8438738.6951400954</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -2562,13 +2565,13 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -2576,25 +2579,25 @@
         <v>43101</v>
       </c>
       <c r="B2">
-        <v>23750.000000037599</v>
+        <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>257516.56999980501</v>
+        <v>468162.81999999995</v>
       </c>
       <c r="D2">
         <v>89397</v>
       </c>
       <c r="E2">
-        <v>370663.56999984261</v>
-      </c>
-      <c r="F2">
-        <v>8999905.9942071997</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>9315862.6005992647</v>
+        <v>605059.82000007527</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" t="s">
+        <v>5</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -2605,25 +2608,25 @@
         <v>43466</v>
       </c>
       <c r="B3">
-        <v>23750.000000037599</v>
+        <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>164617.98540020152</v>
       </c>
       <c r="D3">
-        <v>46913.570000012776</v>
+        <v>89397</v>
       </c>
       <c r="E3">
-        <v>70663.570000050371</v>
+        <v>301514.98540027672</v>
       </c>
       <c r="F3">
-        <v>8229999.9999999981</v>
+        <v>8229999.9999999953</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>8365743.0240577832</v>
+        <v>8378942.1091400944</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -2659,13 +2662,13 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -2673,25 +2676,25 @@
         <v>43101</v>
       </c>
       <c r="B2">
-        <v>23750.000000037599</v>
+        <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>639516.56999980274</v>
+        <v>468162.81999999995</v>
       </c>
       <c r="D2">
         <v>89397</v>
       </c>
       <c r="E2">
-        <v>752663.56999984034</v>
-      </c>
-      <c r="F2">
-        <v>8999905.9942071997</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>9315862.6005992647</v>
+        <v>605059.82000007527</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" t="s">
+        <v>5</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -2702,25 +2705,25 @@
         <v>43466</v>
       </c>
       <c r="B3">
-        <v>23750.000000037599</v>
+        <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>523331.0728996137</v>
+        <v>358617.98539980501</v>
       </c>
       <c r="D3">
         <v>89397</v>
       </c>
       <c r="E3">
-        <v>636478.07289965136</v>
+        <v>495514.98539988021</v>
       </c>
       <c r="F3">
-        <v>8999999.9999775533</v>
+        <v>8999999.9999775514</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>9220479.9720353391</v>
+        <v>9221226.4311176501</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -2756,13 +2759,13 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -2770,25 +2773,25 @@
         <v>43101</v>
       </c>
       <c r="B2">
-        <v>23750.000000037599</v>
+        <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>257516.56999980501</v>
+        <v>468162.81999999995</v>
       </c>
       <c r="D2">
         <v>89397</v>
       </c>
       <c r="E2">
-        <v>370663.56999984261</v>
-      </c>
-      <c r="F2">
-        <v>8999905.9942071997</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>9315862.6005992647</v>
+        <v>605059.82000007527</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" t="s">
+        <v>5</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -2799,25 +2802,25 @@
         <v>43466</v>
       </c>
       <c r="B3">
-        <v>23750.000000037599</v>
+        <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>534791.07289961353</v>
+        <v>740617.98539980256</v>
       </c>
       <c r="D3">
         <v>89397</v>
       </c>
       <c r="E3">
-        <v>647938.07289965113</v>
+        <v>877514.98539987789</v>
       </c>
       <c r="F3">
-        <v>8999999.9999775533</v>
+        <v>8999999.9999775514</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>9182721.3480353393</v>
+        <v>9178823.5011176523</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -2853,13 +2856,13 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -2867,25 +2870,25 @@
         <v>43101</v>
       </c>
       <c r="B2">
-        <v>23750.000000037599</v>
+        <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>639516.56999980274</v>
+        <v>468162.81999999995</v>
       </c>
       <c r="D2">
         <v>89397</v>
       </c>
       <c r="E2">
-        <v>752663.56999984034</v>
-      </c>
-      <c r="F2">
-        <v>8999905.9942071997</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>9315862.6005992647</v>
+        <v>605059.82000007527</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" t="s">
+        <v>5</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -2896,25 +2899,25 @@
         <v>43466</v>
       </c>
       <c r="B3">
-        <v>23750.000000037599</v>
+        <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>523331.0728996137</v>
+        <v>358617.98539980501</v>
       </c>
       <c r="D3">
         <v>89397</v>
       </c>
       <c r="E3">
-        <v>636478.07289965136</v>
+        <v>495514.98539988021</v>
       </c>
       <c r="F3">
-        <v>8999999.9999775533</v>
+        <v>8999999.9999775514</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>9253869.5300353374</v>
+        <v>9246731.1111176517</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -2950,13 +2953,13 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -2964,25 +2967,25 @@
         <v>43101</v>
       </c>
       <c r="B2">
-        <v>23750.000000037599</v>
+        <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>639516.56999980274</v>
+        <v>468162.81999999995</v>
       </c>
       <c r="D2">
         <v>89397</v>
       </c>
       <c r="E2">
-        <v>752663.56999984034</v>
-      </c>
-      <c r="F2">
-        <v>8999905.9942071997</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>9315862.6005992647</v>
+        <v>605059.82000007527</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" t="s">
+        <v>5</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -2993,25 +2996,25 @@
         <v>43466</v>
       </c>
       <c r="B3">
-        <v>23750.000000037599</v>
+        <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>905331.0728996112</v>
+        <v>740617.98539980256</v>
       </c>
       <c r="D3">
         <v>89397</v>
       </c>
       <c r="E3">
-        <v>1018478.0728996487</v>
+        <v>877514.98539987789</v>
       </c>
       <c r="F3">
-        <v>8229999.9999999981</v>
+        <v>8229999.9999999953</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>8544080.4700577836</v>
+        <v>8535857.4891400933</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -3047,13 +3050,13 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -3061,25 +3064,25 @@
         <v>43101</v>
       </c>
       <c r="B2">
-        <v>23750.000000037599</v>
+        <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>639516.56999980274</v>
+        <v>468162.81999999995</v>
       </c>
       <c r="D2">
         <v>89397</v>
       </c>
       <c r="E2">
-        <v>752663.56999984034</v>
-      </c>
-      <c r="F2">
-        <v>8999905.9942071997</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>9315862.6005992647</v>
+        <v>605059.82000007527</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" t="s">
+        <v>5</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -3090,25 +3093,25 @@
         <v>43466</v>
       </c>
       <c r="B3">
-        <v>23750.000000037599</v>
+        <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>905331.0728996112</v>
+        <v>740617.98539980256</v>
       </c>
       <c r="D3">
         <v>89397</v>
       </c>
       <c r="E3">
-        <v>1018478.0728996487</v>
+        <v>877514.98539987789</v>
       </c>
       <c r="F3">
-        <v>8999999.9999775533</v>
+        <v>8999999.9999775514</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>9322938.8360353373</v>
+        <v>9322491.0931176525</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -3144,13 +3147,13 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -3158,25 +3161,25 @@
         <v>43101</v>
       </c>
       <c r="B2">
-        <v>23750.000000037599</v>
+        <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>257516.56999980501</v>
+        <v>468162.81999999995</v>
       </c>
       <c r="D2">
         <v>89397</v>
       </c>
       <c r="E2">
-        <v>370663.56999984261</v>
-      </c>
-      <c r="F2">
-        <v>8999905.9942071997</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>9315862.6005992647</v>
+        <v>605059.82000007527</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" t="s">
+        <v>5</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -3187,25 +3190,25 @@
         <v>43466</v>
       </c>
       <c r="B3">
-        <v>23750.000000037599</v>
+        <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>534791.07289961353</v>
+        <v>740617.98539980256</v>
       </c>
       <c r="D3">
         <v>89397</v>
       </c>
       <c r="E3">
-        <v>647938.07289965113</v>
+        <v>877514.98539987789</v>
       </c>
       <c r="F3">
-        <v>8229999.9999999981</v>
+        <v>8229999.9999999953</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>8477489.750057783</v>
+        <v>8473804.7091400959</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -3241,13 +3244,13 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -3255,25 +3258,25 @@
         <v>43101</v>
       </c>
       <c r="B2">
-        <v>23750.000000037599</v>
+        <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>354516.57</v>
+        <v>468162.81999999995</v>
       </c>
       <c r="D2">
         <v>89397</v>
       </c>
       <c r="E2">
-        <v>467663.57000003767</v>
-      </c>
-      <c r="F2">
-        <v>8999905.9942071997</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>9315862.6005992647</v>
+        <v>605059.82000007527</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" t="s">
+        <v>5</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -3284,25 +3287,25 @@
         <v>43466</v>
       </c>
       <c r="B3">
-        <v>23750.000000037599</v>
+        <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>343881.07290000003</v>
+        <v>455617.98539999995</v>
       </c>
       <c r="D3">
         <v>89397</v>
       </c>
       <c r="E3">
-        <v>457028.07290003763</v>
+        <v>592514.98540007521</v>
       </c>
       <c r="F3">
-        <v>8854562.1209468655</v>
+        <v>8723090.2696897946</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>8998832.8250046521</v>
+        <v>8879500.7588298917</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -3350,13 +3353,13 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -3364,25 +3367,25 @@
         <v>43101</v>
       </c>
       <c r="B2">
-        <v>23750.000000037599</v>
+        <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>354516.57</v>
+        <v>468162.81999999995</v>
       </c>
       <c r="D2">
         <v>89397</v>
       </c>
       <c r="E2">
-        <v>467663.57000003767</v>
-      </c>
-      <c r="F2">
-        <v>8999905.9942071997</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>9315862.6005992647</v>
+        <v>605059.82000007527</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" t="s">
+        <v>5</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -3393,25 +3396,25 @@
         <v>43466</v>
       </c>
       <c r="B3">
-        <v>23750.000000037599</v>
+        <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>246881.07289980506</v>
+        <v>358617.98539980501</v>
       </c>
       <c r="D3">
         <v>89397</v>
       </c>
       <c r="E3">
-        <v>360028.07289984263</v>
+        <v>495514.98539988021</v>
       </c>
       <c r="F3">
-        <v>8229999.9999999981</v>
+        <v>8229999.9999999953</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>8314596.0640577823</v>
+        <v>8320823.8991400944</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -3447,13 +3450,13 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -3461,25 +3464,25 @@
         <v>43101</v>
       </c>
       <c r="B2">
-        <v>23750.000000037599</v>
+        <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>639516.56999980274</v>
+        <v>468162.81999999995</v>
       </c>
       <c r="D2">
         <v>89397</v>
       </c>
       <c r="E2">
-        <v>752663.56999984034</v>
-      </c>
-      <c r="F2">
-        <v>8999905.9942071997</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>9315862.6005992647</v>
+        <v>605059.82000007527</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" t="s">
+        <v>5</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -3490,25 +3493,25 @@
         <v>43466</v>
       </c>
       <c r="B3">
-        <v>23750.000000037599</v>
+        <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>620331.07289980864</v>
+        <v>455617.98539999995</v>
       </c>
       <c r="D3">
         <v>89397</v>
       </c>
       <c r="E3">
-        <v>733478.07289984624</v>
+        <v>592514.98540007521</v>
       </c>
       <c r="F3">
-        <v>8999999.9999775533</v>
+        <v>8999999.9999775514</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>9087757.4640353378</v>
+        <v>9095331.579117652</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -3544,13 +3547,13 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -3558,25 +3561,25 @@
         <v>43101</v>
       </c>
       <c r="B2">
-        <v>23750.000000037599</v>
+        <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>354516.57</v>
+        <v>468162.81999999995</v>
       </c>
       <c r="D2">
         <v>89397</v>
       </c>
       <c r="E2">
-        <v>467663.57000003767</v>
-      </c>
-      <c r="F2">
-        <v>8999905.9942071997</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>9315862.6005992647</v>
+        <v>605059.82000007527</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" t="s">
+        <v>5</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -3587,25 +3590,25 @@
         <v>43466</v>
       </c>
       <c r="B3">
-        <v>23750.000000037599</v>
+        <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>628881.07289980259</v>
+        <v>740617.98539980256</v>
       </c>
       <c r="D3">
         <v>89397</v>
       </c>
       <c r="E3">
-        <v>742028.07289984031</v>
+        <v>877514.98539987789</v>
       </c>
       <c r="F3">
-        <v>8511829.9610227067</v>
+        <v>8810170.4120705463</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>8767557.2750804927</v>
+        <v>9061605.7912106458</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -3641,13 +3644,13 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -3655,25 +3658,25 @@
         <v>43101</v>
       </c>
       <c r="B2">
-        <v>23750.000000037599</v>
+        <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>257516.56999980501</v>
+        <v>468162.81999999995</v>
       </c>
       <c r="D2">
         <v>89397</v>
       </c>
       <c r="E2">
-        <v>370663.56999984261</v>
-      </c>
-      <c r="F2">
-        <v>8999905.9942071997</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>9315862.6005992647</v>
+        <v>605059.82000007527</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" t="s">
+        <v>5</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -3684,25 +3687,25 @@
         <v>43466</v>
       </c>
       <c r="B3">
-        <v>23750.000000037599</v>
+        <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>249791.07289981085</v>
+        <v>455617.98539999995</v>
       </c>
       <c r="D3">
         <v>89397</v>
       </c>
       <c r="E3">
-        <v>362938.07289984846</v>
+        <v>592514.98540007521</v>
       </c>
       <c r="F3">
-        <v>8999999.9999775533</v>
+        <v>8999999.9999775514</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>9219887.1840353366</v>
+        <v>9222322.1591176502</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -3738,13 +3741,13 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -3752,25 +3755,25 @@
         <v>43101</v>
       </c>
       <c r="B2">
-        <v>23750.000000037599</v>
+        <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>63516.570000201522</v>
+        <v>468162.81999999995</v>
       </c>
       <c r="D2">
         <v>89397</v>
       </c>
       <c r="E2">
-        <v>176663.57000023909</v>
-      </c>
-      <c r="F2">
-        <v>8999905.9942071997</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>9315862.6005992647</v>
+        <v>605059.82000007527</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" t="s">
+        <v>5</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -3781,25 +3784,25 @@
         <v>43466</v>
       </c>
       <c r="B3">
-        <v>23750.000000037599</v>
+        <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>358617.98539980501</v>
       </c>
       <c r="D3">
-        <v>52913.570000000538</v>
+        <v>89397</v>
       </c>
       <c r="E3">
-        <v>76663.570000038133</v>
+        <v>495514.98539988021</v>
       </c>
       <c r="F3">
-        <v>8999999.9999775533</v>
+        <v>8999999.9999775514</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>9196925.9240353368</v>
+        <v>9200471.499117652</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -3835,13 +3838,13 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -3849,25 +3852,25 @@
         <v>43101</v>
       </c>
       <c r="B2">
-        <v>23750.000000037599</v>
+        <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>257516.56999980501</v>
+        <v>468162.81999999995</v>
       </c>
       <c r="D2">
         <v>89397</v>
       </c>
       <c r="E2">
-        <v>370663.56999984261</v>
-      </c>
-      <c r="F2">
-        <v>8999905.9942071997</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>9315862.6005992647</v>
+        <v>605059.82000007527</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" t="s">
+        <v>5</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -3878,25 +3881,25 @@
         <v>43466</v>
       </c>
       <c r="B3">
-        <v>23750.000000037599</v>
+        <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>164617.98540020152</v>
       </c>
       <c r="D3">
-        <v>46913.570000012776</v>
+        <v>89397</v>
       </c>
       <c r="E3">
-        <v>70663.570000050371</v>
+        <v>301514.98540027672</v>
       </c>
       <c r="F3">
-        <v>8229999.9999999981</v>
+        <v>8229999.9999999953</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>8455034.3440577816</v>
+        <v>8455084.829140095</v>
       </c>
       <c r="I3">
         <v>0</v>

</xml_diff>

<commit_message>
Updated data in outputs/model file due to test run using new Davis Dam energy method
</commit_message>
<xml_diff>
--- a/Output Data/MtomToCrss_Annual.xlsx
+++ b/Output Data/MtomToCrss_Annual.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\D_Drive\Modeling\MTOM_Production\_DEC18_Post-MTOM-dev\Output Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\MTOM\dev\Output Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12840" windowHeight="13530"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="4245" windowHeight="8535"/>
   </bookViews>
   <sheets>
     <sheet name="Trace38" sheetId="37" r:id="rId1"/>
@@ -583,13 +583,13 @@
         <v>495514.98539988021</v>
       </c>
       <c r="F3">
-        <v>8948862.0448640604</v>
+        <v>8950661.3810616694</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>9136078.9540041573</v>
+        <v>9137878.2902017683</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -874,13 +874,13 @@
         <v>592514.98540007521</v>
       </c>
       <c r="F3">
-        <v>8740699.6356417686</v>
+        <v>8742499.3445590418</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>8890240.5747818686</v>
+        <v>8892040.28369914</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -1165,13 +1165,13 @@
         <v>495514.98539988021</v>
       </c>
       <c r="F3">
-        <v>8989416.0613516401</v>
+        <v>8991215.9277455863</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>9134957.0204917379</v>
+        <v>9136756.886885684</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -1359,13 +1359,13 @@
         <v>877514.98539987789</v>
       </c>
       <c r="F3">
-        <v>8533443.8018583804</v>
+        <v>8549173.4722800888</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>8759816.7209984809</v>
+        <v>8775546.3914201874</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -1553,13 +1553,13 @@
         <v>301514.98540027672</v>
       </c>
       <c r="F3">
-        <v>8863769.7982449085</v>
+        <v>8865569.3160762265</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>9044296.1673850119</v>
+        <v>9046095.6852163263</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -2135,13 +2135,13 @@
         <v>301514.98540027672</v>
       </c>
       <c r="F3">
-        <v>8380749.950453992</v>
+        <v>8382551.3879766222</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>8664809.0955940932</v>
+        <v>8666610.5331167243</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -2320,13 +2320,13 @@
         <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>303290.95565411646</v>
+        <v>336055.68840417598</v>
       </c>
       <c r="D3">
         <v>89397</v>
       </c>
       <c r="E3">
-        <v>440187.95565419167</v>
+        <v>472952.68840425112</v>
       </c>
       <c r="F3">
         <v>8229999.9999999953</v>
@@ -2426,13 +2426,13 @@
         <v>495514.98539988021</v>
       </c>
       <c r="F3">
-        <v>8619895.7065850906</v>
+        <v>8621695.6702742185</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>8804912.1857251916</v>
+        <v>8806712.1494143177</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -3299,13 +3299,13 @@
         <v>592514.98540007521</v>
       </c>
       <c r="F3">
-        <v>8723090.2696897946</v>
+        <v>8723307.2508730888</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>8879500.7588298917</v>
+        <v>8879717.7400131878</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -3602,13 +3602,13 @@
         <v>877514.98539987789</v>
       </c>
       <c r="F3">
-        <v>8810170.4120705463</v>
+        <v>8811971.9339028448</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>9061605.7912106458</v>
+        <v>9063407.313042948</v>
       </c>
       <c r="I3">
         <v>0</v>

</xml_diff>

<commit_message>
January 2019 Official Model Run includes update to CBRFC forecasts and model output files. Model files and ruleset renamed using new naming convention. No other changes to model file and ruleset since last commit
Updated the MTOM_EnsembleOutput file to fix percent exceedance plot formulas
</commit_message>
<xml_diff>
--- a/Output Data/MtomToCrss_Annual.xlsx
+++ b/Output Data/MtomToCrss_Annual.xlsx
@@ -9,46 +9,48 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="4245" windowHeight="8535"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12570" windowHeight="13590"/>
   </bookViews>
   <sheets>
-    <sheet name="Trace38" sheetId="37" r:id="rId1"/>
-    <sheet name="Trace37" sheetId="36" r:id="rId2"/>
-    <sheet name="Trace36" sheetId="35" r:id="rId3"/>
-    <sheet name="Trace35" sheetId="34" r:id="rId4"/>
-    <sheet name="Trace34" sheetId="33" r:id="rId5"/>
-    <sheet name="Trace33" sheetId="32" r:id="rId6"/>
-    <sheet name="Trace32" sheetId="31" r:id="rId7"/>
-    <sheet name="Trace31" sheetId="30" r:id="rId8"/>
-    <sheet name="Trace30" sheetId="29" r:id="rId9"/>
-    <sheet name="Trace29" sheetId="28" r:id="rId10"/>
-    <sheet name="Trace28" sheetId="27" r:id="rId11"/>
-    <sheet name="Trace27" sheetId="26" r:id="rId12"/>
-    <sheet name="Trace26" sheetId="25" r:id="rId13"/>
-    <sheet name="Trace25" sheetId="24" r:id="rId14"/>
-    <sheet name="Trace24" sheetId="23" r:id="rId15"/>
-    <sheet name="Trace23" sheetId="22" r:id="rId16"/>
-    <sheet name="Trace22" sheetId="21" r:id="rId17"/>
-    <sheet name="Trace21" sheetId="20" r:id="rId18"/>
-    <sheet name="Trace20" sheetId="19" r:id="rId19"/>
-    <sheet name="Trace19" sheetId="18" r:id="rId20"/>
-    <sheet name="Trace18" sheetId="17" r:id="rId21"/>
-    <sheet name="Trace17" sheetId="16" r:id="rId22"/>
-    <sheet name="Trace16" sheetId="15" r:id="rId23"/>
-    <sheet name="Trace15" sheetId="14" r:id="rId24"/>
-    <sheet name="Trace14" sheetId="13" r:id="rId25"/>
-    <sheet name="Trace13" sheetId="12" r:id="rId26"/>
-    <sheet name="Trace12" sheetId="11" r:id="rId27"/>
-    <sheet name="Trace11" sheetId="10" r:id="rId28"/>
-    <sheet name="Trace10" sheetId="9" r:id="rId29"/>
-    <sheet name="Trace9" sheetId="8" r:id="rId30"/>
-    <sheet name="Trace8" sheetId="7" r:id="rId31"/>
-    <sheet name="Trace7" sheetId="6" r:id="rId32"/>
-    <sheet name="Trace6" sheetId="5" r:id="rId33"/>
-    <sheet name="Trace5" sheetId="4" r:id="rId34"/>
-    <sheet name="Trace4" sheetId="3" r:id="rId35"/>
-    <sheet name="Trace3" sheetId="2" r:id="rId36"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId37"/>
+    <sheet name="Trace38" sheetId="39" r:id="rId1"/>
+    <sheet name="Trace37" sheetId="38" r:id="rId2"/>
+    <sheet name="Trace36" sheetId="37" r:id="rId3"/>
+    <sheet name="Trace35" sheetId="36" r:id="rId4"/>
+    <sheet name="Trace34" sheetId="35" r:id="rId5"/>
+    <sheet name="Trace33" sheetId="34" r:id="rId6"/>
+    <sheet name="Trace32" sheetId="33" r:id="rId7"/>
+    <sheet name="Trace31" sheetId="32" r:id="rId8"/>
+    <sheet name="Trace30" sheetId="31" r:id="rId9"/>
+    <sheet name="Trace29" sheetId="30" r:id="rId10"/>
+    <sheet name="Trace28" sheetId="29" r:id="rId11"/>
+    <sheet name="Trace27" sheetId="28" r:id="rId12"/>
+    <sheet name="Trace26" sheetId="27" r:id="rId13"/>
+    <sheet name="Trace25" sheetId="26" r:id="rId14"/>
+    <sheet name="Trace24" sheetId="25" r:id="rId15"/>
+    <sheet name="Trace23" sheetId="24" r:id="rId16"/>
+    <sheet name="Trace22" sheetId="23" r:id="rId17"/>
+    <sheet name="Trace21" sheetId="22" r:id="rId18"/>
+    <sheet name="Trace20" sheetId="21" r:id="rId19"/>
+    <sheet name="Trace19" sheetId="20" r:id="rId20"/>
+    <sheet name="Trace18" sheetId="19" r:id="rId21"/>
+    <sheet name="Trace17" sheetId="18" r:id="rId22"/>
+    <sheet name="Trace16" sheetId="17" r:id="rId23"/>
+    <sheet name="Trace15" sheetId="16" r:id="rId24"/>
+    <sheet name="Trace14" sheetId="15" r:id="rId25"/>
+    <sheet name="Trace13" sheetId="14" r:id="rId26"/>
+    <sheet name="Trace12" sheetId="13" r:id="rId27"/>
+    <sheet name="Trace11" sheetId="12" r:id="rId28"/>
+    <sheet name="Trace10" sheetId="11" r:id="rId29"/>
+    <sheet name="Trace9" sheetId="10" r:id="rId30"/>
+    <sheet name="Trace8" sheetId="9" r:id="rId31"/>
+    <sheet name="Trace7" sheetId="8" r:id="rId32"/>
+    <sheet name="Trace6" sheetId="7" r:id="rId33"/>
+    <sheet name="Trace5" sheetId="6" r:id="rId34"/>
+    <sheet name="Trace4" sheetId="5" r:id="rId35"/>
+    <sheet name="Trace3" sheetId="4" r:id="rId36"/>
+    <sheet name="Trace2" sheetId="3" r:id="rId37"/>
+    <sheet name="Trace1" sheetId="2" r:id="rId38"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId39"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -60,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="8">
   <si>
     <t>ICS Credits.BiNationalICS_CA</t>
   </si>
@@ -75,9 +77,6 @@
   </si>
   <si>
     <t>PowellOperation.PowellWYRelease</t>
-  </si>
-  <si>
-    <t>NaN</t>
   </si>
   <si>
     <t>SystemConditions.PowellRelTier</t>
@@ -431,39 +430,39 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>43101</v>
+        <v>43466</v>
       </c>
       <c r="B2">
         <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>468162.81999999995</v>
+        <v>164617.98540020152</v>
       </c>
       <c r="D2">
         <v>89397</v>
       </c>
       <c r="E2">
-        <v>605059.82000007527</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" t="s">
-        <v>5</v>
+        <v>301514.98540027672</v>
+      </c>
+      <c r="F2">
+        <v>8229999.9999999953</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>8397147.5063107386</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -471,31 +470,31 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>43466</v>
+        <v>43831</v>
       </c>
       <c r="B3">
         <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>358617.98539980501</v>
+        <v>164617.98540020172</v>
       </c>
       <c r="D3">
         <v>89397</v>
       </c>
       <c r="E3">
-        <v>495514.98539988021</v>
+        <v>301514.9854002769</v>
       </c>
       <c r="F3">
-        <v>8229999.9999999953</v>
+        <v>7479999.9999999981</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H3">
-        <v>8388765.7051400952</v>
+        <v>7590981.0259999959</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -528,39 +527,39 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>43101</v>
+        <v>43466</v>
       </c>
       <c r="B2">
         <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>468162.81999999995</v>
+        <v>740617.98539980256</v>
       </c>
       <c r="D2">
         <v>89397</v>
       </c>
       <c r="E2">
-        <v>605059.82000007527</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" t="s">
-        <v>5</v>
+        <v>877514.98539987789</v>
+      </c>
+      <c r="F2">
+        <v>8229999.9999999953</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>8498842.6363107394</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -568,31 +567,31 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>43466</v>
+        <v>43831</v>
       </c>
       <c r="B3">
         <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>358617.98539980501</v>
+        <v>740617.98539980256</v>
       </c>
       <c r="D3">
         <v>89397</v>
       </c>
       <c r="E3">
-        <v>495514.98539988021</v>
+        <v>877514.98539987789</v>
       </c>
       <c r="F3">
-        <v>8950661.3810616694</v>
+        <v>7479999.9999999981</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H3">
-        <v>9137878.2902017683</v>
+        <v>7646147.9299999969</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -625,39 +624,39 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>43101</v>
+        <v>43466</v>
       </c>
       <c r="B2">
         <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>468162.81999999995</v>
+        <v>598117.98539990128</v>
       </c>
       <c r="D2">
         <v>89397</v>
       </c>
       <c r="E2">
-        <v>605059.82000007527</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" t="s">
-        <v>5</v>
+        <v>735014.98539997661</v>
+      </c>
+      <c r="F2">
+        <v>8229999.9999999953</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>8413747.2263107393</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -665,28 +664,28 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>43466</v>
+        <v>43831</v>
       </c>
       <c r="B3">
         <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>740617.98539980256</v>
+        <v>866674.49583770882</v>
       </c>
       <c r="D3">
         <v>89397</v>
       </c>
       <c r="E3">
-        <v>877514.98539987789</v>
+        <v>1003571.4958377838</v>
       </c>
       <c r="F3">
-        <v>8999999.9999775514</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>9292478.2691176515</v>
+        <v>9263906.2799775526</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -722,39 +721,39 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>43101</v>
+        <v>43466</v>
       </c>
       <c r="B2">
         <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>468162.81999999995</v>
+        <v>455617.98539999995</v>
       </c>
       <c r="D2">
         <v>89397</v>
       </c>
       <c r="E2">
-        <v>605059.82000007527</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" t="s">
-        <v>5</v>
+        <v>592514.98540007521</v>
+      </c>
+      <c r="F2">
+        <v>8229999.9999999953</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>8370370.4563107397</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -762,31 +761,31 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>43466</v>
+        <v>43831</v>
       </c>
       <c r="B3">
         <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>598117.98539990128</v>
+        <v>455617.98539999995</v>
       </c>
       <c r="D3">
         <v>89397</v>
       </c>
       <c r="E3">
-        <v>735014.98539997661</v>
+        <v>592514.98540007521</v>
       </c>
       <c r="F3">
-        <v>8229999.9999999953</v>
+        <v>7479999.9999999981</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H3">
-        <v>8408732.8391400948</v>
+        <v>7609167.7799999956</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -819,39 +818,39 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>43101</v>
+        <v>43466</v>
       </c>
       <c r="B2">
         <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>468162.81999999995</v>
+        <v>598117.98539990128</v>
       </c>
       <c r="D2">
         <v>89397</v>
       </c>
       <c r="E2">
-        <v>605059.82000007527</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" t="s">
-        <v>5</v>
+        <v>735014.98539997661</v>
+      </c>
+      <c r="F2">
+        <v>8715847.906304691</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>8895069.6426154338</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -859,31 +858,31 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>43466</v>
+        <v>43831</v>
       </c>
       <c r="B3">
         <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>455617.98539999995</v>
+        <v>598117.98539990128</v>
       </c>
       <c r="D3">
         <v>89397</v>
       </c>
       <c r="E3">
-        <v>592514.98540007521</v>
+        <v>735014.98539997661</v>
       </c>
       <c r="F3">
-        <v>8742499.3445590418</v>
+        <v>7479999.9999999981</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H3">
-        <v>8892040.28369914</v>
+        <v>7584398.0899999952</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -916,39 +915,39 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>43101</v>
+        <v>43466</v>
       </c>
       <c r="B2">
         <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>468162.81999999995</v>
+        <v>358617.98539980507</v>
       </c>
       <c r="D2">
         <v>89397</v>
       </c>
       <c r="E2">
-        <v>605059.82000007527</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" t="s">
-        <v>5</v>
+        <v>495514.98539988021</v>
+      </c>
+      <c r="F2">
+        <v>8229999.9999999953</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>8393510.7663107384</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -956,31 +955,31 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>43466</v>
+        <v>43831</v>
       </c>
       <c r="B3">
         <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>598117.98539990128</v>
+        <v>358617.98539980507</v>
       </c>
       <c r="D3">
         <v>89397</v>
       </c>
       <c r="E3">
-        <v>735014.98539997661</v>
+        <v>495514.98539988021</v>
       </c>
       <c r="F3">
-        <v>8229999.9999999953</v>
+        <v>7640907.5547923325</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H3">
-        <v>8413596.5091400947</v>
+        <v>7772554.9947923291</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1013,39 +1012,39 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>43101</v>
+        <v>43466</v>
       </c>
       <c r="B2">
         <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>468162.81999999995</v>
+        <v>358617.98539980507</v>
       </c>
       <c r="D2">
         <v>89397</v>
       </c>
       <c r="E2">
-        <v>605059.82000007527</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" t="s">
-        <v>5</v>
+        <v>495514.98539988021</v>
+      </c>
+      <c r="F2">
+        <v>8229999.9999999953</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>8365625.1263107378</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -1053,13 +1052,13 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>43466</v>
+        <v>43831</v>
       </c>
       <c r="B3">
         <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>358617.98539980501</v>
+        <v>358617.98539980507</v>
       </c>
       <c r="D3">
         <v>89397</v>
@@ -1068,16 +1067,16 @@
         <v>495514.98539988021</v>
       </c>
       <c r="F3">
-        <v>8229999.9999999953</v>
+        <v>7479999.9999999981</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H3">
-        <v>8392216.709140094</v>
+        <v>7588713.6499999976</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1110,39 +1109,39 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>43101</v>
+        <v>43466</v>
       </c>
       <c r="B2">
         <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>468162.81999999995</v>
+        <v>598117.98539990128</v>
       </c>
       <c r="D2">
         <v>89397</v>
       </c>
       <c r="E2">
-        <v>605059.82000007527</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" t="s">
-        <v>5</v>
+        <v>735014.98539997661</v>
+      </c>
+      <c r="F2">
+        <v>8999999.9999775514</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>9192742.7262882963</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -1150,31 +1149,31 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>43466</v>
+        <v>43831</v>
       </c>
       <c r="B3">
         <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>358617.98539980501</v>
+        <v>598117.98539990128</v>
       </c>
       <c r="D3">
         <v>89397</v>
       </c>
       <c r="E3">
-        <v>495514.98539988021</v>
+        <v>735014.98539997661</v>
       </c>
       <c r="F3">
-        <v>8991215.9277455863</v>
+        <v>7479999.9999999981</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H3">
-        <v>9136756.886885684</v>
+        <v>7585477.679999995</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1207,39 +1206,39 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>43101</v>
+        <v>43466</v>
       </c>
       <c r="B2">
         <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>468162.81999999995</v>
+        <v>740617.98539980256</v>
       </c>
       <c r="D2">
         <v>89397</v>
       </c>
       <c r="E2">
-        <v>605059.82000007527</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" t="s">
-        <v>5</v>
+        <v>877514.98539987789</v>
+      </c>
+      <c r="F2">
+        <v>8999999.9999775514</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>9216683.7862882949</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -1247,28 +1246,28 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>43466</v>
+        <v>43831</v>
       </c>
       <c r="B3">
         <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>598117.98539990128</v>
+        <v>862399.49583771161</v>
       </c>
       <c r="D3">
         <v>89397</v>
       </c>
       <c r="E3">
-        <v>735014.98539997661</v>
+        <v>999296.4958377867</v>
       </c>
       <c r="F3">
-        <v>8999999.9999775514</v>
+        <v>8574687.8485893924</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>9197021.5391176511</v>
+        <v>8715315.8785893936</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -1304,39 +1303,39 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>43101</v>
+        <v>43466</v>
       </c>
       <c r="B2">
         <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>468162.81999999995</v>
+        <v>740617.98539980256</v>
       </c>
       <c r="D2">
         <v>89397</v>
       </c>
       <c r="E2">
-        <v>605059.82000007527</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" t="s">
-        <v>5</v>
+        <v>877514.98539987789</v>
+      </c>
+      <c r="F2">
+        <v>8633842.735802548</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>8645148.1321132928</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -1344,28 +1343,28 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>43466</v>
+        <v>43831</v>
       </c>
       <c r="B3">
         <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>740617.98539980256</v>
+        <v>1004899.4958376131</v>
       </c>
       <c r="D3">
         <v>89397</v>
       </c>
       <c r="E3">
-        <v>877514.98539987789</v>
+        <v>1141796.4958376884</v>
       </c>
       <c r="F3">
-        <v>8549173.4722800888</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>8775546.3914201874</v>
+        <v>9203484.9599775542</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -1401,39 +1400,39 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>43101</v>
+        <v>43466</v>
       </c>
       <c r="B2">
         <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>468162.81999999995</v>
+        <v>740617.98539980256</v>
       </c>
       <c r="D2">
         <v>89397</v>
       </c>
       <c r="E2">
-        <v>605059.82000007527</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" t="s">
-        <v>5</v>
+        <v>877514.98539987789</v>
+      </c>
+      <c r="F2">
+        <v>8999999.9999775514</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>9099017.5382882971</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -1441,28 +1440,28 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>43466</v>
+        <v>43831</v>
       </c>
       <c r="B3">
         <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>740617.98539980256</v>
+        <v>1004899.4958376129</v>
       </c>
       <c r="D3">
         <v>89397</v>
       </c>
       <c r="E3">
-        <v>877514.98539987789</v>
+        <v>1141796.495837688</v>
       </c>
       <c r="F3">
-        <v>8999999.9999775514</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>8992754.249117652</v>
+        <v>8910372.509977553</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -1498,39 +1497,39 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>43101</v>
+        <v>43466</v>
       </c>
       <c r="B2">
         <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>468162.81999999995</v>
+        <v>164617.98540020152</v>
       </c>
       <c r="D2">
         <v>89397</v>
       </c>
       <c r="E2">
-        <v>605059.82000007527</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" t="s">
-        <v>5</v>
+        <v>301514.98540027672</v>
+      </c>
+      <c r="F2">
+        <v>8867764.5246292893</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>9025050.8709400352</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -1538,7 +1537,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>43466</v>
+        <v>43831</v>
       </c>
       <c r="B3">
         <v>47500.000000075197</v>
@@ -1553,16 +1552,16 @@
         <v>301514.98540027672</v>
       </c>
       <c r="F3">
-        <v>8865569.3160762265</v>
+        <v>7479999.9999999981</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H3">
-        <v>9046095.6852163263</v>
+        <v>7615931.8499999968</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1595,39 +1594,39 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>43101</v>
+        <v>43466</v>
       </c>
       <c r="B2">
         <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>468162.81999999995</v>
+        <v>740617.98539980256</v>
       </c>
       <c r="D2">
         <v>89397</v>
       </c>
       <c r="E2">
-        <v>605059.82000007527</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" t="s">
-        <v>5</v>
+        <v>877514.98539987789</v>
+      </c>
+      <c r="F2">
+        <v>8999999.9999775514</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>9148785.5442882963</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -1635,28 +1634,28 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>43466</v>
+        <v>43831</v>
       </c>
       <c r="B3">
         <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>740617.98539980256</v>
+        <v>1004899.4958376129</v>
       </c>
       <c r="D3">
         <v>89397</v>
       </c>
       <c r="E3">
-        <v>877514.98539987789</v>
+        <v>1141796.495837688</v>
       </c>
       <c r="F3">
-        <v>8999999.9999775514</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>9102933.0971176531</v>
+        <v>9061671.6859775521</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -1692,39 +1691,39 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>43101</v>
+        <v>43466</v>
       </c>
       <c r="B2">
         <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>468162.81999999995</v>
+        <v>740617.98539980256</v>
       </c>
       <c r="D2">
         <v>89397</v>
       </c>
       <c r="E2">
-        <v>605059.82000007527</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" t="s">
-        <v>5</v>
+        <v>877514.98539987789</v>
+      </c>
+      <c r="F2">
+        <v>8229999.9999999953</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>8543052.252310738</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -1732,28 +1731,28 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>43466</v>
+        <v>43831</v>
       </c>
       <c r="B3">
         <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>740617.98539980256</v>
+        <v>1004899.4958376129</v>
       </c>
       <c r="D3">
         <v>89397</v>
       </c>
       <c r="E3">
-        <v>877514.98539987789</v>
+        <v>1141796.495837688</v>
       </c>
       <c r="F3">
-        <v>8999999.9999775514</v>
+        <v>11134627.059672041</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>9162744.8791176509</v>
+        <v>11263145.791672042</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -1789,39 +1788,39 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>43101</v>
+        <v>43466</v>
       </c>
       <c r="B2">
         <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>468162.81999999995</v>
+        <v>164617.98540020152</v>
       </c>
       <c r="D2">
         <v>89397</v>
       </c>
       <c r="E2">
-        <v>605059.82000007527</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" t="s">
-        <v>5</v>
+        <v>301514.98540027672</v>
+      </c>
+      <c r="F2">
+        <v>8229999.9999999953</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>8391462.0063107405</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -1829,31 +1828,31 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>43466</v>
+        <v>43831</v>
       </c>
       <c r="B3">
         <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>740617.98539980256</v>
+        <v>164617.98540020152</v>
       </c>
       <c r="D3">
         <v>89397</v>
       </c>
       <c r="E3">
-        <v>877514.98539987789</v>
+        <v>301514.98540027672</v>
       </c>
       <c r="F3">
-        <v>8229999.9999999953</v>
+        <v>7479999.9999999981</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H3">
-        <v>8559437.0931400936</v>
+        <v>7762420.3039999977</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1886,39 +1885,39 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>43101</v>
+        <v>43466</v>
       </c>
       <c r="B2">
         <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>468162.81999999995</v>
+        <v>598117.98539990128</v>
       </c>
       <c r="D2">
         <v>89397</v>
       </c>
       <c r="E2">
-        <v>605059.82000007527</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" t="s">
-        <v>5</v>
+        <v>735014.98539997661</v>
+      </c>
+      <c r="F2">
+        <v>8229999.9999999953</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>8651812.1823107377</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -1926,28 +1925,28 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>43466</v>
+        <v>43831</v>
       </c>
       <c r="B3">
         <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>164617.98540020152</v>
+        <v>290674.49583810766</v>
       </c>
       <c r="D3">
         <v>89397</v>
       </c>
       <c r="E3">
-        <v>301514.98540027672</v>
+        <v>427571.4958381828</v>
       </c>
       <c r="F3">
-        <v>8999999.9999775514</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>9171077.2611176502</v>
+        <v>9132878.8059775531</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -1983,39 +1982,39 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>43101</v>
+        <v>43466</v>
       </c>
       <c r="B2">
         <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>468162.81999999995</v>
+        <v>164617.98540020152</v>
       </c>
       <c r="D2">
         <v>89397</v>
       </c>
       <c r="E2">
-        <v>605059.82000007527</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" t="s">
-        <v>5</v>
+        <v>301514.98540027672</v>
+      </c>
+      <c r="F2">
+        <v>8229999.9999999953</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>8499804.9703107402</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -2023,31 +2022,31 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>43466</v>
+        <v>43831</v>
       </c>
       <c r="B3">
         <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>598117.98539990128</v>
+        <v>164617.98540020152</v>
       </c>
       <c r="D3">
         <v>89397</v>
       </c>
       <c r="E3">
-        <v>735014.98539997661</v>
+        <v>301514.98540027672</v>
       </c>
       <c r="F3">
-        <v>8229999.9999999953</v>
+        <v>7479999.9999999981</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H3">
-        <v>8673106.0491400938</v>
+        <v>7889818.2239999976</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2080,39 +2079,39 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>43101</v>
+        <v>43466</v>
       </c>
       <c r="B2">
         <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>468162.81999999995</v>
+        <v>164617.98540020152</v>
       </c>
       <c r="D2">
         <v>89397</v>
       </c>
       <c r="E2">
-        <v>605059.82000007527</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" t="s">
-        <v>5</v>
+        <v>301514.98540027672</v>
+      </c>
+      <c r="F2">
+        <v>8229999.9999999953</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>8451271.9163107388</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -2120,7 +2119,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>43466</v>
+        <v>43831</v>
       </c>
       <c r="B3">
         <v>47500.000000075197</v>
@@ -2135,16 +2134,16 @@
         <v>301514.98540027672</v>
       </c>
       <c r="F3">
-        <v>8382551.3879766222</v>
+        <v>7479999.9999999981</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H3">
-        <v>8666610.5331167243</v>
+        <v>7719478.9159999946</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2177,39 +2176,39 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>43101</v>
+        <v>43466</v>
       </c>
       <c r="B2">
         <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>468162.81999999995</v>
+        <v>428138.37040346104</v>
       </c>
       <c r="D2">
         <v>89397</v>
       </c>
       <c r="E2">
-        <v>605059.82000007527</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" t="s">
-        <v>5</v>
+        <v>565035.37040353625</v>
+      </c>
+      <c r="F2">
+        <v>8229999.9999999953</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>8401691.2083107401</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -2217,31 +2216,31 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>43466</v>
+        <v>43831</v>
       </c>
       <c r="B3">
         <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>164617.98540020152</v>
+        <v>428138.37040346104</v>
       </c>
       <c r="D3">
         <v>89397</v>
       </c>
       <c r="E3">
-        <v>301514.98540027672</v>
+        <v>565035.37040353625</v>
       </c>
       <c r="F3">
-        <v>8229999.9999999953</v>
+        <v>7479999.9999999981</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H3">
-        <v>8457531.0571400952</v>
+        <v>7654589.2299999977</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2274,39 +2273,39 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>43101</v>
+        <v>43466</v>
       </c>
       <c r="B2">
         <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>468162.81999999995</v>
+        <v>358617.98539980507</v>
       </c>
       <c r="D2">
         <v>89397</v>
       </c>
       <c r="E2">
-        <v>605059.82000007527</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" t="s">
-        <v>5</v>
+        <v>495514.98539988021</v>
+      </c>
+      <c r="F2">
+        <v>8229999.9999999953</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>8404922.9663107377</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -2314,31 +2313,31 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>43466</v>
+        <v>43831</v>
       </c>
       <c r="B3">
         <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>336055.68840417598</v>
+        <v>358617.98539980524</v>
       </c>
       <c r="D3">
         <v>89397</v>
       </c>
       <c r="E3">
-        <v>472952.68840425112</v>
+        <v>495514.98539988039</v>
       </c>
       <c r="F3">
-        <v>8229999.9999999953</v>
+        <v>7479999.9999999981</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H3">
-        <v>8413681.6251400951</v>
+        <v>7616493.4259999963</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2371,39 +2370,39 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>43101</v>
+        <v>43466</v>
       </c>
       <c r="B2">
         <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>468162.81999999995</v>
+        <v>164617.98540020152</v>
       </c>
       <c r="D2">
         <v>89397</v>
       </c>
       <c r="E2">
-        <v>605059.82000007527</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" t="s">
-        <v>5</v>
+        <v>301514.98540027672</v>
+      </c>
+      <c r="F2">
+        <v>8229999.9999999953</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>8426433.5423107389</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -2411,31 +2410,31 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>43466</v>
+        <v>43831</v>
       </c>
       <c r="B3">
         <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>358617.98539980501</v>
+        <v>164617.98540020152</v>
       </c>
       <c r="D3">
         <v>89397</v>
       </c>
       <c r="E3">
-        <v>495514.98539988021</v>
+        <v>301514.98540027672</v>
       </c>
       <c r="F3">
-        <v>8621695.6702742185</v>
+        <v>7479999.9999999981</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H3">
-        <v>8806712.1494143177</v>
+        <v>7630597.6699999953</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2468,39 +2467,39 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>43101</v>
+        <v>43466</v>
       </c>
       <c r="B2">
         <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>468162.81999999995</v>
+        <v>358617.98539980507</v>
       </c>
       <c r="D2">
         <v>89397</v>
       </c>
       <c r="E2">
-        <v>605059.82000007527</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" t="s">
-        <v>5</v>
+        <v>495514.98539988021</v>
+      </c>
+      <c r="F2">
+        <v>8229999.9999999953</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>8439066.7343107387</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -2508,31 +2507,31 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>43466</v>
+        <v>43831</v>
       </c>
       <c r="B3">
         <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>164617.98540020152</v>
+        <v>358617.98539980507</v>
       </c>
       <c r="D3">
         <v>89397</v>
       </c>
       <c r="E3">
-        <v>301514.98540027672</v>
+        <v>495514.98539988021</v>
       </c>
       <c r="F3">
-        <v>8229999.9999999953</v>
+        <v>7479999.9999999981</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H3">
-        <v>8438738.6951400954</v>
+        <v>7667833.5499999961</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2565,39 +2564,39 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>43101</v>
+        <v>43466</v>
       </c>
       <c r="B2">
         <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>468162.81999999995</v>
+        <v>358617.98539980507</v>
       </c>
       <c r="D2">
         <v>89397</v>
       </c>
       <c r="E2">
-        <v>605059.82000007527</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" t="s">
-        <v>5</v>
+        <v>495514.98539988021</v>
+      </c>
+      <c r="F2">
+        <v>8229999.9999999953</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>8324544.5563107394</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -2605,31 +2604,31 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>43466</v>
+        <v>43831</v>
       </c>
       <c r="B3">
         <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>164617.98540020152</v>
+        <v>358617.98539980507</v>
       </c>
       <c r="D3">
         <v>89397</v>
       </c>
       <c r="E3">
-        <v>301514.98540027672</v>
+        <v>495514.98539988021</v>
       </c>
       <c r="F3">
-        <v>8229999.9999999953</v>
+        <v>7479999.9999999981</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H3">
-        <v>8378942.1091400944</v>
+        <v>7568058.5399999963</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2662,39 +2661,39 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>43101</v>
+        <v>43466</v>
       </c>
       <c r="B2">
         <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>468162.81999999995</v>
+        <v>740617.98539980256</v>
       </c>
       <c r="D2">
         <v>89397</v>
       </c>
       <c r="E2">
-        <v>605059.82000007527</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" t="s">
-        <v>5</v>
+        <v>877514.98539987789</v>
+      </c>
+      <c r="F2">
+        <v>8999999.9999775514</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>9163944.0222882964</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -2702,28 +2701,28 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>43466</v>
+        <v>43831</v>
       </c>
       <c r="B3">
         <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>358617.98539980501</v>
+        <v>622899.49583761534</v>
       </c>
       <c r="D3">
         <v>89397</v>
       </c>
       <c r="E3">
-        <v>495514.98539988021</v>
+        <v>759796.49583769066</v>
       </c>
       <c r="F3">
-        <v>8999999.9999775514</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>9221226.4311176501</v>
+        <v>9187857.7959775534</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -2759,39 +2758,39 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>43101</v>
+        <v>43466</v>
       </c>
       <c r="B2">
         <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>468162.81999999995</v>
+        <v>358617.98539980507</v>
       </c>
       <c r="D2">
         <v>89397</v>
       </c>
       <c r="E2">
-        <v>605059.82000007527</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" t="s">
-        <v>5</v>
+        <v>495514.98539988021</v>
+      </c>
+      <c r="F2">
+        <v>8724613.8495684564</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>8948392.7098792009</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -2799,31 +2798,31 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>43466</v>
+        <v>43831</v>
       </c>
       <c r="B3">
         <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>740617.98539980256</v>
+        <v>358617.98539980507</v>
       </c>
       <c r="D3">
         <v>89397</v>
       </c>
       <c r="E3">
-        <v>877514.98539987789</v>
+        <v>495514.98539988021</v>
       </c>
       <c r="F3">
-        <v>8999999.9999775514</v>
+        <v>7479999.9999999981</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H3">
-        <v>9178823.5011176523</v>
+        <v>7628032.6279999958</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2856,39 +2855,39 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>43101</v>
+        <v>43466</v>
       </c>
       <c r="B2">
         <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>468162.81999999995</v>
+        <v>740617.98539980256</v>
       </c>
       <c r="D2">
         <v>89397</v>
       </c>
       <c r="E2">
-        <v>605059.82000007527</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" t="s">
-        <v>5</v>
+        <v>877514.98539987789</v>
+      </c>
+      <c r="F2">
+        <v>8229999.9999999953</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>8507629.0463107377</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -2896,28 +2895,28 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>43466</v>
+        <v>43831</v>
       </c>
       <c r="B3">
         <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>358617.98539980501</v>
+        <v>622899.49583761534</v>
       </c>
       <c r="D3">
         <v>89397</v>
       </c>
       <c r="E3">
-        <v>495514.98539988021</v>
+        <v>759796.49583769066</v>
       </c>
       <c r="F3">
-        <v>8999999.9999775514</v>
+        <v>7479999.9999999981</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H3">
-        <v>9246731.1111176517</v>
+        <v>7704903.3319999976</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -2953,39 +2952,39 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>43101</v>
+        <v>43466</v>
       </c>
       <c r="B2">
         <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>468162.81999999995</v>
+        <v>740617.98539980256</v>
       </c>
       <c r="D2">
         <v>89397</v>
       </c>
       <c r="E2">
-        <v>605059.82000007527</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" t="s">
-        <v>5</v>
+        <v>877514.98539987789</v>
+      </c>
+      <c r="F2">
+        <v>8999999.9999775514</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>9298381.7302882969</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -2993,28 +2992,28 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>43466</v>
+        <v>43831</v>
       </c>
       <c r="B3">
         <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>740617.98539980256</v>
+        <v>1004899.4958376129</v>
       </c>
       <c r="D3">
         <v>89397</v>
       </c>
       <c r="E3">
-        <v>877514.98539987789</v>
+        <v>1141796.495837688</v>
       </c>
       <c r="F3">
-        <v>8229999.9999999953</v>
+        <v>10149302.975663755</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>8535857.4891400933</v>
+        <v>10440610.177663758</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -3050,39 +3049,39 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>43101</v>
+        <v>43466</v>
       </c>
       <c r="B2">
         <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>468162.81999999995</v>
+        <v>740617.98539980256</v>
       </c>
       <c r="D2">
         <v>89397</v>
       </c>
       <c r="E2">
-        <v>605059.82000007527</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" t="s">
-        <v>5</v>
+        <v>877514.98539987789</v>
+      </c>
+      <c r="F2">
+        <v>8442454.2726808209</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>8676342.840991566</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -3090,7 +3089,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>43466</v>
+        <v>43831</v>
       </c>
       <c r="B3">
         <v>47500.000000075197</v>
@@ -3105,16 +3104,16 @@
         <v>877514.98539987789</v>
       </c>
       <c r="F3">
-        <v>8999999.9999775514</v>
+        <v>7479999.9999999981</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H3">
-        <v>9322491.0931176525</v>
+        <v>7753849.8819999974</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -3147,39 +3146,39 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>43101</v>
+        <v>43466</v>
       </c>
       <c r="B2">
         <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>468162.81999999995</v>
+        <v>428138.37040346104</v>
       </c>
       <c r="D2">
         <v>89397</v>
       </c>
       <c r="E2">
-        <v>605059.82000007527</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" t="s">
-        <v>5</v>
+        <v>565035.37040353625</v>
+      </c>
+      <c r="F2">
+        <v>8229999.9999999953</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>8402152.338310739</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -3187,31 +3186,31 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>43466</v>
+        <v>43831</v>
       </c>
       <c r="B3">
         <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>740617.98539980256</v>
+        <v>428138.37040346104</v>
       </c>
       <c r="D3">
         <v>89397</v>
       </c>
       <c r="E3">
-        <v>877514.98539987789</v>
+        <v>565035.37040353625</v>
       </c>
       <c r="F3">
-        <v>8229999.9999999953</v>
+        <v>7479999.9999999981</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H3">
-        <v>8473804.7091400959</v>
+        <v>7690604.345999998</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -3244,39 +3243,39 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>43101</v>
+        <v>43466</v>
       </c>
       <c r="B2">
         <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>468162.81999999995</v>
+        <v>455617.98539999995</v>
       </c>
       <c r="D2">
         <v>89397</v>
       </c>
       <c r="E2">
-        <v>605059.82000007527</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" t="s">
-        <v>5</v>
+        <v>592514.98540007521</v>
+      </c>
+      <c r="F2">
+        <v>8675359.689767804</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>8829211.9160785489</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -3284,7 +3283,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>43466</v>
+        <v>43831</v>
       </c>
       <c r="B3">
         <v>47500.000000075197</v>
@@ -3299,16 +3298,16 @@
         <v>592514.98540007521</v>
       </c>
       <c r="F3">
-        <v>8723307.2508730888</v>
+        <v>7479999.9999999981</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H3">
-        <v>8879717.7400131878</v>
+        <v>7579952.9999999972</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -3317,6 +3316,200 @@
 </file>
 
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>43466</v>
+      </c>
+      <c r="B2">
+        <v>47500.000000075197</v>
+      </c>
+      <c r="C2">
+        <v>455617.98539999995</v>
+      </c>
+      <c r="D2">
+        <v>89397</v>
+      </c>
+      <c r="E2">
+        <v>592514.98540007521</v>
+      </c>
+      <c r="F2">
+        <v>8999999.9999775514</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>9151859.2262882963</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>43831</v>
+      </c>
+      <c r="B3">
+        <v>47500.000000075197</v>
+      </c>
+      <c r="C3">
+        <v>443449.49583800184</v>
+      </c>
+      <c r="D3">
+        <v>89397</v>
+      </c>
+      <c r="E3">
+        <v>580346.49583807704</v>
+      </c>
+      <c r="F3">
+        <v>8999999.9999775533</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>9108851.9999775533</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>43466</v>
+      </c>
+      <c r="B2">
+        <v>47500.000000075197</v>
+      </c>
+      <c r="C2">
+        <v>455617.98539999995</v>
+      </c>
+      <c r="D2">
+        <v>89397</v>
+      </c>
+      <c r="E2">
+        <v>592514.98540007521</v>
+      </c>
+      <c r="F2">
+        <v>8229999.9999999953</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>8364785.2263107393</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>43831</v>
+      </c>
+      <c r="B3">
+        <v>47500.000000075197</v>
+      </c>
+      <c r="C3">
+        <v>455617.98539999995</v>
+      </c>
+      <c r="D3">
+        <v>89397</v>
+      </c>
+      <c r="E3">
+        <v>592514.98540007521</v>
+      </c>
+      <c r="F3">
+        <v>7479999.9999999981</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3">
+        <v>7577795.9999999963</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -3353,39 +3546,39 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>43101</v>
+        <v>43466</v>
       </c>
       <c r="B2">
         <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>468162.81999999995</v>
+        <v>455617.98539999995</v>
       </c>
       <c r="D2">
         <v>89397</v>
       </c>
       <c r="E2">
-        <v>605059.82000007527</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" t="s">
-        <v>5</v>
+        <v>592514.98540007521</v>
+      </c>
+      <c r="F2">
+        <v>8229999.9999999953</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>8325028.606310741</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -3393,31 +3586,31 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>43466</v>
+        <v>43831</v>
       </c>
       <c r="B3">
         <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>358617.98539980501</v>
+        <v>455617.98539999995</v>
       </c>
       <c r="D3">
         <v>89397</v>
       </c>
       <c r="E3">
-        <v>495514.98539988021</v>
+        <v>592514.98540007521</v>
       </c>
       <c r="F3">
-        <v>8229999.9999999953</v>
+        <v>7479999.9999999981</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H3">
-        <v>8320823.8991400944</v>
+        <v>7511744.7299999967</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -3450,39 +3643,39 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>43101</v>
+        <v>43466</v>
       </c>
       <c r="B2">
         <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>468162.81999999995</v>
+        <v>740617.98539980256</v>
       </c>
       <c r="D2">
         <v>89397</v>
       </c>
       <c r="E2">
-        <v>605059.82000007527</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" t="s">
-        <v>5</v>
+        <v>877514.98539987789</v>
+      </c>
+      <c r="F2">
+        <v>8999999.9999775514</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>9235340.4062882941</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -3490,28 +3683,28 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>43466</v>
+        <v>43831</v>
       </c>
       <c r="B3">
         <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>455617.98539999995</v>
+        <v>719899.49583781033</v>
       </c>
       <c r="D3">
         <v>89397</v>
       </c>
       <c r="E3">
-        <v>592514.98540007521</v>
+        <v>856796.49583788565</v>
       </c>
       <c r="F3">
-        <v>8999999.9999775514</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>9095331.579117652</v>
+        <v>8291125.7399991108</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -3547,39 +3740,39 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>43101</v>
+        <v>43466</v>
       </c>
       <c r="B2">
         <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>468162.81999999995</v>
+        <v>455617.98539999995</v>
       </c>
       <c r="D2">
         <v>89397</v>
       </c>
       <c r="E2">
-        <v>605059.82000007527</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" t="s">
-        <v>5</v>
+        <v>592514.98540007521</v>
+      </c>
+      <c r="F2">
+        <v>8655277.4687817339</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>8855604.5950924754</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -3587,31 +3780,31 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>43466</v>
+        <v>43831</v>
       </c>
       <c r="B3">
         <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>740617.98539980256</v>
+        <v>455617.98539999995</v>
       </c>
       <c r="D3">
         <v>89397</v>
       </c>
       <c r="E3">
-        <v>877514.98539987789</v>
+        <v>592514.98540007521</v>
       </c>
       <c r="F3">
-        <v>8811971.9339028448</v>
+        <v>7479999.9999999981</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H3">
-        <v>9063407.313042948</v>
+        <v>7692695.0099999979</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -3644,39 +3837,39 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>43101</v>
+        <v>43466</v>
       </c>
       <c r="B2">
         <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>468162.81999999995</v>
+        <v>358617.98539980507</v>
       </c>
       <c r="D2">
         <v>89397</v>
       </c>
       <c r="E2">
-        <v>605059.82000007527</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" t="s">
-        <v>5</v>
+        <v>495514.98539988021</v>
+      </c>
+      <c r="F2">
+        <v>8999999.9999775514</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>9185173.4262882955</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -3684,31 +3877,31 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>43466</v>
+        <v>43831</v>
       </c>
       <c r="B3">
         <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>455617.98539999995</v>
+        <v>358617.98539980507</v>
       </c>
       <c r="D3">
         <v>89397</v>
       </c>
       <c r="E3">
-        <v>592514.98540007521</v>
+        <v>495514.98539988021</v>
       </c>
       <c r="F3">
-        <v>8999999.9999775514</v>
+        <v>7479999.9999999981</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H3">
-        <v>9222322.1591176502</v>
+        <v>7663949.7199999951</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -3741,39 +3934,39 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>43101</v>
+        <v>43466</v>
       </c>
       <c r="B2">
         <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>468162.81999999995</v>
+        <v>164617.98540020152</v>
       </c>
       <c r="D2">
         <v>89397</v>
       </c>
       <c r="E2">
-        <v>605059.82000007527</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" t="s">
-        <v>5</v>
+        <v>301514.98540027672</v>
+      </c>
+      <c r="F2">
+        <v>8999999.9999775514</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>9215604.6462882962</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -3781,31 +3974,31 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>43466</v>
+        <v>43831</v>
       </c>
       <c r="B3">
         <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>358617.98539980501</v>
+        <v>164617.98540020152</v>
       </c>
       <c r="D3">
         <v>89397</v>
       </c>
       <c r="E3">
-        <v>495514.98539988021</v>
+        <v>301514.98540027672</v>
       </c>
       <c r="F3">
-        <v>8999999.9999775514</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>9200471.499117652</v>
+        <v>9160152.0699775536</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -3838,39 +4031,39 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>43101</v>
+        <v>43466</v>
       </c>
       <c r="B2">
         <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>468162.81999999995</v>
+        <v>358617.98539980507</v>
       </c>
       <c r="D2">
         <v>89397</v>
       </c>
       <c r="E2">
-        <v>605059.82000007527</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" t="s">
-        <v>5</v>
+        <v>495514.98539988021</v>
+      </c>
+      <c r="F2">
+        <v>8229999.9999999953</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>8396750.7063107397</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -3878,31 +4071,31 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>43466</v>
+        <v>43831</v>
       </c>
       <c r="B3">
         <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>164617.98540020152</v>
+        <v>358617.98539980507</v>
       </c>
       <c r="D3">
         <v>89397</v>
       </c>
       <c r="E3">
-        <v>301514.98540027672</v>
+        <v>495514.98539988021</v>
       </c>
       <c r="F3">
-        <v>8229999.9999999953</v>
+        <v>7479999.9999999981</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H3">
-        <v>8455084.829140095</v>
+        <v>7666027.3499999968</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
This commit contains the MTOM March 2019 Pre-release model run. This includes updated ensemble forecast, output data, model files and ruleset.
Also in this commit:

Removed development ruleset files.

Removed old ruleset and model files.

Updated model file name manager for the new CRSS DMI output slots.

Renamed updated and tested model file and ruleset using the proper naming convention.
</commit_message>
<xml_diff>
--- a/Output Data/MtomToCrss_Annual.xlsx
+++ b/Output Data/MtomToCrss_Annual.xlsx
@@ -12,45 +12,43 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="12570" windowHeight="13590"/>
   </bookViews>
   <sheets>
-    <sheet name="Trace38" sheetId="39" r:id="rId1"/>
-    <sheet name="Trace37" sheetId="38" r:id="rId2"/>
-    <sheet name="Trace36" sheetId="37" r:id="rId3"/>
-    <sheet name="Trace35" sheetId="36" r:id="rId4"/>
-    <sheet name="Trace34" sheetId="35" r:id="rId5"/>
-    <sheet name="Trace33" sheetId="34" r:id="rId6"/>
-    <sheet name="Trace32" sheetId="33" r:id="rId7"/>
-    <sheet name="Trace31" sheetId="32" r:id="rId8"/>
-    <sheet name="Trace30" sheetId="31" r:id="rId9"/>
-    <sheet name="Trace29" sheetId="30" r:id="rId10"/>
-    <sheet name="Trace28" sheetId="29" r:id="rId11"/>
-    <sheet name="Trace27" sheetId="28" r:id="rId12"/>
-    <sheet name="Trace26" sheetId="27" r:id="rId13"/>
-    <sheet name="Trace25" sheetId="26" r:id="rId14"/>
-    <sheet name="Trace24" sheetId="25" r:id="rId15"/>
-    <sheet name="Trace23" sheetId="24" r:id="rId16"/>
-    <sheet name="Trace22" sheetId="23" r:id="rId17"/>
-    <sheet name="Trace21" sheetId="22" r:id="rId18"/>
-    <sheet name="Trace20" sheetId="21" r:id="rId19"/>
-    <sheet name="Trace19" sheetId="20" r:id="rId20"/>
-    <sheet name="Trace18" sheetId="19" r:id="rId21"/>
-    <sheet name="Trace17" sheetId="18" r:id="rId22"/>
-    <sheet name="Trace16" sheetId="17" r:id="rId23"/>
-    <sheet name="Trace15" sheetId="16" r:id="rId24"/>
-    <sheet name="Trace14" sheetId="15" r:id="rId25"/>
-    <sheet name="Trace13" sheetId="14" r:id="rId26"/>
-    <sheet name="Trace12" sheetId="13" r:id="rId27"/>
-    <sheet name="Trace11" sheetId="12" r:id="rId28"/>
-    <sheet name="Trace10" sheetId="11" r:id="rId29"/>
-    <sheet name="Trace9" sheetId="10" r:id="rId30"/>
-    <sheet name="Trace8" sheetId="9" r:id="rId31"/>
-    <sheet name="Trace7" sheetId="8" r:id="rId32"/>
-    <sheet name="Trace6" sheetId="7" r:id="rId33"/>
-    <sheet name="Trace5" sheetId="6" r:id="rId34"/>
-    <sheet name="Trace4" sheetId="5" r:id="rId35"/>
-    <sheet name="Trace3" sheetId="4" r:id="rId36"/>
-    <sheet name="Trace2" sheetId="3" r:id="rId37"/>
-    <sheet name="Trace1" sheetId="2" r:id="rId38"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId39"/>
+    <sheet name="Trace38" sheetId="37" r:id="rId1"/>
+    <sheet name="Trace37" sheetId="36" r:id="rId2"/>
+    <sheet name="Trace36" sheetId="35" r:id="rId3"/>
+    <sheet name="Trace35" sheetId="34" r:id="rId4"/>
+    <sheet name="Trace34" sheetId="33" r:id="rId5"/>
+    <sheet name="Trace33" sheetId="32" r:id="rId6"/>
+    <sheet name="Trace32" sheetId="31" r:id="rId7"/>
+    <sheet name="Trace31" sheetId="30" r:id="rId8"/>
+    <sheet name="Trace30" sheetId="29" r:id="rId9"/>
+    <sheet name="Trace29" sheetId="28" r:id="rId10"/>
+    <sheet name="Trace28" sheetId="27" r:id="rId11"/>
+    <sheet name="Trace27" sheetId="26" r:id="rId12"/>
+    <sheet name="Trace26" sheetId="25" r:id="rId13"/>
+    <sheet name="Trace25" sheetId="24" r:id="rId14"/>
+    <sheet name="Trace24" sheetId="23" r:id="rId15"/>
+    <sheet name="Trace23" sheetId="22" r:id="rId16"/>
+    <sheet name="Trace22" sheetId="21" r:id="rId17"/>
+    <sheet name="Trace21" sheetId="20" r:id="rId18"/>
+    <sheet name="Trace20" sheetId="19" r:id="rId19"/>
+    <sheet name="Trace19" sheetId="18" r:id="rId20"/>
+    <sheet name="Trace18" sheetId="17" r:id="rId21"/>
+    <sheet name="Trace17" sheetId="16" r:id="rId22"/>
+    <sheet name="Trace16" sheetId="15" r:id="rId23"/>
+    <sheet name="Trace15" sheetId="14" r:id="rId24"/>
+    <sheet name="Trace14" sheetId="13" r:id="rId25"/>
+    <sheet name="Trace13" sheetId="12" r:id="rId26"/>
+    <sheet name="Trace12" sheetId="11" r:id="rId27"/>
+    <sheet name="Trace11" sheetId="10" r:id="rId28"/>
+    <sheet name="Trace10" sheetId="9" r:id="rId29"/>
+    <sheet name="Trace9" sheetId="8" r:id="rId30"/>
+    <sheet name="Trace8" sheetId="7" r:id="rId31"/>
+    <sheet name="Trace7" sheetId="6" r:id="rId32"/>
+    <sheet name="Trace6" sheetId="5" r:id="rId33"/>
+    <sheet name="Trace5" sheetId="4" r:id="rId34"/>
+    <sheet name="Trace4" sheetId="3" r:id="rId35"/>
+    <sheet name="Trace3" sheetId="2" r:id="rId36"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId37"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -62,12 +60,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="10">
   <si>
     <t>ICS Credits.BiNationalICS_CA</t>
   </si>
   <si>
-    <t>ICS Credits.ExtraordinaryConservationICS_CA</t>
+    <t>ICS Credits.ExtraordinaryConservationICS_IID</t>
+  </si>
+  <si>
+    <t>ICS Credits.ExtraordinaryConservationICS_MWD</t>
+  </si>
+  <si>
+    <t>ICS Credits.ExtraordinaryConservationICS_NV</t>
   </si>
   <si>
     <t>ICS Credits.SystemEfficiencyICS_CA</t>
@@ -407,13 +411,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -438,8 +442,14 @@
       <c r="I1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -447,28 +457,34 @@
         <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>164617.98540020152</v>
+        <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>89397</v>
+        <v>175186.8647267684</v>
       </c>
       <c r="E2">
-        <v>301514.98540027672</v>
+        <v>173967.18169986518</v>
       </c>
       <c r="F2">
-        <v>8229999.9999999953</v>
+        <v>89397</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <v>362083.96322684357</v>
       </c>
       <c r="H2">
-        <v>8397147.5063107386</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="I2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>9198607.3185606264</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -476,25 +492,31 @@
         <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>164617.98540020172</v>
+        <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>89397</v>
+        <v>169931.25878496529</v>
       </c>
       <c r="E3">
-        <v>301514.9854002769</v>
+        <v>196393.16624886921</v>
       </c>
       <c r="F3">
-        <v>7479999.9999999981</v>
+        <v>89397</v>
       </c>
       <c r="G3">
-        <v>2</v>
+        <v>356828.40433004237</v>
       </c>
       <c r="H3">
-        <v>7590981.0259999959</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="I3">
         <v>1</v>
+      </c>
+      <c r="J3">
+        <v>8340981.0259991111</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -504,13 +526,13 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -535,8 +557,14 @@
       <c r="I1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -544,28 +572,34 @@
         <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>740617.98539980256</v>
+        <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>89397</v>
+        <v>690617.8868998026</v>
       </c>
       <c r="E2">
+        <v>173967.18169986518</v>
+      </c>
+      <c r="F2">
+        <v>89397</v>
+      </c>
+      <c r="G2">
         <v>877514.98539987789</v>
       </c>
-      <c r="F2">
-        <v>8229999.9999999953</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
       <c r="H2">
-        <v>8498842.6363107394</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="I2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>9275967.7685606275</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -573,25 +607,31 @@
         <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>740617.98539980256</v>
+        <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>89397</v>
+        <v>572899.35029261373</v>
       </c>
       <c r="E3">
-        <v>877514.98539987789</v>
+        <v>196393.16624886921</v>
       </c>
       <c r="F3">
-        <v>7479999.9999999981</v>
+        <v>89397</v>
       </c>
       <c r="G3">
-        <v>2</v>
+        <v>759796.49583769089</v>
       </c>
       <c r="H3">
-        <v>7646147.9299999969</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="I3">
         <v>1</v>
+      </c>
+      <c r="J3">
+        <v>9166147.929977553</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -601,13 +641,13 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -632,8 +672,14 @@
       <c r="I1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -641,28 +687,34 @@
         <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>598117.98539990128</v>
+        <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>89397</v>
+        <v>548117.88689990132</v>
       </c>
       <c r="E2">
+        <v>173967.18169986518</v>
+      </c>
+      <c r="F2">
+        <v>89397</v>
+      </c>
+      <c r="G2">
         <v>735014.98539997661</v>
       </c>
-      <c r="F2">
-        <v>8229999.9999999953</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
       <c r="H2">
-        <v>8413747.2263107393</v>
+        <v>8229999.9999999981</v>
       </c>
       <c r="I2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>8447920.5585830733</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -670,24 +722,30 @@
         <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>866674.49583770882</v>
+        <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>89397</v>
+        <v>816674.35029270698</v>
       </c>
       <c r="E3">
+        <v>196393.16624886921</v>
+      </c>
+      <c r="F3">
+        <v>89397</v>
+      </c>
+      <c r="G3">
         <v>1003571.4958377838</v>
       </c>
-      <c r="F3">
+      <c r="H3">
         <v>8999999.9999775533</v>
       </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3">
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
         <v>9263906.2799775526</v>
       </c>
-      <c r="I3">
+      <c r="K3">
         <v>0</v>
       </c>
     </row>
@@ -698,13 +756,13 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -729,8 +787,14 @@
       <c r="I1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -738,28 +802,34 @@
         <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>455617.98539999995</v>
+        <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>89397</v>
+        <v>405617.88689999998</v>
       </c>
       <c r="E2">
+        <v>173967.18169986518</v>
+      </c>
+      <c r="F2">
+        <v>89397</v>
+      </c>
+      <c r="G2">
         <v>592514.98540007521</v>
       </c>
-      <c r="F2">
-        <v>8229999.9999999953</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
       <c r="H2">
-        <v>8370370.4563107397</v>
+        <v>8984161.4499797802</v>
       </c>
       <c r="I2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>9147860.4785628542</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -767,24 +837,30 @@
         <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>455617.98539999995</v>
+        <v>50000.0985</v>
       </c>
       <c r="D3">
-        <v>89397</v>
+        <v>405617.88689999981</v>
       </c>
       <c r="E3">
-        <v>592514.98540007521</v>
+        <v>202467.18169986518</v>
       </c>
       <c r="F3">
+        <v>89397</v>
+      </c>
+      <c r="G3">
+        <v>592514.98540007509</v>
+      </c>
+      <c r="H3">
         <v>7479999.9999999981</v>
       </c>
-      <c r="G3">
+      <c r="I3">
         <v>2</v>
       </c>
-      <c r="H3">
+      <c r="J3">
         <v>7609167.7799999956</v>
       </c>
-      <c r="I3">
+      <c r="K3">
         <v>1</v>
       </c>
     </row>
@@ -795,13 +871,13 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -826,8 +902,14 @@
       <c r="I1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -835,28 +917,34 @@
         <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>598117.98539990128</v>
+        <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>89397</v>
+        <v>548117.88689990132</v>
       </c>
       <c r="E2">
+        <v>173967.18169986518</v>
+      </c>
+      <c r="F2">
+        <v>89397</v>
+      </c>
+      <c r="G2">
         <v>735014.98539997661</v>
       </c>
-      <c r="F2">
-        <v>8715847.906304691</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
       <c r="H2">
-        <v>8895069.6426154338</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="I2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>9212653.5085606258</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -864,25 +952,31 @@
         <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>598117.98539990128</v>
+        <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>89397</v>
+        <v>531674.35029290419</v>
       </c>
       <c r="E3">
-        <v>735014.98539997661</v>
+        <v>196393.16624886921</v>
       </c>
       <c r="F3">
-        <v>7479999.9999999981</v>
+        <v>89397</v>
       </c>
       <c r="G3">
-        <v>2</v>
+        <v>718571.49583798135</v>
       </c>
       <c r="H3">
-        <v>7584398.0899999952</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="I3">
         <v>1</v>
+      </c>
+      <c r="J3">
+        <v>9104398.0899775531</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -892,13 +986,13 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -923,8 +1017,14 @@
       <c r="I1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -932,28 +1032,34 @@
         <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>358617.98539980507</v>
+        <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>89397</v>
+        <v>309048.56689980475</v>
       </c>
       <c r="E2">
-        <v>495514.98539988021</v>
+        <v>173967.18169986518</v>
       </c>
       <c r="F2">
-        <v>8229999.9999999953</v>
+        <v>89397</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <v>495945.66539987986</v>
       </c>
       <c r="H2">
-        <v>8393510.7663107384</v>
+        <v>8229999.9999999981</v>
       </c>
       <c r="I2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>8443584.0885830726</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -961,24 +1067,30 @@
         <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>358617.98539980507</v>
+        <v>50000.0985</v>
       </c>
       <c r="D3">
-        <v>89397</v>
+        <v>309048.56689980457</v>
       </c>
       <c r="E3">
-        <v>495514.98539988021</v>
+        <v>202467.18169986518</v>
       </c>
       <c r="F3">
-        <v>7640907.5547923325</v>
+        <v>89397</v>
       </c>
       <c r="G3">
-        <v>3</v>
+        <v>495945.66539987968</v>
       </c>
       <c r="H3">
-        <v>7772554.9947923291</v>
+        <v>7479999.9999999981</v>
       </c>
       <c r="I3">
+        <v>2</v>
+      </c>
+      <c r="J3">
+        <v>7611647.4399999948</v>
+      </c>
+      <c r="K3">
         <v>1</v>
       </c>
     </row>
@@ -989,13 +1101,13 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1020,8 +1132,14 @@
       <c r="I1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -1029,28 +1147,34 @@
         <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>358617.98539980507</v>
+        <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>89397</v>
+        <v>309048.56689980475</v>
       </c>
       <c r="E2">
-        <v>495514.98539988021</v>
+        <v>173967.18169986518</v>
       </c>
       <c r="F2">
-        <v>8229999.9999999953</v>
+        <v>89397</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <v>495945.66539987986</v>
       </c>
       <c r="H2">
-        <v>8365625.1263107378</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="I2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>9179778.2385606281</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -1058,25 +1182,31 @@
         <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>358617.98539980507</v>
+        <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>89397</v>
+        <v>202777.10989261558</v>
       </c>
       <c r="E3">
-        <v>495514.98539988021</v>
+        <v>196393.16624886921</v>
       </c>
       <c r="F3">
-        <v>7479999.9999999981</v>
+        <v>89397</v>
       </c>
       <c r="G3">
-        <v>2</v>
+        <v>389674.25543769269</v>
       </c>
       <c r="H3">
-        <v>7588713.6499999976</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="I3">
         <v>1</v>
+      </c>
+      <c r="J3">
+        <v>8338713.64999911</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1086,13 +1216,13 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1117,8 +1247,14 @@
       <c r="I1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -1126,28 +1262,34 @@
         <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>598117.98539990128</v>
+        <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>89397</v>
+        <v>548117.88689990132</v>
       </c>
       <c r="E2">
+        <v>173967.18169986518</v>
+      </c>
+      <c r="F2">
+        <v>89397</v>
+      </c>
+      <c r="G2">
         <v>735014.98539997661</v>
       </c>
-      <c r="F2">
-        <v>8999999.9999775514</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
       <c r="H2">
-        <v>9192742.7262882963</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="I2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>9239257.7585606277</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -1155,25 +1297,31 @@
         <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>598117.98539990128</v>
+        <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>89397</v>
+        <v>434674.35029270942</v>
       </c>
       <c r="E3">
-        <v>735014.98539997661</v>
+        <v>196393.16624886921</v>
       </c>
       <c r="F3">
-        <v>7479999.9999999981</v>
+        <v>89397</v>
       </c>
       <c r="G3">
-        <v>2</v>
+        <v>621571.49583778658</v>
       </c>
       <c r="H3">
-        <v>7585477.679999995</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="I3">
         <v>1</v>
+      </c>
+      <c r="J3">
+        <v>9105477.679977553</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1183,13 +1331,13 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1214,8 +1362,14 @@
       <c r="I1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -1223,28 +1377,34 @@
         <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>740617.98539980256</v>
+        <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>89397</v>
+        <v>690617.8868998026</v>
       </c>
       <c r="E2">
+        <v>173967.18169986518</v>
+      </c>
+      <c r="F2">
+        <v>89397</v>
+      </c>
+      <c r="G2">
         <v>877514.98539987789</v>
       </c>
-      <c r="F2">
-        <v>8999999.9999775514</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
       <c r="H2">
-        <v>9216683.7862882949</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="I2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>9253998.8485606275</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -1252,24 +1412,30 @@
         <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>862399.49583771161</v>
+        <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>89397</v>
+        <v>812399.35029270977</v>
       </c>
       <c r="E3">
+        <v>196393.16624886921</v>
+      </c>
+      <c r="F3">
+        <v>89397</v>
+      </c>
+      <c r="G3">
         <v>999296.4958377867</v>
       </c>
-      <c r="F3">
-        <v>8574687.8485893924</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
       <c r="H3">
-        <v>8715315.8785893936</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>9140628.0299775563</v>
+      </c>
+      <c r="K3">
         <v>0</v>
       </c>
     </row>
@@ -1280,13 +1446,13 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1311,8 +1477,14 @@
       <c r="I1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -1320,28 +1492,34 @@
         <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>740617.98539980256</v>
+        <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>89397</v>
+        <v>690617.8868998026</v>
       </c>
       <c r="E2">
+        <v>173967.18169986518</v>
+      </c>
+      <c r="F2">
+        <v>89397</v>
+      </c>
+      <c r="G2">
         <v>877514.98539987789</v>
       </c>
-      <c r="F2">
-        <v>8633842.735802548</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
       <c r="H2">
-        <v>8645148.1321132928</v>
+        <v>8229999.9999999981</v>
       </c>
       <c r="I2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>8317324.9385830723</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -1349,24 +1527,30 @@
         <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>1004899.4958376131</v>
+        <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>89397</v>
+        <v>954899.35029261105</v>
       </c>
       <c r="E3">
-        <v>1141796.4958376884</v>
+        <v>196393.16624886921</v>
       </c>
       <c r="F3">
+        <v>89397</v>
+      </c>
+      <c r="G3">
+        <v>1141796.495837688</v>
+      </c>
+      <c r="H3">
         <v>8999999.9999775533</v>
       </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3">
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
         <v>9203484.9599775542</v>
       </c>
-      <c r="I3">
+      <c r="K3">
         <v>0</v>
       </c>
     </row>
@@ -1377,13 +1561,13 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1408,8 +1592,14 @@
       <c r="I1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -1417,28 +1607,34 @@
         <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>740617.98539980256</v>
+        <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>89397</v>
+        <v>690617.8868998026</v>
       </c>
       <c r="E2">
+        <v>173967.18169986518</v>
+      </c>
+      <c r="F2">
+        <v>89397</v>
+      </c>
+      <c r="G2">
         <v>877514.98539987789</v>
       </c>
-      <c r="F2">
-        <v>8999999.9999775514</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
       <c r="H2">
-        <v>9099017.5382882971</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="I2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>9142203.1085606273</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -1446,24 +1642,30 @@
         <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>1004899.4958376129</v>
+        <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>89397</v>
+        <v>954899.35029261105</v>
       </c>
       <c r="E3">
+        <v>196393.16624886921</v>
+      </c>
+      <c r="F3">
+        <v>89397</v>
+      </c>
+      <c r="G3">
         <v>1141796.495837688</v>
       </c>
-      <c r="F3">
+      <c r="H3">
         <v>8999999.9999775533</v>
       </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3">
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
         <v>8910372.509977553</v>
       </c>
-      <c r="I3">
+      <c r="K3">
         <v>0</v>
       </c>
     </row>
@@ -1474,13 +1676,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1505,8 +1707,14 @@
       <c r="I1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -1514,54 +1722,66 @@
         <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>164617.98540020152</v>
+        <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>89397</v>
+        <v>175186.8647267684</v>
       </c>
       <c r="E2">
-        <v>301514.98540027672</v>
+        <v>173967.18169986518</v>
       </c>
       <c r="F2">
-        <v>8867764.5246292893</v>
+        <v>89397</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <v>362083.96322684357</v>
       </c>
       <c r="H2">
-        <v>9025050.8709400352</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="I2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>9195953.6685606278</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
       <c r="B3">
-        <v>47500.000000075197</v>
+        <v>23750.000000037599</v>
       </c>
       <c r="C3">
-        <v>164617.98540020152</v>
+        <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>89397</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>301514.98540027672</v>
+        <v>196393.16624886921</v>
       </c>
       <c r="F3">
-        <v>7479999.9999999981</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <v>2</v>
+        <v>73750.145545039501</v>
       </c>
       <c r="H3">
-        <v>7615931.8499999968</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="I3">
         <v>1</v>
+      </c>
+      <c r="J3">
+        <v>9135931.8499775529</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1571,13 +1791,13 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1602,8 +1822,14 @@
       <c r="I1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -1611,28 +1837,34 @@
         <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>740617.98539980256</v>
+        <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>89397</v>
+        <v>690617.8868998026</v>
       </c>
       <c r="E2">
+        <v>173967.18169986518</v>
+      </c>
+      <c r="F2">
+        <v>89397</v>
+      </c>
+      <c r="G2">
         <v>877514.98539987789</v>
       </c>
-      <c r="F2">
-        <v>8999999.9999775514</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
       <c r="H2">
-        <v>9148785.5442882963</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="I2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>9180315.9605606291</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -1640,24 +1872,30 @@
         <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>1004899.4958376129</v>
+        <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>89397</v>
+        <v>954899.35029261105</v>
       </c>
       <c r="E3">
+        <v>196393.16624886921</v>
+      </c>
+      <c r="F3">
+        <v>89397</v>
+      </c>
+      <c r="G3">
         <v>1141796.495837688</v>
       </c>
-      <c r="F3">
-        <v>8999999.9999775533</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
       <c r="H3">
-        <v>9061671.6859775521</v>
+        <v>10992555.326922728</v>
       </c>
       <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>11054227.012922728</v>
+      </c>
+      <c r="K3">
         <v>0</v>
       </c>
     </row>
@@ -1668,13 +1906,13 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1699,8 +1937,14 @@
       <c r="I1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -1708,28 +1952,34 @@
         <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>740617.98539980256</v>
+        <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>89397</v>
+        <v>690617.8868998026</v>
       </c>
       <c r="E2">
+        <v>173967.18169986518</v>
+      </c>
+      <c r="F2">
+        <v>89397</v>
+      </c>
+      <c r="G2">
         <v>877514.98539987789</v>
       </c>
-      <c r="F2">
-        <v>8229999.9999999953</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
       <c r="H2">
-        <v>8543052.252310738</v>
+        <v>10781723.845268941</v>
       </c>
       <c r="I2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>11079329.129852016</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -1737,24 +1987,30 @@
         <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>1004899.4958376129</v>
+        <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>89397</v>
+        <v>954899.35029261105</v>
       </c>
       <c r="E3">
+        <v>196393.16624886921</v>
+      </c>
+      <c r="F3">
+        <v>89397</v>
+      </c>
+      <c r="G3">
         <v>1141796.495837688</v>
       </c>
-      <c r="F3">
-        <v>11134627.059672041</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
       <c r="H3">
-        <v>11263145.791672042</v>
+        <v>10483416.252694307</v>
       </c>
       <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>10611934.984694308</v>
+      </c>
+      <c r="K3">
         <v>0</v>
       </c>
     </row>
@@ -1765,13 +2021,13 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1796,8 +2052,14 @@
       <c r="I1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -1805,28 +2067,34 @@
         <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>164617.98540020152</v>
+        <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>89397</v>
+        <v>175186.8647267684</v>
       </c>
       <c r="E2">
-        <v>301514.98540027672</v>
+        <v>173967.18169986518</v>
       </c>
       <c r="F2">
-        <v>8229999.9999999953</v>
+        <v>89397</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <v>362083.96322684357</v>
       </c>
       <c r="H2">
-        <v>8391462.0063107405</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="I2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>9186224.8985606264</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -1834,24 +2102,30 @@
         <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>164617.98540020152</v>
+        <v>50000.0985</v>
       </c>
       <c r="D3">
-        <v>89397</v>
+        <v>175186.86472676822</v>
       </c>
       <c r="E3">
-        <v>301514.98540027672</v>
+        <v>202467.18169986518</v>
       </c>
       <c r="F3">
+        <v>89397</v>
+      </c>
+      <c r="G3">
+        <v>362083.96322684339</v>
+      </c>
+      <c r="H3">
         <v>7479999.9999999981</v>
       </c>
-      <c r="G3">
+      <c r="I3">
         <v>2</v>
       </c>
-      <c r="H3">
+      <c r="J3">
         <v>7762420.3039999977</v>
       </c>
-      <c r="I3">
+      <c r="K3">
         <v>1</v>
       </c>
     </row>
@@ -1862,13 +2136,13 @@
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1893,8 +2167,14 @@
       <c r="I1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -1902,28 +2182,34 @@
         <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>598117.98539990128</v>
+        <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>89397</v>
+        <v>548117.88689990132</v>
       </c>
       <c r="E2">
+        <v>173967.18169986518</v>
+      </c>
+      <c r="F2">
+        <v>89397</v>
+      </c>
+      <c r="G2">
         <v>735014.98539997661</v>
       </c>
-      <c r="F2">
-        <v>8229999.9999999953</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
       <c r="H2">
-        <v>8651812.1823107377</v>
+        <v>8229999.9999999981</v>
       </c>
       <c r="I2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>8528404.1665830705</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -1931,24 +2217,30 @@
         <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>290674.49583810766</v>
+        <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>89397</v>
+        <v>240674.35029310576</v>
       </c>
       <c r="E3">
+        <v>196393.16624886921</v>
+      </c>
+      <c r="F3">
+        <v>89397</v>
+      </c>
+      <c r="G3">
         <v>427571.4958381828</v>
       </c>
-      <c r="F3">
+      <c r="H3">
         <v>8999999.9999775533</v>
       </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3">
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
         <v>9132878.8059775531</v>
       </c>
-      <c r="I3">
+      <c r="K3">
         <v>0</v>
       </c>
     </row>
@@ -1959,13 +2251,13 @@
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1990,8 +2282,14 @@
       <c r="I1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -1999,28 +2297,34 @@
         <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>164617.98540020152</v>
+        <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>89397</v>
+        <v>175186.8647267684</v>
       </c>
       <c r="E2">
-        <v>301514.98540027672</v>
+        <v>173967.18169986518</v>
       </c>
       <c r="F2">
-        <v>8229999.9999999953</v>
+        <v>89397</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <v>362083.96322684357</v>
       </c>
       <c r="H2">
-        <v>8499804.9703107402</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="I2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>9277531.6285606269</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -2028,25 +2332,31 @@
         <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>164617.98540020152</v>
+        <v>50000.0985</v>
       </c>
       <c r="D3">
-        <v>89397</v>
+        <v>312431.25878486666</v>
       </c>
       <c r="E3">
-        <v>301514.98540027672</v>
+        <v>196393.16624886921</v>
       </c>
       <c r="F3">
-        <v>7479999.9999999981</v>
+        <v>89397</v>
       </c>
       <c r="G3">
-        <v>2</v>
+        <v>499328.4043299437</v>
       </c>
       <c r="H3">
-        <v>7889818.2239999976</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="I3">
         <v>1</v>
+      </c>
+      <c r="J3">
+        <v>8639818.2239991091</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2056,13 +2366,13 @@
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2087,8 +2397,14 @@
       <c r="I1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -2096,54 +2412,66 @@
         <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>164617.98540020152</v>
+        <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>89397</v>
+        <v>175186.8647267684</v>
       </c>
       <c r="E2">
-        <v>301514.98540027672</v>
+        <v>173967.18169986518</v>
       </c>
       <c r="F2">
-        <v>8229999.9999999953</v>
+        <v>89397</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <v>362083.96322684357</v>
       </c>
       <c r="H2">
-        <v>8451271.9163107388</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="I2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>9239105.7565606255</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
       <c r="B3">
-        <v>47500.000000075197</v>
+        <v>23750.000000037599</v>
       </c>
       <c r="C3">
-        <v>164617.98540020152</v>
+        <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>89397</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>301514.98540027672</v>
+        <v>196393.16624886921</v>
       </c>
       <c r="F3">
-        <v>7479999.9999999981</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <v>2</v>
+        <v>73750.145545039501</v>
       </c>
       <c r="H3">
-        <v>7719478.9159999946</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="I3">
         <v>1</v>
+      </c>
+      <c r="J3">
+        <v>9239478.9159775525</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2153,13 +2481,13 @@
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2184,8 +2512,14 @@
       <c r="I1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -2193,54 +2527,66 @@
         <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>428138.37040346104</v>
+        <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>89397</v>
+        <v>175186.8647267684</v>
       </c>
       <c r="E2">
-        <v>565035.37040353625</v>
+        <v>173967.18169986518</v>
       </c>
       <c r="F2">
-        <v>8229999.9999999953</v>
+        <v>89397</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <v>362083.96322684357</v>
       </c>
       <c r="H2">
-        <v>8401691.2083107401</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="I2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>9200550.0425606277</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
       <c r="B3">
-        <v>47500.000000075197</v>
+        <v>23750.000000037599</v>
       </c>
       <c r="C3">
-        <v>428138.37040346104</v>
+        <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>89397</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>565035.37040353625</v>
+        <v>196393.16624886921</v>
       </c>
       <c r="F3">
-        <v>7479999.9999999981</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <v>2</v>
+        <v>73750.145545039501</v>
       </c>
       <c r="H3">
-        <v>7654589.2299999977</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="I3">
         <v>1</v>
+      </c>
+      <c r="J3">
+        <v>9174589.2299775518</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2250,13 +2596,13 @@
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2281,8 +2627,14 @@
       <c r="I1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -2290,28 +2642,34 @@
         <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>358617.98539980507</v>
+        <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>89397</v>
+        <v>309048.56689980475</v>
       </c>
       <c r="E2">
-        <v>495514.98539988021</v>
+        <v>173967.18169986518</v>
       </c>
       <c r="F2">
-        <v>8229999.9999999953</v>
+        <v>89397</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <v>495945.66539987986</v>
       </c>
       <c r="H2">
-        <v>8404922.9663107377</v>
+        <v>8754867.8996782396</v>
       </c>
       <c r="I2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>8945631.170261316</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -2319,24 +2677,30 @@
         <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>358617.98539980524</v>
+        <v>50000.0985</v>
       </c>
       <c r="D3">
-        <v>89397</v>
+        <v>309048.56689980457</v>
       </c>
       <c r="E3">
-        <v>495514.98539988039</v>
+        <v>202467.18169986518</v>
       </c>
       <c r="F3">
+        <v>89397</v>
+      </c>
+      <c r="G3">
+        <v>495945.66539987968</v>
+      </c>
+      <c r="H3">
         <v>7479999.9999999981</v>
       </c>
-      <c r="G3">
+      <c r="I3">
         <v>2</v>
       </c>
-      <c r="H3">
+      <c r="J3">
         <v>7616493.4259999963</v>
       </c>
-      <c r="I3">
+      <c r="K3">
         <v>1</v>
       </c>
     </row>
@@ -2347,13 +2711,13 @@
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2378,8 +2742,14 @@
       <c r="I1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -2387,28 +2757,34 @@
         <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>164617.98540020152</v>
+        <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>89397</v>
+        <v>175186.8647267684</v>
       </c>
       <c r="E2">
-        <v>301514.98540027672</v>
+        <v>173967.18169986518</v>
       </c>
       <c r="F2">
-        <v>8229999.9999999953</v>
+        <v>89397</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <v>362083.96322684357</v>
       </c>
       <c r="H2">
-        <v>8426433.5423107389</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="I2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>9212131.4825606272</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -2416,25 +2792,31 @@
         <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>164617.98540020152</v>
+        <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>89397</v>
+        <v>72931.258784770616</v>
       </c>
       <c r="E3">
-        <v>301514.98540027672</v>
+        <v>196393.16624886921</v>
       </c>
       <c r="F3">
-        <v>7479999.9999999981</v>
+        <v>89397</v>
       </c>
       <c r="G3">
-        <v>2</v>
+        <v>259828.40432984772</v>
       </c>
       <c r="H3">
-        <v>7630597.6699999953</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="I3">
         <v>1</v>
+      </c>
+      <c r="J3">
+        <v>8380597.6699991105</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2444,13 +2826,13 @@
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2475,8 +2857,14 @@
       <c r="I1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -2484,28 +2872,34 @@
         <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>358617.98539980507</v>
+        <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>89397</v>
+        <v>309048.56689980475</v>
       </c>
       <c r="E2">
-        <v>495514.98539988021</v>
+        <v>173967.18169986518</v>
       </c>
       <c r="F2">
-        <v>8229999.9999999953</v>
+        <v>89397</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <v>495945.66539987986</v>
       </c>
       <c r="H2">
-        <v>8439066.7343107387</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="I2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>9232313.8485606257</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -2513,25 +2907,31 @@
         <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>358617.98539980507</v>
+        <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>89397</v>
+        <v>8777.1098930121243</v>
       </c>
       <c r="E3">
-        <v>495514.98539988021</v>
+        <v>196393.16624886921</v>
       </c>
       <c r="F3">
-        <v>7479999.9999999981</v>
+        <v>89397</v>
       </c>
       <c r="G3">
-        <v>2</v>
+        <v>195674.25543808923</v>
       </c>
       <c r="H3">
-        <v>7667833.5499999961</v>
+        <v>8560521.576256413</v>
       </c>
       <c r="I3">
         <v>1</v>
+      </c>
+      <c r="J3">
+        <v>8748355.1262564138</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2541,13 +2941,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2572,8 +2972,14 @@
       <c r="I1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -2581,28 +2987,34 @@
         <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>358617.98539980507</v>
+        <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>89397</v>
+        <v>309048.56689980475</v>
       </c>
       <c r="E2">
-        <v>495514.98539988021</v>
+        <v>173967.18169986518</v>
       </c>
       <c r="F2">
-        <v>8229999.9999999953</v>
+        <v>89397</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <v>495945.66539987986</v>
       </c>
       <c r="H2">
-        <v>8324544.5563107394</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="I2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>9152584.198560629</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -2610,25 +3022,31 @@
         <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>358617.98539980507</v>
+        <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>89397</v>
+        <v>8777.1098930121243</v>
       </c>
       <c r="E3">
-        <v>495514.98539988021</v>
+        <v>196393.16624886921</v>
       </c>
       <c r="F3">
-        <v>7479999.9999999981</v>
+        <v>89397</v>
       </c>
       <c r="G3">
-        <v>2</v>
+        <v>195674.25543808923</v>
       </c>
       <c r="H3">
-        <v>7568058.5399999963</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="I3">
         <v>1</v>
+      </c>
+      <c r="J3">
+        <v>9088058.5399775542</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2638,13 +3056,13 @@
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2669,8 +3087,14 @@
       <c r="I1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -2678,28 +3102,34 @@
         <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>740617.98539980256</v>
+        <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>89397</v>
+        <v>690617.8868998026</v>
       </c>
       <c r="E2">
+        <v>173967.18169986518</v>
+      </c>
+      <c r="F2">
+        <v>89397</v>
+      </c>
+      <c r="G2">
         <v>877514.98539987789</v>
       </c>
-      <c r="F2">
-        <v>8999999.9999775514</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
       <c r="H2">
-        <v>9163944.0222882964</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="I2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>9179712.0325606279</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -2707,24 +3137,30 @@
         <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>622899.49583761534</v>
+        <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>89397</v>
+        <v>572899.35029261373</v>
       </c>
       <c r="E3">
-        <v>759796.49583769066</v>
+        <v>196393.16624886921</v>
       </c>
       <c r="F3">
+        <v>89397</v>
+      </c>
+      <c r="G3">
+        <v>759796.49583769089</v>
+      </c>
+      <c r="H3">
         <v>8999999.9999775533</v>
       </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3">
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
         <v>9187857.7959775534</v>
       </c>
-      <c r="I3">
+      <c r="K3">
         <v>0</v>
       </c>
     </row>
@@ -2735,13 +3171,13 @@
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2766,8 +3202,14 @@
       <c r="I1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -2775,28 +3217,34 @@
         <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>358617.98539980507</v>
+        <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>89397</v>
+        <v>309048.56689980475</v>
       </c>
       <c r="E2">
-        <v>495514.98539988021</v>
+        <v>173967.18169986518</v>
       </c>
       <c r="F2">
-        <v>8724613.8495684564</v>
+        <v>89397</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <v>495945.66539987986</v>
       </c>
       <c r="H2">
-        <v>8948392.7098792009</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="I2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>9229407.5365606286</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -2804,25 +3252,31 @@
         <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>358617.98539980507</v>
+        <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>89397</v>
+        <v>584777.10989261325</v>
       </c>
       <c r="E3">
-        <v>495514.98539988021</v>
+        <v>196393.16624886921</v>
       </c>
       <c r="F3">
-        <v>7479999.9999999981</v>
+        <v>89397</v>
       </c>
       <c r="G3">
-        <v>2</v>
+        <v>771674.25543769042</v>
       </c>
       <c r="H3">
-        <v>7628032.6279999958</v>
+        <v>11992387.379671589</v>
       </c>
       <c r="I3">
         <v>1</v>
+      </c>
+      <c r="J3">
+        <v>12140420.007671589</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2832,13 +3286,13 @@
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2863,8 +3317,14 @@
       <c r="I1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -2872,28 +3332,34 @@
         <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>740617.98539980256</v>
+        <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>89397</v>
+        <v>690617.8868998026</v>
       </c>
       <c r="E2">
+        <v>173967.18169986518</v>
+      </c>
+      <c r="F2">
+        <v>89397</v>
+      </c>
+      <c r="G2">
         <v>877514.98539987789</v>
       </c>
-      <c r="F2">
-        <v>8229999.9999999953</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
       <c r="H2">
-        <v>8507629.0463107377</v>
+        <v>8229999.9999999981</v>
       </c>
       <c r="I2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>8523374.800583072</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -2901,24 +3367,30 @@
         <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>622899.49583761534</v>
+        <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>89397</v>
+        <v>572899.3502926135</v>
       </c>
       <c r="E3">
+        <v>196393.16624886921</v>
+      </c>
+      <c r="F3">
+        <v>89397</v>
+      </c>
+      <c r="G3">
         <v>759796.49583769066</v>
       </c>
-      <c r="F3">
-        <v>7479999.9999999981</v>
-      </c>
-      <c r="G3">
-        <v>2</v>
-      </c>
       <c r="H3">
-        <v>7704903.3319999976</v>
+        <v>11668029.775882941</v>
       </c>
       <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>11892933.107882941</v>
+      </c>
+      <c r="K3">
         <v>0</v>
       </c>
     </row>
@@ -2929,13 +3401,13 @@
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2960,8 +3432,14 @@
       <c r="I1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -2969,28 +3447,34 @@
         <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>740617.98539980256</v>
+        <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>89397</v>
+        <v>690617.8868998026</v>
       </c>
       <c r="E2">
+        <v>173967.18169986518</v>
+      </c>
+      <c r="F2">
+        <v>89397</v>
+      </c>
+      <c r="G2">
         <v>877514.98539987789</v>
       </c>
-      <c r="F2">
-        <v>8999999.9999775514</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
       <c r="H2">
-        <v>9298381.7302882969</v>
+        <v>8229999.9999999981</v>
       </c>
       <c r="I2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>8548233.2685830705</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -2998,24 +3482,30 @@
         <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>1004899.4958376129</v>
+        <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>89397</v>
+        <v>954899.35029261105</v>
       </c>
       <c r="E3">
+        <v>196393.16624886921</v>
+      </c>
+      <c r="F3">
+        <v>89397</v>
+      </c>
+      <c r="G3">
         <v>1141796.495837688</v>
       </c>
-      <c r="F3">
-        <v>10149302.975663755</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
       <c r="H3">
-        <v>10440610.177663758</v>
+        <v>14089432.391883604</v>
       </c>
       <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>14380739.593883602</v>
+      </c>
+      <c r="K3">
         <v>0</v>
       </c>
     </row>
@@ -3026,13 +3516,13 @@
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -3057,8 +3547,14 @@
       <c r="I1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -3066,28 +3562,34 @@
         <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>740617.98539980256</v>
+        <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>89397</v>
+        <v>690617.8868998026</v>
       </c>
       <c r="E2">
+        <v>173967.18169986518</v>
+      </c>
+      <c r="F2">
+        <v>89397</v>
+      </c>
+      <c r="G2">
         <v>877514.98539987789</v>
       </c>
-      <c r="F2">
-        <v>8442454.2726808209</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
       <c r="H2">
-        <v>8676342.840991566</v>
+        <v>8229999.9999999981</v>
       </c>
       <c r="I2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>8478672.8385830726</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -3095,25 +3597,31 @@
         <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>740617.98539980256</v>
+        <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>89397</v>
+        <v>954899.35029261105</v>
       </c>
       <c r="E3">
-        <v>877514.98539987789</v>
+        <v>196393.16624886921</v>
       </c>
       <c r="F3">
-        <v>7479999.9999999981</v>
+        <v>89397</v>
       </c>
       <c r="G3">
-        <v>2</v>
+        <v>1141796.495837688</v>
       </c>
       <c r="H3">
-        <v>7753849.8819999974</v>
+        <v>11310663.895884939</v>
       </c>
       <c r="I3">
         <v>1</v>
+      </c>
+      <c r="J3">
+        <v>11584513.777884938</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -3123,13 +3631,13 @@
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -3154,8 +3662,14 @@
       <c r="I1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -3163,28 +3677,34 @@
         <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>428138.37040346104</v>
+        <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>89397</v>
+        <v>309048.56689980475</v>
       </c>
       <c r="E2">
-        <v>565035.37040353625</v>
+        <v>173967.18169986518</v>
       </c>
       <c r="F2">
-        <v>8229999.9999999953</v>
+        <v>89397</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <v>495945.66539987986</v>
       </c>
       <c r="H2">
-        <v>8402152.338310739</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="I2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>9204651.0665606279</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -3192,25 +3712,31 @@
         <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>428138.37040346104</v>
+        <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>89397</v>
+        <v>584777.10989261325</v>
       </c>
       <c r="E3">
-        <v>565035.37040353625</v>
+        <v>196393.16624886921</v>
       </c>
       <c r="F3">
-        <v>7479999.9999999981</v>
+        <v>89397</v>
       </c>
       <c r="G3">
-        <v>2</v>
+        <v>771674.25543769042</v>
       </c>
       <c r="H3">
-        <v>7690604.345999998</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="I3">
         <v>1</v>
+      </c>
+      <c r="J3">
+        <v>9210604.3459775522</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -3220,13 +3746,13 @@
 
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -3251,8 +3777,14 @@
       <c r="I1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -3260,28 +3792,34 @@
         <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>455617.98539999995</v>
+        <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>89397</v>
+        <v>405617.88689999998</v>
       </c>
       <c r="E2">
+        <v>173967.18169986518</v>
+      </c>
+      <c r="F2">
+        <v>89397</v>
+      </c>
+      <c r="G2">
         <v>592514.98540007521</v>
       </c>
-      <c r="F2">
-        <v>8675359.689767804</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
       <c r="H2">
-        <v>8829211.9160785489</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="I2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>9218164.958560627</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -3289,25 +3827,31 @@
         <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>455617.98539999995</v>
+        <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>89397</v>
+        <v>393449.35029299994</v>
       </c>
       <c r="E3">
-        <v>592514.98540007521</v>
+        <v>196393.16624886921</v>
       </c>
       <c r="F3">
-        <v>7479999.9999999981</v>
+        <v>89397</v>
       </c>
       <c r="G3">
-        <v>2</v>
+        <v>580346.49583807704</v>
       </c>
       <c r="H3">
-        <v>7579952.9999999972</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="I3">
         <v>1</v>
+      </c>
+      <c r="J3">
+        <v>9137627.9999775533</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -3316,200 +3860,6 @@
 </file>
 
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>43466</v>
-      </c>
-      <c r="B2">
-        <v>47500.000000075197</v>
-      </c>
-      <c r="C2">
-        <v>455617.98539999995</v>
-      </c>
-      <c r="D2">
-        <v>89397</v>
-      </c>
-      <c r="E2">
-        <v>592514.98540007521</v>
-      </c>
-      <c r="F2">
-        <v>8999999.9999775514</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>9151859.2262882963</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>43831</v>
-      </c>
-      <c r="B3">
-        <v>47500.000000075197</v>
-      </c>
-      <c r="C3">
-        <v>443449.49583800184</v>
-      </c>
-      <c r="D3">
-        <v>89397</v>
-      </c>
-      <c r="E3">
-        <v>580346.49583807704</v>
-      </c>
-      <c r="F3">
-        <v>8999999.9999775533</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3">
-        <v>9108851.9999775533</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>43466</v>
-      </c>
-      <c r="B2">
-        <v>47500.000000075197</v>
-      </c>
-      <c r="C2">
-        <v>455617.98539999995</v>
-      </c>
-      <c r="D2">
-        <v>89397</v>
-      </c>
-      <c r="E2">
-        <v>592514.98540007521</v>
-      </c>
-      <c r="F2">
-        <v>8229999.9999999953</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>8364785.2263107393</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>43831</v>
-      </c>
-      <c r="B3">
-        <v>47500.000000075197</v>
-      </c>
-      <c r="C3">
-        <v>455617.98539999995</v>
-      </c>
-      <c r="D3">
-        <v>89397</v>
-      </c>
-      <c r="E3">
-        <v>592514.98540007521</v>
-      </c>
-      <c r="F3">
-        <v>7479999.9999999981</v>
-      </c>
-      <c r="G3">
-        <v>2</v>
-      </c>
-      <c r="H3">
-        <v>7577795.9999999963</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -3523,13 +3873,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -3554,8 +3904,14 @@
       <c r="I1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -3563,28 +3919,34 @@
         <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>455617.98539999995</v>
+        <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>89397</v>
+        <v>405617.88689999998</v>
       </c>
       <c r="E2">
+        <v>173967.18169986518</v>
+      </c>
+      <c r="F2">
+        <v>89397</v>
+      </c>
+      <c r="G2">
         <v>592514.98540007521</v>
       </c>
-      <c r="F2">
-        <v>8229999.9999999953</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
       <c r="H2">
-        <v>8325028.606310741</v>
+        <v>8229999.9999999981</v>
       </c>
       <c r="I2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>8382534.8785830718</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -3592,24 +3954,30 @@
         <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>455617.98539999995</v>
+        <v>50000.0985</v>
       </c>
       <c r="D3">
-        <v>89397</v>
+        <v>405617.88689999981</v>
       </c>
       <c r="E3">
-        <v>592514.98540007521</v>
+        <v>202467.18169986518</v>
       </c>
       <c r="F3">
+        <v>89397</v>
+      </c>
+      <c r="G3">
+        <v>592514.98540007509</v>
+      </c>
+      <c r="H3">
         <v>7479999.9999999981</v>
       </c>
-      <c r="G3">
+      <c r="I3">
         <v>2</v>
       </c>
-      <c r="H3">
+      <c r="J3">
         <v>7511744.7299999967</v>
       </c>
-      <c r="I3">
+      <c r="K3">
         <v>1</v>
       </c>
     </row>
@@ -3620,13 +3988,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -3651,8 +4019,14 @@
       <c r="I1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -3660,28 +4034,34 @@
         <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>740617.98539980256</v>
+        <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>89397</v>
+        <v>690617.8868998026</v>
       </c>
       <c r="E2">
+        <v>173967.18169986518</v>
+      </c>
+      <c r="F2">
+        <v>89397</v>
+      </c>
+      <c r="G2">
         <v>877514.98539987789</v>
       </c>
-      <c r="F2">
-        <v>8999999.9999775514</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
       <c r="H2">
-        <v>9235340.4062882941</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="I2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>9262766.2385606263</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -3689,24 +4069,30 @@
         <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>719899.49583781033</v>
+        <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>89397</v>
+        <v>669899.35029280838</v>
       </c>
       <c r="E3">
-        <v>856796.49583788565</v>
+        <v>196393.16624886921</v>
       </c>
       <c r="F3">
-        <v>8229999.9999991106</v>
+        <v>89397</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>856796.49583788554</v>
       </c>
       <c r="H3">
-        <v>8291125.7399991108</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>9061125.7399775516</v>
+      </c>
+      <c r="K3">
         <v>0</v>
       </c>
     </row>
@@ -3717,13 +4103,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -3748,8 +4134,14 @@
       <c r="I1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -3757,28 +4149,34 @@
         <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>455617.98539999995</v>
+        <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>89397</v>
+        <v>405617.88689999998</v>
       </c>
       <c r="E2">
+        <v>173967.18169986518</v>
+      </c>
+      <c r="F2">
+        <v>89397</v>
+      </c>
+      <c r="G2">
         <v>592514.98540007521</v>
       </c>
-      <c r="F2">
-        <v>8655277.4687817339</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
       <c r="H2">
-        <v>8855604.5950924754</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="I2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>9215807.168560626</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -3786,25 +4184,31 @@
         <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>455617.98539999995</v>
+        <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>89397</v>
+        <v>678449.35029280256</v>
       </c>
       <c r="E3">
-        <v>592514.98540007521</v>
+        <v>196393.16624886921</v>
       </c>
       <c r="F3">
-        <v>7479999.9999999981</v>
+        <v>89397</v>
       </c>
       <c r="G3">
-        <v>2</v>
+        <v>865346.49583787972</v>
       </c>
       <c r="H3">
-        <v>7692695.0099999979</v>
+        <v>11462836.566283172</v>
       </c>
       <c r="I3">
         <v>1</v>
+      </c>
+      <c r="J3">
+        <v>11675531.576283168</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -3814,13 +4218,13 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -3845,8 +4249,14 @@
       <c r="I1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -3854,28 +4264,34 @@
         <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>358617.98539980507</v>
+        <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>89397</v>
+        <v>309048.56689980475</v>
       </c>
       <c r="E2">
-        <v>495514.98539988021</v>
+        <v>173967.18169986518</v>
       </c>
       <c r="F2">
-        <v>8999999.9999775514</v>
+        <v>89397</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <v>495945.66539987986</v>
       </c>
       <c r="H2">
-        <v>9185173.4262882955</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="I2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>9209043.7185606286</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -3883,24 +4299,30 @@
         <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>358617.98539980507</v>
+        <v>50000.0985</v>
       </c>
       <c r="D3">
-        <v>89397</v>
+        <v>309048.56689980457</v>
       </c>
       <c r="E3">
-        <v>495514.98539988021</v>
+        <v>202467.18169986518</v>
       </c>
       <c r="F3">
-        <v>7479999.9999999981</v>
+        <v>89397</v>
       </c>
       <c r="G3">
-        <v>2</v>
+        <v>495945.66539987968</v>
       </c>
       <c r="H3">
-        <v>7663949.7199999951</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>9183949.7199775539</v>
+      </c>
+      <c r="K3">
         <v>1</v>
       </c>
     </row>
@@ -3911,13 +4333,13 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -3942,8 +4364,14 @@
       <c r="I1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -3951,28 +4379,34 @@
         <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>164617.98540020152</v>
+        <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>89397</v>
+        <v>175186.8647267684</v>
       </c>
       <c r="E2">
-        <v>301514.98540027672</v>
+        <v>173967.18169986518</v>
       </c>
       <c r="F2">
-        <v>8999999.9999775514</v>
+        <v>89397</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <v>362083.96322684357</v>
       </c>
       <c r="H2">
-        <v>9215604.6462882962</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="I2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>9246578.8885606267</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -3980,24 +4414,30 @@
         <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>164617.98540020152</v>
+        <v>50000.0985</v>
       </c>
       <c r="D3">
-        <v>89397</v>
+        <v>175186.86472676822</v>
       </c>
       <c r="E3">
-        <v>301514.98540027672</v>
+        <v>202467.18169986518</v>
       </c>
       <c r="F3">
-        <v>8999999.9999775533</v>
+        <v>89397</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>362083.96322684339</v>
       </c>
       <c r="H3">
-        <v>9160152.0699775536</v>
+        <v>7479999.9999999981</v>
       </c>
       <c r="I3">
+        <v>2</v>
+      </c>
+      <c r="J3">
+        <v>7640152.0699999966</v>
+      </c>
+      <c r="K3">
         <v>1</v>
       </c>
     </row>
@@ -4008,13 +4448,13 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -4039,8 +4479,14 @@
       <c r="I1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -4048,28 +4494,34 @@
         <v>47500.000000075197</v>
       </c>
       <c r="C2">
-        <v>358617.98539980507</v>
+        <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>89397</v>
+        <v>309048.56689980475</v>
       </c>
       <c r="E2">
-        <v>495514.98539988021</v>
+        <v>173967.18169986518</v>
       </c>
       <c r="F2">
-        <v>8229999.9999999953</v>
+        <v>89397</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <v>495945.66539987986</v>
       </c>
       <c r="H2">
-        <v>8396750.7063107397</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="I2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>9183262.3985606283</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -4077,24 +4529,30 @@
         <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>358617.98539980507</v>
+        <v>50000.0985</v>
       </c>
       <c r="D3">
-        <v>89397</v>
+        <v>309048.56689980457</v>
       </c>
       <c r="E3">
-        <v>495514.98539988021</v>
+        <v>202467.18169986518</v>
       </c>
       <c r="F3">
+        <v>89397</v>
+      </c>
+      <c r="G3">
+        <v>495945.66539987968</v>
+      </c>
+      <c r="H3">
         <v>7479999.9999999981</v>
       </c>
-      <c r="G3">
+      <c r="I3">
         <v>2</v>
       </c>
-      <c r="H3">
+      <c r="J3">
         <v>7666027.3499999968</v>
       </c>
-      <c r="I3">
+      <c r="K3">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Official April 2019 MTOM Run
No model file changes. updated inflow forecast files

Ruleset changes include the following: Added a constraint in Powell after LBDV where it forces the Powell outflow to TARV. Added constraint to make sure deterministic run of MTOM uses 24 MS inputs in delivery and creation of ICS function. Added notes about changes and updated ruleset name to 2.4
</commit_message>
<xml_diff>
--- a/Output Data/MtomToCrss_Annual.xlsx
+++ b/Output Data/MtomToCrss_Annual.xlsx
@@ -12,43 +12,45 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="12570" windowHeight="13590"/>
   </bookViews>
   <sheets>
-    <sheet name="Trace38" sheetId="37" r:id="rId1"/>
-    <sheet name="Trace37" sheetId="36" r:id="rId2"/>
-    <sheet name="Trace36" sheetId="35" r:id="rId3"/>
-    <sheet name="Trace35" sheetId="34" r:id="rId4"/>
-    <sheet name="Trace34" sheetId="33" r:id="rId5"/>
-    <sheet name="Trace33" sheetId="32" r:id="rId6"/>
-    <sheet name="Trace32" sheetId="31" r:id="rId7"/>
-    <sheet name="Trace31" sheetId="30" r:id="rId8"/>
-    <sheet name="Trace30" sheetId="29" r:id="rId9"/>
-    <sheet name="Trace29" sheetId="28" r:id="rId10"/>
-    <sheet name="Trace28" sheetId="27" r:id="rId11"/>
-    <sheet name="Trace27" sheetId="26" r:id="rId12"/>
-    <sheet name="Trace26" sheetId="25" r:id="rId13"/>
-    <sheet name="Trace25" sheetId="24" r:id="rId14"/>
-    <sheet name="Trace24" sheetId="23" r:id="rId15"/>
-    <sheet name="Trace23" sheetId="22" r:id="rId16"/>
-    <sheet name="Trace22" sheetId="21" r:id="rId17"/>
-    <sheet name="Trace21" sheetId="20" r:id="rId18"/>
-    <sheet name="Trace20" sheetId="19" r:id="rId19"/>
-    <sheet name="Trace19" sheetId="18" r:id="rId20"/>
-    <sheet name="Trace18" sheetId="17" r:id="rId21"/>
-    <sheet name="Trace17" sheetId="16" r:id="rId22"/>
-    <sheet name="Trace16" sheetId="15" r:id="rId23"/>
-    <sheet name="Trace15" sheetId="14" r:id="rId24"/>
-    <sheet name="Trace14" sheetId="13" r:id="rId25"/>
-    <sheet name="Trace13" sheetId="12" r:id="rId26"/>
-    <sheet name="Trace12" sheetId="11" r:id="rId27"/>
-    <sheet name="Trace11" sheetId="10" r:id="rId28"/>
-    <sheet name="Trace10" sheetId="9" r:id="rId29"/>
-    <sheet name="Trace9" sheetId="8" r:id="rId30"/>
-    <sheet name="Trace8" sheetId="7" r:id="rId31"/>
-    <sheet name="Trace7" sheetId="6" r:id="rId32"/>
-    <sheet name="Trace6" sheetId="5" r:id="rId33"/>
-    <sheet name="Trace5" sheetId="4" r:id="rId34"/>
-    <sheet name="Trace4" sheetId="3" r:id="rId35"/>
-    <sheet name="Trace3" sheetId="2" r:id="rId36"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId37"/>
+    <sheet name="Trace38" sheetId="39" r:id="rId1"/>
+    <sheet name="Trace37" sheetId="38" r:id="rId2"/>
+    <sheet name="Trace36" sheetId="37" r:id="rId3"/>
+    <sheet name="Trace35" sheetId="36" r:id="rId4"/>
+    <sheet name="Trace34" sheetId="35" r:id="rId5"/>
+    <sheet name="Trace33" sheetId="34" r:id="rId6"/>
+    <sheet name="Trace32" sheetId="33" r:id="rId7"/>
+    <sheet name="Trace31" sheetId="32" r:id="rId8"/>
+    <sheet name="Trace30" sheetId="31" r:id="rId9"/>
+    <sheet name="Trace29" sheetId="30" r:id="rId10"/>
+    <sheet name="Trace28" sheetId="29" r:id="rId11"/>
+    <sheet name="Trace27" sheetId="28" r:id="rId12"/>
+    <sheet name="Trace26" sheetId="27" r:id="rId13"/>
+    <sheet name="Trace25" sheetId="26" r:id="rId14"/>
+    <sheet name="Trace24" sheetId="25" r:id="rId15"/>
+    <sheet name="Trace23" sheetId="24" r:id="rId16"/>
+    <sheet name="Trace22" sheetId="23" r:id="rId17"/>
+    <sheet name="Trace21" sheetId="22" r:id="rId18"/>
+    <sheet name="Trace20" sheetId="21" r:id="rId19"/>
+    <sheet name="Trace19" sheetId="20" r:id="rId20"/>
+    <sheet name="Trace18" sheetId="19" r:id="rId21"/>
+    <sheet name="Trace17" sheetId="18" r:id="rId22"/>
+    <sheet name="Trace16" sheetId="17" r:id="rId23"/>
+    <sheet name="Trace15" sheetId="16" r:id="rId24"/>
+    <sheet name="Trace14" sheetId="15" r:id="rId25"/>
+    <sheet name="Trace13" sheetId="14" r:id="rId26"/>
+    <sheet name="Trace12" sheetId="13" r:id="rId27"/>
+    <sheet name="Trace11" sheetId="12" r:id="rId28"/>
+    <sheet name="Trace10" sheetId="11" r:id="rId29"/>
+    <sheet name="Trace9" sheetId="10" r:id="rId30"/>
+    <sheet name="Trace8" sheetId="9" r:id="rId31"/>
+    <sheet name="Trace7" sheetId="8" r:id="rId32"/>
+    <sheet name="Trace6" sheetId="7" r:id="rId33"/>
+    <sheet name="Trace5" sheetId="6" r:id="rId34"/>
+    <sheet name="Trace4" sheetId="5" r:id="rId35"/>
+    <sheet name="Trace3" sheetId="4" r:id="rId36"/>
+    <sheet name="Trace2" sheetId="3" r:id="rId37"/>
+    <sheet name="Trace1" sheetId="2" r:id="rId38"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId39"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -60,18 +62,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="10">
   <si>
     <t>ICS Credits.BiNationalICS_CA</t>
   </si>
   <si>
-    <t>ICS Credits.ExtraordinaryConservationICS_IID</t>
+    <t>ECICS_Bal_IID</t>
   </si>
   <si>
-    <t>ICS Credits.ExtraordinaryConservationICS_MWD</t>
+    <t>ECICS_Bal_MWD</t>
   </si>
   <si>
-    <t>ICS Credits.ExtraordinaryConservationICS_NV</t>
+    <t>ECICS_Bal_SNWA</t>
   </si>
   <si>
     <t>ICS Credits.SystemEfficiencyICS_CA</t>
@@ -460,7 +462,7 @@
         <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>175186.8647267684</v>
+        <v>784117.83689999999</v>
       </c>
       <c r="E2">
         <v>173967.18169986518</v>
@@ -469,7 +471,7 @@
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>362083.96322684357</v>
+        <v>971014.93540007516</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -478,7 +480,7 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9198607.3185606264</v>
+        <v>9204745.5919337161</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -495,7 +497,7 @@
         <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>169931.25878496529</v>
+        <v>760594.30179299985</v>
       </c>
       <c r="E3">
         <v>196393.16624886921</v>
@@ -504,16 +506,16 @@
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>356828.40433004237</v>
+        <v>947491.44733807701</v>
       </c>
       <c r="H3">
-        <v>8229999.9999991106</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3">
-        <v>8340981.0259991111</v>
+        <v>9110981.0259775538</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -575,7 +577,7 @@
         <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>690617.8868998026</v>
+        <v>784117.83689999999</v>
       </c>
       <c r="E2">
         <v>173967.18169986518</v>
@@ -584,7 +586,7 @@
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>877514.98539987789</v>
+        <v>971014.93540007516</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -593,7 +595,7 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9275967.7685606275</v>
+        <v>9276617.2819337193</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -610,7 +612,7 @@
         <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>572899.35029261373</v>
+        <v>663594.30179280508</v>
       </c>
       <c r="E3">
         <v>196393.16624886921</v>
@@ -619,7 +621,7 @@
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>759796.49583769089</v>
+        <v>850491.44733788224</v>
       </c>
       <c r="H3">
         <v>8999999.9999775533</v>
@@ -690,7 +692,7 @@
         <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>548117.88689990132</v>
+        <v>784117.83689999999</v>
       </c>
       <c r="E2">
         <v>173967.18169986518</v>
@@ -699,16 +701,16 @@
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>735014.98539997661</v>
+        <v>971014.93540007516</v>
       </c>
       <c r="H2">
-        <v>8229999.9999999981</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="I2">
         <v>1</v>
       </c>
       <c r="J2">
-        <v>8447920.5585830733</v>
+        <v>9216103.8919337187</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -725,7 +727,7 @@
         <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>816674.35029270698</v>
+        <v>1045594.3017928025</v>
       </c>
       <c r="E3">
         <v>196393.16624886921</v>
@@ -734,7 +736,7 @@
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>1003571.4958377838</v>
+        <v>1232491.4473378796</v>
       </c>
       <c r="H3">
         <v>8999999.9999775533</v>
@@ -805,7 +807,7 @@
         <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>405617.88689999998</v>
+        <v>784117.83689999999</v>
       </c>
       <c r="E2">
         <v>173967.18169986518</v>
@@ -814,16 +816,16 @@
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>592514.98540007521</v>
+        <v>971014.93540007516</v>
       </c>
       <c r="H2">
-        <v>8984161.4499797802</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="I2">
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9147860.4785628542</v>
+        <v>9166551.50193372</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -837,31 +839,31 @@
         <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>50000.0985</v>
+        <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>405617.88689999981</v>
+        <v>903094.30179290124</v>
       </c>
       <c r="E3">
-        <v>202467.18169986518</v>
+        <v>196393.16624886921</v>
       </c>
       <c r="F3">
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>592514.98540007509</v>
+        <v>1089991.4473379783</v>
       </c>
       <c r="H3">
-        <v>7479999.9999999981</v>
+        <v>9712858.5941786692</v>
       </c>
       <c r="I3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J3">
-        <v>7609167.7799999956</v>
+        <v>9842026.3741786703</v>
       </c>
       <c r="K3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -920,7 +922,7 @@
         <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>548117.88689990132</v>
+        <v>784117.83689999999</v>
       </c>
       <c r="E2">
         <v>173967.18169986518</v>
@@ -929,7 +931,7 @@
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>735014.98539997661</v>
+        <v>971014.93540007516</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -938,7 +940,7 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9212653.5085606258</v>
+        <v>9217222.1119337194</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -955,7 +957,7 @@
         <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>531674.35029290419</v>
+        <v>760594.30179299985</v>
       </c>
       <c r="E3">
         <v>196393.16624886921</v>
@@ -964,7 +966,7 @@
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>718571.49583798135</v>
+        <v>947491.44733807701</v>
       </c>
       <c r="H3">
         <v>8999999.9999775533</v>
@@ -1035,7 +1037,7 @@
         <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>309048.56689980475</v>
+        <v>784117.83689999999</v>
       </c>
       <c r="E2">
         <v>173967.18169986518</v>
@@ -1044,16 +1046,16 @@
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>495945.66539987986</v>
+        <v>971014.93540007516</v>
       </c>
       <c r="H2">
-        <v>8229999.9999999981</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="I2">
         <v>1</v>
       </c>
       <c r="J2">
-        <v>8443584.0885830726</v>
+        <v>9216979.461933719</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -1067,31 +1069,31 @@
         <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>50000.0985</v>
+        <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>309048.56689980457</v>
+        <v>903094.30179290124</v>
       </c>
       <c r="E3">
-        <v>202467.18169986518</v>
+        <v>196393.16624886921</v>
       </c>
       <c r="F3">
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>495945.66539987968</v>
+        <v>1089991.4473379783</v>
       </c>
       <c r="H3">
-        <v>7479999.9999999981</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="I3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J3">
-        <v>7611647.4399999948</v>
+        <v>9131647.4399775527</v>
       </c>
       <c r="K3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1150,7 +1152,7 @@
         <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>309048.56689980475</v>
+        <v>784117.83689999999</v>
       </c>
       <c r="E2">
         <v>173967.18169986518</v>
@@ -1159,7 +1161,7 @@
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>495945.66539987986</v>
+        <v>971014.93540007516</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -1168,7 +1170,7 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9179778.2385606281</v>
+        <v>9186684.3419337198</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -1185,7 +1187,7 @@
         <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>202777.10989261558</v>
+        <v>663594.30179280485</v>
       </c>
       <c r="E3">
         <v>196393.16624886921</v>
@@ -1194,16 +1196,16 @@
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>389674.25543769269</v>
+        <v>850491.44733788201</v>
       </c>
       <c r="H3">
-        <v>8229999.9999991106</v>
+        <v>8855069.1936470252</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3">
-        <v>8338713.64999911</v>
+        <v>8963782.8436470237</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -1265,7 +1267,7 @@
         <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>548117.88689990132</v>
+        <v>784117.83689999999</v>
       </c>
       <c r="E2">
         <v>173967.18169986518</v>
@@ -1274,7 +1276,7 @@
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>735014.98539997661</v>
+        <v>971014.93540007516</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -1283,7 +1285,7 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9239257.7585606277</v>
+        <v>9242730.2619337197</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -1300,7 +1302,7 @@
         <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>434674.35029270942</v>
+        <v>663594.30179280508</v>
       </c>
       <c r="E3">
         <v>196393.16624886921</v>
@@ -1309,7 +1311,7 @@
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>621571.49583778658</v>
+        <v>850491.44733788224</v>
       </c>
       <c r="H3">
         <v>8999999.9999775533</v>
@@ -1380,7 +1382,7 @@
         <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>690617.8868998026</v>
+        <v>784117.83689999999</v>
       </c>
       <c r="E2">
         <v>173967.18169986518</v>
@@ -1389,7 +1391,7 @@
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>877514.98539987789</v>
+        <v>971014.93540007516</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -1398,7 +1400,7 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9253998.8485606275</v>
+        <v>9230358.4719337188</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -1415,7 +1417,7 @@
         <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>812399.35029270977</v>
+        <v>903094.30179290124</v>
       </c>
       <c r="E3">
         <v>196393.16624886921</v>
@@ -1424,7 +1426,7 @@
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>999296.4958377867</v>
+        <v>1089991.4473379783</v>
       </c>
       <c r="H3">
         <v>8999999.9999775533</v>
@@ -1495,7 +1497,7 @@
         <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>690617.8868998026</v>
+        <v>784117.83689999999</v>
       </c>
       <c r="E2">
         <v>173967.18169986518</v>
@@ -1504,16 +1506,16 @@
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>877514.98539987789</v>
+        <v>971014.93540007516</v>
       </c>
       <c r="H2">
-        <v>8229999.9999999981</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="I2">
         <v>1</v>
       </c>
       <c r="J2">
-        <v>8317324.9385830723</v>
+        <v>9115498.6519337185</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -1530,7 +1532,7 @@
         <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>954899.35029261105</v>
+        <v>1045594.3017928025</v>
       </c>
       <c r="E3">
         <v>196393.16624886921</v>
@@ -1539,16 +1541,16 @@
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>1141796.495837688</v>
+        <v>1232491.4473378796</v>
       </c>
       <c r="H3">
-        <v>8999999.9999775533</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3">
-        <v>9203484.9599775542</v>
+        <v>8433484.9599991105</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -1610,7 +1612,7 @@
         <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>690617.8868998026</v>
+        <v>784117.83689999999</v>
       </c>
       <c r="E2">
         <v>173967.18169986518</v>
@@ -1619,7 +1621,7 @@
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>877514.98539987789</v>
+        <v>971014.93540007516</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -1628,7 +1630,7 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9142203.1085606273</v>
+        <v>9160244.5719337184</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -1645,7 +1647,7 @@
         <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>954899.35029261105</v>
+        <v>1045594.3017928025</v>
       </c>
       <c r="E3">
         <v>196393.16624886921</v>
@@ -1654,16 +1656,16 @@
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>1141796.495837688</v>
+        <v>1232491.4473378796</v>
       </c>
       <c r="H3">
-        <v>8999999.9999775533</v>
+        <v>10887492.807684025</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3">
-        <v>8910372.509977553</v>
+        <v>10797865.317684025</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -1725,7 +1727,7 @@
         <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>175186.8647267684</v>
+        <v>784117.83689999999</v>
       </c>
       <c r="E2">
         <v>173967.18169986518</v>
@@ -1734,7 +1736,7 @@
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>362083.96322684357</v>
+        <v>971014.93540007516</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -1743,7 +1745,7 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9195953.6685606278</v>
+        <v>9202557.1019337177</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -1754,22 +1756,22 @@
         <v>43831</v>
       </c>
       <c r="B3">
-        <v>23750.000000037599</v>
+        <v>47500.000000075197</v>
       </c>
       <c r="C3">
         <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>469594.30179320136</v>
       </c>
       <c r="E3">
         <v>196393.16624886921</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>89397</v>
       </c>
       <c r="G3">
-        <v>73750.145545039501</v>
+        <v>656491.44733827852</v>
       </c>
       <c r="H3">
         <v>8999999.9999775533</v>
@@ -1840,7 +1842,7 @@
         <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>690617.8868998026</v>
+        <v>784117.83689999999</v>
       </c>
       <c r="E2">
         <v>173967.18169986518</v>
@@ -1849,7 +1851,7 @@
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>877514.98539987789</v>
+        <v>971014.93540007516</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -1858,7 +1860,7 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9180315.9605606291</v>
+        <v>9203493.3419337198</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -1875,7 +1877,7 @@
         <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>954899.35029261105</v>
+        <v>1045594.3017928025</v>
       </c>
       <c r="E3">
         <v>196393.16624886921</v>
@@ -1884,16 +1886,16 @@
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>1141796.495837688</v>
+        <v>1232491.4473378796</v>
       </c>
       <c r="H3">
-        <v>10992555.326922728</v>
+        <v>11456726.940617843</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3">
-        <v>11054227.012922728</v>
+        <v>11518398.626617841</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -1955,7 +1957,7 @@
         <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>690617.8868998026</v>
+        <v>784117.83689999999</v>
       </c>
       <c r="E2">
         <v>173967.18169986518</v>
@@ -1964,16 +1966,16 @@
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>877514.98539987789</v>
+        <v>971014.93540007516</v>
       </c>
       <c r="H2">
-        <v>10781723.845268941</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="I2">
         <v>1</v>
       </c>
       <c r="J2">
-        <v>11079329.129852016</v>
+        <v>9247681.9079337176</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -1990,7 +1992,7 @@
         <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>954899.35029261105</v>
+        <v>1045594.3017928025</v>
       </c>
       <c r="E3">
         <v>196393.16624886921</v>
@@ -1999,16 +2001,16 @@
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>1141796.495837688</v>
+        <v>1232491.4473378796</v>
       </c>
       <c r="H3">
-        <v>10483416.252694307</v>
+        <v>11984459.9762755</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3">
-        <v>10611934.984694308</v>
+        <v>12112978.708275499</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -2070,7 +2072,7 @@
         <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>175186.8647267684</v>
+        <v>784117.83689999999</v>
       </c>
       <c r="E2">
         <v>173967.18169986518</v>
@@ -2079,7 +2081,7 @@
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>362083.96322684357</v>
+        <v>971014.93540007516</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -2088,7 +2090,7 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9186224.8985606264</v>
+        <v>9181276.6819337197</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -2102,31 +2104,31 @@
         <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>50000.0985</v>
+        <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>175186.86472676822</v>
+        <v>1045594.3017928025</v>
       </c>
       <c r="E3">
-        <v>202467.18169986518</v>
+        <v>196393.16624886921</v>
       </c>
       <c r="F3">
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>362083.96322684339</v>
+        <v>1232491.4473378796</v>
       </c>
       <c r="H3">
-        <v>7479999.9999999981</v>
+        <v>11848797.186601833</v>
       </c>
       <c r="I3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J3">
-        <v>7762420.3039999977</v>
+        <v>12131217.490601834</v>
       </c>
       <c r="K3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2185,7 +2187,7 @@
         <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>548117.88689990132</v>
+        <v>784117.83689999999</v>
       </c>
       <c r="E2">
         <v>173967.18169986518</v>
@@ -2194,16 +2196,16 @@
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>735014.98539997661</v>
+        <v>971014.93540007516</v>
       </c>
       <c r="H2">
-        <v>8229999.9999999981</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="I2">
         <v>1</v>
       </c>
       <c r="J2">
-        <v>8528404.1665830705</v>
+        <v>9244710.9439337198</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -2220,7 +2222,7 @@
         <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>240674.35029310576</v>
+        <v>469594.30179320095</v>
       </c>
       <c r="E3">
         <v>196393.16624886921</v>
@@ -2229,7 +2231,7 @@
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>427571.4958381828</v>
+        <v>656491.44733827817</v>
       </c>
       <c r="H3">
         <v>8999999.9999775533</v>
@@ -2300,7 +2302,7 @@
         <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>175186.8647267684</v>
+        <v>784117.83689999999</v>
       </c>
       <c r="E2">
         <v>173967.18169986518</v>
@@ -2309,7 +2311,7 @@
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>362083.96322684357</v>
+        <v>971014.93540007516</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -2318,7 +2320,7 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9277531.6285606269</v>
+        <v>9250298.2239337191</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -2332,10 +2334,10 @@
         <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>50000.0985</v>
+        <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>312431.25878486666</v>
+        <v>903094.30179290124</v>
       </c>
       <c r="E3">
         <v>196393.16624886921</v>
@@ -2344,16 +2346,16 @@
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>499328.4043299437</v>
+        <v>1089991.4473379783</v>
       </c>
       <c r="H3">
-        <v>8229999.9999991106</v>
+        <v>10163846.826235268</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3">
-        <v>8639818.2239991091</v>
+        <v>10573665.05023527</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -2415,7 +2417,7 @@
         <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>175186.8647267684</v>
+        <v>784117.83689999999</v>
       </c>
       <c r="E2">
         <v>173967.18169986518</v>
@@ -2424,7 +2426,7 @@
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>362083.96322684357</v>
+        <v>971014.93540007516</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -2433,7 +2435,7 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9239105.7565606255</v>
+        <v>9224994.0099337194</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -2444,31 +2446,31 @@
         <v>43831</v>
       </c>
       <c r="B3">
-        <v>23750.000000037599</v>
+        <v>47500.000000075197</v>
       </c>
       <c r="C3">
         <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>469594.30179320136</v>
       </c>
       <c r="E3">
         <v>196393.16624886921</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>89397</v>
       </c>
       <c r="G3">
-        <v>73750.145545039501</v>
+        <v>656491.44733827852</v>
       </c>
       <c r="H3">
-        <v>8999999.9999775533</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3">
-        <v>9239478.9159775525</v>
+        <v>8469478.9159991127</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -2530,7 +2532,7 @@
         <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>175186.8647267684</v>
+        <v>784117.83689999999</v>
       </c>
       <c r="E2">
         <v>173967.18169986518</v>
@@ -2539,7 +2541,7 @@
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>362083.96322684357</v>
+        <v>971014.93540007516</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -2548,7 +2550,7 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9200550.0425606277</v>
+        <v>9203868.1699337177</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -2559,22 +2561,22 @@
         <v>43831</v>
       </c>
       <c r="B3">
-        <v>23750.000000037599</v>
+        <v>47500.000000075197</v>
       </c>
       <c r="C3">
         <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>469594.30179320136</v>
       </c>
       <c r="E3">
         <v>196393.16624886921</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>89397</v>
       </c>
       <c r="G3">
-        <v>73750.145545039501</v>
+        <v>656491.44733827852</v>
       </c>
       <c r="H3">
         <v>8999999.9999775533</v>
@@ -2645,7 +2647,7 @@
         <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>309048.56689980475</v>
+        <v>784117.83689999999</v>
       </c>
       <c r="E2">
         <v>173967.18169986518</v>
@@ -2654,16 +2656,16 @@
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>495945.66539987986</v>
+        <v>971014.93540007516</v>
       </c>
       <c r="H2">
-        <v>8754867.8996782396</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="I2">
         <v>1</v>
       </c>
       <c r="J2">
-        <v>8945631.170261316</v>
+        <v>9198838.5759337191</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -2677,31 +2679,31 @@
         <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>50000.0985</v>
+        <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>309048.56689980457</v>
+        <v>760594.30179299985</v>
       </c>
       <c r="E3">
-        <v>202467.18169986518</v>
+        <v>196393.16624886921</v>
       </c>
       <c r="F3">
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>495945.66539987968</v>
+        <v>947491.44733807701</v>
       </c>
       <c r="H3">
-        <v>7479999.9999999981</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="I3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J3">
-        <v>7616493.4259999963</v>
+        <v>8366493.4259991096</v>
       </c>
       <c r="K3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2760,7 +2762,7 @@
         <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>175186.8647267684</v>
+        <v>784117.83689999999</v>
       </c>
       <c r="E2">
         <v>173967.18169986518</v>
@@ -2769,7 +2771,7 @@
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>362083.96322684357</v>
+        <v>971014.93540007516</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -2778,7 +2780,7 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9212131.4825606272</v>
+        <v>9214828.7199337184</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -2795,7 +2797,7 @@
         <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>72931.258784770616</v>
+        <v>663594.30179280508</v>
       </c>
       <c r="E3">
         <v>196393.16624886921</v>
@@ -2804,16 +2806,16 @@
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>259828.40432984772</v>
+        <v>850491.44733788224</v>
       </c>
       <c r="H3">
-        <v>8229999.9999991106</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3">
-        <v>8380597.6699991105</v>
+        <v>9150597.6699775569</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -2875,7 +2877,7 @@
         <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>309048.56689980475</v>
+        <v>784117.83689999999</v>
       </c>
       <c r="E2">
         <v>173967.18169986518</v>
@@ -2884,7 +2886,7 @@
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>495945.66539987986</v>
+        <v>971014.93540007516</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -2893,7 +2895,7 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9232313.8485606257</v>
+        <v>9238068.1339337192</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -2910,7 +2912,7 @@
         <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>8777.1098930121243</v>
+        <v>469594.30179320136</v>
       </c>
       <c r="E3">
         <v>196393.16624886921</v>
@@ -2919,16 +2921,16 @@
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>195674.25543808923</v>
+        <v>656491.44733827852</v>
       </c>
       <c r="H3">
-        <v>8560521.576256413</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3">
-        <v>8748355.1262564138</v>
+        <v>8417833.5499991123</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -2990,7 +2992,7 @@
         <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>309048.56689980475</v>
+        <v>784117.83689999999</v>
       </c>
       <c r="E2">
         <v>173967.18169986518</v>
@@ -2999,7 +3001,7 @@
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>495945.66539987986</v>
+        <v>971014.93540007516</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -3008,7 +3010,7 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9152584.198560629</v>
+        <v>9172476.3219337184</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -3025,7 +3027,7 @@
         <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>8777.1098930121243</v>
+        <v>469594.30179320136</v>
       </c>
       <c r="E3">
         <v>196393.16624886921</v>
@@ -3034,7 +3036,7 @@
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>195674.25543808923</v>
+        <v>656491.44733827852</v>
       </c>
       <c r="H3">
         <v>8999999.9999775533</v>
@@ -3105,7 +3107,7 @@
         <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>690617.8868998026</v>
+        <v>784117.83689999999</v>
       </c>
       <c r="E2">
         <v>173967.18169986518</v>
@@ -3114,7 +3116,7 @@
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>877514.98539987789</v>
+        <v>971014.93540007516</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -3123,7 +3125,7 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9179712.0325606279</v>
+        <v>9170622.7159337196</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -3140,7 +3142,7 @@
         <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>572899.35029261373</v>
+        <v>663594.30179280508</v>
       </c>
       <c r="E3">
         <v>196393.16624886921</v>
@@ -3149,7 +3151,7 @@
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>759796.49583769089</v>
+        <v>850491.44733788224</v>
       </c>
       <c r="H3">
         <v>8999999.9999775533</v>
@@ -3220,7 +3222,7 @@
         <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>309048.56689980475</v>
+        <v>784117.83689999999</v>
       </c>
       <c r="E2">
         <v>173967.18169986518</v>
@@ -3229,7 +3231,7 @@
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>495945.66539987986</v>
+        <v>971014.93540007516</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -3238,7 +3240,7 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9229407.5365606286</v>
+        <v>9206310.0519337188</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -3255,7 +3257,7 @@
         <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>584777.10989261325</v>
+        <v>1045594.3017928025</v>
       </c>
       <c r="E3">
         <v>196393.16624886921</v>
@@ -3264,16 +3266,16 @@
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>771674.25543769042</v>
+        <v>1232491.4473378796</v>
       </c>
       <c r="H3">
-        <v>11992387.379671589</v>
+        <v>12545893.573614381</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3">
-        <v>12140420.007671589</v>
+        <v>12693926.201614382</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -3335,7 +3337,7 @@
         <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>690617.8868998026</v>
+        <v>784117.83689999999</v>
       </c>
       <c r="E2">
         <v>173967.18169986518</v>
@@ -3344,16 +3346,16 @@
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>877514.98539987789</v>
+        <v>971014.93540007516</v>
       </c>
       <c r="H2">
-        <v>8229999.9999999981</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="I2">
         <v>1</v>
       </c>
       <c r="J2">
-        <v>8523374.800583072</v>
+        <v>9286498.0899337176</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -3370,7 +3372,7 @@
         <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>572899.3502926135</v>
+        <v>663594.30179280485</v>
       </c>
       <c r="E3">
         <v>196393.16624886921</v>
@@ -3379,16 +3381,16 @@
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>759796.49583769066</v>
+        <v>850491.44733788201</v>
       </c>
       <c r="H3">
-        <v>11668029.775882941</v>
+        <v>11554608.722576108</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3">
-        <v>11892933.107882941</v>
+        <v>11779512.054576108</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -3450,7 +3452,7 @@
         <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>690617.8868998026</v>
+        <v>784117.83689999999</v>
       </c>
       <c r="E2">
         <v>173967.18169986518</v>
@@ -3459,16 +3461,16 @@
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>877514.98539987789</v>
+        <v>971014.93540007516</v>
       </c>
       <c r="H2">
-        <v>8229999.9999999981</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="I2">
         <v>1</v>
       </c>
       <c r="J2">
-        <v>8548233.2685830705</v>
+        <v>9281192.4579337183</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -3485,7 +3487,7 @@
         <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>954899.35029261105</v>
+        <v>1045594.3017928025</v>
       </c>
       <c r="E3">
         <v>196393.16624886921</v>
@@ -3494,16 +3496,16 @@
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>1141796.495837688</v>
+        <v>1232491.4473378796</v>
       </c>
       <c r="H3">
-        <v>14089432.391883604</v>
+        <v>13949002.812472591</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3">
-        <v>14380739.593883602</v>
+        <v>14240310.014472591</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -3565,7 +3567,7 @@
         <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>690617.8868998026</v>
+        <v>784117.83689999999</v>
       </c>
       <c r="E2">
         <v>173967.18169986518</v>
@@ -3574,16 +3576,16 @@
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>877514.98539987789</v>
+        <v>971014.93540007516</v>
       </c>
       <c r="H2">
-        <v>8229999.9999999981</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="I2">
         <v>1</v>
       </c>
       <c r="J2">
-        <v>8478672.8385830726</v>
+        <v>9235483.3039337192</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -3600,7 +3602,7 @@
         <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>954899.35029261105</v>
+        <v>1045594.3017928025</v>
       </c>
       <c r="E3">
         <v>196393.16624886921</v>
@@ -3609,16 +3611,16 @@
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>1141796.495837688</v>
+        <v>1232491.4473378796</v>
       </c>
       <c r="H3">
-        <v>11310663.895884939</v>
+        <v>10852344.459874846</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3">
-        <v>11584513.777884938</v>
+        <v>11126194.341874847</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -3680,7 +3682,7 @@
         <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>309048.56689980475</v>
+        <v>784117.83689999999</v>
       </c>
       <c r="E2">
         <v>173967.18169986518</v>
@@ -3689,7 +3691,7 @@
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>495945.66539987986</v>
+        <v>971014.93540007516</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -3698,7 +3700,7 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9204651.0665606279</v>
+        <v>9202672.3259337191</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -3715,7 +3717,7 @@
         <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>584777.10989261325</v>
+        <v>1045594.3017928025</v>
       </c>
       <c r="E3">
         <v>196393.16624886921</v>
@@ -3724,16 +3726,16 @@
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>771674.25543769042</v>
+        <v>1232491.4473378796</v>
       </c>
       <c r="H3">
-        <v>8999999.9999775533</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3">
-        <v>9210604.3459775522</v>
+        <v>8440604.3459991124</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -3795,7 +3797,7 @@
         <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>405617.88689999998</v>
+        <v>784117.83689999999</v>
       </c>
       <c r="E2">
         <v>173967.18169986518</v>
@@ -3804,7 +3806,7 @@
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>592514.98540007521</v>
+        <v>971014.93540007516</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -3813,7 +3815,7 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9218164.958560627</v>
+        <v>9217276.5519337188</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -3830,7 +3832,7 @@
         <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>393449.35029299994</v>
+        <v>808094.30179299996</v>
       </c>
       <c r="E3">
         <v>196393.16624886921</v>
@@ -3839,7 +3841,7 @@
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>580346.49583807704</v>
+        <v>994991.44733807712</v>
       </c>
       <c r="H3">
         <v>8999999.9999775533</v>
@@ -3860,6 +3862,236 @@
 </file>
 
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>43466</v>
+      </c>
+      <c r="B2">
+        <v>47500.000000075197</v>
+      </c>
+      <c r="C2">
+        <v>50000.0985</v>
+      </c>
+      <c r="D2">
+        <v>784117.83689999999</v>
+      </c>
+      <c r="E2">
+        <v>173967.18169986518</v>
+      </c>
+      <c r="F2">
+        <v>89397</v>
+      </c>
+      <c r="G2">
+        <v>971014.93540007516</v>
+      </c>
+      <c r="H2">
+        <v>8999999.9999775533</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>9201566.5519337188</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>43831</v>
+      </c>
+      <c r="B3">
+        <v>47500.000000075197</v>
+      </c>
+      <c r="C3">
+        <v>50000.145545001898</v>
+      </c>
+      <c r="D3">
+        <v>808094.30179299996</v>
+      </c>
+      <c r="E3">
+        <v>196393.16624886921</v>
+      </c>
+      <c r="F3">
+        <v>89397</v>
+      </c>
+      <c r="G3">
+        <v>994991.44733807712</v>
+      </c>
+      <c r="H3">
+        <v>11609246.129619762</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>11754570.12961976</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>43466</v>
+      </c>
+      <c r="B2">
+        <v>47500.000000075197</v>
+      </c>
+      <c r="C2">
+        <v>50000.0985</v>
+      </c>
+      <c r="D2">
+        <v>784117.83689999999</v>
+      </c>
+      <c r="E2">
+        <v>173967.18169986518</v>
+      </c>
+      <c r="F2">
+        <v>89397</v>
+      </c>
+      <c r="G2">
+        <v>971014.93540007516</v>
+      </c>
+      <c r="H2">
+        <v>8999999.9999775533</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>9190029.5519337188</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>43831</v>
+      </c>
+      <c r="B3">
+        <v>47500.000000075197</v>
+      </c>
+      <c r="C3">
+        <v>50000.145545001898</v>
+      </c>
+      <c r="D3">
+        <v>808094.30179299996</v>
+      </c>
+      <c r="E3">
+        <v>196393.16624886921</v>
+      </c>
+      <c r="F3">
+        <v>89397</v>
+      </c>
+      <c r="G3">
+        <v>994991.44733807712</v>
+      </c>
+      <c r="H3">
+        <v>8590739.8193768449</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>8725242.8193768449</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -3922,7 +4154,7 @@
         <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>405617.88689999998</v>
+        <v>784117.83689999999</v>
       </c>
       <c r="E2">
         <v>173967.18169986518</v>
@@ -3931,16 +4163,16 @@
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>592514.98540007521</v>
+        <v>971014.93540007516</v>
       </c>
       <c r="H2">
-        <v>8229999.9999999981</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="I2">
         <v>1</v>
       </c>
       <c r="J2">
-        <v>8382534.8785830718</v>
+        <v>9158290.1219337191</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -3954,31 +4186,31 @@
         <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>50000.0985</v>
+        <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>405617.88689999981</v>
+        <v>663594.30179280508</v>
       </c>
       <c r="E3">
-        <v>202467.18169986518</v>
+        <v>196393.16624886921</v>
       </c>
       <c r="F3">
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>592514.98540007509</v>
+        <v>850491.44733788224</v>
       </c>
       <c r="H3">
-        <v>7479999.9999999981</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="I3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J3">
-        <v>7511744.7299999967</v>
+        <v>8261744.7299991101</v>
       </c>
       <c r="K3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -4037,7 +4269,7 @@
         <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>690617.8868998026</v>
+        <v>784117.83689999999</v>
       </c>
       <c r="E2">
         <v>173967.18169986518</v>
@@ -4046,7 +4278,7 @@
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>877514.98539987789</v>
+        <v>971014.93540007516</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -4055,7 +4287,7 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9262766.2385606263</v>
+        <v>9262806.33193372</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -4072,7 +4304,7 @@
         <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>669899.35029280838</v>
+        <v>760594.30179299985</v>
       </c>
       <c r="E3">
         <v>196393.16624886921</v>
@@ -4081,7 +4313,7 @@
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>856796.49583788554</v>
+        <v>947491.44733807701</v>
       </c>
       <c r="H3">
         <v>8999999.9999775533</v>
@@ -4152,7 +4384,7 @@
         <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>405617.88689999998</v>
+        <v>784117.83689999999</v>
       </c>
       <c r="E2">
         <v>173967.18169986518</v>
@@ -4161,7 +4393,7 @@
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>592514.98540007521</v>
+        <v>971014.93540007516</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -4170,7 +4402,7 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9215807.168560626</v>
+        <v>9219195.5519337188</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -4187,7 +4419,7 @@
         <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>678449.35029280256</v>
+        <v>1045594.3017928025</v>
       </c>
       <c r="E3">
         <v>196393.16624886921</v>
@@ -4196,16 +4428,16 @@
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>865346.49583787972</v>
+        <v>1232491.4473378796</v>
       </c>
       <c r="H3">
-        <v>11462836.566283172</v>
+        <v>13002503.049687358</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3">
-        <v>11675531.576283168</v>
+        <v>13215198.059687356</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -4267,7 +4499,7 @@
         <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>309048.56689980475</v>
+        <v>784117.83689999999</v>
       </c>
       <c r="E2">
         <v>173967.18169986518</v>
@@ -4276,7 +4508,7 @@
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>495945.66539987986</v>
+        <v>971014.93540007516</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -4285,7 +4517,7 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9209043.7185606286</v>
+        <v>9215351.5219337177</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -4299,19 +4531,19 @@
         <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>50000.0985</v>
+        <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>309048.56689980457</v>
+        <v>760594.30179299985</v>
       </c>
       <c r="E3">
-        <v>202467.18169986518</v>
+        <v>196393.16624886921</v>
       </c>
       <c r="F3">
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>495945.66539987968</v>
+        <v>947491.44733807701</v>
       </c>
       <c r="H3">
         <v>8999999.9999775533</v>
@@ -4323,7 +4555,7 @@
         <v>9183949.7199775539</v>
       </c>
       <c r="K3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -4382,7 +4614,7 @@
         <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>175186.8647267684</v>
+        <v>784117.83689999999</v>
       </c>
       <c r="E2">
         <v>173967.18169986518</v>
@@ -4391,7 +4623,7 @@
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>362083.96322684357</v>
+        <v>971014.93540007516</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -4400,7 +4632,7 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9246578.8885606267</v>
+        <v>9239928.6319337189</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -4414,31 +4646,31 @@
         <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>50000.0985</v>
+        <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>175186.86472676822</v>
+        <v>663594.30179280485</v>
       </c>
       <c r="E3">
-        <v>202467.18169986518</v>
+        <v>196393.16624886921</v>
       </c>
       <c r="F3">
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>362083.96322684339</v>
+        <v>850491.44733788201</v>
       </c>
       <c r="H3">
-        <v>7479999.9999999981</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="I3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J3">
-        <v>7640152.0699999966</v>
+        <v>9160152.0699775536</v>
       </c>
       <c r="K3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -4497,7 +4729,7 @@
         <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>309048.56689980475</v>
+        <v>784117.83689999999</v>
       </c>
       <c r="E2">
         <v>173967.18169986518</v>
@@ -4506,7 +4738,7 @@
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>495945.66539987986</v>
+        <v>971014.93540007516</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -4515,7 +4747,7 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9183262.3985606283</v>
+        <v>9191410.7519337181</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -4529,31 +4761,31 @@
         <v>47500.000000075197</v>
       </c>
       <c r="C3">
-        <v>50000.0985</v>
+        <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>309048.56689980457</v>
+        <v>469594.30179320136</v>
       </c>
       <c r="E3">
-        <v>202467.18169986518</v>
+        <v>196393.16624886921</v>
       </c>
       <c r="F3">
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>495945.66539987968</v>
+        <v>656491.44733827852</v>
       </c>
       <c r="H3">
-        <v>7479999.9999999981</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="I3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J3">
-        <v>7666027.3499999968</v>
+        <v>9186027.3499775529</v>
       </c>
       <c r="K3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
MTOM May 2019 Official Release
No Ruleset or Model File changes since last commit

Ruleset and Model File renamed to follow naming convention

Modified the LC water use schedules for a DCP scenario
</commit_message>
<xml_diff>
--- a/Output Data/MtomToCrss_Annual.xlsx
+++ b/Output Data/MtomToCrss_Annual.xlsx
@@ -5,52 +5,50 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\MTOM\dev\Output Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\COM460\RiverWare Models\Monthly Models\MTOM_Production\_MAY19_Production\Output Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12570" windowHeight="13590"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17856" windowHeight="8748"/>
   </bookViews>
   <sheets>
-    <sheet name="Trace38" sheetId="39" r:id="rId1"/>
-    <sheet name="Trace37" sheetId="38" r:id="rId2"/>
-    <sheet name="Trace36" sheetId="37" r:id="rId3"/>
-    <sheet name="Trace35" sheetId="36" r:id="rId4"/>
-    <sheet name="Trace34" sheetId="35" r:id="rId5"/>
-    <sheet name="Trace33" sheetId="34" r:id="rId6"/>
-    <sheet name="Trace32" sheetId="33" r:id="rId7"/>
-    <sheet name="Trace31" sheetId="32" r:id="rId8"/>
-    <sheet name="Trace30" sheetId="31" r:id="rId9"/>
-    <sheet name="Trace29" sheetId="30" r:id="rId10"/>
-    <sheet name="Trace28" sheetId="29" r:id="rId11"/>
-    <sheet name="Trace27" sheetId="28" r:id="rId12"/>
-    <sheet name="Trace26" sheetId="27" r:id="rId13"/>
-    <sheet name="Trace25" sheetId="26" r:id="rId14"/>
-    <sheet name="Trace24" sheetId="25" r:id="rId15"/>
-    <sheet name="Trace23" sheetId="24" r:id="rId16"/>
-    <sheet name="Trace22" sheetId="23" r:id="rId17"/>
-    <sheet name="Trace21" sheetId="22" r:id="rId18"/>
-    <sheet name="Trace20" sheetId="21" r:id="rId19"/>
-    <sheet name="Trace19" sheetId="20" r:id="rId20"/>
-    <sheet name="Trace18" sheetId="19" r:id="rId21"/>
-    <sheet name="Trace17" sheetId="18" r:id="rId22"/>
-    <sheet name="Trace16" sheetId="17" r:id="rId23"/>
-    <sheet name="Trace15" sheetId="16" r:id="rId24"/>
-    <sheet name="Trace14" sheetId="15" r:id="rId25"/>
-    <sheet name="Trace13" sheetId="14" r:id="rId26"/>
-    <sheet name="Trace12" sheetId="13" r:id="rId27"/>
-    <sheet name="Trace11" sheetId="12" r:id="rId28"/>
-    <sheet name="Trace10" sheetId="11" r:id="rId29"/>
-    <sheet name="Trace9" sheetId="10" r:id="rId30"/>
-    <sheet name="Trace8" sheetId="9" r:id="rId31"/>
-    <sheet name="Trace7" sheetId="8" r:id="rId32"/>
-    <sheet name="Trace6" sheetId="7" r:id="rId33"/>
-    <sheet name="Trace5" sheetId="6" r:id="rId34"/>
-    <sheet name="Trace4" sheetId="5" r:id="rId35"/>
-    <sheet name="Trace3" sheetId="4" r:id="rId36"/>
-    <sheet name="Trace2" sheetId="3" r:id="rId37"/>
-    <sheet name="Trace1" sheetId="2" r:id="rId38"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId39"/>
+    <sheet name="Trace38" sheetId="37" r:id="rId1"/>
+    <sheet name="Trace37" sheetId="36" r:id="rId2"/>
+    <sheet name="Trace36" sheetId="35" r:id="rId3"/>
+    <sheet name="Trace35" sheetId="34" r:id="rId4"/>
+    <sheet name="Trace34" sheetId="33" r:id="rId5"/>
+    <sheet name="Trace33" sheetId="32" r:id="rId6"/>
+    <sheet name="Trace32" sheetId="31" r:id="rId7"/>
+    <sheet name="Trace31" sheetId="30" r:id="rId8"/>
+    <sheet name="Trace30" sheetId="29" r:id="rId9"/>
+    <sheet name="Trace29" sheetId="28" r:id="rId10"/>
+    <sheet name="Trace28" sheetId="27" r:id="rId11"/>
+    <sheet name="Trace27" sheetId="26" r:id="rId12"/>
+    <sheet name="Trace26" sheetId="25" r:id="rId13"/>
+    <sheet name="Trace25" sheetId="24" r:id="rId14"/>
+    <sheet name="Trace24" sheetId="23" r:id="rId15"/>
+    <sheet name="Trace23" sheetId="22" r:id="rId16"/>
+    <sheet name="Trace22" sheetId="21" r:id="rId17"/>
+    <sheet name="Trace21" sheetId="20" r:id="rId18"/>
+    <sheet name="Trace20" sheetId="19" r:id="rId19"/>
+    <sheet name="Trace19" sheetId="18" r:id="rId20"/>
+    <sheet name="Trace18" sheetId="17" r:id="rId21"/>
+    <sheet name="Trace17" sheetId="16" r:id="rId22"/>
+    <sheet name="Trace16" sheetId="15" r:id="rId23"/>
+    <sheet name="Trace15" sheetId="14" r:id="rId24"/>
+    <sheet name="Trace14" sheetId="13" r:id="rId25"/>
+    <sheet name="Trace13" sheetId="12" r:id="rId26"/>
+    <sheet name="Trace12" sheetId="11" r:id="rId27"/>
+    <sheet name="Trace11" sheetId="10" r:id="rId28"/>
+    <sheet name="Trace10" sheetId="9" r:id="rId29"/>
+    <sheet name="Trace9" sheetId="8" r:id="rId30"/>
+    <sheet name="Trace8" sheetId="7" r:id="rId31"/>
+    <sheet name="Trace7" sheetId="6" r:id="rId32"/>
+    <sheet name="Trace6" sheetId="5" r:id="rId33"/>
+    <sheet name="Trace5" sheetId="4" r:id="rId34"/>
+    <sheet name="Trace4" sheetId="3" r:id="rId35"/>
+    <sheet name="Trace3" sheetId="2" r:id="rId36"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId37"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -62,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="10">
   <si>
     <t>ICS Credits.BiNationalICS_CA</t>
   </si>
@@ -417,9 +415,9 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -451,7 +449,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -462,16 +460,16 @@
         <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>784117.83689999999</v>
+        <v>874688.89999999991</v>
       </c>
       <c r="E2">
-        <v>173967.18169986518</v>
+        <v>299999.99999979226</v>
       </c>
       <c r="F2">
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>971014.93540007516</v>
+        <v>1061585.998500075</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -480,13 +478,13 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9204745.5919337161</v>
+        <v>9202165.4710313734</v>
       </c>
       <c r="K2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -497,25 +495,25 @@
         <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>760594.30179299985</v>
+        <v>848448.23300000001</v>
       </c>
       <c r="E3">
-        <v>196393.16624886921</v>
+        <v>299999.99999979226</v>
       </c>
       <c r="F3">
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>947491.44733807701</v>
+        <v>1035345.3785450769</v>
       </c>
       <c r="H3">
-        <v>8999999.9999775533</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3">
-        <v>9110981.0259775538</v>
+        <v>8340981.0259991111</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -532,9 +530,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -566,7 +564,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -577,16 +575,16 @@
         <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>784117.83689999999</v>
+        <v>874688.89999999991</v>
       </c>
       <c r="E2">
-        <v>173967.18169986518</v>
+        <v>299999.99999979226</v>
       </c>
       <c r="F2">
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>971014.93540007516</v>
+        <v>1061585.998500075</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -595,13 +593,13 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9276617.2819337193</v>
+        <v>9269230.0310313739</v>
       </c>
       <c r="K2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -612,16 +610,16 @@
         <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>663594.30179280508</v>
+        <v>751448.2329998049</v>
       </c>
       <c r="E3">
-        <v>196393.16624886921</v>
+        <v>299999.99999979226</v>
       </c>
       <c r="F3">
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>850491.44733788224</v>
+        <v>938345.37854488206</v>
       </c>
       <c r="H3">
         <v>8999999.9999775533</v>
@@ -647,9 +645,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -681,7 +679,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -692,16 +690,16 @@
         <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>784117.83689999999</v>
+        <v>874688.89999999991</v>
       </c>
       <c r="E2">
-        <v>173967.18169986518</v>
+        <v>299999.99999979226</v>
       </c>
       <c r="F2">
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>971014.93540007516</v>
+        <v>1061585.998500075</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -710,13 +708,13 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9216103.8919337187</v>
+        <v>9214071.6110313721</v>
       </c>
       <c r="K2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -727,25 +725,25 @@
         <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>1045594.3017928025</v>
+        <v>1133448.2329998026</v>
       </c>
       <c r="E3">
-        <v>196393.16624886921</v>
+        <v>299999.99999979226</v>
       </c>
       <c r="F3">
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>1232491.4473378796</v>
+        <v>1320345.3785448796</v>
       </c>
       <c r="H3">
-        <v>8999999.9999775533</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3">
-        <v>9263906.2799775526</v>
+        <v>8493906.2799991108</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -762,9 +760,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -796,7 +794,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -807,16 +805,16 @@
         <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>784117.83689999999</v>
+        <v>874688.89999999991</v>
       </c>
       <c r="E2">
-        <v>173967.18169986518</v>
+        <v>299999.99999979226</v>
       </c>
       <c r="F2">
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>971014.93540007516</v>
+        <v>1061585.998500075</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -825,13 +823,13 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9166551.50193372</v>
+        <v>9171368.1710313726</v>
       </c>
       <c r="K2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -842,25 +840,25 @@
         <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>903094.30179290124</v>
+        <v>990948.2329999014</v>
       </c>
       <c r="E3">
-        <v>196393.16624886921</v>
+        <v>299999.99999979226</v>
       </c>
       <c r="F3">
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>1089991.4473379783</v>
+        <v>1177845.3785449783</v>
       </c>
       <c r="H3">
-        <v>9712858.5941786692</v>
+        <v>9347088.6732832119</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3">
-        <v>9842026.3741786703</v>
+        <v>9476256.4532832131</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -877,9 +875,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -911,7 +909,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -922,16 +920,16 @@
         <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>784117.83689999999</v>
+        <v>874688.89999999991</v>
       </c>
       <c r="E2">
-        <v>173967.18169986518</v>
+        <v>299999.99999979226</v>
       </c>
       <c r="F2">
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>971014.93540007516</v>
+        <v>1061585.998500075</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -940,13 +938,13 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9217222.1119337194</v>
+        <v>9219705.0910313725</v>
       </c>
       <c r="K2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -957,16 +955,16 @@
         <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>760594.30179299985</v>
+        <v>848448.23299999977</v>
       </c>
       <c r="E3">
-        <v>196393.16624886921</v>
+        <v>299999.99999979226</v>
       </c>
       <c r="F3">
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>947491.44733807701</v>
+        <v>1035345.3785450769</v>
       </c>
       <c r="H3">
         <v>8999999.9999775533</v>
@@ -992,9 +990,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1026,7 +1024,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -1037,16 +1035,16 @@
         <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>784117.83689999999</v>
+        <v>874688.89999999991</v>
       </c>
       <c r="E2">
-        <v>173967.18169986518</v>
+        <v>299999.99999979226</v>
       </c>
       <c r="F2">
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>971014.93540007516</v>
+        <v>1061585.998500075</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -1055,13 +1053,13 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9216979.461933719</v>
+        <v>9210634.0810313728</v>
       </c>
       <c r="K2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -1072,16 +1070,16 @@
         <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>903094.30179290124</v>
+        <v>990948.2329999014</v>
       </c>
       <c r="E3">
-        <v>196393.16624886921</v>
+        <v>299999.99999979226</v>
       </c>
       <c r="F3">
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>1089991.4473379783</v>
+        <v>1177845.3785449783</v>
       </c>
       <c r="H3">
         <v>8999999.9999775533</v>
@@ -1107,9 +1105,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1141,7 +1139,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -1152,16 +1150,16 @@
         <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>784117.83689999999</v>
+        <v>874688.89999999991</v>
       </c>
       <c r="E2">
-        <v>173967.18169986518</v>
+        <v>299999.99999979226</v>
       </c>
       <c r="F2">
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>971014.93540007516</v>
+        <v>1061585.998500075</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -1170,13 +1168,13 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9186684.3419337198</v>
+        <v>9176487.9810313731</v>
       </c>
       <c r="K2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -1187,25 +1185,25 @@
         <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>663594.30179280485</v>
+        <v>751448.23299980513</v>
       </c>
       <c r="E3">
-        <v>196393.16624886921</v>
+        <v>299999.99999979226</v>
       </c>
       <c r="F3">
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>850491.44733788201</v>
+        <v>938345.37854488229</v>
       </c>
       <c r="H3">
-        <v>8855069.1936470252</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3">
-        <v>8963782.8436470237</v>
+        <v>8338713.64999911</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -1222,9 +1220,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1256,7 +1254,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -1267,16 +1265,16 @@
         <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>784117.83689999999</v>
+        <v>874688.89999999991</v>
       </c>
       <c r="E2">
-        <v>173967.18169986518</v>
+        <v>299999.99999979226</v>
       </c>
       <c r="F2">
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>971014.93540007516</v>
+        <v>1061585.998500075</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -1285,13 +1283,13 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9242730.2619337197</v>
+        <v>9238349.8910313733</v>
       </c>
       <c r="K2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -1302,16 +1300,16 @@
         <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>663594.30179280508</v>
+        <v>751448.2329998049</v>
       </c>
       <c r="E3">
-        <v>196393.16624886921</v>
+        <v>299999.99999979226</v>
       </c>
       <c r="F3">
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>850491.44733788224</v>
+        <v>938345.37854488206</v>
       </c>
       <c r="H3">
         <v>8999999.9999775533</v>
@@ -1337,9 +1335,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1371,7 +1369,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -1382,16 +1380,16 @@
         <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>784117.83689999999</v>
+        <v>874688.89999999991</v>
       </c>
       <c r="E2">
-        <v>173967.18169986518</v>
+        <v>299999.99999979226</v>
       </c>
       <c r="F2">
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>971014.93540007516</v>
+        <v>1061585.998500075</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -1400,13 +1398,13 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9230358.4719337188</v>
+        <v>9217958.3110313714</v>
       </c>
       <c r="K2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -1417,25 +1415,25 @@
         <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>903094.30179290124</v>
+        <v>990948.2329999014</v>
       </c>
       <c r="E3">
-        <v>196393.16624886921</v>
+        <v>299999.99999979226</v>
       </c>
       <c r="F3">
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>1089991.4473379783</v>
+        <v>1177845.3785449783</v>
       </c>
       <c r="H3">
-        <v>8999999.9999775533</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3">
-        <v>9140628.0299775563</v>
+        <v>8370628.0299991118</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -1452,9 +1450,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1486,7 +1484,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -1497,16 +1495,16 @@
         <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>784117.83689999999</v>
+        <v>874688.89999999991</v>
       </c>
       <c r="E2">
-        <v>173967.18169986518</v>
+        <v>299999.99999979226</v>
       </c>
       <c r="F2">
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>971014.93540007516</v>
+        <v>1061585.998500075</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -1515,13 +1513,13 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9115498.6519337185</v>
+        <v>9124859.8110313714</v>
       </c>
       <c r="K2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -1532,16 +1530,16 @@
         <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>1045594.3017928025</v>
+        <v>1133448.2329998026</v>
       </c>
       <c r="E3">
-        <v>196393.16624886921</v>
+        <v>299999.99999979226</v>
       </c>
       <c r="F3">
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>1232491.4473378796</v>
+        <v>1320345.3785448796</v>
       </c>
       <c r="H3">
         <v>8229999.9999991106</v>
@@ -1567,9 +1565,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1601,7 +1599,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -1612,16 +1610,16 @@
         <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>784117.83689999999</v>
+        <v>874688.89999999991</v>
       </c>
       <c r="E2">
-        <v>173967.18169986518</v>
+        <v>299999.99999979226</v>
       </c>
       <c r="F2">
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>971014.93540007516</v>
+        <v>1061585.998500075</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -1630,13 +1628,13 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9160244.5719337184</v>
+        <v>9160551.2410313729</v>
       </c>
       <c r="K2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -1647,25 +1645,25 @@
         <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>1045594.3017928025</v>
+        <v>1133448.2329998026</v>
       </c>
       <c r="E3">
-        <v>196393.16624886921</v>
+        <v>299999.99999979226</v>
       </c>
       <c r="F3">
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>1232491.4473378796</v>
+        <v>1320345.3785448796</v>
       </c>
       <c r="H3">
-        <v>10887492.807684025</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3">
-        <v>10797865.317684025</v>
+        <v>8140372.5099991113</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -1682,9 +1680,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1716,7 +1714,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -1727,16 +1725,16 @@
         <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>784117.83689999999</v>
+        <v>874688.89999999991</v>
       </c>
       <c r="E2">
-        <v>173967.18169986518</v>
+        <v>299999.99999979226</v>
       </c>
       <c r="F2">
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>971014.93540007516</v>
+        <v>1061585.998500075</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -1745,13 +1743,13 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9202557.1019337177</v>
+        <v>9199812.8910313714</v>
       </c>
       <c r="K2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -1762,16 +1760,16 @@
         <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>469594.30179320136</v>
+        <v>569203.63171038928</v>
       </c>
       <c r="E3">
-        <v>196393.16624886921</v>
+        <v>299999.99999979226</v>
       </c>
       <c r="F3">
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>656491.44733827852</v>
+        <v>756100.77725546644</v>
       </c>
       <c r="H3">
         <v>8999999.9999775533</v>
@@ -1797,9 +1795,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1831,7 +1829,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -1842,16 +1840,16 @@
         <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>784117.83689999999</v>
+        <v>874688.89999999991</v>
       </c>
       <c r="E2">
-        <v>173967.18169986518</v>
+        <v>299999.99999979226</v>
       </c>
       <c r="F2">
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>971014.93540007516</v>
+        <v>1061585.998500075</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -1860,13 +1858,13 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9203493.3419337198</v>
+        <v>9187004.7050313726</v>
       </c>
       <c r="K2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -1877,25 +1875,25 @@
         <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>1045594.3017928025</v>
+        <v>1133448.2329998026</v>
       </c>
       <c r="E3">
-        <v>196393.16624886921</v>
+        <v>299999.99999979226</v>
       </c>
       <c r="F3">
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>1232491.4473378796</v>
+        <v>1320345.3785448796</v>
       </c>
       <c r="H3">
-        <v>11456726.940617843</v>
+        <v>11911747.235998331</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3">
-        <v>11518398.626617841</v>
+        <v>11973418.921998331</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -1912,9 +1910,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1946,7 +1944,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -1957,16 +1955,16 @@
         <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>784117.83689999999</v>
+        <v>874688.89999999991</v>
       </c>
       <c r="E2">
-        <v>173967.18169986518</v>
+        <v>299999.99999979226</v>
       </c>
       <c r="F2">
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>971014.93540007516</v>
+        <v>1061585.998500075</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -1975,13 +1973,13 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9247681.9079337176</v>
+        <v>9240120.4630313721</v>
       </c>
       <c r="K2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -1992,25 +1990,25 @@
         <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>1045594.3017928025</v>
+        <v>1133448.2329998026</v>
       </c>
       <c r="E3">
-        <v>196393.16624886921</v>
+        <v>299999.99999979226</v>
       </c>
       <c r="F3">
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>1232491.4473378796</v>
+        <v>1320345.3785448796</v>
       </c>
       <c r="H3">
-        <v>11984459.9762755</v>
+        <v>10897893.102191133</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3">
-        <v>12112978.708275499</v>
+        <v>11026411.834191134</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -2027,9 +2025,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2061,7 +2059,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -2072,16 +2070,16 @@
         <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>784117.83689999999</v>
+        <v>874688.89999999991</v>
       </c>
       <c r="E2">
-        <v>173967.18169986518</v>
+        <v>299999.99999979226</v>
       </c>
       <c r="F2">
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>971014.93540007516</v>
+        <v>1061585.998500075</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -2090,13 +2088,13 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9181276.6819337197</v>
+        <v>9180657.8090313729</v>
       </c>
       <c r="K2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -2107,25 +2105,25 @@
         <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>1045594.3017928025</v>
+        <v>1133448.2329998026</v>
       </c>
       <c r="E3">
-        <v>196393.16624886921</v>
+        <v>299999.99999979226</v>
       </c>
       <c r="F3">
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>1232491.4473378796</v>
+        <v>1320345.3785448796</v>
       </c>
       <c r="H3">
-        <v>11848797.186601833</v>
+        <v>11232587.143865276</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3">
-        <v>12131217.490601834</v>
+        <v>11515007.447865276</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -2142,9 +2140,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2176,7 +2174,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -2187,16 +2185,16 @@
         <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>784117.83689999999</v>
+        <v>874688.89999999991</v>
       </c>
       <c r="E2">
-        <v>173967.18169986518</v>
+        <v>299999.99999979226</v>
       </c>
       <c r="F2">
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>971014.93540007516</v>
+        <v>1061585.998500075</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -2205,13 +2203,13 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9244710.9439337198</v>
+        <v>9210596.5830313731</v>
       </c>
       <c r="K2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -2222,16 +2220,16 @@
         <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>469594.30179320095</v>
+        <v>557448.23300020129</v>
       </c>
       <c r="E3">
-        <v>196393.16624886921</v>
+        <v>299999.99999979226</v>
       </c>
       <c r="F3">
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>656491.44733827817</v>
+        <v>744345.37854527857</v>
       </c>
       <c r="H3">
         <v>8999999.9999775533</v>
@@ -2257,9 +2255,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2291,7 +2289,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -2302,16 +2300,16 @@
         <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>784117.83689999999</v>
+        <v>874688.89999999991</v>
       </c>
       <c r="E2">
-        <v>173967.18169986518</v>
+        <v>299999.99999979226</v>
       </c>
       <c r="F2">
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>971014.93540007516</v>
+        <v>1061585.998500075</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -2320,13 +2318,13 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9250298.2239337191</v>
+        <v>9227682.2070313711</v>
       </c>
       <c r="K2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -2337,25 +2335,25 @@
         <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>903094.30179290124</v>
+        <v>990948.2329999014</v>
       </c>
       <c r="E3">
-        <v>196393.16624886921</v>
+        <v>299999.99999979226</v>
       </c>
       <c r="F3">
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>1089991.4473379783</v>
+        <v>1177845.3785449783</v>
       </c>
       <c r="H3">
-        <v>10163846.826235268</v>
+        <v>12390814.127053976</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3">
-        <v>10573665.05023527</v>
+        <v>12800632.351053976</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -2372,9 +2370,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2406,7 +2404,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -2417,16 +2415,16 @@
         <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>784117.83689999999</v>
+        <v>874688.89999999991</v>
       </c>
       <c r="E2">
-        <v>173967.18169986518</v>
+        <v>299999.99999979226</v>
       </c>
       <c r="F2">
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>971014.93540007516</v>
+        <v>1061585.998500075</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -2435,13 +2433,13 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9224994.0099337194</v>
+        <v>9213742.3070313726</v>
       </c>
       <c r="K2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -2452,16 +2450,16 @@
         <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>469594.30179320136</v>
+        <v>569203.63171038928</v>
       </c>
       <c r="E3">
-        <v>196393.16624886921</v>
+        <v>299999.99999979226</v>
       </c>
       <c r="F3">
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>656491.44733827852</v>
+        <v>756100.77725546644</v>
       </c>
       <c r="H3">
         <v>8229999.9999991106</v>
@@ -2487,9 +2485,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2521,7 +2519,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -2532,16 +2530,16 @@
         <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>784117.83689999999</v>
+        <v>874688.89999999991</v>
       </c>
       <c r="E2">
-        <v>173967.18169986518</v>
+        <v>299999.99999979226</v>
       </c>
       <c r="F2">
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>971014.93540007516</v>
+        <v>1061585.998500075</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -2550,13 +2548,13 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9203868.1699337177</v>
+        <v>9206563.8590313718</v>
       </c>
       <c r="K2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -2567,25 +2565,25 @@
         <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>469594.30179320136</v>
+        <v>569203.63171038928</v>
       </c>
       <c r="E3">
-        <v>196393.16624886921</v>
+        <v>299999.99999979226</v>
       </c>
       <c r="F3">
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>656491.44733827852</v>
+        <v>756100.77725546644</v>
       </c>
       <c r="H3">
-        <v>8999999.9999775533</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3">
-        <v>9174589.2299775518</v>
+        <v>8404589.229999112</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -2602,9 +2600,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2636,7 +2634,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -2647,16 +2645,16 @@
         <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>784117.83689999999</v>
+        <v>874688.89999999991</v>
       </c>
       <c r="E2">
-        <v>173967.18169986518</v>
+        <v>299999.99999979226</v>
       </c>
       <c r="F2">
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>971014.93540007516</v>
+        <v>1061585.998500075</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -2665,13 +2663,13 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9198838.5759337191</v>
+        <v>9192975.9250313733</v>
       </c>
       <c r="K2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -2682,16 +2680,16 @@
         <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>760594.30179299985</v>
+        <v>848448.23300000001</v>
       </c>
       <c r="E3">
-        <v>196393.16624886921</v>
+        <v>299999.99999979226</v>
       </c>
       <c r="F3">
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>947491.44733807701</v>
+        <v>1035345.3785450769</v>
       </c>
       <c r="H3">
         <v>8229999.9999991106</v>
@@ -2717,9 +2715,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2751,7 +2749,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -2762,16 +2760,16 @@
         <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>784117.83689999999</v>
+        <v>874688.89999999991</v>
       </c>
       <c r="E2">
-        <v>173967.18169986518</v>
+        <v>299999.99999979226</v>
       </c>
       <c r="F2">
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>971014.93540007516</v>
+        <v>1061585.998500075</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -2780,13 +2778,13 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9214828.7199337184</v>
+        <v>9196473.5150313731</v>
       </c>
       <c r="K2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -2797,25 +2795,25 @@
         <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>663594.30179280508</v>
+        <v>751448.2329998049</v>
       </c>
       <c r="E3">
-        <v>196393.16624886921</v>
+        <v>299999.99999979226</v>
       </c>
       <c r="F3">
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>850491.44733788224</v>
+        <v>938345.37854488206</v>
       </c>
       <c r="H3">
-        <v>8999999.9999775533</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3">
-        <v>9150597.6699775569</v>
+        <v>8380597.6699991105</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -2832,9 +2830,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2866,7 +2864,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -2877,16 +2875,16 @@
         <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>784117.83689999999</v>
+        <v>874688.89999999991</v>
       </c>
       <c r="E2">
-        <v>173967.18169986518</v>
+        <v>299999.99999979226</v>
       </c>
       <c r="F2">
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>971014.93540007516</v>
+        <v>1061585.998500075</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -2895,13 +2893,13 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9238068.1339337192</v>
+        <v>9224638.2990313731</v>
       </c>
       <c r="K2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -2912,16 +2910,16 @@
         <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>469594.30179320136</v>
+        <v>569203.63171038928</v>
       </c>
       <c r="E3">
-        <v>196393.16624886921</v>
+        <v>299999.99999979226</v>
       </c>
       <c r="F3">
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>656491.44733827852</v>
+        <v>756100.77725546644</v>
       </c>
       <c r="H3">
         <v>8229999.9999991106</v>
@@ -2947,9 +2945,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2981,7 +2979,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -2992,16 +2990,16 @@
         <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>784117.83689999999</v>
+        <v>874688.89999999991</v>
       </c>
       <c r="E2">
-        <v>173967.18169986518</v>
+        <v>299999.99999979226</v>
       </c>
       <c r="F2">
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>971014.93540007516</v>
+        <v>1061585.998500075</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -3010,13 +3008,13 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9172476.3219337184</v>
+        <v>9181049.6010313723</v>
       </c>
       <c r="K2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -3027,16 +3025,16 @@
         <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>469594.30179320136</v>
+        <v>569203.63171038928</v>
       </c>
       <c r="E3">
-        <v>196393.16624886921</v>
+        <v>299999.99999979226</v>
       </c>
       <c r="F3">
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>656491.44733827852</v>
+        <v>756100.77725546644</v>
       </c>
       <c r="H3">
         <v>8999999.9999775533</v>
@@ -3062,9 +3060,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -3096,7 +3094,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -3107,16 +3105,16 @@
         <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>784117.83689999999</v>
+        <v>874688.89999999991</v>
       </c>
       <c r="E2">
-        <v>173967.18169986518</v>
+        <v>299999.99999979226</v>
       </c>
       <c r="F2">
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>971014.93540007516</v>
+        <v>1061585.998500075</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -3125,13 +3123,13 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9170622.7159337196</v>
+        <v>9154328.281031372</v>
       </c>
       <c r="K2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -3142,16 +3140,16 @@
         <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>663594.30179280508</v>
+        <v>751448.2329998049</v>
       </c>
       <c r="E3">
-        <v>196393.16624886921</v>
+        <v>299999.99999979226</v>
       </c>
       <c r="F3">
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>850491.44733788224</v>
+        <v>938345.37854488206</v>
       </c>
       <c r="H3">
         <v>8999999.9999775533</v>
@@ -3177,9 +3175,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -3211,7 +3209,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -3222,16 +3220,16 @@
         <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>784117.83689999999</v>
+        <v>874688.89999999991</v>
       </c>
       <c r="E2">
-        <v>173967.18169986518</v>
+        <v>299999.99999979226</v>
       </c>
       <c r="F2">
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>971014.93540007516</v>
+        <v>1061585.998500075</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -3240,13 +3238,13 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9206310.0519337188</v>
+        <v>9185450.1030313727</v>
       </c>
       <c r="K2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -3257,25 +3255,25 @@
         <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>1045594.3017928025</v>
+        <v>1133448.2329998026</v>
       </c>
       <c r="E3">
-        <v>196393.16624886921</v>
+        <v>299999.99999979226</v>
       </c>
       <c r="F3">
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>1232491.4473378796</v>
+        <v>1320345.3785448796</v>
       </c>
       <c r="H3">
-        <v>12545893.573614381</v>
+        <v>11966059.422844531</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3">
-        <v>12693926.201614382</v>
+        <v>12114092.050844532</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -3292,9 +3290,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -3326,7 +3324,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -3337,16 +3335,16 @@
         <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>784117.83689999999</v>
+        <v>874688.89999999991</v>
       </c>
       <c r="E2">
-        <v>173967.18169986518</v>
+        <v>299999.99999979226</v>
       </c>
       <c r="F2">
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>971014.93540007516</v>
+        <v>1061585.998500075</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -3355,13 +3353,13 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9286498.0899337176</v>
+        <v>9268756.3110313714</v>
       </c>
       <c r="K2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -3372,25 +3370,25 @@
         <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>663594.30179280485</v>
+        <v>751448.2329998049</v>
       </c>
       <c r="E3">
-        <v>196393.16624886921</v>
+        <v>299999.99999979226</v>
       </c>
       <c r="F3">
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>850491.44733788201</v>
+        <v>938345.37854488206</v>
       </c>
       <c r="H3">
-        <v>11554608.722576108</v>
+        <v>10602350.610126313</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3">
-        <v>11779512.054576108</v>
+        <v>10827253.942126315</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -3407,9 +3405,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -3441,7 +3439,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -3452,16 +3450,16 @@
         <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>784117.83689999999</v>
+        <v>874688.89999999991</v>
       </c>
       <c r="E2">
-        <v>173967.18169986518</v>
+        <v>299999.99999979226</v>
       </c>
       <c r="F2">
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>971014.93540007516</v>
+        <v>1061585.998500075</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -3470,13 +3468,13 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9281192.4579337183</v>
+        <v>9262570.127031371</v>
       </c>
       <c r="K2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -3487,25 +3485,25 @@
         <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>1045594.3017928025</v>
+        <v>1133448.2329998026</v>
       </c>
       <c r="E3">
-        <v>196393.16624886921</v>
+        <v>299999.99999979226</v>
       </c>
       <c r="F3">
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>1232491.4473378796</v>
+        <v>1320345.3785448796</v>
       </c>
       <c r="H3">
-        <v>13949002.812472591</v>
+        <v>13920385.963511307</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3">
-        <v>14240310.014472591</v>
+        <v>14211693.165511308</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -3522,9 +3520,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -3556,7 +3554,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -3567,16 +3565,16 @@
         <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>784117.83689999999</v>
+        <v>874688.89999999991</v>
       </c>
       <c r="E2">
-        <v>173967.18169986518</v>
+        <v>299999.99999979226</v>
       </c>
       <c r="F2">
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>971014.93540007516</v>
+        <v>1061585.998500075</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -3585,13 +3583,13 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9235483.3039337192</v>
+        <v>9225949.5910313707</v>
       </c>
       <c r="K2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -3602,25 +3600,25 @@
         <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>1045594.3017928025</v>
+        <v>1133448.2329998026</v>
       </c>
       <c r="E3">
-        <v>196393.16624886921</v>
+        <v>299999.99999979226</v>
       </c>
       <c r="F3">
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>1232491.4473378796</v>
+        <v>1320345.3785448796</v>
       </c>
       <c r="H3">
-        <v>10852344.459874846</v>
+        <v>12614602.096068762</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3">
-        <v>11126194.341874847</v>
+        <v>12888451.978068763</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -3637,9 +3635,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -3671,7 +3669,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -3682,16 +3680,16 @@
         <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>784117.83689999999</v>
+        <v>874688.89999999991</v>
       </c>
       <c r="E2">
-        <v>173967.18169986518</v>
+        <v>299999.99999979226</v>
       </c>
       <c r="F2">
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>971014.93540007516</v>
+        <v>1061585.998500075</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -3700,13 +3698,13 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9202672.3259337191</v>
+        <v>9200901.2210313734</v>
       </c>
       <c r="K2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -3717,25 +3715,25 @@
         <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>1045594.3017928025</v>
+        <v>1133448.2329998026</v>
       </c>
       <c r="E3">
-        <v>196393.16624886921</v>
+        <v>299999.99999979226</v>
       </c>
       <c r="F3">
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>1232491.4473378796</v>
+        <v>1320345.3785448796</v>
       </c>
       <c r="H3">
-        <v>8229999.9999991106</v>
+        <v>10282289.249708919</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3">
-        <v>8440604.3459991124</v>
+        <v>10492893.595708918</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -3752,9 +3750,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -3786,7 +3784,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -3797,16 +3795,16 @@
         <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>784117.83689999999</v>
+        <v>874688.89999999991</v>
       </c>
       <c r="E2">
-        <v>173967.18169986518</v>
+        <v>299999.99999979226</v>
       </c>
       <c r="F2">
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>971014.93540007516</v>
+        <v>1061585.998500075</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -3815,13 +3813,13 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9217276.5519337188</v>
+        <v>9209476.861031374</v>
       </c>
       <c r="K2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -3832,16 +3830,16 @@
         <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>808094.30179299996</v>
+        <v>895948.23300000001</v>
       </c>
       <c r="E3">
-        <v>196393.16624886921</v>
+        <v>299999.99999979226</v>
       </c>
       <c r="F3">
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>994991.44733807712</v>
+        <v>1082845.3785450771</v>
       </c>
       <c r="H3">
         <v>8999999.9999775533</v>
@@ -3863,241 +3861,11 @@
 
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>43466</v>
-      </c>
-      <c r="B2">
-        <v>47500.000000075197</v>
-      </c>
-      <c r="C2">
-        <v>50000.0985</v>
-      </c>
-      <c r="D2">
-        <v>784117.83689999999</v>
-      </c>
-      <c r="E2">
-        <v>173967.18169986518</v>
-      </c>
-      <c r="F2">
-        <v>89397</v>
-      </c>
-      <c r="G2">
-        <v>971014.93540007516</v>
-      </c>
-      <c r="H2">
-        <v>8999999.9999775533</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-      <c r="J2">
-        <v>9201566.5519337188</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>43831</v>
-      </c>
-      <c r="B3">
-        <v>47500.000000075197</v>
-      </c>
-      <c r="C3">
-        <v>50000.145545001898</v>
-      </c>
-      <c r="D3">
-        <v>808094.30179299996</v>
-      </c>
-      <c r="E3">
-        <v>196393.16624886921</v>
-      </c>
-      <c r="F3">
-        <v>89397</v>
-      </c>
-      <c r="G3">
-        <v>994991.44733807712</v>
-      </c>
-      <c r="H3">
-        <v>11609246.129619762</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-      <c r="J3">
-        <v>11754570.12961976</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>43466</v>
-      </c>
-      <c r="B2">
-        <v>47500.000000075197</v>
-      </c>
-      <c r="C2">
-        <v>50000.0985</v>
-      </c>
-      <c r="D2">
-        <v>784117.83689999999</v>
-      </c>
-      <c r="E2">
-        <v>173967.18169986518</v>
-      </c>
-      <c r="F2">
-        <v>89397</v>
-      </c>
-      <c r="G2">
-        <v>971014.93540007516</v>
-      </c>
-      <c r="H2">
-        <v>8999999.9999775533</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-      <c r="J2">
-        <v>9190029.5519337188</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>43831</v>
-      </c>
-      <c r="B3">
-        <v>47500.000000075197</v>
-      </c>
-      <c r="C3">
-        <v>50000.145545001898</v>
-      </c>
-      <c r="D3">
-        <v>808094.30179299996</v>
-      </c>
-      <c r="E3">
-        <v>196393.16624886921</v>
-      </c>
-      <c r="F3">
-        <v>89397</v>
-      </c>
-      <c r="G3">
-        <v>994991.44733807712</v>
-      </c>
-      <c r="H3">
-        <v>8590739.8193768449</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-      <c r="J3">
-        <v>8725242.8193768449</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4109,9 +3877,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -4143,7 +3911,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -4154,16 +3922,16 @@
         <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>784117.83689999999</v>
+        <v>874688.89999999991</v>
       </c>
       <c r="E2">
-        <v>173967.18169986518</v>
+        <v>299999.99999979226</v>
       </c>
       <c r="F2">
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>971014.93540007516</v>
+        <v>1061585.998500075</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -4172,13 +3940,13 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9158290.1219337191</v>
+        <v>9160012.7710313722</v>
       </c>
       <c r="K2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -4189,25 +3957,25 @@
         <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>663594.30179280508</v>
+        <v>751448.2329998049</v>
       </c>
       <c r="E3">
-        <v>196393.16624886921</v>
+        <v>299999.99999979226</v>
       </c>
       <c r="F3">
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>850491.44733788224</v>
+        <v>938345.37854488206</v>
       </c>
       <c r="H3">
-        <v>8229999.9999991106</v>
+        <v>8517552.9221072532</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3">
-        <v>8261744.7299991101</v>
+        <v>8549297.6521072537</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -4224,9 +3992,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -4258,7 +4026,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -4269,16 +4037,16 @@
         <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>784117.83689999999</v>
+        <v>874688.89999999991</v>
       </c>
       <c r="E2">
-        <v>173967.18169986518</v>
+        <v>299999.99999979226</v>
       </c>
       <c r="F2">
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>971014.93540007516</v>
+        <v>1061585.998500075</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -4287,13 +4055,13 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9262806.33193372</v>
+        <v>9247417.0410313737</v>
       </c>
       <c r="K2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -4304,16 +4072,16 @@
         <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>760594.30179299985</v>
+        <v>848448.23299999977</v>
       </c>
       <c r="E3">
-        <v>196393.16624886921</v>
+        <v>299999.99999979226</v>
       </c>
       <c r="F3">
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>947491.44733807701</v>
+        <v>1035345.3785450769</v>
       </c>
       <c r="H3">
         <v>8999999.9999775533</v>
@@ -4339,9 +4107,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -4373,7 +4141,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -4384,16 +4152,16 @@
         <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>784117.83689999999</v>
+        <v>874688.89999999991</v>
       </c>
       <c r="E2">
-        <v>173967.18169986518</v>
+        <v>299999.99999979226</v>
       </c>
       <c r="F2">
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>971014.93540007516</v>
+        <v>1061585.998500075</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -4402,13 +4170,13 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9219195.5519337188</v>
+        <v>9213817.8610313721</v>
       </c>
       <c r="K2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -4419,25 +4187,25 @@
         <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>1045594.3017928025</v>
+        <v>1133448.2329998026</v>
       </c>
       <c r="E3">
-        <v>196393.16624886921</v>
+        <v>299999.99999979226</v>
       </c>
       <c r="F3">
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>1232491.4473378796</v>
+        <v>1320345.3785448796</v>
       </c>
       <c r="H3">
-        <v>13002503.049687358</v>
+        <v>12537886.187006619</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3">
-        <v>13215198.059687356</v>
+        <v>12750581.197006619</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -4454,9 +4222,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -4488,7 +4256,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -4499,16 +4267,16 @@
         <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>784117.83689999999</v>
+        <v>874688.89999999991</v>
       </c>
       <c r="E2">
-        <v>173967.18169986518</v>
+        <v>299999.99999979226</v>
       </c>
       <c r="F2">
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>971014.93540007516</v>
+        <v>1061585.998500075</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -4517,13 +4285,13 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9215351.5219337177</v>
+        <v>9215021.3610313721</v>
       </c>
       <c r="K2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -4534,16 +4302,16 @@
         <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>760594.30179299985</v>
+        <v>848448.23299999977</v>
       </c>
       <c r="E3">
-        <v>196393.16624886921</v>
+        <v>299999.99999979226</v>
       </c>
       <c r="F3">
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>947491.44733807701</v>
+        <v>1035345.3785450769</v>
       </c>
       <c r="H3">
         <v>8999999.9999775533</v>
@@ -4569,9 +4337,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -4603,7 +4371,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -4614,16 +4382,16 @@
         <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>784117.83689999999</v>
+        <v>874688.89999999991</v>
       </c>
       <c r="E2">
-        <v>173967.18169986518</v>
+        <v>299999.99999979226</v>
       </c>
       <c r="F2">
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>971014.93540007516</v>
+        <v>1061585.998500075</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -4632,13 +4400,13 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9239928.6319337189</v>
+        <v>9234303.781031372</v>
       </c>
       <c r="K2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -4649,16 +4417,16 @@
         <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>663594.30179280485</v>
+        <v>751448.23299980513</v>
       </c>
       <c r="E3">
-        <v>196393.16624886921</v>
+        <v>299999.99999979226</v>
       </c>
       <c r="F3">
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>850491.44733788201</v>
+        <v>938345.37854488229</v>
       </c>
       <c r="H3">
         <v>8999999.9999775533</v>
@@ -4684,9 +4452,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -4718,7 +4486,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -4729,16 +4497,16 @@
         <v>50000.0985</v>
       </c>
       <c r="D2">
-        <v>784117.83689999999</v>
+        <v>874688.89999999991</v>
       </c>
       <c r="E2">
-        <v>173967.18169986518</v>
+        <v>299999.99999979226</v>
       </c>
       <c r="F2">
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>971014.93540007516</v>
+        <v>1061585.998500075</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -4747,13 +4515,13 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9191410.7519337181</v>
+        <v>9194470.0210313722</v>
       </c>
       <c r="K2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -4764,16 +4532,16 @@
         <v>50000.145545001898</v>
       </c>
       <c r="D3">
-        <v>469594.30179320136</v>
+        <v>569203.63171038928</v>
       </c>
       <c r="E3">
-        <v>196393.16624886921</v>
+        <v>299999.99999979226</v>
       </c>
       <c r="F3">
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>656491.44733827852</v>
+        <v>756100.77725546644</v>
       </c>
       <c r="H3">
         <v>8999999.9999775533</v>

</xml_diff>

<commit_message>
May 2019 Official Run (Updated)
Updated Mead Bank Parameters Table for lower basin in ICS Credits data object
Updated rule for Flaming Gorge
Updated CRIT water use schedule to reflect DCP

Updated ruleset name to v2.6
</commit_message>
<xml_diff>
--- a/Output Data/MtomToCrss_Annual.xlsx
+++ b/Output Data/MtomToCrss_Annual.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\COM460\RiverWare Models\Monthly Models\MTOM_Production\_MAY19_Production\Output Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\D_Drive\Modeling\MTOM-dev\Output Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17856" windowHeight="8748"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22965" windowHeight="13290"/>
   </bookViews>
   <sheets>
     <sheet name="Trace38" sheetId="37" r:id="rId1"/>
@@ -415,9 +415,9 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -449,7 +449,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -463,7 +463,7 @@
         <v>874688.89999999991</v>
       </c>
       <c r="E2">
-        <v>299999.99999979226</v>
+        <v>315218.56000000006</v>
       </c>
       <c r="F2">
         <v>89397</v>
@@ -484,7 +484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -498,7 +498,7 @@
         <v>848448.23300000001</v>
       </c>
       <c r="E3">
-        <v>299999.99999979226</v>
+        <v>377078.50320000004</v>
       </c>
       <c r="F3">
         <v>89397</v>
@@ -530,9 +530,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -564,7 +564,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -578,7 +578,7 @@
         <v>874688.89999999991</v>
       </c>
       <c r="E2">
-        <v>299999.99999979226</v>
+        <v>315218.56000000006</v>
       </c>
       <c r="F2">
         <v>89397</v>
@@ -599,7 +599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -613,7 +613,7 @@
         <v>751448.2329998049</v>
       </c>
       <c r="E3">
-        <v>299999.99999979226</v>
+        <v>377078.50320000004</v>
       </c>
       <c r="F3">
         <v>89397</v>
@@ -645,9 +645,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -679,7 +679,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -693,7 +693,7 @@
         <v>874688.89999999991</v>
       </c>
       <c r="E2">
-        <v>299999.99999979226</v>
+        <v>315218.56000000006</v>
       </c>
       <c r="F2">
         <v>89397</v>
@@ -714,7 +714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -728,7 +728,7 @@
         <v>1133448.2329998026</v>
       </c>
       <c r="E3">
-        <v>299999.99999979226</v>
+        <v>377078.50320000004</v>
       </c>
       <c r="F3">
         <v>89397</v>
@@ -760,9 +760,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -794,7 +794,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -808,7 +808,7 @@
         <v>874688.89999999991</v>
       </c>
       <c r="E2">
-        <v>299999.99999979226</v>
+        <v>315218.56000000006</v>
       </c>
       <c r="F2">
         <v>89397</v>
@@ -829,7 +829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -843,7 +843,7 @@
         <v>990948.2329999014</v>
       </c>
       <c r="E3">
-        <v>299999.99999979226</v>
+        <v>377078.50320000004</v>
       </c>
       <c r="F3">
         <v>89397</v>
@@ -852,13 +852,13 @@
         <v>1177845.3785449783</v>
       </c>
       <c r="H3">
-        <v>9347088.6732832119</v>
+        <v>9348251.9274542443</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3">
-        <v>9476256.4532832131</v>
+        <v>9477419.7074542455</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -875,9 +875,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -909,7 +909,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -923,7 +923,7 @@
         <v>874688.89999999991</v>
       </c>
       <c r="E2">
-        <v>299999.99999979226</v>
+        <v>315218.56000000006</v>
       </c>
       <c r="F2">
         <v>89397</v>
@@ -944,7 +944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -958,7 +958,7 @@
         <v>848448.23299999977</v>
       </c>
       <c r="E3">
-        <v>299999.99999979226</v>
+        <v>377078.50320000004</v>
       </c>
       <c r="F3">
         <v>89397</v>
@@ -990,9 +990,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1024,7 +1024,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -1038,7 +1038,7 @@
         <v>874688.89999999991</v>
       </c>
       <c r="E2">
-        <v>299999.99999979226</v>
+        <v>315218.56000000006</v>
       </c>
       <c r="F2">
         <v>89397</v>
@@ -1059,7 +1059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -1073,7 +1073,7 @@
         <v>990948.2329999014</v>
       </c>
       <c r="E3">
-        <v>299999.99999979226</v>
+        <v>377078.50320000004</v>
       </c>
       <c r="F3">
         <v>89397</v>
@@ -1105,9 +1105,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1139,7 +1139,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -1153,7 +1153,7 @@
         <v>874688.89999999991</v>
       </c>
       <c r="E2">
-        <v>299999.99999979226</v>
+        <v>315218.56000000006</v>
       </c>
       <c r="F2">
         <v>89397</v>
@@ -1174,7 +1174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -1188,7 +1188,7 @@
         <v>751448.23299980513</v>
       </c>
       <c r="E3">
-        <v>299999.99999979226</v>
+        <v>377078.50320000004</v>
       </c>
       <c r="F3">
         <v>89397</v>
@@ -1220,9 +1220,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1254,7 +1254,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -1268,7 +1268,7 @@
         <v>874688.89999999991</v>
       </c>
       <c r="E2">
-        <v>299999.99999979226</v>
+        <v>315218.56000000006</v>
       </c>
       <c r="F2">
         <v>89397</v>
@@ -1289,7 +1289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -1303,7 +1303,7 @@
         <v>751448.2329998049</v>
       </c>
       <c r="E3">
-        <v>299999.99999979226</v>
+        <v>377078.50320000004</v>
       </c>
       <c r="F3">
         <v>89397</v>
@@ -1335,9 +1335,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1369,7 +1369,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -1383,7 +1383,7 @@
         <v>874688.89999999991</v>
       </c>
       <c r="E2">
-        <v>299999.99999979226</v>
+        <v>315218.56000000006</v>
       </c>
       <c r="F2">
         <v>89397</v>
@@ -1404,7 +1404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -1418,7 +1418,7 @@
         <v>990948.2329999014</v>
       </c>
       <c r="E3">
-        <v>299999.99999979226</v>
+        <v>377078.50320000004</v>
       </c>
       <c r="F3">
         <v>89397</v>
@@ -1450,9 +1450,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1484,7 +1484,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -1498,7 +1498,7 @@
         <v>874688.89999999991</v>
       </c>
       <c r="E2">
-        <v>299999.99999979226</v>
+        <v>315218.56000000006</v>
       </c>
       <c r="F2">
         <v>89397</v>
@@ -1519,7 +1519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -1533,7 +1533,7 @@
         <v>1133448.2329998026</v>
       </c>
       <c r="E3">
-        <v>299999.99999979226</v>
+        <v>377078.50320000004</v>
       </c>
       <c r="F3">
         <v>89397</v>
@@ -1565,9 +1565,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1599,7 +1599,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -1613,7 +1613,7 @@
         <v>874688.89999999991</v>
       </c>
       <c r="E2">
-        <v>299999.99999979226</v>
+        <v>315218.56000000006</v>
       </c>
       <c r="F2">
         <v>89397</v>
@@ -1634,7 +1634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -1648,7 +1648,7 @@
         <v>1133448.2329998026</v>
       </c>
       <c r="E3">
-        <v>299999.99999979226</v>
+        <v>377078.50320000004</v>
       </c>
       <c r="F3">
         <v>89397</v>
@@ -1680,9 +1680,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1714,7 +1714,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -1728,7 +1728,7 @@
         <v>874688.89999999991</v>
       </c>
       <c r="E2">
-        <v>299999.99999979226</v>
+        <v>315218.56000000006</v>
       </c>
       <c r="F2">
         <v>89397</v>
@@ -1749,7 +1749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -1763,7 +1763,7 @@
         <v>569203.63171038928</v>
       </c>
       <c r="E3">
-        <v>299999.99999979226</v>
+        <v>377078.50320000004</v>
       </c>
       <c r="F3">
         <v>89397</v>
@@ -1795,9 +1795,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1829,7 +1829,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -1843,7 +1843,7 @@
         <v>874688.89999999991</v>
       </c>
       <c r="E2">
-        <v>299999.99999979226</v>
+        <v>315218.56000000006</v>
       </c>
       <c r="F2">
         <v>89397</v>
@@ -1864,7 +1864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -1878,7 +1878,7 @@
         <v>1133448.2329998026</v>
       </c>
       <c r="E3">
-        <v>299999.99999979226</v>
+        <v>377078.50320000004</v>
       </c>
       <c r="F3">
         <v>89397</v>
@@ -1887,13 +1887,13 @@
         <v>1320345.3785448796</v>
       </c>
       <c r="H3">
-        <v>11911747.235998331</v>
+        <v>11937964.933185101</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3">
-        <v>11973418.921998331</v>
+        <v>11999636.619185098</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -1910,9 +1910,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1944,7 +1944,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -1958,7 +1958,7 @@
         <v>874688.89999999991</v>
       </c>
       <c r="E2">
-        <v>299999.99999979226</v>
+        <v>315218.56000000006</v>
       </c>
       <c r="F2">
         <v>89397</v>
@@ -1979,7 +1979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -1993,7 +1993,7 @@
         <v>1133448.2329998026</v>
       </c>
       <c r="E3">
-        <v>299999.99999979226</v>
+        <v>377078.50320000004</v>
       </c>
       <c r="F3">
         <v>89397</v>
@@ -2002,13 +2002,13 @@
         <v>1320345.3785448796</v>
       </c>
       <c r="H3">
-        <v>10897893.102191133</v>
+        <v>10806309.720770467</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3">
-        <v>11026411.834191134</v>
+        <v>10934828.452770464</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -2025,9 +2025,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2059,7 +2059,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -2073,7 +2073,7 @@
         <v>874688.89999999991</v>
       </c>
       <c r="E2">
-        <v>299999.99999979226</v>
+        <v>315218.56000000006</v>
       </c>
       <c r="F2">
         <v>89397</v>
@@ -2094,7 +2094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -2108,7 +2108,7 @@
         <v>1133448.2329998026</v>
       </c>
       <c r="E3">
-        <v>299999.99999979226</v>
+        <v>377078.50320000004</v>
       </c>
       <c r="F3">
         <v>89397</v>
@@ -2117,13 +2117,13 @@
         <v>1320345.3785448796</v>
       </c>
       <c r="H3">
-        <v>11232587.143865276</v>
+        <v>11061200.617180195</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3">
-        <v>11515007.447865276</v>
+        <v>11343620.921180194</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -2140,9 +2140,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2174,7 +2174,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -2188,7 +2188,7 @@
         <v>874688.89999999991</v>
       </c>
       <c r="E2">
-        <v>299999.99999979226</v>
+        <v>315218.56000000006</v>
       </c>
       <c r="F2">
         <v>89397</v>
@@ -2209,7 +2209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -2223,7 +2223,7 @@
         <v>557448.23300020129</v>
       </c>
       <c r="E3">
-        <v>299999.99999979226</v>
+        <v>377078.50320000004</v>
       </c>
       <c r="F3">
         <v>89397</v>
@@ -2255,9 +2255,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2289,7 +2289,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -2303,7 +2303,7 @@
         <v>874688.89999999991</v>
       </c>
       <c r="E2">
-        <v>299999.99999979226</v>
+        <v>315218.56000000006</v>
       </c>
       <c r="F2">
         <v>89397</v>
@@ -2324,7 +2324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -2338,7 +2338,7 @@
         <v>990948.2329999014</v>
       </c>
       <c r="E3">
-        <v>299999.99999979226</v>
+        <v>377078.50320000004</v>
       </c>
       <c r="F3">
         <v>89397</v>
@@ -2347,13 +2347,13 @@
         <v>1177845.3785449783</v>
       </c>
       <c r="H3">
-        <v>12390814.127053976</v>
+        <v>12156576.581170088</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3">
-        <v>12800632.351053976</v>
+        <v>12566394.805170087</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -2370,9 +2370,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2404,7 +2404,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -2418,7 +2418,7 @@
         <v>874688.89999999991</v>
       </c>
       <c r="E2">
-        <v>299999.99999979226</v>
+        <v>315218.56000000006</v>
       </c>
       <c r="F2">
         <v>89397</v>
@@ -2439,7 +2439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -2453,7 +2453,7 @@
         <v>569203.63171038928</v>
       </c>
       <c r="E3">
-        <v>299999.99999979226</v>
+        <v>377078.50320000004</v>
       </c>
       <c r="F3">
         <v>89397</v>
@@ -2485,9 +2485,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2519,7 +2519,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -2533,7 +2533,7 @@
         <v>874688.89999999991</v>
       </c>
       <c r="E2">
-        <v>299999.99999979226</v>
+        <v>315218.56000000006</v>
       </c>
       <c r="F2">
         <v>89397</v>
@@ -2554,7 +2554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -2568,7 +2568,7 @@
         <v>569203.63171038928</v>
       </c>
       <c r="E3">
-        <v>299999.99999979226</v>
+        <v>377078.50320000004</v>
       </c>
       <c r="F3">
         <v>89397</v>
@@ -2600,9 +2600,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2634,7 +2634,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -2648,7 +2648,7 @@
         <v>874688.89999999991</v>
       </c>
       <c r="E2">
-        <v>299999.99999979226</v>
+        <v>315218.56000000006</v>
       </c>
       <c r="F2">
         <v>89397</v>
@@ -2669,7 +2669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -2683,7 +2683,7 @@
         <v>848448.23300000001</v>
       </c>
       <c r="E3">
-        <v>299999.99999979226</v>
+        <v>377078.50320000004</v>
       </c>
       <c r="F3">
         <v>89397</v>
@@ -2715,9 +2715,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2749,7 +2749,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -2763,7 +2763,7 @@
         <v>874688.89999999991</v>
       </c>
       <c r="E2">
-        <v>299999.99999979226</v>
+        <v>315218.56000000006</v>
       </c>
       <c r="F2">
         <v>89397</v>
@@ -2784,7 +2784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -2798,7 +2798,7 @@
         <v>751448.2329998049</v>
       </c>
       <c r="E3">
-        <v>299999.99999979226</v>
+        <v>377078.50320000004</v>
       </c>
       <c r="F3">
         <v>89397</v>
@@ -2830,9 +2830,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2864,7 +2864,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -2878,7 +2878,7 @@
         <v>874688.89999999991</v>
       </c>
       <c r="E2">
-        <v>299999.99999979226</v>
+        <v>315218.56000000006</v>
       </c>
       <c r="F2">
         <v>89397</v>
@@ -2899,7 +2899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -2913,7 +2913,7 @@
         <v>569203.63171038928</v>
       </c>
       <c r="E3">
-        <v>299999.99999979226</v>
+        <v>377078.50320000004</v>
       </c>
       <c r="F3">
         <v>89397</v>
@@ -2945,9 +2945,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2979,7 +2979,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -2993,7 +2993,7 @@
         <v>874688.89999999991</v>
       </c>
       <c r="E2">
-        <v>299999.99999979226</v>
+        <v>315218.56000000006</v>
       </c>
       <c r="F2">
         <v>89397</v>
@@ -3014,7 +3014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -3028,7 +3028,7 @@
         <v>569203.63171038928</v>
       </c>
       <c r="E3">
-        <v>299999.99999979226</v>
+        <v>377078.50320000004</v>
       </c>
       <c r="F3">
         <v>89397</v>
@@ -3060,9 +3060,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -3094,7 +3094,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -3108,7 +3108,7 @@
         <v>874688.89999999991</v>
       </c>
       <c r="E2">
-        <v>299999.99999979226</v>
+        <v>315218.56000000006</v>
       </c>
       <c r="F2">
         <v>89397</v>
@@ -3129,7 +3129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -3143,7 +3143,7 @@
         <v>751448.2329998049</v>
       </c>
       <c r="E3">
-        <v>299999.99999979226</v>
+        <v>377078.50320000004</v>
       </c>
       <c r="F3">
         <v>89397</v>
@@ -3175,9 +3175,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -3209,7 +3209,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -3223,7 +3223,7 @@
         <v>874688.89999999991</v>
       </c>
       <c r="E2">
-        <v>299999.99999979226</v>
+        <v>315218.56000000006</v>
       </c>
       <c r="F2">
         <v>89397</v>
@@ -3244,7 +3244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -3258,7 +3258,7 @@
         <v>1133448.2329998026</v>
       </c>
       <c r="E3">
-        <v>299999.99999979226</v>
+        <v>377078.50320000004</v>
       </c>
       <c r="F3">
         <v>89397</v>
@@ -3267,13 +3267,13 @@
         <v>1320345.3785448796</v>
       </c>
       <c r="H3">
-        <v>11966059.422844531</v>
+        <v>12006616.126452897</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3">
-        <v>12114092.050844532</v>
+        <v>12154648.754452901</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -3290,9 +3290,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -3324,7 +3324,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -3338,7 +3338,7 @@
         <v>874688.89999999991</v>
       </c>
       <c r="E2">
-        <v>299999.99999979226</v>
+        <v>315218.56000000006</v>
       </c>
       <c r="F2">
         <v>89397</v>
@@ -3359,7 +3359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -3373,7 +3373,7 @@
         <v>751448.2329998049</v>
       </c>
       <c r="E3">
-        <v>299999.99999979226</v>
+        <v>377078.50320000004</v>
       </c>
       <c r="F3">
         <v>89397</v>
@@ -3382,13 +3382,13 @@
         <v>938345.37854488206</v>
       </c>
       <c r="H3">
-        <v>10602350.610126313</v>
+        <v>10639120.274446048</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3">
-        <v>10827253.942126315</v>
+        <v>10864023.606446046</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -3405,9 +3405,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -3439,7 +3439,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -3453,7 +3453,7 @@
         <v>874688.89999999991</v>
       </c>
       <c r="E2">
-        <v>299999.99999979226</v>
+        <v>315218.56000000006</v>
       </c>
       <c r="F2">
         <v>89397</v>
@@ -3474,7 +3474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -3488,7 +3488,7 @@
         <v>1133448.2329998026</v>
       </c>
       <c r="E3">
-        <v>299999.99999979226</v>
+        <v>377078.50320000004</v>
       </c>
       <c r="F3">
         <v>89397</v>
@@ -3497,13 +3497,13 @@
         <v>1320345.3785448796</v>
       </c>
       <c r="H3">
-        <v>13920385.963511307</v>
+        <v>13901991.423403217</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3">
-        <v>14211693.165511308</v>
+        <v>14193298.625403218</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -3520,9 +3520,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -3554,7 +3554,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -3568,7 +3568,7 @@
         <v>874688.89999999991</v>
       </c>
       <c r="E2">
-        <v>299999.99999979226</v>
+        <v>315218.56000000006</v>
       </c>
       <c r="F2">
         <v>89397</v>
@@ -3589,7 +3589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -3603,7 +3603,7 @@
         <v>1133448.2329998026</v>
       </c>
       <c r="E3">
-        <v>299999.99999979226</v>
+        <v>377078.50320000004</v>
       </c>
       <c r="F3">
         <v>89397</v>
@@ -3612,13 +3612,13 @@
         <v>1320345.3785448796</v>
       </c>
       <c r="H3">
-        <v>12614602.096068762</v>
+        <v>12630518.852216702</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3">
-        <v>12888451.978068763</v>
+        <v>12904368.734216701</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -3635,9 +3635,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -3669,7 +3669,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -3683,7 +3683,7 @@
         <v>874688.89999999991</v>
       </c>
       <c r="E2">
-        <v>299999.99999979226</v>
+        <v>315218.56000000006</v>
       </c>
       <c r="F2">
         <v>89397</v>
@@ -3704,7 +3704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -3718,7 +3718,7 @@
         <v>1133448.2329998026</v>
       </c>
       <c r="E3">
-        <v>299999.99999979226</v>
+        <v>377078.50320000004</v>
       </c>
       <c r="F3">
         <v>89397</v>
@@ -3727,13 +3727,13 @@
         <v>1320345.3785448796</v>
       </c>
       <c r="H3">
-        <v>10282289.249708919</v>
+        <v>10283454.571929816</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3">
-        <v>10492893.595708918</v>
+        <v>10494058.917929813</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -3750,9 +3750,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -3784,7 +3784,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -3798,7 +3798,7 @@
         <v>874688.89999999991</v>
       </c>
       <c r="E2">
-        <v>299999.99999979226</v>
+        <v>315218.56000000006</v>
       </c>
       <c r="F2">
         <v>89397</v>
@@ -3819,7 +3819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -3833,7 +3833,7 @@
         <v>895948.23300000001</v>
       </c>
       <c r="E3">
-        <v>299999.99999979226</v>
+        <v>377078.50320000004</v>
       </c>
       <c r="F3">
         <v>89397</v>
@@ -3865,7 +3865,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3877,9 +3877,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -3911,7 +3911,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -3925,7 +3925,7 @@
         <v>874688.89999999991</v>
       </c>
       <c r="E2">
-        <v>299999.99999979226</v>
+        <v>315218.56000000006</v>
       </c>
       <c r="F2">
         <v>89397</v>
@@ -3946,7 +3946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -3960,7 +3960,7 @@
         <v>751448.2329998049</v>
       </c>
       <c r="E3">
-        <v>299999.99999979226</v>
+        <v>377078.50320000004</v>
       </c>
       <c r="F3">
         <v>89397</v>
@@ -3969,13 +3969,13 @@
         <v>938345.37854488206</v>
       </c>
       <c r="H3">
-        <v>8517552.9221072532</v>
+        <v>8539813.1611712184</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3">
-        <v>8549297.6521072537</v>
+        <v>8571557.891171217</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -3992,9 +3992,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -4026,7 +4026,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -4040,7 +4040,7 @@
         <v>874688.89999999991</v>
       </c>
       <c r="E2">
-        <v>299999.99999979226</v>
+        <v>315218.56000000006</v>
       </c>
       <c r="F2">
         <v>89397</v>
@@ -4061,7 +4061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -4075,7 +4075,7 @@
         <v>848448.23299999977</v>
       </c>
       <c r="E3">
-        <v>299999.99999979226</v>
+        <v>377078.50320000004</v>
       </c>
       <c r="F3">
         <v>89397</v>
@@ -4107,9 +4107,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -4141,7 +4141,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -4155,7 +4155,7 @@
         <v>874688.89999999991</v>
       </c>
       <c r="E2">
-        <v>299999.99999979226</v>
+        <v>315218.56000000006</v>
       </c>
       <c r="F2">
         <v>89397</v>
@@ -4176,7 +4176,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -4190,7 +4190,7 @@
         <v>1133448.2329998026</v>
       </c>
       <c r="E3">
-        <v>299999.99999979226</v>
+        <v>377078.50320000004</v>
       </c>
       <c r="F3">
         <v>89397</v>
@@ -4199,13 +4199,13 @@
         <v>1320345.3785448796</v>
       </c>
       <c r="H3">
-        <v>12537886.187006619</v>
+        <v>12592234.043675648</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3">
-        <v>12750581.197006619</v>
+        <v>12804929.053675646</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -4222,9 +4222,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -4256,7 +4256,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -4270,7 +4270,7 @@
         <v>874688.89999999991</v>
       </c>
       <c r="E2">
-        <v>299999.99999979226</v>
+        <v>315218.56000000006</v>
       </c>
       <c r="F2">
         <v>89397</v>
@@ -4291,7 +4291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -4305,7 +4305,7 @@
         <v>848448.23299999977</v>
       </c>
       <c r="E3">
-        <v>299999.99999979226</v>
+        <v>377078.50320000004</v>
       </c>
       <c r="F3">
         <v>89397</v>
@@ -4337,9 +4337,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -4371,7 +4371,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -4385,7 +4385,7 @@
         <v>874688.89999999991</v>
       </c>
       <c r="E2">
-        <v>299999.99999979226</v>
+        <v>315218.56000000006</v>
       </c>
       <c r="F2">
         <v>89397</v>
@@ -4406,7 +4406,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -4420,7 +4420,7 @@
         <v>751448.23299980513</v>
       </c>
       <c r="E3">
-        <v>299999.99999979226</v>
+        <v>377078.50320000004</v>
       </c>
       <c r="F3">
         <v>89397</v>
@@ -4452,9 +4452,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -4486,7 +4486,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43466</v>
       </c>
@@ -4500,7 +4500,7 @@
         <v>874688.89999999991</v>
       </c>
       <c r="E2">
-        <v>299999.99999979226</v>
+        <v>315218.56000000006</v>
       </c>
       <c r="F2">
         <v>89397</v>
@@ -4521,7 +4521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43831</v>
       </c>
@@ -4535,7 +4535,7 @@
         <v>569203.63171038928</v>
       </c>
       <c r="E3">
-        <v>299999.99999979226</v>
+        <v>377078.50320000004</v>
       </c>
       <c r="F3">
         <v>89397</v>

</xml_diff>

<commit_message>
Official June 2019 MTOM Model Run
Updated inflow forecasts

No change to model or ruleset since May release
</commit_message>
<xml_diff>
--- a/Output Data/MtomToCrss_Annual.xlsx
+++ b/Output Data/MtomToCrss_Annual.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\D_Drive\Modeling\MTOM-dev\Output Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\MTOM\Output Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22965" windowHeight="13290"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="9900"/>
   </bookViews>
   <sheets>
     <sheet name="Trace38" sheetId="37" r:id="rId1"/>
@@ -454,10 +454,10 @@
         <v>43466</v>
       </c>
       <c r="B2">
-        <v>47500.000000075197</v>
+        <v>47500</v>
       </c>
       <c r="C2">
-        <v>50000.0985</v>
+        <v>50000.049999999996</v>
       </c>
       <c r="D2">
         <v>874688.89999999991</v>
@@ -469,7 +469,7 @@
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>1061585.998500075</v>
+        <v>1061585.95</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -478,7 +478,7 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9202165.4710313734</v>
+        <v>9275337.19490139</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -489,10 +489,10 @@
         <v>43831</v>
       </c>
       <c r="B3">
-        <v>47500.000000075197</v>
+        <v>47500</v>
       </c>
       <c r="C3">
-        <v>50000.145545001898</v>
+        <v>50000.098500001899</v>
       </c>
       <c r="D3">
         <v>848448.23300000001</v>
@@ -504,7 +504,7 @@
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>1035345.3785450769</v>
+        <v>1035345.331500002</v>
       </c>
       <c r="H3">
         <v>8229999.9999991106</v>
@@ -569,10 +569,10 @@
         <v>43466</v>
       </c>
       <c r="B2">
-        <v>47500.000000075197</v>
+        <v>47500</v>
       </c>
       <c r="C2">
-        <v>50000.0985</v>
+        <v>50000.049999999996</v>
       </c>
       <c r="D2">
         <v>874688.89999999991</v>
@@ -584,7 +584,7 @@
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>1061585.998500075</v>
+        <v>1061585.95</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -593,7 +593,7 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9269230.0310313739</v>
+        <v>9337782.0049013887</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -604,10 +604,10 @@
         <v>43831</v>
       </c>
       <c r="B3">
-        <v>47500.000000075197</v>
+        <v>47500</v>
       </c>
       <c r="C3">
-        <v>50000.145545001898</v>
+        <v>50000.098500001899</v>
       </c>
       <c r="D3">
         <v>751448.2329998049</v>
@@ -619,7 +619,7 @@
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>938345.37854488206</v>
+        <v>938345.33149980684</v>
       </c>
       <c r="H3">
         <v>8999999.9999775533</v>
@@ -684,10 +684,10 @@
         <v>43466</v>
       </c>
       <c r="B2">
-        <v>47500.000000075197</v>
+        <v>47500</v>
       </c>
       <c r="C2">
-        <v>50000.0985</v>
+        <v>50000.049999999996</v>
       </c>
       <c r="D2">
         <v>874688.89999999991</v>
@@ -699,7 +699,7 @@
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>1061585.998500075</v>
+        <v>1061585.95</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -708,7 +708,7 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9214071.6110313721</v>
+        <v>9292471.1549013872</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -719,10 +719,10 @@
         <v>43831</v>
       </c>
       <c r="B3">
-        <v>47500.000000075197</v>
+        <v>47500</v>
       </c>
       <c r="C3">
-        <v>50000.145545001898</v>
+        <v>50000.098500001899</v>
       </c>
       <c r="D3">
         <v>1133448.2329998026</v>
@@ -734,7 +734,7 @@
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>1320345.3785448796</v>
+        <v>1320345.3314998045</v>
       </c>
       <c r="H3">
         <v>8229999.9999991106</v>
@@ -799,10 +799,10 @@
         <v>43466</v>
       </c>
       <c r="B2">
-        <v>47500.000000075197</v>
+        <v>47500</v>
       </c>
       <c r="C2">
-        <v>50000.0985</v>
+        <v>50000.049999999996</v>
       </c>
       <c r="D2">
         <v>874688.89999999991</v>
@@ -814,7 +814,7 @@
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>1061585.998500075</v>
+        <v>1061585.95</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -823,7 +823,7 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9171368.1710313726</v>
+        <v>9248351.6049013883</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -834,10 +834,10 @@
         <v>43831</v>
       </c>
       <c r="B3">
-        <v>47500.000000075197</v>
+        <v>47500</v>
       </c>
       <c r="C3">
-        <v>50000.145545001898</v>
+        <v>50000.098500001899</v>
       </c>
       <c r="D3">
         <v>990948.2329999014</v>
@@ -849,16 +849,16 @@
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>1177845.3785449783</v>
+        <v>1177845.3314999032</v>
       </c>
       <c r="H3">
-        <v>9348251.9274542443</v>
+        <v>10925516.667347979</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3">
-        <v>9477419.7074542455</v>
+        <v>11054684.44734798</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -914,10 +914,10 @@
         <v>43466</v>
       </c>
       <c r="B2">
-        <v>47500.000000075197</v>
+        <v>47500</v>
       </c>
       <c r="C2">
-        <v>50000.0985</v>
+        <v>50000.049999999996</v>
       </c>
       <c r="D2">
         <v>874688.89999999991</v>
@@ -929,7 +929,7 @@
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>1061585.998500075</v>
+        <v>1061585.95</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -938,7 +938,7 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9219705.0910313725</v>
+        <v>9292587.9649013877</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -949,10 +949,10 @@
         <v>43831</v>
       </c>
       <c r="B3">
-        <v>47500.000000075197</v>
+        <v>47500</v>
       </c>
       <c r="C3">
-        <v>50000.145545001898</v>
+        <v>50000.098500001899</v>
       </c>
       <c r="D3">
         <v>848448.23299999977</v>
@@ -964,7 +964,7 @@
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>1035345.3785450769</v>
+        <v>1035345.3315000017</v>
       </c>
       <c r="H3">
         <v>8999999.9999775533</v>
@@ -1029,10 +1029,10 @@
         <v>43466</v>
       </c>
       <c r="B2">
-        <v>47500.000000075197</v>
+        <v>47500</v>
       </c>
       <c r="C2">
-        <v>50000.0985</v>
+        <v>50000.049999999996</v>
       </c>
       <c r="D2">
         <v>874688.89999999991</v>
@@ -1044,7 +1044,7 @@
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>1061585.998500075</v>
+        <v>1061585.95</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -1053,7 +1053,7 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9210634.0810313728</v>
+        <v>9278310.4349013884</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -1064,10 +1064,10 @@
         <v>43831</v>
       </c>
       <c r="B3">
-        <v>47500.000000075197</v>
+        <v>47500</v>
       </c>
       <c r="C3">
-        <v>50000.145545001898</v>
+        <v>50000.098500001899</v>
       </c>
       <c r="D3">
         <v>990948.2329999014</v>
@@ -1079,7 +1079,7 @@
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>1177845.3785449783</v>
+        <v>1177845.3314999032</v>
       </c>
       <c r="H3">
         <v>8999999.9999775533</v>
@@ -1144,10 +1144,10 @@
         <v>43466</v>
       </c>
       <c r="B2">
-        <v>47500.000000075197</v>
+        <v>47500</v>
       </c>
       <c r="C2">
-        <v>50000.0985</v>
+        <v>50000.049999999996</v>
       </c>
       <c r="D2">
         <v>874688.89999999991</v>
@@ -1159,7 +1159,7 @@
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>1061585.998500075</v>
+        <v>1061585.95</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -1168,7 +1168,7 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9176487.9810313731</v>
+        <v>9247963.6349013895</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -1179,10 +1179,10 @@
         <v>43831</v>
       </c>
       <c r="B3">
-        <v>47500.000000075197</v>
+        <v>47500</v>
       </c>
       <c r="C3">
-        <v>50000.145545001898</v>
+        <v>50000.098500001899</v>
       </c>
       <c r="D3">
         <v>751448.23299980513</v>
@@ -1194,16 +1194,16 @@
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>938345.37854488229</v>
+        <v>938345.33149980707</v>
       </c>
       <c r="H3">
-        <v>8229999.9999991106</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3">
-        <v>8338713.64999911</v>
+        <v>9108713.6499775536</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -1259,10 +1259,10 @@
         <v>43466</v>
       </c>
       <c r="B2">
-        <v>47500.000000075197</v>
+        <v>47500</v>
       </c>
       <c r="C2">
-        <v>50000.0985</v>
+        <v>50000.049999999996</v>
       </c>
       <c r="D2">
         <v>874688.89999999991</v>
@@ -1274,7 +1274,7 @@
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>1061585.998500075</v>
+        <v>1061585.95</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -1283,7 +1283,7 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9238349.8910313733</v>
+        <v>9297580.0849013906</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -1294,10 +1294,10 @@
         <v>43831</v>
       </c>
       <c r="B3">
-        <v>47500.000000075197</v>
+        <v>47500</v>
       </c>
       <c r="C3">
-        <v>50000.145545001898</v>
+        <v>50000.098500001899</v>
       </c>
       <c r="D3">
         <v>751448.2329998049</v>
@@ -1309,7 +1309,7 @@
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>938345.37854488206</v>
+        <v>938345.33149980684</v>
       </c>
       <c r="H3">
         <v>8999999.9999775533</v>
@@ -1374,10 +1374,10 @@
         <v>43466</v>
       </c>
       <c r="B2">
-        <v>47500.000000075197</v>
+        <v>47500</v>
       </c>
       <c r="C2">
-        <v>50000.0985</v>
+        <v>50000.049999999996</v>
       </c>
       <c r="D2">
         <v>874688.89999999991</v>
@@ -1389,7 +1389,7 @@
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>1061585.998500075</v>
+        <v>1061585.95</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -1398,7 +1398,7 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9217958.3110313714</v>
+        <v>9290843.2449013889</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -1409,10 +1409,10 @@
         <v>43831</v>
       </c>
       <c r="B3">
-        <v>47500.000000075197</v>
+        <v>47500</v>
       </c>
       <c r="C3">
-        <v>50000.145545001898</v>
+        <v>50000.098500001899</v>
       </c>
       <c r="D3">
         <v>990948.2329999014</v>
@@ -1424,7 +1424,7 @@
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>1177845.3785449783</v>
+        <v>1177845.3314999032</v>
       </c>
       <c r="H3">
         <v>8229999.9999991106</v>
@@ -1489,10 +1489,10 @@
         <v>43466</v>
       </c>
       <c r="B2">
-        <v>47500.000000075197</v>
+        <v>47500</v>
       </c>
       <c r="C2">
-        <v>50000.0985</v>
+        <v>50000.049999999996</v>
       </c>
       <c r="D2">
         <v>874688.89999999991</v>
@@ -1504,7 +1504,7 @@
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>1061585.998500075</v>
+        <v>1061585.95</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -1513,7 +1513,7 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9124859.8110313714</v>
+        <v>9212088.0749013871</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -1524,10 +1524,10 @@
         <v>43831</v>
       </c>
       <c r="B3">
-        <v>47500.000000075197</v>
+        <v>47500</v>
       </c>
       <c r="C3">
-        <v>50000.145545001898</v>
+        <v>50000.098500001899</v>
       </c>
       <c r="D3">
         <v>1133448.2329998026</v>
@@ -1539,16 +1539,16 @@
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>1320345.3785448796</v>
+        <v>1320345.3314998045</v>
       </c>
       <c r="H3">
-        <v>8229999.9999991106</v>
+        <v>10462213.89303853</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3">
-        <v>8433484.9599991105</v>
+        <v>10665698.853038529</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -1604,10 +1604,10 @@
         <v>43466</v>
       </c>
       <c r="B2">
-        <v>47500.000000075197</v>
+        <v>47500</v>
       </c>
       <c r="C2">
-        <v>50000.0985</v>
+        <v>50000.049999999996</v>
       </c>
       <c r="D2">
         <v>874688.89999999991</v>
@@ -1619,7 +1619,7 @@
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>1061585.998500075</v>
+        <v>1061585.95</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -1628,7 +1628,7 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9160551.2410313729</v>
+        <v>9235057.4549013898</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -1639,10 +1639,10 @@
         <v>43831</v>
       </c>
       <c r="B3">
-        <v>47500.000000075197</v>
+        <v>47500</v>
       </c>
       <c r="C3">
-        <v>50000.145545001898</v>
+        <v>50000.098500001899</v>
       </c>
       <c r="D3">
         <v>1133448.2329998026</v>
@@ -1654,7 +1654,7 @@
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>1320345.3785448796</v>
+        <v>1320345.3314998045</v>
       </c>
       <c r="H3">
         <v>8229999.9999991106</v>
@@ -1719,10 +1719,10 @@
         <v>43466</v>
       </c>
       <c r="B2">
-        <v>47500.000000075197</v>
+        <v>47500</v>
       </c>
       <c r="C2">
-        <v>50000.0985</v>
+        <v>50000.049999999996</v>
       </c>
       <c r="D2">
         <v>874688.89999999991</v>
@@ -1734,7 +1734,7 @@
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>1061585.998500075</v>
+        <v>1061585.95</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -1743,7 +1743,7 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9199812.8910313714</v>
+        <v>9277396.2749013882</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -1754,10 +1754,10 @@
         <v>43831</v>
       </c>
       <c r="B3">
-        <v>47500.000000075197</v>
+        <v>47500</v>
       </c>
       <c r="C3">
-        <v>50000.145545001898</v>
+        <v>50000.098500001899</v>
       </c>
       <c r="D3">
         <v>569203.63171038928</v>
@@ -1769,7 +1769,7 @@
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>756100.77725546644</v>
+        <v>756100.73021039122</v>
       </c>
       <c r="H3">
         <v>8999999.9999775533</v>
@@ -1834,10 +1834,10 @@
         <v>43466</v>
       </c>
       <c r="B2">
-        <v>47500.000000075197</v>
+        <v>47500</v>
       </c>
       <c r="C2">
-        <v>50000.0985</v>
+        <v>50000.049999999996</v>
       </c>
       <c r="D2">
         <v>874688.89999999991</v>
@@ -1849,7 +1849,7 @@
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>1061585.998500075</v>
+        <v>1061585.95</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -1858,7 +1858,7 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9187004.7050313726</v>
+        <v>9264022.5189013891</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -1869,10 +1869,10 @@
         <v>43831</v>
       </c>
       <c r="B3">
-        <v>47500.000000075197</v>
+        <v>47500</v>
       </c>
       <c r="C3">
-        <v>50000.145545001898</v>
+        <v>50000.098500001899</v>
       </c>
       <c r="D3">
         <v>1133448.2329998026</v>
@@ -1884,16 +1884,16 @@
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>1320345.3785448796</v>
+        <v>1320345.3314998045</v>
       </c>
       <c r="H3">
-        <v>11937964.933185101</v>
+        <v>13460123.801266972</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3">
-        <v>11999636.619185098</v>
+        <v>13521795.487266971</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -1949,10 +1949,10 @@
         <v>43466</v>
       </c>
       <c r="B2">
-        <v>47500.000000075197</v>
+        <v>47500</v>
       </c>
       <c r="C2">
-        <v>50000.0985</v>
+        <v>50000.049999999996</v>
       </c>
       <c r="D2">
         <v>874688.89999999991</v>
@@ -1964,7 +1964,7 @@
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>1061585.998500075</v>
+        <v>1061585.95</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -1973,7 +1973,7 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9240120.4630313721</v>
+        <v>9293363.1729013901</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -1984,10 +1984,10 @@
         <v>43831</v>
       </c>
       <c r="B3">
-        <v>47500.000000075197</v>
+        <v>47500</v>
       </c>
       <c r="C3">
-        <v>50000.145545001898</v>
+        <v>50000.098500001899</v>
       </c>
       <c r="D3">
         <v>1133448.2329998026</v>
@@ -1999,16 +1999,16 @@
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>1320345.3785448796</v>
+        <v>1320345.3314998045</v>
       </c>
       <c r="H3">
-        <v>10806309.720770467</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3">
-        <v>10934828.452770464</v>
+        <v>8358518.7319991095</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -2064,10 +2064,10 @@
         <v>43466</v>
       </c>
       <c r="B2">
-        <v>47500.000000075197</v>
+        <v>47500</v>
       </c>
       <c r="C2">
-        <v>50000.0985</v>
+        <v>50000.049999999996</v>
       </c>
       <c r="D2">
         <v>874688.89999999991</v>
@@ -2079,7 +2079,7 @@
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>1061585.998500075</v>
+        <v>1061585.95</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -2088,7 +2088,7 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9180657.8090313729</v>
+        <v>9253654.346901387</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -2099,10 +2099,10 @@
         <v>43831</v>
       </c>
       <c r="B3">
-        <v>47500.000000075197</v>
+        <v>47500</v>
       </c>
       <c r="C3">
-        <v>50000.145545001898</v>
+        <v>50000.098500001899</v>
       </c>
       <c r="D3">
         <v>1133448.2329998026</v>
@@ -2114,16 +2114,16 @@
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>1320345.3785448796</v>
+        <v>1320345.3314998045</v>
       </c>
       <c r="H3">
-        <v>11061200.617180195</v>
+        <v>12714602.927197708</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3">
-        <v>11343620.921180194</v>
+        <v>12997023.231197709</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -2179,10 +2179,10 @@
         <v>43466</v>
       </c>
       <c r="B2">
-        <v>47500.000000075197</v>
+        <v>47500</v>
       </c>
       <c r="C2">
-        <v>50000.0985</v>
+        <v>50000.049999999996</v>
       </c>
       <c r="D2">
         <v>874688.89999999991</v>
@@ -2194,7 +2194,7 @@
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>1061585.998500075</v>
+        <v>1061585.95</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -2203,7 +2203,7 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9210596.5830313731</v>
+        <v>9262908.5909013879</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -2214,10 +2214,10 @@
         <v>43831</v>
       </c>
       <c r="B3">
-        <v>47500.000000075197</v>
+        <v>47500</v>
       </c>
       <c r="C3">
-        <v>50000.145545001898</v>
+        <v>50000.098500001899</v>
       </c>
       <c r="D3">
         <v>557448.23300020129</v>
@@ -2229,7 +2229,7 @@
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>744345.37854527857</v>
+        <v>744345.33150020323</v>
       </c>
       <c r="H3">
         <v>8999999.9999775533</v>
@@ -2294,10 +2294,10 @@
         <v>43466</v>
       </c>
       <c r="B2">
-        <v>47500.000000075197</v>
+        <v>47500</v>
       </c>
       <c r="C2">
-        <v>50000.0985</v>
+        <v>50000.049999999996</v>
       </c>
       <c r="D2">
         <v>874688.89999999991</v>
@@ -2309,7 +2309,7 @@
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>1061585.998500075</v>
+        <v>1061585.95</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -2318,7 +2318,7 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9227682.2070313711</v>
+        <v>9292563.0229013879</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -2329,10 +2329,10 @@
         <v>43831</v>
       </c>
       <c r="B3">
-        <v>47500.000000075197</v>
+        <v>47500</v>
       </c>
       <c r="C3">
-        <v>50000.145545001898</v>
+        <v>50000.098500001899</v>
       </c>
       <c r="D3">
         <v>990948.2329999014</v>
@@ -2344,16 +2344,16 @@
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>1177845.3785449783</v>
+        <v>1177845.3314999032</v>
       </c>
       <c r="H3">
-        <v>12156576.581170088</v>
+        <v>12565291.705921445</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3">
-        <v>12566394.805170087</v>
+        <v>12975109.929921445</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -2409,10 +2409,10 @@
         <v>43466</v>
       </c>
       <c r="B2">
-        <v>47500.000000075197</v>
+        <v>47500</v>
       </c>
       <c r="C2">
-        <v>50000.0985</v>
+        <v>50000.049999999996</v>
       </c>
       <c r="D2">
         <v>874688.89999999991</v>
@@ -2424,7 +2424,7 @@
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>1061585.998500075</v>
+        <v>1061585.95</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -2433,7 +2433,7 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9213742.3070313726</v>
+        <v>9286993.3809013888</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -2444,10 +2444,10 @@
         <v>43831</v>
       </c>
       <c r="B3">
-        <v>47500.000000075197</v>
+        <v>47500</v>
       </c>
       <c r="C3">
-        <v>50000.145545001898</v>
+        <v>50000.098500001899</v>
       </c>
       <c r="D3">
         <v>569203.63171038928</v>
@@ -2459,7 +2459,7 @@
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>756100.77725546644</v>
+        <v>756100.73021039122</v>
       </c>
       <c r="H3">
         <v>8229999.9999991106</v>
@@ -2524,10 +2524,10 @@
         <v>43466</v>
       </c>
       <c r="B2">
-        <v>47500.000000075197</v>
+        <v>47500</v>
       </c>
       <c r="C2">
-        <v>50000.0985</v>
+        <v>50000.049999999996</v>
       </c>
       <c r="D2">
         <v>874688.89999999991</v>
@@ -2539,7 +2539,7 @@
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>1061585.998500075</v>
+        <v>1061585.95</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -2548,7 +2548,7 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9206563.8590313718</v>
+        <v>9292062.1349013895</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -2559,10 +2559,10 @@
         <v>43831</v>
       </c>
       <c r="B3">
-        <v>47500.000000075197</v>
+        <v>47500</v>
       </c>
       <c r="C3">
-        <v>50000.145545001898</v>
+        <v>50000.098500001899</v>
       </c>
       <c r="D3">
         <v>569203.63171038928</v>
@@ -2574,7 +2574,7 @@
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>756100.77725546644</v>
+        <v>756100.73021039122</v>
       </c>
       <c r="H3">
         <v>8229999.9999991106</v>
@@ -2639,10 +2639,10 @@
         <v>43466</v>
       </c>
       <c r="B2">
-        <v>47500.000000075197</v>
+        <v>47500</v>
       </c>
       <c r="C2">
-        <v>50000.0985</v>
+        <v>50000.049999999996</v>
       </c>
       <c r="D2">
         <v>874688.89999999991</v>
@@ -2654,7 +2654,7 @@
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>1061585.998500075</v>
+        <v>1061585.95</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -2663,7 +2663,7 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9192975.9250313733</v>
+        <v>9281972.09290139</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -2674,10 +2674,10 @@
         <v>43831</v>
       </c>
       <c r="B3">
-        <v>47500.000000075197</v>
+        <v>47500</v>
       </c>
       <c r="C3">
-        <v>50000.145545001898</v>
+        <v>50000.098500001899</v>
       </c>
       <c r="D3">
         <v>848448.23300000001</v>
@@ -2689,7 +2689,7 @@
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>1035345.3785450769</v>
+        <v>1035345.331500002</v>
       </c>
       <c r="H3">
         <v>8229999.9999991106</v>
@@ -2754,10 +2754,10 @@
         <v>43466</v>
       </c>
       <c r="B2">
-        <v>47500.000000075197</v>
+        <v>47500</v>
       </c>
       <c r="C2">
-        <v>50000.0985</v>
+        <v>50000.049999999996</v>
       </c>
       <c r="D2">
         <v>874688.89999999991</v>
@@ -2769,7 +2769,7 @@
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>1061585.998500075</v>
+        <v>1061585.95</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -2778,7 +2778,7 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9196473.5150313731</v>
+        <v>9264101.7149013896</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -2789,10 +2789,10 @@
         <v>43831</v>
       </c>
       <c r="B3">
-        <v>47500.000000075197</v>
+        <v>47500</v>
       </c>
       <c r="C3">
-        <v>50000.145545001898</v>
+        <v>50000.098500001899</v>
       </c>
       <c r="D3">
         <v>751448.2329998049</v>
@@ -2804,7 +2804,7 @@
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>938345.37854488206</v>
+        <v>938345.33149980684</v>
       </c>
       <c r="H3">
         <v>8229999.9999991106</v>
@@ -2869,10 +2869,10 @@
         <v>43466</v>
       </c>
       <c r="B2">
-        <v>47500.000000075197</v>
+        <v>47500</v>
       </c>
       <c r="C2">
-        <v>50000.0985</v>
+        <v>50000.049999999996</v>
       </c>
       <c r="D2">
         <v>874688.89999999991</v>
@@ -2884,7 +2884,7 @@
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>1061585.998500075</v>
+        <v>1061585.95</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -2893,7 +2893,7 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9224638.2990313731</v>
+        <v>9296944.8629013896</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -2904,10 +2904,10 @@
         <v>43831</v>
       </c>
       <c r="B3">
-        <v>47500.000000075197</v>
+        <v>47500</v>
       </c>
       <c r="C3">
-        <v>50000.145545001898</v>
+        <v>50000.098500001899</v>
       </c>
       <c r="D3">
         <v>569203.63171038928</v>
@@ -2919,7 +2919,7 @@
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>756100.77725546644</v>
+        <v>756100.73021039122</v>
       </c>
       <c r="H3">
         <v>8229999.9999991106</v>
@@ -2984,10 +2984,10 @@
         <v>43466</v>
       </c>
       <c r="B2">
-        <v>47500.000000075197</v>
+        <v>47500</v>
       </c>
       <c r="C2">
-        <v>50000.0985</v>
+        <v>50000.049999999996</v>
       </c>
       <c r="D2">
         <v>874688.89999999991</v>
@@ -2999,7 +2999,7 @@
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>1061585.998500075</v>
+        <v>1061585.95</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -3008,7 +3008,7 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9181049.6010313723</v>
+        <v>9262386.8149013892</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -3019,10 +3019,10 @@
         <v>43831</v>
       </c>
       <c r="B3">
-        <v>47500.000000075197</v>
+        <v>47500</v>
       </c>
       <c r="C3">
-        <v>50000.145545001898</v>
+        <v>50000.098500001899</v>
       </c>
       <c r="D3">
         <v>569203.63171038928</v>
@@ -3034,7 +3034,7 @@
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>756100.77725546644</v>
+        <v>756100.73021039122</v>
       </c>
       <c r="H3">
         <v>8999999.9999775533</v>
@@ -3099,10 +3099,10 @@
         <v>43466</v>
       </c>
       <c r="B2">
-        <v>47500.000000075197</v>
+        <v>47500</v>
       </c>
       <c r="C2">
-        <v>50000.0985</v>
+        <v>50000.049999999996</v>
       </c>
       <c r="D2">
         <v>874688.89999999991</v>
@@ -3114,7 +3114,7 @@
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>1061585.998500075</v>
+        <v>1061585.95</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -3123,7 +3123,7 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9154328.281031372</v>
+        <v>9252473.3329013884</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -3134,10 +3134,10 @@
         <v>43831</v>
       </c>
       <c r="B3">
-        <v>47500.000000075197</v>
+        <v>47500</v>
       </c>
       <c r="C3">
-        <v>50000.145545001898</v>
+        <v>50000.098500001899</v>
       </c>
       <c r="D3">
         <v>751448.2329998049</v>
@@ -3149,16 +3149,16 @@
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>938345.37854488206</v>
+        <v>938345.33149980684</v>
       </c>
       <c r="H3">
-        <v>8999999.9999775533</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3">
-        <v>9187857.7959775534</v>
+        <v>8417857.7959991079</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -3214,10 +3214,10 @@
         <v>43466</v>
       </c>
       <c r="B2">
-        <v>47500.000000075197</v>
+        <v>47500</v>
       </c>
       <c r="C2">
-        <v>50000.0985</v>
+        <v>50000.049999999996</v>
       </c>
       <c r="D2">
         <v>874688.89999999991</v>
@@ -3229,7 +3229,7 @@
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>1061585.998500075</v>
+        <v>1061585.95</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -3238,7 +3238,7 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9185450.1030313727</v>
+        <v>9268290.4149013888</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -3249,10 +3249,10 @@
         <v>43831</v>
       </c>
       <c r="B3">
-        <v>47500.000000075197</v>
+        <v>47500</v>
       </c>
       <c r="C3">
-        <v>50000.145545001898</v>
+        <v>50000.098500001899</v>
       </c>
       <c r="D3">
         <v>1133448.2329998026</v>
@@ -3264,16 +3264,16 @@
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>1320345.3785448796</v>
+        <v>1320345.3314998045</v>
       </c>
       <c r="H3">
-        <v>12006616.126452897</v>
+        <v>12794246.357282687</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3">
-        <v>12154648.754452901</v>
+        <v>12942278.985282689</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -3329,10 +3329,10 @@
         <v>43466</v>
       </c>
       <c r="B2">
-        <v>47500.000000075197</v>
+        <v>47500</v>
       </c>
       <c r="C2">
-        <v>50000.0985</v>
+        <v>50000.049999999996</v>
       </c>
       <c r="D2">
         <v>874688.89999999991</v>
@@ -3344,7 +3344,7 @@
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>1061585.998500075</v>
+        <v>1061585.95</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -3353,7 +3353,7 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9268756.3110313714</v>
+        <v>9342402.6629013885</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -3364,10 +3364,10 @@
         <v>43831</v>
       </c>
       <c r="B3">
-        <v>47500.000000075197</v>
+        <v>47500</v>
       </c>
       <c r="C3">
-        <v>50000.145545001898</v>
+        <v>50000.098500001899</v>
       </c>
       <c r="D3">
         <v>751448.2329998049</v>
@@ -3379,16 +3379,16 @@
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>938345.37854488206</v>
+        <v>938345.33149980684</v>
       </c>
       <c r="H3">
-        <v>10639120.274446048</v>
+        <v>11921803.089697666</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3">
-        <v>10864023.606446046</v>
+        <v>12146706.421697667</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -3444,10 +3444,10 @@
         <v>43466</v>
       </c>
       <c r="B2">
-        <v>47500.000000075197</v>
+        <v>47500</v>
       </c>
       <c r="C2">
-        <v>50000.0985</v>
+        <v>50000.049999999996</v>
       </c>
       <c r="D2">
         <v>874688.89999999991</v>
@@ -3459,7 +3459,7 @@
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>1061585.998500075</v>
+        <v>1061585.95</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -3468,7 +3468,7 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9262570.127031371</v>
+        <v>9302422.898901388</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -3479,10 +3479,10 @@
         <v>43831</v>
       </c>
       <c r="B3">
-        <v>47500.000000075197</v>
+        <v>47500</v>
       </c>
       <c r="C3">
-        <v>50000.145545001898</v>
+        <v>50000.098500001899</v>
       </c>
       <c r="D3">
         <v>1133448.2329998026</v>
@@ -3494,16 +3494,16 @@
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>1320345.3785448796</v>
+        <v>1320345.3314998045</v>
       </c>
       <c r="H3">
-        <v>13901991.423403217</v>
+        <v>13046650.177576242</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3">
-        <v>14193298.625403218</v>
+        <v>13337957.379576243</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -3559,10 +3559,10 @@
         <v>43466</v>
       </c>
       <c r="B2">
-        <v>47500.000000075197</v>
+        <v>47500</v>
       </c>
       <c r="C2">
-        <v>50000.0985</v>
+        <v>50000.049999999996</v>
       </c>
       <c r="D2">
         <v>874688.89999999991</v>
@@ -3574,7 +3574,7 @@
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>1061585.998500075</v>
+        <v>1061585.95</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -3583,7 +3583,7 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9225949.5910313707</v>
+        <v>9287921.5889013875</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -3594,10 +3594,10 @@
         <v>43831</v>
       </c>
       <c r="B3">
-        <v>47500.000000075197</v>
+        <v>47500</v>
       </c>
       <c r="C3">
-        <v>50000.145545001898</v>
+        <v>50000.098500001899</v>
       </c>
       <c r="D3">
         <v>1133448.2329998026</v>
@@ -3609,16 +3609,16 @@
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>1320345.3785448796</v>
+        <v>1320345.3314998045</v>
       </c>
       <c r="H3">
-        <v>12630518.852216702</v>
+        <v>13037129.757488618</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3">
-        <v>12904368.734216701</v>
+        <v>13310979.639488619</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -3674,10 +3674,10 @@
         <v>43466</v>
       </c>
       <c r="B2">
-        <v>47500.000000075197</v>
+        <v>47500</v>
       </c>
       <c r="C2">
-        <v>50000.0985</v>
+        <v>50000.049999999996</v>
       </c>
       <c r="D2">
         <v>874688.89999999991</v>
@@ -3689,7 +3689,7 @@
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>1061585.998500075</v>
+        <v>1061585.95</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -3698,7 +3698,7 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9200901.2210313734</v>
+        <v>9273274.7689013872</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -3709,10 +3709,10 @@
         <v>43831</v>
       </c>
       <c r="B3">
-        <v>47500.000000075197</v>
+        <v>47500</v>
       </c>
       <c r="C3">
-        <v>50000.145545001898</v>
+        <v>50000.098500001899</v>
       </c>
       <c r="D3">
         <v>1133448.2329998026</v>
@@ -3724,16 +3724,16 @@
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>1320345.3785448796</v>
+        <v>1320345.3314998045</v>
       </c>
       <c r="H3">
-        <v>10283454.571929816</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3">
-        <v>10494058.917929813</v>
+        <v>8440604.3459991124</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -3789,10 +3789,10 @@
         <v>43466</v>
       </c>
       <c r="B2">
-        <v>47500.000000075197</v>
+        <v>47500</v>
       </c>
       <c r="C2">
-        <v>50000.0985</v>
+        <v>50000.049999999996</v>
       </c>
       <c r="D2">
         <v>874688.89999999991</v>
@@ -3804,7 +3804,7 @@
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>1061585.998500075</v>
+        <v>1061585.95</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -3813,7 +3813,7 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9209476.861031374</v>
+        <v>9281186.0049013887</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -3824,10 +3824,10 @@
         <v>43831</v>
       </c>
       <c r="B3">
-        <v>47500.000000075197</v>
+        <v>47500</v>
       </c>
       <c r="C3">
-        <v>50000.145545001898</v>
+        <v>50000.098500001899</v>
       </c>
       <c r="D3">
         <v>895948.23300000001</v>
@@ -3839,7 +3839,7 @@
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>1082845.3785450771</v>
+        <v>1082845.3315000017</v>
       </c>
       <c r="H3">
         <v>8999999.9999775533</v>
@@ -3916,10 +3916,10 @@
         <v>43466</v>
       </c>
       <c r="B2">
-        <v>47500.000000075197</v>
+        <v>47500</v>
       </c>
       <c r="C2">
-        <v>50000.0985</v>
+        <v>50000.049999999996</v>
       </c>
       <c r="D2">
         <v>874688.89999999991</v>
@@ -3931,7 +3931,7 @@
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>1061585.998500075</v>
+        <v>1061585.95</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -3940,7 +3940,7 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9160012.7710313722</v>
+        <v>9237608.7249013893</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -3951,10 +3951,10 @@
         <v>43831</v>
       </c>
       <c r="B3">
-        <v>47500.000000075197</v>
+        <v>47500</v>
       </c>
       <c r="C3">
-        <v>50000.145545001898</v>
+        <v>50000.098500001899</v>
       </c>
       <c r="D3">
         <v>751448.2329998049</v>
@@ -3966,16 +3966,16 @@
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>938345.37854488206</v>
+        <v>938345.33149980684</v>
       </c>
       <c r="H3">
-        <v>8539813.1611712184</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3">
-        <v>8571557.891171217</v>
+        <v>9031744.7299775537</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -4031,10 +4031,10 @@
         <v>43466</v>
       </c>
       <c r="B2">
-        <v>47500.000000075197</v>
+        <v>47500</v>
       </c>
       <c r="C2">
-        <v>50000.0985</v>
+        <v>50000.049999999996</v>
       </c>
       <c r="D2">
         <v>874688.89999999991</v>
@@ -4046,7 +4046,7 @@
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>1061585.998500075</v>
+        <v>1061585.95</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -4055,7 +4055,7 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9247417.0410313737</v>
+        <v>9310462.284901388</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -4066,10 +4066,10 @@
         <v>43831</v>
       </c>
       <c r="B3">
-        <v>47500.000000075197</v>
+        <v>47500</v>
       </c>
       <c r="C3">
-        <v>50000.145545001898</v>
+        <v>50000.098500001899</v>
       </c>
       <c r="D3">
         <v>848448.23299999977</v>
@@ -4081,7 +4081,7 @@
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>1035345.3785450769</v>
+        <v>1035345.3315000017</v>
       </c>
       <c r="H3">
         <v>8999999.9999775533</v>
@@ -4146,10 +4146,10 @@
         <v>43466</v>
       </c>
       <c r="B2">
-        <v>47500.000000075197</v>
+        <v>47500</v>
       </c>
       <c r="C2">
-        <v>50000.0985</v>
+        <v>50000.049999999996</v>
       </c>
       <c r="D2">
         <v>874688.89999999991</v>
@@ -4161,7 +4161,7 @@
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>1061585.998500075</v>
+        <v>1061585.95</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -4170,7 +4170,7 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9213817.8610313721</v>
+        <v>9285846.5549013875</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -4181,10 +4181,10 @@
         <v>43831</v>
       </c>
       <c r="B3">
-        <v>47500.000000075197</v>
+        <v>47500</v>
       </c>
       <c r="C3">
-        <v>50000.145545001898</v>
+        <v>50000.098500001899</v>
       </c>
       <c r="D3">
         <v>1133448.2329998026</v>
@@ -4196,16 +4196,16 @@
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>1320345.3785448796</v>
+        <v>1320345.3314998045</v>
       </c>
       <c r="H3">
-        <v>12592234.043675648</v>
+        <v>13392255.5075387</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3">
-        <v>12804929.053675646</v>
+        <v>13604950.517538698</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -4261,10 +4261,10 @@
         <v>43466</v>
       </c>
       <c r="B2">
-        <v>47500.000000075197</v>
+        <v>47500</v>
       </c>
       <c r="C2">
-        <v>50000.0985</v>
+        <v>50000.049999999996</v>
       </c>
       <c r="D2">
         <v>874688.89999999991</v>
@@ -4276,7 +4276,7 @@
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>1061585.998500075</v>
+        <v>1061585.95</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -4285,7 +4285,7 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9215021.3610313721</v>
+        <v>9293634.5249013882</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -4296,10 +4296,10 @@
         <v>43831</v>
       </c>
       <c r="B3">
-        <v>47500.000000075197</v>
+        <v>47500</v>
       </c>
       <c r="C3">
-        <v>50000.145545001898</v>
+        <v>50000.098500001899</v>
       </c>
       <c r="D3">
         <v>848448.23299999977</v>
@@ -4311,7 +4311,7 @@
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>1035345.3785450769</v>
+        <v>1035345.3315000017</v>
       </c>
       <c r="H3">
         <v>8999999.9999775533</v>
@@ -4376,10 +4376,10 @@
         <v>43466</v>
       </c>
       <c r="B2">
-        <v>47500.000000075197</v>
+        <v>47500</v>
       </c>
       <c r="C2">
-        <v>50000.0985</v>
+        <v>50000.049999999996</v>
       </c>
       <c r="D2">
         <v>874688.89999999991</v>
@@ -4391,7 +4391,7 @@
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>1061585.998500075</v>
+        <v>1061585.95</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -4400,7 +4400,7 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9234303.781031372</v>
+        <v>9299988.9349013884</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -4411,10 +4411,10 @@
         <v>43831</v>
       </c>
       <c r="B3">
-        <v>47500.000000075197</v>
+        <v>47500</v>
       </c>
       <c r="C3">
-        <v>50000.145545001898</v>
+        <v>50000.098500001899</v>
       </c>
       <c r="D3">
         <v>751448.23299980513</v>
@@ -4426,7 +4426,7 @@
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>938345.37854488229</v>
+        <v>938345.33149980707</v>
       </c>
       <c r="H3">
         <v>8999999.9999775533</v>
@@ -4491,10 +4491,10 @@
         <v>43466</v>
       </c>
       <c r="B2">
-        <v>47500.000000075197</v>
+        <v>47500</v>
       </c>
       <c r="C2">
-        <v>50000.0985</v>
+        <v>50000.049999999996</v>
       </c>
       <c r="D2">
         <v>874688.89999999991</v>
@@ -4506,7 +4506,7 @@
         <v>89397</v>
       </c>
       <c r="G2">
-        <v>1061585.998500075</v>
+        <v>1061585.95</v>
       </c>
       <c r="H2">
         <v>8999999.9999775533</v>
@@ -4515,7 +4515,7 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>9194470.0210313722</v>
+        <v>9272014.3749013878</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -4526,10 +4526,10 @@
         <v>43831</v>
       </c>
       <c r="B3">
-        <v>47500.000000075197</v>
+        <v>47500</v>
       </c>
       <c r="C3">
-        <v>50000.145545001898</v>
+        <v>50000.098500001899</v>
       </c>
       <c r="D3">
         <v>569203.63171038928</v>
@@ -4541,16 +4541,16 @@
         <v>89397</v>
       </c>
       <c r="G3">
-        <v>756100.77725546644</v>
+        <v>756100.73021039122</v>
       </c>
       <c r="H3">
-        <v>8999999.9999775533</v>
+        <v>11301875.684094502</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3">
-        <v>9186027.3499775529</v>
+        <v>11487903.034094499</v>
       </c>
       <c r="K3">
         <v>0</v>

</xml_diff>

<commit_message>
MTOM_V3.0.202001: MTOM model file updated with Conor's flaming gorge changes and notes for slots
EnsembleOutput, MTOM_EnsembleOutput, MtomToCrss_Annual, MtomToCrss_Monthly: Files updated to reflect conors change to FG logic. NO change to current year results. Outyears affected
</commit_message>
<xml_diff>
--- a/Output Data/MtomToCrss_Annual.xlsx
+++ b/Output Data/MtomToCrss_Annual.xlsx
@@ -2958,13 +2958,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>13740081.942341445</v>
+        <v>13712432.070248161</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>13801753.628341442</v>
+        <v>13774103.756248161</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -6174,13 +6174,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>12399531.458360245</v>
+        <v>11750117.627780363</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>12612226.468360247</v>
+        <v>11962812.637780361</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -7581,13 +7581,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>13347858.941506747</v>
+        <v>12703858.994271697</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>13621708.823506748</v>
+        <v>12977708.876271699</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -8184,13 +8184,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>12412898.071815122</v>
+        <v>12005874.347986775</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>12560930.699815122</v>
+        <v>12153906.975986775</v>
       </c>
       <c r="U3">
         <v>0</v>

</xml_diff>

<commit_message>
February 2020 Official Run for CRSS
MTOM Ruleset updated so MWD diversion adjustment happens in Jan, Feb, Mar of year 1.
Updated Ensemble inflow forecasts for Feb run
Updated Output spreadsheets
Updated ruleset and model file names to reflect changes/new run
</commit_message>
<xml_diff>
--- a/Output Data/MtomToCrss_Annual.xlsx
+++ b/Output Data/MtomToCrss_Annual.xlsx
@@ -6,51 +6,49 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Trace1" sheetId="1" r:id="rId2"/>
-    <sheet name="Trace2" sheetId="2" r:id="rId4"/>
-    <sheet name="Trace3" sheetId="3" r:id="rId5"/>
-    <sheet name="Trace4" sheetId="4" r:id="rId6"/>
-    <sheet name="Trace5" sheetId="5" r:id="rId7"/>
-    <sheet name="Trace6" sheetId="6" r:id="rId8"/>
-    <sheet name="Trace7" sheetId="7" r:id="rId9"/>
-    <sheet name="Trace8" sheetId="8" r:id="rId10"/>
-    <sheet name="Trace9" sheetId="9" r:id="rId11"/>
-    <sheet name="Trace10" sheetId="10" r:id="rId12"/>
-    <sheet name="Trace11" sheetId="11" r:id="rId13"/>
-    <sheet name="Trace12" sheetId="12" r:id="rId14"/>
-    <sheet name="Trace13" sheetId="13" r:id="rId15"/>
-    <sheet name="Trace14" sheetId="14" r:id="rId16"/>
-    <sheet name="Trace15" sheetId="15" r:id="rId17"/>
-    <sheet name="Trace16" sheetId="16" r:id="rId18"/>
-    <sheet name="Trace17" sheetId="17" r:id="rId19"/>
-    <sheet name="Trace18" sheetId="18" r:id="rId20"/>
-    <sheet name="Trace19" sheetId="19" r:id="rId21"/>
-    <sheet name="Trace20" sheetId="20" r:id="rId22"/>
-    <sheet name="Trace21" sheetId="21" r:id="rId23"/>
-    <sheet name="Trace22" sheetId="22" r:id="rId24"/>
-    <sheet name="Trace23" sheetId="23" r:id="rId25"/>
-    <sheet name="Trace24" sheetId="24" r:id="rId26"/>
-    <sheet name="Trace25" sheetId="25" r:id="rId27"/>
-    <sheet name="Trace26" sheetId="26" r:id="rId28"/>
-    <sheet name="Trace27" sheetId="27" r:id="rId29"/>
-    <sheet name="Trace28" sheetId="28" r:id="rId30"/>
-    <sheet name="Trace29" sheetId="29" r:id="rId31"/>
-    <sheet name="Trace30" sheetId="30" r:id="rId32"/>
-    <sheet name="Trace31" sheetId="31" r:id="rId33"/>
-    <sheet name="Trace32" sheetId="32" r:id="rId34"/>
-    <sheet name="Trace33" sheetId="33" r:id="rId35"/>
-    <sheet name="Trace34" sheetId="34" r:id="rId36"/>
-    <sheet name="Trace35" sheetId="35" r:id="rId37"/>
-    <sheet name="Trace36" sheetId="36" r:id="rId38"/>
-    <sheet name="Trace37" sheetId="37" r:id="rId39"/>
-    <sheet name="Trace38" sheetId="38" r:id="rId40"/>
+    <sheet name="Trace3" sheetId="1" r:id="rId2"/>
+    <sheet name="Trace4" sheetId="2" r:id="rId4"/>
+    <sheet name="Trace5" sheetId="3" r:id="rId5"/>
+    <sheet name="Trace6" sheetId="4" r:id="rId6"/>
+    <sheet name="Trace7" sheetId="5" r:id="rId7"/>
+    <sheet name="Trace8" sheetId="6" r:id="rId8"/>
+    <sheet name="Trace9" sheetId="7" r:id="rId9"/>
+    <sheet name="Trace10" sheetId="8" r:id="rId10"/>
+    <sheet name="Trace11" sheetId="9" r:id="rId11"/>
+    <sheet name="Trace12" sheetId="10" r:id="rId12"/>
+    <sheet name="Trace13" sheetId="11" r:id="rId13"/>
+    <sheet name="Trace14" sheetId="12" r:id="rId14"/>
+    <sheet name="Trace15" sheetId="13" r:id="rId15"/>
+    <sheet name="Trace16" sheetId="14" r:id="rId16"/>
+    <sheet name="Trace17" sheetId="15" r:id="rId17"/>
+    <sheet name="Trace18" sheetId="16" r:id="rId18"/>
+    <sheet name="Trace19" sheetId="17" r:id="rId19"/>
+    <sheet name="Trace20" sheetId="18" r:id="rId20"/>
+    <sheet name="Trace21" sheetId="19" r:id="rId21"/>
+    <sheet name="Trace22" sheetId="20" r:id="rId22"/>
+    <sheet name="Trace23" sheetId="21" r:id="rId23"/>
+    <sheet name="Trace24" sheetId="22" r:id="rId24"/>
+    <sheet name="Trace25" sheetId="23" r:id="rId25"/>
+    <sheet name="Trace26" sheetId="24" r:id="rId26"/>
+    <sheet name="Trace27" sheetId="25" r:id="rId27"/>
+    <sheet name="Trace28" sheetId="26" r:id="rId28"/>
+    <sheet name="Trace29" sheetId="27" r:id="rId29"/>
+    <sheet name="Trace30" sheetId="28" r:id="rId30"/>
+    <sheet name="Trace31" sheetId="29" r:id="rId31"/>
+    <sheet name="Trace32" sheetId="30" r:id="rId32"/>
+    <sheet name="Trace33" sheetId="31" r:id="rId33"/>
+    <sheet name="Trace34" sheetId="32" r:id="rId34"/>
+    <sheet name="Trace35" sheetId="33" r:id="rId35"/>
+    <sheet name="Trace36" sheetId="34" r:id="rId36"/>
+    <sheet name="Trace37" sheetId="35" r:id="rId37"/>
+    <sheet name="Trace38" sheetId="36" r:id="rId38"/>
   </sheets>
   <calcPr calcId="125725" fullCalcOnLoad="true"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:xdr="http://purl.oclc.org/ooxml/drawingml/spreadsheetDrawing" count="760" uniqueCount="20">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:xdr="http://purl.oclc.org/ooxml/drawingml/spreadsheetDrawing" count="720" uniqueCount="20">
   <si>
     <t>DCP BWSCP Flags.LB DCP BWSP</t>
   </si>
@@ -134,7 +132,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="267">
+  <borders count="505">
     <border>
       <start/>
       <end/>
@@ -408,11 +406,249 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="267">
+  <cellXfs count="505">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -756,6 +992,312 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="266" xfId="0" applyNumberFormat="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="267" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="268" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="269" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="270" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="271" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="272" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="273" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="274" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="275" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="276" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="277" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="278" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="279" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="280" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="281" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="282" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="283" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="284" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="285" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="286" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="287" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="288" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="289" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="290" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="291" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="292" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="293" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="294" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="295" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="296" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="297" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="298" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="299" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="300" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="301" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="302" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="303" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="304" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="305" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="306" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="307" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="308" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="309" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="310" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="311" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="312" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="313" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="314" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="315" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="316" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="317" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="318" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="319" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="320" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="321" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="322" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="323" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="324" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="325" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="326" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="327" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="328" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="329" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="330" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="331" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="332" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="333" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="334" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="335" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="336" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="337" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="338" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="339" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="340" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="341" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="342" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="343" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="344" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="345" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="346" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="347" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="348" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="349" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="350" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="351" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="352" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="353" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="354" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="355" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="356" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="357" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="358" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="359" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="360" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="361" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="362" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="363" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="364" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="365" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="366" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="367" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="368" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="369" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="370" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="371" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="372" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="373" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="374" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="375" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="376" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="377" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="378" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="379" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="380" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="381" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="382" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="383" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="384" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="385" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="386" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="387" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="388" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="389" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="390" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="391" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="392" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="393" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="394" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="395" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="396" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="397" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="398" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="399" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="400" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="401" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="402" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="403" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="404" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="405" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="406" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="407" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="408" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="409" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="410" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="411" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="412" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="413" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="414" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="415" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="416" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="417" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="418" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="419" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="420" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="421" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="422" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="423" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="424" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="425" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="426" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="427" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="428" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="429" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="430" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="431" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="432" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="433" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="434" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="435" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="436" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="437" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="438" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="439" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="440" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="441" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="442" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="443" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="444" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="445" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="446" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="447" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="448" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="449" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="450" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="451" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="452" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="453" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="454" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="455" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="456" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="457" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="458" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="459" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="460" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="461" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="462" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="463" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="464" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="465" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="466" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="467" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="468" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="469" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="470" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="471" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="472" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="473" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="474" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="475" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="476" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="477" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="478" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="479" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="480" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="481" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="482" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="483" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="484" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="485" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="486" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="487" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="488" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="489" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="490" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="491" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="492" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="493" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="494" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="495" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="496" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="497" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="498" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="499" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="500" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="501" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="502" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="503" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="504" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -856,7 +1398,7 @@
         <v>480594.69699999999</v>
       </c>
       <c r="I2">
-        <v>1095844.5999999999</v>
+        <v>1097690.5</v>
       </c>
       <c r="J2">
         <v>285431.99699999997</v>
@@ -874,7 +1416,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1045844.6</v>
+        <v>1047690.5</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -883,13 +1425,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8358843.7387190023</v>
+        <v>8388617.0990332533</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -903,13 +1445,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>29999.999699999997</v>
+        <v>24300</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>29999.999699999997</v>
+        <v>24300</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -921,7 +1463,7 @@
         <v>483294.69699999993</v>
       </c>
       <c r="I3">
-        <v>1259360.2</v>
+        <v>1261206.0999999999</v>
       </c>
       <c r="J3">
         <v>285431.99699999997</v>
@@ -939,7 +1481,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1209360.2</v>
+        <v>1211206.0999999999</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -948,13 +1490,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8803567.5082156733</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>8938070.5082156751</v>
+        <v>9137627.9999775533</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -1084,13 +1626,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8409636.2467190046</v>
+        <v>8373008.8290332509</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -1104,13 +1646,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>29999.999699999997</v>
+        <v>24300</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>29999.999699999997</v>
+        <v>24300</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -1122,7 +1664,7 @@
         <v>483294.69699999993</v>
       </c>
       <c r="I3">
-        <v>513861.00000000675</v>
+        <v>813860.99999979988</v>
       </c>
       <c r="J3">
         <v>285431.99699999997</v>
@@ -1140,7 +1682,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>463861.00000000675</v>
+        <v>763860.99999979977</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -1149,13 +1691,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8229999.9999991106</v>
+        <v>8714241.2454313841</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>8417833.5499991123</v>
+        <v>8850734.6714313831</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -1285,13 +1827,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8397003.0547190029</v>
+        <v>8369752.0770332525</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -1305,13 +1847,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>29999.999699999997</v>
+        <v>24300</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>29999.999699999997</v>
+        <v>24300</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -1323,7 +1865,7 @@
         <v>483294.69699999993</v>
       </c>
       <c r="I3">
-        <v>513861.00000000687</v>
+        <v>313861.00000041554</v>
       </c>
       <c r="J3">
         <v>285431.99699999997</v>
@@ -1341,7 +1883,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>463861.00000000681</v>
+        <v>263861.00000041554</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -1350,13 +1892,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8229999.9999991106</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>8380597.6699991105</v>
+        <v>9174589.2299775518</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -1459,7 +2001,7 @@
         <v>480594.69699999999</v>
       </c>
       <c r="I2">
-        <v>813860.99999979907</v>
+        <v>613861.0000002078</v>
       </c>
       <c r="J2">
         <v>285431.99699999997</v>
@@ -1477,7 +2019,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>763860.99999979907</v>
+        <v>563861.0000002078</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -1486,13 +2028,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8375492.4787190035</v>
+        <v>8420218.8750332519</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -1506,13 +2048,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>29999.999699999997</v>
+        <v>24300</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>29999.999699999997</v>
+        <v>24300</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -1524,7 +2066,7 @@
         <v>483294.69699999993</v>
       </c>
       <c r="I3">
-        <v>813860.99999979942</v>
+        <v>313861.00000041554</v>
       </c>
       <c r="J3">
         <v>285431.99699999997</v>
@@ -1542,7 +2084,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>763860.99999979942</v>
+        <v>263861.00000041554</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -1557,7 +2099,7 @@
         <v>1</v>
       </c>
       <c r="T3">
-        <v>8366493.4259991096</v>
+        <v>8469478.9159991127</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -1660,7 +2202,7 @@
         <v>480594.69699999999</v>
       </c>
       <c r="I2">
-        <v>906235.80000430183</v>
+        <v>613861.0000002078</v>
       </c>
       <c r="J2">
         <v>285431.99699999997</v>
@@ -1678,7 +2220,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>856235.80000430183</v>
+        <v>563861.0000002078</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -1687,13 +2229,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8372260.720719004</v>
+        <v>8466740.6050332543</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -1707,13 +2249,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>29999.999699999997</v>
+        <v>24300</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>29999.999699999997</v>
+        <v>24300</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -1725,7 +2267,7 @@
         <v>483294.69699999993</v>
       </c>
       <c r="I3">
-        <v>606235.80000450963</v>
+        <v>763861.00000010396</v>
       </c>
       <c r="J3">
         <v>285431.99699999997</v>
@@ -1743,7 +2285,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>556235.80000450963</v>
+        <v>713861.00000010396</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -1752,13 +2294,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8999999.9999775533</v>
+        <v>9428522.0439325348</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>9174589.2299775518</v>
+        <v>9838340.2679325324</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -1861,7 +2403,7 @@
         <v>480594.69699999999</v>
       </c>
       <c r="I2">
-        <v>613861.0000002078</v>
+        <v>1048860.9999999066</v>
       </c>
       <c r="J2">
         <v>285431.99699999997</v>
@@ -1879,7 +2421,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>563861.0000002078</v>
+        <v>998860.99999990652</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -1888,13 +2430,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8421841.4287190046</v>
+        <v>8535845.9710332509</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -1905,28 +2447,28 @@
         <v>44197</v>
       </c>
       <c r="B3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3">
-        <v>29999.999699999997</v>
+        <v>0</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>29999.999699999997</v>
+        <v>0</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>7999.9999999998645</v>
+        <v>0</v>
       </c>
       <c r="H3">
         <v>483294.69699999993</v>
       </c>
       <c r="I3">
-        <v>313861.00000041554</v>
+        <v>748861.00000011432</v>
       </c>
       <c r="J3">
         <v>285431.99699999997</v>
@@ -1944,10 +2486,10 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>263861.00000041554</v>
+        <v>698861.00000011432</v>
       </c>
       <c r="P3">
-        <v>469427.99999962631</v>
+        <v>477427.99999962613</v>
       </c>
       <c r="Q3">
         <v>0</v>
@@ -1959,7 +2501,7 @@
         <v>1</v>
       </c>
       <c r="T3">
-        <v>8469478.9159991127</v>
+        <v>8362878.8059991114</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -2089,13 +2631,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8470374.482719006</v>
+        <v>8362630.2730332529</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -2106,28 +2648,28 @@
         <v>44197</v>
       </c>
       <c r="B3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>24300</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>24300</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>7999.9999999998645</v>
       </c>
       <c r="H3">
         <v>483294.69699999993</v>
       </c>
       <c r="I3">
-        <v>763861.00000010396</v>
+        <v>913861</v>
       </c>
       <c r="J3">
         <v>285431.99699999997</v>
@@ -2145,22 +2687,22 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>713861.00000010396</v>
+        <v>863861</v>
       </c>
       <c r="P3">
-        <v>488482.60999962612</v>
+        <v>469427.99999962631</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>9064960.2924137004</v>
+        <v>10837705.370753584</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>9474778.5164136998</v>
+        <v>11120125.674753584</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -2263,7 +2805,7 @@
         <v>480594.69699999999</v>
       </c>
       <c r="I2">
-        <v>1048860.9999999066</v>
+        <v>1183860.999999813</v>
       </c>
       <c r="J2">
         <v>285431.99699999997</v>
@@ -2281,7 +2823,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>998860.99999990652</v>
+        <v>1133860.999999813</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -2290,13 +2832,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>9504058.8189741056</v>
+        <v>9799204.6629683357</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>9896440.5136931129</v>
+        <v>10061978.228001589</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -2328,7 +2870,7 @@
         <v>483294.69699999993</v>
       </c>
       <c r="I3">
-        <v>748861.00000011432</v>
+        <v>1453860.9999996261</v>
       </c>
       <c r="J3">
         <v>285431.99699999997</v>
@@ -2346,22 +2888,22 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>698861.00000011432</v>
+        <v>1403860.9999996261</v>
       </c>
       <c r="P3">
-        <v>477427.99999962613</v>
+        <v>466373.38999962609</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>9180669.6271031033</v>
+        <v>11955559.365453757</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>9313548.4331031032</v>
+        <v>12084078.097453758</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -2464,7 +3006,7 @@
         <v>480594.69699999999</v>
       </c>
       <c r="I2">
-        <v>613861.0000002078</v>
+        <v>1183860.999999813</v>
       </c>
       <c r="J2">
         <v>285431.99699999997</v>
@@ -2482,7 +3024,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>563861.0000002078</v>
+        <v>1133860.999999813</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -2491,13 +3033,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8362031.5187190045</v>
+        <v>8352671.9550332529</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -2511,13 +3053,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>29999.999699999997</v>
+        <v>24300</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>29999.999699999997</v>
+        <v>24300</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -2529,7 +3071,7 @@
         <v>483294.69699999993</v>
       </c>
       <c r="I3">
-        <v>913861</v>
+        <v>1453860.9999996261</v>
       </c>
       <c r="J3">
         <v>285431.99699999997</v>
@@ -2547,7 +3089,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>863861</v>
+        <v>1403860.9999996261</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -2556,13 +3098,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>10522899.815068083</v>
+        <v>11162359.50971056</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>10805320.119068084</v>
+        <v>11224031.195710558</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -2692,13 +3234,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>10974646.714388685</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>11258268.479107693</v>
+        <v>8301363.9890332539</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -2709,22 +3251,22 @@
         <v>44197</v>
       </c>
       <c r="B3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>24300</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>24300</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>7999.9999999998645</v>
       </c>
       <c r="H3">
         <v>483294.69699999993</v>
@@ -2751,19 +3293,19 @@
         <v>1403860.9999996261</v>
       </c>
       <c r="P3">
-        <v>466373.38999962609</v>
+        <v>469427.99999962631</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>12125874.640943892</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>12254393.372943891</v>
+        <v>8140372.5099991113</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -2893,13 +3435,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8349355.0567190023</v>
+        <v>8238819.7290332541</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -2910,28 +3452,28 @@
         <v>44197</v>
       </c>
       <c r="B3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3">
-        <v>29999.999699999997</v>
+        <v>0</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>29999.999699999997</v>
+        <v>0</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>7999.9999999998645</v>
+        <v>0</v>
       </c>
       <c r="H3">
         <v>483294.69699999993</v>
       </c>
       <c r="I3">
-        <v>1453860.9999996261</v>
+        <v>1453860.9999996268</v>
       </c>
       <c r="J3">
         <v>285431.99699999997</v>
@@ -2949,22 +3491,22 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1403860.9999996261</v>
+        <v>1403860.9999996268</v>
       </c>
       <c r="P3">
-        <v>469427.99999962631</v>
+        <v>477427.99999962613</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>13712432.070248161</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>13774103.756248161</v>
+        <v>8433484.9599991105</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -3067,7 +3609,7 @@
         <v>480594.69699999999</v>
       </c>
       <c r="I2">
-        <v>1095844.5999999999</v>
+        <v>813860.99999979907</v>
       </c>
       <c r="J2">
         <v>285431.99699999997</v>
@@ -3085,7 +3627,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1045844.6</v>
+        <v>763860.99999979907</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -3094,13 +3636,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8383578.7387190033</v>
+        <v>8379169.8810332529</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -3114,13 +3656,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>29999.999699999997</v>
+        <v>24300</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>29999.999699999997</v>
+        <v>24300</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -3132,7 +3674,7 @@
         <v>483294.69699999993</v>
       </c>
       <c r="I3">
-        <v>1259360.2</v>
+        <v>1093860.9999996321</v>
       </c>
       <c r="J3">
         <v>285431.99699999997</v>
@@ -3150,7 +3692,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1209360.2</v>
+        <v>1043860.9999996321</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -3159,13 +3701,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>11817853.32527641</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>11963177.325276406</v>
+        <v>8440604.3459991124</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -3295,13 +3837,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8299587.0507190032</v>
+        <v>8421968.0990332514</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -3315,13 +3857,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>29999.999699999997</v>
+        <v>24300</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>29999.999699999997</v>
+        <v>24300</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -3333,7 +3875,7 @@
         <v>483294.69699999993</v>
       </c>
       <c r="I3">
-        <v>1453860.9999996261</v>
+        <v>1318860.9999997194</v>
       </c>
       <c r="J3">
         <v>285431.99699999997</v>
@@ -3351,7 +3893,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1403860.9999996261</v>
+        <v>1268860.9999997194</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -3360,13 +3902,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>11048656.323729711</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>10959028.83372971</v>
+        <v>8370628.0299991099</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -3469,7 +4011,7 @@
         <v>480594.69699999999</v>
       </c>
       <c r="I2">
-        <v>1183860.999999813</v>
+        <v>1048860.9999999066</v>
       </c>
       <c r="J2">
         <v>285431.99699999997</v>
@@ -3487,7 +4029,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1133860.999999813</v>
+        <v>998860.99999990652</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -3496,13 +4038,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8211874.9087190032</v>
+        <v>8404077.359033253</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -3516,13 +4058,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>29999.999699999997</v>
+        <v>24300</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>29999.999699999997</v>
+        <v>24300</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -3534,7 +4076,7 @@
         <v>483294.69699999993</v>
       </c>
       <c r="I3">
-        <v>1453860.9999996263</v>
+        <v>948860.99999970547</v>
       </c>
       <c r="J3">
         <v>285431.99699999997</v>
@@ -3552,7 +4094,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1403860.9999996263</v>
+        <v>898860.99999970547</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -3561,13 +4103,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8229999.9999991106</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>8433484.9599991105</v>
+        <v>9105477.679977553</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -3670,7 +4212,7 @@
         <v>480594.69699999999</v>
       </c>
       <c r="I2">
-        <v>1183860.999999813</v>
+        <v>813860.99999979907</v>
       </c>
       <c r="J2">
         <v>285431.99699999997</v>
@@ -3688,7 +4230,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1133860.999999813</v>
+        <v>763860.99999979907</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -3697,13 +4239,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8417253.2987190038</v>
+        <v>8345625.5190332523</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -3717,13 +4259,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>29999.999699999997</v>
+        <v>24300</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>29999.999699999997</v>
+        <v>24300</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -3735,7 +4277,7 @@
         <v>483294.69699999993</v>
       </c>
       <c r="I3">
-        <v>1318860.9999997194</v>
+        <v>713860.99999959802</v>
       </c>
       <c r="J3">
         <v>285431.99699999997</v>
@@ -3753,7 +4295,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1268860.9999997194</v>
+        <v>663860.99999959802</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -3762,13 +4304,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8999999.9999775533</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>9140628.0299775563</v>
+        <v>8338713.64999911</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -3871,7 +4413,7 @@
         <v>480594.69699999999</v>
       </c>
       <c r="I2">
-        <v>1048860.9999999066</v>
+        <v>813860.99999979907</v>
       </c>
       <c r="J2">
         <v>285431.99699999997</v>
@@ -3889,7 +4431,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>998860.99999990652</v>
+        <v>763860.99999979907</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -3898,13 +4440,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8393312.2387190033</v>
+        <v>8378109.2990332516</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -3918,13 +4460,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>29999.999699999997</v>
+        <v>24300</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>29999.999699999997</v>
+        <v>24300</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -3936,7 +4478,7 @@
         <v>483294.69699999993</v>
       </c>
       <c r="I3">
-        <v>948860.99999970547</v>
+        <v>958860.99999972573</v>
       </c>
       <c r="J3">
         <v>285431.99699999997</v>
@@ -3954,7 +4496,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>898860.99999970547</v>
+        <v>908860.99999972573</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -3963,13 +4505,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8999999.9999775533</v>
+        <v>8977212.0037249625</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>9105477.679977553</v>
+        <v>9108859.4437249638</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -4072,7 +4614,7 @@
         <v>480594.69699999999</v>
       </c>
       <c r="I2">
-        <v>813860.99999979907</v>
+        <v>1048860.9999999066</v>
       </c>
       <c r="J2">
         <v>285431.99699999997</v>
@@ -4090,7 +4632,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>763860.99999979907</v>
+        <v>998860.99999990652</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -4099,13 +4641,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8336194.6387190036</v>
+        <v>8384089.6590332529</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -4119,13 +4661,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>29999.999699999997</v>
+        <v>24300</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>29999.999699999997</v>
+        <v>24300</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -4137,7 +4679,7 @@
         <v>483294.69699999993</v>
       </c>
       <c r="I3">
-        <v>713860.99999959802</v>
+        <v>1048860.9999999066</v>
       </c>
       <c r="J3">
         <v>285431.99699999997</v>
@@ -4155,7 +4697,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>663860.99999959802</v>
+        <v>998860.99999990652</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -4164,13 +4706,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8229999.9999991106</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>8338713.64999911</v>
+        <v>9104398.0899775531</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -4273,7 +4815,7 @@
         <v>480594.69699999999</v>
       </c>
       <c r="I2">
-        <v>813860.99999979907</v>
+        <v>913861</v>
       </c>
       <c r="J2">
         <v>285431.99699999997</v>
@@ -4291,7 +4833,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>763860.99999979907</v>
+        <v>863861</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -4300,13 +4842,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8364080.2787190014</v>
+        <v>8341387.7390332529</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -4320,13 +4862,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>29999.999699999997</v>
+        <v>24300</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>29999.999699999997</v>
+        <v>24300</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -4338,7 +4880,7 @@
         <v>483294.69699999993</v>
       </c>
       <c r="I3">
-        <v>958860.99999972573</v>
+        <v>1048860.9999999066</v>
       </c>
       <c r="J3">
         <v>285431.99699999997</v>
@@ -4356,7 +4898,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>908860.99999972573</v>
+        <v>998860.99999990652</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -4365,13 +4907,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>7479999.9999999981</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="S3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T3">
-        <v>7611647.4399999948</v>
+        <v>8359167.7799991118</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -4501,13 +5043,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8379791.2487190031</v>
+        <v>8389179.7690332532</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -4518,28 +5060,28 @@
         <v>44197</v>
       </c>
       <c r="B3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3">
-        <v>29999.999699999997</v>
+        <v>0</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>29999.999699999997</v>
+        <v>0</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>7999.9999999998645</v>
+        <v>0</v>
       </c>
       <c r="H3">
         <v>483294.69699999993</v>
       </c>
       <c r="I3">
-        <v>1048860.9999999066</v>
+        <v>1318860.9999997194</v>
       </c>
       <c r="J3">
         <v>285431.99699999997</v>
@@ -4557,22 +5099,22 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>998860.99999990652</v>
+        <v>1268860.9999997194</v>
       </c>
       <c r="P3">
-        <v>469427.99999962631</v>
+        <v>477427.99999962613</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8999999.9999775533</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>9104398.0899775531</v>
+        <v>8493906.2799991108</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -4675,7 +5217,7 @@
         <v>480594.69699999999</v>
       </c>
       <c r="I2">
-        <v>913861</v>
+        <v>1183860.999999813</v>
       </c>
       <c r="J2">
         <v>285431.99699999997</v>
@@ -4693,7 +5235,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>863861</v>
+        <v>1133860.999999813</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -4702,13 +5244,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8340939.9687190047</v>
+        <v>8459395.0790332537</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -4722,13 +5264,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>29999.999699999997</v>
+        <v>24300</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>29999.999699999997</v>
+        <v>24300</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -4740,7 +5282,7 @@
         <v>483294.69699999993</v>
       </c>
       <c r="I3">
-        <v>1048860.9999999066</v>
+        <v>1083860.9999996119</v>
       </c>
       <c r="J3">
         <v>285431.99699999997</v>
@@ -4758,7 +5300,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>998860.99999990652</v>
+        <v>1033860.9999996119</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -4767,13 +5309,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8229999.9999991106</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>8359167.7799991118</v>
+        <v>9166147.929977553</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -4876,7 +5418,7 @@
         <v>480594.69699999999</v>
       </c>
       <c r="I2">
-        <v>1048860.9999999066</v>
+        <v>813860.99999979907</v>
       </c>
       <c r="J2">
         <v>285431.99699999997</v>
@@ -4894,7 +5436,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>998860.99999990652</v>
+        <v>763860.99999979907</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -4903,13 +5445,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8384316.7387190042</v>
+        <v>8359934.0990332542</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -4920,28 +5462,28 @@
         <v>44197</v>
       </c>
       <c r="B3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>24300</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>24300</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>7999.9999999998645</v>
       </c>
       <c r="H3">
         <v>483294.69699999993</v>
       </c>
       <c r="I3">
-        <v>1318860.9999997194</v>
+        <v>513861.00000000675</v>
       </c>
       <c r="J3">
         <v>285431.99699999997</v>
@@ -4959,22 +5501,22 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1268860.9999997194</v>
+        <v>463861.00000000675</v>
       </c>
       <c r="P3">
-        <v>477427.99999962613</v>
+        <v>469427.99999962631</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8229999.9999991106</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>8493906.2799991108</v>
+        <v>9186027.3499775529</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -5077,7 +5619,7 @@
         <v>480594.69699999999</v>
       </c>
       <c r="I2">
-        <v>1183860.999999813</v>
+        <v>613861.0000002078</v>
       </c>
       <c r="J2">
         <v>285431.99699999997</v>
@@ -5095,7 +5637,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1133860.999999813</v>
+        <v>563861.0000002078</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -5104,13 +5646,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8469412.1487190034</v>
+        <v>8418277.9990332499</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -5124,13 +5666,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>29999.999699999997</v>
+        <v>24300</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>29999.999699999997</v>
+        <v>24300</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -5142,7 +5684,7 @@
         <v>483294.69699999993</v>
       </c>
       <c r="I3">
-        <v>1083860.9999996119</v>
+        <v>513861.00000000687</v>
       </c>
       <c r="J3">
         <v>285431.99699999997</v>
@@ -5160,7 +5702,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1033860.9999996119</v>
+        <v>463861.00000000681</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -5175,7 +5717,7 @@
         <v>1</v>
       </c>
       <c r="T3">
-        <v>9166147.929977553</v>
+        <v>9160152.0699775536</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -5278,7 +5820,7 @@
         <v>480594.69699999999</v>
       </c>
       <c r="I2">
-        <v>1095844.5999999999</v>
+        <v>1183860.999999813</v>
       </c>
       <c r="J2">
         <v>285431.99699999997</v>
@@ -5296,7 +5838,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1045844.6</v>
+        <v>1133860.999999813</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -5305,13 +5847,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8384705.7387190033</v>
+        <v>8435305.189033255</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -5322,28 +5864,28 @@
         <v>44197</v>
       </c>
       <c r="B3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3">
-        <v>29999.999699999997</v>
+        <v>0</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>29999.999699999997</v>
+        <v>0</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>7999.9999999998645</v>
+        <v>0</v>
       </c>
       <c r="H3">
         <v>483294.69699999993</v>
       </c>
       <c r="I3">
-        <v>1259360.2</v>
+        <v>1453860.9999996261</v>
       </c>
       <c r="J3">
         <v>285431.99699999997</v>
@@ -5361,22 +5903,22 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1209360.2</v>
+        <v>1403860.9999996261</v>
       </c>
       <c r="P3">
-        <v>469427.99999962631</v>
+        <v>488482.60999962612</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8999999.9999775533</v>
+        <v>10778293.13521014</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>9137627.9999775533</v>
+        <v>11052143.017210139</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -5506,13 +6048,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8367320.2187190037</v>
+        <v>8381215.9290332515</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -5526,13 +6068,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>29999.999699999997</v>
+        <v>24300</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>29999.999699999997</v>
+        <v>24300</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -5544,7 +6086,7 @@
         <v>483294.69699999993</v>
       </c>
       <c r="I3">
-        <v>513861.00000000675</v>
+        <v>813860.99999979907</v>
       </c>
       <c r="J3">
         <v>285431.99699999997</v>
@@ -5562,7 +6104,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>463861.00000000675</v>
+        <v>763860.99999979907</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -5577,7 +6119,7 @@
         <v>1</v>
       </c>
       <c r="T3">
-        <v>9186027.3499775529</v>
+        <v>9183949.7199775539</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -5680,7 +6222,7 @@
         <v>480594.69699999999</v>
       </c>
       <c r="I2">
-        <v>613861.0000002078</v>
+        <v>913861</v>
       </c>
       <c r="J2">
         <v>285431.99699999997</v>
@@ -5698,7 +6240,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>563861.0000002078</v>
+        <v>863861</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -5707,13 +6249,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8416174.1587190032</v>
+        <v>8391165.6090332512</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -5727,13 +6269,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>29999.999699999997</v>
+        <v>24300</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>29999.999699999997</v>
+        <v>24300</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -5745,7 +6287,7 @@
         <v>483294.69699999993</v>
       </c>
       <c r="I3">
-        <v>513861.00000000687</v>
+        <v>1183860.999999813</v>
       </c>
       <c r="J3">
         <v>285431.99699999997</v>
@@ -5763,7 +6305,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>463861.00000000681</v>
+        <v>1133860.999999813</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -5772,13 +6314,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8999999.9999775533</v>
+        <v>11342951.210518882</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>9160152.0699775536</v>
+        <v>11555646.220518883</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -5881,7 +6423,7 @@
         <v>480594.69699999999</v>
       </c>
       <c r="I2">
-        <v>813860.99999979907</v>
+        <v>1183860.999999813</v>
       </c>
       <c r="J2">
         <v>285431.99699999997</v>
@@ -5899,7 +6441,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>763860.99999979907</v>
+        <v>1133860.999999813</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -5908,13 +6450,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8385742.9387190016</v>
+        <v>8436236.8790332507</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -5928,13 +6470,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>29999.999699999997</v>
+        <v>24300</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>29999.999699999997</v>
+        <v>24300</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -5946,7 +6488,7 @@
         <v>483294.69699999993</v>
       </c>
       <c r="I3">
-        <v>813860.99999979907</v>
+        <v>1183860.999999813</v>
       </c>
       <c r="J3">
         <v>285431.99699999997</v>
@@ -5964,7 +6506,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>763860.99999979907</v>
+        <v>1133860.999999813</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -5979,7 +6521,7 @@
         <v>1</v>
       </c>
       <c r="T3">
-        <v>9183949.7199775539</v>
+        <v>9061125.7399775553</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -6109,13 +6651,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8400896.6387190055</v>
+        <v>8315798.3690332538</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -6129,13 +6671,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>29999.999699999997</v>
+        <v>24300</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>29999.999699999997</v>
+        <v>24300</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -6147,7 +6689,7 @@
         <v>483294.69699999993</v>
       </c>
       <c r="I3">
-        <v>1183860.999999813</v>
+        <v>813860.99999979907</v>
       </c>
       <c r="J3">
         <v>285431.99699999997</v>
@@ -6165,7 +6707,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1133860.999999813</v>
+        <v>763860.99999979907</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -6174,13 +6716,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>11750117.627780363</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>11962812.637780361</v>
+        <v>8261744.7299991101</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -6283,7 +6825,7 @@
         <v>480594.69699999999</v>
       </c>
       <c r="I2">
-        <v>1183860.999999813</v>
+        <v>813860.99999979907</v>
       </c>
       <c r="J2">
         <v>285431.99699999997</v>
@@ -6301,7 +6843,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1133860.999999813</v>
+        <v>763860.99999979907</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -6310,13 +6852,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8435909.918719003</v>
+        <v>8309709.8290332528</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -6330,13 +6872,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>29999.999699999997</v>
+        <v>24300</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>29999.999699999997</v>
+        <v>24300</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -6348,7 +6890,7 @@
         <v>483294.69699999993</v>
       </c>
       <c r="I3">
-        <v>1183860.999999813</v>
+        <v>513861.00000000675</v>
       </c>
       <c r="J3">
         <v>285431.99699999997</v>
@@ -6366,7 +6908,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1133860.999999813</v>
+        <v>463861.00000000675</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -6381,7 +6923,7 @@
         <v>1</v>
       </c>
       <c r="T3">
-        <v>9061125.7399775553</v>
+        <v>9088058.5399775542</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -6484,7 +7026,7 @@
         <v>480594.69699999999</v>
       </c>
       <c r="I2">
-        <v>913861</v>
+        <v>613861.0000002078</v>
       </c>
       <c r="J2">
         <v>285431.99699999997</v>
@@ -6502,7 +7044,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>863861</v>
+        <v>563861.0000002078</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -6511,13 +7053,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8295598.118719005</v>
+        <v>8362018.0490332544</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -6531,13 +7073,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>29999.999699999997</v>
+        <v>24300</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>29999.999699999997</v>
+        <v>24300</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -6549,7 +7091,7 @@
         <v>483294.69699999993</v>
       </c>
       <c r="I3">
-        <v>813860.99999979907</v>
+        <v>313861.00000041554</v>
       </c>
       <c r="J3">
         <v>285431.99699999997</v>
@@ -6567,7 +7109,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>763860.99999979907</v>
+        <v>263861.00000041554</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -6576,13 +7118,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8229999.9999991106</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>8261744.7299991101</v>
+        <v>9135931.8499775529</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -6685,7 +7227,7 @@
         <v>480594.69699999999</v>
       </c>
       <c r="I2">
-        <v>813860.99999979907</v>
+        <v>613861.0000002078</v>
       </c>
       <c r="J2">
         <v>285431.99699999997</v>
@@ -6703,7 +7245,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>763860.99999979907</v>
+        <v>563861.0000002078</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -6712,13 +7254,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8295114.0687190033</v>
+        <v>8366599.0990332542</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -6732,13 +7274,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>29999.999699999997</v>
+        <v>24300</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>29999.999699999997</v>
+        <v>24300</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -6750,7 +7292,7 @@
         <v>483294.69699999993</v>
       </c>
       <c r="I3">
-        <v>513861.00000000675</v>
+        <v>613861.00000020862</v>
       </c>
       <c r="J3">
         <v>285431.99699999997</v>
@@ -6768,7 +7310,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>463861.00000000675</v>
+        <v>563861.00000020862</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -6783,409 +7325,7 @@
         <v>1</v>
       </c>
       <c r="T3">
-        <v>9088058.5399775542</v>
-      </c>
-      <c r="U3">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:xdr="http://purl.oclc.org/ooxml/drawingml/spreadsheetDrawing">
-  <dimension ref="A1:U3"/>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="B1" s="259" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="259" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="259" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="259" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="259" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="259" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="259" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="259" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="259" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="259" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="259" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="259" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="259" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="259" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" s="259" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="259" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" s="259" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" s="259" t="s">
-        <v>17</v>
-      </c>
-      <c r="T1" s="259" t="s">
-        <v>18</v>
-      </c>
-      <c r="U1" s="259" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="257">
-        <v>43831</v>
-      </c>
-      <c r="B2">
-        <v>7</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>480594.69699999999</v>
-      </c>
-      <c r="I2">
-        <v>613861.0000002078</v>
-      </c>
-      <c r="J2">
-        <v>285431.99699999997</v>
-      </c>
-      <c r="K2">
-        <v>9009.3999999999996</v>
-      </c>
-      <c r="L2">
-        <v>180000</v>
-      </c>
-      <c r="M2">
-        <v>50000</v>
-      </c>
-      <c r="N2">
-        <v>6153.3000000000002</v>
-      </c>
-      <c r="O2">
-        <v>563861.0000002078</v>
-      </c>
-      <c r="P2">
-        <v>409927.99999981304</v>
-      </c>
-      <c r="Q2">
-        <v>0</v>
-      </c>
-      <c r="R2">
-        <v>8229999.9999999953</v>
-      </c>
-      <c r="S2">
-        <v>1</v>
-      </c>
-      <c r="T2">
-        <v>8357855.8587190043</v>
-      </c>
-      <c r="U2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="257">
-        <v>44197</v>
-      </c>
-      <c r="B3">
-        <v>7</v>
-      </c>
-      <c r="C3">
-        <v>29999.999699999997</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>29999.999699999997</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>7999.9999999998645</v>
-      </c>
-      <c r="H3">
-        <v>483294.69699999993</v>
-      </c>
-      <c r="I3">
-        <v>313861.00000041554</v>
-      </c>
-      <c r="J3">
-        <v>285431.99699999997</v>
-      </c>
-      <c r="K3">
-        <v>11709.4</v>
-      </c>
-      <c r="L3">
-        <v>180000</v>
-      </c>
-      <c r="M3">
-        <v>50000</v>
-      </c>
-      <c r="N3">
-        <v>6153.3000000000002</v>
-      </c>
-      <c r="O3">
-        <v>263861.00000041554</v>
-      </c>
-      <c r="P3">
-        <v>469427.99999962631</v>
-      </c>
-      <c r="Q3">
-        <v>0</v>
-      </c>
-      <c r="R3">
-        <v>8999999.9999775533</v>
-      </c>
-      <c r="S3">
-        <v>1</v>
-      </c>
-      <c r="T3">
-        <v>9135931.8499775529</v>
-      </c>
-      <c r="U3">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:xdr="http://purl.oclc.org/ooxml/drawingml/spreadsheetDrawing">
-  <dimension ref="A1:U3"/>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="B1" s="266" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="266" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="266" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="266" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="266" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="266" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="266" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="266" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="266" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="266" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="266" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="266" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="266" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="266" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" s="266" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="266" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" s="266" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" s="266" t="s">
-        <v>17</v>
-      </c>
-      <c r="T1" s="266" t="s">
-        <v>18</v>
-      </c>
-      <c r="U1" s="266" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="264">
-        <v>43831</v>
-      </c>
-      <c r="B2">
-        <v>7</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>480594.69699999999</v>
-      </c>
-      <c r="I2">
-        <v>613861.0000002078</v>
-      </c>
-      <c r="J2">
-        <v>285431.99699999997</v>
-      </c>
-      <c r="K2">
-        <v>9009.3999999999996</v>
-      </c>
-      <c r="L2">
-        <v>180000</v>
-      </c>
-      <c r="M2">
-        <v>50000</v>
-      </c>
-      <c r="N2">
-        <v>6153.3000000000002</v>
-      </c>
-      <c r="O2">
-        <v>563861.0000002078</v>
-      </c>
-      <c r="P2">
-        <v>409927.99999981304</v>
-      </c>
-      <c r="Q2">
-        <v>0</v>
-      </c>
-      <c r="R2">
-        <v>8229999.9999999953</v>
-      </c>
-      <c r="S2">
-        <v>1</v>
-      </c>
-      <c r="T2">
-        <v>8367717.0187190045</v>
-      </c>
-      <c r="U2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="264">
-        <v>44197</v>
-      </c>
-      <c r="B3">
-        <v>7</v>
-      </c>
-      <c r="C3">
-        <v>29999.999699999997</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>29999.999699999997</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>7999.9999999998645</v>
-      </c>
-      <c r="H3">
-        <v>483294.69699999993</v>
-      </c>
-      <c r="I3">
-        <v>613861.00000020827</v>
-      </c>
-      <c r="J3">
-        <v>285431.99699999997</v>
-      </c>
-      <c r="K3">
-        <v>11709.4</v>
-      </c>
-      <c r="L3">
-        <v>180000</v>
-      </c>
-      <c r="M3">
-        <v>50000</v>
-      </c>
-      <c r="N3">
-        <v>6153.3000000000002</v>
-      </c>
-      <c r="O3">
-        <v>563861.00000020815</v>
-      </c>
-      <c r="P3">
-        <v>469427.99999962631</v>
-      </c>
-      <c r="Q3">
-        <v>0</v>
-      </c>
-      <c r="R3">
-        <v>8480334.9247879162</v>
-      </c>
-      <c r="S3">
-        <v>1</v>
-      </c>
-      <c r="T3">
-        <v>8591315.9507879168</v>
+        <v>9110981.0259775538</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -7288,7 +7428,7 @@
         <v>480594.69699999999</v>
       </c>
       <c r="I2">
-        <v>906235.80000430183</v>
+        <v>1183860.999999813</v>
       </c>
       <c r="J2">
         <v>285431.99699999997</v>
@@ -7306,7 +7446,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>856235.80000430183</v>
+        <v>1133860.999999813</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -7315,13 +7455,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8372721.8507190049</v>
+        <v>8500385.8210332524</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -7332,28 +7472,28 @@
         <v>44197</v>
       </c>
       <c r="B3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3">
-        <v>29999.999699999997</v>
+        <v>0</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>29999.999699999997</v>
+        <v>0</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>7999.9999999998645</v>
+        <v>0</v>
       </c>
       <c r="H3">
         <v>483294.69699999993</v>
       </c>
       <c r="I3">
-        <v>1176998.3200036848</v>
+        <v>1453860.9999996261</v>
       </c>
       <c r="J3">
         <v>285431.99699999997</v>
@@ -7371,22 +7511,22 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1126998.3200036846</v>
+        <v>1403860.9999996261</v>
       </c>
       <c r="P3">
-        <v>469427.99999962631</v>
+        <v>477427.99999962613</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8229999.9999991106</v>
+        <v>13624090.298644044</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>8440604.3459991124</v>
+        <v>13915397.500644045</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -7516,13 +7656,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8434458.0807190053</v>
+        <v>8472835.3090332542</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -7533,28 +7673,28 @@
         <v>44197</v>
       </c>
       <c r="B3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3">
-        <v>29999.999699999997</v>
+        <v>0</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>29999.999699999997</v>
+        <v>0</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>7999.9999999998645</v>
+        <v>0</v>
       </c>
       <c r="H3">
         <v>483294.69699999993</v>
       </c>
       <c r="I3">
-        <v>1453860.9999996261</v>
+        <v>1083860.9999996119</v>
       </c>
       <c r="J3">
         <v>285431.99699999997</v>
@@ -7572,22 +7712,22 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1403860.9999996261</v>
+        <v>1033860.9999996119</v>
       </c>
       <c r="P3">
-        <v>469427.99999962631</v>
+        <v>477427.99999962613</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>12703858.994271697</v>
+        <v>10415454.195548035</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>12977708.876271699</v>
+        <v>10640357.527548036</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -7690,7 +7830,7 @@
         <v>480594.69699999999</v>
       </c>
       <c r="I2">
-        <v>1183860.999999813</v>
+        <v>813860.99999979907</v>
       </c>
       <c r="J2">
         <v>285431.99699999997</v>
@@ -7708,7 +7848,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1133860.999999813</v>
+        <v>763860.99999979907</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -7717,13 +7857,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8498951.2427190021</v>
+        <v>8412722.4750332516</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -7734,28 +7874,28 @@
         <v>44197</v>
       </c>
       <c r="B3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>24300</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>24300</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>7999.9999999998645</v>
       </c>
       <c r="H3">
         <v>483294.69699999993</v>
       </c>
       <c r="I3">
-        <v>1453860.9999996261</v>
+        <v>1093860.9999996321</v>
       </c>
       <c r="J3">
         <v>285431.99699999997</v>
@@ -7773,22 +7913,22 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1403860.9999996261</v>
+        <v>1043860.9999996321</v>
       </c>
       <c r="P3">
-        <v>477427.99999962613</v>
+        <v>469427.99999962631</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>13799263.92287196</v>
+        <v>12352353.423652945</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>14090571.12487196</v>
+        <v>12500386.051652946</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -7918,13 +8058,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8478198.5587190036</v>
+        <v>8365797.7570332531</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -7935,22 +8075,22 @@
         <v>44197</v>
       </c>
       <c r="B3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>24300</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>24300</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>7999.9999999998645</v>
       </c>
       <c r="H3">
         <v>483294.69699999993</v>
@@ -7977,19 +8117,19 @@
         <v>1033860.9999996119</v>
       </c>
       <c r="P3">
-        <v>477427.99999962613</v>
+        <v>469427.99999962631</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>10574473.267596161</v>
+        <v>11031228.415133042</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>10799376.59959616</v>
+        <v>11219086.211133042</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -8119,13 +8259,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8424348.3727190029</v>
+        <v>8416761.01103325</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -8139,13 +8279,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>29999.999699999997</v>
+        <v>24300</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>29999.999699999997</v>
+        <v>24300</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -8157,7 +8297,7 @@
         <v>483294.69699999993</v>
       </c>
       <c r="I3">
-        <v>1093860.9999996321</v>
+        <v>513861.00000000675</v>
       </c>
       <c r="J3">
         <v>285431.99699999997</v>
@@ -8175,7 +8315,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1043860.9999996321</v>
+        <v>463861.00000000675</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -8184,13 +8324,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>12005874.347986775</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>12153906.975986775</v>
+        <v>8417833.5499991123</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -8293,7 +8433,7 @@
         <v>480594.69699999999</v>
       </c>
       <c r="I2">
-        <v>1183860.999999813</v>
+        <v>613861.0000002078</v>
       </c>
       <c r="J2">
         <v>285431.99699999997</v>
@@ -8311,7 +8451,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1133860.999999813</v>
+        <v>563861.0000002078</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -8320,13 +8460,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8364513.5347190024</v>
+        <v>8394107.3810332529</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -8340,13 +8480,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>29999.999699999997</v>
+        <v>24300</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>29999.999699999997</v>
+        <v>24300</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -8358,7 +8498,7 @@
         <v>483294.69699999993</v>
       </c>
       <c r="I3">
-        <v>1083860.9999996119</v>
+        <v>513861.00000000687</v>
       </c>
       <c r="J3">
         <v>285431.99699999997</v>
@@ -8376,7 +8516,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1033860.9999996119</v>
+        <v>463861.00000000681</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -8391,7 +8531,7 @@
         <v>1</v>
       </c>
       <c r="T3">
-        <v>9187857.7959775534</v>
+        <v>9150597.6699775551</v>
       </c>
       <c r="U3">
         <v>0</v>

</xml_diff>

<commit_message>
March 2020 MTOM Run
Update to ensemble forecast, model file, and output files. No updates to model file or ruleset since the February run. Model file naming convention updated
</commit_message>
<xml_diff>
--- a/Output Data/MtomToCrss_Annual.xlsx
+++ b/Output Data/MtomToCrss_Annual.xlsx
@@ -132,7 +132,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="505">
+  <borders count="253">
     <border>
       <start/>
       <end/>
@@ -392,263 +392,11 @@
     <border/>
     <border/>
     <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="505">
+  <cellXfs count="253">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -974,330 +722,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="252" xfId="0" applyNumberFormat="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="253" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="254" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="255" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="256" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="257" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="258" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="259" xfId="0" applyNumberFormat="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="260" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="261" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="262" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="263" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="264" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="265" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="266" xfId="0" applyNumberFormat="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="267" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="268" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="269" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="270" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="271" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="272" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="273" xfId="0" applyNumberFormat="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="274" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="275" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="276" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="277" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="278" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="279" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="280" xfId="0" applyNumberFormat="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="281" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="282" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="283" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="284" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="285" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="286" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="287" xfId="0" applyNumberFormat="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="288" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="289" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="290" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="291" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="292" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="293" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="294" xfId="0" applyNumberFormat="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="295" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="296" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="297" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="298" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="299" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="300" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="301" xfId="0" applyNumberFormat="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="302" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="303" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="304" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="305" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="306" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="307" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="308" xfId="0" applyNumberFormat="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="309" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="310" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="311" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="312" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="313" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="314" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="315" xfId="0" applyNumberFormat="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="316" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="317" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="318" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="319" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="320" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="321" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="322" xfId="0" applyNumberFormat="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="323" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="324" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="325" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="326" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="327" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="328" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="329" xfId="0" applyNumberFormat="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="330" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="331" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="332" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="333" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="334" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="335" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="336" xfId="0" applyNumberFormat="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="337" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="338" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="339" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="340" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="341" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="342" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="343" xfId="0" applyNumberFormat="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="344" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="345" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="346" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="347" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="348" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="349" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="350" xfId="0" applyNumberFormat="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="351" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="352" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="353" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="354" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="355" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="356" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="357" xfId="0" applyNumberFormat="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="358" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="359" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="360" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="361" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="362" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="363" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="364" xfId="0" applyNumberFormat="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="365" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="366" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="367" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="368" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="369" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="370" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="371" xfId="0" applyNumberFormat="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="372" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="373" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="374" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="375" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="376" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="377" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="378" xfId="0" applyNumberFormat="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="379" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="380" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="381" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="382" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="383" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="384" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="385" xfId="0" applyNumberFormat="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="386" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="387" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="388" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="389" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="390" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="391" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="392" xfId="0" applyNumberFormat="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="393" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="394" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="395" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="396" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="397" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="398" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="399" xfId="0" applyNumberFormat="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="400" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="401" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="402" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="403" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="404" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="405" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="406" xfId="0" applyNumberFormat="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="407" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="408" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="409" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="410" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="411" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="412" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="413" xfId="0" applyNumberFormat="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="414" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="415" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="416" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="417" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="418" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="419" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="420" xfId="0" applyNumberFormat="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="421" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="422" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="423" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="424" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="425" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="426" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="427" xfId="0" applyNumberFormat="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="428" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="429" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="430" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="431" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="432" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="433" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="434" xfId="0" applyNumberFormat="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="435" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="436" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="437" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="438" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="439" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="440" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="441" xfId="0" applyNumberFormat="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="442" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="443" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="444" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="445" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="446" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="447" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="448" xfId="0" applyNumberFormat="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="449" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="450" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="451" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="452" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="453" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="454" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="455" xfId="0" applyNumberFormat="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="456" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="457" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="458" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="459" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="460" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="461" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="462" xfId="0" applyNumberFormat="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="463" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="464" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="465" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="466" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="467" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="468" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="469" xfId="0" applyNumberFormat="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="470" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="471" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="472" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="473" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="474" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="475" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="476" xfId="0" applyNumberFormat="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="477" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="478" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="479" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="480" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="481" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="482" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="483" xfId="0" applyNumberFormat="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="484" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="485" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="486" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="487" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="488" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="489" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="490" xfId="0" applyNumberFormat="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="491" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="492" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="493" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="494" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="495" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="496" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="497" xfId="0" applyNumberFormat="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="498" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="499" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="500" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="501" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="502" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="503" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="504" xfId="0" applyNumberFormat="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1395,13 +819,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>480594.40000000002</v>
       </c>
       <c r="I2">
-        <v>1097690.5</v>
+        <v>925054.30000000005</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -1416,10 +840,10 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1047690.5</v>
+        <v>875054.29999999993</v>
       </c>
       <c r="P2">
-        <v>409927.99999981304</v>
+        <v>407756.29999981303</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -1431,7 +855,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8388617.0990332533</v>
+        <v>8424446.4063992016</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -1445,13 +869,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>24300</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>24300</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -1460,13 +884,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>483294.39999999991</v>
       </c>
       <c r="I3">
-        <v>1261206.0999999999</v>
+        <v>1088569.8999999999</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -1481,10 +905,10 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1211206.0999999999</v>
+        <v>1038569.8999999999</v>
       </c>
       <c r="P3">
-        <v>469427.99999962631</v>
+        <v>432670.19999962609</v>
       </c>
       <c r="Q3">
         <v>0</v>
@@ -1496,7 +920,7 @@
         <v>1</v>
       </c>
       <c r="T3">
-        <v>9137627.9999775533</v>
+        <v>9157545.9999775533</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -1596,13 +1020,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>480594.40000000002</v>
       </c>
       <c r="I2">
         <v>813860.99999979907</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -1620,7 +1044,7 @@
         <v>763860.99999979907</v>
       </c>
       <c r="P2">
-        <v>409927.99999981304</v>
+        <v>407756.29999981303</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -1632,7 +1056,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8373008.8290332509</v>
+        <v>8376056.7183992025</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -1646,13 +1070,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>24300</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>24300</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -1661,13 +1085,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>483294.39999999991</v>
       </c>
       <c r="I3">
         <v>813860.99999979988</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -1685,19 +1109,19 @@
         <v>763860.99999979977</v>
       </c>
       <c r="P3">
-        <v>469427.99999962631</v>
+        <v>432670.19999962609</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8714241.2454313841</v>
+        <v>8452802.8367139585</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>8850734.6714313831</v>
+        <v>8589296.2627139594</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -1797,13 +1221,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>480594.40000000002</v>
       </c>
       <c r="I2">
         <v>613861.0000002078</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -1821,7 +1245,7 @@
         <v>563861.0000002078</v>
       </c>
       <c r="P2">
-        <v>409927.99999981304</v>
+        <v>407756.29999981303</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -1833,7 +1257,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8369752.0770332525</v>
+        <v>8385843.4903992014</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -1847,13 +1271,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>24300</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>24300</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -1862,13 +1286,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>483294.39999999991</v>
       </c>
       <c r="I3">
         <v>313861.00000041554</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -1886,7 +1310,7 @@
         <v>263861.00000041554</v>
       </c>
       <c r="P3">
-        <v>469427.99999962631</v>
+        <v>432670.19999962609</v>
       </c>
       <c r="Q3">
         <v>0</v>
@@ -1998,13 +1422,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>480594.40000000002</v>
       </c>
       <c r="I2">
         <v>613861.0000002078</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -2022,7 +1446,7 @@
         <v>563861.0000002078</v>
       </c>
       <c r="P2">
-        <v>409927.99999981304</v>
+        <v>407756.29999981303</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -2034,7 +1458,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8420218.8750332519</v>
+        <v>8424399.204399202</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -2048,13 +1472,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>24300</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>24300</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -2063,13 +1487,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>483294.39999999991</v>
       </c>
       <c r="I3">
         <v>313861.00000041554</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -2087,19 +1511,19 @@
         <v>263861.00000041554</v>
       </c>
       <c r="P3">
-        <v>469427.99999962631</v>
+        <v>432670.19999962609</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8229999.9999991106</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>8469478.9159991127</v>
+        <v>9239478.9159775525</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -2199,13 +1623,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>480594.40000000002</v>
       </c>
       <c r="I2">
         <v>613861.0000002078</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -2223,7 +1647,7 @@
         <v>563861.0000002078</v>
       </c>
       <c r="P2">
-        <v>409927.99999981304</v>
+        <v>407756.29999981303</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -2235,7 +1659,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8466740.6050332543</v>
+        <v>8462825.0763992034</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -2249,13 +1673,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>24300</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>24300</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -2264,13 +1688,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>483294.39999999991</v>
       </c>
       <c r="I3">
         <v>763861.00000010396</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -2288,19 +1712,19 @@
         <v>713861.00000010396</v>
       </c>
       <c r="P3">
-        <v>469427.99999962631</v>
+        <v>432670.19999962609</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>9428522.0439325348</v>
+        <v>9882374.4327692855</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>9838340.2679325324</v>
+        <v>10292192.656769285</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -2400,13 +1824,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>480594.40000000002</v>
       </c>
       <c r="I2">
         <v>1048860.9999999066</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -2424,7 +1848,7 @@
         <v>998860.99999990652</v>
       </c>
       <c r="P2">
-        <v>409927.99999981304</v>
+        <v>407756.29999981303</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -2436,7 +1860,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8535845.9710332509</v>
+        <v>8483697.6143992003</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -2465,13 +1889,13 @@
         <v>0</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>483294.39999999991</v>
       </c>
       <c r="I3">
         <v>748861.00000011432</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -2489,19 +1913,19 @@
         <v>698861.00000011432</v>
       </c>
       <c r="P3">
-        <v>477427.99999962613</v>
+        <v>440670.19999962603</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8229999.9999991106</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>8362878.8059991114</v>
+        <v>9132878.8059775531</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -2601,13 +2025,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>480594.40000000002</v>
       </c>
       <c r="I2">
         <v>613861.0000002078</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -2625,7 +2049,7 @@
         <v>563861.0000002078</v>
       </c>
       <c r="P2">
-        <v>409927.99999981304</v>
+        <v>407756.29999981303</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -2637,7 +2061,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8362630.2730332529</v>
+        <v>8371518.346399202</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -2651,13 +2075,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>24300</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>24300</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -2666,13 +2090,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>483294.39999999991</v>
       </c>
       <c r="I3">
         <v>913861</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -2690,19 +2114,19 @@
         <v>863861</v>
       </c>
       <c r="P3">
-        <v>469427.99999962631</v>
+        <v>432670.19999962609</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>10837705.370753584</v>
+        <v>10764807.687744044</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>11120125.674753584</v>
+        <v>11047227.991744043</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -2802,13 +2226,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>480594.40000000002</v>
       </c>
       <c r="I2">
         <v>1183860.999999813</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -2826,19 +2250,19 @@
         <v>1133860.999999813</v>
       </c>
       <c r="P2">
-        <v>409927.99999981304</v>
+        <v>407756.29999981303</v>
       </c>
       <c r="Q2">
         <v>0</v>
       </c>
       <c r="R2">
-        <v>9799204.6629683357</v>
+        <v>9859719.1852401458</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>10061978.228001589</v>
+        <v>10112617.917639352</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -2867,13 +2291,13 @@
         <v>0</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>483294.39999999991</v>
       </c>
       <c r="I3">
         <v>1453860.9999996261</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -2891,19 +2315,19 @@
         <v>1403860.9999996261</v>
       </c>
       <c r="P3">
-        <v>466373.38999962609</v>
+        <v>427122.94999960525</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>11955559.365453757</v>
+        <v>11200310.097028736</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>12084078.097453758</v>
+        <v>11328828.829028735</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -3003,13 +2427,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>480594.40000000002</v>
       </c>
       <c r="I2">
         <v>1183860.999999813</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -3027,7 +2451,7 @@
         <v>1133860.999999813</v>
       </c>
       <c r="P2">
-        <v>409927.99999981304</v>
+        <v>407756.29999981303</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -3039,7 +2463,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8352671.9550332529</v>
+        <v>8365609.4083992019</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -3053,13 +2477,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>24300</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>24300</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -3068,13 +2492,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>483294.39999999991</v>
       </c>
       <c r="I3">
         <v>1453860.9999996261</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -3092,19 +2516,19 @@
         <v>1403860.9999996261</v>
       </c>
       <c r="P3">
-        <v>469427.99999962631</v>
+        <v>432670.19999962609</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>11162359.50971056</v>
+        <v>11177339.920068583</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>11224031.195710558</v>
+        <v>11239011.606068581</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -3204,13 +2628,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>480594.40000000002</v>
       </c>
       <c r="I2">
         <v>1183860.999999813</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -3228,7 +2652,7 @@
         <v>1133860.999999813</v>
       </c>
       <c r="P2">
-        <v>409927.99999981304</v>
+        <v>407756.29999981303</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -3240,7 +2664,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8301363.9890332539</v>
+        <v>8327496.5563992029</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -3254,13 +2678,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>24300</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>24300</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -3269,13 +2693,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>483294.39999999991</v>
       </c>
       <c r="I3">
         <v>1453860.9999996261</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -3293,7 +2717,7 @@
         <v>1403860.9999996261</v>
       </c>
       <c r="P3">
-        <v>469427.99999962631</v>
+        <v>432670.19999962609</v>
       </c>
       <c r="Q3">
         <v>0</v>
@@ -3405,13 +2829,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>480594.40000000002</v>
       </c>
       <c r="I2">
         <v>1183860.999999813</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -3429,7 +2853,7 @@
         <v>1133860.999999813</v>
       </c>
       <c r="P2">
-        <v>409927.99999981304</v>
+        <v>407756.29999981303</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -3441,7 +2865,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8238819.7290332541</v>
+        <v>8272618.386399202</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -3470,13 +2894,13 @@
         <v>0</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>483294.39999999991</v>
       </c>
       <c r="I3">
         <v>1453860.9999996268</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -3494,7 +2918,7 @@
         <v>1403860.9999996268</v>
       </c>
       <c r="P3">
-        <v>477427.99999962613</v>
+        <v>440670.19999962603</v>
       </c>
       <c r="Q3">
         <v>0</v>
@@ -3606,13 +3030,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>480594.40000000002</v>
       </c>
       <c r="I2">
         <v>813860.99999979907</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -3630,7 +3054,7 @@
         <v>763860.99999979907</v>
       </c>
       <c r="P2">
-        <v>409927.99999981304</v>
+        <v>407756.29999981303</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -3642,7 +3066,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8379169.8810332529</v>
+        <v>8389944.5143992007</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -3656,13 +3080,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>24300</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>24300</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -3671,13 +3095,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>483294.39999999991</v>
       </c>
       <c r="I3">
         <v>1093860.9999996321</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -3695,7 +3119,7 @@
         <v>1043860.9999996321</v>
       </c>
       <c r="P3">
-        <v>469427.99999962631</v>
+        <v>432670.19999962609</v>
       </c>
       <c r="Q3">
         <v>0</v>
@@ -3807,13 +3231,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>480594.40000000002</v>
       </c>
       <c r="I2">
         <v>1183860.999999813</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -3831,7 +3255,7 @@
         <v>1133860.999999813</v>
       </c>
       <c r="P2">
-        <v>409927.99999981304</v>
+        <v>407756.29999981303</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -3843,7 +3267,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8421968.0990332514</v>
+        <v>8439292.2963992022</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -3857,13 +3281,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>24300</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>24300</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -3872,13 +3296,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>483294.39999999991</v>
       </c>
       <c r="I3">
         <v>1318860.9999997194</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -3896,19 +3320,19 @@
         <v>1268860.9999997194</v>
       </c>
       <c r="P3">
-        <v>469427.99999962631</v>
+        <v>432670.19999962609</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8229999.9999991106</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>8370628.0299991099</v>
+        <v>9140628.0299775563</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -4008,13 +3432,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>480594.40000000002</v>
       </c>
       <c r="I2">
         <v>1048860.9999999066</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -4032,7 +3456,7 @@
         <v>998860.99999990652</v>
       </c>
       <c r="P2">
-        <v>409927.99999981304</v>
+        <v>407756.29999981303</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -4044,7 +3468,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8404077.359033253</v>
+        <v>8424551.2063992042</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -4058,13 +3482,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>24300</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>24300</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -4073,13 +3497,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>483294.39999999991</v>
       </c>
       <c r="I3">
         <v>948860.99999970547</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -4097,7 +3521,7 @@
         <v>898860.99999970547</v>
       </c>
       <c r="P3">
-        <v>469427.99999962631</v>
+        <v>432670.19999962609</v>
       </c>
       <c r="Q3">
         <v>0</v>
@@ -4209,13 +3633,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>480594.40000000002</v>
       </c>
       <c r="I2">
         <v>813860.99999979907</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -4233,7 +3657,7 @@
         <v>763860.99999979907</v>
       </c>
       <c r="P2">
-        <v>409927.99999981304</v>
+        <v>407756.29999981303</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -4245,7 +3669,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8345625.5190332523</v>
+        <v>8365071.6863992019</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -4259,13 +3683,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>24300</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>24300</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -4274,13 +3698,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>483294.39999999991</v>
       </c>
       <c r="I3">
         <v>713860.99999959802</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -4298,7 +3722,7 @@
         <v>663860.99999959802</v>
       </c>
       <c r="P3">
-        <v>469427.99999962631</v>
+        <v>432670.19999962609</v>
       </c>
       <c r="Q3">
         <v>0</v>
@@ -4410,13 +3834,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>480594.40000000002</v>
       </c>
       <c r="I2">
         <v>813860.99999979907</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -4434,7 +3858,7 @@
         <v>763860.99999979907</v>
       </c>
       <c r="P2">
-        <v>409927.99999981304</v>
+        <v>407756.29999981303</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -4446,7 +3870,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8378109.2990332516</v>
+        <v>8398877.5363992024</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -4460,13 +3884,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>24300</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>24300</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -4475,13 +3899,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>483294.39999999991</v>
       </c>
       <c r="I3">
         <v>958860.99999972573</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -4499,19 +3923,19 @@
         <v>908860.99999972573</v>
       </c>
       <c r="P3">
-        <v>469427.99999962631</v>
+        <v>432670.19999962609</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8977212.0037249625</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>9108859.4437249638</v>
+        <v>9131647.4399775527</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -4611,13 +4035,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>480594.40000000002</v>
       </c>
       <c r="I2">
         <v>1048860.9999999066</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -4635,7 +4059,7 @@
         <v>998860.99999990652</v>
       </c>
       <c r="P2">
-        <v>409927.99999981304</v>
+        <v>407756.29999981303</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -4647,7 +4071,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8384089.6590332529</v>
+        <v>8397946.9563992023</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -4661,13 +4085,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>24300</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>24300</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -4676,13 +4100,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>483294.39999999991</v>
       </c>
       <c r="I3">
         <v>1048860.9999999066</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -4700,7 +4124,7 @@
         <v>998860.99999990652</v>
       </c>
       <c r="P3">
-        <v>469427.99999962631</v>
+        <v>432670.19999962609</v>
       </c>
       <c r="Q3">
         <v>0</v>
@@ -4812,13 +4236,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>480594.40000000002</v>
       </c>
       <c r="I2">
         <v>913861</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -4836,7 +4260,7 @@
         <v>863861</v>
       </c>
       <c r="P2">
-        <v>409927.99999981304</v>
+        <v>407756.29999981303</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -4848,7 +4272,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8341387.7390332529</v>
+        <v>8348992.4763992019</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -4862,13 +4286,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>24300</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>24300</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -4877,13 +4301,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>483294.39999999991</v>
       </c>
       <c r="I3">
         <v>1048860.9999999066</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -4901,7 +4325,7 @@
         <v>998860.99999990652</v>
       </c>
       <c r="P3">
-        <v>469427.99999962631</v>
+        <v>432670.19999962609</v>
       </c>
       <c r="Q3">
         <v>0</v>
@@ -5013,13 +4437,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>480594.40000000002</v>
       </c>
       <c r="I2">
         <v>1048860.9999999066</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -5037,7 +4461,7 @@
         <v>998860.99999990652</v>
       </c>
       <c r="P2">
-        <v>409927.99999981304</v>
+        <v>407756.29999981303</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -5049,7 +4473,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8389179.7690332532</v>
+        <v>8403214.0063992012</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -5078,13 +4502,13 @@
         <v>0</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>483294.39999999991</v>
       </c>
       <c r="I3">
         <v>1318860.9999997194</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -5102,7 +4526,7 @@
         <v>1268860.9999997194</v>
       </c>
       <c r="P3">
-        <v>477427.99999962613</v>
+        <v>440670.19999962603</v>
       </c>
       <c r="Q3">
         <v>0</v>
@@ -5214,13 +4638,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>480594.40000000002</v>
       </c>
       <c r="I2">
         <v>1183860.999999813</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -5238,7 +4662,7 @@
         <v>1133860.999999813</v>
       </c>
       <c r="P2">
-        <v>409927.99999981304</v>
+        <v>407756.29999981303</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -5250,7 +4674,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8459395.0790332537</v>
+        <v>8461261.2163992021</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -5264,13 +4688,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>24300</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>24300</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -5279,13 +4703,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>483294.39999999991</v>
       </c>
       <c r="I3">
         <v>1083860.9999996119</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -5303,7 +4727,7 @@
         <v>1033860.9999996119</v>
       </c>
       <c r="P3">
-        <v>469427.99999962631</v>
+        <v>432670.19999962609</v>
       </c>
       <c r="Q3">
         <v>0</v>
@@ -5415,13 +4839,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>480594.40000000002</v>
       </c>
       <c r="I2">
         <v>813860.99999979907</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -5439,7 +4863,7 @@
         <v>763860.99999979907</v>
       </c>
       <c r="P2">
-        <v>409927.99999981304</v>
+        <v>407756.29999981303</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -5451,7 +4875,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8359934.0990332542</v>
+        <v>8368555.8463992029</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -5465,13 +4889,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>24300</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>24300</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -5480,13 +4904,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>483294.39999999991</v>
       </c>
       <c r="I3">
         <v>513861.00000000675</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -5504,7 +4928,7 @@
         <v>463861.00000000675</v>
       </c>
       <c r="P3">
-        <v>469427.99999962631</v>
+        <v>432670.19999962609</v>
       </c>
       <c r="Q3">
         <v>0</v>
@@ -5616,13 +5040,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>480594.40000000002</v>
       </c>
       <c r="I2">
         <v>613861.0000002078</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -5640,7 +5064,7 @@
         <v>563861.0000002078</v>
       </c>
       <c r="P2">
-        <v>409927.99999981304</v>
+        <v>407756.29999981303</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -5652,7 +5076,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8418277.9990332499</v>
+        <v>8431872.3363992013</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -5666,13 +5090,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>24300</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>24300</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -5681,13 +5105,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>483294.39999999991</v>
       </c>
       <c r="I3">
         <v>513861.00000000687</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -5705,7 +5129,7 @@
         <v>463861.00000000681</v>
       </c>
       <c r="P3">
-        <v>469427.99999962631</v>
+        <v>432670.19999962609</v>
       </c>
       <c r="Q3">
         <v>0</v>
@@ -5817,13 +5241,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>480594.40000000002</v>
       </c>
       <c r="I2">
         <v>1183860.999999813</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -5841,7 +5265,7 @@
         <v>1133860.999999813</v>
       </c>
       <c r="P2">
-        <v>409927.99999981304</v>
+        <v>407756.29999981303</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -5853,7 +5277,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8435305.189033255</v>
+        <v>8433966.2863992024</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -5882,13 +5306,13 @@
         <v>0</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>483294.39999999991</v>
       </c>
       <c r="I3">
         <v>1453860.9999996261</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -5906,19 +5330,19 @@
         <v>1403860.9999996261</v>
       </c>
       <c r="P3">
-        <v>488482.60999962612</v>
+        <v>453454.11499962612</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>10778293.13521014</v>
+        <v>11432128.04575788</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>11052143.017210139</v>
+        <v>11705977.92775788</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -6018,13 +5442,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>480594.40000000002</v>
       </c>
       <c r="I2">
         <v>813860.99999979907</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -6042,7 +5466,7 @@
         <v>763860.99999979907</v>
       </c>
       <c r="P2">
-        <v>409927.99999981304</v>
+        <v>407756.29999981303</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -6054,7 +5478,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8381215.9290332515</v>
+        <v>8394337.1663992014</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -6068,13 +5492,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>24300</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>24300</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -6083,13 +5507,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>483294.39999999991</v>
       </c>
       <c r="I3">
         <v>813860.99999979907</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -6107,7 +5531,7 @@
         <v>763860.99999979907</v>
       </c>
       <c r="P3">
-        <v>469427.99999962631</v>
+        <v>432670.19999962609</v>
       </c>
       <c r="Q3">
         <v>0</v>
@@ -6219,13 +5643,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>480594.40000000002</v>
       </c>
       <c r="I2">
         <v>913861</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -6243,7 +5667,7 @@
         <v>863861</v>
       </c>
       <c r="P2">
-        <v>409927.99999981304</v>
+        <v>407756.29999981303</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -6255,7 +5679,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8391165.6090332512</v>
+        <v>8401100.6163992025</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -6269,13 +5693,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>24300</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>24300</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -6284,13 +5708,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>483294.39999999991</v>
       </c>
       <c r="I3">
         <v>1183860.999999813</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -6308,19 +5732,19 @@
         <v>1133860.999999813</v>
       </c>
       <c r="P3">
-        <v>469427.99999962631</v>
+        <v>432670.19999962609</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>11342951.210518882</v>
+        <v>11383296.242107842</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>11555646.220518883</v>
+        <v>11595991.252107842</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -6420,13 +5844,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>480594.40000000002</v>
       </c>
       <c r="I2">
         <v>1183860.999999813</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -6444,7 +5868,7 @@
         <v>1133860.999999813</v>
       </c>
       <c r="P2">
-        <v>409927.99999981304</v>
+        <v>407756.29999981303</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -6456,7 +5880,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8436236.8790332507</v>
+        <v>8448059.6863992009</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -6470,13 +5894,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>24300</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>24300</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -6485,13 +5909,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>483294.39999999991</v>
       </c>
       <c r="I3">
         <v>1183860.999999813</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -6509,7 +5933,7 @@
         <v>1133860.999999813</v>
       </c>
       <c r="P3">
-        <v>469427.99999962631</v>
+        <v>432670.19999962609</v>
       </c>
       <c r="Q3">
         <v>0</v>
@@ -6621,13 +6045,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>480594.40000000002</v>
       </c>
       <c r="I2">
         <v>913861</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -6645,7 +6069,7 @@
         <v>863861</v>
       </c>
       <c r="P2">
-        <v>409927.99999981304</v>
+        <v>407756.29999981303</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -6657,7 +6081,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8315798.3690332538</v>
+        <v>8337828.3263992034</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -6671,13 +6095,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>24300</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>24300</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -6686,13 +6110,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>483294.39999999991</v>
       </c>
       <c r="I3">
         <v>813860.99999979907</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -6710,7 +6134,7 @@
         <v>763860.99999979907</v>
       </c>
       <c r="P3">
-        <v>469427.99999962631</v>
+        <v>432670.19999962609</v>
       </c>
       <c r="Q3">
         <v>0</v>
@@ -6822,13 +6246,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>480594.40000000002</v>
       </c>
       <c r="I2">
         <v>813860.99999979907</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -6846,7 +6270,7 @@
         <v>763860.99999979907</v>
       </c>
       <c r="P2">
-        <v>409927.99999981304</v>
+        <v>407756.29999981303</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -6858,7 +6282,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8309709.8290332528</v>
+        <v>8337877.6463992</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -6872,13 +6296,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>24300</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>24300</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -6887,13 +6311,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>483294.39999999991</v>
       </c>
       <c r="I3">
         <v>513861.00000000675</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -6911,7 +6335,7 @@
         <v>463861.00000000675</v>
       </c>
       <c r="P3">
-        <v>469427.99999962631</v>
+        <v>432670.19999962609</v>
       </c>
       <c r="Q3">
         <v>0</v>
@@ -7023,13 +6447,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>480594.40000000002</v>
       </c>
       <c r="I2">
         <v>613861.0000002078</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -7047,7 +6471,7 @@
         <v>563861.0000002078</v>
       </c>
       <c r="P2">
-        <v>409927.99999981304</v>
+        <v>407756.29999981303</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -7059,7 +6483,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8362018.0490332544</v>
+        <v>8381247.1163992044</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -7073,13 +6497,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>24300</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>24300</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -7088,13 +6512,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>483294.39999999991</v>
       </c>
       <c r="I3">
         <v>313861.00000041554</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -7112,7 +6536,7 @@
         <v>263861.00000041554</v>
       </c>
       <c r="P3">
-        <v>469427.99999962631</v>
+        <v>432670.19999962609</v>
       </c>
       <c r="Q3">
         <v>0</v>
@@ -7224,13 +6648,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>480594.40000000002</v>
       </c>
       <c r="I2">
         <v>613861.0000002078</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -7248,7 +6672,7 @@
         <v>563861.0000002078</v>
       </c>
       <c r="P2">
-        <v>409927.99999981304</v>
+        <v>407756.29999981303</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -7260,7 +6684,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8366599.0990332542</v>
+        <v>8383900.7663992029</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -7274,13 +6698,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>24300</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>24300</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -7289,13 +6713,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>483294.39999999991</v>
       </c>
       <c r="I3">
         <v>613861.00000020862</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -7313,7 +6737,7 @@
         <v>563861.00000020862</v>
       </c>
       <c r="P3">
-        <v>469427.99999962631</v>
+        <v>432670.19999962609</v>
       </c>
       <c r="Q3">
         <v>0</v>
@@ -7425,13 +6849,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>480594.40000000002</v>
       </c>
       <c r="I2">
         <v>1183860.999999813</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -7449,7 +6873,7 @@
         <v>1133860.999999813</v>
       </c>
       <c r="P2">
-        <v>409927.99999981304</v>
+        <v>407756.29999981303</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -7461,7 +6885,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8500385.8210332524</v>
+        <v>8503526.7163992003</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -7490,13 +6914,13 @@
         <v>0</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>483294.39999999991</v>
       </c>
       <c r="I3">
         <v>1453860.9999996261</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -7514,19 +6938,19 @@
         <v>1403860.9999996261</v>
       </c>
       <c r="P3">
-        <v>477427.99999962613</v>
+        <v>440670.19999962603</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>13624090.298644044</v>
+        <v>13207358.43426156</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>13915397.500644045</v>
+        <v>13498665.636261562</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -7626,13 +7050,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>480594.40000000002</v>
       </c>
       <c r="I2">
         <v>1183860.999999813</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -7650,7 +7074,7 @@
         <v>1133860.999999813</v>
       </c>
       <c r="P2">
-        <v>409927.99999981304</v>
+        <v>407756.29999981303</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -7662,7 +7086,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8472835.3090332542</v>
+        <v>8478668.2483992018</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -7691,13 +7115,13 @@
         <v>0</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>483294.39999999991</v>
       </c>
       <c r="I3">
         <v>1083860.9999996119</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -7715,19 +7139,19 @@
         <v>1033860.9999996119</v>
       </c>
       <c r="P3">
-        <v>477427.99999962613</v>
+        <v>440670.19999962603</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>10415454.195548035</v>
+        <v>11252641.823397283</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>10640357.527548036</v>
+        <v>11477545.155397281</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -7827,13 +7251,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>480594.40000000002</v>
       </c>
       <c r="I2">
         <v>813860.99999979907</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -7851,7 +7275,7 @@
         <v>763860.99999979907</v>
       </c>
       <c r="P2">
-        <v>409927.99999981304</v>
+        <v>407756.29999981303</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -7863,7 +7287,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8412722.4750332516</v>
+        <v>8414700.9843992013</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -7877,13 +7301,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>24300</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>24300</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -7892,13 +7316,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>483294.39999999991</v>
       </c>
       <c r="I3">
         <v>1093860.9999996321</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -7916,19 +7340,19 @@
         <v>1043860.9999996321</v>
       </c>
       <c r="P3">
-        <v>469427.99999962631</v>
+        <v>432670.19999962609</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>12352353.423652945</v>
+        <v>12852219.990416728</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>12500386.051652946</v>
+        <v>13000252.618416728</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -8028,13 +7452,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>480594.40000000002</v>
       </c>
       <c r="I2">
         <v>1183860.999999813</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -8052,7 +7476,7 @@
         <v>1133860.999999813</v>
       </c>
       <c r="P2">
-        <v>409927.99999981304</v>
+        <v>407756.29999981303</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -8064,7 +7488,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8365797.7570332531</v>
+        <v>8365005.4803992016</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -8078,13 +7502,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>24300</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>24300</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -8093,13 +7517,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>483294.39999999991</v>
       </c>
       <c r="I3">
         <v>1083860.9999996119</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -8117,19 +7541,19 @@
         <v>1033860.9999996119</v>
       </c>
       <c r="P3">
-        <v>469427.99999962631</v>
+        <v>432670.19999962609</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>11031228.415133042</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>11219086.211133042</v>
+        <v>9187857.7959775534</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -8229,13 +7653,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>480594.40000000002</v>
       </c>
       <c r="I2">
         <v>813860.99999979907</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -8253,7 +7677,7 @@
         <v>763860.99999979907</v>
       </c>
       <c r="P2">
-        <v>409927.99999981304</v>
+        <v>407756.29999981303</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -8265,7 +7689,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8416761.01103325</v>
+        <v>8417607.2963992003</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -8279,13 +7703,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>24300</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>24300</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -8294,13 +7718,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>483294.39999999991</v>
       </c>
       <c r="I3">
         <v>513861.00000000675</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -8318,19 +7742,19 @@
         <v>463861.00000000675</v>
       </c>
       <c r="P3">
-        <v>469427.99999962631</v>
+        <v>432670.19999962609</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8229999.9999991106</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>8417833.5499991123</v>
+        <v>9187833.549977554</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -8430,13 +7854,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>480594.40000000002</v>
       </c>
       <c r="I2">
         <v>613861.0000002078</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -8454,7 +7878,7 @@
         <v>563861.0000002078</v>
       </c>
       <c r="P2">
-        <v>409927.99999981304</v>
+        <v>407756.29999981303</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -8466,7 +7890,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8394107.3810332529</v>
+        <v>8397424.9303992018</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -8480,13 +7904,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>24300</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>24300</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -8495,13 +7919,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>483294.39999999991</v>
       </c>
       <c r="I3">
         <v>513861.00000000687</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -8519,7 +7943,7 @@
         <v>463861.00000000681</v>
       </c>
       <c r="P3">
-        <v>469427.99999962631</v>
+        <v>432670.19999962609</v>
       </c>
       <c r="Q3">
         <v>0</v>

</xml_diff>

<commit_message>
Ruleset: Updated Mexico Accounting Adjustment to incorporate outyear shortage schedule logic, CA Diversion logic updated to fire correctly in January, Mx Accounting updated with proper execution constraints, NV ICS Delivery updated to allow SNWA to take all DCP ICS in flood control, MWD ICS Creation and Delivery updated to allow MWD to take up to their Normal Operational Maximum in non-surplus conditions, SNWA surplus ICS delivery and entitlement rules updated per SNWA guidance
Model file: MWD_NormalOpMax and SNWA Quantified and FC Entitlement slots added, GreenBelowFlamingGorge:FlowAtJensen method updated, CAP FC and SNWA Quanitifed and FC Entitlements removed from initialization ruleset
</commit_message>
<xml_diff>
--- a/Output Data/MtomToCrss_Annual.xlsx
+++ b/Output Data/MtomToCrss_Annual.xlsx
@@ -6,51 +6,49 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Trace1" sheetId="1" r:id="rId2"/>
-    <sheet name="Trace2" sheetId="2" r:id="rId4"/>
-    <sheet name="Trace3" sheetId="3" r:id="rId5"/>
-    <sheet name="Trace4" sheetId="4" r:id="rId6"/>
-    <sheet name="Trace5" sheetId="5" r:id="rId7"/>
-    <sheet name="Trace6" sheetId="6" r:id="rId8"/>
-    <sheet name="Trace7" sheetId="7" r:id="rId9"/>
-    <sheet name="Trace8" sheetId="8" r:id="rId10"/>
-    <sheet name="Trace9" sheetId="9" r:id="rId11"/>
-    <sheet name="Trace10" sheetId="10" r:id="rId12"/>
-    <sheet name="Trace11" sheetId="11" r:id="rId13"/>
-    <sheet name="Trace12" sheetId="12" r:id="rId14"/>
-    <sheet name="Trace13" sheetId="13" r:id="rId15"/>
-    <sheet name="Trace14" sheetId="14" r:id="rId16"/>
-    <sheet name="Trace15" sheetId="15" r:id="rId17"/>
-    <sheet name="Trace16" sheetId="16" r:id="rId18"/>
-    <sheet name="Trace17" sheetId="17" r:id="rId19"/>
-    <sheet name="Trace18" sheetId="18" r:id="rId20"/>
-    <sheet name="Trace19" sheetId="19" r:id="rId21"/>
-    <sheet name="Trace20" sheetId="20" r:id="rId22"/>
-    <sheet name="Trace21" sheetId="21" r:id="rId23"/>
-    <sheet name="Trace22" sheetId="22" r:id="rId24"/>
-    <sheet name="Trace23" sheetId="23" r:id="rId25"/>
-    <sheet name="Trace24" sheetId="24" r:id="rId26"/>
-    <sheet name="Trace25" sheetId="25" r:id="rId27"/>
-    <sheet name="Trace26" sheetId="26" r:id="rId28"/>
-    <sheet name="Trace27" sheetId="27" r:id="rId29"/>
-    <sheet name="Trace28" sheetId="28" r:id="rId30"/>
-    <sheet name="Trace29" sheetId="29" r:id="rId31"/>
-    <sheet name="Trace30" sheetId="30" r:id="rId32"/>
-    <sheet name="Trace31" sheetId="31" r:id="rId33"/>
-    <sheet name="Trace32" sheetId="32" r:id="rId34"/>
-    <sheet name="Trace33" sheetId="33" r:id="rId35"/>
-    <sheet name="Trace34" sheetId="34" r:id="rId36"/>
-    <sheet name="Trace35" sheetId="35" r:id="rId37"/>
-    <sheet name="Trace36" sheetId="36" r:id="rId38"/>
-    <sheet name="Trace37" sheetId="37" r:id="rId39"/>
-    <sheet name="Trace38" sheetId="38" r:id="rId40"/>
+    <sheet name="Trace3" sheetId="1" r:id="rId2"/>
+    <sheet name="Trace4" sheetId="2" r:id="rId4"/>
+    <sheet name="Trace5" sheetId="3" r:id="rId5"/>
+    <sheet name="Trace6" sheetId="4" r:id="rId6"/>
+    <sheet name="Trace7" sheetId="5" r:id="rId7"/>
+    <sheet name="Trace8" sheetId="6" r:id="rId8"/>
+    <sheet name="Trace9" sheetId="7" r:id="rId9"/>
+    <sheet name="Trace10" sheetId="8" r:id="rId10"/>
+    <sheet name="Trace11" sheetId="9" r:id="rId11"/>
+    <sheet name="Trace12" sheetId="10" r:id="rId12"/>
+    <sheet name="Trace13" sheetId="11" r:id="rId13"/>
+    <sheet name="Trace14" sheetId="12" r:id="rId14"/>
+    <sheet name="Trace15" sheetId="13" r:id="rId15"/>
+    <sheet name="Trace16" sheetId="14" r:id="rId16"/>
+    <sheet name="Trace17" sheetId="15" r:id="rId17"/>
+    <sheet name="Trace18" sheetId="16" r:id="rId18"/>
+    <sheet name="Trace19" sheetId="17" r:id="rId19"/>
+    <sheet name="Trace20" sheetId="18" r:id="rId20"/>
+    <sheet name="Trace21" sheetId="19" r:id="rId21"/>
+    <sheet name="Trace22" sheetId="20" r:id="rId22"/>
+    <sheet name="Trace23" sheetId="21" r:id="rId23"/>
+    <sheet name="Trace24" sheetId="22" r:id="rId24"/>
+    <sheet name="Trace25" sheetId="23" r:id="rId25"/>
+    <sheet name="Trace26" sheetId="24" r:id="rId26"/>
+    <sheet name="Trace27" sheetId="25" r:id="rId27"/>
+    <sheet name="Trace28" sheetId="26" r:id="rId28"/>
+    <sheet name="Trace29" sheetId="27" r:id="rId29"/>
+    <sheet name="Trace30" sheetId="28" r:id="rId30"/>
+    <sheet name="Trace31" sheetId="29" r:id="rId31"/>
+    <sheet name="Trace32" sheetId="30" r:id="rId32"/>
+    <sheet name="Trace33" sheetId="31" r:id="rId33"/>
+    <sheet name="Trace34" sheetId="32" r:id="rId34"/>
+    <sheet name="Trace35" sheetId="33" r:id="rId35"/>
+    <sheet name="Trace36" sheetId="34" r:id="rId36"/>
+    <sheet name="Trace37" sheetId="35" r:id="rId37"/>
+    <sheet name="Trace38" sheetId="36" r:id="rId38"/>
   </sheets>
   <calcPr calcId="125725" fullCalcOnLoad="true"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:xdr="http://purl.oclc.org/ooxml/drawingml/spreadsheetDrawing" count="760" uniqueCount="20">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:xdr="http://purl.oclc.org/ooxml/drawingml/spreadsheetDrawing" count="720" uniqueCount="20">
   <si>
     <t>DCP BWSCP Flags.LB DCP BWSP</t>
   </si>
@@ -134,7 +132,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="267">
+  <borders count="253">
     <border>
       <start/>
       <end/>
@@ -394,25 +392,11 @@
     <border/>
     <border/>
     <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="267">
+  <cellXfs count="253">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -738,24 +722,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="252" xfId="0" applyNumberFormat="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="253" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="254" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="255" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="256" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="257" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="258" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="259" xfId="0" applyNumberFormat="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="260" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="261" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="262" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="263" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="264" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="265" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="266" xfId="0" applyNumberFormat="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -853,13 +819,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>480594.40000000002</v>
       </c>
       <c r="I2">
-        <v>1095844.5999999999</v>
+        <v>925054.30000000005</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -874,22 +840,22 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1045844.6</v>
+        <v>875054.29999999993</v>
       </c>
       <c r="P2">
-        <v>409927.99999981304</v>
+        <v>407756.29999981303</v>
       </c>
       <c r="Q2">
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8358843.7387190023</v>
+        <v>8424446.4063992016</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -903,13 +869,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>29999.999699999997</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>29999.999699999997</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -918,13 +884,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>483294.39999999991</v>
       </c>
       <c r="I3">
-        <v>1259360.2</v>
+        <v>1088569.8999999999</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -939,22 +905,22 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1209360.2</v>
+        <v>1038569.8999999999</v>
       </c>
       <c r="P3">
-        <v>469427.99999962631</v>
+        <v>432670.19999962609</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8803567.5082156733</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>8938070.5082156751</v>
+        <v>9157545.9999775533</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -1054,13 +1020,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>480594.40000000002</v>
       </c>
       <c r="I2">
         <v>813860.99999979907</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -1078,19 +1044,19 @@
         <v>763860.99999979907</v>
       </c>
       <c r="P2">
-        <v>409927.99999981304</v>
+        <v>407756.29999981303</v>
       </c>
       <c r="Q2">
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8409636.2467190046</v>
+        <v>8376056.7183992025</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -1104,13 +1070,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>29999.999699999997</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>29999.999699999997</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -1119,13 +1085,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>483294.39999999991</v>
       </c>
       <c r="I3">
-        <v>513861.00000000675</v>
+        <v>732930.80000053381</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -1140,22 +1106,22 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>463861.00000000675</v>
+        <v>682930.80000053381</v>
       </c>
       <c r="P3">
-        <v>469427.99999962631</v>
+        <v>432670.19999962609</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8229999.9999991106</v>
+        <v>8513764.6899629459</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>8417833.5499991123</v>
+        <v>8650258.1159629468</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -1255,13 +1221,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>480594.40000000002</v>
       </c>
       <c r="I2">
         <v>613861.0000002078</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -1279,19 +1245,19 @@
         <v>563861.0000002078</v>
       </c>
       <c r="P2">
-        <v>409927.99999981304</v>
+        <v>407756.29999981303</v>
       </c>
       <c r="Q2">
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8397003.0547190029</v>
+        <v>8385843.4903992014</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -1305,13 +1271,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>29999.999699999997</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>29999.999699999997</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -1320,13 +1286,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>483294.39999999991</v>
       </c>
       <c r="I3">
-        <v>513861.00000000687</v>
+        <v>342812.00000094209</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -1341,22 +1307,22 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>463861.00000000681</v>
+        <v>292812.00000094209</v>
       </c>
       <c r="P3">
-        <v>469427.99999962631</v>
+        <v>432670.19999962609</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8229999.9999991106</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>8380597.6699991105</v>
+        <v>9174589.2299775518</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -1456,13 +1422,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>480594.40000000002</v>
       </c>
       <c r="I2">
-        <v>813860.99999979907</v>
+        <v>613861.0000002078</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -1477,22 +1443,22 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>763860.99999979907</v>
+        <v>563861.0000002078</v>
       </c>
       <c r="P2">
-        <v>409927.99999981304</v>
+        <v>407756.29999981303</v>
       </c>
       <c r="Q2">
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8375492.4787190035</v>
+        <v>8424399.204399202</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -1506,13 +1472,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>29999.999699999997</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>29999.999699999997</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -1521,13 +1487,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>483294.39999999991</v>
       </c>
       <c r="I3">
-        <v>813860.99999979942</v>
+        <v>342812.00000094209</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -1542,22 +1508,22 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>763860.99999979942</v>
+        <v>292812.00000094209</v>
       </c>
       <c r="P3">
-        <v>469427.99999962631</v>
+        <v>432670.19999962609</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8229999.9999991106</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>8366493.4259991096</v>
+        <v>9239478.9159775525</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -1657,13 +1623,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>480594.40000000002</v>
       </c>
       <c r="I2">
-        <v>906235.80000430183</v>
+        <v>613861.0000002078</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -1678,22 +1644,22 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>856235.80000430183</v>
+        <v>563861.0000002078</v>
       </c>
       <c r="P2">
-        <v>409927.99999981304</v>
+        <v>407756.29999981303</v>
       </c>
       <c r="Q2">
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8372260.720719004</v>
+        <v>8462825.0763992034</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -1707,13 +1673,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>29999.999699999997</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>29999.999699999997</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -1722,13 +1688,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>483294.39999999991</v>
       </c>
       <c r="I3">
-        <v>606235.80000450963</v>
+        <v>763861.00000010396</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -1743,22 +1709,22 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>556235.80000450963</v>
+        <v>713861.00000010396</v>
       </c>
       <c r="P3">
-        <v>469427.99999962631</v>
+        <v>432670.19999962609</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8999999.9999775533</v>
+        <v>9882374.4327692855</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>9174589.2299775518</v>
+        <v>10292192.656769285</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -1858,13 +1824,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>480594.40000000002</v>
       </c>
       <c r="I2">
-        <v>613861.0000002078</v>
+        <v>1048860.9999999066</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -1879,22 +1845,22 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>563861.0000002078</v>
+        <v>998860.99999990652</v>
       </c>
       <c r="P2">
-        <v>409927.99999981304</v>
+        <v>407756.29999981303</v>
       </c>
       <c r="Q2">
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8421841.4287190046</v>
+        <v>8483697.6143992003</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -1905,31 +1871,31 @@
         <v>44197</v>
       </c>
       <c r="B3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3">
-        <v>29999.999699999997</v>
+        <v>0</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>29999.999699999997</v>
+        <v>0</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>7999.9999999998645</v>
+        <v>0</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>483294.39999999991</v>
       </c>
       <c r="I3">
-        <v>313861.00000041554</v>
+        <v>757672.60000064119</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -1944,22 +1910,22 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>263861.00000041554</v>
+        <v>707672.60000064108</v>
       </c>
       <c r="P3">
-        <v>469427.99999962631</v>
+        <v>440670.19999962603</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8229999.9999991106</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>8469478.9159991127</v>
+        <v>9132878.8059775531</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -2059,13 +2025,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>480594.40000000002</v>
       </c>
       <c r="I2">
         <v>613861.0000002078</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -2083,19 +2049,19 @@
         <v>563861.0000002078</v>
       </c>
       <c r="P2">
-        <v>409927.99999981304</v>
+        <v>407756.29999981303</v>
       </c>
       <c r="Q2">
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8470374.482719006</v>
+        <v>8371518.346399202</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -2106,31 +2072,31 @@
         <v>44197</v>
       </c>
       <c r="B3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>483294.39999999991</v>
       </c>
       <c r="I3">
-        <v>763861.00000010396</v>
+        <v>913861</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -2145,22 +2111,22 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>713861.00000010396</v>
+        <v>863861</v>
       </c>
       <c r="P3">
-        <v>488482.60999962612</v>
+        <v>432670.19999962609</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>9064960.2924137004</v>
+        <v>10765571.96773139</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>9474778.5164136998</v>
+        <v>11047992.27173139</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -2260,13 +2226,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>480594.40000000002</v>
       </c>
       <c r="I2">
-        <v>1048860.9999999066</v>
+        <v>1183860.999999813</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -2281,22 +2247,22 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>998860.99999990652</v>
+        <v>1133860.999999813</v>
       </c>
       <c r="P2">
-        <v>409927.99999981304</v>
+        <v>407756.29999981303</v>
       </c>
       <c r="Q2">
         <v>0</v>
       </c>
       <c r="R2">
-        <v>9504058.8189741056</v>
+        <v>9859718.0564116705</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>9896440.5136931129</v>
+        <v>10112616.788810877</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -2325,13 +2291,13 @@
         <v>0</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>483294.39999999991</v>
       </c>
       <c r="I3">
-        <v>748861.00000011432</v>
+        <v>1453860.9999996261</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -2346,22 +2312,22 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>698861.00000011432</v>
+        <v>1403860.9999996261</v>
       </c>
       <c r="P3">
-        <v>477427.99999962613</v>
+        <v>427122.94999960525</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>9180669.6271031033</v>
+        <v>11200311.196348004</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>9313548.4331031032</v>
+        <v>11328829.928348003</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -2461,13 +2427,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>480594.40000000002</v>
       </c>
       <c r="I2">
-        <v>613861.0000002078</v>
+        <v>1183860.999999813</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -2482,22 +2448,22 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>563861.0000002078</v>
+        <v>1133860.999999813</v>
       </c>
       <c r="P2">
-        <v>409927.99999981304</v>
+        <v>407756.29999981303</v>
       </c>
       <c r="Q2">
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8362031.5187190045</v>
+        <v>8365609.4083992019</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -2511,13 +2477,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>29999.999699999997</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>29999.999699999997</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -2526,13 +2492,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>483294.39999999991</v>
       </c>
       <c r="I3">
-        <v>913861</v>
+        <v>1453860.9999996261</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -2547,22 +2513,22 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>863861</v>
+        <v>1403860.9999996261</v>
       </c>
       <c r="P3">
-        <v>469427.99999962631</v>
+        <v>432670.19999962609</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>10522899.815068083</v>
+        <v>11178103.423867302</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>10805320.119068084</v>
+        <v>11239775.109867303</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -2662,13 +2628,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>480594.40000000002</v>
       </c>
       <c r="I2">
         <v>1183860.999999813</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -2686,19 +2652,19 @@
         <v>1133860.999999813</v>
       </c>
       <c r="P2">
-        <v>409927.99999981304</v>
+        <v>407756.29999981303</v>
       </c>
       <c r="Q2">
         <v>0</v>
       </c>
       <c r="R2">
-        <v>10974646.714388685</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>11258268.479107693</v>
+        <v>8327496.5563992029</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -2709,31 +2675,31 @@
         <v>44197</v>
       </c>
       <c r="B3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>483294.39999999991</v>
       </c>
       <c r="I3">
         <v>1453860.9999996261</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -2751,19 +2717,19 @@
         <v>1403860.9999996261</v>
       </c>
       <c r="P3">
-        <v>466373.38999962609</v>
+        <v>432670.19999962609</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>12125874.640943892</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>12254393.372943891</v>
+        <v>8140372.5099991113</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -2863,13 +2829,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>480594.40000000002</v>
       </c>
       <c r="I2">
         <v>1183860.999999813</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -2887,19 +2853,19 @@
         <v>1133860.999999813</v>
       </c>
       <c r="P2">
-        <v>409927.99999981304</v>
+        <v>407756.29999981303</v>
       </c>
       <c r="Q2">
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8349355.0567190023</v>
+        <v>8272618.386399202</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -2910,31 +2876,31 @@
         <v>44197</v>
       </c>
       <c r="B3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3">
-        <v>29999.999699999997</v>
+        <v>0</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>29999.999699999997</v>
+        <v>0</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>7999.9999999998645</v>
+        <v>0</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>483294.39999999991</v>
       </c>
       <c r="I3">
         <v>1453860.9999996261</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -2952,19 +2918,19 @@
         <v>1403860.9999996261</v>
       </c>
       <c r="P3">
-        <v>469427.99999962631</v>
+        <v>440670.19999962603</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>13712432.070248161</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>13774103.756248161</v>
+        <v>8433484.9599991105</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -3064,13 +3030,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>480594.40000000002</v>
       </c>
       <c r="I2">
-        <v>1095844.5999999999</v>
+        <v>813860.99999979907</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -3085,22 +3051,22 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1045844.6</v>
+        <v>763860.99999979907</v>
       </c>
       <c r="P2">
-        <v>409927.99999981304</v>
+        <v>407756.29999981303</v>
       </c>
       <c r="Q2">
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8383578.7387190033</v>
+        <v>8389944.5143992007</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -3114,13 +3080,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>29999.999699999997</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>29999.999699999997</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -3129,13 +3095,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>483294.39999999991</v>
       </c>
       <c r="I3">
-        <v>1259360.2</v>
+        <v>1093860.9999996321</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -3150,22 +3116,22 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1209360.2</v>
+        <v>1043860.9999996321</v>
       </c>
       <c r="P3">
-        <v>469427.99999962631</v>
+        <v>432670.19999962609</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>11817853.32527641</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>11963177.325276406</v>
+        <v>8440604.3459991124</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -3265,13 +3231,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>480594.40000000002</v>
       </c>
       <c r="I2">
         <v>1183860.999999813</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -3289,19 +3255,19 @@
         <v>1133860.999999813</v>
       </c>
       <c r="P2">
-        <v>409927.99999981304</v>
+        <v>407756.29999981303</v>
       </c>
       <c r="Q2">
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8299587.0507190032</v>
+        <v>8439292.2963992022</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -3315,13 +3281,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>29999.999699999997</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>29999.999699999997</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -3330,13 +3296,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>483294.39999999991</v>
       </c>
       <c r="I3">
-        <v>1453860.9999996261</v>
+        <v>1318860.9999997194</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -3351,22 +3317,22 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1403860.9999996261</v>
+        <v>1268860.9999997194</v>
       </c>
       <c r="P3">
-        <v>469427.99999962631</v>
+        <v>432670.19999962609</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>11048656.323729711</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>10959028.83372971</v>
+        <v>9140628.0299775563</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -3466,13 +3432,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>480594.40000000002</v>
       </c>
       <c r="I2">
-        <v>1183860.999999813</v>
+        <v>1048860.9999999066</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -3487,22 +3453,22 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1133860.999999813</v>
+        <v>998860.99999990652</v>
       </c>
       <c r="P2">
-        <v>409927.99999981304</v>
+        <v>407756.29999981303</v>
       </c>
       <c r="Q2">
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8211874.9087190032</v>
+        <v>8424551.2063992042</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -3516,13 +3482,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>29999.999699999997</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>29999.999699999997</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -3531,13 +3497,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>483294.39999999991</v>
       </c>
       <c r="I3">
-        <v>1453860.9999996263</v>
+        <v>948860.99999970547</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -3552,22 +3518,22 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1403860.9999996263</v>
+        <v>898860.99999970547</v>
       </c>
       <c r="P3">
-        <v>469427.99999962631</v>
+        <v>432670.19999962609</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8229999.9999991106</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>8433484.9599991105</v>
+        <v>9105477.679977553</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -3667,13 +3633,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>480594.40000000002</v>
       </c>
       <c r="I2">
-        <v>1183860.999999813</v>
+        <v>813860.99999979907</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -3688,22 +3654,22 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1133860.999999813</v>
+        <v>763860.99999979907</v>
       </c>
       <c r="P2">
-        <v>409927.99999981304</v>
+        <v>407756.29999981303</v>
       </c>
       <c r="Q2">
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8417253.2987190038</v>
+        <v>8365071.6863992019</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -3717,13 +3683,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>29999.999699999997</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>29999.999699999997</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -3732,13 +3698,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>483294.39999999991</v>
       </c>
       <c r="I3">
-        <v>1318860.9999997194</v>
+        <v>713860.99999959802</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -3753,22 +3719,22 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1268860.9999997194</v>
+        <v>663860.99999959802</v>
       </c>
       <c r="P3">
-        <v>469427.99999962631</v>
+        <v>432670.19999962609</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8999999.9999775533</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>9140628.0299775563</v>
+        <v>8338713.64999911</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -3868,13 +3834,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>480594.40000000002</v>
       </c>
       <c r="I2">
-        <v>1048860.9999999066</v>
+        <v>813860.99999979907</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -3889,22 +3855,22 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>998860.99999990652</v>
+        <v>763860.99999979907</v>
       </c>
       <c r="P2">
-        <v>409927.99999981304</v>
+        <v>407756.29999981303</v>
       </c>
       <c r="Q2">
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8393312.2387190033</v>
+        <v>8398877.5363992024</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -3918,13 +3884,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>29999.999699999997</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>29999.999699999997</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -3933,13 +3899,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>483294.39999999991</v>
       </c>
       <c r="I3">
-        <v>948860.99999970547</v>
+        <v>958860.99999972573</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -3954,10 +3920,10 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>898860.99999970547</v>
+        <v>908860.99999972573</v>
       </c>
       <c r="P3">
-        <v>469427.99999962631</v>
+        <v>432670.19999962609</v>
       </c>
       <c r="Q3">
         <v>0</v>
@@ -3969,7 +3935,7 @@
         <v>1</v>
       </c>
       <c r="T3">
-        <v>9105477.679977553</v>
+        <v>9131647.4399775527</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -4069,13 +4035,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>480594.40000000002</v>
       </c>
       <c r="I2">
-        <v>813860.99999979907</v>
+        <v>1048860.9999999066</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -4090,22 +4056,22 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>763860.99999979907</v>
+        <v>998860.99999990652</v>
       </c>
       <c r="P2">
-        <v>409927.99999981304</v>
+        <v>407756.29999981303</v>
       </c>
       <c r="Q2">
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8336194.6387190036</v>
+        <v>8397946.9563992023</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -4119,13 +4085,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>29999.999699999997</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>29999.999699999997</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -4134,13 +4100,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>483294.39999999991</v>
       </c>
       <c r="I3">
-        <v>713860.99999959802</v>
+        <v>1048860.9999999066</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -4155,22 +4121,22 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>663860.99999959802</v>
+        <v>998860.99999990652</v>
       </c>
       <c r="P3">
-        <v>469427.99999962631</v>
+        <v>432670.19999962609</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8229999.9999991106</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>8338713.64999911</v>
+        <v>9104398.0899775531</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -4270,13 +4236,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>480594.40000000002</v>
       </c>
       <c r="I2">
-        <v>813860.99999979907</v>
+        <v>913861</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -4291,22 +4257,22 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>763860.99999979907</v>
+        <v>863861</v>
       </c>
       <c r="P2">
-        <v>409927.99999981304</v>
+        <v>407756.29999981303</v>
       </c>
       <c r="Q2">
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8364080.2787190014</v>
+        <v>8348992.4763992019</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -4320,13 +4286,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>29999.999699999997</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>29999.999699999997</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -4335,13 +4301,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>483294.39999999991</v>
       </c>
       <c r="I3">
-        <v>958860.99999972573</v>
+        <v>1048860.9999999066</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -4356,22 +4322,22 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>908860.99999972573</v>
+        <v>998860.99999990652</v>
       </c>
       <c r="P3">
-        <v>469427.99999962631</v>
+        <v>432670.19999962609</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>7479999.9999999981</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="S3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T3">
-        <v>7611647.4399999948</v>
+        <v>8359167.7799991118</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -4471,13 +4437,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>480594.40000000002</v>
       </c>
       <c r="I2">
         <v>1048860.9999999066</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -4495,19 +4461,19 @@
         <v>998860.99999990652</v>
       </c>
       <c r="P2">
-        <v>409927.99999981304</v>
+        <v>407756.29999981303</v>
       </c>
       <c r="Q2">
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8379791.2487190031</v>
+        <v>8403214.0063992012</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -4518,31 +4484,31 @@
         <v>44197</v>
       </c>
       <c r="B3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3">
-        <v>29999.999699999997</v>
+        <v>0</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>29999.999699999997</v>
+        <v>0</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>7999.9999999998645</v>
+        <v>0</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>483294.39999999991</v>
       </c>
       <c r="I3">
-        <v>1048860.9999999066</v>
+        <v>1318860.9999997194</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -4557,22 +4523,22 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>998860.99999990652</v>
+        <v>1268860.9999997194</v>
       </c>
       <c r="P3">
-        <v>469427.99999962631</v>
+        <v>440670.19999962603</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8999999.9999775533</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>9104398.0899775531</v>
+        <v>8493906.2799991108</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -4672,13 +4638,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>480594.40000000002</v>
       </c>
       <c r="I2">
-        <v>913861</v>
+        <v>1183860.999999813</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -4693,22 +4659,22 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>863861</v>
+        <v>1133860.999999813</v>
       </c>
       <c r="P2">
-        <v>409927.99999981304</v>
+        <v>407756.29999981303</v>
       </c>
       <c r="Q2">
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8340939.9687190047</v>
+        <v>8461261.2163992021</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -4722,13 +4688,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>29999.999699999997</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>29999.999699999997</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -4737,13 +4703,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>483294.39999999991</v>
       </c>
       <c r="I3">
-        <v>1048860.9999999066</v>
+        <v>1083860.9999996119</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -4758,22 +4724,22 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>998860.99999990652</v>
+        <v>1033860.9999996119</v>
       </c>
       <c r="P3">
-        <v>469427.99999962631</v>
+        <v>432670.19999962609</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8229999.9999991106</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>8359167.7799991118</v>
+        <v>9166147.929977553</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -4873,13 +4839,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>480594.40000000002</v>
       </c>
       <c r="I2">
-        <v>1048860.9999999066</v>
+        <v>813860.99999979907</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -4894,22 +4860,22 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>998860.99999990652</v>
+        <v>763860.99999979907</v>
       </c>
       <c r="P2">
-        <v>409927.99999981304</v>
+        <v>407756.29999981303</v>
       </c>
       <c r="Q2">
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8384316.7387190042</v>
+        <v>8368555.8463992029</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -4920,31 +4886,31 @@
         <v>44197</v>
       </c>
       <c r="B3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>483294.39999999991</v>
       </c>
       <c r="I3">
-        <v>1318860.9999997194</v>
+        <v>542812.0000005333</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -4959,22 +4925,22 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1268860.9999997194</v>
+        <v>492812.0000005333</v>
       </c>
       <c r="P3">
-        <v>477427.99999962613</v>
+        <v>432670.19999962609</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8229999.9999991106</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>8493906.2799991108</v>
+        <v>9186027.3499775529</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -5074,13 +5040,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>480594.40000000002</v>
       </c>
       <c r="I2">
-        <v>1183860.999999813</v>
+        <v>613861.0000002078</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -5095,22 +5061,22 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1133860.999999813</v>
+        <v>563861.0000002078</v>
       </c>
       <c r="P2">
-        <v>409927.99999981304</v>
+        <v>407756.29999981303</v>
       </c>
       <c r="Q2">
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8469412.1487190034</v>
+        <v>8431872.3363992013</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -5124,13 +5090,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>29999.999699999997</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>29999.999699999997</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -5139,13 +5105,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>483294.39999999991</v>
       </c>
       <c r="I3">
-        <v>1083860.9999996119</v>
+        <v>513861.00000000687</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -5160,10 +5126,10 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1033860.9999996119</v>
+        <v>463861.00000000681</v>
       </c>
       <c r="P3">
-        <v>469427.99999962631</v>
+        <v>432670.19999962609</v>
       </c>
       <c r="Q3">
         <v>0</v>
@@ -5175,7 +5141,7 @@
         <v>1</v>
       </c>
       <c r="T3">
-        <v>9166147.929977553</v>
+        <v>9160152.0699775536</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -5275,13 +5241,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>480594.40000000002</v>
       </c>
       <c r="I2">
-        <v>1095844.5999999999</v>
+        <v>1183860.999999813</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -5296,22 +5262,22 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1045844.6</v>
+        <v>1133860.999999813</v>
       </c>
       <c r="P2">
-        <v>409927.99999981304</v>
+        <v>407756.29999981303</v>
       </c>
       <c r="Q2">
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8384705.7387190033</v>
+        <v>8433966.2863992024</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -5322,31 +5288,31 @@
         <v>44197</v>
       </c>
       <c r="B3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3">
-        <v>29999.999699999997</v>
+        <v>0</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>29999.999699999997</v>
+        <v>0</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>7999.9999999998645</v>
+        <v>0</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>483294.39999999991</v>
       </c>
       <c r="I3">
-        <v>1259360.2</v>
+        <v>1453860.9999996261</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -5361,22 +5327,22 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1209360.2</v>
+        <v>1403860.9999996261</v>
       </c>
       <c r="P3">
-        <v>469427.99999962631</v>
+        <v>453454.11499962612</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8999999.9999775533</v>
+        <v>11432128.04575788</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>9137627.9999775533</v>
+        <v>11705977.92775788</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -5476,13 +5442,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>480594.40000000002</v>
       </c>
       <c r="I2">
         <v>813860.99999979907</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -5500,19 +5466,19 @@
         <v>763860.99999979907</v>
       </c>
       <c r="P2">
-        <v>409927.99999981304</v>
+        <v>407756.29999981303</v>
       </c>
       <c r="Q2">
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8367320.2187190037</v>
+        <v>8394337.1663992014</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -5526,13 +5492,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>29999.999699999997</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>29999.999699999997</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -5541,13 +5507,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>483294.39999999991</v>
       </c>
       <c r="I3">
-        <v>513861.00000000675</v>
+        <v>813860.99999979907</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -5562,10 +5528,10 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>463861.00000000675</v>
+        <v>763860.99999979907</v>
       </c>
       <c r="P3">
-        <v>469427.99999962631</v>
+        <v>432670.19999962609</v>
       </c>
       <c r="Q3">
         <v>0</v>
@@ -5577,7 +5543,7 @@
         <v>1</v>
       </c>
       <c r="T3">
-        <v>9186027.3499775529</v>
+        <v>9183949.7199775539</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -5677,13 +5643,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>480594.40000000002</v>
       </c>
       <c r="I2">
-        <v>613861.0000002078</v>
+        <v>913861</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -5698,22 +5664,22 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>563861.0000002078</v>
+        <v>863861</v>
       </c>
       <c r="P2">
-        <v>409927.99999981304</v>
+        <v>407756.29999981303</v>
       </c>
       <c r="Q2">
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8416174.1587190032</v>
+        <v>8401100.6163992025</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -5727,13 +5693,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>29999.999699999997</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>29999.999699999997</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -5742,13 +5708,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>483294.39999999991</v>
       </c>
       <c r="I3">
-        <v>513861.00000000687</v>
+        <v>1183860.999999813</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -5763,22 +5729,22 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>463861.00000000681</v>
+        <v>1133860.999999813</v>
       </c>
       <c r="P3">
-        <v>469427.99999962631</v>
+        <v>432670.19999962609</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8999999.9999775533</v>
+        <v>11383296.242107842</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>9160152.0699775536</v>
+        <v>11595991.252107842</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -5878,13 +5844,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>480594.40000000002</v>
       </c>
       <c r="I2">
-        <v>813860.99999979907</v>
+        <v>1183860.999999813</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -5899,22 +5865,22 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>763860.99999979907</v>
+        <v>1133860.999999813</v>
       </c>
       <c r="P2">
-        <v>409927.99999981304</v>
+        <v>407756.29999981303</v>
       </c>
       <c r="Q2">
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8385742.9387190016</v>
+        <v>8448059.6863992009</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -5928,13 +5894,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>29999.999699999997</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>29999.999699999997</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -5943,13 +5909,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>483294.39999999991</v>
       </c>
       <c r="I3">
-        <v>813860.99999979907</v>
+        <v>1183860.999999813</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -5964,10 +5930,10 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>763860.99999979907</v>
+        <v>1133860.999999813</v>
       </c>
       <c r="P3">
-        <v>469427.99999962631</v>
+        <v>432670.19999962609</v>
       </c>
       <c r="Q3">
         <v>0</v>
@@ -5979,7 +5945,7 @@
         <v>1</v>
       </c>
       <c r="T3">
-        <v>9183949.7199775539</v>
+        <v>9061125.7399775553</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -6079,13 +6045,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>480594.40000000002</v>
       </c>
       <c r="I2">
         <v>913861</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -6103,19 +6069,19 @@
         <v>863861</v>
       </c>
       <c r="P2">
-        <v>409927.99999981304</v>
+        <v>407756.29999981303</v>
       </c>
       <c r="Q2">
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8400896.6387190055</v>
+        <v>8337828.3263992034</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -6129,13 +6095,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>29999.999699999997</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>29999.999699999997</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -6144,13 +6110,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>483294.39999999991</v>
       </c>
       <c r="I3">
-        <v>1183860.999999813</v>
+        <v>813860.99999979907</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -6165,22 +6131,22 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1133860.999999813</v>
+        <v>763860.99999979907</v>
       </c>
       <c r="P3">
-        <v>469427.99999962631</v>
+        <v>432670.19999962609</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>11750117.627780363</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>11962812.637780361</v>
+        <v>8261744.7299991101</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -6280,13 +6246,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>480594.40000000002</v>
       </c>
       <c r="I2">
-        <v>1183860.999999813</v>
+        <v>813860.99999979907</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -6301,22 +6267,22 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1133860.999999813</v>
+        <v>763860.99999979907</v>
       </c>
       <c r="P2">
-        <v>409927.99999981304</v>
+        <v>407756.29999981303</v>
       </c>
       <c r="Q2">
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8435909.918719003</v>
+        <v>8337877.6463992</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -6330,13 +6296,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>29999.999699999997</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>29999.999699999997</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -6345,13 +6311,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>483294.39999999991</v>
       </c>
       <c r="I3">
-        <v>1183860.999999813</v>
+        <v>542812.0000005333</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -6366,10 +6332,10 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1133860.999999813</v>
+        <v>492812.0000005333</v>
       </c>
       <c r="P3">
-        <v>469427.99999962631</v>
+        <v>432670.19999962609</v>
       </c>
       <c r="Q3">
         <v>0</v>
@@ -6381,7 +6347,7 @@
         <v>1</v>
       </c>
       <c r="T3">
-        <v>9061125.7399775553</v>
+        <v>9088058.5399775542</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -6481,13 +6447,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>480594.40000000002</v>
       </c>
       <c r="I2">
-        <v>913861</v>
+        <v>613861.0000002078</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -6502,22 +6468,22 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>863861</v>
+        <v>563861.0000002078</v>
       </c>
       <c r="P2">
-        <v>409927.99999981304</v>
+        <v>407756.29999981303</v>
       </c>
       <c r="Q2">
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8295598.118719005</v>
+        <v>8381247.1163992044</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -6531,13 +6497,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>29999.999699999997</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>29999.999699999997</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -6546,13 +6512,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>483294.39999999991</v>
       </c>
       <c r="I3">
-        <v>813860.99999979907</v>
+        <v>342812.00000094209</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -6567,22 +6533,22 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>763860.99999979907</v>
+        <v>292812.00000094209</v>
       </c>
       <c r="P3">
-        <v>469427.99999962631</v>
+        <v>432670.19999962609</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8229999.9999991106</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>8261744.7299991101</v>
+        <v>9135931.8499775529</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -6682,13 +6648,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>480594.40000000002</v>
       </c>
       <c r="I2">
-        <v>813860.99999979907</v>
+        <v>613861.0000002078</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -6703,22 +6669,22 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>763860.99999979907</v>
+        <v>563861.0000002078</v>
       </c>
       <c r="P2">
-        <v>409927.99999981304</v>
+        <v>407756.29999981303</v>
       </c>
       <c r="Q2">
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8295114.0687190033</v>
+        <v>8383900.7663992029</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -6732,13 +6698,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>29999.999699999997</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>29999.999699999997</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -6747,13 +6713,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>483294.39999999991</v>
       </c>
       <c r="I3">
-        <v>513861.00000000675</v>
+        <v>532930.80000094266</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -6768,10 +6734,10 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>463861.00000000675</v>
+        <v>482930.8000009426</v>
       </c>
       <c r="P3">
-        <v>469427.99999962631</v>
+        <v>432670.19999962609</v>
       </c>
       <c r="Q3">
         <v>0</v>
@@ -6783,409 +6749,7 @@
         <v>1</v>
       </c>
       <c r="T3">
-        <v>9088058.5399775542</v>
-      </c>
-      <c r="U3">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:xdr="http://purl.oclc.org/ooxml/drawingml/spreadsheetDrawing">
-  <dimension ref="A1:U3"/>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="B1" s="259" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="259" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="259" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="259" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="259" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="259" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="259" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="259" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="259" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="259" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="259" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="259" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="259" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="259" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" s="259" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="259" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" s="259" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" s="259" t="s">
-        <v>17</v>
-      </c>
-      <c r="T1" s="259" t="s">
-        <v>18</v>
-      </c>
-      <c r="U1" s="259" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="257">
-        <v>43831</v>
-      </c>
-      <c r="B2">
-        <v>7</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>480594.69699999999</v>
-      </c>
-      <c r="I2">
-        <v>613861.0000002078</v>
-      </c>
-      <c r="J2">
-        <v>285431.99699999997</v>
-      </c>
-      <c r="K2">
-        <v>9009.3999999999996</v>
-      </c>
-      <c r="L2">
-        <v>180000</v>
-      </c>
-      <c r="M2">
-        <v>50000</v>
-      </c>
-      <c r="N2">
-        <v>6153.3000000000002</v>
-      </c>
-      <c r="O2">
-        <v>563861.0000002078</v>
-      </c>
-      <c r="P2">
-        <v>409927.99999981304</v>
-      </c>
-      <c r="Q2">
-        <v>0</v>
-      </c>
-      <c r="R2">
-        <v>8229999.9999999953</v>
-      </c>
-      <c r="S2">
-        <v>1</v>
-      </c>
-      <c r="T2">
-        <v>8357855.8587190043</v>
-      </c>
-      <c r="U2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="257">
-        <v>44197</v>
-      </c>
-      <c r="B3">
-        <v>7</v>
-      </c>
-      <c r="C3">
-        <v>29999.999699999997</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>29999.999699999997</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>7999.9999999998645</v>
-      </c>
-      <c r="H3">
-        <v>483294.69699999993</v>
-      </c>
-      <c r="I3">
-        <v>313861.00000041554</v>
-      </c>
-      <c r="J3">
-        <v>285431.99699999997</v>
-      </c>
-      <c r="K3">
-        <v>11709.4</v>
-      </c>
-      <c r="L3">
-        <v>180000</v>
-      </c>
-      <c r="M3">
-        <v>50000</v>
-      </c>
-      <c r="N3">
-        <v>6153.3000000000002</v>
-      </c>
-      <c r="O3">
-        <v>263861.00000041554</v>
-      </c>
-      <c r="P3">
-        <v>469427.99999962631</v>
-      </c>
-      <c r="Q3">
-        <v>0</v>
-      </c>
-      <c r="R3">
-        <v>8999999.9999775533</v>
-      </c>
-      <c r="S3">
-        <v>1</v>
-      </c>
-      <c r="T3">
-        <v>9135931.8499775529</v>
-      </c>
-      <c r="U3">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:xdr="http://purl.oclc.org/ooxml/drawingml/spreadsheetDrawing">
-  <dimension ref="A1:U3"/>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="B1" s="266" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="266" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="266" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="266" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="266" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="266" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="266" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="266" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="266" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="266" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="266" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="266" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="266" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="266" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" s="266" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="266" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" s="266" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" s="266" t="s">
-        <v>17</v>
-      </c>
-      <c r="T1" s="266" t="s">
-        <v>18</v>
-      </c>
-      <c r="U1" s="266" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="264">
-        <v>43831</v>
-      </c>
-      <c r="B2">
-        <v>7</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>480594.69699999999</v>
-      </c>
-      <c r="I2">
-        <v>613861.0000002078</v>
-      </c>
-      <c r="J2">
-        <v>285431.99699999997</v>
-      </c>
-      <c r="K2">
-        <v>9009.3999999999996</v>
-      </c>
-      <c r="L2">
-        <v>180000</v>
-      </c>
-      <c r="M2">
-        <v>50000</v>
-      </c>
-      <c r="N2">
-        <v>6153.3000000000002</v>
-      </c>
-      <c r="O2">
-        <v>563861.0000002078</v>
-      </c>
-      <c r="P2">
-        <v>409927.99999981304</v>
-      </c>
-      <c r="Q2">
-        <v>0</v>
-      </c>
-      <c r="R2">
-        <v>8229999.9999999953</v>
-      </c>
-      <c r="S2">
-        <v>1</v>
-      </c>
-      <c r="T2">
-        <v>8367717.0187190045</v>
-      </c>
-      <c r="U2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="264">
-        <v>44197</v>
-      </c>
-      <c r="B3">
-        <v>7</v>
-      </c>
-      <c r="C3">
-        <v>29999.999699999997</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>29999.999699999997</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>7999.9999999998645</v>
-      </c>
-      <c r="H3">
-        <v>483294.69699999993</v>
-      </c>
-      <c r="I3">
-        <v>613861.00000020827</v>
-      </c>
-      <c r="J3">
-        <v>285431.99699999997</v>
-      </c>
-      <c r="K3">
-        <v>11709.4</v>
-      </c>
-      <c r="L3">
-        <v>180000</v>
-      </c>
-      <c r="M3">
-        <v>50000</v>
-      </c>
-      <c r="N3">
-        <v>6153.3000000000002</v>
-      </c>
-      <c r="O3">
-        <v>563861.00000020815</v>
-      </c>
-      <c r="P3">
-        <v>469427.99999962631</v>
-      </c>
-      <c r="Q3">
-        <v>0</v>
-      </c>
-      <c r="R3">
-        <v>8480334.9247879162</v>
-      </c>
-      <c r="S3">
-        <v>1</v>
-      </c>
-      <c r="T3">
-        <v>8591315.9507879168</v>
+        <v>9110981.0259775538</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -7285,13 +6849,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>480594.40000000002</v>
       </c>
       <c r="I2">
-        <v>906235.80000430183</v>
+        <v>1183860.999999813</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -7306,22 +6870,22 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>856235.80000430183</v>
+        <v>1133860.999999813</v>
       </c>
       <c r="P2">
-        <v>409927.99999981304</v>
+        <v>407756.29999981303</v>
       </c>
       <c r="Q2">
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8372721.8507190049</v>
+        <v>8503526.7163992003</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -7332,31 +6896,31 @@
         <v>44197</v>
       </c>
       <c r="B3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3">
-        <v>29999.999699999997</v>
+        <v>0</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>29999.999699999997</v>
+        <v>0</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>7999.9999999998645</v>
+        <v>0</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>483294.39999999991</v>
       </c>
       <c r="I3">
-        <v>1176998.3200036848</v>
+        <v>1453860.9999996261</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -7371,22 +6935,22 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1126998.3200036846</v>
+        <v>1403860.9999996261</v>
       </c>
       <c r="P3">
-        <v>469427.99999962631</v>
+        <v>440670.19999962603</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8229999.9999991106</v>
+        <v>13207358.43426156</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>8440604.3459991124</v>
+        <v>13498665.636261562</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -7486,13 +7050,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>480594.40000000002</v>
       </c>
       <c r="I2">
         <v>1183860.999999813</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -7510,19 +7074,19 @@
         <v>1133860.999999813</v>
       </c>
       <c r="P2">
-        <v>409927.99999981304</v>
+        <v>407756.29999981303</v>
       </c>
       <c r="Q2">
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8434458.0807190053</v>
+        <v>8478668.2483992018</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -7533,31 +7097,31 @@
         <v>44197</v>
       </c>
       <c r="B3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3">
-        <v>29999.999699999997</v>
+        <v>0</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>29999.999699999997</v>
+        <v>0</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>7999.9999999998645</v>
+        <v>0</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>483294.39999999991</v>
       </c>
       <c r="I3">
-        <v>1453860.9999996261</v>
+        <v>1083860.9999996119</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -7572,22 +7136,22 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1403860.9999996261</v>
+        <v>1033860.9999996119</v>
       </c>
       <c r="P3">
-        <v>469427.99999962631</v>
+        <v>440670.19999962603</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>12703858.994271697</v>
+        <v>11252641.823397283</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>12977708.876271699</v>
+        <v>11477545.155397281</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -7687,13 +7251,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>480594.40000000002</v>
       </c>
       <c r="I2">
-        <v>1183860.999999813</v>
+        <v>813860.99999979907</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -7708,22 +7272,22 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1133860.999999813</v>
+        <v>763860.99999979907</v>
       </c>
       <c r="P2">
-        <v>409927.99999981304</v>
+        <v>407756.29999981303</v>
       </c>
       <c r="Q2">
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8498951.2427190021</v>
+        <v>8414700.9843992013</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -7734,31 +7298,31 @@
         <v>44197</v>
       </c>
       <c r="B3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>483294.39999999991</v>
       </c>
       <c r="I3">
-        <v>1453860.9999996261</v>
+        <v>1093860.9999996321</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -7773,22 +7337,22 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1403860.9999996261</v>
+        <v>1043860.9999996321</v>
       </c>
       <c r="P3">
-        <v>477427.99999962613</v>
+        <v>432670.19999962609</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>13799263.92287196</v>
+        <v>12852219.990416728</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>14090571.12487196</v>
+        <v>13000252.618416728</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -7888,13 +7452,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>480594.40000000002</v>
       </c>
       <c r="I2">
         <v>1183860.999999813</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -7912,19 +7476,19 @@
         <v>1133860.999999813</v>
       </c>
       <c r="P2">
-        <v>409927.99999981304</v>
+        <v>407756.29999981303</v>
       </c>
       <c r="Q2">
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8478198.5587190036</v>
+        <v>8365005.4803992016</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -7935,31 +7499,31 @@
         <v>44197</v>
       </c>
       <c r="B3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>483294.39999999991</v>
       </c>
       <c r="I3">
         <v>1083860.9999996119</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -7977,19 +7541,19 @@
         <v>1033860.9999996119</v>
       </c>
       <c r="P3">
-        <v>477427.99999962613</v>
+        <v>432670.19999962609</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>10574473.267596161</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>10799376.59959616</v>
+        <v>9187857.7959775534</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -8089,13 +7653,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>480594.40000000002</v>
       </c>
       <c r="I2">
         <v>813860.99999979907</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -8113,19 +7677,19 @@
         <v>763860.99999979907</v>
       </c>
       <c r="P2">
-        <v>409927.99999981304</v>
+        <v>407756.29999981303</v>
       </c>
       <c r="Q2">
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8424348.3727190029</v>
+        <v>8417607.2963992003</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -8139,13 +7703,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>29999.999699999997</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>29999.999699999997</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -8154,13 +7718,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>483294.39999999991</v>
       </c>
       <c r="I3">
-        <v>1093860.9999996321</v>
+        <v>542812.0000005333</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -8175,22 +7739,22 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1043860.9999996321</v>
+        <v>492812.0000005333</v>
       </c>
       <c r="P3">
-        <v>469427.99999962631</v>
+        <v>432670.19999962609</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>12005874.347986775</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>12153906.975986775</v>
+        <v>9187833.549977554</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -8290,13 +7854,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>480594.40000000002</v>
       </c>
       <c r="I2">
-        <v>1183860.999999813</v>
+        <v>613861.0000002078</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -8311,22 +7875,22 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1133860.999999813</v>
+        <v>563861.0000002078</v>
       </c>
       <c r="P2">
-        <v>409927.99999981304</v>
+        <v>407756.29999981303</v>
       </c>
       <c r="Q2">
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8364513.5347190024</v>
+        <v>8397424.9303992018</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -8340,13 +7904,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>29999.999699999997</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>29999.999699999997</v>
+        <v>29999.700000000001</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -8355,13 +7919,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>483294.39999999991</v>
       </c>
       <c r="I3">
-        <v>1083860.9999996119</v>
+        <v>513861.00000000687</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>285431.70000000001</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -8376,10 +7940,10 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1033860.9999996119</v>
+        <v>463861.00000000681</v>
       </c>
       <c r="P3">
-        <v>469427.99999962631</v>
+        <v>432670.19999962609</v>
       </c>
       <c r="Q3">
         <v>0</v>
@@ -8391,7 +7955,7 @@
         <v>1</v>
       </c>
       <c r="T3">
-        <v>9187857.7959775534</v>
+        <v>9150597.6699775551</v>
       </c>
       <c r="U3">
         <v>0</v>

</xml_diff>

<commit_message>
Updated Ensemble forecast files to reflect latest from April 2020 run
Updated the MTOM Ensemble output file to fix errors in named ranges
Update to model file and ruleset which includes the following (MTOM_Rules_V3.2_SB_LCAprilUpdates_BalajiUpdates.rls, MTOM_V3.1.202003_SB_LCAprilUpdates):
	Update to taylor park tables
	Updated set outyear volume initialization rule
	updated Mead data in UBRueCurve
	Updated MWD ICS calculation rule to use forecasted water available vs the sum of the diversion requested
	Moved powellData3525 Monthly flag to UB Reservoir DMI
	redid naming of Binational Water Scarcity Contingency Plan flags
</commit_message>
<xml_diff>
--- a/Output Data/MtomToCrss_Annual.xlsx
+++ b/Output Data/MtomToCrss_Annual.xlsx
@@ -6,49 +6,51 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Trace3" sheetId="1" r:id="rId2"/>
-    <sheet name="Trace4" sheetId="2" r:id="rId4"/>
-    <sheet name="Trace5" sheetId="3" r:id="rId5"/>
-    <sheet name="Trace6" sheetId="4" r:id="rId6"/>
-    <sheet name="Trace7" sheetId="5" r:id="rId7"/>
-    <sheet name="Trace8" sheetId="6" r:id="rId8"/>
-    <sheet name="Trace9" sheetId="7" r:id="rId9"/>
-    <sheet name="Trace10" sheetId="8" r:id="rId10"/>
-    <sheet name="Trace11" sheetId="9" r:id="rId11"/>
-    <sheet name="Trace12" sheetId="10" r:id="rId12"/>
-    <sheet name="Trace13" sheetId="11" r:id="rId13"/>
-    <sheet name="Trace14" sheetId="12" r:id="rId14"/>
-    <sheet name="Trace15" sheetId="13" r:id="rId15"/>
-    <sheet name="Trace16" sheetId="14" r:id="rId16"/>
-    <sheet name="Trace17" sheetId="15" r:id="rId17"/>
-    <sheet name="Trace18" sheetId="16" r:id="rId18"/>
-    <sheet name="Trace19" sheetId="17" r:id="rId19"/>
-    <sheet name="Trace20" sheetId="18" r:id="rId20"/>
-    <sheet name="Trace21" sheetId="19" r:id="rId21"/>
-    <sheet name="Trace22" sheetId="20" r:id="rId22"/>
-    <sheet name="Trace23" sheetId="21" r:id="rId23"/>
-    <sheet name="Trace24" sheetId="22" r:id="rId24"/>
-    <sheet name="Trace25" sheetId="23" r:id="rId25"/>
-    <sheet name="Trace26" sheetId="24" r:id="rId26"/>
-    <sheet name="Trace27" sheetId="25" r:id="rId27"/>
-    <sheet name="Trace28" sheetId="26" r:id="rId28"/>
-    <sheet name="Trace29" sheetId="27" r:id="rId29"/>
-    <sheet name="Trace30" sheetId="28" r:id="rId30"/>
-    <sheet name="Trace31" sheetId="29" r:id="rId31"/>
-    <sheet name="Trace32" sheetId="30" r:id="rId32"/>
-    <sheet name="Trace33" sheetId="31" r:id="rId33"/>
-    <sheet name="Trace34" sheetId="32" r:id="rId34"/>
-    <sheet name="Trace35" sheetId="33" r:id="rId35"/>
-    <sheet name="Trace36" sheetId="34" r:id="rId36"/>
-    <sheet name="Trace37" sheetId="35" r:id="rId37"/>
-    <sheet name="Trace38" sheetId="36" r:id="rId38"/>
+    <sheet name="Trace1" sheetId="1" r:id="rId2"/>
+    <sheet name="Trace2" sheetId="2" r:id="rId4"/>
+    <sheet name="Trace3" sheetId="3" r:id="rId5"/>
+    <sheet name="Trace4" sheetId="4" r:id="rId6"/>
+    <sheet name="Trace5" sheetId="5" r:id="rId7"/>
+    <sheet name="Trace6" sheetId="6" r:id="rId8"/>
+    <sheet name="Trace7" sheetId="7" r:id="rId9"/>
+    <sheet name="Trace8" sheetId="8" r:id="rId10"/>
+    <sheet name="Trace9" sheetId="9" r:id="rId11"/>
+    <sheet name="Trace10" sheetId="10" r:id="rId12"/>
+    <sheet name="Trace11" sheetId="11" r:id="rId13"/>
+    <sheet name="Trace12" sheetId="12" r:id="rId14"/>
+    <sheet name="Trace13" sheetId="13" r:id="rId15"/>
+    <sheet name="Trace14" sheetId="14" r:id="rId16"/>
+    <sheet name="Trace15" sheetId="15" r:id="rId17"/>
+    <sheet name="Trace16" sheetId="16" r:id="rId18"/>
+    <sheet name="Trace17" sheetId="17" r:id="rId19"/>
+    <sheet name="Trace18" sheetId="18" r:id="rId20"/>
+    <sheet name="Trace19" sheetId="19" r:id="rId21"/>
+    <sheet name="Trace20" sheetId="20" r:id="rId22"/>
+    <sheet name="Trace21" sheetId="21" r:id="rId23"/>
+    <sheet name="Trace22" sheetId="22" r:id="rId24"/>
+    <sheet name="Trace23" sheetId="23" r:id="rId25"/>
+    <sheet name="Trace24" sheetId="24" r:id="rId26"/>
+    <sheet name="Trace25" sheetId="25" r:id="rId27"/>
+    <sheet name="Trace26" sheetId="26" r:id="rId28"/>
+    <sheet name="Trace27" sheetId="27" r:id="rId29"/>
+    <sheet name="Trace28" sheetId="28" r:id="rId30"/>
+    <sheet name="Trace29" sheetId="29" r:id="rId31"/>
+    <sheet name="Trace30" sheetId="30" r:id="rId32"/>
+    <sheet name="Trace31" sheetId="31" r:id="rId33"/>
+    <sheet name="Trace32" sheetId="32" r:id="rId34"/>
+    <sheet name="Trace33" sheetId="33" r:id="rId35"/>
+    <sheet name="Trace34" sheetId="34" r:id="rId36"/>
+    <sheet name="Trace35" sheetId="35" r:id="rId37"/>
+    <sheet name="Trace36" sheetId="36" r:id="rId38"/>
+    <sheet name="Trace37" sheetId="37" r:id="rId39"/>
+    <sheet name="Trace38" sheetId="38" r:id="rId40"/>
   </sheets>
   <calcPr calcId="125725" fullCalcOnLoad="true"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:xdr="http://purl.oclc.org/ooxml/drawingml/spreadsheetDrawing" count="720" uniqueCount="20">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:xdr="http://purl.oclc.org/ooxml/drawingml/spreadsheetDrawing" count="760" uniqueCount="20">
   <si>
     <t>DCP BWSCP Flags.LB DCP BWSP</t>
   </si>
@@ -132,7 +134,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="505">
+  <borders count="267">
     <border>
       <start/>
       <end/>
@@ -406,249 +408,11 @@
     <border/>
     <border/>
     <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="505">
+  <cellXfs count="267">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -992,312 +756,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="266" xfId="0" applyNumberFormat="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="267" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="268" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="269" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="270" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="271" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="272" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="273" xfId="0" applyNumberFormat="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="274" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="275" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="276" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="277" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="278" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="279" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="280" xfId="0" applyNumberFormat="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="281" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="282" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="283" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="284" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="285" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="286" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="287" xfId="0" applyNumberFormat="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="288" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="289" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="290" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="291" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="292" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="293" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="294" xfId="0" applyNumberFormat="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="295" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="296" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="297" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="298" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="299" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="300" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="301" xfId="0" applyNumberFormat="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="302" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="303" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="304" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="305" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="306" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="307" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="308" xfId="0" applyNumberFormat="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="309" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="310" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="311" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="312" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="313" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="314" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="315" xfId="0" applyNumberFormat="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="316" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="317" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="318" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="319" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="320" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="321" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="322" xfId="0" applyNumberFormat="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="323" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="324" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="325" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="326" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="327" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="328" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="329" xfId="0" applyNumberFormat="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="330" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="331" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="332" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="333" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="334" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="335" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="336" xfId="0" applyNumberFormat="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="337" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="338" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="339" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="340" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="341" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="342" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="343" xfId="0" applyNumberFormat="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="344" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="345" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="346" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="347" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="348" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="349" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="350" xfId="0" applyNumberFormat="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="351" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="352" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="353" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="354" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="355" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="356" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="357" xfId="0" applyNumberFormat="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="358" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="359" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="360" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="361" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="362" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="363" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="364" xfId="0" applyNumberFormat="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="365" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="366" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="367" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="368" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="369" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="370" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="371" xfId="0" applyNumberFormat="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="372" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="373" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="374" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="375" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="376" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="377" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="378" xfId="0" applyNumberFormat="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="379" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="380" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="381" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="382" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="383" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="384" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="385" xfId="0" applyNumberFormat="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="386" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="387" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="388" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="389" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="390" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="391" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="392" xfId="0" applyNumberFormat="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="393" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="394" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="395" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="396" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="397" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="398" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="399" xfId="0" applyNumberFormat="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="400" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="401" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="402" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="403" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="404" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="405" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="406" xfId="0" applyNumberFormat="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="407" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="408" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="409" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="410" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="411" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="412" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="413" xfId="0" applyNumberFormat="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="414" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="415" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="416" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="417" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="418" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="419" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="420" xfId="0" applyNumberFormat="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="421" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="422" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="423" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="424" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="425" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="426" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="427" xfId="0" applyNumberFormat="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="428" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="429" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="430" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="431" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="432" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="433" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="434" xfId="0" applyNumberFormat="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="435" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="436" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="437" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="438" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="439" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="440" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="441" xfId="0" applyNumberFormat="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="442" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="443" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="444" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="445" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="446" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="447" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="448" xfId="0" applyNumberFormat="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="449" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="450" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="451" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="452" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="453" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="454" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="455" xfId="0" applyNumberFormat="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="456" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="457" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="458" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="459" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="460" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="461" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="462" xfId="0" applyNumberFormat="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="463" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="464" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="465" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="466" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="467" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="468" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="469" xfId="0" applyNumberFormat="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="470" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="471" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="472" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="473" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="474" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="475" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="476" xfId="0" applyNumberFormat="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="477" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="478" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="479" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="480" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="481" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="482" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="483" xfId="0" applyNumberFormat="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="484" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="485" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="486" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="487" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="488" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="489" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="490" xfId="0" applyNumberFormat="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="491" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="492" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="493" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="494" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="495" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="496" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="497" xfId="0" applyNumberFormat="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="498" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="499" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="500" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="501" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="502" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="503" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="504" xfId="0" applyNumberFormat="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1395,13 +853,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1097690.5</v>
+        <v>1015561.9</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>280632</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -1416,7 +874,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1047690.5</v>
+        <v>965561.89999999991</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -1431,7 +889,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8388617.0990332533</v>
+        <v>8402103.3535112683</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -1445,13 +903,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>24300</v>
+        <v>27000</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>24300</v>
+        <v>27000</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -1460,13 +918,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1261206.0999999999</v>
+        <v>1026080.2</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>280632</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -1481,7 +939,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1211206.0999999999</v>
+        <v>976080.19999999995</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -1496,7 +954,7 @@
         <v>1</v>
       </c>
       <c r="T3">
-        <v>9137627.9999775533</v>
+        <v>9140895.9999775533</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -1596,13 +1054,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>813860.99999979907</v>
+        <v>1015561.9</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>280632</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -1617,7 +1075,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>763860.99999979907</v>
+        <v>965561.89999999991</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -1632,7 +1090,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8373008.8290332509</v>
+        <v>8448537.9355112668</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -1646,13 +1104,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>24300</v>
+        <v>27000</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>24300</v>
+        <v>27000</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -1661,13 +1119,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>813860.99999979988</v>
+        <v>744512.90000073425</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>280632</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -1682,7 +1140,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>763860.99999979977</v>
+        <v>694512.90000073425</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -1691,13 +1149,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8714241.2454313841</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>8850734.6714313831</v>
+        <v>8417833.5499991123</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -1797,13 +1255,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>613861.0000002078</v>
+        <v>1015561.9</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>280632</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -1818,7 +1276,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>563861.0000002078</v>
+        <v>965561.89999999991</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -1833,7 +1291,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8369752.0770332525</v>
+        <v>8425298.5215112679</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -1847,13 +1305,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>24300</v>
+        <v>27000</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>24300</v>
+        <v>27000</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -1862,13 +1320,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>313861.00000041554</v>
+        <v>915561.89999979886</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>280632</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -1883,7 +1341,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>263861.00000041554</v>
+        <v>865561.89999979897</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -1892,13 +1350,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8999999.9999775533</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>9174589.2299775518</v>
+        <v>8380597.6699991105</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -1998,13 +1456,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>613861.0000002078</v>
+        <v>1015561.9</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>280632</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -2019,7 +1477,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>563861.0000002078</v>
+        <v>965561.89999999991</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -2034,7 +1492,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8420218.8750332519</v>
+        <v>8409308.3775112685</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -2048,13 +1506,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>24300</v>
+        <v>27000</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>24300</v>
+        <v>27000</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -2063,13 +1521,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>313861.00000041554</v>
+        <v>934631.70000073477</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>280632</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -2084,7 +1542,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>263861.00000041554</v>
+        <v>884631.70000073477</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -2099,7 +1557,7 @@
         <v>1</v>
       </c>
       <c r="T3">
-        <v>8469478.9159991127</v>
+        <v>8366493.4259991096</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -2199,13 +1657,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>613861.0000002078</v>
+        <v>1015561.9</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>280632</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -2220,7 +1678,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>563861.0000002078</v>
+        <v>965561.89999999991</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -2235,7 +1693,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8466740.6050332543</v>
+        <v>8414337.971511269</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -2249,13 +1707,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>24300</v>
+        <v>27000</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>24300</v>
+        <v>27000</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -2264,13 +1722,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>763861.00000010396</v>
+        <v>744512.90000073425</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>280632</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -2285,7 +1743,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>713861.00000010396</v>
+        <v>694512.90000073425</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -2294,13 +1752,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>9428522.0439325348</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>9838340.2679325324</v>
+        <v>8404589.229999112</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -2400,13 +1858,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1048860.9999999066</v>
+        <v>1015561.9</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>280632</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -2421,7 +1879,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>998860.99999990652</v>
+        <v>965561.89999999991</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -2436,7 +1894,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8535845.9710332509</v>
+        <v>8435463.8115112688</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -2447,31 +1905,31 @@
         <v>44197</v>
       </c>
       <c r="B3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>27000</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>27000</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>748861.00000011432</v>
+        <v>744512.90000073425</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>280632</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -2486,10 +1944,10 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>698861.00000011432</v>
+        <v>694512.90000073425</v>
       </c>
       <c r="P3">
-        <v>477427.99999962613</v>
+        <v>469427.99999962631</v>
       </c>
       <c r="Q3">
         <v>0</v>
@@ -2501,7 +1959,7 @@
         <v>1</v>
       </c>
       <c r="T3">
-        <v>8362878.8059991114</v>
+        <v>8469478.9159991127</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -2601,13 +2059,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>613861.0000002078</v>
+        <v>1015561.9</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>280632</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -2622,7 +2080,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>563861.0000002078</v>
+        <v>965561.89999999991</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -2637,7 +2095,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8362630.2730332529</v>
+        <v>8460768.0255112685</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -2651,13 +2109,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>24300</v>
+        <v>27000</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>24300</v>
+        <v>27000</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -2666,13 +2124,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>913861</v>
+        <v>1150561.8999999065</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>280632</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -2687,7 +2145,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>863861</v>
+        <v>1100561.8999999065</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -2696,13 +2154,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>10837705.370753584</v>
+        <v>9387640.1928784847</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>11120125.674753584</v>
+        <v>9797458.4168784823</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -2802,13 +2260,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1183860.999999813</v>
+        <v>1015561.9</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>280632</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -2823,7 +2281,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1133860.999999813</v>
+        <v>965561.89999999991</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -2832,13 +2290,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>9799204.6629683357</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>10061978.228001589</v>
+        <v>8455180.7455112673</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -2849,31 +2307,31 @@
         <v>44197</v>
       </c>
       <c r="B3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>27000</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>27000</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1453860.9999996261</v>
+        <v>724373.50000073458</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>280632</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -2888,22 +2346,22 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1403860.9999996261</v>
+        <v>674373.50000073458</v>
       </c>
       <c r="P3">
-        <v>466373.38999962609</v>
+        <v>469427.99999962631</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>11955559.365453757</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>12084078.097453758</v>
+        <v>9132878.8059775531</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -3003,13 +2461,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1183860.999999813</v>
+        <v>1015561.9</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>280632</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -3024,7 +2482,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1133860.999999813</v>
+        <v>965561.89999999991</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -3039,7 +2497,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8352671.9550332529</v>
+        <v>8391746.4835112691</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -3053,13 +2511,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>24300</v>
+        <v>27000</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>24300</v>
+        <v>27000</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -3068,13 +2526,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1453860.9999996261</v>
+        <v>1285561.8999998129</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>280632</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -3089,7 +2547,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1403860.9999996261</v>
+        <v>1235561.8999998129</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -3098,13 +2556,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>11162359.50971056</v>
+        <v>10791412.168028634</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>11224031.195710558</v>
+        <v>11073832.472028634</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -3204,13 +2662,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1183860.999999813</v>
+        <v>1015561.9</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>280632</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -3225,7 +2683,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1133860.999999813</v>
+        <v>965561.89999999991</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -3240,7 +2698,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8301363.9890332539</v>
+        <v>8458151.709511267</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -3254,13 +2712,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>24300</v>
+        <v>27000</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>24300</v>
+        <v>27000</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -3269,13 +2727,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1453860.9999996261</v>
+        <v>1285561.8999998129</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>280632</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -3290,7 +2748,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1403860.9999996261</v>
+        <v>1235561.8999998129</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -3299,13 +2757,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8229999.9999991106</v>
+        <v>10915274.757822959</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>8140372.5099991113</v>
+        <v>11043793.489822958</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -3405,13 +2863,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1183860.999999813</v>
+        <v>1015561.9</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>280632</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -3426,7 +2884,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1133860.999999813</v>
+        <v>965561.89999999991</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -3441,7 +2899,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8238819.7290332541</v>
+        <v>8413963.1435112692</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -3452,31 +2910,31 @@
         <v>44197</v>
       </c>
       <c r="B3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>27000</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>27000</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1453860.9999996268</v>
+        <v>1285561.8999998129</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>280632</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -3491,22 +2949,22 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1403860.9999996268</v>
+        <v>1235561.8999998129</v>
       </c>
       <c r="P3">
-        <v>477427.99999962613</v>
+        <v>469427.99999962631</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8229999.9999991106</v>
+        <v>11113631.211655125</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>8433484.9599991105</v>
+        <v>11175302.897655124</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -3606,13 +3064,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>813860.99999979907</v>
+        <v>1015561.9</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>280632</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -3627,7 +3085,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>763860.99999979907</v>
+        <v>965561.89999999991</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -3642,7 +3100,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8379169.8810332529</v>
+        <v>8421280.3535112664</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -3656,13 +3114,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>24300</v>
+        <v>27000</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>24300</v>
+        <v>27000</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -3671,13 +3129,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1093860.9999996321</v>
+        <v>1026080.2</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>280632</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -3692,7 +3150,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1043860.9999996321</v>
+        <v>976080.19999999995</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -3701,13 +3159,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8229999.9999991106</v>
+        <v>11189768.765059674</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>8440604.3459991124</v>
+        <v>11352226.765059674</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -3807,13 +3265,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1183860.999999813</v>
+        <v>1015561.9</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>280632</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -3828,7 +3286,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1133860.999999813</v>
+        <v>965561.89999999991</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -3843,7 +3301,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8421968.0990332514</v>
+        <v>8370714.3735112697</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -3857,13 +3315,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>24300</v>
+        <v>27000</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>24300</v>
+        <v>27000</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -3872,13 +3330,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1318860.9999997194</v>
+        <v>1285561.8999998129</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>280632</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -3893,7 +3351,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1268860.9999997194</v>
+        <v>1235561.8999998129</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -3908,7 +3366,7 @@
         <v>1</v>
       </c>
       <c r="T3">
-        <v>8370628.0299991099</v>
+        <v>8140372.5099991113</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -4008,13 +3466,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1048860.9999999066</v>
+        <v>1015561.9</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>280632</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -4029,7 +3487,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>998860.99999990652</v>
+        <v>965561.89999999991</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -4044,7 +3502,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8404077.359033253</v>
+        <v>8325968.4535112707</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -4058,13 +3516,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>24300</v>
+        <v>27000</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>24300</v>
+        <v>27000</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -4073,13 +3531,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>948860.99999970547</v>
+        <v>1285561.8999998129</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>280632</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -4094,7 +3552,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>898860.99999970547</v>
+        <v>1235561.8999998129</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -4103,13 +3561,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8999999.9999775533</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>9105477.679977553</v>
+        <v>8433484.9599991105</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -4209,13 +3667,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>813860.99999979907</v>
+        <v>1015561.9</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>280632</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -4230,7 +3688,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>763860.99999979907</v>
+        <v>965561.89999999991</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -4245,7 +3703,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8345625.5190332523</v>
+        <v>8440828.2735112682</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -4259,13 +3717,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>24300</v>
+        <v>27000</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>24300</v>
+        <v>27000</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -4274,13 +3732,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>713860.99999959802</v>
+        <v>1150561.8999999065</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>280632</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -4295,7 +3753,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>663860.99999959802</v>
+        <v>1100561.8999999065</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -4304,13 +3762,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8229999.9999991106</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>8338713.64999911</v>
+        <v>9140628.0299775563</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -4410,13 +3868,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>813860.99999979907</v>
+        <v>1015561.9</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>280632</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -4431,7 +3889,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>763860.99999979907</v>
+        <v>965561.89999999991</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -4446,7 +3904,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8378109.2990332516</v>
+        <v>8453200.0635112692</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -4460,13 +3918,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>24300</v>
+        <v>27000</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>24300</v>
+        <v>27000</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -4475,13 +3933,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>958860.99999972573</v>
+        <v>915561.89999979886</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>280632</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -4496,7 +3954,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>908860.99999972573</v>
+        <v>865561.89999979897</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -4505,13 +3963,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8977212.0037249625</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>9108859.4437249638</v>
+        <v>9105477.679977553</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -4611,13 +4069,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1048860.9999999066</v>
+        <v>1015561.9</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>280632</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -4632,7 +4090,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>998860.99999990652</v>
+        <v>965561.89999999991</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -4647,7 +4105,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8384089.6590332529</v>
+        <v>8397154.1435112692</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -4661,13 +4119,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>24300</v>
+        <v>27000</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>24300</v>
+        <v>27000</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -4676,13 +4134,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1048860.9999999066</v>
+        <v>915561.89999979886</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>280632</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -4697,7 +4155,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>998860.99999990652</v>
+        <v>865561.89999979897</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -4706,13 +4164,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8999999.9999775533</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>9104398.0899775531</v>
+        <v>8338713.64999911</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -4812,13 +4270,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>913861</v>
+        <v>1015561.9</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>280632</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -4833,7 +4291,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>863861</v>
+        <v>965561.89999999991</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -4848,7 +4306,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8341387.7390332529</v>
+        <v>8427449.2635112684</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -4862,13 +4320,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>24300</v>
+        <v>27000</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>24300</v>
+        <v>27000</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -4877,13 +4335,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1048860.9999999066</v>
+        <v>1150561.8999999065</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>280632</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -4898,7 +4356,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>998860.99999990652</v>
+        <v>1100561.8999999065</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -4907,13 +4365,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8229999.9999991106</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>8359167.7799991118</v>
+        <v>9131647.4399775527</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -5013,13 +4471,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1048860.9999999066</v>
+        <v>1015561.9</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>280632</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -5034,7 +4492,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>998860.99999990652</v>
+        <v>965561.89999999991</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -5049,7 +4507,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8389179.7690332532</v>
+        <v>8427691.9135112688</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -5060,31 +4518,31 @@
         <v>44197</v>
       </c>
       <c r="B3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>27000</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>27000</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1318860.9999997194</v>
+        <v>1015561.9</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>280632</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -5099,22 +4557,22 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1268860.9999997194</v>
+        <v>965561.89999999991</v>
       </c>
       <c r="P3">
-        <v>477427.99999962613</v>
+        <v>469427.99999962631</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8229999.9999991106</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>8493906.2799991108</v>
+        <v>9104398.0899775531</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -5214,13 +4672,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1183860.999999813</v>
+        <v>1015561.9</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>280632</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -5235,7 +4693,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1133860.999999813</v>
+        <v>965561.89999999991</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -5250,7 +4708,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8459395.0790332537</v>
+        <v>8377021.3035112685</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -5264,13 +4722,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>24300</v>
+        <v>27000</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>24300</v>
+        <v>27000</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -5279,13 +4737,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1083860.9999996119</v>
+        <v>1150561.8999999065</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>280632</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -5300,7 +4758,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1033860.9999996119</v>
+        <v>1100561.8999999065</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -5309,13 +4767,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8999999.9999775533</v>
+        <v>9474668.5477565899</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>9166147.929977553</v>
+        <v>9603836.3277565893</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -5415,13 +4873,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>813860.99999979907</v>
+        <v>1015561.9</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>280632</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -5436,7 +4894,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>763860.99999979907</v>
+        <v>965561.89999999991</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -5451,7 +4909,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8359934.0990332542</v>
+        <v>8426573.6935112681</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -5465,13 +4923,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>24300</v>
+        <v>27000</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>24300</v>
+        <v>27000</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -5480,13 +4938,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>513861.00000000675</v>
+        <v>1285561.8999998129</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>280632</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -5501,7 +4959,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>463861.00000000675</v>
+        <v>1235561.8999998129</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -5510,13 +4968,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8999999.9999775533</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>9186027.3499775529</v>
+        <v>8493906.2799991108</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -5616,13 +5074,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>613861.0000002078</v>
+        <v>1015561.9</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>280632</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -5637,7 +5095,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>563861.0000002078</v>
+        <v>965561.89999999991</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -5652,7 +5110,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8418277.9990332499</v>
+        <v>8487087.0835112706</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -5666,13 +5124,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>24300</v>
+        <v>27000</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>24300</v>
+        <v>27000</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -5681,13 +5139,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>513861.00000000687</v>
+        <v>915561.89999979886</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>280632</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -5702,7 +5160,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>463861.00000000681</v>
+        <v>865561.89999979897</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -5717,7 +5175,7 @@
         <v>1</v>
       </c>
       <c r="T3">
-        <v>9160152.0699775536</v>
+        <v>9166147.929977553</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -5817,13 +5275,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1183860.999999813</v>
+        <v>1015561.9</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>280632</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -5838,7 +5296,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1133860.999999813</v>
+        <v>965561.89999999991</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -5853,7 +5311,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8435305.189033255</v>
+        <v>8448689.3535112701</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -5864,31 +5322,31 @@
         <v>44197</v>
       </c>
       <c r="B3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>27000</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>27000</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1453860.9999996261</v>
+        <v>1026080.2</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>280632</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -5903,22 +5361,22 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1403860.9999996261</v>
+        <v>976080.19999999995</v>
       </c>
       <c r="P3">
-        <v>488482.60999962612</v>
+        <v>469427.99999962631</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>10778293.13521014</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>11052143.017210139</v>
+        <v>9157545.9999775533</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -6018,13 +5476,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>813860.99999979907</v>
+        <v>1015561.9</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>280632</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -6039,7 +5497,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>763860.99999979907</v>
+        <v>965561.89999999991</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -6054,7 +5512,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8381215.9290332515</v>
+        <v>8401880.5535112675</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -6068,13 +5526,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>24300</v>
+        <v>27000</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>24300</v>
+        <v>27000</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -6083,13 +5541,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>813860.99999979907</v>
+        <v>744512.90000073425</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>280632</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -6104,7 +5562,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>763860.99999979907</v>
+        <v>694512.90000073425</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -6119,7 +5577,7 @@
         <v>1</v>
       </c>
       <c r="T3">
-        <v>9183949.7199775539</v>
+        <v>9186027.3499775529</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -6219,13 +5677,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>913861</v>
+        <v>1015561.9</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>280632</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -6240,7 +5698,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>863861</v>
+        <v>965561.89999999991</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -6255,7 +5713,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8391165.6090332512</v>
+        <v>8450398.4335112683</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -6269,13 +5727,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>24300</v>
+        <v>27000</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>24300</v>
+        <v>27000</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -6284,13 +5742,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1183860.999999813</v>
+        <v>915561.89999979886</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>280632</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -6305,7 +5763,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1133860.999999813</v>
+        <v>865561.89999979897</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -6314,13 +5772,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>11342951.210518882</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>11555646.220518883</v>
+        <v>9160152.0699775536</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -6420,13 +5878,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1183860.999999813</v>
+        <v>1015561.9</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>280632</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -6441,7 +5899,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1133860.999999813</v>
+        <v>965561.89999999991</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -6456,7 +5914,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8436236.8790332507</v>
+        <v>8425821.3235112689</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -6470,13 +5928,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>24300</v>
+        <v>27000</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>24300</v>
+        <v>27000</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -6485,13 +5943,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1183860.999999813</v>
+        <v>1015561.9</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>280632</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -6506,7 +5964,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1133860.999999813</v>
+        <v>965561.89999999991</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -6521,7 +5979,7 @@
         <v>1</v>
       </c>
       <c r="T3">
-        <v>9061125.7399775553</v>
+        <v>9183949.7199775539</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -6621,13 +6079,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>913861</v>
+        <v>1015561.9</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>280632</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -6642,7 +6100,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>863861</v>
+        <v>965561.89999999991</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -6657,7 +6115,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8315798.3690332538</v>
+        <v>8429665.3535112683</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -6671,13 +6129,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>24300</v>
+        <v>27000</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>24300</v>
+        <v>27000</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -6686,13 +6144,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>813860.99999979907</v>
+        <v>1285561.8999998129</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>280632</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -6707,7 +6165,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>763860.99999979907</v>
+        <v>1235561.8999998129</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -6716,13 +6174,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8229999.9999991106</v>
+        <v>11693420.497816993</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>8261744.7299991101</v>
+        <v>11906115.507816993</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -6822,13 +6280,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>813860.99999979907</v>
+        <v>1015561.9</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>280632</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -6843,7 +6301,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>763860.99999979907</v>
+        <v>965561.89999999991</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -6858,7 +6316,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8309709.8290332528</v>
+        <v>8473276.1335112676</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -6872,13 +6330,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>24300</v>
+        <v>27000</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>24300</v>
+        <v>27000</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -6887,13 +6345,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>513861.00000000675</v>
+        <v>1015561.9</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>280632</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -6908,7 +6366,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>463861.00000000675</v>
+        <v>965561.89999999991</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -6923,7 +6381,7 @@
         <v>1</v>
       </c>
       <c r="T3">
-        <v>9088058.5399775542</v>
+        <v>9061125.7399775553</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -7023,13 +6481,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>613861.0000002078</v>
+        <v>1015561.9</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>280632</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -7044,7 +6502,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>563861.0000002078</v>
+        <v>965561.89999999991</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -7059,7 +6517,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8362018.0490332544</v>
+        <v>8368759.9235112704</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -7073,13 +6531,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>24300</v>
+        <v>27000</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>24300</v>
+        <v>27000</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -7088,13 +6546,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>313861.00000041554</v>
+        <v>915561.89999979886</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>280632</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -7109,7 +6567,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>263861.00000041554</v>
+        <v>865561.89999979897</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -7118,13 +6576,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8999999.9999775533</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>9135931.8499775529</v>
+        <v>8261744.7299991101</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -7224,13 +6682,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>613861.0000002078</v>
+        <v>1015561.9</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>280632</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -7245,7 +6703,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>563861.0000002078</v>
+        <v>965561.89999999991</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -7260,7 +6718,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8366599.0990332542</v>
+        <v>8382946.1235112678</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -7274,13 +6732,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>24300</v>
+        <v>27000</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>24300</v>
+        <v>27000</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -7289,13 +6747,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>613861.00000020862</v>
+        <v>744512.90000073425</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>280632</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -7310,7 +6768,409 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>563861.00000020862</v>
+        <v>694512.90000073425</v>
+      </c>
+      <c r="P3">
+        <v>469427.99999962631</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>8999999.9999775533</v>
+      </c>
+      <c r="S3">
+        <v>1</v>
+      </c>
+      <c r="T3">
+        <v>9088058.5399775542</v>
+      </c>
+      <c r="U3">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:xdr="http://purl.oclc.org/ooxml/drawingml/spreadsheetDrawing">
+  <dimension ref="A1:U3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="259" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="259" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="259" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="259" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="259" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="259" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="259" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="259" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="259" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="259" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="259" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="259" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="259" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="259" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="259" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="259" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="259" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" s="259" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" s="259" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" s="259" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="257">
+        <v>43831</v>
+      </c>
+      <c r="B2">
+        <v>7</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>475794.70000000001</v>
+      </c>
+      <c r="I2">
+        <v>1015561.9</v>
+      </c>
+      <c r="J2">
+        <v>280632</v>
+      </c>
+      <c r="K2">
+        <v>9009.3999999999996</v>
+      </c>
+      <c r="L2">
+        <v>180000</v>
+      </c>
+      <c r="M2">
+        <v>50000</v>
+      </c>
+      <c r="N2">
+        <v>6153.3000000000002</v>
+      </c>
+      <c r="O2">
+        <v>965561.89999999991</v>
+      </c>
+      <c r="P2">
+        <v>409927.99999981304</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>8229999.9999999963</v>
+      </c>
+      <c r="S2">
+        <v>1</v>
+      </c>
+      <c r="T2">
+        <v>8413026.903511269</v>
+      </c>
+      <c r="U2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="257">
+        <v>44197</v>
+      </c>
+      <c r="B3">
+        <v>7</v>
+      </c>
+      <c r="C3">
+        <v>27000</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>27000</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>7999.9999999998645</v>
+      </c>
+      <c r="H3">
+        <v>478494.70000000001</v>
+      </c>
+      <c r="I3">
+        <v>744512.90000073425</v>
+      </c>
+      <c r="J3">
+        <v>280632</v>
+      </c>
+      <c r="K3">
+        <v>11709.4</v>
+      </c>
+      <c r="L3">
+        <v>180000</v>
+      </c>
+      <c r="M3">
+        <v>50000</v>
+      </c>
+      <c r="N3">
+        <v>6153.3000000000002</v>
+      </c>
+      <c r="O3">
+        <v>694512.90000073425</v>
+      </c>
+      <c r="P3">
+        <v>469427.99999962631</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>8999999.9999775533</v>
+      </c>
+      <c r="S3">
+        <v>1</v>
+      </c>
+      <c r="T3">
+        <v>9135931.8499775529</v>
+      </c>
+      <c r="U3">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:xdr="http://purl.oclc.org/ooxml/drawingml/spreadsheetDrawing">
+  <dimension ref="A1:U3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="266" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="266" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="266" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="266" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="266" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="266" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="266" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="266" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="266" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="266" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="266" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="266" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="266" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="266" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="266" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="266" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="266" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" s="266" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" s="266" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" s="266" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="264">
+        <v>43831</v>
+      </c>
+      <c r="B2">
+        <v>7</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>475794.70000000001</v>
+      </c>
+      <c r="I2">
+        <v>1015561.9</v>
+      </c>
+      <c r="J2">
+        <v>280632</v>
+      </c>
+      <c r="K2">
+        <v>9009.3999999999996</v>
+      </c>
+      <c r="L2">
+        <v>180000</v>
+      </c>
+      <c r="M2">
+        <v>50000</v>
+      </c>
+      <c r="N2">
+        <v>6153.3000000000002</v>
+      </c>
+      <c r="O2">
+        <v>965561.89999999991</v>
+      </c>
+      <c r="P2">
+        <v>409927.99999981304</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>8229999.9999999963</v>
+      </c>
+      <c r="S2">
+        <v>1</v>
+      </c>
+      <c r="T2">
+        <v>8415215.3935112692</v>
+      </c>
+      <c r="U2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="264">
+        <v>44197</v>
+      </c>
+      <c r="B3">
+        <v>7</v>
+      </c>
+      <c r="C3">
+        <v>27000</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>27000</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>7999.9999999998645</v>
+      </c>
+      <c r="H3">
+        <v>478494.70000000001</v>
+      </c>
+      <c r="I3">
+        <v>934631.70000073477</v>
+      </c>
+      <c r="J3">
+        <v>280632</v>
+      </c>
+      <c r="K3">
+        <v>11709.4</v>
+      </c>
+      <c r="L3">
+        <v>180000</v>
+      </c>
+      <c r="M3">
+        <v>50000</v>
+      </c>
+      <c r="N3">
+        <v>6153.3000000000002</v>
+      </c>
+      <c r="O3">
+        <v>884631.70000073477</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -7425,13 +7285,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1183860.999999813</v>
+        <v>1015561.9</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>280632</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -7446,7 +7306,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1133860.999999813</v>
+        <v>965561.89999999991</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -7461,7 +7321,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8500385.8210332524</v>
+        <v>8413142.1275112685</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -7472,31 +7332,31 @@
         <v>44197</v>
       </c>
       <c r="B3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>27000</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>27000</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1453860.9999996261</v>
+        <v>1285561.8999998129</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>280632</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -7511,22 +7371,22 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1403860.9999996261</v>
+        <v>1235561.8999998129</v>
       </c>
       <c r="P3">
-        <v>477427.99999962613</v>
+        <v>469427.99999962631</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>13624090.298644044</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>13915397.500644045</v>
+        <v>8440604.3459991124</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -7626,13 +7486,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1183860.999999813</v>
+        <v>1015561.9</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>280632</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -7647,7 +7507,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1133860.999999813</v>
+        <v>965561.89999999991</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -7662,7 +7522,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8472835.3090332542</v>
+        <v>8445953.1055112705</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -7673,31 +7533,31 @@
         <v>44197</v>
       </c>
       <c r="B3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>27000</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>27000</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1083860.9999996119</v>
+        <v>1285561.8999998129</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>280632</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -7712,22 +7572,22 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1033860.9999996119</v>
+        <v>1235561.8999998129</v>
       </c>
       <c r="P3">
-        <v>477427.99999962613</v>
+        <v>469427.99999962631</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>10415454.195548035</v>
+        <v>10240882.338121932</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>10640357.527548036</v>
+        <v>10514732.220121933</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -7827,13 +7687,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>813860.99999979907</v>
+        <v>1015561.9</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>280632</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -7848,7 +7708,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>763860.99999979907</v>
+        <v>965561.89999999991</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -7863,7 +7723,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8412722.4750332516</v>
+        <v>8491662.2595112678</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -7874,31 +7734,31 @@
         <v>44197</v>
       </c>
       <c r="B3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3">
-        <v>24300</v>
+        <v>0</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>24300</v>
+        <v>0</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>7999.9999999998645</v>
+        <v>0</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1093860.9999996321</v>
+        <v>1285561.8999998129</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>280632</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -7913,22 +7773,22 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1043860.9999996321</v>
+        <v>1235561.8999998129</v>
       </c>
       <c r="P3">
-        <v>469427.99999962631</v>
+        <v>477427.99999962613</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>12352353.423652945</v>
+        <v>12234397.571883366</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>12500386.051652946</v>
+        <v>12525704.773883365</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -8028,13 +7888,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1183860.999999813</v>
+        <v>1015561.9</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>280632</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -8049,7 +7909,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1133860.999999813</v>
+        <v>965561.89999999991</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -8064,7 +7924,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8365797.7570332531</v>
+        <v>8496967.8915112689</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -8075,31 +7935,31 @@
         <v>44197</v>
       </c>
       <c r="B3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3">
-        <v>24300</v>
+        <v>0</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>24300</v>
+        <v>0</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>7999.9999999998645</v>
+        <v>0</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1083860.9999996119</v>
+        <v>915561.89999979886</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>280632</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -8114,22 +7974,22 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1033860.9999996119</v>
+        <v>865561.89999979897</v>
       </c>
       <c r="P3">
-        <v>469427.99999962631</v>
+        <v>477427.99999962613</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>11031228.415133042</v>
+        <v>10685471.283219829</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>11219086.211133042</v>
+        <v>10910374.615219831</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -8229,13 +8089,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>813860.99999979907</v>
+        <v>1015561.9</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>280632</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -8250,7 +8110,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>763860.99999979907</v>
+        <v>965561.89999999991</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -8265,7 +8125,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8416761.01103325</v>
+        <v>8416779.8535112683</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -8279,13 +8139,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>24300</v>
+        <v>27000</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>24300</v>
+        <v>27000</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -8294,13 +8154,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>513861.00000000675</v>
+        <v>1285561.8999998129</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>280632</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -8315,7 +8175,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>463861.00000000675</v>
+        <v>1235561.8999998129</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -8324,13 +8184,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8229999.9999991106</v>
+        <v>11012755.625578197</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>8417833.5499991123</v>
+        <v>11160788.253578197</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -8430,13 +8290,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>480594.69699999999</v>
+        <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>613861.0000002078</v>
+        <v>1015561.9</v>
       </c>
       <c r="J2">
-        <v>285431.99699999997</v>
+        <v>280632</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -8451,7 +8311,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>563861.0000002078</v>
+        <v>965561.89999999991</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -8466,7 +8326,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8394107.3810332529</v>
+        <v>8381092.5175112681</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -8480,13 +8340,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>24300</v>
+        <v>27000</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>24300</v>
+        <v>27000</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -8495,13 +8355,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>483294.69699999993</v>
+        <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>513861.00000000687</v>
+        <v>915561.89999979886</v>
       </c>
       <c r="J3">
-        <v>285431.99699999997</v>
+        <v>280632</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -8516,7 +8376,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>463861.00000000681</v>
+        <v>865561.89999979897</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -8531,7 +8391,7 @@
         <v>1</v>
       </c>
       <c r="T3">
-        <v>9150597.6699775551</v>
+        <v>9187857.7959775534</v>
       </c>
       <c r="U3">
         <v>0</v>

</xml_diff>

<commit_message>
Updated MTOM output files and April model file with run testing new development ruleset
</commit_message>
<xml_diff>
--- a/Output Data/MtomToCrss_Annual.xlsx
+++ b/Output Data/MtomToCrss_Annual.xlsx
@@ -52,7 +52,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:xdr="http://purl.oclc.org/ooxml/drawingml/spreadsheetDrawing" count="760" uniqueCount="20">
   <si>
-    <t>DCP BWSCP Flags.LB DCP BWSP</t>
+    <t>DCP BWSCP Flags.LB DCP BWSCP</t>
   </si>
   <si>
     <t>DCP_Bal_AZ</t>
@@ -889,7 +889,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8390599.2212679628</v>
+        <v>8402103.3535112683</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -1090,7 +1090,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8437033.8032679614</v>
+        <v>8448537.9355112668</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -1122,7 +1122,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>744512.90000073425</v>
+        <v>748403.90000073391</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -1140,7 +1140,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>694512.90000073425</v>
+        <v>698403.90000073391</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -1291,7 +1291,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8413794.3892679643</v>
+        <v>8425298.5215112679</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -1492,7 +1492,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8397804.245267963</v>
+        <v>8409308.3775112685</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -1524,7 +1524,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>934631.70000073477</v>
+        <v>938522.70000073418</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -1542,7 +1542,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>884631.70000073477</v>
+        <v>888522.70000073418</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -1693,7 +1693,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8402833.8392679635</v>
+        <v>8414337.971511269</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -1725,7 +1725,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>744512.90000073425</v>
+        <v>748403.90000073391</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -1743,7 +1743,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>694512.90000073425</v>
+        <v>698403.90000073391</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -1894,7 +1894,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8423959.6792679615</v>
+        <v>8435463.8115112688</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -1926,7 +1926,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>744512.90000073425</v>
+        <v>748403.90000073391</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -1944,7 +1944,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>694512.90000073425</v>
+        <v>698403.90000073391</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -2095,7 +2095,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8449263.8932679631</v>
+        <v>8460768.0255112685</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -2296,7 +2296,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8443676.6132679619</v>
+        <v>8455180.7455112673</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -2328,7 +2328,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>724373.50000073458</v>
+        <v>728264.500000734</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -2346,7 +2346,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>674373.50000073458</v>
+        <v>678264.500000734</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -2497,7 +2497,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8380242.3512679636</v>
+        <v>8391746.4835112691</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -2698,7 +2698,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8446647.5772679616</v>
+        <v>8458151.709511267</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -2757,13 +2757,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>10915457.500681803</v>
+        <v>10911678.653545434</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>11043976.232681802</v>
+        <v>11040197.385545431</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -2899,7 +2899,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8402459.0112679619</v>
+        <v>8413963.1435112692</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -2958,13 +2958,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>11113814.760207748</v>
+        <v>11110018.693070415</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>11175486.446207749</v>
+        <v>11171690.379070412</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -3100,7 +3100,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8409776.2212679628</v>
+        <v>8421280.3535112664</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -3159,13 +3159,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>11189952.34396366</v>
+        <v>11185968.501632852</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>11352410.34396366</v>
+        <v>11348426.501632851</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -3301,7 +3301,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8359210.2412679633</v>
+        <v>8370714.3735112697</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -3502,7 +3502,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8314464.3212679643</v>
+        <v>8325968.4535112707</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -3703,7 +3703,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8429324.1412679628</v>
+        <v>8440828.2735112682</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -3904,7 +3904,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8441695.9312679619</v>
+        <v>8453200.0635112692</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -4105,7 +4105,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8385650.0112679629</v>
+        <v>8397154.1435112692</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -4306,7 +4306,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8415945.1312679611</v>
+        <v>8427449.2635112684</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -4507,7 +4507,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8416187.7812679633</v>
+        <v>8427691.9135112688</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -4708,7 +4708,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8365517.1712679639</v>
+        <v>8377021.3035112685</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -4767,13 +4767,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>9474851.5391911156</v>
+        <v>9470964.2728192639</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>9604019.319191115</v>
+        <v>9600132.0528192632</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -4909,7 +4909,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8415069.5612679627</v>
+        <v>8426573.6935112681</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -5110,7 +5110,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8475582.9512679633</v>
+        <v>8487087.0835112706</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -5311,7 +5311,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8437185.2212679628</v>
+        <v>8448689.3535112701</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -5512,7 +5512,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8390376.4212679639</v>
+        <v>8401880.5535112675</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -5544,7 +5544,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>744512.90000073425</v>
+        <v>748403.90000073391</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -5562,7 +5562,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>694512.90000073425</v>
+        <v>698403.90000073391</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -5713,7 +5713,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8438894.301267961</v>
+        <v>8450398.4335112683</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -5914,7 +5914,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8414317.1912679616</v>
+        <v>8425821.3235112689</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -6115,7 +6115,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8418161.2212679628</v>
+        <v>8429665.3535112683</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -6316,7 +6316,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8461772.0012679603</v>
+        <v>8473276.1335112676</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -6517,7 +6517,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8357255.7912679631</v>
+        <v>8368759.9235112704</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -6718,7 +6718,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8371441.9912679614</v>
+        <v>8382946.1235112678</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -6750,7 +6750,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>744512.90000073425</v>
+        <v>748403.90000073391</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -6768,7 +6768,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>694512.90000073425</v>
+        <v>698403.90000073391</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -6919,7 +6919,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8401522.7712679636</v>
+        <v>8413026.903511269</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -6951,7 +6951,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>744512.90000073425</v>
+        <v>748403.90000073391</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -6969,7 +6969,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>694512.90000073425</v>
+        <v>698403.90000073391</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -7120,7 +7120,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8403711.2612679638</v>
+        <v>8415215.3935112692</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -7152,7 +7152,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>934631.70000073477</v>
+        <v>938522.70000073418</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -7170,7 +7170,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>884631.70000073477</v>
+        <v>888522.70000073418</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -7321,7 +7321,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8401637.9952679612</v>
+        <v>8413142.1275112685</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -7522,7 +7522,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8434448.9732679632</v>
+        <v>8445953.1055112705</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -7581,13 +7581,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>10241065.278277993</v>
+        <v>10237282.93242478</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>10514915.160277991</v>
+        <v>10511132.814424779</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -7723,7 +7723,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8480158.1272679623</v>
+        <v>8491662.2595112678</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -7924,7 +7924,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8485463.7592679635</v>
+        <v>8496967.8915112689</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -7983,13 +7983,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>10685654.154853787</v>
+        <v>10681328.641753327</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>10910557.48685379</v>
+        <v>10906231.973753328</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -8125,7 +8125,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8405275.7212679628</v>
+        <v>8416779.8535112683</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -8326,7 +8326,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8369588.3852679627</v>
+        <v>8381092.5175112681</v>
       </c>
       <c r="U2">
         <v>0</v>

</xml_diff>

<commit_message>
May Model Run. Includes updates to the following:
Output files
ensemble forecast file
Model file name incremented and saved with latest run
Fix to Hoover outflow calculation in ruleset to take into account MWD returns to the system. Ruleset name incremented
</commit_message>
<xml_diff>
--- a/Output Data/MtomToCrss_Annual.xlsx
+++ b/Output Data/MtomToCrss_Annual.xlsx
@@ -6,51 +6,49 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Trace1" sheetId="1" r:id="rId2"/>
-    <sheet name="Trace2" sheetId="2" r:id="rId4"/>
-    <sheet name="Trace3" sheetId="3" r:id="rId5"/>
-    <sheet name="Trace4" sheetId="4" r:id="rId6"/>
-    <sheet name="Trace5" sheetId="5" r:id="rId7"/>
-    <sheet name="Trace6" sheetId="6" r:id="rId8"/>
-    <sheet name="Trace7" sheetId="7" r:id="rId9"/>
-    <sheet name="Trace8" sheetId="8" r:id="rId10"/>
-    <sheet name="Trace9" sheetId="9" r:id="rId11"/>
-    <sheet name="Trace10" sheetId="10" r:id="rId12"/>
-    <sheet name="Trace11" sheetId="11" r:id="rId13"/>
-    <sheet name="Trace12" sheetId="12" r:id="rId14"/>
-    <sheet name="Trace13" sheetId="13" r:id="rId15"/>
-    <sheet name="Trace14" sheetId="14" r:id="rId16"/>
-    <sheet name="Trace15" sheetId="15" r:id="rId17"/>
-    <sheet name="Trace16" sheetId="16" r:id="rId18"/>
-    <sheet name="Trace17" sheetId="17" r:id="rId19"/>
-    <sheet name="Trace18" sheetId="18" r:id="rId20"/>
-    <sheet name="Trace19" sheetId="19" r:id="rId21"/>
-    <sheet name="Trace20" sheetId="20" r:id="rId22"/>
-    <sheet name="Trace21" sheetId="21" r:id="rId23"/>
-    <sheet name="Trace22" sheetId="22" r:id="rId24"/>
-    <sheet name="Trace23" sheetId="23" r:id="rId25"/>
-    <sheet name="Trace24" sheetId="24" r:id="rId26"/>
-    <sheet name="Trace25" sheetId="25" r:id="rId27"/>
-    <sheet name="Trace26" sheetId="26" r:id="rId28"/>
-    <sheet name="Trace27" sheetId="27" r:id="rId29"/>
-    <sheet name="Trace28" sheetId="28" r:id="rId30"/>
-    <sheet name="Trace29" sheetId="29" r:id="rId31"/>
-    <sheet name="Trace30" sheetId="30" r:id="rId32"/>
-    <sheet name="Trace31" sheetId="31" r:id="rId33"/>
-    <sheet name="Trace32" sheetId="32" r:id="rId34"/>
-    <sheet name="Trace33" sheetId="33" r:id="rId35"/>
-    <sheet name="Trace34" sheetId="34" r:id="rId36"/>
-    <sheet name="Trace35" sheetId="35" r:id="rId37"/>
-    <sheet name="Trace36" sheetId="36" r:id="rId38"/>
-    <sheet name="Trace37" sheetId="37" r:id="rId39"/>
-    <sheet name="Trace38" sheetId="38" r:id="rId40"/>
+    <sheet name="Trace3" sheetId="1" r:id="rId2"/>
+    <sheet name="Trace4" sheetId="2" r:id="rId4"/>
+    <sheet name="Trace5" sheetId="3" r:id="rId5"/>
+    <sheet name="Trace6" sheetId="4" r:id="rId6"/>
+    <sheet name="Trace7" sheetId="5" r:id="rId7"/>
+    <sheet name="Trace8" sheetId="6" r:id="rId8"/>
+    <sheet name="Trace9" sheetId="7" r:id="rId9"/>
+    <sheet name="Trace10" sheetId="8" r:id="rId10"/>
+    <sheet name="Trace11" sheetId="9" r:id="rId11"/>
+    <sheet name="Trace12" sheetId="10" r:id="rId12"/>
+    <sheet name="Trace13" sheetId="11" r:id="rId13"/>
+    <sheet name="Trace14" sheetId="12" r:id="rId14"/>
+    <sheet name="Trace15" sheetId="13" r:id="rId15"/>
+    <sheet name="Trace16" sheetId="14" r:id="rId16"/>
+    <sheet name="Trace17" sheetId="15" r:id="rId17"/>
+    <sheet name="Trace18" sheetId="16" r:id="rId18"/>
+    <sheet name="Trace19" sheetId="17" r:id="rId19"/>
+    <sheet name="Trace20" sheetId="18" r:id="rId20"/>
+    <sheet name="Trace21" sheetId="19" r:id="rId21"/>
+    <sheet name="Trace22" sheetId="20" r:id="rId22"/>
+    <sheet name="Trace23" sheetId="21" r:id="rId23"/>
+    <sheet name="Trace24" sheetId="22" r:id="rId24"/>
+    <sheet name="Trace25" sheetId="23" r:id="rId25"/>
+    <sheet name="Trace26" sheetId="24" r:id="rId26"/>
+    <sheet name="Trace27" sheetId="25" r:id="rId27"/>
+    <sheet name="Trace28" sheetId="26" r:id="rId28"/>
+    <sheet name="Trace29" sheetId="27" r:id="rId29"/>
+    <sheet name="Trace30" sheetId="28" r:id="rId30"/>
+    <sheet name="Trace31" sheetId="29" r:id="rId31"/>
+    <sheet name="Trace32" sheetId="30" r:id="rId32"/>
+    <sheet name="Trace33" sheetId="31" r:id="rId33"/>
+    <sheet name="Trace34" sheetId="32" r:id="rId34"/>
+    <sheet name="Trace35" sheetId="33" r:id="rId35"/>
+    <sheet name="Trace36" sheetId="34" r:id="rId36"/>
+    <sheet name="Trace37" sheetId="35" r:id="rId37"/>
+    <sheet name="Trace38" sheetId="36" r:id="rId38"/>
   </sheets>
   <calcPr calcId="125725" fullCalcOnLoad="true"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:xdr="http://purl.oclc.org/ooxml/drawingml/spreadsheetDrawing" count="760" uniqueCount="20">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:xdr="http://purl.oclc.org/ooxml/drawingml/spreadsheetDrawing" count="720" uniqueCount="20">
   <si>
     <t>DCP BWSCP Flags.LB DCP BWSCP</t>
   </si>
@@ -134,7 +132,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="267">
+  <borders count="253">
     <border>
       <start/>
       <end/>
@@ -394,25 +392,11 @@
     <border/>
     <border/>
     <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="267">
+  <cellXfs count="253">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -738,24 +722,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="252" xfId="0" applyNumberFormat="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="253" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="254" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="255" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="256" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="257" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="258" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="259" xfId="0" applyNumberFormat="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="260" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="261" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="262" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="263" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="264" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="265" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="266" xfId="0" applyNumberFormat="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -856,7 +822,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1015561.9</v>
+        <v>1112298.3999999999</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -874,7 +840,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>965561.89999999991</v>
+        <v>1062298.3999999999</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -883,13 +849,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999963</v>
+        <v>8229999.9999999953</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8402103.3535112683</v>
+        <v>8476736.365043832</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -921,7 +887,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1026080.2</v>
+        <v>1122816.7</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -939,7 +905,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>976080.19999999995</v>
+        <v>1072816.7</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -954,7 +920,7 @@
         <v>1</v>
       </c>
       <c r="T3">
-        <v>9140895.9999775533</v>
+        <v>9157545.9999775533</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -1057,7 +1023,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1015561.9</v>
+        <v>1112298.3999999999</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -1075,7 +1041,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>965561.89999999991</v>
+        <v>1062298.3999999999</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -1084,13 +1050,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999963</v>
+        <v>8229999.9999999953</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8448537.9355112668</v>
+        <v>8440135.4290438313</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -1122,7 +1088,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>748403.90000073391</v>
+        <v>1035259.2000007342</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -1140,7 +1106,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>698403.90000073391</v>
+        <v>985259.20000073418</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -1155,7 +1121,7 @@
         <v>1</v>
       </c>
       <c r="T3">
-        <v>8417833.5499991123</v>
+        <v>8366493.4259991096</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -1258,7 +1224,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1015561.9</v>
+        <v>1112298.3999999999</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -1276,7 +1242,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>965561.89999999991</v>
+        <v>1062298.3999999999</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -1285,13 +1251,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999963</v>
+        <v>8229999.9999999953</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8425298.5215112679</v>
+        <v>8453723.3630438298</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -1323,7 +1289,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>915561.89999979886</v>
+        <v>845140.40000073391</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -1341,7 +1307,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>865561.89999979897</v>
+        <v>795140.40000073379</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -1356,7 +1322,7 @@
         <v>1</v>
       </c>
       <c r="T3">
-        <v>8380597.6699991105</v>
+        <v>8404589.229999112</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -1459,7 +1425,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1015561.9</v>
+        <v>1112298.3999999999</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -1477,7 +1443,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>965561.89999999991</v>
+        <v>1062298.3999999999</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -1486,13 +1452,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999963</v>
+        <v>8229999.9999999953</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8409308.3775112685</v>
+        <v>8460901.8110438287</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -1524,7 +1490,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>938522.70000073418</v>
+        <v>845140.40000073391</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -1542,7 +1508,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>888522.70000073418</v>
+        <v>795140.40000073379</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -1557,7 +1523,7 @@
         <v>1</v>
       </c>
       <c r="T3">
-        <v>8366493.4259991096</v>
+        <v>8469478.9159991127</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -1660,7 +1626,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1015561.9</v>
+        <v>1112298.3999999999</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -1678,7 +1644,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>965561.89999999991</v>
+        <v>1062298.3999999999</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -1687,13 +1653,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999963</v>
+        <v>8229999.9999999953</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8414337.971511269</v>
+        <v>8474841.711043831</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -1704,28 +1670,28 @@
         <v>44197</v>
       </c>
       <c r="B3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3">
-        <v>27000</v>
+        <v>0</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>27000</v>
+        <v>0</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>7999.9999999998645</v>
+        <v>0</v>
       </c>
       <c r="H3">
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>748403.90000073391</v>
+        <v>1247298.3999999065</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -1743,22 +1709,22 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>698403.90000073391</v>
+        <v>1197298.3999999063</v>
       </c>
       <c r="P3">
-        <v>469427.99999962631</v>
+        <v>488482.60999962612</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8229999.9999991106</v>
+        <v>9581985.128784582</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>8404589.229999112</v>
+        <v>9991803.3527845815</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -1861,7 +1827,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1015561.9</v>
+        <v>1112298.3999999999</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -1879,7 +1845,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>965561.89999999991</v>
+        <v>1062298.3999999999</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -1888,13 +1854,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999963</v>
+        <v>8229999.9999999953</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8435463.8115112688</v>
+        <v>8457756.0870438293</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -1926,7 +1892,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>748403.90000073391</v>
+        <v>825001.000000734</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -1944,7 +1910,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>698403.90000073391</v>
+        <v>775001.000000734</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -1953,13 +1919,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8229999.9999991106</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>8469478.9159991127</v>
+        <v>9132878.8059775531</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -2062,7 +2028,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1015561.9</v>
+        <v>1112298.3999999999</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -2080,7 +2046,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>965561.89999999991</v>
+        <v>1062298.3999999999</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -2089,13 +2055,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999963</v>
+        <v>8229999.9999999953</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8460768.0255112685</v>
+        <v>8427817.3130438291</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -2127,7 +2093,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1150561.8999999065</v>
+        <v>1382298.3999998129</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -2145,7 +2111,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1100561.8999999065</v>
+        <v>1332298.3999998129</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -2154,13 +2120,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>9387640.1928784847</v>
+        <v>10040648.238941355</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>9797458.4168784823</v>
+        <v>10323068.542941358</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -2263,7 +2229,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1015561.9</v>
+        <v>1112298.3999999999</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -2281,7 +2247,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>965561.89999999991</v>
+        <v>1062298.3999999999</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -2290,13 +2256,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999963</v>
+        <v>8229999.9999999953</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8455180.7455112673</v>
+        <v>8487279.9670438282</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -2307,28 +2273,28 @@
         <v>44197</v>
       </c>
       <c r="B3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3">
-        <v>27000</v>
+        <v>0</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>27000</v>
+        <v>0</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>7999.9999999998645</v>
+        <v>0</v>
       </c>
       <c r="H3">
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>728264.500000734</v>
+        <v>1382298.3999998129</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -2346,22 +2312,22 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>678264.500000734</v>
+        <v>1332298.3999998129</v>
       </c>
       <c r="P3">
-        <v>469427.99999962631</v>
+        <v>466373.38999962609</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8999999.9999775533</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>9132878.8059775531</v>
+        <v>8358518.7319991095</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -2464,7 +2430,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1015561.9</v>
+        <v>1112298.3999999999</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -2482,7 +2448,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>965561.89999999991</v>
+        <v>1062298.3999999999</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -2491,13 +2457,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999963</v>
+        <v>8229999.9999999953</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8391746.4835112691</v>
+        <v>8434164.2090438306</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -2529,7 +2495,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1285561.8999998129</v>
+        <v>1382298.3999998129</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -2547,7 +2513,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1235561.8999998129</v>
+        <v>1332298.3999998129</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -2556,13 +2522,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>10791412.168028634</v>
+        <v>10980119.270413974</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>11073832.472028634</v>
+        <v>11041790.956413973</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -2665,7 +2631,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1015561.9</v>
+        <v>1112298.3999999999</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -2683,7 +2649,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>965561.89999999991</v>
+        <v>1062298.3999999999</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -2692,13 +2658,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999963</v>
+        <v>8229999.9999999953</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8458151.709511267</v>
+        <v>8407710.7450438309</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -2730,7 +2696,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1285561.8999998129</v>
+        <v>1382298.3999998129</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -2748,7 +2714,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1235561.8999998129</v>
+        <v>1332298.3999998129</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -2757,13 +2723,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>10911678.653545434</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>11040197.385545431</v>
+        <v>8140372.5099991113</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -2866,7 +2832,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1015561.9</v>
+        <v>1112298.3999999999</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -2884,7 +2850,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>965561.89999999991</v>
+        <v>1062298.3999999999</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -2893,13 +2859,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999963</v>
+        <v>8229999.9999999953</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8413963.1435112692</v>
+        <v>8372019.3150438312</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -2931,7 +2897,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1285561.8999998129</v>
+        <v>1382298.3999998129</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -2949,7 +2915,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1235561.8999998129</v>
+        <v>1332298.3999998129</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -2958,13 +2924,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>11110018.693070415</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>11171690.379070412</v>
+        <v>8433484.9599991105</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -3067,7 +3033,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1015561.9</v>
+        <v>1112298.3999999999</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -3085,7 +3051,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>965561.89999999991</v>
+        <v>1062298.3999999999</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -3094,13 +3060,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999963</v>
+        <v>8229999.9999999953</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8421280.3535112664</v>
+        <v>8448060.7250438295</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -3132,7 +3098,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1026080.2</v>
+        <v>1382298.3999998129</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -3150,7 +3116,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>976080.19999999995</v>
+        <v>1332298.3999998129</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -3159,13 +3125,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>11185968.501632852</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>11348426.501632851</v>
+        <v>8440604.3459991124</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -3268,7 +3234,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1015561.9</v>
+        <v>1112298.3999999999</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -3286,7 +3252,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>965561.89999999991</v>
+        <v>1062298.3999999999</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -3295,13 +3261,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999963</v>
+        <v>8229999.9999999953</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8370714.3735112697</v>
+        <v>8465117.8150438294</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -3333,7 +3299,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1285561.8999998129</v>
+        <v>1247298.3999999065</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -3351,7 +3317,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1235561.8999998129</v>
+        <v>1197298.3999999063</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -3366,7 +3332,7 @@
         <v>1</v>
       </c>
       <c r="T3">
-        <v>8140372.5099991113</v>
+        <v>8370628.0299991099</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -3469,7 +3435,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1015561.9</v>
+        <v>1112298.3999999999</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -3487,7 +3453,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>965561.89999999991</v>
+        <v>1062298.3999999999</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -3496,13 +3462,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999963</v>
+        <v>8229999.9999999953</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8325968.4535112707</v>
+        <v>8485509.3950438295</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -3534,7 +3500,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1285561.8999998129</v>
+        <v>1012298.3999997991</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -3552,7 +3518,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1235561.8999998129</v>
+        <v>962298.39999979909</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -3561,13 +3527,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8229999.9999991106</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>8433484.9599991105</v>
+        <v>9105477.679977553</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -3670,7 +3636,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1015561.9</v>
+        <v>1112298.3999999999</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -3688,7 +3654,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>965561.89999999991</v>
+        <v>1062298.3999999999</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -3697,13 +3663,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999963</v>
+        <v>8229999.9999999953</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8440828.2735112682</v>
+        <v>8423647.4850438293</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -3735,7 +3701,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1150561.8999999065</v>
+        <v>1012298.3999997991</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -3753,7 +3719,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1100561.8999999065</v>
+        <v>962298.39999979909</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -3762,13 +3728,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8999999.9999775533</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>9140628.0299775563</v>
+        <v>8338713.64999911</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -3871,7 +3837,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1015561.9</v>
+        <v>1112298.3999999999</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -3889,7 +3855,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>965561.89999999991</v>
+        <v>1062298.3999999999</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -3898,13 +3864,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999963</v>
+        <v>8229999.9999999953</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8453200.0635112692</v>
+        <v>8457793.5850438289</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -3936,7 +3902,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>915561.89999979886</v>
+        <v>1247298.3999999065</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -3954,7 +3920,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>865561.89999979897</v>
+        <v>1197298.3999999063</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -3969,7 +3935,7 @@
         <v>1</v>
       </c>
       <c r="T3">
-        <v>9105477.679977553</v>
+        <v>9131647.4399775527</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -4072,7 +4038,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1015561.9</v>
+        <v>1112298.3999999999</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -4090,7 +4056,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>965561.89999999991</v>
+        <v>1062298.3999999999</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -4099,13 +4065,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999963</v>
+        <v>8229999.9999999953</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8397154.1435112692</v>
+        <v>8466864.5950438306</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -4137,7 +4103,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>915561.89999979886</v>
+        <v>1112298.3999999999</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -4155,7 +4121,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>865561.89999979897</v>
+        <v>1062298.3999999999</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -4164,13 +4130,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8229999.9999991106</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>8338713.64999911</v>
+        <v>9104398.0899775531</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -4273,7 +4239,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1015561.9</v>
+        <v>1112298.3999999999</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -4291,7 +4257,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>965561.89999999991</v>
+        <v>1062298.3999999999</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -4300,13 +4266,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999963</v>
+        <v>8229999.9999999953</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8427449.2635112684</v>
+        <v>8418527.6750438306</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -4338,7 +4304,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1150561.8999999065</v>
+        <v>1247298.3999999065</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -4356,7 +4322,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1100561.8999999065</v>
+        <v>1197298.3999999063</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -4365,13 +4331,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8999999.9999775533</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>9131647.4399775527</v>
+        <v>8359167.7799991118</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -4474,7 +4440,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1015561.9</v>
+        <v>1112298.3999999999</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -4492,7 +4458,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>965561.89999999991</v>
+        <v>1062298.3999999999</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -4501,13 +4467,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999963</v>
+        <v>8229999.9999999953</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8427691.9135112688</v>
+        <v>8461231.1150438301</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -4539,7 +4505,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1015561.9</v>
+        <v>1382298.3999998129</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -4557,7 +4523,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>965561.89999999991</v>
+        <v>1332298.3999998129</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -4566,13 +4532,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8999999.9999775533</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>9104398.0899775531</v>
+        <v>8493906.2799991108</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -4675,7 +4641,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1015561.9</v>
+        <v>1112298.3999999999</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -4693,7 +4659,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>965561.89999999991</v>
+        <v>1062298.3999999999</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -4702,13 +4668,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999963</v>
+        <v>8229999.9999999953</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8377021.3035112685</v>
+        <v>8516389.5350438301</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -4740,7 +4706,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1150561.8999999065</v>
+        <v>1012298.3999997991</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -4758,7 +4724,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1100561.8999999065</v>
+        <v>962298.39999979909</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -4767,13 +4733,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>9470964.2728192639</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>9600132.0528192632</v>
+        <v>9166147.929977553</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -4876,7 +4842,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1015561.9</v>
+        <v>1112298.3999999999</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -4894,7 +4860,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>965561.89999999991</v>
+        <v>1062298.3999999999</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -4903,13 +4869,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999963</v>
+        <v>8229999.9999999953</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8426573.6935112681</v>
+        <v>8441629.5250438284</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -4941,7 +4907,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1285561.8999998129</v>
+        <v>845140.40000073391</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -4959,7 +4925,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1235561.8999998129</v>
+        <v>795140.40000073379</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -4968,13 +4934,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8229999.9999991106</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>8493906.2799991108</v>
+        <v>9186027.3499775529</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -5077,7 +5043,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1015561.9</v>
+        <v>1112298.3999999999</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -5095,7 +5061,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>965561.89999999991</v>
+        <v>1062298.3999999999</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -5104,13 +5070,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999963</v>
+        <v>8229999.9999999953</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8487087.0835112706</v>
+        <v>8481463.2850438301</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -5142,7 +5108,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>915561.89999979886</v>
+        <v>1012298.3999997991</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -5160,7 +5126,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>865561.89999979897</v>
+        <v>962298.39999979909</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -5175,7 +5141,7 @@
         <v>1</v>
       </c>
       <c r="T3">
-        <v>9166147.929977553</v>
+        <v>9160152.0699775536</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -5278,7 +5244,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1015561.9</v>
+        <v>1112298.3999999999</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -5296,7 +5262,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>965561.89999999991</v>
+        <v>1062298.3999999999</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -5305,13 +5271,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999963</v>
+        <v>8229999.9999999953</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8448689.3535112701</v>
+        <v>8473109.0950438306</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -5343,7 +5309,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1026080.2</v>
+        <v>1382298.3999998129</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -5361,7 +5327,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>976080.19999999995</v>
+        <v>1332298.3999998129</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -5370,13 +5336,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8999999.9999775533</v>
+        <v>10129573.009568132</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>9157545.9999775533</v>
+        <v>10403422.891568134</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -5479,7 +5445,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1015561.9</v>
+        <v>1112298.3999999999</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -5497,7 +5463,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>965561.89999999991</v>
+        <v>1062298.3999999999</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -5506,13 +5472,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999963</v>
+        <v>8229999.9999999953</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8401880.5535112675</v>
+        <v>8462180.8650438301</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -5544,7 +5510,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>748403.90000073391</v>
+        <v>1112298.3999999999</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -5562,7 +5528,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>698403.90000073391</v>
+        <v>1062298.3999999999</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -5577,7 +5543,7 @@
         <v>1</v>
       </c>
       <c r="T3">
-        <v>9186027.3499775529</v>
+        <v>9183949.7199775539</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -5680,7 +5646,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1015561.9</v>
+        <v>1112298.3999999999</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -5698,7 +5664,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>965561.89999999991</v>
+        <v>1062298.3999999999</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -5707,13 +5673,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999963</v>
+        <v>8229999.9999999953</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8450398.4335112683</v>
+        <v>8460977.3650438301</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -5745,7 +5711,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>915561.89999979886</v>
+        <v>1382298.3999998129</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -5763,7 +5729,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>865561.89999979897</v>
+        <v>1332298.3999998129</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -5772,13 +5738,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8999999.9999775533</v>
+        <v>10604397.497815507</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>9160152.0699775536</v>
+        <v>10817092.507815503</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -5881,7 +5847,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1015561.9</v>
+        <v>1112298.3999999999</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -5899,7 +5865,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>965561.89999999991</v>
+        <v>1062298.3999999999</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -5908,13 +5874,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999963</v>
+        <v>8229999.9999999953</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8425821.3235112689</v>
+        <v>8494576.545043828</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -5946,7 +5912,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1015561.9</v>
+        <v>1112298.3999999999</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -5964,7 +5930,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>965561.89999999991</v>
+        <v>1062298.3999999999</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -5973,13 +5939,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8999999.9999775533</v>
+        <v>8496555.0153858438</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>9183949.7199775539</v>
+        <v>8557680.755385844</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -6082,7 +6048,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1015561.9</v>
+        <v>1112298.3999999999</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -6100,7 +6066,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>965561.89999999991</v>
+        <v>1062298.3999999999</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -6109,13 +6075,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999963</v>
+        <v>8229999.9999999953</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8429665.3535112683</v>
+        <v>8407172.2750438303</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -6147,7 +6113,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1285561.8999998129</v>
+        <v>1012298.3999997991</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -6165,7 +6131,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1235561.8999998129</v>
+        <v>962298.39999979909</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -6174,13 +6140,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>11693420.497816993</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>11906115.507816993</v>
+        <v>8261744.7299991101</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -6283,7 +6249,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1015561.9</v>
+        <v>1112298.3999999999</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -6301,7 +6267,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>965561.89999999991</v>
+        <v>1062298.3999999999</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -6310,13 +6276,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999963</v>
+        <v>8229999.9999999953</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8473276.1335112676</v>
+        <v>8428209.1050438285</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -6348,7 +6314,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1015561.9</v>
+        <v>845140.40000073391</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -6366,7 +6332,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>965561.89999999991</v>
+        <v>795140.40000073379</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -6381,7 +6347,7 @@
         <v>1</v>
       </c>
       <c r="T3">
-        <v>9061125.7399775553</v>
+        <v>9088058.5399775542</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -6484,7 +6450,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1015561.9</v>
+        <v>1112298.3999999999</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -6502,7 +6468,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>965561.89999999991</v>
+        <v>1062298.3999999999</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -6511,13 +6477,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999963</v>
+        <v>8229999.9999999953</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8368759.9235112704</v>
+        <v>8446972.3950438313</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -6549,7 +6515,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>915561.89999979886</v>
+        <v>845140.40000073391</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -6567,7 +6533,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>865561.89999979897</v>
+        <v>795140.40000073379</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -6576,13 +6542,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8229999.9999991106</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>8261744.7299991101</v>
+        <v>9135931.8499775529</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -6685,7 +6651,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1015561.9</v>
+        <v>1112298.3999999999</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -6703,7 +6669,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>965561.89999999991</v>
+        <v>1062298.3999999999</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -6712,13 +6678,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999963</v>
+        <v>8229999.9999999953</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8382946.1235112678</v>
+        <v>8449324.9750438314</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -6750,7 +6716,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>748403.90000073391</v>
+        <v>1035259.2000007342</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -6768,7 +6734,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>698403.90000073391</v>
+        <v>985259.20000073418</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -6777,415 +6743,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8999999.9999775533</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>9088058.5399775542</v>
-      </c>
-      <c r="U3">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:xdr="http://purl.oclc.org/ooxml/drawingml/spreadsheetDrawing">
-  <dimension ref="A1:U3"/>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="B1" s="259" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="259" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="259" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="259" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="259" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="259" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="259" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="259" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="259" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="259" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="259" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="259" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="259" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="259" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" s="259" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="259" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" s="259" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" s="259" t="s">
-        <v>17</v>
-      </c>
-      <c r="T1" s="259" t="s">
-        <v>18</v>
-      </c>
-      <c r="U1" s="259" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="257">
-        <v>43831</v>
-      </c>
-      <c r="B2">
-        <v>7</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>475794.70000000001</v>
-      </c>
-      <c r="I2">
-        <v>1015561.9</v>
-      </c>
-      <c r="J2">
-        <v>280632</v>
-      </c>
-      <c r="K2">
-        <v>9009.3999999999996</v>
-      </c>
-      <c r="L2">
-        <v>180000</v>
-      </c>
-      <c r="M2">
-        <v>50000</v>
-      </c>
-      <c r="N2">
-        <v>6153.3000000000002</v>
-      </c>
-      <c r="O2">
-        <v>965561.89999999991</v>
-      </c>
-      <c r="P2">
-        <v>409927.99999981304</v>
-      </c>
-      <c r="Q2">
-        <v>0</v>
-      </c>
-      <c r="R2">
-        <v>8229999.9999999963</v>
-      </c>
-      <c r="S2">
-        <v>1</v>
-      </c>
-      <c r="T2">
-        <v>8413026.903511269</v>
-      </c>
-      <c r="U2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="257">
-        <v>44197</v>
-      </c>
-      <c r="B3">
-        <v>7</v>
-      </c>
-      <c r="C3">
-        <v>27000</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>27000</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>7999.9999999998645</v>
-      </c>
-      <c r="H3">
-        <v>478494.70000000001</v>
-      </c>
-      <c r="I3">
-        <v>748403.90000073391</v>
-      </c>
-      <c r="J3">
-        <v>280632</v>
-      </c>
-      <c r="K3">
-        <v>11709.4</v>
-      </c>
-      <c r="L3">
-        <v>180000</v>
-      </c>
-      <c r="M3">
-        <v>50000</v>
-      </c>
-      <c r="N3">
-        <v>6153.3000000000002</v>
-      </c>
-      <c r="O3">
-        <v>698403.90000073391</v>
-      </c>
-      <c r="P3">
-        <v>469427.99999962631</v>
-      </c>
-      <c r="Q3">
-        <v>0</v>
-      </c>
-      <c r="R3">
-        <v>8999999.9999775533</v>
-      </c>
-      <c r="S3">
-        <v>1</v>
-      </c>
-      <c r="T3">
-        <v>9135931.8499775529</v>
-      </c>
-      <c r="U3">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:xdr="http://purl.oclc.org/ooxml/drawingml/spreadsheetDrawing">
-  <dimension ref="A1:U3"/>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="B1" s="266" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="266" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="266" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="266" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="266" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="266" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="266" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="266" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="266" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="266" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="266" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="266" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="266" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="266" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" s="266" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="266" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" s="266" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" s="266" t="s">
-        <v>17</v>
-      </c>
-      <c r="T1" s="266" t="s">
-        <v>18</v>
-      </c>
-      <c r="U1" s="266" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="264">
-        <v>43831</v>
-      </c>
-      <c r="B2">
-        <v>7</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>475794.70000000001</v>
-      </c>
-      <c r="I2">
-        <v>1015561.9</v>
-      </c>
-      <c r="J2">
-        <v>280632</v>
-      </c>
-      <c r="K2">
-        <v>9009.3999999999996</v>
-      </c>
-      <c r="L2">
-        <v>180000</v>
-      </c>
-      <c r="M2">
-        <v>50000</v>
-      </c>
-      <c r="N2">
-        <v>6153.3000000000002</v>
-      </c>
-      <c r="O2">
-        <v>965561.89999999991</v>
-      </c>
-      <c r="P2">
-        <v>409927.99999981304</v>
-      </c>
-      <c r="Q2">
-        <v>0</v>
-      </c>
-      <c r="R2">
-        <v>8229999.9999999963</v>
-      </c>
-      <c r="S2">
-        <v>1</v>
-      </c>
-      <c r="T2">
-        <v>8415215.3935112692</v>
-      </c>
-      <c r="U2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="264">
-        <v>44197</v>
-      </c>
-      <c r="B3">
-        <v>7</v>
-      </c>
-      <c r="C3">
-        <v>27000</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>27000</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>7999.9999999998645</v>
-      </c>
-      <c r="H3">
-        <v>478494.70000000001</v>
-      </c>
-      <c r="I3">
-        <v>938522.70000073418</v>
-      </c>
-      <c r="J3">
-        <v>280632</v>
-      </c>
-      <c r="K3">
-        <v>11709.4</v>
-      </c>
-      <c r="L3">
-        <v>180000</v>
-      </c>
-      <c r="M3">
-        <v>50000</v>
-      </c>
-      <c r="N3">
-        <v>6153.3000000000002</v>
-      </c>
-      <c r="O3">
-        <v>888522.70000073418</v>
-      </c>
-      <c r="P3">
-        <v>469427.99999962631</v>
-      </c>
-      <c r="Q3">
-        <v>0</v>
-      </c>
-      <c r="R3">
-        <v>8999999.9999775533</v>
-      </c>
-      <c r="S3">
-        <v>1</v>
-      </c>
-      <c r="T3">
-        <v>9110981.0259775538</v>
+        <v>8340981.0259991111</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -7288,7 +6852,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1015561.9</v>
+        <v>1112298.3999999999</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -7306,7 +6870,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>965561.89999999991</v>
+        <v>1062298.3999999999</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -7315,13 +6879,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999963</v>
+        <v>8229999.9999999953</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8413142.1275112685</v>
+        <v>8509729.631043829</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -7332,28 +6896,28 @@
         <v>44197</v>
       </c>
       <c r="B3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3">
-        <v>27000</v>
+        <v>0</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>27000</v>
+        <v>0</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>7999.9999999998645</v>
+        <v>0</v>
       </c>
       <c r="H3">
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1285561.8999998129</v>
+        <v>1382298.3999998129</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -7371,22 +6935,22 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1235561.8999998129</v>
+        <v>1332298.3999998129</v>
       </c>
       <c r="P3">
-        <v>469427.99999962631</v>
+        <v>477427.99999962613</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8229999.9999991106</v>
+        <v>10789883.326399432</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>8440604.3459991124</v>
+        <v>11081190.528399434</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -7489,7 +7053,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1015561.9</v>
+        <v>1112298.3999999999</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -7507,7 +7071,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>965561.89999999991</v>
+        <v>1062298.3999999999</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -7516,13 +7080,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999963</v>
+        <v>8229999.9999999953</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8445953.1055112705</v>
+        <v>8515915.8150438312</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -7533,28 +7097,28 @@
         <v>44197</v>
       </c>
       <c r="B3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3">
-        <v>27000</v>
+        <v>0</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>27000</v>
+        <v>0</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>7999.9999999998645</v>
+        <v>0</v>
       </c>
       <c r="H3">
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1285561.8999998129</v>
+        <v>1012298.3999997991</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -7572,22 +7136,22 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1235561.8999998129</v>
+        <v>962298.39999979909</v>
       </c>
       <c r="P3">
-        <v>469427.99999962631</v>
+        <v>477427.99999962613</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>10237282.93242478</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>10511132.814424779</v>
+        <v>8454903.3319991101</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -7690,7 +7254,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1015561.9</v>
+        <v>1112298.3999999999</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -7708,7 +7272,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>965561.89999999991</v>
+        <v>1062298.3999999999</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -7717,13 +7281,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999963</v>
+        <v>8229999.9999999953</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8491662.2595112678</v>
+        <v>8432609.6070438307</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -7734,28 +7298,28 @@
         <v>44197</v>
       </c>
       <c r="B3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>27000</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>27000</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>7999.9999999998645</v>
       </c>
       <c r="H3">
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1285561.8999998129</v>
+        <v>1382298.3999998129</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -7773,22 +7337,22 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1235561.8999998129</v>
+        <v>1332298.3999998129</v>
       </c>
       <c r="P3">
-        <v>477427.99999962613</v>
+        <v>469427.99999962631</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>12234397.571883366</v>
+        <v>10841692.351223463</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>12525704.773883365</v>
+        <v>10989724.979223462</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -7891,7 +7455,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1015561.9</v>
+        <v>1112298.3999999999</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -7909,7 +7473,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>965561.89999999991</v>
+        <v>1062298.3999999999</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -7918,13 +7482,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999963</v>
+        <v>8229999.9999999953</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8496967.8915112689</v>
+        <v>8401487.7850438319</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -7935,28 +7499,28 @@
         <v>44197</v>
       </c>
       <c r="B3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>27000</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>27000</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>7999.9999999998645</v>
       </c>
       <c r="H3">
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>915561.89999979886</v>
+        <v>1012298.3999997991</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -7974,22 +7538,22 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>865561.89999979897</v>
+        <v>962298.39999979909</v>
       </c>
       <c r="P3">
-        <v>477427.99999962613</v>
+        <v>469427.99999962631</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>10681328.641753327</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>10906231.973753328</v>
+        <v>9187857.7959775534</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -8092,7 +7656,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1015561.9</v>
+        <v>1112298.3999999999</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -8110,7 +7674,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>965561.89999999991</v>
+        <v>1062298.3999999999</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -8119,13 +7683,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999963</v>
+        <v>8229999.9999999953</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8416779.8535112683</v>
+        <v>8471797.8030438293</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -8136,28 +7700,28 @@
         <v>44197</v>
       </c>
       <c r="B3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3">
-        <v>27000</v>
+        <v>0</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>27000</v>
+        <v>0</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>7999.9999999998645</v>
+        <v>0</v>
       </c>
       <c r="H3">
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1285561.8999998129</v>
+        <v>845140.40000073391</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -8175,22 +7739,22 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1235561.8999998129</v>
+        <v>795140.40000073379</v>
       </c>
       <c r="P3">
-        <v>469427.99999962631</v>
+        <v>477427.99999962613</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>11012755.625578197</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>11160788.253578197</v>
+        <v>8417833.5499991123</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -8293,7 +7857,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1015561.9</v>
+        <v>1112298.3999999999</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -8311,7 +7875,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>965561.89999999991</v>
+        <v>1062298.3999999999</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -8320,13 +7884,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999963</v>
+        <v>8229999.9999999953</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8381092.5175112681</v>
+        <v>8443633.0190438293</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -8358,7 +7922,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>915561.89999979886</v>
+        <v>1012298.3999997991</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -8376,7 +7940,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>865561.89999979897</v>
+        <v>962298.39999979909</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -8385,13 +7949,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8999999.9999775533</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>9187857.7959775534</v>
+        <v>8380597.6699991105</v>
       </c>
       <c r="U3">
         <v>0</v>

</xml_diff>

<commit_message>
FIRST PASS - June 2020 MTOM Run
Updated Forecast and model output files
Updated ruleset to 3.6.9000 - ruleset fix to  change SNWP outyear schedule distribution to match 24 MS
Updated Model file with proper naming convention. Loaded model file with June data
</commit_message>
<xml_diff>
--- a/Output Data/MtomToCrss_Annual.xlsx
+++ b/Output Data/MtomToCrss_Annual.xlsx
@@ -822,7 +822,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1112298.3999999999</v>
+        <v>1097381.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -840,7 +840,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1062298.3999999999</v>
+        <v>1047381.8000000002</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -849,13 +849,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8476736.365043832</v>
+        <v>8511047.6559112687</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -887,7 +887,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1122816.7</v>
+        <v>1107900.1000000001</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -905,7 +905,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1072816.7</v>
+        <v>1057900.1000000001</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -1023,7 +1023,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1112298.3999999999</v>
+        <v>1097381.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -1041,7 +1041,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1062298.3999999999</v>
+        <v>1047381.8000000002</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -1050,13 +1050,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8440135.4290438313</v>
+        <v>8497172.7439112682</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -1088,7 +1088,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1035259.2000007342</v>
+        <v>1020342.6000007343</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -1106,7 +1106,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>985259.20000073418</v>
+        <v>970342.60000073432</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -1224,7 +1224,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1112298.3999999999</v>
+        <v>1097381.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -1242,7 +1242,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1062298.3999999999</v>
+        <v>1047381.8000000002</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -1251,13 +1251,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8453723.3630438298</v>
+        <v>8507262.7859112676</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -1289,7 +1289,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>845140.40000073391</v>
+        <v>830223.80000073405</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -1307,7 +1307,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>795140.40000073379</v>
+        <v>780223.80000073405</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -1425,7 +1425,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1112298.3999999999</v>
+        <v>1097381.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -1443,7 +1443,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1062298.3999999999</v>
+        <v>1047381.8000000002</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -1452,13 +1452,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8460901.8110438287</v>
+        <v>8502194.0319112688</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -1490,7 +1490,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>845140.40000073391</v>
+        <v>830223.80000073405</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -1508,7 +1508,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>795140.40000073379</v>
+        <v>780223.80000073405</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -1626,7 +1626,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1112298.3999999999</v>
+        <v>1097381.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -1644,7 +1644,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1062298.3999999999</v>
+        <v>1047381.8000000002</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -1653,13 +1653,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8474841.711043831</v>
+        <v>8507763.6739112679</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -1670,28 +1670,28 @@
         <v>44197</v>
       </c>
       <c r="B3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>27000</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>27000</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>7999.9999999998645</v>
       </c>
       <c r="H3">
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1247298.3999999065</v>
+        <v>1232381.7999999067</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -1709,22 +1709,22 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1197298.3999999063</v>
+        <v>1182381.7999999067</v>
       </c>
       <c r="P3">
-        <v>488482.60999962612</v>
+        <v>469427.99999962631</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>9581985.128784582</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>9991803.3527845815</v>
+        <v>8639818.2239991091</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -1827,7 +1827,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1112298.3999999999</v>
+        <v>1097381.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -1845,7 +1845,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1062298.3999999999</v>
+        <v>1047381.8000000002</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -1854,13 +1854,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8457756.0870438293</v>
+        <v>8478109.2419112679</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -1892,7 +1892,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>825001.000000734</v>
+        <v>810084.40000073414</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -1910,7 +1910,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>775001.000000734</v>
+        <v>760084.40000073414</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -1919,13 +1919,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8999999.9999775533</v>
+        <v>8998583.5788952913</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>9132878.8059775531</v>
+        <v>9131462.384895293</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -2028,7 +2028,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1112298.3999999999</v>
+        <v>1097381.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -2046,7 +2046,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1062298.3999999999</v>
+        <v>1047381.8000000002</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -2055,13 +2055,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8427817.3130438291</v>
+        <v>8468854.9979112688</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -2093,7 +2093,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1382298.3999998129</v>
+        <v>1367381.7999998131</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -2111,7 +2111,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1332298.3999998129</v>
+        <v>1317381.7999998131</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -2120,13 +2120,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>10040648.238941355</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>10323068.542941358</v>
+        <v>8512420.3039991111</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -2229,7 +2229,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1112298.3999999999</v>
+        <v>1097381.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -2247,7 +2247,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1062298.3999999999</v>
+        <v>1047381.8000000002</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -2256,13 +2256,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8487279.9670438282</v>
+        <v>8508563.8239112683</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -2273,28 +2273,28 @@
         <v>44197</v>
       </c>
       <c r="B3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>27000</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>27000</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>7999.9999999998645</v>
       </c>
       <c r="H3">
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1382298.3999998129</v>
+        <v>1367381.7999998131</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -2312,10 +2312,10 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1332298.3999998129</v>
+        <v>1317381.7999998131</v>
       </c>
       <c r="P3">
-        <v>466373.38999962609</v>
+        <v>469427.99999962631</v>
       </c>
       <c r="Q3">
         <v>0</v>
@@ -2430,7 +2430,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1112298.3999999999</v>
+        <v>1097381.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -2448,7 +2448,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1062298.3999999999</v>
+        <v>1047381.8000000002</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -2457,13 +2457,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8434164.2090438306</v>
+        <v>8479223.1699112691</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -2495,7 +2495,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1382298.3999998129</v>
+        <v>1367381.7999998131</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -2513,7 +2513,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1332298.3999998129</v>
+        <v>1317381.7999998131</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -2522,13 +2522,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>10980119.270413974</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>11041790.956413973</v>
+        <v>9061671.6859775539</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -2631,7 +2631,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1112298.3999999999</v>
+        <v>1097381.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -2649,7 +2649,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1062298.3999999999</v>
+        <v>1047381.8000000002</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -2658,13 +2658,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8407710.7450438309</v>
+        <v>8450258.1059112679</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -2696,7 +2696,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1382298.3999998129</v>
+        <v>1367381.7999998131</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -2714,7 +2714,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1332298.3999998129</v>
+        <v>1317381.7999998131</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -2832,7 +2832,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1112298.3999999999</v>
+        <v>1097381.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -2850,7 +2850,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1062298.3999999999</v>
+        <v>1047381.8000000002</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -2859,13 +2859,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8372019.3150438312</v>
+        <v>8427288.725911269</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -2897,7 +2897,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1382298.3999998129</v>
+        <v>1367381.7999998131</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -2915,7 +2915,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1332298.3999998129</v>
+        <v>1317381.7999998131</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -3033,7 +3033,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1112298.3999999999</v>
+        <v>1097381.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -3051,7 +3051,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1062298.3999999999</v>
+        <v>1047381.8000000002</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -3060,13 +3060,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8448060.7250438295</v>
+        <v>8488475.4199112691</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -3098,7 +3098,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1382298.3999998129</v>
+        <v>1367381.7999998131</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -3116,7 +3116,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1332298.3999998129</v>
+        <v>1317381.7999998131</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -3234,7 +3234,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1112298.3999999999</v>
+        <v>1097381.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -3252,7 +3252,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1062298.3999999999</v>
+        <v>1047381.8000000002</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -3261,13 +3261,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8465117.8150438294</v>
+        <v>8506043.8959112689</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -3299,7 +3299,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1247298.3999999065</v>
+        <v>1232381.7999999067</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -3317,7 +3317,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1197298.3999999063</v>
+        <v>1182381.7999999067</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -3435,7 +3435,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1112298.3999999999</v>
+        <v>1097381.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -3453,7 +3453,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1062298.3999999999</v>
+        <v>1047381.8000000002</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -3462,13 +3462,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8485509.3950438295</v>
+        <v>8512780.7359112687</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -3500,7 +3500,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1012298.3999997991</v>
+        <v>997381.79999979911</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -3518,7 +3518,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>962298.39999979909</v>
+        <v>947381.799999799</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -3636,7 +3636,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1112298.3999999999</v>
+        <v>1097381.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -3654,7 +3654,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1062298.3999999999</v>
+        <v>1047381.8000000002</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -3663,13 +3663,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8423647.4850438293</v>
+        <v>8463164.2859112695</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -3701,7 +3701,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1012298.3999997991</v>
+        <v>997381.79999979911</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -3719,7 +3719,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>962298.39999979909</v>
+        <v>947381.799999799</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -3837,7 +3837,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1112298.3999999999</v>
+        <v>1097381.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -3855,7 +3855,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1062298.3999999999</v>
+        <v>1047381.8000000002</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -3864,13 +3864,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8457793.5850438289</v>
+        <v>8493511.0859112665</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -3902,7 +3902,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1247298.3999999065</v>
+        <v>1232381.7999999067</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -3920,7 +3920,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1197298.3999999063</v>
+        <v>1182381.7999999067</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -4038,7 +4038,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1112298.3999999999</v>
+        <v>1097381.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -4056,7 +4056,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1062298.3999999999</v>
+        <v>1047381.8000000002</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -4065,13 +4065,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8466864.5950438306</v>
+        <v>8507788.6159112677</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -4103,7 +4103,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1112298.3999999999</v>
+        <v>1097381.8</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -4121,7 +4121,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1062298.3999999999</v>
+        <v>1047381.8000000002</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -4239,7 +4239,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1112298.3999999999</v>
+        <v>1097381.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -4257,7 +4257,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1062298.3999999999</v>
+        <v>1047381.8000000002</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -4266,13 +4266,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8418527.6750438306</v>
+        <v>8463552.2559112683</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -4304,7 +4304,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1247298.3999999065</v>
+        <v>1232381.7999999067</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -4322,7 +4322,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1197298.3999999063</v>
+        <v>1182381.7999999067</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -4440,7 +4440,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1112298.3999999999</v>
+        <v>1097381.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -4458,7 +4458,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1062298.3999999999</v>
+        <v>1047381.8000000002</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -4467,13 +4467,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8461231.1150438301</v>
+        <v>8507671.8059112672</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -4505,7 +4505,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1382298.3999998129</v>
+        <v>1367381.7999998131</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -4523,7 +4523,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1332298.3999998129</v>
+        <v>1317381.7999998131</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -4532,13 +4532,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8229999.9999991106</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>8493906.2799991108</v>
+        <v>9263906.2799775526</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -4641,7 +4641,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1112298.3999999999</v>
+        <v>1097381.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -4659,7 +4659,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1062298.3999999999</v>
+        <v>1047381.8000000002</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -4668,13 +4668,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8516389.5350438301</v>
+        <v>8552982.6559112687</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -4706,7 +4706,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1012298.3999997991</v>
+        <v>997381.79999979911</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -4724,7 +4724,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>962298.39999979909</v>
+        <v>947381.799999799</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -4842,7 +4842,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1112298.3999999999</v>
+        <v>1097381.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -4860,7 +4860,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1062298.3999999999</v>
+        <v>1047381.8000000002</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -4869,13 +4869,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8441629.5250438284</v>
+        <v>8487215.0259112678</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -4907,7 +4907,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>845140.40000073391</v>
+        <v>830223.80000073405</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -4925,7 +4925,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>795140.40000073379</v>
+        <v>780223.80000073405</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -5043,7 +5043,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1112298.3999999999</v>
+        <v>1097381.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -5061,7 +5061,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1062298.3999999999</v>
+        <v>1047381.8000000002</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -5070,13 +5070,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8481463.2850438301</v>
+        <v>8515189.5859112684</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -5108,7 +5108,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1012298.3999997991</v>
+        <v>997381.79999979911</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -5126,7 +5126,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>962298.39999979909</v>
+        <v>947381.799999799</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -5244,7 +5244,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1112298.3999999999</v>
+        <v>1097381.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -5262,7 +5262,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1062298.3999999999</v>
+        <v>1047381.8000000002</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -5271,13 +5271,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8473109.0950438306</v>
+        <v>8503122.2399112694</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -5309,7 +5309,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1382298.3999998129</v>
+        <v>1367381.7999998131</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -5327,7 +5327,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1332298.3999998129</v>
+        <v>1317381.7999998131</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -5336,13 +5336,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>10129573.009568132</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>10403422.891568134</v>
+        <v>8503849.8819991108</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -5445,7 +5445,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1112298.3999999999</v>
+        <v>1097381.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -5463,7 +5463,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1062298.3999999999</v>
+        <v>1047381.8000000002</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -5472,13 +5472,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8462180.8650438301</v>
+        <v>8508835.1759112664</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -5510,7 +5510,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1112298.3999999999</v>
+        <v>1097381.8</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -5528,7 +5528,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1062298.3999999999</v>
+        <v>1047381.8000000002</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -5646,7 +5646,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1112298.3999999999</v>
+        <v>1097381.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -5664,7 +5664,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1062298.3999999999</v>
+        <v>1047381.8000000002</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -5673,13 +5673,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8460977.3650438301</v>
+        <v>8501047.2059112675</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -5711,7 +5711,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1382298.3999998129</v>
+        <v>1367381.7999998131</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -5729,7 +5729,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1332298.3999998129</v>
+        <v>1317381.7999998131</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -5738,13 +5738,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>10604397.497815507</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>10817092.507815503</v>
+        <v>8442695.0099991094</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -5847,7 +5847,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1112298.3999999999</v>
+        <v>1097381.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -5865,7 +5865,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1062298.3999999999</v>
+        <v>1047381.8000000002</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -5874,13 +5874,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8494576.545043828</v>
+        <v>8525662.935911268</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -5912,7 +5912,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1112298.3999999999</v>
+        <v>1097381.8</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -5930,7 +5930,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1062298.3999999999</v>
+        <v>1047381.8000000002</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -5939,13 +5939,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8496555.0153858438</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>8557680.755385844</v>
+        <v>8291125.7399991108</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -6048,7 +6048,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1112298.3999999999</v>
+        <v>1097381.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -6066,7 +6066,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1062298.3999999999</v>
+        <v>1047381.8000000002</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -6075,13 +6075,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8407172.2750438303</v>
+        <v>8452809.3759112693</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -6113,7 +6113,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1012298.3999997991</v>
+        <v>997381.79999979911</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -6131,7 +6131,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>962298.39999979909</v>
+        <v>947381.799999799</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -6249,7 +6249,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1112298.3999999999</v>
+        <v>1097381.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -6267,7 +6267,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1062298.3999999999</v>
+        <v>1047381.8000000002</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -6276,13 +6276,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8428209.1050438285</v>
+        <v>8477587.4659112673</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -6314,7 +6314,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>845140.40000073391</v>
+        <v>830223.80000073405</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -6332,7 +6332,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>795140.40000073379</v>
+        <v>780223.80000073405</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -6450,7 +6450,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1112298.3999999999</v>
+        <v>1097381.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -6468,7 +6468,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1062298.3999999999</v>
+        <v>1047381.8000000002</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -6477,13 +6477,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8446972.3950438313</v>
+        <v>8492596.9259112701</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -6515,7 +6515,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>845140.40000073391</v>
+        <v>830223.80000073405</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -6533,7 +6533,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>795140.40000073379</v>
+        <v>780223.80000073405</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -6651,7 +6651,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1112298.3999999999</v>
+        <v>1097381.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -6669,7 +6669,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1062298.3999999999</v>
+        <v>1047381.8000000002</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -6678,13 +6678,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8449324.9750438314</v>
+        <v>8490537.8459112681</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -6716,7 +6716,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1035259.2000007342</v>
+        <v>1020342.6000007343</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -6734,7 +6734,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>985259.20000073418</v>
+        <v>970342.60000073432</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -6852,7 +6852,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1112298.3999999999</v>
+        <v>1097381.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -6870,7 +6870,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1062298.3999999999</v>
+        <v>1047381.8000000002</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -6879,13 +6879,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8509729.631043829</v>
+        <v>8517623.5499112662</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -6917,7 +6917,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1382298.3999998129</v>
+        <v>1367381.7999998131</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -6935,7 +6935,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1332298.3999998129</v>
+        <v>1317381.7999998131</v>
       </c>
       <c r="P3">
         <v>477427.99999962613</v>
@@ -6944,13 +6944,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>10789883.326399432</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>11081190.528399434</v>
+        <v>8521307.2019991111</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -7053,7 +7053,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1112298.3999999999</v>
+        <v>1097381.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -7071,7 +7071,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1062298.3999999999</v>
+        <v>1047381.8000000002</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -7080,13 +7080,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8515915.8150438312</v>
+        <v>8557603.3139112685</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -7118,7 +7118,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1012298.3999997991</v>
+        <v>997381.79999979911</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -7136,7 +7136,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>962298.39999979909</v>
+        <v>947381.799999799</v>
       </c>
       <c r="P3">
         <v>477427.99999962613</v>
@@ -7254,7 +7254,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1112298.3999999999</v>
+        <v>1097381.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -7272,7 +7272,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1062298.3999999999</v>
+        <v>1047381.8000000002</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -7281,13 +7281,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8432609.6070438307</v>
+        <v>8483491.0659112688</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -7319,7 +7319,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1382298.3999998129</v>
+        <v>1367381.7999998131</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -7337,7 +7337,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1332298.3999998129</v>
+        <v>1317381.7999998131</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -7346,13 +7346,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>10841692.351223463</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>10989724.979223462</v>
+        <v>8378032.6279991101</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -7455,7 +7455,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1112298.3999999999</v>
+        <v>1097381.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -7473,7 +7473,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1062298.3999999999</v>
+        <v>1047381.8000000002</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -7482,13 +7482,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8401487.7850438319</v>
+        <v>8467673.9839112684</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -7520,7 +7520,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1012298.3999997991</v>
+        <v>997381.79999979911</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -7538,7 +7538,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>962298.39999979909</v>
+        <v>947381.799999799</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -7656,7 +7656,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1112298.3999999999</v>
+        <v>1097381.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -7674,7 +7674,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1062298.3999999999</v>
+        <v>1047381.8000000002</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -7683,13 +7683,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8471797.8030438293</v>
+        <v>8512145.5139112677</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -7700,28 +7700,28 @@
         <v>44197</v>
       </c>
       <c r="B3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>27000</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>27000</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>7999.9999999998645</v>
       </c>
       <c r="H3">
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>845140.40000073391</v>
+        <v>830223.80000073405</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -7739,10 +7739,10 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>795140.40000073379</v>
+        <v>780223.80000073405</v>
       </c>
       <c r="P3">
-        <v>477427.99999962613</v>
+        <v>469427.99999962631</v>
       </c>
       <c r="Q3">
         <v>0</v>
@@ -7857,7 +7857,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1112298.3999999999</v>
+        <v>1097381.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -7875,7 +7875,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1062298.3999999999</v>
+        <v>1047381.8000000002</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -7884,13 +7884,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8443633.0190438293</v>
+        <v>8479302.3659112677</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -7922,7 +7922,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1012298.3999997991</v>
+        <v>997381.79999979911</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -7940,7 +7940,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>962298.39999979909</v>
+        <v>947381.799999799</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>

</xml_diff>

<commit_message>
FIRST PASS - June Run
Updated output files with first pass of June MTOM run
UPdated integrated development model with various updates to get model to run (changes to ICS slots, change to evap tax percent, updated max controlled release at Taylor Park)
Updated MX percentages in shortage monthly percent table to match 2021 distribution
Added development ruleset used on June operational run with updated SNWA distribution
</commit_message>
<xml_diff>
--- a/Output Data/MtomToCrss_Annual.xlsx
+++ b/Output Data/MtomToCrss_Annual.xlsx
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:xdr="http://purl.oclc.org/ooxml/drawingml/spreadsheetDrawing" count="720" uniqueCount="20">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:xdr="http://purl.oclc.org/ooxml/drawingml/spreadsheetDrawing" count="756" uniqueCount="21">
   <si>
     <t>DCP BWSCP Flags.LB DCP BWSCP</t>
   </si>
@@ -105,6 +105,9 @@
   </si>
   <si>
     <t>PowellOperation.Compact Point Volume</t>
+  </si>
+  <si>
+    <t>NaN</t>
   </si>
   <si>
     <t>SystemConditions.LBShortageTier</t>
@@ -793,7 +796,7 @@
         <v>18</v>
       </c>
       <c r="U1" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2">
@@ -822,7 +825,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1112298.3999999999</v>
+        <v>1097381.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -840,7 +843,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1062298.3999999999</v>
+        <v>1047381.8000000002</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -849,13 +852,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
-      <c r="T2">
-        <v>8476736.365043832</v>
+      <c r="T2" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -887,7 +890,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1122816.7</v>
+        <v>1107900.1000000001</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -905,7 +908,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1072816.7</v>
+        <v>1057900.1000000001</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -994,7 +997,7 @@
         <v>18</v>
       </c>
       <c r="U1" s="70" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2">
@@ -1023,7 +1026,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1112298.3999999999</v>
+        <v>1097381.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -1041,7 +1044,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1062298.3999999999</v>
+        <v>1047381.8000000002</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -1050,13 +1053,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
-      <c r="T2">
-        <v>8440135.4290438313</v>
+      <c r="T2" s="69" t="s">
+        <v>19</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -1088,7 +1091,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1035259.2000007342</v>
+        <v>1020342.6000007343</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -1106,7 +1109,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>985259.20000073418</v>
+        <v>970342.60000073432</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -1195,7 +1198,7 @@
         <v>18</v>
       </c>
       <c r="U1" s="77" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2">
@@ -1224,7 +1227,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1112298.3999999999</v>
+        <v>1097381.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -1242,7 +1245,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1062298.3999999999</v>
+        <v>1047381.8000000002</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -1251,13 +1254,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
-      <c r="T2">
-        <v>8453723.3630438298</v>
+      <c r="T2" s="76" t="s">
+        <v>19</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -1289,7 +1292,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>845140.40000073391</v>
+        <v>830223.80000073405</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -1307,7 +1310,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>795140.40000073379</v>
+        <v>780223.80000073405</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -1396,7 +1399,7 @@
         <v>18</v>
       </c>
       <c r="U1" s="84" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2">
@@ -1425,7 +1428,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1112298.3999999999</v>
+        <v>1097381.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -1443,7 +1446,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1062298.3999999999</v>
+        <v>1047381.8000000002</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -1452,13 +1455,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
-      <c r="T2">
-        <v>8460901.8110438287</v>
+      <c r="T2" s="83" t="s">
+        <v>19</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -1490,7 +1493,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>845140.40000073391</v>
+        <v>830223.80000073405</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -1508,7 +1511,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>795140.40000073379</v>
+        <v>780223.80000073405</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -1597,7 +1600,7 @@
         <v>18</v>
       </c>
       <c r="U1" s="91" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2">
@@ -1626,7 +1629,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1112298.3999999999</v>
+        <v>1097381.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -1644,7 +1647,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1062298.3999999999</v>
+        <v>1047381.8000000002</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -1653,13 +1656,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
-      <c r="T2">
-        <v>8474841.711043831</v>
+      <c r="T2" s="90" t="s">
+        <v>19</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -1670,28 +1673,28 @@
         <v>44197</v>
       </c>
       <c r="B3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>27000</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>27000</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>7999.9999999998645</v>
       </c>
       <c r="H3">
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1247298.3999999065</v>
+        <v>1232381.7999999067</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -1709,22 +1712,22 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1197298.3999999063</v>
+        <v>1182381.7999999067</v>
       </c>
       <c r="P3">
-        <v>488482.60999962612</v>
+        <v>469427.99999962631</v>
       </c>
       <c r="Q3">
         <v>0</v>
       </c>
       <c r="R3">
-        <v>9581985.128784582</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>9991803.3527845815</v>
+        <v>8639818.2239991091</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -1798,7 +1801,7 @@
         <v>18</v>
       </c>
       <c r="U1" s="98" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2">
@@ -1827,7 +1830,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1112298.3999999999</v>
+        <v>1097381.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -1845,7 +1848,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1062298.3999999999</v>
+        <v>1047381.8000000002</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -1854,13 +1857,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
-      <c r="T2">
-        <v>8457756.0870438293</v>
+      <c r="T2" s="97" t="s">
+        <v>19</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -1892,7 +1895,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>825001.000000734</v>
+        <v>810084.40000073414</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -1910,7 +1913,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>775001.000000734</v>
+        <v>760084.40000073414</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -1999,7 +2002,7 @@
         <v>18</v>
       </c>
       <c r="U1" s="105" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2">
@@ -2028,7 +2031,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1112298.3999999999</v>
+        <v>1097381.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -2046,7 +2049,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1062298.3999999999</v>
+        <v>1047381.8000000002</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -2055,13 +2058,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
-      <c r="T2">
-        <v>8427817.3130438291</v>
+      <c r="T2" s="104" t="s">
+        <v>19</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -2093,7 +2096,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1382298.3999998129</v>
+        <v>1367381.7999998131</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -2111,7 +2114,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1332298.3999998129</v>
+        <v>1317381.7999998131</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -2120,13 +2123,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>10040648.238941355</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>10323068.542941358</v>
+        <v>8512420.3039991111</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -2200,7 +2203,7 @@
         <v>18</v>
       </c>
       <c r="U1" s="112" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2">
@@ -2229,7 +2232,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1112298.3999999999</v>
+        <v>1097381.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -2247,7 +2250,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1062298.3999999999</v>
+        <v>1047381.8000000002</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -2256,13 +2259,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
-      <c r="T2">
-        <v>8487279.9670438282</v>
+      <c r="T2" s="111" t="s">
+        <v>19</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -2273,28 +2276,28 @@
         <v>44197</v>
       </c>
       <c r="B3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>27000</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>27000</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>7999.9999999998645</v>
       </c>
       <c r="H3">
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1382298.3999998129</v>
+        <v>1367381.7999998131</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -2312,10 +2315,10 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1332298.3999998129</v>
+        <v>1317381.7999998131</v>
       </c>
       <c r="P3">
-        <v>466373.38999962609</v>
+        <v>469427.99999962631</v>
       </c>
       <c r="Q3">
         <v>0</v>
@@ -2401,7 +2404,7 @@
         <v>18</v>
       </c>
       <c r="U1" s="119" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2">
@@ -2430,7 +2433,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1112298.3999999999</v>
+        <v>1097381.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -2448,7 +2451,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1062298.3999999999</v>
+        <v>1047381.8000000002</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -2457,13 +2460,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
-      <c r="T2">
-        <v>8434164.2090438306</v>
+      <c r="T2" s="118" t="s">
+        <v>19</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -2495,7 +2498,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1382298.3999998129</v>
+        <v>1367381.7999998131</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -2513,7 +2516,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1332298.3999998129</v>
+        <v>1317381.7999998131</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -2522,13 +2525,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>10980119.270413974</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>11041790.956413973</v>
+        <v>9061671.6859775539</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -2602,7 +2605,7 @@
         <v>18</v>
       </c>
       <c r="U1" s="126" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2">
@@ -2631,7 +2634,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1112298.3999999999</v>
+        <v>1097381.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -2649,7 +2652,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1062298.3999999999</v>
+        <v>1047381.8000000002</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -2658,13 +2661,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
-      <c r="T2">
-        <v>8407710.7450438309</v>
+      <c r="T2" s="125" t="s">
+        <v>19</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -2696,7 +2699,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1382298.3999998129</v>
+        <v>1367381.7999998131</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -2714,7 +2717,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1332298.3999998129</v>
+        <v>1317381.7999998131</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -2803,7 +2806,7 @@
         <v>18</v>
       </c>
       <c r="U1" s="133" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2">
@@ -2832,7 +2835,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1112298.3999999999</v>
+        <v>1097381.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -2850,7 +2853,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1062298.3999999999</v>
+        <v>1047381.8000000002</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -2859,13 +2862,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
-      <c r="T2">
-        <v>8372019.3150438312</v>
+      <c r="T2" s="132" t="s">
+        <v>19</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -2897,7 +2900,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1382298.3999998129</v>
+        <v>1367381.7999998131</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -2915,7 +2918,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1332298.3999998129</v>
+        <v>1317381.7999998131</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -3004,7 +3007,7 @@
         <v>18</v>
       </c>
       <c r="U1" s="14" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2">
@@ -3033,7 +3036,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1112298.3999999999</v>
+        <v>1097381.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -3051,7 +3054,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1062298.3999999999</v>
+        <v>1047381.8000000002</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -3060,13 +3063,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
-      <c r="T2">
-        <v>8448060.7250438295</v>
+      <c r="T2" s="13" t="s">
+        <v>19</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -3098,7 +3101,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1382298.3999998129</v>
+        <v>1367381.7999998131</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -3116,7 +3119,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1332298.3999998129</v>
+        <v>1317381.7999998131</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -3205,7 +3208,7 @@
         <v>18</v>
       </c>
       <c r="U1" s="140" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2">
@@ -3234,7 +3237,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1112298.3999999999</v>
+        <v>1097381.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -3252,7 +3255,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1062298.3999999999</v>
+        <v>1047381.8000000002</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -3261,13 +3264,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
-      <c r="T2">
-        <v>8465117.8150438294</v>
+      <c r="T2" s="139" t="s">
+        <v>19</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -3299,7 +3302,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1247298.3999999065</v>
+        <v>1232381.7999999067</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -3317,7 +3320,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1197298.3999999063</v>
+        <v>1182381.7999999067</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -3406,7 +3409,7 @@
         <v>18</v>
       </c>
       <c r="U1" s="147" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2">
@@ -3435,7 +3438,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1112298.3999999999</v>
+        <v>1097381.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -3453,7 +3456,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1062298.3999999999</v>
+        <v>1047381.8000000002</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -3462,13 +3465,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
-      <c r="T2">
-        <v>8485509.3950438295</v>
+      <c r="T2" s="146" t="s">
+        <v>19</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -3500,7 +3503,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1012298.3999997991</v>
+        <v>997381.79999979911</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -3518,7 +3521,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>962298.39999979909</v>
+        <v>947381.799999799</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -3607,7 +3610,7 @@
         <v>18</v>
       </c>
       <c r="U1" s="154" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2">
@@ -3636,7 +3639,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1112298.3999999999</v>
+        <v>1097381.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -3654,7 +3657,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1062298.3999999999</v>
+        <v>1047381.8000000002</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -3663,13 +3666,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
-      <c r="T2">
-        <v>8423647.4850438293</v>
+      <c r="T2" s="153" t="s">
+        <v>19</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -3701,7 +3704,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1012298.3999997991</v>
+        <v>997381.79999979911</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -3719,7 +3722,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>962298.39999979909</v>
+        <v>947381.799999799</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -3808,7 +3811,7 @@
         <v>18</v>
       </c>
       <c r="U1" s="161" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2">
@@ -3837,7 +3840,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1112298.3999999999</v>
+        <v>1097381.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -3855,7 +3858,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1062298.3999999999</v>
+        <v>1047381.8000000002</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -3864,13 +3867,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
-      <c r="T2">
-        <v>8457793.5850438289</v>
+      <c r="T2" s="160" t="s">
+        <v>19</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -3902,7 +3905,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1247298.3999999065</v>
+        <v>1232381.7999999067</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -3920,7 +3923,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1197298.3999999063</v>
+        <v>1182381.7999999067</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -4009,7 +4012,7 @@
         <v>18</v>
       </c>
       <c r="U1" s="168" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2">
@@ -4038,7 +4041,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1112298.3999999999</v>
+        <v>1097381.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -4056,7 +4059,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1062298.3999999999</v>
+        <v>1047381.8000000002</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -4065,13 +4068,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
-      <c r="T2">
-        <v>8466864.5950438306</v>
+      <c r="T2" s="167" t="s">
+        <v>19</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -4103,7 +4106,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1112298.3999999999</v>
+        <v>1097381.8</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -4121,7 +4124,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1062298.3999999999</v>
+        <v>1047381.8000000002</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -4210,7 +4213,7 @@
         <v>18</v>
       </c>
       <c r="U1" s="175" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2">
@@ -4239,7 +4242,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1112298.3999999999</v>
+        <v>1097381.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -4257,7 +4260,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1062298.3999999999</v>
+        <v>1047381.8000000002</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -4266,13 +4269,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
-      <c r="T2">
-        <v>8418527.6750438306</v>
+      <c r="T2" s="174" t="s">
+        <v>19</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -4304,7 +4307,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1247298.3999999065</v>
+        <v>1232381.7999999067</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -4322,7 +4325,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1197298.3999999063</v>
+        <v>1182381.7999999067</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -4411,7 +4414,7 @@
         <v>18</v>
       </c>
       <c r="U1" s="182" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2">
@@ -4440,7 +4443,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1112298.3999999999</v>
+        <v>1097381.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -4458,7 +4461,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1062298.3999999999</v>
+        <v>1047381.8000000002</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -4467,13 +4470,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
-      <c r="T2">
-        <v>8461231.1150438301</v>
+      <c r="T2" s="181" t="s">
+        <v>19</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -4505,7 +4508,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1382298.3999998129</v>
+        <v>1367381.7999998131</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -4523,7 +4526,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1332298.3999998129</v>
+        <v>1317381.7999998131</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -4532,13 +4535,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8229999.9999991106</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>8493906.2799991108</v>
+        <v>9263906.2799775526</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -4612,7 +4615,7 @@
         <v>18</v>
       </c>
       <c r="U1" s="189" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2">
@@ -4641,7 +4644,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1112298.3999999999</v>
+        <v>1097381.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -4659,7 +4662,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1062298.3999999999</v>
+        <v>1047381.8000000002</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -4668,13 +4671,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
-      <c r="T2">
-        <v>8516389.5350438301</v>
+      <c r="T2" s="188" t="s">
+        <v>19</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -4706,7 +4709,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1012298.3999997991</v>
+        <v>997381.79999979911</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -4724,7 +4727,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>962298.39999979909</v>
+        <v>947381.799999799</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -4813,7 +4816,7 @@
         <v>18</v>
       </c>
       <c r="U1" s="196" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2">
@@ -4842,7 +4845,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1112298.3999999999</v>
+        <v>1097381.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -4860,7 +4863,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1062298.3999999999</v>
+        <v>1047381.8000000002</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -4869,13 +4872,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
-      <c r="T2">
-        <v>8441629.5250438284</v>
+      <c r="T2" s="195" t="s">
+        <v>19</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -4907,7 +4910,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>845140.40000073391</v>
+        <v>830223.80000073405</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -4925,7 +4928,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>795140.40000073379</v>
+        <v>780223.80000073405</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -5014,7 +5017,7 @@
         <v>18</v>
       </c>
       <c r="U1" s="203" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2">
@@ -5043,7 +5046,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1112298.3999999999</v>
+        <v>1097381.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -5061,7 +5064,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1062298.3999999999</v>
+        <v>1047381.8000000002</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -5070,13 +5073,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
-      <c r="T2">
-        <v>8481463.2850438301</v>
+      <c r="T2" s="202" t="s">
+        <v>19</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -5108,7 +5111,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1012298.3999997991</v>
+        <v>997381.79999979911</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -5126,7 +5129,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>962298.39999979909</v>
+        <v>947381.799999799</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -5215,7 +5218,7 @@
         <v>18</v>
       </c>
       <c r="U1" s="21" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2">
@@ -5244,7 +5247,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1112298.3999999999</v>
+        <v>1097381.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -5262,7 +5265,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1062298.3999999999</v>
+        <v>1047381.8000000002</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -5271,13 +5274,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
-      <c r="T2">
-        <v>8473109.0950438306</v>
+      <c r="T2" s="20" t="s">
+        <v>19</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -5309,7 +5312,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1382298.3999998129</v>
+        <v>1367381.7999998131</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -5327,7 +5330,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1332298.3999998129</v>
+        <v>1317381.7999998131</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -5336,13 +5339,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>10129573.009568132</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>10403422.891568134</v>
+        <v>8503849.8819991108</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -5416,7 +5419,7 @@
         <v>18</v>
       </c>
       <c r="U1" s="210" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2">
@@ -5445,7 +5448,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1112298.3999999999</v>
+        <v>1097381.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -5463,7 +5466,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1062298.3999999999</v>
+        <v>1047381.8000000002</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -5472,13 +5475,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
-      <c r="T2">
-        <v>8462180.8650438301</v>
+      <c r="T2" s="209" t="s">
+        <v>19</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -5510,7 +5513,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1112298.3999999999</v>
+        <v>1097381.8</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -5528,7 +5531,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1062298.3999999999</v>
+        <v>1047381.8000000002</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -5617,7 +5620,7 @@
         <v>18</v>
       </c>
       <c r="U1" s="217" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2">
@@ -5646,7 +5649,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1112298.3999999999</v>
+        <v>1097381.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -5664,7 +5667,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1062298.3999999999</v>
+        <v>1047381.8000000002</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -5673,13 +5676,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
-      <c r="T2">
-        <v>8460977.3650438301</v>
+      <c r="T2" s="216" t="s">
+        <v>19</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -5711,7 +5714,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1382298.3999998129</v>
+        <v>1367381.7999998131</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -5729,7 +5732,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1332298.3999998129</v>
+        <v>1317381.7999998131</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -5738,13 +5741,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>10604397.497815507</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>10817092.507815503</v>
+        <v>8442695.0099991094</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -5818,7 +5821,7 @@
         <v>18</v>
       </c>
       <c r="U1" s="224" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2">
@@ -5847,7 +5850,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1112298.3999999999</v>
+        <v>1097381.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -5865,7 +5868,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1062298.3999999999</v>
+        <v>1047381.8000000002</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -5874,13 +5877,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
-      <c r="T2">
-        <v>8494576.545043828</v>
+      <c r="T2" s="223" t="s">
+        <v>19</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -5912,7 +5915,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1112298.3999999999</v>
+        <v>1097381.8</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -5930,7 +5933,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1062298.3999999999</v>
+        <v>1047381.8000000002</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -5939,13 +5942,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8496555.0153858438</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>8557680.755385844</v>
+        <v>8291125.7399991108</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -6019,7 +6022,7 @@
         <v>18</v>
       </c>
       <c r="U1" s="231" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2">
@@ -6048,7 +6051,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1112298.3999999999</v>
+        <v>1097381.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -6066,7 +6069,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1062298.3999999999</v>
+        <v>1047381.8000000002</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -6075,13 +6078,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
-      <c r="T2">
-        <v>8407172.2750438303</v>
+      <c r="T2" s="230" t="s">
+        <v>19</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -6113,7 +6116,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1012298.3999997991</v>
+        <v>997381.79999979911</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -6131,7 +6134,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>962298.39999979909</v>
+        <v>947381.799999799</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -6220,7 +6223,7 @@
         <v>18</v>
       </c>
       <c r="U1" s="238" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2">
@@ -6249,7 +6252,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1112298.3999999999</v>
+        <v>1097381.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -6267,7 +6270,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1062298.3999999999</v>
+        <v>1047381.8000000002</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -6276,13 +6279,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
-      <c r="T2">
-        <v>8428209.1050438285</v>
+      <c r="T2" s="237" t="s">
+        <v>19</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -6314,7 +6317,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>845140.40000073391</v>
+        <v>830223.80000073405</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -6332,7 +6335,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>795140.40000073379</v>
+        <v>780223.80000073405</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -6421,7 +6424,7 @@
         <v>18</v>
       </c>
       <c r="U1" s="245" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2">
@@ -6450,7 +6453,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1112298.3999999999</v>
+        <v>1097381.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -6468,7 +6471,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1062298.3999999999</v>
+        <v>1047381.8000000002</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -6477,13 +6480,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
-      <c r="T2">
-        <v>8446972.3950438313</v>
+      <c r="T2" s="244" t="s">
+        <v>19</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -6515,7 +6518,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>845140.40000073391</v>
+        <v>830223.80000073405</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -6533,7 +6536,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>795140.40000073379</v>
+        <v>780223.80000073405</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -6622,7 +6625,7 @@
         <v>18</v>
       </c>
       <c r="U1" s="252" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2">
@@ -6651,7 +6654,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1112298.3999999999</v>
+        <v>1097381.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -6669,7 +6672,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1062298.3999999999</v>
+        <v>1047381.8000000002</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -6678,13 +6681,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
-      <c r="T2">
-        <v>8449324.9750438314</v>
+      <c r="T2" s="251" t="s">
+        <v>19</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -6716,7 +6719,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1035259.2000007342</v>
+        <v>1020342.6000007343</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -6734,7 +6737,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>985259.20000073418</v>
+        <v>970342.60000073432</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -6823,7 +6826,7 @@
         <v>18</v>
       </c>
       <c r="U1" s="28" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2">
@@ -6852,7 +6855,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1112298.3999999999</v>
+        <v>1097381.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -6870,7 +6873,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1062298.3999999999</v>
+        <v>1047381.8000000002</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -6879,13 +6882,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
-      <c r="T2">
-        <v>8509729.631043829</v>
+      <c r="T2" s="27" t="s">
+        <v>19</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -6917,7 +6920,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1382298.3999998129</v>
+        <v>1367381.7999998131</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -6935,7 +6938,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1332298.3999998129</v>
+        <v>1317381.7999998131</v>
       </c>
       <c r="P3">
         <v>477427.99999962613</v>
@@ -6944,13 +6947,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>10789883.326399432</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>11081190.528399434</v>
+        <v>8521307.2019991111</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -7024,7 +7027,7 @@
         <v>18</v>
       </c>
       <c r="U1" s="35" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2">
@@ -7053,7 +7056,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1112298.3999999999</v>
+        <v>1097381.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -7071,7 +7074,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1062298.3999999999</v>
+        <v>1047381.8000000002</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -7080,13 +7083,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
-      <c r="T2">
-        <v>8515915.8150438312</v>
+      <c r="T2" s="34" t="s">
+        <v>19</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -7118,7 +7121,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1012298.3999997991</v>
+        <v>997381.79999979911</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -7136,7 +7139,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>962298.39999979909</v>
+        <v>947381.799999799</v>
       </c>
       <c r="P3">
         <v>477427.99999962613</v>
@@ -7225,7 +7228,7 @@
         <v>18</v>
       </c>
       <c r="U1" s="42" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2">
@@ -7254,7 +7257,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1112298.3999999999</v>
+        <v>1097381.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -7272,7 +7275,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1062298.3999999999</v>
+        <v>1047381.8000000002</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -7281,13 +7284,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
-      <c r="T2">
-        <v>8432609.6070438307</v>
+      <c r="T2" s="41" t="s">
+        <v>19</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -7319,7 +7322,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1382298.3999998129</v>
+        <v>1367381.7999998131</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -7337,7 +7340,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1332298.3999998129</v>
+        <v>1317381.7999998131</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -7346,13 +7349,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>10841692.351223463</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>10989724.979223462</v>
+        <v>8378032.6279991101</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -7426,7 +7429,7 @@
         <v>18</v>
       </c>
       <c r="U1" s="49" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2">
@@ -7455,7 +7458,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1112298.3999999999</v>
+        <v>1097381.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -7473,7 +7476,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1062298.3999999999</v>
+        <v>1047381.8000000002</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -7482,13 +7485,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
-      <c r="T2">
-        <v>8401487.7850438319</v>
+      <c r="T2" s="48" t="s">
+        <v>19</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -7520,7 +7523,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1012298.3999997991</v>
+        <v>997381.79999979911</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -7538,7 +7541,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>962298.39999979909</v>
+        <v>947381.799999799</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -7627,7 +7630,7 @@
         <v>18</v>
       </c>
       <c r="U1" s="56" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2">
@@ -7656,7 +7659,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1112298.3999999999</v>
+        <v>1097381.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -7674,7 +7677,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1062298.3999999999</v>
+        <v>1047381.8000000002</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -7683,13 +7686,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
-      <c r="T2">
-        <v>8471797.8030438293</v>
+      <c r="T2" s="55" t="s">
+        <v>19</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -7700,28 +7703,28 @@
         <v>44197</v>
       </c>
       <c r="B3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>27000</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>27000</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>7999.9999999998645</v>
       </c>
       <c r="H3">
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>845140.40000073391</v>
+        <v>830223.80000073405</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -7739,10 +7742,10 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>795140.40000073379</v>
+        <v>780223.80000073405</v>
       </c>
       <c r="P3">
-        <v>477427.99999962613</v>
+        <v>469427.99999962631</v>
       </c>
       <c r="Q3">
         <v>0</v>
@@ -7828,7 +7831,7 @@
         <v>18</v>
       </c>
       <c r="U1" s="63" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2">
@@ -7857,7 +7860,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1112298.3999999999</v>
+        <v>1097381.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -7875,7 +7878,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1062298.3999999999</v>
+        <v>1047381.8000000002</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -7884,13 +7887,13 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>8229999.9999999953</v>
+        <v>8229999.9999999963</v>
       </c>
       <c r="S2">
         <v>1</v>
       </c>
-      <c r="T2">
-        <v>8443633.0190438293</v>
+      <c r="T2" s="62" t="s">
+        <v>19</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -7922,7 +7925,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1012298.3999997991</v>
+        <v>997381.79999979911</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -7940,7 +7943,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>962298.39999979909</v>
+        <v>947381.799999799</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -7949,13 +7952,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8229999.9999991106</v>
+        <v>8622692.9817536902</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>8380597.6699991105</v>
+        <v>8773290.6517536901</v>
       </c>
       <c r="U3">
         <v>0</v>

</xml_diff>

<commit_message>
THIRD PASS - Deterministic and MRM run
updated model file to include updated MX percentages equal to the schedule distribution from accounting in 2021
</commit_message>
<xml_diff>
--- a/Output Data/MtomToCrss_Annual.xlsx
+++ b/Output Data/MtomToCrss_Annual.xlsx
@@ -855,7 +855,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8511047.6559112687</v>
+        <v>8504660.8790714014</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -1056,7 +1056,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8497172.7439112682</v>
+        <v>8490785.967071401</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -1257,7 +1257,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8507262.7859112676</v>
+        <v>8500876.0090714004</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -1458,7 +1458,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8502194.0319112688</v>
+        <v>8495807.2550713997</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -1659,7 +1659,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8507763.6739112679</v>
+        <v>8501376.8970714007</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -1860,7 +1860,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8478109.2419112679</v>
+        <v>8471722.4650714006</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -1919,13 +1919,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8998583.5788952913</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>9131462.384895293</v>
+        <v>9132878.8059775531</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -2061,7 +2061,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8468854.9979112688</v>
+        <v>8462468.2210714016</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -2262,7 +2262,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8508563.8239112683</v>
+        <v>8502177.047071401</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -2463,7 +2463,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8479223.1699112691</v>
+        <v>8472836.3930714</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -2664,7 +2664,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8450258.1059112679</v>
+        <v>8443871.3290714025</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -2865,7 +2865,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8427288.725911269</v>
+        <v>8420901.9490714017</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -3066,7 +3066,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8488475.4199112691</v>
+        <v>8482088.6430714</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -3267,7 +3267,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8506043.8959112689</v>
+        <v>8499657.1190714017</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -3468,7 +3468,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8512780.7359112687</v>
+        <v>8506393.9590714015</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -3669,7 +3669,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8463164.2859112695</v>
+        <v>8456777.5090714004</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -3870,7 +3870,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8493511.0859112665</v>
+        <v>8487124.3090713993</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -4071,7 +4071,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8507788.6159112677</v>
+        <v>8501401.8390714023</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -4272,7 +4272,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8463552.2559112683</v>
+        <v>8457165.4790714029</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -4473,7 +4473,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8507671.8059112672</v>
+        <v>8501285.0290714018</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -4674,7 +4674,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8552982.6559112687</v>
+        <v>8546595.8790713996</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -4875,7 +4875,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8487215.0259112678</v>
+        <v>8480828.2490714006</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -5076,7 +5076,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8515189.5859112684</v>
+        <v>8508802.8090713993</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -5277,7 +5277,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8503122.2399112694</v>
+        <v>8496735.4630714022</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -5478,7 +5478,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8508835.1759112664</v>
+        <v>8502448.399071401</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -5679,7 +5679,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8501047.2059112675</v>
+        <v>8494660.4290714003</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -5880,7 +5880,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8525662.935911268</v>
+        <v>8519276.1590714008</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -6081,7 +6081,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8452809.3759112693</v>
+        <v>8446422.5990714021</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -6282,7 +6282,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8477587.4659112673</v>
+        <v>8471200.6890714001</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -6483,7 +6483,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8492596.9259112701</v>
+        <v>8486210.149071401</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -6684,7 +6684,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8490537.8459112681</v>
+        <v>8484151.0690714009</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -6885,7 +6885,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8517623.5499112662</v>
+        <v>8511236.7730714008</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -7086,7 +7086,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8557603.3139112685</v>
+        <v>8551216.5370714013</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -7287,7 +7287,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8483491.0659112688</v>
+        <v>8477104.2890713997</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -7488,7 +7488,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8467673.9839112684</v>
+        <v>8461287.2070714012</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -7689,7 +7689,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8512145.5139112677</v>
+        <v>8505758.7370714005</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -7890,7 +7890,7 @@
         <v>1</v>
       </c>
       <c r="T2">
-        <v>8479302.3659112677</v>
+        <v>8472915.5890714005</v>
       </c>
       <c r="U2">
         <v>0</v>
@@ -7949,13 +7949,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8229999.9999991106</v>
+        <v>8622692.9817537088</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>8380597.6699991105</v>
+        <v>8773290.6517537106</v>
       </c>
       <c r="U3">
         <v>0</v>

</xml_diff>

<commit_message>
July 2020 MTOM Run - Unofficial
Updated forecast and output files. Removed old MTOM model file (prior to integration)
Updated model file to include output DMI changes  and a script to change flags to 24MS mode
No changes to the ruleset made since the June 2020 MTOM run
</commit_message>
<xml_diff>
--- a/Output Data/MtomToCrss_Annual.xlsx
+++ b/Output Data/MtomToCrss_Annual.xlsx
@@ -825,7 +825,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1097381.8</v>
+        <v>1111349.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -843,7 +843,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1047381.8000000002</v>
+        <v>1061349.8</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -890,7 +890,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1107900.1000000001</v>
+        <v>1121868.0999999999</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -908,7 +908,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1057900.1000000001</v>
+        <v>1071868.0999999999</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -1026,7 +1026,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1097381.8</v>
+        <v>1111349.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -1044,7 +1044,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1047381.8000000002</v>
+        <v>1061349.8</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -1091,7 +1091,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1020342.6000007343</v>
+        <v>1034310.6000007342</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -1109,7 +1109,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>970342.60000073432</v>
+        <v>984310.60000073421</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -1227,7 +1227,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1097381.8</v>
+        <v>1111349.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -1245,7 +1245,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1047381.8000000002</v>
+        <v>1061349.8</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -1292,7 +1292,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>830223.80000073405</v>
+        <v>844191.80000073393</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -1310,7 +1310,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>780223.80000073405</v>
+        <v>794191.80000073381</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -1428,7 +1428,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1097381.8</v>
+        <v>1111349.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -1446,7 +1446,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1047381.8000000002</v>
+        <v>1061349.8</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -1493,7 +1493,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>830223.80000073405</v>
+        <v>844191.80000073393</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -1511,7 +1511,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>780223.80000073405</v>
+        <v>794191.80000073381</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -1629,7 +1629,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1097381.8</v>
+        <v>1111349.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -1647,7 +1647,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1047381.8000000002</v>
+        <v>1061349.8</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -1694,7 +1694,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1232381.7999999067</v>
+        <v>1246349.7999999064</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -1712,7 +1712,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1182381.7999999067</v>
+        <v>1196349.7999999064</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -1830,7 +1830,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1097381.8</v>
+        <v>1111349.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -1848,7 +1848,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1047381.8000000002</v>
+        <v>1061349.8</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -1895,7 +1895,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>810084.40000073414</v>
+        <v>824052.40000073402</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -1913,7 +1913,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>760084.40000073414</v>
+        <v>774052.40000073402</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -1922,13 +1922,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8999999.9999775533</v>
+        <v>8893069.1459096484</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>9132878.8059775531</v>
+        <v>9025947.9519096464</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -2031,7 +2031,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1097381.8</v>
+        <v>1111349.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -2049,7 +2049,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1047381.8000000002</v>
+        <v>1061349.8</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -2096,7 +2096,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1367381.7999998131</v>
+        <v>1381349.7999998129</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -2114,7 +2114,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1317381.7999998131</v>
+        <v>1331349.7999998129</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -2123,13 +2123,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8229999.9999991106</v>
+        <v>10070815.792776028</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>8512420.3039991111</v>
+        <v>10353236.096776025</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -2232,7 +2232,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1097381.8</v>
+        <v>1111349.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -2250,7 +2250,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1047381.8000000002</v>
+        <v>1061349.8</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -2297,7 +2297,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1367381.7999998131</v>
+        <v>1381349.7999998129</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -2315,7 +2315,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1317381.7999998131</v>
+        <v>1331349.7999998129</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -2433,7 +2433,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1097381.8</v>
+        <v>1111349.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -2451,7 +2451,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1047381.8000000002</v>
+        <v>1061349.8</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -2498,7 +2498,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1367381.7999998131</v>
+        <v>1381349.7999998129</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -2516,7 +2516,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1317381.7999998131</v>
+        <v>1331349.7999998129</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -2634,7 +2634,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1097381.8</v>
+        <v>1111349.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -2652,7 +2652,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1047381.8000000002</v>
+        <v>1061349.8</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -2699,7 +2699,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1367381.7999998131</v>
+        <v>1381349.7999998129</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -2717,7 +2717,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1317381.7999998131</v>
+        <v>1331349.7999998129</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -2835,7 +2835,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1097381.8</v>
+        <v>1111349.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -2853,7 +2853,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1047381.8000000002</v>
+        <v>1061349.8</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -2900,7 +2900,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1367381.7999998131</v>
+        <v>1381349.7999998129</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -2918,7 +2918,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1317381.7999998131</v>
+        <v>1331349.7999998129</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -3036,7 +3036,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1097381.8</v>
+        <v>1111349.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -3054,7 +3054,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1047381.8000000002</v>
+        <v>1061349.8</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -3101,7 +3101,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1367381.7999998131</v>
+        <v>1381349.7999998129</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -3119,7 +3119,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1317381.7999998131</v>
+        <v>1331349.7999998129</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -3237,7 +3237,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1097381.8</v>
+        <v>1111349.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -3255,7 +3255,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1047381.8000000002</v>
+        <v>1061349.8</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -3302,7 +3302,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1232381.7999999067</v>
+        <v>1246349.7999999064</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -3320,7 +3320,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1182381.7999999067</v>
+        <v>1196349.7999999064</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -3329,13 +3329,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8229999.9999991106</v>
+        <v>8588074.1001150701</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>8370628.0299991099</v>
+        <v>8728702.1301150694</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -3438,7 +3438,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1097381.8</v>
+        <v>1111349.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -3456,7 +3456,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1047381.8000000002</v>
+        <v>1061349.8</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -3503,7 +3503,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>997381.79999979911</v>
+        <v>1011349.7999997991</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -3521,7 +3521,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>947381.799999799</v>
+        <v>961349.799999799</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -3639,7 +3639,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1097381.8</v>
+        <v>1111349.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -3657,7 +3657,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1047381.8000000002</v>
+        <v>1061349.8</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -3704,7 +3704,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>997381.79999979911</v>
+        <v>1011349.7999997991</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -3722,7 +3722,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>947381.799999799</v>
+        <v>961349.799999799</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -3840,7 +3840,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1097381.8</v>
+        <v>1111349.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -3858,7 +3858,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1047381.8000000002</v>
+        <v>1061349.8</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -3905,7 +3905,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1232381.7999999067</v>
+        <v>1246349.7999999064</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -3923,7 +3923,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1182381.7999999067</v>
+        <v>1196349.7999999064</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -4041,7 +4041,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1097381.8</v>
+        <v>1111349.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -4059,7 +4059,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1047381.8000000002</v>
+        <v>1061349.8</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -4106,7 +4106,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1097381.8</v>
+        <v>1111349.8</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -4124,7 +4124,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1047381.8000000002</v>
+        <v>1061349.8</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -4242,7 +4242,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1097381.8</v>
+        <v>1111349.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -4260,7 +4260,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1047381.8000000002</v>
+        <v>1061349.8</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -4307,7 +4307,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1232381.7999999067</v>
+        <v>1246349.7999999064</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -4325,7 +4325,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1182381.7999999067</v>
+        <v>1196349.7999999064</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -4443,7 +4443,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1097381.8</v>
+        <v>1111349.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -4461,7 +4461,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1047381.8000000002</v>
+        <v>1061349.8</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -4508,7 +4508,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1367381.7999998131</v>
+        <v>1381349.7999998129</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -4526,7 +4526,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1317381.7999998131</v>
+        <v>1331349.7999998129</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -4644,7 +4644,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1097381.8</v>
+        <v>1111349.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -4662,7 +4662,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1047381.8000000002</v>
+        <v>1061349.8</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -4709,7 +4709,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>997381.79999979911</v>
+        <v>1011349.7999997991</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -4727,7 +4727,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>947381.799999799</v>
+        <v>961349.799999799</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -4845,7 +4845,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1097381.8</v>
+        <v>1111349.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -4863,7 +4863,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1047381.8000000002</v>
+        <v>1061349.8</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -4910,7 +4910,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>830223.80000073405</v>
+        <v>844191.80000073393</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -4928,7 +4928,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>780223.80000073405</v>
+        <v>794191.80000073381</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -5046,7 +5046,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1097381.8</v>
+        <v>1111349.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -5064,7 +5064,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1047381.8000000002</v>
+        <v>1061349.8</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -5111,7 +5111,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>997381.79999979911</v>
+        <v>1011349.7999997991</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -5129,7 +5129,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>947381.799999799</v>
+        <v>961349.799999799</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -5247,7 +5247,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1097381.8</v>
+        <v>1111349.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -5265,7 +5265,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1047381.8000000002</v>
+        <v>1061349.8</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -5312,7 +5312,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1367381.7999998131</v>
+        <v>1381349.7999998129</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -5330,7 +5330,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1317381.7999998131</v>
+        <v>1331349.7999998129</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -5448,7 +5448,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1097381.8</v>
+        <v>1111349.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -5466,7 +5466,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1047381.8000000002</v>
+        <v>1061349.8</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -5513,7 +5513,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1097381.8</v>
+        <v>1111349.8</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -5531,7 +5531,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1047381.8000000002</v>
+        <v>1061349.8</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -5649,7 +5649,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1097381.8</v>
+        <v>1111349.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -5667,7 +5667,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1047381.8000000002</v>
+        <v>1061349.8</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -5714,7 +5714,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1367381.7999998131</v>
+        <v>1381349.7999998129</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -5732,7 +5732,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1317381.7999998131</v>
+        <v>1331349.7999998129</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -5850,7 +5850,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1097381.8</v>
+        <v>1111349.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -5868,7 +5868,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1047381.8000000002</v>
+        <v>1061349.8</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -5915,7 +5915,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1097381.8</v>
+        <v>1111349.8</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -5933,7 +5933,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1047381.8000000002</v>
+        <v>1061349.8</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -6051,7 +6051,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1097381.8</v>
+        <v>1111349.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -6069,7 +6069,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1047381.8000000002</v>
+        <v>1061349.8</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -6116,7 +6116,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>997381.79999979911</v>
+        <v>1011349.7999997991</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -6134,7 +6134,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>947381.799999799</v>
+        <v>961349.799999799</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -6252,7 +6252,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1097381.8</v>
+        <v>1111349.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -6270,7 +6270,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1047381.8000000002</v>
+        <v>1061349.8</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -6317,7 +6317,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>830223.80000073405</v>
+        <v>844191.80000073393</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -6335,7 +6335,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>780223.80000073405</v>
+        <v>794191.80000073381</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -6453,7 +6453,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1097381.8</v>
+        <v>1111349.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -6471,7 +6471,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1047381.8000000002</v>
+        <v>1061349.8</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -6518,7 +6518,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>830223.80000073405</v>
+        <v>844191.80000073393</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -6536,7 +6536,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>780223.80000073405</v>
+        <v>794191.80000073381</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -6654,7 +6654,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1097381.8</v>
+        <v>1111349.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -6672,7 +6672,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1047381.8000000002</v>
+        <v>1061349.8</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -6719,7 +6719,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1020342.6000007343</v>
+        <v>1034310.6000007342</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -6737,7 +6737,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>970342.60000073432</v>
+        <v>984310.60000073421</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -6855,7 +6855,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1097381.8</v>
+        <v>1111349.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -6873,7 +6873,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1047381.8000000002</v>
+        <v>1061349.8</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -6920,7 +6920,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1367381.7999998131</v>
+        <v>1381349.7999998129</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -6938,7 +6938,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1317381.7999998131</v>
+        <v>1331349.7999998129</v>
       </c>
       <c r="P3">
         <v>477427.99999962613</v>
@@ -7056,7 +7056,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1097381.8</v>
+        <v>1111349.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -7074,7 +7074,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1047381.8000000002</v>
+        <v>1061349.8</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -7121,7 +7121,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>997381.79999979911</v>
+        <v>1011349.7999997991</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -7139,7 +7139,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>947381.799999799</v>
+        <v>961349.799999799</v>
       </c>
       <c r="P3">
         <v>477427.99999962613</v>
@@ -7257,7 +7257,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1097381.8</v>
+        <v>1111349.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -7275,7 +7275,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1047381.8000000002</v>
+        <v>1061349.8</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -7322,7 +7322,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>1367381.7999998131</v>
+        <v>1381349.7999998129</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -7340,7 +7340,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1317381.7999998131</v>
+        <v>1331349.7999998129</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -7458,7 +7458,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1097381.8</v>
+        <v>1111349.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -7476,7 +7476,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1047381.8000000002</v>
+        <v>1061349.8</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -7523,7 +7523,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>997381.79999979911</v>
+        <v>1011349.7999997991</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -7541,7 +7541,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>947381.799999799</v>
+        <v>961349.799999799</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -7659,7 +7659,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1097381.8</v>
+        <v>1111349.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -7677,7 +7677,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1047381.8000000002</v>
+        <v>1061349.8</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -7724,7 +7724,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>830223.80000073405</v>
+        <v>844191.80000073393</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -7742,7 +7742,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>780223.80000073405</v>
+        <v>794191.80000073381</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -7860,7 +7860,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1097381.8</v>
+        <v>1111349.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -7878,7 +7878,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1047381.8000000002</v>
+        <v>1061349.8</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -7925,7 +7925,7 @@
         <v>478494.70000000001</v>
       </c>
       <c r="I3">
-        <v>997381.79999979911</v>
+        <v>1011349.7999997991</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -7943,7 +7943,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>947381.799999799</v>
+        <v>961349.799999799</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -7952,13 +7952,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8622692.9817536902</v>
+        <v>8617531.5292699412</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>8773290.6517536901</v>
+        <v>8768129.1992699411</v>
       </c>
       <c r="U3">
         <v>0</v>

</xml_diff>

<commit_message>
MTOM ensemble output files and inflow forecast files for July run
</commit_message>
<xml_diff>
--- a/Output Data/MtomToCrss_Annual.xlsx
+++ b/Output Data/MtomToCrss_Annual.xlsx
@@ -825,7 +825,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1097381.8</v>
+        <v>1111349.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -843,7 +843,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1047381.8000000002</v>
+        <v>1061349.8</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -887,10 +887,10 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>478494.70000000001</v>
+        <v>478494.6999999999</v>
       </c>
       <c r="I3">
-        <v>1107900.1000000001</v>
+        <v>1121868.0999999999</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -908,7 +908,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1057900.1000000001</v>
+        <v>1071868.0999999999</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -1026,7 +1026,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1097381.8</v>
+        <v>1111349.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -1044,7 +1044,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1047381.8000000002</v>
+        <v>1061349.8</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -1088,10 +1088,10 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>478494.70000000001</v>
+        <v>478494.6999999999</v>
       </c>
       <c r="I3">
-        <v>1020342.6000007343</v>
+        <v>1034310.6000007342</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -1109,7 +1109,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>970342.60000073432</v>
+        <v>984310.60000073421</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -1227,7 +1227,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1097381.8</v>
+        <v>1111349.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -1245,7 +1245,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1047381.8000000002</v>
+        <v>1061349.8</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -1289,10 +1289,10 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>478494.70000000001</v>
+        <v>478494.6999999999</v>
       </c>
       <c r="I3">
-        <v>830223.80000073405</v>
+        <v>844191.80000073393</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -1310,7 +1310,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>780223.80000073405</v>
+        <v>794191.80000073381</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -1428,7 +1428,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1097381.8</v>
+        <v>1111349.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -1446,7 +1446,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1047381.8000000002</v>
+        <v>1061349.8</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -1490,10 +1490,10 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>478494.70000000001</v>
+        <v>478494.6999999999</v>
       </c>
       <c r="I3">
-        <v>830223.80000073405</v>
+        <v>844191.80000073393</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -1511,7 +1511,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>780223.80000073405</v>
+        <v>794191.80000073381</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -1629,7 +1629,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1097381.8</v>
+        <v>1111349.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -1647,7 +1647,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1047381.8000000002</v>
+        <v>1061349.8</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -1691,10 +1691,10 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>478494.70000000001</v>
+        <v>478494.6999999999</v>
       </c>
       <c r="I3">
-        <v>1232381.7999999067</v>
+        <v>1246349.7999999064</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -1712,7 +1712,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1182381.7999999067</v>
+        <v>1196349.7999999064</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -1830,7 +1830,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1097381.8</v>
+        <v>1111349.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -1848,7 +1848,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1047381.8000000002</v>
+        <v>1061349.8</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -1892,10 +1892,10 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>478494.70000000001</v>
+        <v>478494.6999999999</v>
       </c>
       <c r="I3">
-        <v>810084.40000073414</v>
+        <v>824052.40000073402</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -1913,7 +1913,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>760084.40000073414</v>
+        <v>774052.40000073402</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -1922,13 +1922,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8999999.9999775533</v>
+        <v>8893094.8003986292</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>9132878.8059775531</v>
+        <v>9025973.6063986272</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -2031,7 +2031,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1097381.8</v>
+        <v>1111349.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -2049,7 +2049,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1047381.8000000002</v>
+        <v>1061349.8</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -2093,10 +2093,10 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>478494.70000000001</v>
+        <v>478494.6999999999</v>
       </c>
       <c r="I3">
-        <v>1367381.7999998131</v>
+        <v>1381349.7999998129</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -2114,7 +2114,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1317381.7999998131</v>
+        <v>1331349.7999998129</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -2123,13 +2123,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8229999.9999991106</v>
+        <v>10070866.820511926</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>8512420.3039991111</v>
+        <v>10353287.124511926</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -2232,7 +2232,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1097381.8</v>
+        <v>1111349.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -2250,7 +2250,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1047381.8000000002</v>
+        <v>1061349.8</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -2294,10 +2294,10 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>478494.70000000001</v>
+        <v>478494.6999999999</v>
       </c>
       <c r="I3">
-        <v>1367381.7999998131</v>
+        <v>1381349.7999998129</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -2315,7 +2315,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1317381.7999998131</v>
+        <v>1331349.7999998129</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -2433,7 +2433,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1097381.8</v>
+        <v>1111349.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -2451,7 +2451,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1047381.8000000002</v>
+        <v>1061349.8</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -2495,10 +2495,10 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>478494.70000000001</v>
+        <v>478494.6999999999</v>
       </c>
       <c r="I3">
-        <v>1367381.7999998131</v>
+        <v>1381349.7999998129</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -2516,7 +2516,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1317381.7999998131</v>
+        <v>1331349.7999998129</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -2634,7 +2634,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1097381.8</v>
+        <v>1111349.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -2652,7 +2652,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1047381.8000000002</v>
+        <v>1061349.8</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -2696,10 +2696,10 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>478494.70000000001</v>
+        <v>478494.6999999999</v>
       </c>
       <c r="I3">
-        <v>1367381.7999998131</v>
+        <v>1381349.7999998129</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -2717,7 +2717,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1317381.7999998131</v>
+        <v>1331349.7999998129</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -2835,7 +2835,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1097381.8</v>
+        <v>1111349.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -2853,7 +2853,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1047381.8000000002</v>
+        <v>1061349.8</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -2897,10 +2897,10 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>478494.70000000001</v>
+        <v>478494.6999999999</v>
       </c>
       <c r="I3">
-        <v>1367381.7999998131</v>
+        <v>1381349.7999998129</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -2918,7 +2918,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1317381.7999998131</v>
+        <v>1331349.7999998129</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -3036,7 +3036,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1097381.8</v>
+        <v>1111349.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -3054,7 +3054,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1047381.8000000002</v>
+        <v>1061349.8</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -3098,10 +3098,10 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>478494.70000000001</v>
+        <v>478494.6999999999</v>
       </c>
       <c r="I3">
-        <v>1367381.7999998131</v>
+        <v>1381349.7999998129</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -3119,7 +3119,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1317381.7999998131</v>
+        <v>1331349.7999998129</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -3237,7 +3237,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1097381.8</v>
+        <v>1111349.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -3255,7 +3255,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1047381.8000000002</v>
+        <v>1061349.8</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -3299,10 +3299,10 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>478494.70000000001</v>
+        <v>478494.6999999999</v>
       </c>
       <c r="I3">
-        <v>1232381.7999999067</v>
+        <v>1246349.7999999064</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -3320,7 +3320,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1182381.7999999067</v>
+        <v>1196349.7999999064</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -3329,13 +3329,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8229999.9999991106</v>
+        <v>8588099.7840172537</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>8370628.0299991099</v>
+        <v>8728727.8140172567</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -3438,7 +3438,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1097381.8</v>
+        <v>1111349.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -3456,7 +3456,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1047381.8000000002</v>
+        <v>1061349.8</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -3500,10 +3500,10 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>478494.70000000001</v>
+        <v>478494.6999999999</v>
       </c>
       <c r="I3">
-        <v>997381.79999979911</v>
+        <v>1011349.7999997991</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -3521,7 +3521,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>947381.799999799</v>
+        <v>961349.799999799</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -3639,7 +3639,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1097381.8</v>
+        <v>1111349.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -3657,7 +3657,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1047381.8000000002</v>
+        <v>1061349.8</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -3701,10 +3701,10 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>478494.70000000001</v>
+        <v>478494.6999999999</v>
       </c>
       <c r="I3">
-        <v>997381.79999979911</v>
+        <v>1011349.7999997991</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -3722,7 +3722,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>947381.799999799</v>
+        <v>961349.799999799</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -3840,7 +3840,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1097381.8</v>
+        <v>1111349.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -3858,7 +3858,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1047381.8000000002</v>
+        <v>1061349.8</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -3902,10 +3902,10 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>478494.70000000001</v>
+        <v>478494.6999999999</v>
       </c>
       <c r="I3">
-        <v>1232381.7999999067</v>
+        <v>1246349.7999999064</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -3923,7 +3923,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1182381.7999999067</v>
+        <v>1196349.7999999064</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -4041,7 +4041,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1097381.8</v>
+        <v>1111349.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -4059,7 +4059,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1047381.8000000002</v>
+        <v>1061349.8</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -4103,10 +4103,10 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>478494.70000000001</v>
+        <v>478494.6999999999</v>
       </c>
       <c r="I3">
-        <v>1097381.8</v>
+        <v>1111349.8</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -4124,7 +4124,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1047381.8000000002</v>
+        <v>1061349.8</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -4242,7 +4242,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1097381.8</v>
+        <v>1111349.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -4260,7 +4260,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1047381.8000000002</v>
+        <v>1061349.8</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -4304,10 +4304,10 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>478494.70000000001</v>
+        <v>478494.6999999999</v>
       </c>
       <c r="I3">
-        <v>1232381.7999999067</v>
+        <v>1246349.7999999064</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -4325,7 +4325,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1182381.7999999067</v>
+        <v>1196349.7999999064</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -4443,7 +4443,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1097381.8</v>
+        <v>1111349.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -4461,7 +4461,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1047381.8000000002</v>
+        <v>1061349.8</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -4505,10 +4505,10 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>478494.70000000001</v>
+        <v>478494.6999999999</v>
       </c>
       <c r="I3">
-        <v>1367381.7999998131</v>
+        <v>1381349.7999998129</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -4526,7 +4526,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1317381.7999998131</v>
+        <v>1331349.7999998129</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -4644,7 +4644,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1097381.8</v>
+        <v>1111349.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -4662,7 +4662,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1047381.8000000002</v>
+        <v>1061349.8</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -4706,10 +4706,10 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>478494.70000000001</v>
+        <v>478494.6999999999</v>
       </c>
       <c r="I3">
-        <v>997381.79999979911</v>
+        <v>1011349.7999997991</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -4727,7 +4727,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>947381.799999799</v>
+        <v>961349.799999799</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -4845,7 +4845,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1097381.8</v>
+        <v>1111349.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -4863,7 +4863,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1047381.8000000002</v>
+        <v>1061349.8</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -4907,10 +4907,10 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>478494.70000000001</v>
+        <v>478494.6999999999</v>
       </c>
       <c r="I3">
-        <v>830223.80000073405</v>
+        <v>844191.80000073393</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -4928,7 +4928,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>780223.80000073405</v>
+        <v>794191.80000073381</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -5046,7 +5046,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1097381.8</v>
+        <v>1111349.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -5064,7 +5064,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1047381.8000000002</v>
+        <v>1061349.8</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -5108,10 +5108,10 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>478494.70000000001</v>
+        <v>478494.6999999999</v>
       </c>
       <c r="I3">
-        <v>997381.79999979911</v>
+        <v>1011349.7999997991</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -5129,7 +5129,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>947381.799999799</v>
+        <v>961349.799999799</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -5247,7 +5247,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1097381.8</v>
+        <v>1111349.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -5265,7 +5265,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1047381.8000000002</v>
+        <v>1061349.8</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -5309,10 +5309,10 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>478494.70000000001</v>
+        <v>478494.6999999999</v>
       </c>
       <c r="I3">
-        <v>1367381.7999998131</v>
+        <v>1381349.7999998129</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -5330,7 +5330,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1317381.7999998131</v>
+        <v>1331349.7999998129</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -5448,7 +5448,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1097381.8</v>
+        <v>1111349.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -5466,7 +5466,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1047381.8000000002</v>
+        <v>1061349.8</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -5510,10 +5510,10 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>478494.70000000001</v>
+        <v>478494.6999999999</v>
       </c>
       <c r="I3">
-        <v>1097381.8</v>
+        <v>1111349.8</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -5531,7 +5531,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1047381.8000000002</v>
+        <v>1061349.8</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -5649,7 +5649,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1097381.8</v>
+        <v>1111349.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -5667,7 +5667,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1047381.8000000002</v>
+        <v>1061349.8</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -5711,10 +5711,10 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>478494.70000000001</v>
+        <v>478494.6999999999</v>
       </c>
       <c r="I3">
-        <v>1367381.7999998131</v>
+        <v>1381349.7999998129</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -5732,7 +5732,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1317381.7999998131</v>
+        <v>1331349.7999998129</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -5850,7 +5850,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1097381.8</v>
+        <v>1111349.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -5868,7 +5868,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1047381.8000000002</v>
+        <v>1061349.8</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -5912,10 +5912,10 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>478494.70000000001</v>
+        <v>478494.6999999999</v>
       </c>
       <c r="I3">
-        <v>1097381.8</v>
+        <v>1111349.8</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -5933,7 +5933,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1047381.8000000002</v>
+        <v>1061349.8</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -6051,7 +6051,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1097381.8</v>
+        <v>1111349.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -6069,7 +6069,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1047381.8000000002</v>
+        <v>1061349.8</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -6113,10 +6113,10 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>478494.70000000001</v>
+        <v>478494.6999999999</v>
       </c>
       <c r="I3">
-        <v>997381.79999979911</v>
+        <v>1011349.7999997991</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -6134,7 +6134,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>947381.799999799</v>
+        <v>961349.799999799</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -6252,7 +6252,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1097381.8</v>
+        <v>1111349.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -6270,7 +6270,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1047381.8000000002</v>
+        <v>1061349.8</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -6314,10 +6314,10 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>478494.70000000001</v>
+        <v>478494.6999999999</v>
       </c>
       <c r="I3">
-        <v>830223.80000073405</v>
+        <v>844191.80000073393</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -6335,7 +6335,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>780223.80000073405</v>
+        <v>794191.80000073381</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -6453,7 +6453,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1097381.8</v>
+        <v>1111349.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -6471,7 +6471,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1047381.8000000002</v>
+        <v>1061349.8</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -6515,10 +6515,10 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>478494.70000000001</v>
+        <v>478494.6999999999</v>
       </c>
       <c r="I3">
-        <v>830223.80000073405</v>
+        <v>844191.80000073393</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -6536,7 +6536,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>780223.80000073405</v>
+        <v>794191.80000073381</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -6654,7 +6654,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1097381.8</v>
+        <v>1111349.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -6672,7 +6672,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1047381.8000000002</v>
+        <v>1061349.8</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -6716,10 +6716,10 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>478494.70000000001</v>
+        <v>478494.6999999999</v>
       </c>
       <c r="I3">
-        <v>1020342.6000007343</v>
+        <v>1034310.6000007342</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -6737,7 +6737,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>970342.60000073432</v>
+        <v>984310.60000073421</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -6855,7 +6855,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1097381.8</v>
+        <v>1111349.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -6873,7 +6873,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1047381.8000000002</v>
+        <v>1061349.8</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -6917,13 +6917,13 @@
         <v>0</v>
       </c>
       <c r="H3">
-        <v>478494.70000000001</v>
+        <v>505494.69999999995</v>
       </c>
       <c r="I3">
-        <v>1367381.7999998131</v>
+        <v>1381349.7999998129</v>
       </c>
       <c r="J3">
-        <v>280632</v>
+        <v>307632</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -6938,7 +6938,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1317381.7999998131</v>
+        <v>1331349.7999998129</v>
       </c>
       <c r="P3">
         <v>477427.99999962613</v>
@@ -7056,7 +7056,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1097381.8</v>
+        <v>1111349.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -7074,7 +7074,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1047381.8000000002</v>
+        <v>1061349.8</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -7118,13 +7118,13 @@
         <v>0</v>
       </c>
       <c r="H3">
-        <v>478494.70000000001</v>
+        <v>505494.69999999995</v>
       </c>
       <c r="I3">
-        <v>997381.79999979911</v>
+        <v>1011349.7999997991</v>
       </c>
       <c r="J3">
-        <v>280632</v>
+        <v>307632</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
@@ -7139,7 +7139,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>947381.799999799</v>
+        <v>961349.799999799</v>
       </c>
       <c r="P3">
         <v>477427.99999962613</v>
@@ -7257,7 +7257,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1097381.8</v>
+        <v>1111349.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -7275,7 +7275,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1047381.8000000002</v>
+        <v>1061349.8</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -7319,10 +7319,10 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>478494.70000000001</v>
+        <v>478494.6999999999</v>
       </c>
       <c r="I3">
-        <v>1367381.7999998131</v>
+        <v>1381349.7999998129</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -7340,7 +7340,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>1317381.7999998131</v>
+        <v>1331349.7999998129</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -7458,7 +7458,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1097381.8</v>
+        <v>1111349.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -7476,7 +7476,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1047381.8000000002</v>
+        <v>1061349.8</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -7520,10 +7520,10 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>478494.70000000001</v>
+        <v>478494.6999999999</v>
       </c>
       <c r="I3">
-        <v>997381.79999979911</v>
+        <v>1011349.7999997991</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -7541,7 +7541,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>947381.799999799</v>
+        <v>961349.799999799</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -7659,7 +7659,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1097381.8</v>
+        <v>1111349.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -7677,7 +7677,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1047381.8000000002</v>
+        <v>1061349.8</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -7721,10 +7721,10 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>478494.70000000001</v>
+        <v>478494.6999999999</v>
       </c>
       <c r="I3">
-        <v>830223.80000073405</v>
+        <v>844191.80000073393</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -7742,7 +7742,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>780223.80000073405</v>
+        <v>794191.80000073381</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -7860,7 +7860,7 @@
         <v>475794.70000000001</v>
       </c>
       <c r="I2">
-        <v>1097381.8</v>
+        <v>1111349.8</v>
       </c>
       <c r="J2">
         <v>280632</v>
@@ -7878,7 +7878,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1047381.8000000002</v>
+        <v>1061349.8</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -7922,10 +7922,10 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>478494.70000000001</v>
+        <v>478494.6999999999</v>
       </c>
       <c r="I3">
-        <v>997381.79999979911</v>
+        <v>1011349.7999997991</v>
       </c>
       <c r="J3">
         <v>280632</v>
@@ -7943,7 +7943,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O3">
-        <v>947381.799999799</v>
+        <v>961349.799999799</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -7952,13 +7952,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8622692.9817536902</v>
+        <v>8617557.2119312715</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>8773290.6517536901</v>
+        <v>8768154.8819312695</v>
       </c>
       <c r="U3">
         <v>0</v>

</xml_diff>

<commit_message>
August 2020 MTOM Run
No changes to model file and ruleset (compared to July)
Updated ensemble forecast and output files
Model file updated with august run data and name changed accordingly
</commit_message>
<xml_diff>
--- a/Output Data/MtomToCrss_Annual.xlsx
+++ b/Output Data/MtomToCrss_Annual.xlsx
@@ -6,49 +6,51 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Trace3" sheetId="1" r:id="rId2"/>
-    <sheet name="Trace4" sheetId="2" r:id="rId4"/>
-    <sheet name="Trace5" sheetId="3" r:id="rId5"/>
-    <sheet name="Trace6" sheetId="4" r:id="rId6"/>
-    <sheet name="Trace7" sheetId="5" r:id="rId7"/>
-    <sheet name="Trace8" sheetId="6" r:id="rId8"/>
-    <sheet name="Trace9" sheetId="7" r:id="rId9"/>
-    <sheet name="Trace10" sheetId="8" r:id="rId10"/>
-    <sheet name="Trace11" sheetId="9" r:id="rId11"/>
-    <sheet name="Trace12" sheetId="10" r:id="rId12"/>
-    <sheet name="Trace13" sheetId="11" r:id="rId13"/>
-    <sheet name="Trace14" sheetId="12" r:id="rId14"/>
-    <sheet name="Trace15" sheetId="13" r:id="rId15"/>
-    <sheet name="Trace16" sheetId="14" r:id="rId16"/>
-    <sheet name="Trace17" sheetId="15" r:id="rId17"/>
-    <sheet name="Trace18" sheetId="16" r:id="rId18"/>
-    <sheet name="Trace19" sheetId="17" r:id="rId19"/>
-    <sheet name="Trace20" sheetId="18" r:id="rId20"/>
-    <sheet name="Trace21" sheetId="19" r:id="rId21"/>
-    <sheet name="Trace22" sheetId="20" r:id="rId22"/>
-    <sheet name="Trace23" sheetId="21" r:id="rId23"/>
-    <sheet name="Trace24" sheetId="22" r:id="rId24"/>
-    <sheet name="Trace25" sheetId="23" r:id="rId25"/>
-    <sheet name="Trace26" sheetId="24" r:id="rId26"/>
-    <sheet name="Trace27" sheetId="25" r:id="rId27"/>
-    <sheet name="Trace28" sheetId="26" r:id="rId28"/>
-    <sheet name="Trace29" sheetId="27" r:id="rId29"/>
-    <sheet name="Trace30" sheetId="28" r:id="rId30"/>
-    <sheet name="Trace31" sheetId="29" r:id="rId31"/>
-    <sheet name="Trace32" sheetId="30" r:id="rId32"/>
-    <sheet name="Trace33" sheetId="31" r:id="rId33"/>
-    <sheet name="Trace34" sheetId="32" r:id="rId34"/>
-    <sheet name="Trace35" sheetId="33" r:id="rId35"/>
-    <sheet name="Trace36" sheetId="34" r:id="rId36"/>
-    <sheet name="Trace37" sheetId="35" r:id="rId37"/>
-    <sheet name="Trace38" sheetId="36" r:id="rId38"/>
+    <sheet name="Trace1" sheetId="1" r:id="rId2"/>
+    <sheet name="Trace2" sheetId="2" r:id="rId4"/>
+    <sheet name="Trace3" sheetId="3" r:id="rId5"/>
+    <sheet name="Trace4" sheetId="4" r:id="rId6"/>
+    <sheet name="Trace5" sheetId="5" r:id="rId7"/>
+    <sheet name="Trace6" sheetId="6" r:id="rId8"/>
+    <sheet name="Trace7" sheetId="7" r:id="rId9"/>
+    <sheet name="Trace8" sheetId="8" r:id="rId10"/>
+    <sheet name="Trace9" sheetId="9" r:id="rId11"/>
+    <sheet name="Trace10" sheetId="10" r:id="rId12"/>
+    <sheet name="Trace11" sheetId="11" r:id="rId13"/>
+    <sheet name="Trace12" sheetId="12" r:id="rId14"/>
+    <sheet name="Trace13" sheetId="13" r:id="rId15"/>
+    <sheet name="Trace14" sheetId="14" r:id="rId16"/>
+    <sheet name="Trace15" sheetId="15" r:id="rId17"/>
+    <sheet name="Trace16" sheetId="16" r:id="rId18"/>
+    <sheet name="Trace17" sheetId="17" r:id="rId19"/>
+    <sheet name="Trace18" sheetId="18" r:id="rId20"/>
+    <sheet name="Trace19" sheetId="19" r:id="rId21"/>
+    <sheet name="Trace20" sheetId="20" r:id="rId22"/>
+    <sheet name="Trace21" sheetId="21" r:id="rId23"/>
+    <sheet name="Trace22" sheetId="22" r:id="rId24"/>
+    <sheet name="Trace23" sheetId="23" r:id="rId25"/>
+    <sheet name="Trace24" sheetId="24" r:id="rId26"/>
+    <sheet name="Trace25" sheetId="25" r:id="rId27"/>
+    <sheet name="Trace26" sheetId="26" r:id="rId28"/>
+    <sheet name="Trace27" sheetId="27" r:id="rId29"/>
+    <sheet name="Trace28" sheetId="28" r:id="rId30"/>
+    <sheet name="Trace29" sheetId="29" r:id="rId31"/>
+    <sheet name="Trace30" sheetId="30" r:id="rId32"/>
+    <sheet name="Trace31" sheetId="31" r:id="rId33"/>
+    <sheet name="Trace32" sheetId="32" r:id="rId34"/>
+    <sheet name="Trace33" sheetId="33" r:id="rId35"/>
+    <sheet name="Trace34" sheetId="34" r:id="rId36"/>
+    <sheet name="Trace35" sheetId="35" r:id="rId37"/>
+    <sheet name="Trace36" sheetId="36" r:id="rId38"/>
+    <sheet name="Trace37" sheetId="37" r:id="rId39"/>
+    <sheet name="Trace38" sheetId="38" r:id="rId40"/>
   </sheets>
   <calcPr calcId="125725" fullCalcOnLoad="true"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:xdr="http://purl.oclc.org/ooxml/drawingml/spreadsheetDrawing" count="756" uniqueCount="21">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:xdr="http://purl.oclc.org/ooxml/drawingml/spreadsheetDrawing" count="798" uniqueCount="21">
   <si>
     <t>DCP BWSCP Flags.LB DCP BWSCP</t>
   </si>
@@ -135,7 +137,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="253">
+  <borders count="267">
     <border>
       <start/>
       <end/>
@@ -395,11 +397,25 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="253">
+  <cellXfs count="267">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -725,6 +741,24 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="252" xfId="0" applyNumberFormat="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="253" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="254" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="255" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="256" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="257" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="258" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="259" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="260" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="261" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="262" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="263" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="264" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="265" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="266" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -822,13 +856,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>475794.70000000001</v>
+        <v>487619.69999999995</v>
       </c>
       <c r="I2">
-        <v>1111349.8</v>
+        <v>1133506</v>
       </c>
       <c r="J2">
-        <v>280632</v>
+        <v>292457</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -843,7 +877,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1061349.8</v>
+        <v>1083506</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -872,13 +906,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>27000</v>
+        <v>45000</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>27000</v>
+        <v>45000</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -887,28 +921,28 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>478494.70000000001</v>
+        <v>537119.69999999995</v>
       </c>
       <c r="I3">
-        <v>1121868.0999999999</v>
+        <v>1252024.3</v>
       </c>
       <c r="J3">
-        <v>280632</v>
+        <v>292457</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
       </c>
       <c r="L3">
-        <v>180000</v>
+        <v>220499.99999999997</v>
       </c>
       <c r="M3">
         <v>50000</v>
       </c>
       <c r="N3">
-        <v>6153.3000000000002</v>
+        <v>12453.300000000001</v>
       </c>
       <c r="O3">
-        <v>1071868.0999999999</v>
+        <v>1202024.2999999998</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -917,13 +951,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8999999.9999775533</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>9157545.9999775533</v>
+        <v>8367990.9999991106</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -1023,13 +1057,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>475794.70000000001</v>
+        <v>487619.69999999995</v>
       </c>
       <c r="I2">
-        <v>1111349.8</v>
+        <v>1133506</v>
       </c>
       <c r="J2">
-        <v>280632</v>
+        <v>292457</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -1044,7 +1078,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1061349.8</v>
+        <v>1083506</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -1073,13 +1107,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>27000</v>
+        <v>45000</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>27000</v>
+        <v>45000</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -1088,28 +1122,28 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>478494.70000000001</v>
+        <v>537119.69999999995</v>
       </c>
       <c r="I3">
-        <v>1034310.6000007342</v>
+        <v>866348.00000073388</v>
       </c>
       <c r="J3">
-        <v>280632</v>
+        <v>292457</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
       </c>
       <c r="L3">
-        <v>180000</v>
+        <v>220499.99999999997</v>
       </c>
       <c r="M3">
         <v>50000</v>
       </c>
       <c r="N3">
-        <v>6153.3000000000002</v>
+        <v>12453.300000000001</v>
       </c>
       <c r="O3">
-        <v>984310.60000073421</v>
+        <v>816348.00000073388</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -1124,7 +1158,7 @@
         <v>1</v>
       </c>
       <c r="T3">
-        <v>8366493.4259991096</v>
+        <v>8417833.5499991123</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -1224,13 +1258,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>475794.70000000001</v>
+        <v>487619.69999999995</v>
       </c>
       <c r="I2">
-        <v>1111349.8</v>
+        <v>1133506</v>
       </c>
       <c r="J2">
-        <v>280632</v>
+        <v>292457</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -1245,7 +1279,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1061349.8</v>
+        <v>1083506</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -1274,13 +1308,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>27000</v>
+        <v>45000</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>27000</v>
+        <v>45000</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -1289,28 +1323,28 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>478494.70000000001</v>
+        <v>537119.69999999995</v>
       </c>
       <c r="I3">
-        <v>844191.80000073393</v>
+        <v>1033505.9999997988</v>
       </c>
       <c r="J3">
-        <v>280632</v>
+        <v>292457</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
       </c>
       <c r="L3">
-        <v>180000</v>
+        <v>220499.99999999997</v>
       </c>
       <c r="M3">
         <v>50000</v>
       </c>
       <c r="N3">
-        <v>6153.3000000000002</v>
+        <v>12453.300000000001</v>
       </c>
       <c r="O3">
-        <v>794191.80000073381</v>
+        <v>983505.99999979883</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -1319,13 +1353,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8229999.9999991106</v>
+        <v>8460446.2459286824</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>8404589.229999112</v>
+        <v>8611043.9159286842</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -1425,13 +1459,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>475794.70000000001</v>
+        <v>487619.69999999995</v>
       </c>
       <c r="I2">
-        <v>1111349.8</v>
+        <v>1133506</v>
       </c>
       <c r="J2">
-        <v>280632</v>
+        <v>292457</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -1446,7 +1480,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1061349.8</v>
+        <v>1083506</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -1475,13 +1509,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>27000</v>
+        <v>45000</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>27000</v>
+        <v>45000</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -1490,28 +1524,28 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>478494.70000000001</v>
+        <v>537119.69999999995</v>
       </c>
       <c r="I3">
-        <v>844191.80000073393</v>
+        <v>1056466.8000007342</v>
       </c>
       <c r="J3">
-        <v>280632</v>
+        <v>292457</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
       </c>
       <c r="L3">
-        <v>180000</v>
+        <v>220499.99999999997</v>
       </c>
       <c r="M3">
         <v>50000</v>
       </c>
       <c r="N3">
-        <v>6153.3000000000002</v>
+        <v>12453.300000000001</v>
       </c>
       <c r="O3">
-        <v>794191.80000073381</v>
+        <v>1006466.8000007342</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -1526,7 +1560,7 @@
         <v>1</v>
       </c>
       <c r="T3">
-        <v>8469478.9159991127</v>
+        <v>8366493.4259991096</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -1626,13 +1660,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>475794.70000000001</v>
+        <v>487619.69999999995</v>
       </c>
       <c r="I2">
-        <v>1111349.8</v>
+        <v>1133506</v>
       </c>
       <c r="J2">
-        <v>280632</v>
+        <v>292457</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -1647,7 +1681,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1061349.8</v>
+        <v>1083506</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -1676,13 +1710,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>27000</v>
+        <v>45000</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>27000</v>
+        <v>45000</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -1691,28 +1725,28 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>478494.70000000001</v>
+        <v>537119.69999999995</v>
       </c>
       <c r="I3">
-        <v>1246349.7999999064</v>
+        <v>866348.00000073388</v>
       </c>
       <c r="J3">
-        <v>280632</v>
+        <v>292457</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
       </c>
       <c r="L3">
-        <v>180000</v>
+        <v>220499.99999999997</v>
       </c>
       <c r="M3">
         <v>50000</v>
       </c>
       <c r="N3">
-        <v>6153.3000000000002</v>
+        <v>12453.300000000001</v>
       </c>
       <c r="O3">
-        <v>1196349.7999999064</v>
+        <v>816348.00000073388</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -1727,7 +1761,7 @@
         <v>1</v>
       </c>
       <c r="T3">
-        <v>8639818.2239991091</v>
+        <v>8404589.229999112</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -1827,13 +1861,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>475794.70000000001</v>
+        <v>487619.69999999995</v>
       </c>
       <c r="I2">
-        <v>1111349.8</v>
+        <v>1133506</v>
       </c>
       <c r="J2">
-        <v>280632</v>
+        <v>292457</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -1848,7 +1882,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1061349.8</v>
+        <v>1083506</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -1877,13 +1911,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>27000</v>
+        <v>45000</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>27000</v>
+        <v>45000</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -1892,28 +1926,28 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>478494.70000000001</v>
+        <v>537119.69999999995</v>
       </c>
       <c r="I3">
-        <v>824052.40000073402</v>
+        <v>866348.00000073388</v>
       </c>
       <c r="J3">
-        <v>280632</v>
+        <v>292457</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
       </c>
       <c r="L3">
-        <v>180000</v>
+        <v>220499.99999999997</v>
       </c>
       <c r="M3">
         <v>50000</v>
       </c>
       <c r="N3">
-        <v>6153.3000000000002</v>
+        <v>12453.300000000001</v>
       </c>
       <c r="O3">
-        <v>774052.40000073402</v>
+        <v>816348.00000073388</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -1922,13 +1956,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8893069.1459096484</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>9025947.9519096464</v>
+        <v>8469478.9159991127</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -2028,13 +2062,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>475794.70000000001</v>
+        <v>487619.69999999995</v>
       </c>
       <c r="I2">
-        <v>1111349.8</v>
+        <v>1133506</v>
       </c>
       <c r="J2">
-        <v>280632</v>
+        <v>292457</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -2049,7 +2083,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1061349.8</v>
+        <v>1083506</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -2078,13 +2112,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>27000</v>
+        <v>45000</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>27000</v>
+        <v>45000</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -2093,28 +2127,28 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>478494.70000000001</v>
+        <v>537119.69999999995</v>
       </c>
       <c r="I3">
-        <v>1381349.7999998129</v>
+        <v>1268505.9999999064</v>
       </c>
       <c r="J3">
-        <v>280632</v>
+        <v>292457</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
       </c>
       <c r="L3">
-        <v>180000</v>
+        <v>220499.99999999997</v>
       </c>
       <c r="M3">
         <v>50000</v>
       </c>
       <c r="N3">
-        <v>6153.3000000000002</v>
+        <v>12453.300000000001</v>
       </c>
       <c r="O3">
-        <v>1331349.7999998129</v>
+        <v>1218505.9999999064</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -2123,13 +2157,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>10070815.792776028</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>10353236.096776025</v>
+        <v>8639818.2239991091</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -2229,13 +2263,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>475794.70000000001</v>
+        <v>487619.69999999995</v>
       </c>
       <c r="I2">
-        <v>1111349.8</v>
+        <v>1133506</v>
       </c>
       <c r="J2">
-        <v>280632</v>
+        <v>292457</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -2250,7 +2284,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1061349.8</v>
+        <v>1083506</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -2279,13 +2313,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>27000</v>
+        <v>45000</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>27000</v>
+        <v>45000</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -2294,28 +2328,28 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>478494.70000000001</v>
+        <v>537119.69999999995</v>
       </c>
       <c r="I3">
-        <v>1381349.7999998129</v>
+        <v>846208.60000073398</v>
       </c>
       <c r="J3">
-        <v>280632</v>
+        <v>292457</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
       </c>
       <c r="L3">
-        <v>180000</v>
+        <v>220499.99999999997</v>
       </c>
       <c r="M3">
         <v>50000</v>
       </c>
       <c r="N3">
-        <v>6153.3000000000002</v>
+        <v>12453.300000000001</v>
       </c>
       <c r="O3">
-        <v>1331349.7999998129</v>
+        <v>796208.60000073398</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -2324,13 +2358,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8229999.9999991106</v>
+        <v>8669702.1254661772</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>8358518.7319991095</v>
+        <v>8802580.9314661752</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -2430,13 +2464,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>475794.70000000001</v>
+        <v>487619.69999999995</v>
       </c>
       <c r="I2">
-        <v>1111349.8</v>
+        <v>1133506</v>
       </c>
       <c r="J2">
-        <v>280632</v>
+        <v>292457</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -2451,7 +2485,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1061349.8</v>
+        <v>1083506</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -2480,13 +2514,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>27000</v>
+        <v>45000</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>27000</v>
+        <v>45000</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -2495,28 +2529,28 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>478494.70000000001</v>
+        <v>537119.69999999995</v>
       </c>
       <c r="I3">
-        <v>1381349.7999998129</v>
+        <v>1403505.999999813</v>
       </c>
       <c r="J3">
-        <v>280632</v>
+        <v>292457</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
       </c>
       <c r="L3">
-        <v>180000</v>
+        <v>220499.99999999997</v>
       </c>
       <c r="M3">
         <v>50000</v>
       </c>
       <c r="N3">
-        <v>6153.3000000000002</v>
+        <v>12453.300000000001</v>
       </c>
       <c r="O3">
-        <v>1331349.7999998129</v>
+        <v>1353505.9999998128</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -2525,13 +2559,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8999999.9999775533</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>9061671.6859775539</v>
+        <v>8512420.3039991111</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -2631,13 +2665,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>475794.70000000001</v>
+        <v>487619.69999999995</v>
       </c>
       <c r="I2">
-        <v>1111349.8</v>
+        <v>1133506</v>
       </c>
       <c r="J2">
-        <v>280632</v>
+        <v>292457</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -2652,7 +2686,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1061349.8</v>
+        <v>1083506</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -2681,13 +2715,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>27000</v>
+        <v>45000</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>27000</v>
+        <v>45000</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -2696,28 +2730,28 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>478494.70000000001</v>
+        <v>537119.69999999995</v>
       </c>
       <c r="I3">
-        <v>1381349.7999998129</v>
+        <v>1403505.999999813</v>
       </c>
       <c r="J3">
-        <v>280632</v>
+        <v>292457</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
       </c>
       <c r="L3">
-        <v>180000</v>
+        <v>220499.99999999997</v>
       </c>
       <c r="M3">
         <v>50000</v>
       </c>
       <c r="N3">
-        <v>6153.3000000000002</v>
+        <v>12453.300000000001</v>
       </c>
       <c r="O3">
-        <v>1331349.7999998129</v>
+        <v>1353505.9999998128</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -2726,13 +2760,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8229999.9999991106</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>8140372.5099991113</v>
+        <v>9128518.731977554</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -2832,13 +2866,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>475794.70000000001</v>
+        <v>487619.69999999995</v>
       </c>
       <c r="I2">
-        <v>1111349.8</v>
+        <v>1133506</v>
       </c>
       <c r="J2">
-        <v>280632</v>
+        <v>292457</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -2853,7 +2887,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1061349.8</v>
+        <v>1083506</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -2882,13 +2916,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>27000</v>
+        <v>45000</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>27000</v>
+        <v>45000</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -2897,28 +2931,28 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>478494.70000000001</v>
+        <v>537119.69999999995</v>
       </c>
       <c r="I3">
-        <v>1381349.7999998129</v>
+        <v>1403505.999999813</v>
       </c>
       <c r="J3">
-        <v>280632</v>
+        <v>292457</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
       </c>
       <c r="L3">
-        <v>180000</v>
+        <v>220499.99999999997</v>
       </c>
       <c r="M3">
         <v>50000</v>
       </c>
       <c r="N3">
-        <v>6153.3000000000002</v>
+        <v>12453.300000000001</v>
       </c>
       <c r="O3">
-        <v>1331349.7999998129</v>
+        <v>1353505.9999998128</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -2927,13 +2961,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8229999.9999991106</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>8433484.9599991105</v>
+        <v>9061671.6859775539</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -3033,13 +3067,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>475794.70000000001</v>
+        <v>487619.69999999995</v>
       </c>
       <c r="I2">
-        <v>1111349.8</v>
+        <v>1133506</v>
       </c>
       <c r="J2">
-        <v>280632</v>
+        <v>292457</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -3054,7 +3088,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1061349.8</v>
+        <v>1083506</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -3083,13 +3117,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>27000</v>
+        <v>45000</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>27000</v>
+        <v>45000</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -3098,28 +3132,28 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>478494.70000000001</v>
+        <v>537119.69999999995</v>
       </c>
       <c r="I3">
-        <v>1381349.7999998129</v>
+        <v>1252024.3</v>
       </c>
       <c r="J3">
-        <v>280632</v>
+        <v>292457</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
       </c>
       <c r="L3">
-        <v>180000</v>
+        <v>220499.99999999997</v>
       </c>
       <c r="M3">
         <v>50000</v>
       </c>
       <c r="N3">
-        <v>6153.3000000000002</v>
+        <v>12453.300000000001</v>
       </c>
       <c r="O3">
-        <v>1331349.7999998129</v>
+        <v>1202024.2999999998</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -3134,7 +3168,7 @@
         <v>1</v>
       </c>
       <c r="T3">
-        <v>8440604.3459991124</v>
+        <v>8417587.9999991078</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -3234,13 +3268,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>475794.70000000001</v>
+        <v>487619.69999999995</v>
       </c>
       <c r="I2">
-        <v>1111349.8</v>
+        <v>1133506</v>
       </c>
       <c r="J2">
-        <v>280632</v>
+        <v>292457</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -3255,7 +3289,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1061349.8</v>
+        <v>1083506</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -3284,13 +3318,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>27000</v>
+        <v>45000</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>27000</v>
+        <v>45000</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -3299,28 +3333,28 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>478494.70000000001</v>
+        <v>537119.69999999995</v>
       </c>
       <c r="I3">
-        <v>1246349.7999999064</v>
+        <v>1403505.999999813</v>
       </c>
       <c r="J3">
-        <v>280632</v>
+        <v>292457</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
       </c>
       <c r="L3">
-        <v>180000</v>
+        <v>220499.99999999997</v>
       </c>
       <c r="M3">
         <v>50000</v>
       </c>
       <c r="N3">
-        <v>6153.3000000000002</v>
+        <v>12453.300000000001</v>
       </c>
       <c r="O3">
-        <v>1196349.7999999064</v>
+        <v>1353505.9999998128</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -3329,13 +3363,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8588074.1001150701</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>8728702.1301150694</v>
+        <v>8140372.5099991113</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -3435,13 +3469,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>475794.70000000001</v>
+        <v>487619.69999999995</v>
       </c>
       <c r="I2">
-        <v>1111349.8</v>
+        <v>1133506</v>
       </c>
       <c r="J2">
-        <v>280632</v>
+        <v>292457</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -3456,7 +3490,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1061349.8</v>
+        <v>1083506</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -3485,13 +3519,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>27000</v>
+        <v>45000</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>27000</v>
+        <v>45000</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -3500,28 +3534,28 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>478494.70000000001</v>
+        <v>537119.69999999995</v>
       </c>
       <c r="I3">
-        <v>1011349.7999997991</v>
+        <v>1403505.999999813</v>
       </c>
       <c r="J3">
-        <v>280632</v>
+        <v>292457</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
       </c>
       <c r="L3">
-        <v>180000</v>
+        <v>220499.99999999997</v>
       </c>
       <c r="M3">
         <v>50000</v>
       </c>
       <c r="N3">
-        <v>6153.3000000000002</v>
+        <v>12453.300000000001</v>
       </c>
       <c r="O3">
-        <v>961349.799999799</v>
+        <v>1353505.9999998128</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -3530,13 +3564,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8999999.9999775533</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>9105477.679977553</v>
+        <v>8433484.9599991105</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -3636,13 +3670,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>475794.70000000001</v>
+        <v>487619.69999999995</v>
       </c>
       <c r="I2">
-        <v>1111349.8</v>
+        <v>1133506</v>
       </c>
       <c r="J2">
-        <v>280632</v>
+        <v>292457</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -3657,7 +3691,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1061349.8</v>
+        <v>1083506</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -3686,13 +3720,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>27000</v>
+        <v>45000</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>27000</v>
+        <v>45000</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -3701,28 +3735,28 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>478494.70000000001</v>
+        <v>537119.69999999995</v>
       </c>
       <c r="I3">
-        <v>1011349.7999997991</v>
+        <v>1268505.9999999064</v>
       </c>
       <c r="J3">
-        <v>280632</v>
+        <v>292457</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
       </c>
       <c r="L3">
-        <v>180000</v>
+        <v>220499.99999999997</v>
       </c>
       <c r="M3">
         <v>50000</v>
       </c>
       <c r="N3">
-        <v>6153.3000000000002</v>
+        <v>12453.300000000001</v>
       </c>
       <c r="O3">
-        <v>961349.799999799</v>
+        <v>1218505.9999999064</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -3731,13 +3765,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8229999.9999991106</v>
+        <v>8337047.6218461366</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>8338713.64999911</v>
+        <v>8477675.6518461388</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -3837,13 +3871,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>475794.70000000001</v>
+        <v>487619.69999999995</v>
       </c>
       <c r="I2">
-        <v>1111349.8</v>
+        <v>1133506</v>
       </c>
       <c r="J2">
-        <v>280632</v>
+        <v>292457</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -3858,7 +3892,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1061349.8</v>
+        <v>1083506</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -3887,13 +3921,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>27000</v>
+        <v>45000</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>27000</v>
+        <v>45000</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -3902,28 +3936,28 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>478494.70000000001</v>
+        <v>537119.69999999995</v>
       </c>
       <c r="I3">
-        <v>1246349.7999999064</v>
+        <v>1033505.9999997988</v>
       </c>
       <c r="J3">
-        <v>280632</v>
+        <v>292457</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
       </c>
       <c r="L3">
-        <v>180000</v>
+        <v>220499.99999999997</v>
       </c>
       <c r="M3">
         <v>50000</v>
       </c>
       <c r="N3">
-        <v>6153.3000000000002</v>
+        <v>12453.300000000001</v>
       </c>
       <c r="O3">
-        <v>1196349.7999999064</v>
+        <v>983505.99999979883</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -3932,13 +3966,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8999999.9999775533</v>
+        <v>8952976.5088214558</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>9131647.4399775527</v>
+        <v>9058454.1888214555</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -4038,13 +4072,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>475794.70000000001</v>
+        <v>487619.69999999995</v>
       </c>
       <c r="I2">
-        <v>1111349.8</v>
+        <v>1133506</v>
       </c>
       <c r="J2">
-        <v>280632</v>
+        <v>292457</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -4059,7 +4093,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1061349.8</v>
+        <v>1083506</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -4088,13 +4122,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>27000</v>
+        <v>45000</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>27000</v>
+        <v>45000</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -4103,28 +4137,28 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>478494.70000000001</v>
+        <v>537119.69999999995</v>
       </c>
       <c r="I3">
-        <v>1111349.8</v>
+        <v>1033505.9999997988</v>
       </c>
       <c r="J3">
-        <v>280632</v>
+        <v>292457</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
       </c>
       <c r="L3">
-        <v>180000</v>
+        <v>220499.99999999997</v>
       </c>
       <c r="M3">
         <v>50000</v>
       </c>
       <c r="N3">
-        <v>6153.3000000000002</v>
+        <v>12453.300000000001</v>
       </c>
       <c r="O3">
-        <v>1061349.8</v>
+        <v>983505.99999979883</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -4133,13 +4167,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8999999.9999775533</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>9104398.0899775531</v>
+        <v>8338713.64999911</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -4239,13 +4273,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>475794.70000000001</v>
+        <v>487619.69999999995</v>
       </c>
       <c r="I2">
-        <v>1111349.8</v>
+        <v>1133506</v>
       </c>
       <c r="J2">
-        <v>280632</v>
+        <v>292457</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -4260,7 +4294,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1061349.8</v>
+        <v>1083506</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -4289,13 +4323,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>27000</v>
+        <v>45000</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>27000</v>
+        <v>45000</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -4304,28 +4338,28 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>478494.70000000001</v>
+        <v>537119.69999999995</v>
       </c>
       <c r="I3">
-        <v>1246349.7999999064</v>
+        <v>1268505.9999999064</v>
       </c>
       <c r="J3">
-        <v>280632</v>
+        <v>292457</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
       </c>
       <c r="L3">
-        <v>180000</v>
+        <v>220499.99999999997</v>
       </c>
       <c r="M3">
         <v>50000</v>
       </c>
       <c r="N3">
-        <v>6153.3000000000002</v>
+        <v>12453.300000000001</v>
       </c>
       <c r="O3">
-        <v>1196349.7999999064</v>
+        <v>1218505.9999999064</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -4334,13 +4368,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8229999.9999991106</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>8359167.7799991118</v>
+        <v>9131647.4399775527</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -4440,13 +4474,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>475794.70000000001</v>
+        <v>487619.69999999995</v>
       </c>
       <c r="I2">
-        <v>1111349.8</v>
+        <v>1133506</v>
       </c>
       <c r="J2">
-        <v>280632</v>
+        <v>292457</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -4461,7 +4495,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1061349.8</v>
+        <v>1083506</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -4490,13 +4524,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>27000</v>
+        <v>45000</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>27000</v>
+        <v>45000</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -4505,28 +4539,28 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>478494.70000000001</v>
+        <v>537119.69999999995</v>
       </c>
       <c r="I3">
-        <v>1381349.7999998129</v>
+        <v>1133506</v>
       </c>
       <c r="J3">
-        <v>280632</v>
+        <v>292457</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
       </c>
       <c r="L3">
-        <v>180000</v>
+        <v>220499.99999999997</v>
       </c>
       <c r="M3">
         <v>50000</v>
       </c>
       <c r="N3">
-        <v>6153.3000000000002</v>
+        <v>12453.300000000001</v>
       </c>
       <c r="O3">
-        <v>1331349.7999998129</v>
+        <v>1083506</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -4535,13 +4569,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8999999.9999775533</v>
+        <v>8856470.4421879835</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>9263906.2799775526</v>
+        <v>8960868.5321879834</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -4641,13 +4675,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>475794.70000000001</v>
+        <v>487619.69999999995</v>
       </c>
       <c r="I2">
-        <v>1111349.8</v>
+        <v>1133506</v>
       </c>
       <c r="J2">
-        <v>280632</v>
+        <v>292457</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -4662,7 +4696,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1061349.8</v>
+        <v>1083506</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -4691,13 +4725,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>27000</v>
+        <v>45000</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>27000</v>
+        <v>45000</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -4706,28 +4740,28 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>478494.70000000001</v>
+        <v>537119.69999999995</v>
       </c>
       <c r="I3">
-        <v>1011349.7999997991</v>
+        <v>1268505.9999999064</v>
       </c>
       <c r="J3">
-        <v>280632</v>
+        <v>292457</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
       </c>
       <c r="L3">
-        <v>180000</v>
+        <v>220499.99999999997</v>
       </c>
       <c r="M3">
         <v>50000</v>
       </c>
       <c r="N3">
-        <v>6153.3000000000002</v>
+        <v>12453.300000000001</v>
       </c>
       <c r="O3">
-        <v>961349.799999799</v>
+        <v>1218505.9999999064</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -4736,13 +4770,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8999999.9999775533</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>9166147.929977553</v>
+        <v>8359167.7799991118</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -4842,13 +4876,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>475794.70000000001</v>
+        <v>487619.69999999995</v>
       </c>
       <c r="I2">
-        <v>1111349.8</v>
+        <v>1133506</v>
       </c>
       <c r="J2">
-        <v>280632</v>
+        <v>292457</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -4863,7 +4897,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1061349.8</v>
+        <v>1083506</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -4892,13 +4926,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>27000</v>
+        <v>45000</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>27000</v>
+        <v>45000</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -4907,28 +4941,28 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>478494.70000000001</v>
+        <v>537119.69999999995</v>
       </c>
       <c r="I3">
-        <v>844191.80000073393</v>
+        <v>1403505.999999813</v>
       </c>
       <c r="J3">
-        <v>280632</v>
+        <v>292457</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
       </c>
       <c r="L3">
-        <v>180000</v>
+        <v>220499.99999999997</v>
       </c>
       <c r="M3">
         <v>50000</v>
       </c>
       <c r="N3">
-        <v>6153.3000000000002</v>
+        <v>12453.300000000001</v>
       </c>
       <c r="O3">
-        <v>794191.80000073381</v>
+        <v>1353505.9999998128</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -4943,7 +4977,7 @@
         <v>1</v>
       </c>
       <c r="T3">
-        <v>9186027.3499775529</v>
+        <v>9263906.2799775526</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -5043,13 +5077,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>475794.70000000001</v>
+        <v>487619.69999999995</v>
       </c>
       <c r="I2">
-        <v>1111349.8</v>
+        <v>1133506</v>
       </c>
       <c r="J2">
-        <v>280632</v>
+        <v>292457</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -5064,7 +5098,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1061349.8</v>
+        <v>1083506</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -5093,13 +5127,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>27000</v>
+        <v>45000</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>27000</v>
+        <v>45000</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -5108,28 +5142,28 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>478494.70000000001</v>
+        <v>537119.69999999995</v>
       </c>
       <c r="I3">
-        <v>1011349.7999997991</v>
+        <v>1033505.9999997988</v>
       </c>
       <c r="J3">
-        <v>280632</v>
+        <v>292457</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
       </c>
       <c r="L3">
-        <v>180000</v>
+        <v>220499.99999999997</v>
       </c>
       <c r="M3">
         <v>50000</v>
       </c>
       <c r="N3">
-        <v>6153.3000000000002</v>
+        <v>12453.300000000001</v>
       </c>
       <c r="O3">
-        <v>961349.799999799</v>
+        <v>983505.99999979883</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -5144,7 +5178,7 @@
         <v>1</v>
       </c>
       <c r="T3">
-        <v>9160152.0699775536</v>
+        <v>9166147.929977553</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -5244,13 +5278,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>475794.70000000001</v>
+        <v>487619.69999999995</v>
       </c>
       <c r="I2">
-        <v>1111349.8</v>
+        <v>1133506</v>
       </c>
       <c r="J2">
-        <v>280632</v>
+        <v>292457</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -5265,7 +5299,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1061349.8</v>
+        <v>1083506</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -5294,13 +5328,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>27000</v>
+        <v>45000</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>27000</v>
+        <v>45000</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -5309,28 +5343,28 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>478494.70000000001</v>
+        <v>537119.69999999995</v>
       </c>
       <c r="I3">
-        <v>1381349.7999998129</v>
+        <v>1252024.3</v>
       </c>
       <c r="J3">
-        <v>280632</v>
+        <v>292457</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
       </c>
       <c r="L3">
-        <v>180000</v>
+        <v>220499.99999999997</v>
       </c>
       <c r="M3">
         <v>50000</v>
       </c>
       <c r="N3">
-        <v>6153.3000000000002</v>
+        <v>12453.300000000001</v>
       </c>
       <c r="O3">
-        <v>1331349.7999998129</v>
+        <v>1202024.2999999998</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -5339,13 +5373,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8229999.9999991106</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>8503849.8819991108</v>
+        <v>9157545.9999775533</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -5445,13 +5479,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>475794.70000000001</v>
+        <v>487619.69999999995</v>
       </c>
       <c r="I2">
-        <v>1111349.8</v>
+        <v>1133506</v>
       </c>
       <c r="J2">
-        <v>280632</v>
+        <v>292457</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -5466,7 +5500,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1061349.8</v>
+        <v>1083506</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -5495,13 +5529,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>27000</v>
+        <v>45000</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>27000</v>
+        <v>45000</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -5510,28 +5544,28 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>478494.70000000001</v>
+        <v>537119.69999999995</v>
       </c>
       <c r="I3">
-        <v>1111349.8</v>
+        <v>866348.00000073388</v>
       </c>
       <c r="J3">
-        <v>280632</v>
+        <v>292457</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
       </c>
       <c r="L3">
-        <v>180000</v>
+        <v>220499.99999999997</v>
       </c>
       <c r="M3">
         <v>50000</v>
       </c>
       <c r="N3">
-        <v>6153.3000000000002</v>
+        <v>12453.300000000001</v>
       </c>
       <c r="O3">
-        <v>1061349.8</v>
+        <v>816348.00000073388</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -5546,7 +5580,7 @@
         <v>1</v>
       </c>
       <c r="T3">
-        <v>9183949.7199775539</v>
+        <v>9186027.3499775529</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -5646,13 +5680,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>475794.70000000001</v>
+        <v>487619.69999999995</v>
       </c>
       <c r="I2">
-        <v>1111349.8</v>
+        <v>1133506</v>
       </c>
       <c r="J2">
-        <v>280632</v>
+        <v>292457</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -5667,7 +5701,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1061349.8</v>
+        <v>1083506</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -5696,13 +5730,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>27000</v>
+        <v>45000</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>27000</v>
+        <v>45000</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -5711,28 +5745,28 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>478494.70000000001</v>
+        <v>537119.69999999995</v>
       </c>
       <c r="I3">
-        <v>1381349.7999998129</v>
+        <v>1033505.9999997988</v>
       </c>
       <c r="J3">
-        <v>280632</v>
+        <v>292457</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
       </c>
       <c r="L3">
-        <v>180000</v>
+        <v>220499.99999999997</v>
       </c>
       <c r="M3">
         <v>50000</v>
       </c>
       <c r="N3">
-        <v>6153.3000000000002</v>
+        <v>12453.300000000001</v>
       </c>
       <c r="O3">
-        <v>1331349.7999998129</v>
+        <v>983505.99999979883</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -5741,13 +5775,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8229999.9999991106</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>8442695.0099991094</v>
+        <v>9160152.0699775536</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -5847,13 +5881,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>475794.70000000001</v>
+        <v>487619.69999999995</v>
       </c>
       <c r="I2">
-        <v>1111349.8</v>
+        <v>1133506</v>
       </c>
       <c r="J2">
-        <v>280632</v>
+        <v>292457</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -5868,7 +5902,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1061349.8</v>
+        <v>1083506</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -5897,13 +5931,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>27000</v>
+        <v>45000</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>27000</v>
+        <v>45000</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -5912,28 +5946,28 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>478494.70000000001</v>
+        <v>537119.69999999995</v>
       </c>
       <c r="I3">
-        <v>1111349.8</v>
+        <v>1133506</v>
       </c>
       <c r="J3">
-        <v>280632</v>
+        <v>292457</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
       </c>
       <c r="L3">
-        <v>180000</v>
+        <v>220499.99999999997</v>
       </c>
       <c r="M3">
         <v>50000</v>
       </c>
       <c r="N3">
-        <v>6153.3000000000002</v>
+        <v>12453.300000000001</v>
       </c>
       <c r="O3">
-        <v>1061349.8</v>
+        <v>1083506</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -5942,13 +5976,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8229999.9999991106</v>
+        <v>8892014.4977661427</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>8291125.7399991108</v>
+        <v>9075964.2177661415</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -6048,13 +6082,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>475794.70000000001</v>
+        <v>487619.69999999995</v>
       </c>
       <c r="I2">
-        <v>1111349.8</v>
+        <v>1133506</v>
       </c>
       <c r="J2">
-        <v>280632</v>
+        <v>292457</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -6069,7 +6103,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1061349.8</v>
+        <v>1083506</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -6098,13 +6132,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>27000</v>
+        <v>45000</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>27000</v>
+        <v>45000</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -6113,28 +6147,28 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>478494.70000000001</v>
+        <v>537119.69999999995</v>
       </c>
       <c r="I3">
-        <v>1011349.7999997991</v>
+        <v>1403505.999999813</v>
       </c>
       <c r="J3">
-        <v>280632</v>
+        <v>292457</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
       </c>
       <c r="L3">
-        <v>180000</v>
+        <v>220499.99999999997</v>
       </c>
       <c r="M3">
         <v>50000</v>
       </c>
       <c r="N3">
-        <v>6153.3000000000002</v>
+        <v>12453.300000000001</v>
       </c>
       <c r="O3">
-        <v>961349.799999799</v>
+        <v>1353505.9999998128</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -6149,7 +6183,7 @@
         <v>1</v>
       </c>
       <c r="T3">
-        <v>8261744.7299991101</v>
+        <v>8442695.0099991094</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -6249,13 +6283,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>475794.70000000001</v>
+        <v>487619.69999999995</v>
       </c>
       <c r="I2">
-        <v>1111349.8</v>
+        <v>1133506</v>
       </c>
       <c r="J2">
-        <v>280632</v>
+        <v>292457</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -6270,7 +6304,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1061349.8</v>
+        <v>1083506</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -6299,13 +6333,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>27000</v>
+        <v>45000</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>27000</v>
+        <v>45000</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -6314,28 +6348,28 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>478494.70000000001</v>
+        <v>537119.69999999995</v>
       </c>
       <c r="I3">
-        <v>844191.80000073393</v>
+        <v>1133506</v>
       </c>
       <c r="J3">
-        <v>280632</v>
+        <v>292457</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
       </c>
       <c r="L3">
-        <v>180000</v>
+        <v>220499.99999999997</v>
       </c>
       <c r="M3">
         <v>50000</v>
       </c>
       <c r="N3">
-        <v>6153.3000000000002</v>
+        <v>12453.300000000001</v>
       </c>
       <c r="O3">
-        <v>794191.80000073381</v>
+        <v>1083506</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -6344,13 +6378,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8999999.9999775533</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>9088058.5399775542</v>
+        <v>8291125.7399991108</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -6450,13 +6484,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>475794.70000000001</v>
+        <v>487619.69999999995</v>
       </c>
       <c r="I2">
-        <v>1111349.8</v>
+        <v>1133506</v>
       </c>
       <c r="J2">
-        <v>280632</v>
+        <v>292457</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -6471,7 +6505,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1061349.8</v>
+        <v>1083506</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -6500,13 +6534,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>27000</v>
+        <v>45000</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>27000</v>
+        <v>45000</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -6515,28 +6549,28 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>478494.70000000001</v>
+        <v>537119.69999999995</v>
       </c>
       <c r="I3">
-        <v>844191.80000073393</v>
+        <v>1033505.9999997988</v>
       </c>
       <c r="J3">
-        <v>280632</v>
+        <v>292457</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
       </c>
       <c r="L3">
-        <v>180000</v>
+        <v>220499.99999999997</v>
       </c>
       <c r="M3">
         <v>50000</v>
       </c>
       <c r="N3">
-        <v>6153.3000000000002</v>
+        <v>12453.300000000001</v>
       </c>
       <c r="O3">
-        <v>794191.80000073381</v>
+        <v>983505.99999979883</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -6545,13 +6579,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8999999.9999775533</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>9135931.8499775529</v>
+        <v>8261744.7299991101</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -6651,13 +6685,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>475794.70000000001</v>
+        <v>487619.69999999995</v>
       </c>
       <c r="I2">
-        <v>1111349.8</v>
+        <v>1133506</v>
       </c>
       <c r="J2">
-        <v>280632</v>
+        <v>292457</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -6672,7 +6706,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1061349.8</v>
+        <v>1083506</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -6701,13 +6735,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>27000</v>
+        <v>45000</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>27000</v>
+        <v>45000</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -6716,28 +6750,430 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>478494.70000000001</v>
+        <v>537119.69999999995</v>
       </c>
       <c r="I3">
-        <v>1034310.6000007342</v>
+        <v>866348.00000073388</v>
       </c>
       <c r="J3">
-        <v>280632</v>
+        <v>292457</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
       </c>
       <c r="L3">
-        <v>180000</v>
+        <v>220499.99999999997</v>
       </c>
       <c r="M3">
         <v>50000</v>
       </c>
       <c r="N3">
+        <v>12453.300000000001</v>
+      </c>
+      <c r="O3">
+        <v>816348.00000073388</v>
+      </c>
+      <c r="P3">
+        <v>469427.99999962631</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>8999999.9999775533</v>
+      </c>
+      <c r="S3">
+        <v>1</v>
+      </c>
+      <c r="T3">
+        <v>9088058.5399775542</v>
+      </c>
+      <c r="U3">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:xdr="http://purl.oclc.org/ooxml/drawingml/spreadsheetDrawing">
+  <dimension ref="A1:U3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="259" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="259" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="259" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="259" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="259" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="259" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="259" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="259" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="259" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="259" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="259" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="259" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="259" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="259" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="259" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="259" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="259" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" s="259" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" s="259" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" s="259" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="257">
+        <v>43831</v>
+      </c>
+      <c r="B2">
+        <v>7</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>487619.69999999995</v>
+      </c>
+      <c r="I2">
+        <v>1133506</v>
+      </c>
+      <c r="J2">
+        <v>292457</v>
+      </c>
+      <c r="K2">
+        <v>9009.3999999999996</v>
+      </c>
+      <c r="L2">
+        <v>180000</v>
+      </c>
+      <c r="M2">
+        <v>50000</v>
+      </c>
+      <c r="N2">
         <v>6153.3000000000002</v>
       </c>
+      <c r="O2">
+        <v>1083506</v>
+      </c>
+      <c r="P2">
+        <v>409927.99999981304</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>8229999.9999999963</v>
+      </c>
+      <c r="S2">
+        <v>1</v>
+      </c>
+      <c r="T2" s="258" t="s">
+        <v>19</v>
+      </c>
+      <c r="U2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="257">
+        <v>44197</v>
+      </c>
+      <c r="B3">
+        <v>7</v>
+      </c>
+      <c r="C3">
+        <v>45000</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>45000</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>7999.9999999998645</v>
+      </c>
+      <c r="H3">
+        <v>537119.69999999995</v>
+      </c>
+      <c r="I3">
+        <v>866348.00000073388</v>
+      </c>
+      <c r="J3">
+        <v>292457</v>
+      </c>
+      <c r="K3">
+        <v>11709.4</v>
+      </c>
+      <c r="L3">
+        <v>220499.99999999997</v>
+      </c>
+      <c r="M3">
+        <v>50000</v>
+      </c>
+      <c r="N3">
+        <v>12453.300000000001</v>
+      </c>
       <c r="O3">
-        <v>984310.60000073421</v>
+        <v>816348.00000073388</v>
+      </c>
+      <c r="P3">
+        <v>469427.99999962631</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>8999999.9999775533</v>
+      </c>
+      <c r="S3">
+        <v>1</v>
+      </c>
+      <c r="T3">
+        <v>9135931.8499775529</v>
+      </c>
+      <c r="U3">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:xdr="http://purl.oclc.org/ooxml/drawingml/spreadsheetDrawing">
+  <dimension ref="A1:U3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="266" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="266" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="266" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="266" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="266" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="266" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="266" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="266" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="266" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="266" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="266" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="266" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="266" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="266" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="266" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="266" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="266" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" s="266" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" s="266" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" s="266" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="264">
+        <v>43831</v>
+      </c>
+      <c r="B2">
+        <v>7</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>487619.69999999995</v>
+      </c>
+      <c r="I2">
+        <v>1133506</v>
+      </c>
+      <c r="J2">
+        <v>292457</v>
+      </c>
+      <c r="K2">
+        <v>9009.3999999999996</v>
+      </c>
+      <c r="L2">
+        <v>180000</v>
+      </c>
+      <c r="M2">
+        <v>50000</v>
+      </c>
+      <c r="N2">
+        <v>6153.3000000000002</v>
+      </c>
+      <c r="O2">
+        <v>1083506</v>
+      </c>
+      <c r="P2">
+        <v>409927.99999981304</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>8229999.9999999963</v>
+      </c>
+      <c r="S2">
+        <v>1</v>
+      </c>
+      <c r="T2" s="265" t="s">
+        <v>19</v>
+      </c>
+      <c r="U2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="264">
+        <v>44197</v>
+      </c>
+      <c r="B3">
+        <v>7</v>
+      </c>
+      <c r="C3">
+        <v>45000</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>45000</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>7999.9999999998645</v>
+      </c>
+      <c r="H3">
+        <v>537119.69999999995</v>
+      </c>
+      <c r="I3">
+        <v>1056466.8000007342</v>
+      </c>
+      <c r="J3">
+        <v>292457</v>
+      </c>
+      <c r="K3">
+        <v>11709.4</v>
+      </c>
+      <c r="L3">
+        <v>220499.99999999997</v>
+      </c>
+      <c r="M3">
+        <v>50000</v>
+      </c>
+      <c r="N3">
+        <v>12453.300000000001</v>
+      </c>
+      <c r="O3">
+        <v>1006466.8000007342</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -6852,13 +7288,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>475794.70000000001</v>
+        <v>487619.69999999995</v>
       </c>
       <c r="I2">
-        <v>1111349.8</v>
+        <v>1133506</v>
       </c>
       <c r="J2">
-        <v>280632</v>
+        <v>292457</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -6873,7 +7309,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1061349.8</v>
+        <v>1083506</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -6899,49 +7335,49 @@
         <v>44197</v>
       </c>
       <c r="B3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>45000</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>45000</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>478494.70000000001</v>
+        <v>537119.69999999995</v>
       </c>
       <c r="I3">
-        <v>1381349.7999998129</v>
+        <v>1403505.999999813</v>
       </c>
       <c r="J3">
-        <v>280632</v>
+        <v>292457</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
       </c>
       <c r="L3">
-        <v>180000</v>
+        <v>220499.99999999997</v>
       </c>
       <c r="M3">
         <v>50000</v>
       </c>
       <c r="N3">
-        <v>6153.3000000000002</v>
+        <v>12453.300000000001</v>
       </c>
       <c r="O3">
-        <v>1331349.7999998129</v>
+        <v>1353505.9999998128</v>
       </c>
       <c r="P3">
-        <v>477427.99999962613</v>
+        <v>469427.99999962631</v>
       </c>
       <c r="Q3">
         <v>0</v>
@@ -6953,7 +7389,7 @@
         <v>1</v>
       </c>
       <c r="T3">
-        <v>8521307.2019991111</v>
+        <v>8440604.3459991124</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -7053,13 +7489,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>475794.70000000001</v>
+        <v>487619.69999999995</v>
       </c>
       <c r="I2">
-        <v>1111349.8</v>
+        <v>1133506</v>
       </c>
       <c r="J2">
-        <v>280632</v>
+        <v>292457</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -7074,7 +7510,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1061349.8</v>
+        <v>1083506</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -7100,49 +7536,49 @@
         <v>44197</v>
       </c>
       <c r="B3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>45000</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>45000</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>478494.70000000001</v>
+        <v>537119.69999999995</v>
       </c>
       <c r="I3">
-        <v>1011349.7999997991</v>
+        <v>1403505.999999813</v>
       </c>
       <c r="J3">
-        <v>280632</v>
+        <v>292457</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
       </c>
       <c r="L3">
-        <v>180000</v>
+        <v>220499.99999999997</v>
       </c>
       <c r="M3">
         <v>50000</v>
       </c>
       <c r="N3">
-        <v>6153.3000000000002</v>
+        <v>12453.300000000001</v>
       </c>
       <c r="O3">
-        <v>961349.799999799</v>
+        <v>1353505.9999998128</v>
       </c>
       <c r="P3">
-        <v>477427.99999962613</v>
+        <v>469427.99999962631</v>
       </c>
       <c r="Q3">
         <v>0</v>
@@ -7154,7 +7590,7 @@
         <v>1</v>
       </c>
       <c r="T3">
-        <v>8454903.3319991101</v>
+        <v>8503849.8819991108</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -7254,13 +7690,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>475794.70000000001</v>
+        <v>487619.69999999995</v>
       </c>
       <c r="I2">
-        <v>1111349.8</v>
+        <v>1133506</v>
       </c>
       <c r="J2">
-        <v>280632</v>
+        <v>292457</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -7275,7 +7711,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1061349.8</v>
+        <v>1083506</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -7304,13 +7740,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>27000</v>
+        <v>45000</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>27000</v>
+        <v>45000</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -7319,28 +7755,28 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>478494.70000000001</v>
+        <v>537119.69999999995</v>
       </c>
       <c r="I3">
-        <v>1381349.7999998129</v>
+        <v>1403505.999999813</v>
       </c>
       <c r="J3">
-        <v>280632</v>
+        <v>292457</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
       </c>
       <c r="L3">
-        <v>180000</v>
+        <v>220499.99999999997</v>
       </c>
       <c r="M3">
         <v>50000</v>
       </c>
       <c r="N3">
-        <v>6153.3000000000002</v>
+        <v>12453.300000000001</v>
       </c>
       <c r="O3">
-        <v>1331349.7999998129</v>
+        <v>1353505.9999998128</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -7355,7 +7791,7 @@
         <v>1</v>
       </c>
       <c r="T3">
-        <v>8378032.6279991101</v>
+        <v>8521307.2019991111</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -7455,13 +7891,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>475794.70000000001</v>
+        <v>487619.69999999995</v>
       </c>
       <c r="I2">
-        <v>1111349.8</v>
+        <v>1133506</v>
       </c>
       <c r="J2">
-        <v>280632</v>
+        <v>292457</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -7476,7 +7912,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1061349.8</v>
+        <v>1083506</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -7505,13 +7941,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>27000</v>
+        <v>45000</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>27000</v>
+        <v>45000</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -7520,28 +7956,28 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>478494.70000000001</v>
+        <v>537119.69999999995</v>
       </c>
       <c r="I3">
-        <v>1011349.7999997991</v>
+        <v>1033505.9999997988</v>
       </c>
       <c r="J3">
-        <v>280632</v>
+        <v>292457</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
       </c>
       <c r="L3">
-        <v>180000</v>
+        <v>220499.99999999997</v>
       </c>
       <c r="M3">
         <v>50000</v>
       </c>
       <c r="N3">
-        <v>6153.3000000000002</v>
+        <v>12453.300000000001</v>
       </c>
       <c r="O3">
-        <v>961349.799999799</v>
+        <v>983505.99999979883</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -7550,13 +7986,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8999999.9999775533</v>
+        <v>8229999.9999991106</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>9187857.7959775534</v>
+        <v>8454903.3319991101</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -7656,13 +8092,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>475794.70000000001</v>
+        <v>487619.69999999995</v>
       </c>
       <c r="I2">
-        <v>1111349.8</v>
+        <v>1133506</v>
       </c>
       <c r="J2">
-        <v>280632</v>
+        <v>292457</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -7677,7 +8113,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1061349.8</v>
+        <v>1083506</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -7706,13 +8142,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>27000</v>
+        <v>45000</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>27000</v>
+        <v>45000</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -7721,28 +8157,28 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>478494.70000000001</v>
+        <v>537119.69999999995</v>
       </c>
       <c r="I3">
-        <v>844191.80000073393</v>
+        <v>1403505.999999813</v>
       </c>
       <c r="J3">
-        <v>280632</v>
+        <v>292457</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
       </c>
       <c r="L3">
-        <v>180000</v>
+        <v>220499.99999999997</v>
       </c>
       <c r="M3">
         <v>50000</v>
       </c>
       <c r="N3">
-        <v>6153.3000000000002</v>
+        <v>12453.300000000001</v>
       </c>
       <c r="O3">
-        <v>794191.80000073381</v>
+        <v>1353505.9999998128</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -7757,7 +8193,7 @@
         <v>1</v>
       </c>
       <c r="T3">
-        <v>8417833.5499991123</v>
+        <v>8378032.6279991101</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -7857,13 +8293,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>475794.70000000001</v>
+        <v>487619.69999999995</v>
       </c>
       <c r="I2">
-        <v>1111349.8</v>
+        <v>1133506</v>
       </c>
       <c r="J2">
-        <v>280632</v>
+        <v>292457</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -7878,7 +8314,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1061349.8</v>
+        <v>1083506</v>
       </c>
       <c r="P2">
         <v>409927.99999981304</v>
@@ -7907,13 +8343,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>27000</v>
+        <v>45000</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>27000</v>
+        <v>45000</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -7922,28 +8358,28 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>478494.70000000001</v>
+        <v>537119.69999999995</v>
       </c>
       <c r="I3">
-        <v>1011349.7999997991</v>
+        <v>1033505.9999997988</v>
       </c>
       <c r="J3">
-        <v>280632</v>
+        <v>292457</v>
       </c>
       <c r="K3">
         <v>11709.4</v>
       </c>
       <c r="L3">
-        <v>180000</v>
+        <v>220499.99999999997</v>
       </c>
       <c r="M3">
         <v>50000</v>
       </c>
       <c r="N3">
-        <v>6153.3000000000002</v>
+        <v>12453.300000000001</v>
       </c>
       <c r="O3">
-        <v>961349.799999799</v>
+        <v>983505.99999979883</v>
       </c>
       <c r="P3">
         <v>469427.99999962631</v>
@@ -7952,13 +8388,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8617531.5292699412</v>
+        <v>8999999.9999775533</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
       <c r="T3">
-        <v>8768129.1992699411</v>
+        <v>9187857.7959775534</v>
       </c>
       <c r="U3">
         <v>0</v>

</xml_diff>

<commit_message>
Updated model file to 24MS_MTOM_V1.0.202011.9008. This model file includes all updates done during the integration process
Updated ruleset file to 24 24MS_MTOM_V1.0.9008.rls. This model file includes all the updates done during the integration process.

These changes were made because there were errors noticed in the operational model file and ruleset that had been fixed in the integration development.

Updated output files
</commit_message>
<xml_diff>
--- a/Output Data/MtomToCrss_Annual.xlsx
+++ b/Output Data/MtomToCrss_Annual.xlsx
@@ -6,51 +6,49 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Trace1" sheetId="1" r:id="rId2"/>
-    <sheet name="Trace2" sheetId="2" r:id="rId4"/>
-    <sheet name="Trace3" sheetId="3" r:id="rId5"/>
-    <sheet name="Trace4" sheetId="4" r:id="rId6"/>
-    <sheet name="Trace5" sheetId="5" r:id="rId7"/>
-    <sheet name="Trace6" sheetId="6" r:id="rId8"/>
-    <sheet name="Trace7" sheetId="7" r:id="rId9"/>
-    <sheet name="Trace8" sheetId="8" r:id="rId10"/>
-    <sheet name="Trace9" sheetId="9" r:id="rId11"/>
-    <sheet name="Trace10" sheetId="10" r:id="rId12"/>
-    <sheet name="Trace11" sheetId="11" r:id="rId13"/>
-    <sheet name="Trace12" sheetId="12" r:id="rId14"/>
-    <sheet name="Trace13" sheetId="13" r:id="rId15"/>
-    <sheet name="Trace14" sheetId="14" r:id="rId16"/>
-    <sheet name="Trace15" sheetId="15" r:id="rId17"/>
-    <sheet name="Trace16" sheetId="16" r:id="rId18"/>
-    <sheet name="Trace17" sheetId="17" r:id="rId19"/>
-    <sheet name="Trace18" sheetId="18" r:id="rId20"/>
-    <sheet name="Trace19" sheetId="19" r:id="rId21"/>
-    <sheet name="Trace20" sheetId="20" r:id="rId22"/>
-    <sheet name="Trace21" sheetId="21" r:id="rId23"/>
-    <sheet name="Trace22" sheetId="22" r:id="rId24"/>
-    <sheet name="Trace23" sheetId="23" r:id="rId25"/>
-    <sheet name="Trace24" sheetId="24" r:id="rId26"/>
-    <sheet name="Trace25" sheetId="25" r:id="rId27"/>
-    <sheet name="Trace26" sheetId="26" r:id="rId28"/>
-    <sheet name="Trace27" sheetId="27" r:id="rId29"/>
-    <sheet name="Trace28" sheetId="28" r:id="rId30"/>
-    <sheet name="Trace29" sheetId="29" r:id="rId31"/>
-    <sheet name="Trace30" sheetId="30" r:id="rId32"/>
-    <sheet name="Trace31" sheetId="31" r:id="rId33"/>
-    <sheet name="Trace32" sheetId="32" r:id="rId34"/>
-    <sheet name="Trace33" sheetId="33" r:id="rId35"/>
-    <sheet name="Trace34" sheetId="34" r:id="rId36"/>
-    <sheet name="Trace35" sheetId="35" r:id="rId37"/>
-    <sheet name="Trace36" sheetId="36" r:id="rId38"/>
-    <sheet name="Trace37" sheetId="37" r:id="rId39"/>
-    <sheet name="Trace38" sheetId="38" r:id="rId40"/>
+    <sheet name="Trace3" sheetId="1" r:id="rId2"/>
+    <sheet name="Trace4" sheetId="2" r:id="rId4"/>
+    <sheet name="Trace5" sheetId="3" r:id="rId5"/>
+    <sheet name="Trace6" sheetId="4" r:id="rId6"/>
+    <sheet name="Trace7" sheetId="5" r:id="rId7"/>
+    <sheet name="Trace8" sheetId="6" r:id="rId8"/>
+    <sheet name="Trace9" sheetId="7" r:id="rId9"/>
+    <sheet name="Trace10" sheetId="8" r:id="rId10"/>
+    <sheet name="Trace11" sheetId="9" r:id="rId11"/>
+    <sheet name="Trace12" sheetId="10" r:id="rId12"/>
+    <sheet name="Trace13" sheetId="11" r:id="rId13"/>
+    <sheet name="Trace14" sheetId="12" r:id="rId14"/>
+    <sheet name="Trace15" sheetId="13" r:id="rId15"/>
+    <sheet name="Trace16" sheetId="14" r:id="rId16"/>
+    <sheet name="Trace17" sheetId="15" r:id="rId17"/>
+    <sheet name="Trace18" sheetId="16" r:id="rId18"/>
+    <sheet name="Trace19" sheetId="17" r:id="rId19"/>
+    <sheet name="Trace20" sheetId="18" r:id="rId20"/>
+    <sheet name="Trace21" sheetId="19" r:id="rId21"/>
+    <sheet name="Trace22" sheetId="20" r:id="rId22"/>
+    <sheet name="Trace23" sheetId="21" r:id="rId23"/>
+    <sheet name="Trace24" sheetId="22" r:id="rId24"/>
+    <sheet name="Trace25" sheetId="23" r:id="rId25"/>
+    <sheet name="Trace26" sheetId="24" r:id="rId26"/>
+    <sheet name="Trace27" sheetId="25" r:id="rId27"/>
+    <sheet name="Trace28" sheetId="26" r:id="rId28"/>
+    <sheet name="Trace29" sheetId="27" r:id="rId29"/>
+    <sheet name="Trace30" sheetId="28" r:id="rId30"/>
+    <sheet name="Trace31" sheetId="29" r:id="rId31"/>
+    <sheet name="Trace32" sheetId="30" r:id="rId32"/>
+    <sheet name="Trace33" sheetId="31" r:id="rId33"/>
+    <sheet name="Trace34" sheetId="32" r:id="rId34"/>
+    <sheet name="Trace35" sheetId="33" r:id="rId35"/>
+    <sheet name="Trace36" sheetId="34" r:id="rId36"/>
+    <sheet name="Trace37" sheetId="35" r:id="rId37"/>
+    <sheet name="Trace38" sheetId="36" r:id="rId38"/>
   </sheets>
   <calcPr calcId="125725" fullCalcOnLoad="true"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:xdr="http://purl.oclc.org/ooxml/drawingml/spreadsheetDrawing" count="836" uniqueCount="21">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:xdr="http://purl.oclc.org/ooxml/drawingml/spreadsheetDrawing" count="828" uniqueCount="21">
   <si>
     <t>DCP BWSCP Flags.LB DCP BWSCP</t>
   </si>
@@ -137,7 +135,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="267">
+  <borders count="253">
     <border>
       <start/>
       <end/>
@@ -397,25 +395,11 @@
     <border/>
     <border/>
     <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
-    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="267">
+  <cellXfs count="253">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -741,24 +725,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="252" xfId="0" applyNumberFormat="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="253" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="254" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="255" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="256" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="257" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="258" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="259" xfId="0" applyNumberFormat="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="260" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="261" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="262" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="263" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="264" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="265" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="266" xfId="0" applyNumberFormat="true" applyAlignment="true">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -859,7 +825,7 @@
         <v>485340.90000000002</v>
       </c>
       <c r="I2">
-        <v>1201250.3</v>
+        <v>1218836.3</v>
       </c>
       <c r="J2">
         <v>290178.20000000001</v>
@@ -877,7 +843,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1151250.3</v>
+        <v>1168836.3</v>
       </c>
       <c r="P2">
         <v>402312.99999981298</v>
@@ -924,7 +890,7 @@
         <v>536289.89999999991</v>
       </c>
       <c r="I3">
-        <v>1313229.2</v>
+        <v>1364423.8999999999</v>
       </c>
       <c r="J3">
         <v>290178.20000000001</v>
@@ -942,7 +908,7 @@
         <v>12385.800000000001</v>
       </c>
       <c r="O3">
-        <v>1263229.2</v>
+        <v>1314423.8999999999</v>
       </c>
       <c r="P3">
         <v>461812.99999962619</v>
@@ -951,13 +917,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8229999.9999991106</v>
+        <v>8290517.7212618599</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
-      <c r="T3">
-        <v>8367990.9999991087</v>
+      <c r="T3" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -1057,13 +1023,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>485340.90000000002</v>
+        <v>436704</v>
       </c>
       <c r="I2">
-        <v>1201250.3</v>
+        <v>1218836.3</v>
       </c>
       <c r="J2">
-        <v>290178.20000000001</v>
+        <v>241541.29999999999</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -1078,7 +1044,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1151250.3</v>
+        <v>1168836.3</v>
       </c>
       <c r="P2">
         <v>402312.99999981298</v>
@@ -1107,13 +1073,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>45000</v>
+        <v>29506.000000000102</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>45000</v>
+        <v>29506.000000000102</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -1122,13 +1088,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>536289.89999999991</v>
+        <v>487652.99999999994</v>
       </c>
       <c r="I3">
-        <v>926826.30000073416</v>
+        <v>1171607.3000007339</v>
       </c>
       <c r="J3">
-        <v>290178.20000000001</v>
+        <v>241541.29999999999</v>
       </c>
       <c r="K3">
         <v>13225.9</v>
@@ -1143,7 +1109,7 @@
         <v>12385.800000000001</v>
       </c>
       <c r="O3">
-        <v>876826.30000073405</v>
+        <v>1121607.3000007339</v>
       </c>
       <c r="P3">
         <v>461812.99999962619</v>
@@ -1152,13 +1118,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8229999.9999991106</v>
+        <v>8229999.9999999953</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
-      <c r="T3">
-        <v>8417833.5499991104</v>
+      <c r="T3" s="69" t="s">
+        <v>18</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -1258,13 +1224,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>485340.90000000002</v>
+        <v>436704</v>
       </c>
       <c r="I2">
-        <v>1201250.3</v>
+        <v>1218836.3</v>
       </c>
       <c r="J2">
-        <v>290178.20000000001</v>
+        <v>241541.29999999999</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -1279,7 +1245,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1151250.3</v>
+        <v>1168836.3</v>
       </c>
       <c r="P2">
         <v>402312.99999981298</v>
@@ -1308,13 +1274,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>45000</v>
+        <v>29506.000000000102</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>45000</v>
+        <v>29506.000000000102</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -1323,13 +1289,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>536289.89999999991</v>
+        <v>487652.99999999994</v>
       </c>
       <c r="I3">
-        <v>1101250.2999997991</v>
+        <v>981755.30000073381</v>
       </c>
       <c r="J3">
-        <v>290178.20000000001</v>
+        <v>241541.29999999999</v>
       </c>
       <c r="K3">
         <v>13225.9</v>
@@ -1344,7 +1310,7 @@
         <v>12385.800000000001</v>
       </c>
       <c r="O3">
-        <v>1051250.2999997991</v>
+        <v>931755.30000073381</v>
       </c>
       <c r="P3">
         <v>461812.99999962619</v>
@@ -1353,13 +1319,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8229999.9999991106</v>
+        <v>8229999.9999999953</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
-      <c r="T3">
-        <v>8380597.6699991105</v>
+      <c r="T3" s="76" t="s">
+        <v>18</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -1459,13 +1425,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>485340.90000000002</v>
+        <v>436704</v>
       </c>
       <c r="I2">
-        <v>1201250.3</v>
+        <v>1218836.3</v>
       </c>
       <c r="J2">
-        <v>290178.20000000001</v>
+        <v>241541.29999999999</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -1480,7 +1446,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1151250.3</v>
+        <v>1168836.3</v>
       </c>
       <c r="P2">
         <v>402312.99999981298</v>
@@ -1509,13 +1475,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>45000</v>
+        <v>29506.000000000102</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>45000</v>
+        <v>29506.000000000102</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -1524,13 +1490,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>536289.89999999991</v>
+        <v>487652.99999999994</v>
       </c>
       <c r="I3">
-        <v>1117671.7000007343</v>
+        <v>981755.30000073381</v>
       </c>
       <c r="J3">
-        <v>290178.20000000001</v>
+        <v>241541.29999999999</v>
       </c>
       <c r="K3">
         <v>13225.9</v>
@@ -1545,7 +1511,7 @@
         <v>12385.800000000001</v>
       </c>
       <c r="O3">
-        <v>1067671.7000007343</v>
+        <v>931755.30000073381</v>
       </c>
       <c r="P3">
         <v>461812.99999962619</v>
@@ -1554,13 +1520,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8229999.9999991106</v>
+        <v>8229999.9999999953</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
-      <c r="T3">
-        <v>8366493.4259991096</v>
+      <c r="T3" s="83" t="s">
+        <v>18</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -1660,13 +1626,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>485340.90000000002</v>
+        <v>436704</v>
       </c>
       <c r="I2">
-        <v>1201250.3</v>
+        <v>1218836.3</v>
       </c>
       <c r="J2">
-        <v>290178.20000000001</v>
+        <v>241541.29999999999</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -1681,7 +1647,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1151250.3</v>
+        <v>1168836.3</v>
       </c>
       <c r="P2">
         <v>402312.99999981298</v>
@@ -1710,13 +1676,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>45000</v>
+        <v>29506.000000000102</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>45000</v>
+        <v>29506.000000000102</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -1725,13 +1691,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>536289.89999999991</v>
+        <v>487652.99999999994</v>
       </c>
       <c r="I3">
-        <v>926826.30000073416</v>
+        <v>1353836.2999999064</v>
       </c>
       <c r="J3">
-        <v>290178.20000000001</v>
+        <v>241541.29999999999</v>
       </c>
       <c r="K3">
         <v>13225.9</v>
@@ -1746,7 +1712,7 @@
         <v>12385.800000000001</v>
       </c>
       <c r="O3">
-        <v>876826.30000073405</v>
+        <v>1303836.2999999064</v>
       </c>
       <c r="P3">
         <v>461812.99999962619</v>
@@ -1755,13 +1721,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8542845.9828952551</v>
+        <v>8229999.9999999953</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
-      <c r="T3">
-        <v>8717435.2128952537</v>
+      <c r="T3" s="90" t="s">
+        <v>18</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -1861,13 +1827,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>485340.90000000002</v>
+        <v>436704</v>
       </c>
       <c r="I2">
-        <v>1201250.3</v>
+        <v>1218836.3</v>
       </c>
       <c r="J2">
-        <v>290178.20000000001</v>
+        <v>241541.29999999999</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -1882,7 +1848,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1151250.3</v>
+        <v>1168836.3</v>
       </c>
       <c r="P2">
         <v>402312.99999981298</v>
@@ -1911,13 +1877,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>45000</v>
+        <v>29506.000000000102</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>45000</v>
+        <v>29506.000000000102</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -1926,13 +1892,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>536289.89999999991</v>
+        <v>487652.99999999994</v>
       </c>
       <c r="I3">
-        <v>926826.30000073416</v>
+        <v>960324.30000073428</v>
       </c>
       <c r="J3">
-        <v>290178.20000000001</v>
+        <v>241541.29999999999</v>
       </c>
       <c r="K3">
         <v>13225.9</v>
@@ -1947,7 +1913,7 @@
         <v>12385.800000000001</v>
       </c>
       <c r="O3">
-        <v>876826.30000073405</v>
+        <v>910324.30000073416</v>
       </c>
       <c r="P3">
         <v>461812.99999962619</v>
@@ -1956,13 +1922,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8229999.9999991106</v>
+        <v>8999999.9999775551</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
-      <c r="T3">
-        <v>8469478.9159991127</v>
+      <c r="T3" s="97" t="s">
+        <v>18</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -2062,13 +2028,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>485340.90000000002</v>
+        <v>436704</v>
       </c>
       <c r="I2">
-        <v>1201250.3</v>
+        <v>1218836.3</v>
       </c>
       <c r="J2">
-        <v>290178.20000000001</v>
+        <v>241541.29999999999</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -2083,7 +2049,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1151250.3</v>
+        <v>1168836.3</v>
       </c>
       <c r="P2">
         <v>402312.99999981298</v>
@@ -2112,13 +2078,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>45000</v>
+        <v>29506.000000000102</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>45000</v>
+        <v>29506.000000000102</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -2127,13 +2093,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>536289.89999999991</v>
+        <v>487652.99999999994</v>
       </c>
       <c r="I3">
-        <v>1336250.2999999064</v>
+        <v>1488836.2999998129</v>
       </c>
       <c r="J3">
-        <v>290178.20000000001</v>
+        <v>241541.29999999999</v>
       </c>
       <c r="K3">
         <v>13225.9</v>
@@ -2148,7 +2114,7 @@
         <v>12385.800000000001</v>
       </c>
       <c r="O3">
-        <v>1286250.2999999064</v>
+        <v>1438836.2999998129</v>
       </c>
       <c r="P3">
         <v>461812.99999962619</v>
@@ -2157,13 +2123,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8229999.9999991106</v>
+        <v>8229999.9999999953</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
-      <c r="T3">
-        <v>8639818.2239991091</v>
+      <c r="T3" s="104" t="s">
+        <v>18</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -2263,13 +2229,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>485340.90000000002</v>
+        <v>436704</v>
       </c>
       <c r="I2">
-        <v>1201250.3</v>
+        <v>1218836.3</v>
       </c>
       <c r="J2">
-        <v>290178.20000000001</v>
+        <v>241541.29999999999</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -2284,7 +2250,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1151250.3</v>
+        <v>1168836.3</v>
       </c>
       <c r="P2">
         <v>402312.99999981298</v>
@@ -2313,13 +2279,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>45000</v>
+        <v>29506.000000000102</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>45000</v>
+        <v>29506.000000000102</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -2328,13 +2294,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>536289.89999999991</v>
+        <v>487652.99999999994</v>
       </c>
       <c r="I3">
-        <v>906323.60000073502</v>
+        <v>1488836.2999998129</v>
       </c>
       <c r="J3">
-        <v>290178.20000000001</v>
+        <v>241541.29999999999</v>
       </c>
       <c r="K3">
         <v>13225.9</v>
@@ -2349,7 +2315,7 @@
         <v>12385.800000000001</v>
       </c>
       <c r="O3">
-        <v>856323.60000073502</v>
+        <v>1438836.2999998129</v>
       </c>
       <c r="P3">
         <v>461812.99999962619</v>
@@ -2358,13 +2324,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8229999.9999991106</v>
+        <v>8999999.9999775551</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
-      <c r="T3">
-        <v>8362878.8059991114</v>
+      <c r="T3" s="111" t="s">
+        <v>18</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -2464,13 +2430,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>485340.90000000002</v>
+        <v>436704</v>
       </c>
       <c r="I2">
-        <v>1201250.3</v>
+        <v>1218836.3</v>
       </c>
       <c r="J2">
-        <v>290178.20000000001</v>
+        <v>241541.29999999999</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -2485,7 +2451,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1151250.3</v>
+        <v>1168836.3</v>
       </c>
       <c r="P2">
         <v>402312.99999981298</v>
@@ -2514,13 +2480,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>45000</v>
+        <v>29506.000000000102</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>45000</v>
+        <v>29506.000000000102</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -2529,13 +2495,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>536289.89999999991</v>
+        <v>487652.99999999994</v>
       </c>
       <c r="I3">
-        <v>1471250.2999998131</v>
+        <v>1488836.2999998129</v>
       </c>
       <c r="J3">
-        <v>290178.20000000001</v>
+        <v>241541.29999999999</v>
       </c>
       <c r="K3">
         <v>13225.9</v>
@@ -2550,7 +2516,7 @@
         <v>12385.800000000001</v>
       </c>
       <c r="O3">
-        <v>1421250.2999998129</v>
+        <v>1438836.2999998129</v>
       </c>
       <c r="P3">
         <v>461812.99999962619</v>
@@ -2559,13 +2525,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8229999.9999991106</v>
+        <v>8999999.9999775551</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
-      <c r="T3">
-        <v>8512420.3039991111</v>
+      <c r="T3" s="118" t="s">
+        <v>18</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -2665,13 +2631,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>485340.90000000002</v>
+        <v>436704</v>
       </c>
       <c r="I2">
-        <v>1201250.3</v>
+        <v>1218836.3</v>
       </c>
       <c r="J2">
-        <v>290178.20000000001</v>
+        <v>241541.29999999999</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -2686,7 +2652,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1151250.3</v>
+        <v>1168836.3</v>
       </c>
       <c r="P2">
         <v>402312.99999981298</v>
@@ -2715,13 +2681,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>45000</v>
+        <v>29506.000000000102</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>45000</v>
+        <v>29506.000000000102</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -2730,13 +2696,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>536289.89999999991</v>
+        <v>487652.99999999994</v>
       </c>
       <c r="I3">
-        <v>1471250.2999998131</v>
+        <v>1488836.2999998129</v>
       </c>
       <c r="J3">
-        <v>290178.20000000001</v>
+        <v>241541.29999999999</v>
       </c>
       <c r="K3">
         <v>13225.9</v>
@@ -2751,7 +2717,7 @@
         <v>12385.800000000001</v>
       </c>
       <c r="O3">
-        <v>1421250.2999998129</v>
+        <v>1438836.2999998129</v>
       </c>
       <c r="P3">
         <v>461812.99999962619</v>
@@ -2760,13 +2726,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8999999.9999775533</v>
+        <v>8229999.9999999953</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
-      <c r="T3">
-        <v>9128518.731977554</v>
+      <c r="T3" s="125" t="s">
+        <v>18</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -2866,13 +2832,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>485340.90000000002</v>
+        <v>436704</v>
       </c>
       <c r="I2">
-        <v>1201250.3</v>
+        <v>1218836.3</v>
       </c>
       <c r="J2">
-        <v>290178.20000000001</v>
+        <v>241541.29999999999</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -2887,7 +2853,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1151250.3</v>
+        <v>1168836.3</v>
       </c>
       <c r="P2">
         <v>402312.99999981298</v>
@@ -2916,13 +2882,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>45000</v>
+        <v>29506.000000000102</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>45000</v>
+        <v>29506.000000000102</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -2931,13 +2897,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>536289.89999999991</v>
+        <v>487652.99999999994</v>
       </c>
       <c r="I3">
-        <v>1471250.2999998131</v>
+        <v>1488836.2999998129</v>
       </c>
       <c r="J3">
-        <v>290178.20000000001</v>
+        <v>241541.29999999999</v>
       </c>
       <c r="K3">
         <v>13225.9</v>
@@ -2952,7 +2918,7 @@
         <v>12385.800000000001</v>
       </c>
       <c r="O3">
-        <v>1421250.2999998129</v>
+        <v>1438836.2999998129</v>
       </c>
       <c r="P3">
         <v>461812.99999962619</v>
@@ -2961,13 +2927,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8999999.9999775533</v>
+        <v>8229999.9999999953</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
-      <c r="T3">
-        <v>9061671.6859775521</v>
+      <c r="T3" s="132" t="s">
+        <v>18</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -3067,13 +3033,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>485340.90000000002</v>
+        <v>436704</v>
       </c>
       <c r="I2">
-        <v>1201250.3</v>
+        <v>1218836.3</v>
       </c>
       <c r="J2">
-        <v>290178.20000000001</v>
+        <v>241541.29999999999</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -3088,7 +3054,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1151250.3</v>
+        <v>1168836.3</v>
       </c>
       <c r="P2">
         <v>402312.99999981298</v>
@@ -3117,13 +3083,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>45000</v>
+        <v>29506.000000000102</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>45000</v>
+        <v>29506.000000000102</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -3132,13 +3098,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>536289.89999999991</v>
+        <v>487652.99999999994</v>
       </c>
       <c r="I3">
-        <v>1313229.2</v>
+        <v>1488836.2999998129</v>
       </c>
       <c r="J3">
-        <v>290178.20000000001</v>
+        <v>241541.29999999999</v>
       </c>
       <c r="K3">
         <v>13225.9</v>
@@ -3153,7 +3119,7 @@
         <v>12385.800000000001</v>
       </c>
       <c r="O3">
-        <v>1263229.2</v>
+        <v>1438836.2999998129</v>
       </c>
       <c r="P3">
         <v>461812.99999962619</v>
@@ -3162,13 +3128,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8229999.9999991106</v>
+        <v>8229999.9999999953</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
-      <c r="T3">
-        <v>8417587.9999991078</v>
+      <c r="T3" s="13" t="s">
+        <v>18</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -3268,13 +3234,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>485340.90000000002</v>
+        <v>436704</v>
       </c>
       <c r="I2">
-        <v>1201250.3</v>
+        <v>1218836.3</v>
       </c>
       <c r="J2">
-        <v>290178.20000000001</v>
+        <v>241541.29999999999</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -3289,7 +3255,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1151250.3</v>
+        <v>1168836.3</v>
       </c>
       <c r="P2">
         <v>402312.99999981298</v>
@@ -3318,13 +3284,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>45000</v>
+        <v>29506.000000000102</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>45000</v>
+        <v>29506.000000000102</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -3333,13 +3299,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>536289.89999999991</v>
+        <v>487652.99999999994</v>
       </c>
       <c r="I3">
-        <v>1471250.2999998131</v>
+        <v>1353836.2999999064</v>
       </c>
       <c r="J3">
-        <v>290178.20000000001</v>
+        <v>241541.29999999999</v>
       </c>
       <c r="K3">
         <v>13225.9</v>
@@ -3354,7 +3320,7 @@
         <v>12385.800000000001</v>
       </c>
       <c r="O3">
-        <v>1421250.2999998129</v>
+        <v>1303836.2999999064</v>
       </c>
       <c r="P3">
         <v>461812.99999962619</v>
@@ -3363,13 +3329,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8229999.9999991106</v>
+        <v>8760961.6169850398</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
-      <c r="T3">
-        <v>8140372.5099991113</v>
+      <c r="T3" s="139" t="s">
+        <v>18</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -3469,13 +3435,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>485340.90000000002</v>
+        <v>436704</v>
       </c>
       <c r="I2">
-        <v>1201250.3</v>
+        <v>1218836.3</v>
       </c>
       <c r="J2">
-        <v>290178.20000000001</v>
+        <v>241541.29999999999</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -3490,7 +3456,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1151250.3</v>
+        <v>1168836.3</v>
       </c>
       <c r="P2">
         <v>402312.99999981298</v>
@@ -3519,13 +3485,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>45000</v>
+        <v>29506.000000000102</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>45000</v>
+        <v>29506.000000000102</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -3534,13 +3500,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>536289.89999999991</v>
+        <v>487652.99999999994</v>
       </c>
       <c r="I3">
-        <v>1471250.2999998131</v>
+        <v>1118836.2999997989</v>
       </c>
       <c r="J3">
-        <v>290178.20000000001</v>
+        <v>241541.29999999999</v>
       </c>
       <c r="K3">
         <v>13225.9</v>
@@ -3555,7 +3521,7 @@
         <v>12385.800000000001</v>
       </c>
       <c r="O3">
-        <v>1421250.2999998129</v>
+        <v>1068836.2999997989</v>
       </c>
       <c r="P3">
         <v>461812.99999962619</v>
@@ -3564,13 +3530,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8229999.9999991106</v>
+        <v>8229999.9999999953</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
-      <c r="T3">
-        <v>8433484.9599991105</v>
+      <c r="T3" s="146" t="s">
+        <v>18</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -3670,13 +3636,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>485340.90000000002</v>
+        <v>436704</v>
       </c>
       <c r="I2">
-        <v>1201250.3</v>
+        <v>1218836.3</v>
       </c>
       <c r="J2">
-        <v>290178.20000000001</v>
+        <v>241541.29999999999</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -3691,7 +3657,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1151250.3</v>
+        <v>1168836.3</v>
       </c>
       <c r="P2">
         <v>402312.99999981298</v>
@@ -3720,13 +3686,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>45000</v>
+        <v>29506.000000000102</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>45000</v>
+        <v>29506.000000000102</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -3735,13 +3701,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>536289.89999999991</v>
+        <v>487652.99999999994</v>
       </c>
       <c r="I3">
-        <v>1336250.2999999064</v>
+        <v>1118836.2999997989</v>
       </c>
       <c r="J3">
-        <v>290178.20000000001</v>
+        <v>241541.29999999999</v>
       </c>
       <c r="K3">
         <v>13225.9</v>
@@ -3756,7 +3722,7 @@
         <v>12385.800000000001</v>
       </c>
       <c r="O3">
-        <v>1286250.2999999064</v>
+        <v>1068836.2999997989</v>
       </c>
       <c r="P3">
         <v>461812.99999962619</v>
@@ -3765,13 +3731,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8229999.9999991106</v>
+        <v>8229999.9999999953</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
-      <c r="T3">
-        <v>8370628.0299991099</v>
+      <c r="T3" s="153" t="s">
+        <v>18</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -3871,13 +3837,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>485340.90000000002</v>
+        <v>436704</v>
       </c>
       <c r="I2">
-        <v>1201250.3</v>
+        <v>1218836.3</v>
       </c>
       <c r="J2">
-        <v>290178.20000000001</v>
+        <v>241541.29999999999</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -3892,7 +3858,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1151250.3</v>
+        <v>1168836.3</v>
       </c>
       <c r="P2">
         <v>402312.99999981298</v>
@@ -3921,13 +3887,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>45000</v>
+        <v>29506.000000000102</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>45000</v>
+        <v>29506.000000000102</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -3936,13 +3902,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>536289.89999999991</v>
+        <v>487652.99999999994</v>
       </c>
       <c r="I3">
-        <v>1101250.2999997991</v>
+        <v>1353836.2999999064</v>
       </c>
       <c r="J3">
-        <v>290178.20000000001</v>
+        <v>241541.29999999999</v>
       </c>
       <c r="K3">
         <v>13225.9</v>
@@ -3957,7 +3923,7 @@
         <v>12385.800000000001</v>
       </c>
       <c r="O3">
-        <v>1051250.2999997991</v>
+        <v>1303836.2999999064</v>
       </c>
       <c r="P3">
         <v>461812.99999962619</v>
@@ -3966,13 +3932,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8400992.5909666829</v>
+        <v>8229999.9999999953</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
-      <c r="T3">
-        <v>8506470.2709666844</v>
+      <c r="T3" s="160" t="s">
+        <v>18</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -4072,13 +4038,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>485340.90000000002</v>
+        <v>436704</v>
       </c>
       <c r="I2">
-        <v>1201250.3</v>
+        <v>1218836.3</v>
       </c>
       <c r="J2">
-        <v>290178.20000000001</v>
+        <v>241541.29999999999</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -4093,7 +4059,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1151250.3</v>
+        <v>1168836.3</v>
       </c>
       <c r="P2">
         <v>402312.99999981298</v>
@@ -4122,13 +4088,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>45000</v>
+        <v>29506.000000000102</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>45000</v>
+        <v>29506.000000000102</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -4137,13 +4103,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>536289.89999999991</v>
+        <v>487652.99999999994</v>
       </c>
       <c r="I3">
-        <v>1101250.2999997991</v>
+        <v>1218836.3</v>
       </c>
       <c r="J3">
-        <v>290178.20000000001</v>
+        <v>241541.29999999999</v>
       </c>
       <c r="K3">
         <v>13225.9</v>
@@ -4158,7 +4124,7 @@
         <v>12385.800000000001</v>
       </c>
       <c r="O3">
-        <v>1051250.2999997991</v>
+        <v>1168836.3</v>
       </c>
       <c r="P3">
         <v>461812.99999962619</v>
@@ -4167,13 +4133,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8229999.9999991106</v>
+        <v>8458314.289126141</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
-      <c r="T3">
-        <v>8338713.64999911</v>
+      <c r="T3" s="167" t="s">
+        <v>18</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -4273,13 +4239,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>485340.90000000002</v>
+        <v>436704</v>
       </c>
       <c r="I2">
-        <v>1201250.3</v>
+        <v>1218836.3</v>
       </c>
       <c r="J2">
-        <v>290178.20000000001</v>
+        <v>241541.29999999999</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -4294,7 +4260,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1151250.3</v>
+        <v>1168836.3</v>
       </c>
       <c r="P2">
         <v>402312.99999981298</v>
@@ -4323,13 +4289,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>45000</v>
+        <v>29506.000000000102</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>45000</v>
+        <v>29506.000000000102</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -4338,13 +4304,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>536289.89999999991</v>
+        <v>487652.99999999994</v>
       </c>
       <c r="I3">
-        <v>1336250.2999999064</v>
+        <v>1353836.2999999064</v>
       </c>
       <c r="J3">
-        <v>290178.20000000001</v>
+        <v>241541.29999999999</v>
       </c>
       <c r="K3">
         <v>13225.9</v>
@@ -4359,7 +4325,7 @@
         <v>12385.800000000001</v>
       </c>
       <c r="O3">
-        <v>1286250.2999999064</v>
+        <v>1303836.2999999064</v>
       </c>
       <c r="P3">
         <v>461812.99999962619</v>
@@ -4368,13 +4334,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8781161.2817281336</v>
+        <v>8229999.9999999953</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
-      <c r="T3">
-        <v>8912808.721728133</v>
+      <c r="T3" s="174" t="s">
+        <v>18</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -4474,13 +4440,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>485340.90000000002</v>
+        <v>436704</v>
       </c>
       <c r="I2">
-        <v>1201250.3</v>
+        <v>1218836.3</v>
       </c>
       <c r="J2">
-        <v>290178.20000000001</v>
+        <v>241541.29999999999</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -4495,7 +4461,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1151250.3</v>
+        <v>1168836.3</v>
       </c>
       <c r="P2">
         <v>402312.99999981298</v>
@@ -4524,13 +4490,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>45000</v>
+        <v>29506.000000000102</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>45000</v>
+        <v>29506.000000000102</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -4539,13 +4505,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>536289.89999999991</v>
+        <v>487652.99999999994</v>
       </c>
       <c r="I3">
-        <v>1201250.3</v>
+        <v>1488836.2999998129</v>
       </c>
       <c r="J3">
-        <v>290178.20000000001</v>
+        <v>241541.29999999999</v>
       </c>
       <c r="K3">
         <v>13225.9</v>
@@ -4560,7 +4526,7 @@
         <v>12385.800000000001</v>
       </c>
       <c r="O3">
-        <v>1151250.3</v>
+        <v>1438836.2999998129</v>
       </c>
       <c r="P3">
         <v>461812.99999962619</v>
@@ -4569,13 +4535,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8229999.9999991106</v>
+        <v>8999999.9999775551</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
-      <c r="T3">
-        <v>8334398.0899991114</v>
+      <c r="T3" s="181" t="s">
+        <v>18</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -4675,13 +4641,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>485340.90000000002</v>
+        <v>436704</v>
       </c>
       <c r="I2">
-        <v>1201250.3</v>
+        <v>1218836.3</v>
       </c>
       <c r="J2">
-        <v>290178.20000000001</v>
+        <v>241541.29999999999</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -4696,7 +4662,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1151250.3</v>
+        <v>1168836.3</v>
       </c>
       <c r="P2">
         <v>402312.99999981298</v>
@@ -4725,13 +4691,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>45000</v>
+        <v>29506.000000000102</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>45000</v>
+        <v>29506.000000000102</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -4740,13 +4706,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>536289.89999999991</v>
+        <v>487652.99999999994</v>
       </c>
       <c r="I3">
-        <v>1336250.2999999064</v>
+        <v>1118836.2999997989</v>
       </c>
       <c r="J3">
-        <v>290178.20000000001</v>
+        <v>241541.29999999999</v>
       </c>
       <c r="K3">
         <v>13225.9</v>
@@ -4761,7 +4727,7 @@
         <v>12385.800000000001</v>
       </c>
       <c r="O3">
-        <v>1286250.2999999064</v>
+        <v>1068836.2999997989</v>
       </c>
       <c r="P3">
         <v>461812.99999962619</v>
@@ -4770,13 +4736,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8229999.9999991106</v>
+        <v>8646414.1810467541</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
-      <c r="T3">
-        <v>8359167.7799991118</v>
+      <c r="T3" s="188" t="s">
+        <v>18</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -4876,13 +4842,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>485340.90000000002</v>
+        <v>436704</v>
       </c>
       <c r="I2">
-        <v>1201250.3</v>
+        <v>1218836.3</v>
       </c>
       <c r="J2">
-        <v>290178.20000000001</v>
+        <v>241541.29999999999</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -4897,7 +4863,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1151250.3</v>
+        <v>1168836.3</v>
       </c>
       <c r="P2">
         <v>402312.99999981298</v>
@@ -4926,13 +4892,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>45000</v>
+        <v>29506.000000000102</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>45000</v>
+        <v>29506.000000000102</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -4941,13 +4907,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>536289.89999999991</v>
+        <v>487652.99999999994</v>
       </c>
       <c r="I3">
-        <v>1471250.2999998131</v>
+        <v>981755.30000073381</v>
       </c>
       <c r="J3">
-        <v>290178.20000000001</v>
+        <v>241541.29999999999</v>
       </c>
       <c r="K3">
         <v>13225.9</v>
@@ -4962,7 +4928,7 @@
         <v>12385.800000000001</v>
       </c>
       <c r="O3">
-        <v>1421250.2999998129</v>
+        <v>931755.30000073381</v>
       </c>
       <c r="P3">
         <v>461812.99999962619</v>
@@ -4971,13 +4937,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8726284.3734898679</v>
+        <v>8229999.9999999953</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
-      <c r="T3">
-        <v>8990190.6534898672</v>
+      <c r="T3" s="195" t="s">
+        <v>18</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -5077,13 +5043,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>485340.90000000002</v>
+        <v>436704</v>
       </c>
       <c r="I2">
-        <v>1201250.3</v>
+        <v>1218836.3</v>
       </c>
       <c r="J2">
-        <v>290178.20000000001</v>
+        <v>241541.29999999999</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -5098,7 +5064,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1151250.3</v>
+        <v>1168836.3</v>
       </c>
       <c r="P2">
         <v>402312.99999981298</v>
@@ -5127,13 +5093,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>45000</v>
+        <v>29506.000000000102</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>45000</v>
+        <v>29506.000000000102</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -5142,13 +5108,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>536289.89999999991</v>
+        <v>487652.99999999994</v>
       </c>
       <c r="I3">
-        <v>1101250.2999997991</v>
+        <v>1118836.2999997989</v>
       </c>
       <c r="J3">
-        <v>290178.20000000001</v>
+        <v>241541.29999999999</v>
       </c>
       <c r="K3">
         <v>13225.9</v>
@@ -5163,7 +5129,7 @@
         <v>12385.800000000001</v>
       </c>
       <c r="O3">
-        <v>1051250.2999997991</v>
+        <v>1068836.2999997989</v>
       </c>
       <c r="P3">
         <v>461812.99999962619</v>
@@ -5172,13 +5138,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8486272.647033304</v>
+        <v>8999999.9999775551</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
-      <c r="T3">
-        <v>8652420.5770333074</v>
+      <c r="T3" s="202" t="s">
+        <v>18</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -5278,13 +5244,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>485340.90000000002</v>
+        <v>436704</v>
       </c>
       <c r="I2">
-        <v>1201250.3</v>
+        <v>1218836.3</v>
       </c>
       <c r="J2">
-        <v>290178.20000000001</v>
+        <v>241541.29999999999</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -5299,7 +5265,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1151250.3</v>
+        <v>1168836.3</v>
       </c>
       <c r="P2">
         <v>402312.99999981298</v>
@@ -5328,13 +5294,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>45000</v>
+        <v>29506.000000000102</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>45000</v>
+        <v>29506.000000000102</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -5343,13 +5309,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>536289.89999999991</v>
+        <v>487652.99999999994</v>
       </c>
       <c r="I3">
-        <v>1313229.2</v>
+        <v>1488836.2999998129</v>
       </c>
       <c r="J3">
-        <v>290178.20000000001</v>
+        <v>241541.29999999999</v>
       </c>
       <c r="K3">
         <v>13225.9</v>
@@ -5364,7 +5330,7 @@
         <v>12385.800000000001</v>
       </c>
       <c r="O3">
-        <v>1263229.2</v>
+        <v>1438836.2999998129</v>
       </c>
       <c r="P3">
         <v>461812.99999962619</v>
@@ -5373,13 +5339,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8787576.5345334224</v>
+        <v>8229999.9999999953</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
-      <c r="T3">
-        <v>8945122.5345334224</v>
+      <c r="T3" s="20" t="s">
+        <v>18</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -5479,13 +5445,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>485340.90000000002</v>
+        <v>436704</v>
       </c>
       <c r="I2">
-        <v>1201250.3</v>
+        <v>1218836.3</v>
       </c>
       <c r="J2">
-        <v>290178.20000000001</v>
+        <v>241541.29999999999</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -5500,7 +5466,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1151250.3</v>
+        <v>1168836.3</v>
       </c>
       <c r="P2">
         <v>402312.99999981298</v>
@@ -5529,13 +5495,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>45000</v>
+        <v>29506.000000000102</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>45000</v>
+        <v>29506.000000000102</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -5544,13 +5510,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>536289.89999999991</v>
+        <v>487652.99999999994</v>
       </c>
       <c r="I3">
-        <v>926826.30000073416</v>
+        <v>1218836.3</v>
       </c>
       <c r="J3">
-        <v>290178.20000000001</v>
+        <v>241541.29999999999</v>
       </c>
       <c r="K3">
         <v>13225.9</v>
@@ -5565,7 +5531,7 @@
         <v>12385.800000000001</v>
       </c>
       <c r="O3">
-        <v>876826.30000073405</v>
+        <v>1168836.3</v>
       </c>
       <c r="P3">
         <v>461812.99999962619</v>
@@ -5574,13 +5540,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8999999.9999775533</v>
+        <v>8999999.9999775551</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
-      <c r="T3">
-        <v>9186027.3499775529</v>
+      <c r="T3" s="209" t="s">
+        <v>18</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -5680,13 +5646,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>485340.90000000002</v>
+        <v>436704</v>
       </c>
       <c r="I2">
-        <v>1201250.3</v>
+        <v>1218836.3</v>
       </c>
       <c r="J2">
-        <v>290178.20000000001</v>
+        <v>241541.29999999999</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -5701,7 +5667,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1151250.3</v>
+        <v>1168836.3</v>
       </c>
       <c r="P2">
         <v>402312.99999981298</v>
@@ -5730,13 +5696,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>45000</v>
+        <v>29506.000000000102</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>45000</v>
+        <v>29506.000000000102</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -5745,13 +5711,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>536289.89999999991</v>
+        <v>487652.99999999994</v>
       </c>
       <c r="I3">
-        <v>1101250.2999997991</v>
+        <v>1488836.2999998129</v>
       </c>
       <c r="J3">
-        <v>290178.20000000001</v>
+        <v>241541.29999999999</v>
       </c>
       <c r="K3">
         <v>13225.9</v>
@@ -5766,7 +5732,7 @@
         <v>12385.800000000001</v>
       </c>
       <c r="O3">
-        <v>1051250.2999997991</v>
+        <v>1438836.2999998129</v>
       </c>
       <c r="P3">
         <v>461812.99999962619</v>
@@ -5775,13 +5741,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8999999.9999775533</v>
+        <v>8229999.9999999953</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
-      <c r="T3">
-        <v>9160152.0699775536</v>
+      <c r="T3" s="216" t="s">
+        <v>18</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -5881,13 +5847,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>485340.90000000002</v>
+        <v>436704</v>
       </c>
       <c r="I2">
-        <v>1201250.3</v>
+        <v>1218836.3</v>
       </c>
       <c r="J2">
-        <v>290178.20000000001</v>
+        <v>241541.29999999999</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -5902,7 +5868,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1151250.3</v>
+        <v>1168836.3</v>
       </c>
       <c r="P2">
         <v>402312.99999981298</v>
@@ -5931,13 +5897,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>45000</v>
+        <v>29506.000000000102</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>45000</v>
+        <v>29506.000000000102</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -5946,13 +5912,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>536289.89999999991</v>
+        <v>487652.99999999994</v>
       </c>
       <c r="I3">
-        <v>1201250.3</v>
+        <v>1218836.3</v>
       </c>
       <c r="J3">
-        <v>290178.20000000001</v>
+        <v>241541.29999999999</v>
       </c>
       <c r="K3">
         <v>13225.9</v>
@@ -5967,7 +5933,7 @@
         <v>12385.800000000001</v>
       </c>
       <c r="O3">
-        <v>1151250.3</v>
+        <v>1168836.3</v>
       </c>
       <c r="P3">
         <v>461812.99999962619</v>
@@ -5976,13 +5942,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8528036.1567402072</v>
+        <v>8999999.9999775551</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
-      <c r="T3">
-        <v>8711985.8767402079</v>
+      <c r="T3" s="223" t="s">
+        <v>18</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -6082,13 +6048,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>485340.90000000002</v>
+        <v>436704</v>
       </c>
       <c r="I2">
-        <v>1201250.3</v>
+        <v>1218836.3</v>
       </c>
       <c r="J2">
-        <v>290178.20000000001</v>
+        <v>241541.29999999999</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -6103,7 +6069,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1151250.3</v>
+        <v>1168836.3</v>
       </c>
       <c r="P2">
         <v>402312.99999981298</v>
@@ -6132,13 +6098,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>45000</v>
+        <v>29506.000000000102</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>45000</v>
+        <v>29506.000000000102</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -6147,13 +6113,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>536289.89999999991</v>
+        <v>487652.99999999994</v>
       </c>
       <c r="I3">
-        <v>1471250.2999998131</v>
+        <v>1118836.2999997989</v>
       </c>
       <c r="J3">
-        <v>290178.20000000001</v>
+        <v>241541.29999999999</v>
       </c>
       <c r="K3">
         <v>13225.9</v>
@@ -6168,7 +6134,7 @@
         <v>12385.800000000001</v>
       </c>
       <c r="O3">
-        <v>1421250.2999998129</v>
+        <v>1068836.2999997989</v>
       </c>
       <c r="P3">
         <v>461812.99999962619</v>
@@ -6177,13 +6143,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8229999.9999991106</v>
+        <v>8229999.9999999953</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
-      <c r="T3">
-        <v>8442695.0099991094</v>
+      <c r="T3" s="230" t="s">
+        <v>18</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -6283,13 +6249,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>485340.90000000002</v>
+        <v>436704</v>
       </c>
       <c r="I2">
-        <v>1201250.3</v>
+        <v>1218836.3</v>
       </c>
       <c r="J2">
-        <v>290178.20000000001</v>
+        <v>241541.29999999999</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -6304,7 +6270,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1151250.3</v>
+        <v>1168836.3</v>
       </c>
       <c r="P2">
         <v>402312.99999981298</v>
@@ -6333,13 +6299,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>45000</v>
+        <v>29506.000000000102</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>45000</v>
+        <v>29506.000000000102</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -6348,13 +6314,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>536289.89999999991</v>
+        <v>487652.99999999994</v>
       </c>
       <c r="I3">
-        <v>1201250.3</v>
+        <v>981755.30000073381</v>
       </c>
       <c r="J3">
-        <v>290178.20000000001</v>
+        <v>241541.29999999999</v>
       </c>
       <c r="K3">
         <v>13225.9</v>
@@ -6369,7 +6335,7 @@
         <v>12385.800000000001</v>
       </c>
       <c r="O3">
-        <v>1151250.3</v>
+        <v>931755.30000073381</v>
       </c>
       <c r="P3">
         <v>461812.99999962619</v>
@@ -6378,13 +6344,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8229999.9999991106</v>
+        <v>8229999.9999999953</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
-      <c r="T3">
-        <v>8291125.7399991108</v>
+      <c r="T3" s="237" t="s">
+        <v>18</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -6484,13 +6450,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>485340.90000000002</v>
+        <v>436704</v>
       </c>
       <c r="I2">
-        <v>1201250.3</v>
+        <v>1218836.3</v>
       </c>
       <c r="J2">
-        <v>290178.20000000001</v>
+        <v>241541.29999999999</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -6505,7 +6471,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1151250.3</v>
+        <v>1168836.3</v>
       </c>
       <c r="P2">
         <v>402312.99999981298</v>
@@ -6534,13 +6500,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>45000</v>
+        <v>29506.000000000102</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>45000</v>
+        <v>29506.000000000102</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -6549,13 +6515,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>536289.89999999991</v>
+        <v>487652.99999999994</v>
       </c>
       <c r="I3">
-        <v>1101250.2999997991</v>
+        <v>981755.30000073381</v>
       </c>
       <c r="J3">
-        <v>290178.20000000001</v>
+        <v>241541.29999999999</v>
       </c>
       <c r="K3">
         <v>13225.9</v>
@@ -6570,7 +6536,7 @@
         <v>12385.800000000001</v>
       </c>
       <c r="O3">
-        <v>1051250.2999997991</v>
+        <v>931755.30000073381</v>
       </c>
       <c r="P3">
         <v>461812.99999962619</v>
@@ -6579,13 +6545,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8229999.9999991106</v>
+        <v>8470004.4250868037</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
-      <c r="T3">
-        <v>8261744.7299991101</v>
+      <c r="T3" s="244" t="s">
+        <v>18</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -6685,13 +6651,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>485340.90000000002</v>
+        <v>436704</v>
       </c>
       <c r="I2">
-        <v>1201250.3</v>
+        <v>1218836.3</v>
       </c>
       <c r="J2">
-        <v>290178.20000000001</v>
+        <v>241541.29999999999</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -6706,7 +6672,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1151250.3</v>
+        <v>1168836.3</v>
       </c>
       <c r="P2">
         <v>402312.99999981298</v>
@@ -6735,13 +6701,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>45000</v>
+        <v>29506.000000000102</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>45000</v>
+        <v>29506.000000000102</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -6750,13 +6716,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>536289.89999999991</v>
+        <v>487652.99999999994</v>
       </c>
       <c r="I3">
-        <v>926826.30000073416</v>
+        <v>1171607.3000007339</v>
       </c>
       <c r="J3">
-        <v>290178.20000000001</v>
+        <v>241541.29999999999</v>
       </c>
       <c r="K3">
         <v>13225.9</v>
@@ -6771,7 +6737,7 @@
         <v>12385.800000000001</v>
       </c>
       <c r="O3">
-        <v>876826.30000073405</v>
+        <v>1121607.3000007339</v>
       </c>
       <c r="P3">
         <v>461812.99999962619</v>
@@ -6780,415 +6746,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8999999.9999775533</v>
+        <v>8229999.9999999953</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
-      <c r="T3">
-        <v>9088058.5399775542</v>
-      </c>
-      <c r="U3">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:xdr="http://purl.oclc.org/ooxml/drawingml/spreadsheetDrawing">
-  <dimension ref="A1:U3"/>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="B1" s="259" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="259" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="259" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="259" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="259" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="259" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="259" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="259" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="259" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="259" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="259" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="259" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="259" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="259" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" s="259" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="259" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" s="259" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" s="259" t="s">
-        <v>17</v>
-      </c>
-      <c r="T1" s="259" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" s="259" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="257">
-        <v>43831</v>
-      </c>
-      <c r="B2">
-        <v>7</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>485340.90000000002</v>
-      </c>
-      <c r="I2">
-        <v>1201250.3</v>
-      </c>
-      <c r="J2">
-        <v>290178.20000000001</v>
-      </c>
-      <c r="K2">
-        <v>9009.3999999999996</v>
-      </c>
-      <c r="L2">
-        <v>180000</v>
-      </c>
-      <c r="M2">
-        <v>50000</v>
-      </c>
-      <c r="N2">
-        <v>6153.3000000000002</v>
-      </c>
-      <c r="O2">
-        <v>1151250.3</v>
-      </c>
-      <c r="P2">
-        <v>402312.99999981298</v>
-      </c>
-      <c r="Q2">
-        <v>0</v>
-      </c>
-      <c r="R2">
-        <v>8230092.9884342412</v>
-      </c>
-      <c r="S2" s="258" t="s">
-        <v>18</v>
-      </c>
-      <c r="T2" s="258" t="s">
-        <v>18</v>
-      </c>
-      <c r="U2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="257">
-        <v>44197</v>
-      </c>
-      <c r="B3">
-        <v>7</v>
-      </c>
-      <c r="C3">
-        <v>45000</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>45000</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>7999.9999999998645</v>
-      </c>
-      <c r="H3">
-        <v>536289.89999999991</v>
-      </c>
-      <c r="I3">
-        <v>926826.30000073416</v>
-      </c>
-      <c r="J3">
-        <v>290178.20000000001</v>
-      </c>
-      <c r="K3">
-        <v>13225.9</v>
-      </c>
-      <c r="L3">
-        <v>220499.99999999997</v>
-      </c>
-      <c r="M3">
-        <v>50000</v>
-      </c>
-      <c r="N3">
-        <v>12385.800000000001</v>
-      </c>
-      <c r="O3">
-        <v>876826.30000073405</v>
-      </c>
-      <c r="P3">
-        <v>461812.99999962619</v>
-      </c>
-      <c r="Q3">
-        <v>0</v>
-      </c>
-      <c r="R3">
-        <v>8229999.9999991106</v>
-      </c>
-      <c r="S3">
-        <v>1</v>
-      </c>
-      <c r="T3">
-        <v>8365931.8499991121</v>
-      </c>
-      <c r="U3">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:xdr="http://purl.oclc.org/ooxml/drawingml/spreadsheetDrawing">
-  <dimension ref="A1:U3"/>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="B1" s="266" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="266" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="266" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="266" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="266" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="266" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="266" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="266" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="266" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="266" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="266" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="266" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="266" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="266" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" s="266" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="266" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" s="266" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" s="266" t="s">
-        <v>17</v>
-      </c>
-      <c r="T1" s="266" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" s="266" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="264">
-        <v>43831</v>
-      </c>
-      <c r="B2">
-        <v>7</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>485340.90000000002</v>
-      </c>
-      <c r="I2">
-        <v>1201250.3</v>
-      </c>
-      <c r="J2">
-        <v>290178.20000000001</v>
-      </c>
-      <c r="K2">
-        <v>9009.3999999999996</v>
-      </c>
-      <c r="L2">
-        <v>180000</v>
-      </c>
-      <c r="M2">
-        <v>50000</v>
-      </c>
-      <c r="N2">
-        <v>6153.3000000000002</v>
-      </c>
-      <c r="O2">
-        <v>1151250.3</v>
-      </c>
-      <c r="P2">
-        <v>402312.99999981298</v>
-      </c>
-      <c r="Q2">
-        <v>0</v>
-      </c>
-      <c r="R2">
-        <v>8230092.9884342412</v>
-      </c>
-      <c r="S2" s="265" t="s">
-        <v>18</v>
-      </c>
-      <c r="T2" s="265" t="s">
-        <v>18</v>
-      </c>
-      <c r="U2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="264">
-        <v>44197</v>
-      </c>
-      <c r="B3">
-        <v>7</v>
-      </c>
-      <c r="C3">
-        <v>45000</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>45000</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>7999.9999999998645</v>
-      </c>
-      <c r="H3">
-        <v>536289.89999999991</v>
-      </c>
-      <c r="I3">
-        <v>1117671.7000007343</v>
-      </c>
-      <c r="J3">
-        <v>290178.20000000001</v>
-      </c>
-      <c r="K3">
-        <v>13225.9</v>
-      </c>
-      <c r="L3">
-        <v>220499.99999999997</v>
-      </c>
-      <c r="M3">
-        <v>50000</v>
-      </c>
-      <c r="N3">
-        <v>12385.800000000001</v>
-      </c>
-      <c r="O3">
-        <v>1067671.7000007343</v>
-      </c>
-      <c r="P3">
-        <v>461812.99999962619</v>
-      </c>
-      <c r="Q3">
-        <v>0</v>
-      </c>
-      <c r="R3">
-        <v>8229999.9999991106</v>
-      </c>
-      <c r="S3">
-        <v>1</v>
-      </c>
-      <c r="T3">
-        <v>8340981.0259991111</v>
+      <c r="T3" s="251" t="s">
+        <v>18</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -7288,13 +6852,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>485340.90000000002</v>
+        <v>436704</v>
       </c>
       <c r="I2">
-        <v>1201250.3</v>
+        <v>1218836.3</v>
       </c>
       <c r="J2">
-        <v>290178.20000000001</v>
+        <v>241541.29999999999</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -7309,7 +6873,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1151250.3</v>
+        <v>1168836.3</v>
       </c>
       <c r="P2">
         <v>402312.99999981298</v>
@@ -7338,13 +6902,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>45000</v>
+        <v>29506.000000000102</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>45000</v>
+        <v>29506.000000000102</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -7353,13 +6917,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>536289.89999999991</v>
+        <v>487652.99999999994</v>
       </c>
       <c r="I3">
-        <v>1471250.2999998131</v>
+        <v>1488836.2999998129</v>
       </c>
       <c r="J3">
-        <v>290178.20000000001</v>
+        <v>241541.29999999999</v>
       </c>
       <c r="K3">
         <v>13225.9</v>
@@ -7374,7 +6938,7 @@
         <v>12385.800000000001</v>
       </c>
       <c r="O3">
-        <v>1421250.2999998129</v>
+        <v>1438836.2999998129</v>
       </c>
       <c r="P3">
         <v>461812.99999962619</v>
@@ -7383,13 +6947,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8229999.9999991106</v>
+        <v>8229999.9999999953</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
-      <c r="T3">
-        <v>8440604.3459991124</v>
+      <c r="T3" s="27" t="s">
+        <v>18</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -7489,13 +7053,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>485340.90000000002</v>
+        <v>436704</v>
       </c>
       <c r="I2">
-        <v>1201250.3</v>
+        <v>1218836.3</v>
       </c>
       <c r="J2">
-        <v>290178.20000000001</v>
+        <v>241541.29999999999</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -7510,7 +7074,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1151250.3</v>
+        <v>1168836.3</v>
       </c>
       <c r="P2">
         <v>402312.99999981298</v>
@@ -7539,13 +7103,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>45000</v>
+        <v>29506.000000000102</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>45000</v>
+        <v>29506.000000000102</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -7554,13 +7118,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>536289.89999999991</v>
+        <v>487652.99999999994</v>
       </c>
       <c r="I3">
-        <v>1471250.2999998131</v>
+        <v>1118836.2999997989</v>
       </c>
       <c r="J3">
-        <v>290178.20000000001</v>
+        <v>241541.29999999999</v>
       </c>
       <c r="K3">
         <v>13225.9</v>
@@ -7575,7 +7139,7 @@
         <v>12385.800000000001</v>
       </c>
       <c r="O3">
-        <v>1421250.2999998129</v>
+        <v>1068836.2999997989</v>
       </c>
       <c r="P3">
         <v>461812.99999962619</v>
@@ -7584,13 +7148,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8229999.9999991106</v>
+        <v>8229999.9999999953</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
-      <c r="T3">
-        <v>8503849.8819991108</v>
+      <c r="T3" s="34" t="s">
+        <v>18</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -7690,13 +7254,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>485340.90000000002</v>
+        <v>436704</v>
       </c>
       <c r="I2">
-        <v>1201250.3</v>
+        <v>1218836.3</v>
       </c>
       <c r="J2">
-        <v>290178.20000000001</v>
+        <v>241541.29999999999</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -7711,7 +7275,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1151250.3</v>
+        <v>1168836.3</v>
       </c>
       <c r="P2">
         <v>402312.99999981298</v>
@@ -7740,13 +7304,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>45000</v>
+        <v>29506.000000000102</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>45000</v>
+        <v>29506.000000000102</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -7755,13 +7319,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>536289.89999999991</v>
+        <v>487652.99999999994</v>
       </c>
       <c r="I3">
-        <v>1471250.2999998131</v>
+        <v>1488836.2999998129</v>
       </c>
       <c r="J3">
-        <v>290178.20000000001</v>
+        <v>241541.29999999999</v>
       </c>
       <c r="K3">
         <v>13225.9</v>
@@ -7776,7 +7340,7 @@
         <v>12385.800000000001</v>
       </c>
       <c r="O3">
-        <v>1421250.2999998129</v>
+        <v>1438836.2999998129</v>
       </c>
       <c r="P3">
         <v>461812.99999962619</v>
@@ -7785,13 +7349,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8229999.9999991106</v>
+        <v>8999999.9999775551</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
-      <c r="T3">
-        <v>8521307.2019991111</v>
+      <c r="T3" s="41" t="s">
+        <v>18</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -7891,13 +7455,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>485340.90000000002</v>
+        <v>436704</v>
       </c>
       <c r="I2">
-        <v>1201250.3</v>
+        <v>1218836.3</v>
       </c>
       <c r="J2">
-        <v>290178.20000000001</v>
+        <v>241541.29999999999</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -7912,7 +7476,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1151250.3</v>
+        <v>1168836.3</v>
       </c>
       <c r="P2">
         <v>402312.99999981298</v>
@@ -7941,13 +7505,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>45000</v>
+        <v>29506.000000000102</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>45000</v>
+        <v>29506.000000000102</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -7956,13 +7520,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>536289.89999999991</v>
+        <v>487652.99999999994</v>
       </c>
       <c r="I3">
-        <v>1101250.2999997991</v>
+        <v>1118836.2999997989</v>
       </c>
       <c r="J3">
-        <v>290178.20000000001</v>
+        <v>241541.29999999999</v>
       </c>
       <c r="K3">
         <v>13225.9</v>
@@ -7977,7 +7541,7 @@
         <v>12385.800000000001</v>
       </c>
       <c r="O3">
-        <v>1051250.2999997991</v>
+        <v>1068836.2999997989</v>
       </c>
       <c r="P3">
         <v>461812.99999962619</v>
@@ -7986,13 +7550,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8229999.9999991106</v>
+        <v>8999999.9999775551</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
-      <c r="T3">
-        <v>8454903.3319991101</v>
+      <c r="T3" s="48" t="s">
+        <v>18</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -8092,13 +7656,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>485340.90000000002</v>
+        <v>436704</v>
       </c>
       <c r="I2">
-        <v>1201250.3</v>
+        <v>1218836.3</v>
       </c>
       <c r="J2">
-        <v>290178.20000000001</v>
+        <v>241541.29999999999</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -8113,7 +7677,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1151250.3</v>
+        <v>1168836.3</v>
       </c>
       <c r="P2">
         <v>402312.99999981298</v>
@@ -8142,13 +7706,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>45000</v>
+        <v>29506.000000000102</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>45000</v>
+        <v>29506.000000000102</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -8157,13 +7721,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>536289.89999999991</v>
+        <v>487652.99999999994</v>
       </c>
       <c r="I3">
-        <v>1471250.2999998131</v>
+        <v>981755.30000073381</v>
       </c>
       <c r="J3">
-        <v>290178.20000000001</v>
+        <v>241541.29999999999</v>
       </c>
       <c r="K3">
         <v>13225.9</v>
@@ -8178,7 +7742,7 @@
         <v>12385.800000000001</v>
       </c>
       <c r="O3">
-        <v>1421250.2999998129</v>
+        <v>931755.30000073381</v>
       </c>
       <c r="P3">
         <v>461812.99999962619</v>
@@ -8187,13 +7751,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8999999.9999775533</v>
+        <v>8229999.9999999953</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
-      <c r="T3">
-        <v>9148032.6279775519</v>
+      <c r="T3" s="55" t="s">
+        <v>18</v>
       </c>
       <c r="U3">
         <v>0</v>
@@ -8293,13 +7857,13 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>485340.90000000002</v>
+        <v>436704</v>
       </c>
       <c r="I2">
-        <v>1201250.3</v>
+        <v>1218836.3</v>
       </c>
       <c r="J2">
-        <v>290178.20000000001</v>
+        <v>241541.29999999999</v>
       </c>
       <c r="K2">
         <v>9009.3999999999996</v>
@@ -8314,7 +7878,7 @@
         <v>6153.3000000000002</v>
       </c>
       <c r="O2">
-        <v>1151250.3</v>
+        <v>1168836.3</v>
       </c>
       <c r="P2">
         <v>402312.99999981298</v>
@@ -8343,13 +7907,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>45000</v>
+        <v>29506.000000000102</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>45000</v>
+        <v>29506.000000000102</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -8358,13 +7922,13 @@
         <v>7999.9999999998645</v>
       </c>
       <c r="H3">
-        <v>536289.89999999991</v>
+        <v>487652.99999999994</v>
       </c>
       <c r="I3">
-        <v>1101250.2999997991</v>
+        <v>1118836.2999997989</v>
       </c>
       <c r="J3">
-        <v>290178.20000000001</v>
+        <v>241541.29999999999</v>
       </c>
       <c r="K3">
         <v>13225.9</v>
@@ -8379,7 +7943,7 @@
         <v>12385.800000000001</v>
       </c>
       <c r="O3">
-        <v>1051250.2999997991</v>
+        <v>1068836.2999997989</v>
       </c>
       <c r="P3">
         <v>461812.99999962619</v>
@@ -8388,13 +7952,13 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8229999.9999991106</v>
+        <v>8229999.9999999953</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
-      <c r="T3">
-        <v>8417857.7959991079</v>
+      <c r="T3" s="62" t="s">
+        <v>18</v>
       </c>
       <c r="U3">
         <v>0</v>

</xml_diff>

<commit_message>
December 2020 MTOM Run
Initialized model file with December 2020 information. Used .9010 model file and ruleset for MTOM run
Updated Output files
</commit_message>
<xml_diff>
--- a/Output Data/MtomToCrss_Annual.xlsx
+++ b/Output Data/MtomToCrss_Annual.xlsx
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:xdr="http://purl.oclc.org/ooxml/drawingml/spreadsheetDrawing" count="828" uniqueCount="21">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:xdr="http://purl.oclc.org/ooxml/drawingml/spreadsheetDrawing" count="972" uniqueCount="21">
   <si>
     <t>DCP BWSCP Flags.LB DCP BWSCP</t>
   </si>
@@ -135,7 +135,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="253">
+  <borders count="505">
     <border>
       <start/>
       <end/>
@@ -395,11 +395,263 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="253">
+  <cellXfs count="505">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -725,6 +977,330 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="252" xfId="0" applyNumberFormat="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="253" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="254" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="255" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="256" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="257" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="258" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="259" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="260" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="261" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="262" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="263" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="264" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="265" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="266" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="267" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="268" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="269" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="270" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="271" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="272" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="273" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="274" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="275" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="276" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="277" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="278" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="279" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="280" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="281" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="282" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="283" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="284" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="285" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="286" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="287" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="288" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="289" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="290" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="291" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="292" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="293" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="294" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="295" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="296" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="297" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="298" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="299" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="300" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="301" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="302" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="303" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="304" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="305" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="306" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="307" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="308" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="309" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="310" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="311" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="312" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="313" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="314" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="315" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="316" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="317" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="318" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="319" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="320" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="321" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="322" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="323" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="324" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="325" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="326" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="327" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="328" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="329" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="330" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="331" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="332" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="333" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="334" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="335" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="336" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="337" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="338" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="339" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="340" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="341" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="342" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="343" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="344" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="345" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="346" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="347" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="348" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="349" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="350" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="351" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="352" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="353" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="354" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="355" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="356" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="357" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="358" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="359" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="360" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="361" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="362" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="363" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="364" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="365" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="366" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="367" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="368" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="369" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="370" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="371" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="372" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="373" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="374" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="375" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="376" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="377" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="378" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="379" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="380" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="381" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="382" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="383" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="384" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="385" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="386" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="387" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="388" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="389" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="390" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="391" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="392" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="393" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="394" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="395" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="396" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="397" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="398" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="399" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="400" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="401" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="402" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="403" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="404" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="405" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="406" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="407" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="408" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="409" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="410" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="411" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="412" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="413" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="414" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="415" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="416" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="417" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="418" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="419" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="420" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="421" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="422" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="423" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="424" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="425" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="426" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="427" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="428" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="429" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="430" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="431" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="432" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="433" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="434" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="435" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="436" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="437" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="438" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="439" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="440" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="441" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="442" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="443" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="444" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="445" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="446" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="447" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="448" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="449" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="450" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="451" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="452" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="453" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="454" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="455" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="456" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="457" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="458" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="459" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="460" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="461" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="462" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="463" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="464" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="465" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="466" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="467" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="468" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="469" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="470" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="471" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="472" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="473" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="474" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="475" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="476" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="477" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="478" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="479" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="480" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="481" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="482" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="483" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="484" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="485" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="486" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="487" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="488" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="489" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="490" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="491" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="492" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="493" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="494" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="495" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="496" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="497" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="498" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="499" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="500" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="501" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="502" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="503" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="504" xfId="0" applyNumberFormat="true" applyAlignment="true">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -851,13 +1427,13 @@
       <c r="Q2">
         <v>0</v>
       </c>
-      <c r="R2">
-        <v>8230092.9884342412</v>
-      </c>
-      <c r="S2" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="T2" s="6" t="s">
+      <c r="R2" s="258" t="s">
+        <v>18</v>
+      </c>
+      <c r="S2" s="258" t="s">
+        <v>18</v>
+      </c>
+      <c r="T2" s="258" t="s">
         <v>18</v>
       </c>
       <c r="U2">
@@ -890,7 +1466,7 @@
         <v>523904.09999999992</v>
       </c>
       <c r="I3">
-        <v>1142769.4000000001</v>
+        <v>1251226.4000000001</v>
       </c>
       <c r="J3">
         <v>290178.20000000001</v>
@@ -908,7 +1484,7 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <v>1092769.3999999999</v>
+        <v>1201226.4000000001</v>
       </c>
       <c r="P3">
         <v>461812.99999962619</v>
@@ -922,7 +1498,7 @@
       <c r="S3">
         <v>1</v>
       </c>
-      <c r="T3" s="6" t="s">
+      <c r="T3" s="258" t="s">
         <v>18</v>
       </c>
       <c r="U3">
@@ -1052,13 +1628,13 @@
       <c r="Q2">
         <v>0</v>
       </c>
-      <c r="R2">
-        <v>8230092.9884342412</v>
-      </c>
-      <c r="S2" s="69" t="s">
-        <v>18</v>
-      </c>
-      <c r="T2" s="69" t="s">
+      <c r="R2" s="321" t="s">
+        <v>18</v>
+      </c>
+      <c r="S2" s="321" t="s">
+        <v>18</v>
+      </c>
+      <c r="T2" s="321" t="s">
         <v>18</v>
       </c>
       <c r="U2">
@@ -1123,7 +1699,7 @@
       <c r="S3">
         <v>1</v>
       </c>
-      <c r="T3" s="69" t="s">
+      <c r="T3" s="321" t="s">
         <v>18</v>
       </c>
       <c r="U3">
@@ -1253,13 +1829,13 @@
       <c r="Q2">
         <v>0</v>
       </c>
-      <c r="R2">
-        <v>8230092.9884342412</v>
-      </c>
-      <c r="S2" s="76" t="s">
-        <v>18</v>
-      </c>
-      <c r="T2" s="76" t="s">
+      <c r="R2" s="328" t="s">
+        <v>18</v>
+      </c>
+      <c r="S2" s="328" t="s">
+        <v>18</v>
+      </c>
+      <c r="T2" s="328" t="s">
         <v>18</v>
       </c>
       <c r="U2">
@@ -1324,7 +1900,7 @@
       <c r="S3">
         <v>1</v>
       </c>
-      <c r="T3" s="76" t="s">
+      <c r="T3" s="328" t="s">
         <v>18</v>
       </c>
       <c r="U3">
@@ -1454,13 +2030,13 @@
       <c r="Q2">
         <v>0</v>
       </c>
-      <c r="R2">
-        <v>8230092.9884342412</v>
-      </c>
-      <c r="S2" s="83" t="s">
-        <v>18</v>
-      </c>
-      <c r="T2" s="83" t="s">
+      <c r="R2" s="335" t="s">
+        <v>18</v>
+      </c>
+      <c r="S2" s="335" t="s">
+        <v>18</v>
+      </c>
+      <c r="T2" s="335" t="s">
         <v>18</v>
       </c>
       <c r="U2">
@@ -1525,7 +2101,7 @@
       <c r="S3">
         <v>1</v>
       </c>
-      <c r="T3" s="83" t="s">
+      <c r="T3" s="335" t="s">
         <v>18</v>
       </c>
       <c r="U3">
@@ -1655,13 +2231,13 @@
       <c r="Q2">
         <v>0</v>
       </c>
-      <c r="R2">
-        <v>8230092.9884342412</v>
-      </c>
-      <c r="S2" s="90" t="s">
-        <v>18</v>
-      </c>
-      <c r="T2" s="90" t="s">
+      <c r="R2" s="342" t="s">
+        <v>18</v>
+      </c>
+      <c r="S2" s="342" t="s">
+        <v>18</v>
+      </c>
+      <c r="T2" s="342" t="s">
         <v>18</v>
       </c>
       <c r="U2">
@@ -1726,7 +2302,7 @@
       <c r="S3">
         <v>1</v>
       </c>
-      <c r="T3" s="90" t="s">
+      <c r="T3" s="342" t="s">
         <v>18</v>
       </c>
       <c r="U3">
@@ -1856,13 +2432,13 @@
       <c r="Q2">
         <v>0</v>
       </c>
-      <c r="R2">
-        <v>8230092.9884342412</v>
-      </c>
-      <c r="S2" s="97" t="s">
-        <v>18</v>
-      </c>
-      <c r="T2" s="97" t="s">
+      <c r="R2" s="349" t="s">
+        <v>18</v>
+      </c>
+      <c r="S2" s="349" t="s">
+        <v>18</v>
+      </c>
+      <c r="T2" s="349" t="s">
         <v>18</v>
       </c>
       <c r="U2">
@@ -1927,7 +2503,7 @@
       <c r="S3">
         <v>1</v>
       </c>
-      <c r="T3" s="97" t="s">
+      <c r="T3" s="349" t="s">
         <v>18</v>
       </c>
       <c r="U3">
@@ -2057,13 +2633,13 @@
       <c r="Q2">
         <v>0</v>
       </c>
-      <c r="R2">
-        <v>8230092.9884342412</v>
-      </c>
-      <c r="S2" s="104" t="s">
-        <v>18</v>
-      </c>
-      <c r="T2" s="104" t="s">
+      <c r="R2" s="356" t="s">
+        <v>18</v>
+      </c>
+      <c r="S2" s="356" t="s">
+        <v>18</v>
+      </c>
+      <c r="T2" s="356" t="s">
         <v>18</v>
       </c>
       <c r="U2">
@@ -2128,7 +2704,7 @@
       <c r="S3">
         <v>1</v>
       </c>
-      <c r="T3" s="104" t="s">
+      <c r="T3" s="356" t="s">
         <v>18</v>
       </c>
       <c r="U3">
@@ -2258,13 +2834,13 @@
       <c r="Q2">
         <v>0</v>
       </c>
-      <c r="R2">
-        <v>8230092.9884342412</v>
-      </c>
-      <c r="S2" s="111" t="s">
-        <v>18</v>
-      </c>
-      <c r="T2" s="111" t="s">
+      <c r="R2" s="363" t="s">
+        <v>18</v>
+      </c>
+      <c r="S2" s="363" t="s">
+        <v>18</v>
+      </c>
+      <c r="T2" s="363" t="s">
         <v>18</v>
       </c>
       <c r="U2">
@@ -2329,7 +2905,7 @@
       <c r="S3">
         <v>1</v>
       </c>
-      <c r="T3" s="111" t="s">
+      <c r="T3" s="363" t="s">
         <v>18</v>
       </c>
       <c r="U3">
@@ -2459,13 +3035,13 @@
       <c r="Q2">
         <v>0</v>
       </c>
-      <c r="R2">
-        <v>8230092.9884342412</v>
-      </c>
-      <c r="S2" s="118" t="s">
-        <v>18</v>
-      </c>
-      <c r="T2" s="118" t="s">
+      <c r="R2" s="370" t="s">
+        <v>18</v>
+      </c>
+      <c r="S2" s="370" t="s">
+        <v>18</v>
+      </c>
+      <c r="T2" s="370" t="s">
         <v>18</v>
       </c>
       <c r="U2">
@@ -2525,12 +3101,12 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8880884.8170844074</v>
+        <v>8877608.6906365566</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
-      <c r="T3" s="118" t="s">
+      <c r="T3" s="370" t="s">
         <v>18</v>
       </c>
       <c r="U3">
@@ -2660,13 +3236,13 @@
       <c r="Q2">
         <v>0</v>
       </c>
-      <c r="R2">
-        <v>8230092.9884342412</v>
-      </c>
-      <c r="S2" s="125" t="s">
-        <v>18</v>
-      </c>
-      <c r="T2" s="125" t="s">
+      <c r="R2" s="377" t="s">
+        <v>18</v>
+      </c>
+      <c r="S2" s="377" t="s">
+        <v>18</v>
+      </c>
+      <c r="T2" s="377" t="s">
         <v>18</v>
       </c>
       <c r="U2">
@@ -2731,7 +3307,7 @@
       <c r="S3">
         <v>1</v>
       </c>
-      <c r="T3" s="125" t="s">
+      <c r="T3" s="377" t="s">
         <v>18</v>
       </c>
       <c r="U3">
@@ -2861,13 +3437,13 @@
       <c r="Q2">
         <v>0</v>
       </c>
-      <c r="R2">
-        <v>8230092.9884342412</v>
-      </c>
-      <c r="S2" s="132" t="s">
-        <v>18</v>
-      </c>
-      <c r="T2" s="132" t="s">
+      <c r="R2" s="384" t="s">
+        <v>18</v>
+      </c>
+      <c r="S2" s="384" t="s">
+        <v>18</v>
+      </c>
+      <c r="T2" s="384" t="s">
         <v>18</v>
       </c>
       <c r="U2">
@@ -2932,7 +3508,7 @@
       <c r="S3">
         <v>1</v>
       </c>
-      <c r="T3" s="132" t="s">
+      <c r="T3" s="384" t="s">
         <v>18</v>
       </c>
       <c r="U3">
@@ -3062,13 +3638,13 @@
       <c r="Q2">
         <v>0</v>
       </c>
-      <c r="R2">
-        <v>8230092.9884342412</v>
-      </c>
-      <c r="S2" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="T2" s="13" t="s">
+      <c r="R2" s="265" t="s">
+        <v>18</v>
+      </c>
+      <c r="S2" s="265" t="s">
+        <v>18</v>
+      </c>
+      <c r="T2" s="265" t="s">
         <v>18</v>
       </c>
       <c r="U2">
@@ -3133,7 +3709,7 @@
       <c r="S3">
         <v>1</v>
       </c>
-      <c r="T3" s="13" t="s">
+      <c r="T3" s="265" t="s">
         <v>18</v>
       </c>
       <c r="U3">
@@ -3263,13 +3839,13 @@
       <c r="Q2">
         <v>0</v>
       </c>
-      <c r="R2">
-        <v>8230092.9884342412</v>
-      </c>
-      <c r="S2" s="139" t="s">
-        <v>18</v>
-      </c>
-      <c r="T2" s="139" t="s">
+      <c r="R2" s="391" t="s">
+        <v>18</v>
+      </c>
+      <c r="S2" s="391" t="s">
+        <v>18</v>
+      </c>
+      <c r="T2" s="391" t="s">
         <v>18</v>
       </c>
       <c r="U2">
@@ -3329,12 +3905,12 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8794061.3615832161</v>
+        <v>8789886.9269561004</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
-      <c r="T3" s="139" t="s">
+      <c r="T3" s="391" t="s">
         <v>18</v>
       </c>
       <c r="U3">
@@ -3464,13 +4040,13 @@
       <c r="Q2">
         <v>0</v>
       </c>
-      <c r="R2">
-        <v>8230092.9884342412</v>
-      </c>
-      <c r="S2" s="146" t="s">
-        <v>18</v>
-      </c>
-      <c r="T2" s="146" t="s">
+      <c r="R2" s="398" t="s">
+        <v>18</v>
+      </c>
+      <c r="S2" s="398" t="s">
+        <v>18</v>
+      </c>
+      <c r="T2" s="398" t="s">
         <v>18</v>
       </c>
       <c r="U2">
@@ -3530,12 +4106,12 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8383303.9160785768</v>
+        <v>8379846.2227119338</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
-      <c r="T3" s="146" t="s">
+      <c r="T3" s="398" t="s">
         <v>18</v>
       </c>
       <c r="U3">
@@ -3665,13 +4241,13 @@
       <c r="Q2">
         <v>0</v>
       </c>
-      <c r="R2">
-        <v>8230092.9884342412</v>
-      </c>
-      <c r="S2" s="153" t="s">
-        <v>18</v>
-      </c>
-      <c r="T2" s="153" t="s">
+      <c r="R2" s="405" t="s">
+        <v>18</v>
+      </c>
+      <c r="S2" s="405" t="s">
+        <v>18</v>
+      </c>
+      <c r="T2" s="405" t="s">
         <v>18</v>
       </c>
       <c r="U2">
@@ -3736,7 +4312,7 @@
       <c r="S3">
         <v>1</v>
       </c>
-      <c r="T3" s="153" t="s">
+      <c r="T3" s="405" t="s">
         <v>18</v>
       </c>
       <c r="U3">
@@ -3866,13 +4442,13 @@
       <c r="Q2">
         <v>0</v>
       </c>
-      <c r="R2">
-        <v>8230092.9884342412</v>
-      </c>
-      <c r="S2" s="160" t="s">
-        <v>18</v>
-      </c>
-      <c r="T2" s="160" t="s">
+      <c r="R2" s="412" t="s">
+        <v>18</v>
+      </c>
+      <c r="S2" s="412" t="s">
+        <v>18</v>
+      </c>
+      <c r="T2" s="412" t="s">
         <v>18</v>
       </c>
       <c r="U2">
@@ -3937,7 +4513,7 @@
       <c r="S3">
         <v>1</v>
       </c>
-      <c r="T3" s="160" t="s">
+      <c r="T3" s="412" t="s">
         <v>18</v>
       </c>
       <c r="U3">
@@ -4067,13 +4643,13 @@
       <c r="Q2">
         <v>0</v>
       </c>
-      <c r="R2">
-        <v>8230092.9884342412</v>
-      </c>
-      <c r="S2" s="167" t="s">
-        <v>18</v>
-      </c>
-      <c r="T2" s="167" t="s">
+      <c r="R2" s="419" t="s">
+        <v>18</v>
+      </c>
+      <c r="S2" s="419" t="s">
+        <v>18</v>
+      </c>
+      <c r="T2" s="419" t="s">
         <v>18</v>
       </c>
       <c r="U2">
@@ -4138,7 +4714,7 @@
       <c r="S3">
         <v>1</v>
       </c>
-      <c r="T3" s="167" t="s">
+      <c r="T3" s="419" t="s">
         <v>18</v>
       </c>
       <c r="U3">
@@ -4268,13 +4844,13 @@
       <c r="Q2">
         <v>0</v>
       </c>
-      <c r="R2">
-        <v>8230092.9884342412</v>
-      </c>
-      <c r="S2" s="174" t="s">
-        <v>18</v>
-      </c>
-      <c r="T2" s="174" t="s">
+      <c r="R2" s="426" t="s">
+        <v>18</v>
+      </c>
+      <c r="S2" s="426" t="s">
+        <v>18</v>
+      </c>
+      <c r="T2" s="426" t="s">
         <v>18</v>
       </c>
       <c r="U2">
@@ -4339,7 +4915,7 @@
       <c r="S3">
         <v>1</v>
       </c>
-      <c r="T3" s="174" t="s">
+      <c r="T3" s="426" t="s">
         <v>18</v>
       </c>
       <c r="U3">
@@ -4469,13 +5045,13 @@
       <c r="Q2">
         <v>0</v>
       </c>
-      <c r="R2">
-        <v>8230092.9884342412</v>
-      </c>
-      <c r="S2" s="181" t="s">
-        <v>18</v>
-      </c>
-      <c r="T2" s="181" t="s">
+      <c r="R2" s="433" t="s">
+        <v>18</v>
+      </c>
+      <c r="S2" s="433" t="s">
+        <v>18</v>
+      </c>
+      <c r="T2" s="433" t="s">
         <v>18</v>
       </c>
       <c r="U2">
@@ -4535,12 +5111,12 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8982884.9955622014</v>
+        <v>8979483.5237538498</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
-      <c r="T3" s="181" t="s">
+      <c r="T3" s="433" t="s">
         <v>18</v>
       </c>
       <c r="U3">
@@ -4670,13 +5246,13 @@
       <c r="Q2">
         <v>0</v>
       </c>
-      <c r="R2">
-        <v>8230092.9884342412</v>
-      </c>
-      <c r="S2" s="188" t="s">
-        <v>18</v>
-      </c>
-      <c r="T2" s="188" t="s">
+      <c r="R2" s="440" t="s">
+        <v>18</v>
+      </c>
+      <c r="S2" s="440" t="s">
+        <v>18</v>
+      </c>
+      <c r="T2" s="440" t="s">
         <v>18</v>
       </c>
       <c r="U2">
@@ -4741,7 +5317,7 @@
       <c r="S3">
         <v>1</v>
       </c>
-      <c r="T3" s="188" t="s">
+      <c r="T3" s="440" t="s">
         <v>18</v>
       </c>
       <c r="U3">
@@ -4871,13 +5447,13 @@
       <c r="Q2">
         <v>0</v>
       </c>
-      <c r="R2">
-        <v>8230092.9884342412</v>
-      </c>
-      <c r="S2" s="195" t="s">
-        <v>18</v>
-      </c>
-      <c r="T2" s="195" t="s">
+      <c r="R2" s="447" t="s">
+        <v>18</v>
+      </c>
+      <c r="S2" s="447" t="s">
+        <v>18</v>
+      </c>
+      <c r="T2" s="447" t="s">
         <v>18</v>
       </c>
       <c r="U2">
@@ -4942,7 +5518,7 @@
       <c r="S3">
         <v>1</v>
       </c>
-      <c r="T3" s="195" t="s">
+      <c r="T3" s="447" t="s">
         <v>18</v>
       </c>
       <c r="U3">
@@ -5072,13 +5648,13 @@
       <c r="Q2">
         <v>0</v>
       </c>
-      <c r="R2">
-        <v>8230092.9884342412</v>
-      </c>
-      <c r="S2" s="202" t="s">
-        <v>18</v>
-      </c>
-      <c r="T2" s="202" t="s">
+      <c r="R2" s="454" t="s">
+        <v>18</v>
+      </c>
+      <c r="S2" s="454" t="s">
+        <v>18</v>
+      </c>
+      <c r="T2" s="454" t="s">
         <v>18</v>
       </c>
       <c r="U2">
@@ -5143,7 +5719,7 @@
       <c r="S3">
         <v>1</v>
       </c>
-      <c r="T3" s="202" t="s">
+      <c r="T3" s="454" t="s">
         <v>18</v>
       </c>
       <c r="U3">
@@ -5273,13 +5849,13 @@
       <c r="Q2">
         <v>0</v>
       </c>
-      <c r="R2">
-        <v>8230092.9884342412</v>
-      </c>
-      <c r="S2" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="T2" s="20" t="s">
+      <c r="R2" s="272" t="s">
+        <v>18</v>
+      </c>
+      <c r="S2" s="272" t="s">
+        <v>18</v>
+      </c>
+      <c r="T2" s="272" t="s">
         <v>18</v>
       </c>
       <c r="U2">
@@ -5344,7 +5920,7 @@
       <c r="S3">
         <v>1</v>
       </c>
-      <c r="T3" s="20" t="s">
+      <c r="T3" s="272" t="s">
         <v>18</v>
       </c>
       <c r="U3">
@@ -5474,13 +6050,13 @@
       <c r="Q2">
         <v>0</v>
       </c>
-      <c r="R2">
-        <v>8230092.9884342412</v>
-      </c>
-      <c r="S2" s="209" t="s">
-        <v>18</v>
-      </c>
-      <c r="T2" s="209" t="s">
+      <c r="R2" s="461" t="s">
+        <v>18</v>
+      </c>
+      <c r="S2" s="461" t="s">
+        <v>18</v>
+      </c>
+      <c r="T2" s="461" t="s">
         <v>18</v>
       </c>
       <c r="U2">
@@ -5545,7 +6121,7 @@
       <c r="S3">
         <v>1</v>
       </c>
-      <c r="T3" s="209" t="s">
+      <c r="T3" s="461" t="s">
         <v>18</v>
       </c>
       <c r="U3">
@@ -5675,13 +6251,13 @@
       <c r="Q2">
         <v>0</v>
       </c>
-      <c r="R2">
-        <v>8230092.9884342412</v>
-      </c>
-      <c r="S2" s="216" t="s">
-        <v>18</v>
-      </c>
-      <c r="T2" s="216" t="s">
+      <c r="R2" s="468" t="s">
+        <v>18</v>
+      </c>
+      <c r="S2" s="468" t="s">
+        <v>18</v>
+      </c>
+      <c r="T2" s="468" t="s">
         <v>18</v>
       </c>
       <c r="U2">
@@ -5746,7 +6322,7 @@
       <c r="S3">
         <v>1</v>
       </c>
-      <c r="T3" s="216" t="s">
+      <c r="T3" s="468" t="s">
         <v>18</v>
       </c>
       <c r="U3">
@@ -5876,13 +6452,13 @@
       <c r="Q2">
         <v>0</v>
       </c>
-      <c r="R2">
-        <v>8230092.9884342412</v>
-      </c>
-      <c r="S2" s="223" t="s">
-        <v>18</v>
-      </c>
-      <c r="T2" s="223" t="s">
+      <c r="R2" s="475" t="s">
+        <v>18</v>
+      </c>
+      <c r="S2" s="475" t="s">
+        <v>18</v>
+      </c>
+      <c r="T2" s="475" t="s">
         <v>18</v>
       </c>
       <c r="U2">
@@ -5947,7 +6523,7 @@
       <c r="S3">
         <v>1</v>
       </c>
-      <c r="T3" s="223" t="s">
+      <c r="T3" s="475" t="s">
         <v>18</v>
       </c>
       <c r="U3">
@@ -6077,13 +6653,13 @@
       <c r="Q2">
         <v>0</v>
       </c>
-      <c r="R2">
-        <v>8230092.9884342412</v>
-      </c>
-      <c r="S2" s="230" t="s">
-        <v>18</v>
-      </c>
-      <c r="T2" s="230" t="s">
+      <c r="R2" s="482" t="s">
+        <v>18</v>
+      </c>
+      <c r="S2" s="482" t="s">
+        <v>18</v>
+      </c>
+      <c r="T2" s="482" t="s">
         <v>18</v>
       </c>
       <c r="U2">
@@ -6148,7 +6724,7 @@
       <c r="S3">
         <v>1</v>
       </c>
-      <c r="T3" s="230" t="s">
+      <c r="T3" s="482" t="s">
         <v>18</v>
       </c>
       <c r="U3">
@@ -6278,13 +6854,13 @@
       <c r="Q2">
         <v>0</v>
       </c>
-      <c r="R2">
-        <v>8230092.9884342412</v>
-      </c>
-      <c r="S2" s="237" t="s">
-        <v>18</v>
-      </c>
-      <c r="T2" s="237" t="s">
+      <c r="R2" s="489" t="s">
+        <v>18</v>
+      </c>
+      <c r="S2" s="489" t="s">
+        <v>18</v>
+      </c>
+      <c r="T2" s="489" t="s">
         <v>18</v>
       </c>
       <c r="U2">
@@ -6349,7 +6925,7 @@
       <c r="S3">
         <v>1</v>
       </c>
-      <c r="T3" s="237" t="s">
+      <c r="T3" s="489" t="s">
         <v>18</v>
       </c>
       <c r="U3">
@@ -6479,13 +7055,13 @@
       <c r="Q2">
         <v>0</v>
       </c>
-      <c r="R2">
-        <v>8230092.9884342412</v>
-      </c>
-      <c r="S2" s="244" t="s">
-        <v>18</v>
-      </c>
-      <c r="T2" s="244" t="s">
+      <c r="R2" s="496" t="s">
+        <v>18</v>
+      </c>
+      <c r="S2" s="496" t="s">
+        <v>18</v>
+      </c>
+      <c r="T2" s="496" t="s">
         <v>18</v>
       </c>
       <c r="U2">
@@ -6550,7 +7126,7 @@
       <c r="S3">
         <v>1</v>
       </c>
-      <c r="T3" s="244" t="s">
+      <c r="T3" s="496" t="s">
         <v>18</v>
       </c>
       <c r="U3">
@@ -6680,13 +7256,13 @@
       <c r="Q2">
         <v>0</v>
       </c>
-      <c r="R2">
-        <v>8230092.9884342412</v>
-      </c>
-      <c r="S2" s="251" t="s">
-        <v>18</v>
-      </c>
-      <c r="T2" s="251" t="s">
+      <c r="R2" s="503" t="s">
+        <v>18</v>
+      </c>
+      <c r="S2" s="503" t="s">
+        <v>18</v>
+      </c>
+      <c r="T2" s="503" t="s">
         <v>18</v>
       </c>
       <c r="U2">
@@ -6751,7 +7327,7 @@
       <c r="S3">
         <v>1</v>
       </c>
-      <c r="T3" s="251" t="s">
+      <c r="T3" s="503" t="s">
         <v>18</v>
       </c>
       <c r="U3">
@@ -6881,13 +7457,13 @@
       <c r="Q2">
         <v>0</v>
       </c>
-      <c r="R2">
-        <v>8230092.9884342412</v>
-      </c>
-      <c r="S2" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="T2" s="27" t="s">
+      <c r="R2" s="279" t="s">
+        <v>18</v>
+      </c>
+      <c r="S2" s="279" t="s">
+        <v>18</v>
+      </c>
+      <c r="T2" s="279" t="s">
         <v>18</v>
       </c>
       <c r="U2">
@@ -6952,7 +7528,7 @@
       <c r="S3">
         <v>1</v>
       </c>
-      <c r="T3" s="27" t="s">
+      <c r="T3" s="279" t="s">
         <v>18</v>
       </c>
       <c r="U3">
@@ -7082,13 +7658,13 @@
       <c r="Q2">
         <v>0</v>
       </c>
-      <c r="R2">
-        <v>8230092.9884342412</v>
-      </c>
-      <c r="S2" s="34" t="s">
-        <v>18</v>
-      </c>
-      <c r="T2" s="34" t="s">
+      <c r="R2" s="286" t="s">
+        <v>18</v>
+      </c>
+      <c r="S2" s="286" t="s">
+        <v>18</v>
+      </c>
+      <c r="T2" s="286" t="s">
         <v>18</v>
       </c>
       <c r="U2">
@@ -7153,7 +7729,7 @@
       <c r="S3">
         <v>1</v>
       </c>
-      <c r="T3" s="34" t="s">
+      <c r="T3" s="286" t="s">
         <v>18</v>
       </c>
       <c r="U3">
@@ -7283,13 +7859,13 @@
       <c r="Q2">
         <v>0</v>
       </c>
-      <c r="R2">
-        <v>8230092.9884342412</v>
-      </c>
-      <c r="S2" s="41" t="s">
-        <v>18</v>
-      </c>
-      <c r="T2" s="41" t="s">
+      <c r="R2" s="293" t="s">
+        <v>18</v>
+      </c>
+      <c r="S2" s="293" t="s">
+        <v>18</v>
+      </c>
+      <c r="T2" s="293" t="s">
         <v>18</v>
       </c>
       <c r="U2">
@@ -7349,12 +7925,12 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>8906662.5461460892</v>
+        <v>8906098.6459059492</v>
       </c>
       <c r="S3">
         <v>1</v>
       </c>
-      <c r="T3" s="41" t="s">
+      <c r="T3" s="293" t="s">
         <v>18</v>
       </c>
       <c r="U3">
@@ -7484,13 +8060,13 @@
       <c r="Q2">
         <v>0</v>
       </c>
-      <c r="R2">
-        <v>8230092.9884342412</v>
-      </c>
-      <c r="S2" s="48" t="s">
-        <v>18</v>
-      </c>
-      <c r="T2" s="48" t="s">
+      <c r="R2" s="300" t="s">
+        <v>18</v>
+      </c>
+      <c r="S2" s="300" t="s">
+        <v>18</v>
+      </c>
+      <c r="T2" s="300" t="s">
         <v>18</v>
       </c>
       <c r="U2">
@@ -7555,7 +8131,7 @@
       <c r="S3">
         <v>1</v>
       </c>
-      <c r="T3" s="48" t="s">
+      <c r="T3" s="300" t="s">
         <v>18</v>
       </c>
       <c r="U3">
@@ -7685,13 +8261,13 @@
       <c r="Q2">
         <v>0</v>
       </c>
-      <c r="R2">
-        <v>8230092.9884342412</v>
-      </c>
-      <c r="S2" s="55" t="s">
-        <v>18</v>
-      </c>
-      <c r="T2" s="55" t="s">
+      <c r="R2" s="307" t="s">
+        <v>18</v>
+      </c>
+      <c r="S2" s="307" t="s">
+        <v>18</v>
+      </c>
+      <c r="T2" s="307" t="s">
         <v>18</v>
       </c>
       <c r="U2">
@@ -7756,7 +8332,7 @@
       <c r="S3">
         <v>1</v>
       </c>
-      <c r="T3" s="55" t="s">
+      <c r="T3" s="307" t="s">
         <v>18</v>
       </c>
       <c r="U3">
@@ -7886,13 +8462,13 @@
       <c r="Q2">
         <v>0</v>
       </c>
-      <c r="R2">
-        <v>8230092.9884342412</v>
-      </c>
-      <c r="S2" s="62" t="s">
-        <v>18</v>
-      </c>
-      <c r="T2" s="62" t="s">
+      <c r="R2" s="314" t="s">
+        <v>18</v>
+      </c>
+      <c r="S2" s="314" t="s">
+        <v>18</v>
+      </c>
+      <c r="T2" s="314" t="s">
         <v>18</v>
       </c>
       <c r="U2">
@@ -7957,7 +8533,7 @@
       <c r="S3">
         <v>1</v>
       </c>
-      <c r="T3" s="62" t="s">
+      <c r="T3" s="314" t="s">
         <v>18</v>
       </c>
       <c r="U3">

</xml_diff>